<commit_message>
14 April data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="165" windowWidth="15375" windowHeight="7875"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -12,10 +18,16 @@
     <sheet name="Total Cases by Race" sheetId="3" r:id="rId3"/>
     <sheet name="Lives Lost by Race" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -240,7 +252,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -335,6 +347,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,28 +654,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AN75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM63" sqref="AM63:AM75"/>
+      <selection pane="topRight" activeCell="AN76" sqref="AN76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="62.44140625" customWidth="1"/>
+    <col min="40" max="40" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -774,8 +788,11 @@
       <c r="AM1" s="1">
         <v>43933</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN1" s="1">
+        <v>43934</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -799,7 +816,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -896,8 +913,11 @@
       <c r="AM3">
         <v>10934</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN3" s="19">
+        <v>11518</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1015,8 +1035,11 @@
       <c r="AM4">
         <v>1955</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN4" s="19">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1116,8 +1139,11 @@
       <c r="AM5">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1187,11 +1213,14 @@
       <c r="AM6">
         <v>507</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN6">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1255,8 +1284,11 @@
       <c r="AM8">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1320,8 +1352,11 @@
       <c r="AM9">
         <v>444</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN9">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1385,8 +1420,11 @@
       <c r="AM10">
         <v>218</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN10">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1450,13 +1488,16 @@
       <c r="AM11">
         <v>226</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN11">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1464,7 +1505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1531,8 +1572,11 @@
       <c r="AL15">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1545,8 +1589,11 @@
       <c r="AL16">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1559,8 +1606,11 @@
       <c r="AL17">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1618,8 +1668,11 @@
       <c r="AL18">
         <v>183</v>
       </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN18">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1677,8 +1730,11 @@
       <c r="AL19">
         <v>227</v>
       </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN19">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1736,13 +1792,16 @@
       <c r="AL20">
         <v>353</v>
       </c>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN20">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1809,8 +1868,11 @@
       <c r="AL23">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN23">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -1823,8 +1885,11 @@
       <c r="AL24">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN24">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -1837,8 +1902,11 @@
       <c r="AL25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -1896,8 +1964,11 @@
       <c r="AL26">
         <v>224</v>
       </c>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN26">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -1955,8 +2026,11 @@
       <c r="AL27">
         <v>290</v>
       </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN27">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -2014,13 +2088,16 @@
       <c r="AL28">
         <v>364</v>
       </c>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN28">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -2078,8 +2155,11 @@
       <c r="AL31">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -2089,8 +2169,11 @@
       <c r="AL32">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN32">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2100,8 +2183,11 @@
       <c r="AL33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
@@ -2159,8 +2245,11 @@
       <c r="AL34">
         <v>159</v>
       </c>
-    </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN34">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
@@ -2215,8 +2304,11 @@
       <c r="AL35">
         <v>174</v>
       </c>
-    </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
@@ -2274,13 +2366,16 @@
       <c r="AL36">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN36">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
@@ -2341,8 +2436,11 @@
       <c r="AL39">
         <v>52</v>
       </c>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN39">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -2355,8 +2453,11 @@
       <c r="AL40">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN40">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -2369,8 +2470,11 @@
       <c r="AL41">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -2428,8 +2532,11 @@
       <c r="AL42">
         <v>224</v>
       </c>
-    </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN42">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>18</v>
       </c>
@@ -2442,8 +2549,11 @@
       <c r="AL43">
         <v>267</v>
       </c>
-    </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN43">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -2453,13 +2563,16 @@
       <c r="AL44">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>20</v>
       </c>
@@ -2505,8 +2618,11 @@
       <c r="AL47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>20</v>
       </c>
@@ -2516,8 +2632,11 @@
       <c r="AL48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -2527,8 +2646,11 @@
       <c r="AL49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>20</v>
       </c>
@@ -2574,8 +2696,11 @@
       <c r="AL50">
         <v>87</v>
       </c>
-    </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN50">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>20</v>
       </c>
@@ -2621,8 +2746,11 @@
       <c r="AL51">
         <v>92</v>
       </c>
-    </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN51">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -2668,8 +2796,11 @@
       <c r="AL52">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>22</v>
       </c>
@@ -2715,8 +2846,11 @@
       <c r="AL54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>22</v>
       </c>
@@ -2726,8 +2860,11 @@
       <c r="AL55">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>22</v>
       </c>
@@ -2737,8 +2874,11 @@
       <c r="AL56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>22</v>
       </c>
@@ -2784,8 +2924,11 @@
       <c r="AL57">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -2831,8 +2974,11 @@
       <c r="AL58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>22</v>
       </c>
@@ -2878,8 +3024,11 @@
       <c r="AL59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>22</v>
       </c>
@@ -2889,13 +3038,16 @@
       <c r="AL60">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>24</v>
       </c>
@@ -2941,8 +3093,11 @@
       <c r="AM63">
         <v>48</v>
       </c>
-    </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>24</v>
       </c>
@@ -2988,8 +3143,11 @@
       <c r="AM64">
         <v>248</v>
       </c>
-    </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN64">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>24</v>
       </c>
@@ -3035,8 +3193,11 @@
       <c r="AM65">
         <v>248</v>
       </c>
-    </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN65">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>33</v>
       </c>
@@ -3082,8 +3243,11 @@
       <c r="AM67">
         <v>38</v>
       </c>
-    </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN67">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>33</v>
       </c>
@@ -3129,8 +3293,11 @@
       <c r="AM68">
         <v>33</v>
       </c>
-    </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN68">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>33</v>
       </c>
@@ -3176,8 +3343,11 @@
       <c r="AM69">
         <v>71</v>
       </c>
-    </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN69">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>33</v>
       </c>
@@ -3223,8 +3393,11 @@
       <c r="AM70">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN70">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>34</v>
       </c>
@@ -3270,8 +3443,11 @@
       <c r="AM72">
         <v>21</v>
       </c>
-    </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN72">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>34</v>
       </c>
@@ -3317,8 +3493,11 @@
       <c r="AM73">
         <v>144</v>
       </c>
-    </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN73">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>34</v>
       </c>
@@ -3352,8 +3531,11 @@
       <c r="AM74">
         <v>144</v>
       </c>
-    </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN74">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="75" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>34</v>
       </c>
@@ -3397,6 +3579,9 @@
         <v>2</v>
       </c>
       <c r="AM75">
+        <v>2</v>
+      </c>
+      <c r="AN75">
         <v>2</v>
       </c>
     </row>
@@ -3407,20 +3592,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:O11"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N11"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -3463,8 +3649,11 @@
       <c r="N2" s="9">
         <v>43933</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="9">
+        <v>43934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -3507,8 +3696,11 @@
       <c r="N3">
         <v>223</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -3551,8 +3743,11 @@
       <c r="N4">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -3595,8 +3790,11 @@
       <c r="N5">
         <v>146</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -3639,8 +3837,11 @@
       <c r="N6">
         <v>312</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -3683,8 +3884,11 @@
       <c r="N7">
         <v>257</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -3727,8 +3931,11 @@
       <c r="N8">
         <v>288</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -3771,8 +3978,11 @@
       <c r="N9">
         <v>292</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -3815,8 +4025,11 @@
       <c r="N10">
         <v>228</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
@@ -3858,6 +4071,9 @@
       </c>
       <c r="N11">
         <v>29</v>
+      </c>
+      <c r="O11">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3867,20 +4083,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -3906,8 +4123,11 @@
       <c r="I2" s="9">
         <v>43933</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="9">
+        <v>43934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>41</v>
       </c>
@@ -3915,7 +4135,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
@@ -3943,8 +4163,11 @@
       <c r="I4">
         <v>1955</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -3972,8 +4195,11 @@
       <c r="I5">
         <v>391</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -4001,8 +4227,11 @@
       <c r="I6">
         <v>365</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -4030,8 +4259,11 @@
       <c r="I7">
         <v>884</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
@@ -4059,8 +4291,11 @@
       <c r="I8">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>45</v>
       </c>
@@ -4088,8 +4323,11 @@
       <c r="I9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>55</v>
       </c>
@@ -4113,8 +4351,11 @@
       <c r="I10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -4142,8 +4383,11 @@
       <c r="I11">
         <v>256</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
@@ -4171,8 +4415,11 @@
       <c r="I12">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -4183,7 +4430,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
@@ -4211,8 +4458,11 @@
       <c r="I14">
         <v>496</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
@@ -4240,8 +4490,11 @@
       <c r="I15">
         <v>263</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
@@ -4269,8 +4522,11 @@
       <c r="I16">
         <v>1191</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>47</v>
       </c>
@@ -4297,6 +4553,9 @@
       </c>
       <c r="I17">
         <v>5</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -4306,19 +4565,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -4343,14 +4603,17 @@
       <c r="I1" s="9">
         <v>43933</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="9">
+        <v>43934</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>54</v>
       </c>
@@ -4379,8 +4642,11 @@
       <c r="I3">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
@@ -4408,8 +4674,11 @@
       <c r="I4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -4437,8 +4706,11 @@
       <c r="I5">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>51</v>
       </c>
@@ -4466,8 +4738,11 @@
       <c r="I6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -4495,8 +4770,11 @@
       <c r="I7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
@@ -4522,10 +4800,275 @@
         <v>0</v>
       </c>
       <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
+    <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <xsd:import namespace="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8e61eea9-d51d-4f9c-960b-1b037651d93e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="248ed0f8-11d3-4141-bb91-6b69a0801941" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
17 April data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{6FAC7698-CF08-4F3E-987E-2BB2033184DF}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="Total Cases by Race" sheetId="3" r:id="rId3"/>
     <sheet name="Lives Lost by Race" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -264,7 +258,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -367,7 +361,6 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,29 +667,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <pane xSplit="2" topLeftCell="AP1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AQ38" sqref="AQ38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" customWidth="1"/>
-    <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="40" max="42" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="40" max="43" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -817,8 +810,11 @@
       <c r="AP1" s="1">
         <v>43936</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ1" s="1">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -842,7 +838,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -948,8 +944,11 @@
       <c r="AP3">
         <v>12150</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ3">
+        <v>12643</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1076,8 +1075,11 @@
       <c r="AP4">
         <v>2350</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ4">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1186,8 +1188,11 @@
       <c r="AP5">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1266,11 +1271,14 @@
       <c r="AP6">
         <v>552</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ6">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1343,8 +1351,11 @@
       <c r="AP8">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ8">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1417,8 +1428,11 @@
       <c r="AP9">
         <v>443</v>
       </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ9">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1491,8 +1505,11 @@
       <c r="AP10">
         <v>203</v>
       </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ10">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1565,13 +1582,16 @@
       <c r="AP11">
         <v>240</v>
       </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ11">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1579,7 +1599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1655,8 +1675,11 @@
       <c r="AP15">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1678,8 +1701,11 @@
       <c r="AP16">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ16">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1701,8 +1727,11 @@
       <c r="AP17">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ17">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1769,8 +1798,11 @@
       <c r="AP18">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ18">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1837,8 +1869,11 @@
       <c r="AP19">
         <v>127</v>
       </c>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ19">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1905,13 +1940,16 @@
       <c r="AP20">
         <v>476</v>
       </c>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ20">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1987,8 +2025,11 @@
       <c r="AP23">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ23">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2010,8 +2051,11 @@
       <c r="AP24">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ24">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -2033,8 +2077,11 @@
       <c r="AP25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2101,8 +2148,11 @@
       <c r="AP26">
         <v>178</v>
       </c>
-    </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ26">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -2169,8 +2219,11 @@
       <c r="AP27">
         <v>236</v>
       </c>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ27">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -2237,13 +2290,16 @@
       <c r="AP28">
         <v>496</v>
       </c>
-    </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ28">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -2310,8 +2366,11 @@
       <c r="AP31">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -2330,8 +2389,11 @@
       <c r="AP32">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2350,8 +2412,11 @@
       <c r="AP33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
@@ -2418,8 +2483,11 @@
       <c r="AP34">
         <v>149</v>
       </c>
-    </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ34">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
@@ -2483,8 +2551,11 @@
       <c r="AP35">
         <v>168</v>
       </c>
-    </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
@@ -2551,13 +2622,16 @@
       <c r="AP36">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ36">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
@@ -2627,8 +2701,11 @@
       <c r="AP39">
         <v>62</v>
       </c>
-    </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ39">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -2650,8 +2727,11 @@
       <c r="AP40">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ40">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -2673,8 +2753,11 @@
       <c r="AP41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ41">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -2741,8 +2824,11 @@
       <c r="AP42">
         <v>414</v>
       </c>
-    </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ42">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>18</v>
       </c>
@@ -2764,8 +2850,11 @@
       <c r="AP43">
         <v>435</v>
       </c>
-    </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ43">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="44" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -2784,8 +2873,11 @@
       <c r="AP44">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -2798,16 +2890,19 @@
       <c r="AP45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>20</v>
       </c>
@@ -2862,8 +2957,11 @@
       <c r="AP48">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ48">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -2882,8 +2980,11 @@
       <c r="AP49">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>20</v>
       </c>
@@ -2902,8 +3003,11 @@
       <c r="AP50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>20</v>
       </c>
@@ -2958,8 +3062,11 @@
       <c r="AP51">
         <v>62</v>
       </c>
-    </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ51">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -3014,8 +3121,11 @@
       <c r="AP52">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ52">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>20</v>
       </c>
@@ -3070,8 +3180,11 @@
       <c r="AP53">
         <v>40</v>
       </c>
-    </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ53">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>20</v>
       </c>
@@ -3084,8 +3197,11 @@
       <c r="AP54">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>22</v>
       </c>
@@ -3140,8 +3256,11 @@
       <c r="AP56">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>22</v>
       </c>
@@ -3160,8 +3279,11 @@
       <c r="AP57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -3180,8 +3302,11 @@
       <c r="AP58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>22</v>
       </c>
@@ -3236,8 +3361,11 @@
       <c r="AP59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>22</v>
       </c>
@@ -3292,8 +3420,11 @@
       <c r="AP60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>22</v>
       </c>
@@ -3348,8 +3479,11 @@
       <c r="AP61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -3368,13 +3502,16 @@
       <c r="AP62">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>24</v>
       </c>
@@ -3429,8 +3566,11 @@
       <c r="AP65">
         <v>77</v>
       </c>
-    </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ65">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>24</v>
       </c>
@@ -3485,8 +3625,11 @@
       <c r="AP66">
         <v>301</v>
       </c>
-    </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ66">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="67" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>24</v>
       </c>
@@ -3541,8 +3684,11 @@
       <c r="AP67">
         <v>257</v>
       </c>
-    </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ67">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="68" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>24</v>
       </c>
@@ -3555,8 +3701,11 @@
       <c r="AP68">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>33</v>
       </c>
@@ -3611,8 +3760,11 @@
       <c r="AP70">
         <v>47</v>
       </c>
-    </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ70">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>33</v>
       </c>
@@ -3667,8 +3819,11 @@
       <c r="AP71">
         <v>24</v>
       </c>
-    </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ71">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>33</v>
       </c>
@@ -3723,8 +3878,11 @@
       <c r="AP72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ72">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>33</v>
       </c>
@@ -3779,8 +3937,11 @@
       <c r="AP73">
         <v>19</v>
       </c>
-    </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ73">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>34</v>
       </c>
@@ -3835,8 +3996,11 @@
       <c r="AP75">
         <v>32</v>
       </c>
-    </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ75">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>34</v>
       </c>
@@ -3891,8 +4055,11 @@
       <c r="AP76">
         <v>105</v>
       </c>
-    </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>34</v>
       </c>
@@ -3935,8 +4102,11 @@
       <c r="AP77">
         <v>105</v>
       </c>
-    </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ77">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>34</v>
       </c>
@@ -3991,8 +4161,11 @@
       <c r="AP78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
@@ -4003,6 +4176,9 @@
         <v>4</v>
       </c>
       <c r="AP79">
+        <v>4</v>
+      </c>
+      <c r="AQ79">
         <v>4</v>
       </c>
     </row>
@@ -4013,21 +4189,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:Q11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="15" max="17" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -4076,11 +4252,14 @@
       <c r="P2" s="9">
         <v>43935</v>
       </c>
-      <c r="Q2" s="21">
+      <c r="Q2" s="9">
         <v>43936</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" s="9">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -4132,8 +4311,11 @@
       <c r="Q3">
         <v>264</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -4185,8 +4367,11 @@
       <c r="Q4">
         <v>193</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -4238,8 +4423,11 @@
       <c r="Q5">
         <v>169</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -4291,8 +4479,11 @@
       <c r="Q6">
         <v>389</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -4344,8 +4535,11 @@
       <c r="Q7">
         <v>311</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -4397,8 +4591,11 @@
       <c r="Q8">
         <v>313</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -4450,8 +4647,11 @@
       <c r="Q9">
         <v>361</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -4503,8 +4703,11 @@
       <c r="Q10">
         <v>293</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
@@ -4555,6 +4758,9 @@
       </c>
       <c r="Q11">
         <v>57</v>
+      </c>
+      <c r="R11">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4564,21 +4770,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M17"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -4613,8 +4819,11 @@
       <c r="L2" s="9">
         <v>43936</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="9">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>41</v>
       </c>
@@ -4622,7 +4831,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
@@ -4659,8 +4868,11 @@
       <c r="L4">
         <v>2350</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -4697,8 +4909,11 @@
       <c r="L5">
         <v>404</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -4735,8 +4950,11 @@
       <c r="L6">
         <v>439</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -4773,8 +4991,11 @@
       <c r="L7">
         <v>1089</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
@@ -4811,8 +5032,11 @@
       <c r="L8">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>45</v>
       </c>
@@ -4849,8 +5073,11 @@
       <c r="L9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>55</v>
       </c>
@@ -4883,8 +5110,11 @@
       <c r="L10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -4921,8 +5151,11 @@
       <c r="L11">
         <v>345</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
@@ -4959,8 +5192,11 @@
       <c r="L12">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -4971,7 +5207,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
@@ -5008,8 +5244,11 @@
       <c r="L14">
         <v>539</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
@@ -5046,8 +5285,11 @@
       <c r="L15">
         <v>361</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
@@ -5084,8 +5326,11 @@
       <c r="L16">
         <v>1445</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>47</v>
       </c>
@@ -5121,6 +5366,9 @@
       </c>
       <c r="L17">
         <v>5</v>
+      </c>
+      <c r="M17">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -5130,20 +5378,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -5177,14 +5425,17 @@
       <c r="L1" s="9">
         <v>43936</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="9">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>54</v>
       </c>
@@ -5222,8 +5473,11 @@
       <c r="L3">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
@@ -5260,8 +5514,11 @@
       <c r="L4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -5298,8 +5555,11 @@
       <c r="L5">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>51</v>
       </c>
@@ -5336,8 +5596,11 @@
       <c r="L6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -5374,8 +5637,11 @@
       <c r="L7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
@@ -5410,6 +5676,9 @@
         <v>0</v>
       </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>0</v>
       </c>
     </row>
@@ -5419,6 +5688,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -5621,22 +5905,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5653,29 +5947,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
20 April data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="532" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5633416B-E455-4ECA-9444-D36F0D8B3267}"/>
+  <xr:revisionPtr revIDLastSave="666" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2C2F0EE6-02F6-4A27-9C9B-DB5F0031253F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Total Cases by Ward" sheetId="2" r:id="rId2"/>
     <sheet name="Total Cases by Race" sheetId="3" r:id="rId3"/>
     <sheet name="Lives Lost by Race" sheetId="4" r:id="rId4"/>
+    <sheet name="Lives Lost by Ward" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="77">
   <si>
     <t>Testing</t>
   </si>
@@ -262,6 +263,9 @@
   </si>
   <si>
     <t>Total Number of Lives Lost Among Personnel</t>
+  </si>
+  <si>
+    <t>Homeless</t>
   </si>
 </sst>
 </file>
@@ -324,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,6 +374,12 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,21 +694,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS80"/>
+  <dimension ref="A1:AT80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AS81" sqref="AS81"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AT1" sqref="AT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.5546875" customWidth="1"/>
     <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="40" max="45" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="46" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -828,8 +838,11 @@
       <c r="AS1" s="1">
         <v>43939</v>
       </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT1" s="1">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -853,7 +866,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -968,8 +981,11 @@
       <c r="AS3">
         <v>13699</v>
       </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT3">
+        <v>14113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1105,8 +1121,11 @@
       <c r="AS4">
         <v>2793</v>
       </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT4">
+        <v>2927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1224,8 +1243,11 @@
       <c r="AS5">
         <v>96</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1313,11 +1335,14 @@
       <c r="AS6">
         <v>622</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT6">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1399,8 +1424,11 @@
       <c r="AS8">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1482,8 +1510,11 @@
       <c r="AS9">
         <v>443</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT9">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1565,8 +1596,11 @@
       <c r="AS10">
         <v>203</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT10">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1648,13 +1682,16 @@
       <c r="AS11">
         <v>240</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT11">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1662,7 +1699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1747,8 +1784,11 @@
       <c r="AS15">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1779,8 +1819,11 @@
       <c r="AS16">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1811,8 +1854,11 @@
       <c r="AS17">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1888,8 +1934,11 @@
       <c r="AS18">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1965,8 +2014,11 @@
       <c r="AS19">
         <v>136</v>
       </c>
-    </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT19">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2042,13 +2094,16 @@
       <c r="AS20">
         <v>528</v>
       </c>
-    </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT20">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -2133,8 +2188,11 @@
       <c r="AS23">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT23">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2165,8 +2223,11 @@
       <c r="AS24">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -2197,8 +2258,11 @@
       <c r="AS25">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2274,8 +2338,11 @@
       <c r="AS26">
         <v>136</v>
       </c>
-    </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT26">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -2351,8 +2418,11 @@
       <c r="AS27">
         <v>196</v>
       </c>
-    </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT27">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -2428,13 +2498,16 @@
       <c r="AS28">
         <v>580</v>
       </c>
-    </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT28">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -2510,8 +2583,11 @@
       <c r="AS31">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -2539,8 +2615,11 @@
       <c r="AS32">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT32">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2568,8 +2647,11 @@
       <c r="AS33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
@@ -2645,8 +2727,11 @@
       <c r="AS34">
         <v>134</v>
       </c>
-    </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT34">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
@@ -2719,8 +2804,11 @@
       <c r="AS35">
         <v>152</v>
       </c>
-    </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
@@ -2796,8 +2884,11 @@
       <c r="AS36">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT36">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
@@ -2807,16 +2898,19 @@
       <c r="AS37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -2895,8 +2989,11 @@
       <c r="AS40">
         <v>82</v>
       </c>
-    </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT40">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -2927,8 +3024,11 @@
       <c r="AS41">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -2959,8 +3059,11 @@
       <c r="AS42">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>18</v>
       </c>
@@ -3036,8 +3139,11 @@
       <c r="AS43">
         <v>849</v>
       </c>
-    </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT43">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -3068,8 +3174,11 @@
       <c r="AS44">
         <v>880</v>
       </c>
-    </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT44">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -3097,8 +3206,11 @@
       <c r="AS45">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>18</v>
       </c>
@@ -3120,16 +3232,19 @@
       <c r="AS46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -3193,8 +3308,11 @@
       <c r="AS49">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT49">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>20</v>
       </c>
@@ -3222,8 +3340,11 @@
       <c r="AS50">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT50">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>20</v>
       </c>
@@ -3251,8 +3372,11 @@
       <c r="AS51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -3316,8 +3440,11 @@
       <c r="AS52">
         <v>64</v>
       </c>
-    </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT52">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>20</v>
       </c>
@@ -3381,8 +3508,11 @@
       <c r="AS53">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT53">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>20</v>
       </c>
@@ -3446,8 +3576,11 @@
       <c r="AS54">
         <v>50</v>
       </c>
-    </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT54">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>20</v>
       </c>
@@ -3469,8 +3602,11 @@
       <c r="AS55">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>22</v>
       </c>
@@ -3534,8 +3670,11 @@
       <c r="AS57">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT57">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -3563,8 +3702,11 @@
       <c r="AS58">
         <v>7</v>
       </c>
-    </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>22</v>
       </c>
@@ -3592,8 +3734,11 @@
       <c r="AS59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>22</v>
       </c>
@@ -3657,8 +3802,11 @@
       <c r="AS60">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT60">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>22</v>
       </c>
@@ -3722,8 +3870,11 @@
       <c r="AS61">
         <v>17</v>
       </c>
-    </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT61">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -3787,8 +3938,11 @@
       <c r="AS62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>22</v>
       </c>
@@ -3816,13 +3970,16 @@
       <c r="AS63">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:46" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>24</v>
       </c>
@@ -3886,8 +4043,11 @@
       <c r="AS66">
         <v>94</v>
       </c>
-    </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT66">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>24</v>
       </c>
@@ -3951,8 +4111,11 @@
       <c r="AS67">
         <v>280</v>
       </c>
-    </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT67">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>24</v>
       </c>
@@ -4016,8 +4179,11 @@
       <c r="AS68">
         <v>243</v>
       </c>
-    </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT68">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -4039,8 +4205,11 @@
       <c r="AS69">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT69">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>33</v>
       </c>
@@ -4104,8 +4273,11 @@
       <c r="AS71">
         <v>56</v>
       </c>
-    </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT71">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>33</v>
       </c>
@@ -4169,8 +4341,11 @@
       <c r="AS72">
         <v>26</v>
       </c>
-    </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT72">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>33</v>
       </c>
@@ -4234,8 +4409,11 @@
       <c r="AS73">
         <v>82</v>
       </c>
-    </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT73">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>33</v>
       </c>
@@ -4299,8 +4477,11 @@
       <c r="AS74">
         <v>22</v>
       </c>
-    </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT74">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>34</v>
       </c>
@@ -4364,8 +4545,11 @@
       <c r="AS76">
         <v>36</v>
       </c>
-    </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT76">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>34</v>
       </c>
@@ -4429,8 +4613,11 @@
       <c r="AS77">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT77">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>34</v>
       </c>
@@ -4482,8 +4669,11 @@
       <c r="AS78">
         <v>74</v>
       </c>
-    </row>
-    <row r="79" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT78">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
@@ -4547,8 +4737,11 @@
       <c r="AS79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AT79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
@@ -4568,6 +4761,9 @@
         <v>4</v>
       </c>
       <c r="AS80">
+        <v>4</v>
+      </c>
+      <c r="AT80">
         <v>4</v>
       </c>
     </row>
@@ -4579,10 +4775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:T11"/>
+  <dimension ref="A2:U11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4592,7 +4788,7 @@
     <col min="15" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -4653,8 +4849,11 @@
       <c r="T2" s="9">
         <v>43939</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U2" s="9">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -4715,8 +4914,11 @@
       <c r="T3">
         <v>330</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -4777,8 +4979,11 @@
       <c r="T4">
         <v>218</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -4839,8 +5044,11 @@
       <c r="T5">
         <v>211</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U5">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -4901,8 +5109,11 @@
       <c r="T6">
         <v>477</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U6">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -4963,8 +5174,11 @@
       <c r="T7">
         <v>363</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U7">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -5025,8 +5239,11 @@
       <c r="T8">
         <v>355</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U8">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -5087,8 +5304,11 @@
       <c r="T9">
         <v>440</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U9">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -5149,8 +5369,11 @@
       <c r="T10">
         <v>354</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U10">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
@@ -5210,6 +5433,9 @@
       </c>
       <c r="T11">
         <v>45</v>
+      </c>
+      <c r="U11">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -5220,10 +5446,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:O17"/>
+  <dimension ref="A2:P17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5233,7 +5459,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -5277,8 +5503,11 @@
       <c r="O2" s="9">
         <v>43939</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="9">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>41</v>
       </c>
@@ -5286,7 +5515,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
@@ -5332,8 +5561,11 @@
       <c r="O4">
         <v>2793</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>2927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -5379,8 +5611,11 @@
       <c r="O5">
         <v>358</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -5426,8 +5661,11 @@
       <c r="O6">
         <v>548</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -5473,8 +5711,11 @@
       <c r="O7">
         <v>1403</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
@@ -5520,8 +5761,11 @@
       <c r="O8">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>45</v>
       </c>
@@ -5567,8 +5811,11 @@
       <c r="O9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>55</v>
       </c>
@@ -5610,8 +5857,11 @@
       <c r="O10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -5657,8 +5907,11 @@
       <c r="O11">
         <v>390</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
@@ -5704,8 +5957,11 @@
       <c r="O12">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -5716,7 +5972,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
@@ -5762,8 +6018,11 @@
       <c r="O14">
         <v>500</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
@@ -5809,8 +6068,11 @@
       <c r="O15">
         <v>494</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
@@ -5856,8 +6118,11 @@
       <c r="O16">
         <v>1783</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>47</v>
       </c>
@@ -5901,6 +6166,9 @@
         <v>7</v>
       </c>
       <c r="O17">
+        <v>16</v>
+      </c>
+      <c r="P17">
         <v>16</v>
       </c>
     </row>
@@ -5912,10 +6180,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5924,7 +6192,7 @@
     <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -5967,14 +6235,17 @@
       <c r="O1" s="9">
         <v>43939</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="9">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>54</v>
       </c>
@@ -6021,8 +6292,11 @@
       <c r="O3">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
@@ -6068,8 +6342,11 @@
       <c r="O4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -6115,8 +6392,11 @@
       <c r="O5">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>51</v>
       </c>
@@ -6162,8 +6442,11 @@
       <c r="O6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -6209,8 +6492,11 @@
       <c r="O7">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
@@ -6254,6 +6540,123 @@
         <v>0</v>
       </c>
       <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DE713F-971D-4CE1-B1A8-BE60A2507C58}">
+  <dimension ref="A2:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="9">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="21">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="22">
         <v>0</v>
       </c>
     </row>
@@ -6466,18 +6869,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6500,26 +6903,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
21 April data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="666" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2C2F0EE6-02F6-4A27-9C9B-DB5F0031253F}"/>
+  <xr:revisionPtr revIDLastSave="774" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{09447612-0F80-4C50-B99D-BE02F3D0BAEA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,21 +694,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT80"/>
+  <dimension ref="A1:AU80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AT1" sqref="AT1"/>
+      <selection pane="topRight" activeCell="AU1" sqref="AU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.5546875" customWidth="1"/>
     <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="40" max="46" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="47" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -841,8 +841,11 @@
       <c r="AT1" s="1">
         <v>43940</v>
       </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU1" s="1">
+        <v>43941</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -866,7 +869,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -984,8 +987,11 @@
       <c r="AT3">
         <v>14113</v>
       </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU3">
+        <v>14939</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1124,8 +1130,11 @@
       <c r="AT4">
         <v>2927</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU4">
+        <v>3098</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1246,8 +1255,11 @@
       <c r="AT5">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1338,11 +1350,14 @@
       <c r="AT6">
         <v>630</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU6">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1427,8 +1442,11 @@
       <c r="AT8">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1513,8 +1531,11 @@
       <c r="AT9">
         <v>444</v>
       </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU9">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1599,8 +1620,11 @@
       <c r="AT10">
         <v>198</v>
       </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU10">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1685,13 +1709,16 @@
       <c r="AT11">
         <v>246</v>
       </c>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU11">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1699,7 +1726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1787,8 +1814,11 @@
       <c r="AT15">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1822,8 +1852,11 @@
       <c r="AT16">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1857,8 +1890,11 @@
       <c r="AT17">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1937,8 +1973,11 @@
       <c r="AT18">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU18">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2017,8 +2056,11 @@
       <c r="AT19">
         <v>139</v>
       </c>
-    </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU19">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2097,13 +2139,16 @@
       <c r="AT20">
         <v>544</v>
       </c>
-    </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU20">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -2191,8 +2236,11 @@
       <c r="AT23">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2226,8 +2274,11 @@
       <c r="AT24">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU24">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -2261,8 +2312,11 @@
       <c r="AT25">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2341,8 +2395,11 @@
       <c r="AT26">
         <v>135</v>
       </c>
-    </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU26">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -2421,8 +2478,11 @@
       <c r="AT27">
         <v>196</v>
       </c>
-    </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU27">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -2501,13 +2561,16 @@
       <c r="AT28">
         <v>580</v>
       </c>
-    </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU28">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -2586,8 +2649,11 @@
       <c r="AT31">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU31">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -2618,8 +2684,11 @@
       <c r="AT32">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2650,8 +2719,11 @@
       <c r="AT33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
@@ -2730,8 +2802,11 @@
       <c r="AT34">
         <v>134</v>
       </c>
-    </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU34">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
@@ -2807,8 +2882,11 @@
       <c r="AT35">
         <v>152</v>
       </c>
-    </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
@@ -2887,8 +2965,11 @@
       <c r="AT36">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU36">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
@@ -2901,16 +2982,19 @@
       <c r="AT37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -2992,8 +3076,11 @@
       <c r="AT40">
         <v>90</v>
       </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU40">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -3027,8 +3114,11 @@
       <c r="AT41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU41">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -3062,8 +3152,11 @@
       <c r="AT42">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU42">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>18</v>
       </c>
@@ -3142,8 +3235,11 @@
       <c r="AT43">
         <v>840</v>
       </c>
-    </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU43">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -3177,8 +3273,11 @@
       <c r="AT44">
         <v>880</v>
       </c>
-    </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU44">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -3209,8 +3308,11 @@
       <c r="AT45">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>18</v>
       </c>
@@ -3235,16 +3337,19 @@
       <c r="AT46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -3311,8 +3416,11 @@
       <c r="AT49">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU49">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>20</v>
       </c>
@@ -3343,8 +3451,11 @@
       <c r="AT50">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU50">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>20</v>
       </c>
@@ -3375,8 +3486,11 @@
       <c r="AT51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -3443,8 +3557,11 @@
       <c r="AT52">
         <v>64</v>
       </c>
-    </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU52">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>20</v>
       </c>
@@ -3511,8 +3628,11 @@
       <c r="AT53">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU53">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>20</v>
       </c>
@@ -3579,8 +3699,11 @@
       <c r="AT54">
         <v>50</v>
       </c>
-    </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU54">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>20</v>
       </c>
@@ -3605,8 +3728,11 @@
       <c r="AT55">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>22</v>
       </c>
@@ -3673,8 +3799,11 @@
       <c r="AT57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU57">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -3705,8 +3834,11 @@
       <c r="AT58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>22</v>
       </c>
@@ -3737,8 +3869,11 @@
       <c r="AT59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>22</v>
       </c>
@@ -3805,8 +3940,11 @@
       <c r="AT60">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU60">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>22</v>
       </c>
@@ -3873,8 +4011,11 @@
       <c r="AT61">
         <v>19</v>
       </c>
-    </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU61">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -3941,8 +4082,11 @@
       <c r="AT62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>22</v>
       </c>
@@ -3973,13 +4117,16 @@
       <c r="AT63">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>24</v>
       </c>
@@ -4046,8 +4193,11 @@
       <c r="AT66">
         <v>107</v>
       </c>
-    </row>
-    <row r="67" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU66">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>24</v>
       </c>
@@ -4114,8 +4264,11 @@
       <c r="AT67">
         <v>227</v>
       </c>
-    </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU67">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>24</v>
       </c>
@@ -4182,8 +4335,11 @@
       <c r="AT68">
         <v>227</v>
       </c>
-    </row>
-    <row r="69" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU68">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -4208,8 +4364,11 @@
       <c r="AT69">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>33</v>
       </c>
@@ -4276,8 +4435,11 @@
       <c r="AT71">
         <v>57</v>
       </c>
-    </row>
-    <row r="72" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU71">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>33</v>
       </c>
@@ -4344,8 +4506,11 @@
       <c r="AT72">
         <v>26</v>
       </c>
-    </row>
-    <row r="73" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU72">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>33</v>
       </c>
@@ -4412,8 +4577,11 @@
       <c r="AT73">
         <v>83</v>
       </c>
-    </row>
-    <row r="74" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU73">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>33</v>
       </c>
@@ -4480,8 +4648,11 @@
       <c r="AT74">
         <v>22</v>
       </c>
-    </row>
-    <row r="76" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU74">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>34</v>
       </c>
@@ -4548,8 +4719,11 @@
       <c r="AT76">
         <v>37</v>
       </c>
-    </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU76">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>34</v>
       </c>
@@ -4616,8 +4790,11 @@
       <c r="AT77">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU77">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>34</v>
       </c>
@@ -4672,8 +4849,11 @@
       <c r="AT78">
         <v>74</v>
       </c>
-    </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU78">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
@@ -4740,8 +4920,11 @@
       <c r="AT79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
@@ -4765,6 +4948,9 @@
       </c>
       <c r="AT80">
         <v>4</v>
+      </c>
+      <c r="AU80">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4775,10 +4961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:U11"/>
+  <dimension ref="A2:V11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4788,7 +4974,7 @@
     <col min="15" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -4852,8 +5038,11 @@
       <c r="U2" s="9">
         <v>43940</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V2" s="9">
+        <v>43941</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -4917,8 +5106,11 @@
       <c r="U3">
         <v>344</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -4982,8 +5174,11 @@
       <c r="U4">
         <v>225</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V4">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -5047,8 +5242,11 @@
       <c r="U5">
         <v>226</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -5112,8 +5310,11 @@
       <c r="U6">
         <v>499</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V6">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -5177,8 +5378,11 @@
       <c r="U7">
         <v>383</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V7">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -5242,8 +5446,11 @@
       <c r="U8">
         <v>366</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V8">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -5307,8 +5514,11 @@
       <c r="U9">
         <v>454</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V9">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -5372,8 +5582,11 @@
       <c r="U10">
         <v>376</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V10">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
@@ -5436,6 +5649,9 @@
       </c>
       <c r="U11">
         <v>54</v>
+      </c>
+      <c r="V11">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -5446,10 +5662,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:P17"/>
+  <dimension ref="A2:Q17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5459,7 +5675,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -5506,8 +5722,11 @@
       <c r="P2" s="9">
         <v>43940</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="9">
+        <v>43941</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>41</v>
       </c>
@@ -5515,7 +5734,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
@@ -5564,8 +5783,11 @@
       <c r="P4">
         <v>2927</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4">
+        <v>3098</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -5614,8 +5836,11 @@
       <c r="P5">
         <v>406</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -5664,8 +5889,11 @@
       <c r="P6">
         <v>553</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -5714,8 +5942,11 @@
       <c r="P7">
         <v>1458</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q7">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
@@ -5764,8 +5995,11 @@
       <c r="P8">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q8">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>45</v>
       </c>
@@ -5814,8 +6048,11 @@
       <c r="P9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>55</v>
       </c>
@@ -5860,8 +6097,11 @@
       <c r="P10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -5910,8 +6150,11 @@
       <c r="P11">
         <v>415</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q11">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
@@ -5960,8 +6203,11 @@
       <c r="P12">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -5972,7 +6218,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
@@ -6021,8 +6267,11 @@
       <c r="P14">
         <v>563</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
@@ -6071,8 +6320,11 @@
       <c r="P15">
         <v>516</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q15">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
@@ -6121,8 +6373,11 @@
       <c r="P16">
         <v>1832</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q16">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>47</v>
       </c>
@@ -6170,6 +6425,9 @@
       </c>
       <c r="P17">
         <v>16</v>
+      </c>
+      <c r="Q17">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -6180,10 +6438,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6192,7 +6450,7 @@
     <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -6238,14 +6496,17 @@
       <c r="P1" s="9">
         <v>43940</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" s="9">
+        <v>43941</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>54</v>
       </c>
@@ -6295,8 +6556,11 @@
       <c r="P3">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
@@ -6345,8 +6609,11 @@
       <c r="P4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -6395,8 +6662,11 @@
       <c r="P5">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>51</v>
       </c>
@@ -6445,8 +6715,11 @@
       <c r="P6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -6495,8 +6768,11 @@
       <c r="P7">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
@@ -6543,6 +6819,9 @@
         <v>0</v>
       </c>
       <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
         <v>0</v>
       </c>
     </row>
@@ -6553,10 +6832,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DE713F-971D-4CE1-B1A8-BE60A2507C58}">
-  <dimension ref="A2:B13"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6564,99 +6843,135 @@
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="9">
         <v>43940</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="9">
+        <v>43941</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="21">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="22">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="22">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
       <c r="B6" s="22">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="22">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
       <c r="B8" s="22">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
       <c r="B9" s="22">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
       <c r="B10" s="22">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
       <c r="B11" s="22">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="22">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="22">
+        <v>0</v>
+      </c>
+      <c r="C13">
         <v>0</v>
       </c>
     </row>
@@ -6666,6 +6981,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -6868,12 +7189,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6884,6 +7199,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6902,23 +7234,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
22 April data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="774" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{09447612-0F80-4C50-B99D-BE02F3D0BAEA}"/>
+  <xr:revisionPtr revIDLastSave="891" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8F7DA878-B662-4C02-B902-71F07586E99C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,7 +265,7 @@
     <t>Total Number of Lives Lost Among Personnel</t>
   </si>
   <si>
-    <t>Homeless</t>
+    <t>Experienced Homelessness</t>
   </si>
 </sst>
 </file>
@@ -694,21 +694,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU80"/>
+  <dimension ref="A1:AV80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AU1" sqref="AU1"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.5546875" customWidth="1"/>
     <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="40" max="47" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="48" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -844,8 +844,11 @@
       <c r="AU1" s="1">
         <v>43941</v>
       </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV1" s="1">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -869,7 +872,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -990,8 +993,11 @@
       <c r="AU3">
         <v>14939</v>
       </c>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV3">
+        <v>15502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1133,8 +1139,11 @@
       <c r="AU4">
         <v>3098</v>
       </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV4">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1258,8 +1267,11 @@
       <c r="AU5">
         <v>112</v>
       </c>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1353,11 +1365,14 @@
       <c r="AU6">
         <v>636</v>
       </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV6">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1445,8 +1460,11 @@
       <c r="AU8">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1534,8 +1552,11 @@
       <c r="AU9">
         <v>444</v>
       </c>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV9">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1623,8 +1644,11 @@
       <c r="AU10">
         <v>198</v>
       </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1712,13 +1736,16 @@
       <c r="AU11">
         <v>246</v>
       </c>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV11">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1726,7 +1753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1817,8 +1844,11 @@
       <c r="AU15">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1855,8 +1885,11 @@
       <c r="AU16">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1893,8 +1926,11 @@
       <c r="AU17">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1976,8 +2012,11 @@
       <c r="AU18">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV18">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2059,8 +2098,11 @@
       <c r="AU19">
         <v>131</v>
       </c>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV19">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2142,13 +2184,16 @@
       <c r="AU20">
         <v>561</v>
       </c>
-    </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV20">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -2239,8 +2284,11 @@
       <c r="AU23">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV23">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2277,8 +2325,11 @@
       <c r="AU24">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -2315,8 +2366,11 @@
       <c r="AU25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2398,8 +2452,11 @@
       <c r="AU26">
         <v>124</v>
       </c>
-    </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV26">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -2481,8 +2538,11 @@
       <c r="AU27">
         <v>186</v>
       </c>
-    </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV27">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -2564,13 +2624,16 @@
       <c r="AU28">
         <v>583</v>
       </c>
-    </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV28">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -2652,8 +2715,11 @@
       <c r="AU31">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV31">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -2687,8 +2753,11 @@
       <c r="AU32">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2722,8 +2791,11 @@
       <c r="AU33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
@@ -2805,8 +2877,11 @@
       <c r="AU34">
         <v>125</v>
       </c>
-    </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV34">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
@@ -2885,8 +2960,11 @@
       <c r="AU35">
         <v>144</v>
       </c>
-    </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
@@ -2968,8 +3046,11 @@
       <c r="AU36">
         <v>95</v>
       </c>
-    </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
@@ -2985,16 +3066,19 @@
       <c r="AU37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -3079,8 +3163,11 @@
       <c r="AU40">
         <v>96</v>
       </c>
-    </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV40">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -3117,8 +3204,11 @@
       <c r="AU41">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -3155,8 +3245,11 @@
       <c r="AU42">
         <v>52</v>
       </c>
-    </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV42">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>18</v>
       </c>
@@ -3238,8 +3331,11 @@
       <c r="AU43">
         <v>954</v>
       </c>
-    </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV43">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="44" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -3276,8 +3372,11 @@
       <c r="AU44">
         <v>998</v>
       </c>
-    </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV44">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="45" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -3311,8 +3410,11 @@
       <c r="AU45">
         <v>52</v>
       </c>
-    </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>18</v>
       </c>
@@ -3340,16 +3442,19 @@
       <c r="AU46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -3419,8 +3524,11 @@
       <c r="AU49">
         <v>18</v>
       </c>
-    </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV49">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>20</v>
       </c>
@@ -3454,8 +3562,11 @@
       <c r="AU50">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV50">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>20</v>
       </c>
@@ -3489,8 +3600,11 @@
       <c r="AU51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -3560,8 +3674,11 @@
       <c r="AU52">
         <v>60</v>
       </c>
-    </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV52">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>20</v>
       </c>
@@ -3631,8 +3748,11 @@
       <c r="AU53">
         <v>76</v>
       </c>
-    </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV53">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>20</v>
       </c>
@@ -3702,8 +3822,11 @@
       <c r="AU54">
         <v>57</v>
       </c>
-    </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV54">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>20</v>
       </c>
@@ -3731,8 +3854,11 @@
       <c r="AU55">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>22</v>
       </c>
@@ -3802,8 +3928,11 @@
       <c r="AU57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV57">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -3837,8 +3966,11 @@
       <c r="AU58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>22</v>
       </c>
@@ -3872,8 +4004,11 @@
       <c r="AU59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>22</v>
       </c>
@@ -3943,8 +4078,11 @@
       <c r="AU60">
         <v>36</v>
       </c>
-    </row>
-    <row r="61" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV60">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>22</v>
       </c>
@@ -4014,8 +4152,11 @@
       <c r="AU61">
         <v>44</v>
       </c>
-    </row>
-    <row r="62" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV61">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -4085,8 +4226,11 @@
       <c r="AU62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>22</v>
       </c>
@@ -4120,13 +4264,16 @@
       <c r="AU63">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>24</v>
       </c>
@@ -4196,8 +4343,11 @@
       <c r="AU66">
         <v>121</v>
       </c>
-    </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV66">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>24</v>
       </c>
@@ -4267,8 +4417,11 @@
       <c r="AU67">
         <v>243</v>
       </c>
-    </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV67">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>24</v>
       </c>
@@ -4338,8 +4491,11 @@
       <c r="AU68">
         <v>222</v>
       </c>
-    </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV68">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="69" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -4367,8 +4523,11 @@
       <c r="AU69">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>33</v>
       </c>
@@ -4438,8 +4597,11 @@
       <c r="AU71">
         <v>59</v>
       </c>
-    </row>
-    <row r="72" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV71">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>33</v>
       </c>
@@ -4509,8 +4671,11 @@
       <c r="AU72">
         <v>30</v>
       </c>
-    </row>
-    <row r="73" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV72">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>33</v>
       </c>
@@ -4580,8 +4745,11 @@
       <c r="AU73">
         <v>89</v>
       </c>
-    </row>
-    <row r="74" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV73">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>33</v>
       </c>
@@ -4651,8 +4819,11 @@
       <c r="AU74">
         <v>22</v>
       </c>
-    </row>
-    <row r="76" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV74">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>34</v>
       </c>
@@ -4722,8 +4893,11 @@
       <c r="AU76">
         <v>41</v>
       </c>
-    </row>
-    <row r="77" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV76">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>34</v>
       </c>
@@ -4793,8 +4967,11 @@
       <c r="AU77">
         <v>33</v>
       </c>
-    </row>
-    <row r="78" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV77">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>34</v>
       </c>
@@ -4852,8 +5029,11 @@
       <c r="AU78">
         <v>33</v>
       </c>
-    </row>
-    <row r="79" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV78">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
@@ -4923,8 +5103,11 @@
       <c r="AU79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
@@ -4951,6 +5134,9 @@
       </c>
       <c r="AU80">
         <v>5</v>
+      </c>
+      <c r="AV80">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -4961,10 +5147,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:V11"/>
+  <dimension ref="A2:W11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4974,7 +5160,7 @@
     <col min="15" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -5041,8 +5227,11 @@
       <c r="V2" s="9">
         <v>43941</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W2" s="9">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -5109,8 +5298,11 @@
       <c r="V3">
         <v>355</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -5177,8 +5369,11 @@
       <c r="V4">
         <v>228</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W4">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -5245,8 +5440,11 @@
       <c r="V5">
         <v>223</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W5">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -5313,8 +5511,11 @@
       <c r="V6">
         <v>515</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W6">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -5381,8 +5582,11 @@
       <c r="V7">
         <v>404</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W7">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -5449,8 +5653,11 @@
       <c r="V8">
         <v>374</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W8">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -5517,8 +5724,11 @@
       <c r="V9">
         <v>482</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W9">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -5585,8 +5795,11 @@
       <c r="V10">
         <v>445</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W10">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
@@ -5652,6 +5865,9 @@
       </c>
       <c r="V11">
         <v>72</v>
+      </c>
+      <c r="W11">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -5662,10 +5878,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:Q17"/>
+  <dimension ref="A2:R17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5675,7 +5891,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -5725,8 +5941,11 @@
       <c r="Q2" s="9">
         <v>43941</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R2" s="9">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>41</v>
       </c>
@@ -5734,7 +5953,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
@@ -5786,8 +6005,11 @@
       <c r="Q4">
         <v>3098</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -5839,8 +6061,11 @@
       <c r="Q5">
         <v>470</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -5892,8 +6117,11 @@
       <c r="Q6">
         <v>565</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -5945,8 +6173,11 @@
       <c r="Q7">
         <v>1517</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
@@ -5998,8 +6229,11 @@
       <c r="Q8">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>45</v>
       </c>
@@ -6051,8 +6285,11 @@
       <c r="Q9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>55</v>
       </c>
@@ -6100,8 +6337,11 @@
       <c r="Q10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -6153,8 +6393,11 @@
       <c r="Q11">
         <v>450</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
@@ -6206,8 +6449,11 @@
       <c r="Q12">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -6218,7 +6464,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
@@ -6270,8 +6516,11 @@
       <c r="Q14">
         <v>615</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
@@ -6323,8 +6572,11 @@
       <c r="Q15">
         <v>555</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
@@ -6376,8 +6628,11 @@
       <c r="Q16">
         <v>1914</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R16">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>47</v>
       </c>
@@ -6427,6 +6682,9 @@
         <v>16</v>
       </c>
       <c r="Q17">
+        <v>14</v>
+      </c>
+      <c r="R17">
         <v>14</v>
       </c>
     </row>
@@ -6438,10 +6696,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6450,7 +6708,7 @@
     <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -6499,14 +6757,17 @@
       <c r="Q1" s="9">
         <v>43941</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="9">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>54</v>
       </c>
@@ -6559,8 +6820,11 @@
       <c r="Q3">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
@@ -6612,8 +6876,11 @@
       <c r="Q4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -6665,8 +6932,11 @@
       <c r="Q5">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>51</v>
       </c>
@@ -6718,8 +6988,11 @@
       <c r="Q6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -6771,8 +7044,11 @@
       <c r="Q7">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
@@ -6822,6 +7098,9 @@
         <v>0</v>
       </c>
       <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
         <v>0</v>
       </c>
     </row>
@@ -6832,10 +7111,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DE713F-971D-4CE1-B1A8-BE60A2507C58}">
-  <dimension ref="A2:C13"/>
+  <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6843,7 +7122,7 @@
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -6853,8 +7132,11 @@
       <c r="C2" s="9">
         <v>43941</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="9">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>54</v>
       </c>
@@ -6864,8 +7146,11 @@
       <c r="C3">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -6875,8 +7160,11 @@
       <c r="C4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -6886,8 +7174,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -6897,8 +7188,11 @@
       <c r="C6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -6908,8 +7202,11 @@
       <c r="C7">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -6919,8 +7216,11 @@
       <c r="C8">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -6930,8 +7230,11 @@
       <c r="C9">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -6941,8 +7244,11 @@
       <c r="C10">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -6952,8 +7258,11 @@
       <c r="C11">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>76</v>
       </c>
@@ -6963,8 +7272,11 @@
       <c r="C12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>39</v>
       </c>
@@ -6972,6 +7284,9 @@
         <v>0</v>
       </c>
       <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>0</v>
       </c>
     </row>
@@ -6981,12 +7296,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -7189,6 +7498,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7199,23 +7514,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7234,6 +7532,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
23 April data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="891" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8F7DA878-B662-4C02-B902-71F07586E99C}"/>
+  <xr:revisionPtr revIDLastSave="1000" documentId="8_{C884A327-19F6-4EC6-805C-F52B66916DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5423C21D-8DD5-42AF-ADAE-F3E8306C78DA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,21 +694,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV80"/>
+  <dimension ref="A1:AW80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <pane xSplit="2" topLeftCell="AR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AX13" sqref="AX13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.5546875" customWidth="1"/>
     <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="40" max="48" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="49" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -847,8 +847,11 @@
       <c r="AV1" s="1">
         <v>43942</v>
       </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW1" s="1">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -872,7 +875,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -996,8 +999,11 @@
       <c r="AV3">
         <v>15502</v>
       </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW3">
+        <v>15930</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1142,8 +1148,11 @@
       <c r="AV4">
         <v>3206</v>
       </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW4">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1270,8 +1279,11 @@
       <c r="AV5">
         <v>127</v>
       </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW5">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1368,11 +1380,14 @@
       <c r="AV6">
         <v>645</v>
       </c>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW6">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1463,8 +1478,11 @@
       <c r="AV8">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1555,8 +1573,11 @@
       <c r="AV9">
         <v>444</v>
       </c>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW9">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1647,8 +1668,11 @@
       <c r="AV10">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1739,13 +1763,16 @@
       <c r="AV11">
         <v>244</v>
       </c>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW11">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1753,7 +1780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1847,8 +1874,11 @@
       <c r="AV15">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1888,8 +1918,11 @@
       <c r="AV16">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW16">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1929,8 +1962,11 @@
       <c r="AV17">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2015,8 +2051,11 @@
       <c r="AV18">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW18">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2101,8 +2140,11 @@
       <c r="AV19">
         <v>143</v>
       </c>
-    </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW19">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2187,13 +2229,16 @@
       <c r="AV20">
         <v>589</v>
       </c>
-    </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW20">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -2287,8 +2332,11 @@
       <c r="AV23">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW23">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -2328,8 +2376,11 @@
       <c r="AV24">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW24">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -2364,13 +2415,16 @@
         <v>21</v>
       </c>
       <c r="AU25">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="AV25">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2455,8 +2509,11 @@
       <c r="AV26">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW26">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -2541,8 +2598,11 @@
       <c r="AV27">
         <v>170</v>
       </c>
-    </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW27">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -2627,13 +2687,16 @@
       <c r="AV28">
         <v>640</v>
       </c>
-    </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW28">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -2718,8 +2781,11 @@
       <c r="AV31">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -2756,8 +2822,11 @@
       <c r="AV32">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW32">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2794,8 +2863,11 @@
       <c r="AV33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
@@ -2880,8 +2952,11 @@
       <c r="AV34">
         <v>126</v>
       </c>
-    </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW34">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
@@ -2963,8 +3038,11 @@
       <c r="AV35">
         <v>145</v>
       </c>
-    </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
@@ -3049,8 +3127,11 @@
       <c r="AV36">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW36">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
@@ -3069,16 +3150,19 @@
       <c r="AV37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -3166,8 +3250,11 @@
       <c r="AV40">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW40">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -3207,8 +3294,11 @@
       <c r="AV41">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW41">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -3248,8 +3338,11 @@
       <c r="AV42">
         <v>52</v>
       </c>
-    </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW42">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>18</v>
       </c>
@@ -3334,8 +3427,11 @@
       <c r="AV43">
         <v>1014</v>
       </c>
-    </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW43">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="44" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -3375,8 +3471,11 @@
       <c r="AV44">
         <v>1059</v>
       </c>
-    </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW44">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="45" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -3413,8 +3512,11 @@
       <c r="AV45">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>18</v>
       </c>
@@ -3445,16 +3547,19 @@
       <c r="AV46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -3527,8 +3632,11 @@
       <c r="AV49">
         <v>19</v>
       </c>
-    </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>20</v>
       </c>
@@ -3563,10 +3671,13 @@
         <v>16</v>
       </c>
       <c r="AV50">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="AW50">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>20</v>
       </c>
@@ -3603,8 +3714,11 @@
       <c r="AV51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -3677,8 +3791,11 @@
       <c r="AV52">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW52">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>20</v>
       </c>
@@ -3751,8 +3868,11 @@
       <c r="AV53">
         <v>66</v>
       </c>
-    </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW53">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>20</v>
       </c>
@@ -3825,8 +3945,11 @@
       <c r="AV54">
         <v>68</v>
       </c>
-    </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW54">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>20</v>
       </c>
@@ -3857,8 +3980,11 @@
       <c r="AV55">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>22</v>
       </c>
@@ -3931,8 +4057,11 @@
       <c r="AV57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW57">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -3969,8 +4098,11 @@
       <c r="AV58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>22</v>
       </c>
@@ -4007,8 +4139,11 @@
       <c r="AV59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>22</v>
       </c>
@@ -4081,8 +4216,11 @@
       <c r="AV60">
         <v>38</v>
       </c>
-    </row>
-    <row r="61" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW60">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>22</v>
       </c>
@@ -4155,8 +4293,11 @@
       <c r="AV61">
         <v>46</v>
       </c>
-    </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW61">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -4229,8 +4370,11 @@
       <c r="AV62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>22</v>
       </c>
@@ -4267,13 +4411,16 @@
       <c r="AV63">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>24</v>
       </c>
@@ -4346,8 +4493,11 @@
       <c r="AV66">
         <v>131</v>
       </c>
-    </row>
-    <row r="67" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW66">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>24</v>
       </c>
@@ -4420,8 +4570,11 @@
       <c r="AV67">
         <v>253</v>
       </c>
-    </row>
-    <row r="68" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW67">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="68" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>24</v>
       </c>
@@ -4494,8 +4647,11 @@
       <c r="AV68">
         <v>236</v>
       </c>
-    </row>
-    <row r="69" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW68">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -4526,8 +4682,11 @@
       <c r="AV69">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>33</v>
       </c>
@@ -4600,8 +4759,11 @@
       <c r="AV71">
         <v>66</v>
       </c>
-    </row>
-    <row r="72" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW71">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>33</v>
       </c>
@@ -4674,8 +4836,11 @@
       <c r="AV72">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW72">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>33</v>
       </c>
@@ -4748,8 +4913,11 @@
       <c r="AV73">
         <v>85</v>
       </c>
-    </row>
-    <row r="74" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW73">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>33</v>
       </c>
@@ -4822,8 +4990,11 @@
       <c r="AV74">
         <v>77</v>
       </c>
-    </row>
-    <row r="76" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW74">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>34</v>
       </c>
@@ -4896,8 +5067,11 @@
       <c r="AV76">
         <v>41</v>
       </c>
-    </row>
-    <row r="77" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW76">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>34</v>
       </c>
@@ -4970,8 +5144,11 @@
       <c r="AV77">
         <v>29</v>
       </c>
-    </row>
-    <row r="78" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW77">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>34</v>
       </c>
@@ -5032,8 +5209,11 @@
       <c r="AV78">
         <v>29</v>
       </c>
-    </row>
-    <row r="79" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW78">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
@@ -5106,8 +5286,11 @@
       <c r="AV79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
@@ -5136,6 +5319,9 @@
         <v>5</v>
       </c>
       <c r="AV80">
+        <v>6</v>
+      </c>
+      <c r="AW80">
         <v>6</v>
       </c>
     </row>
@@ -5147,10 +5333,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:W11"/>
+  <dimension ref="A2:X11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5160,7 +5346,7 @@
     <col min="15" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -5230,8 +5416,11 @@
       <c r="W2" s="9">
         <v>43942</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X2" s="9">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -5301,8 +5490,11 @@
       <c r="W3">
         <v>359</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -5372,8 +5564,11 @@
       <c r="W4">
         <v>234</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -5443,8 +5638,11 @@
       <c r="W5">
         <v>215</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X5">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -5514,8 +5712,11 @@
       <c r="W6">
         <v>543</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X6">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -5585,8 +5786,11 @@
       <c r="W7">
         <v>429</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X7">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -5656,8 +5860,11 @@
       <c r="W8">
         <v>387</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X8">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -5727,8 +5934,11 @@
       <c r="W9">
         <v>492</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X9">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -5798,8 +6008,11 @@
       <c r="W10">
         <v>458</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X10">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
@@ -5868,6 +6081,9 @@
       </c>
       <c r="W11">
         <v>89</v>
+      </c>
+      <c r="X11">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -5878,10 +6094,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:R17"/>
+  <dimension ref="A2:S17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5891,7 +6107,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -5944,8 +6160,11 @@
       <c r="R2" s="9">
         <v>43942</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="9">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>41</v>
       </c>
@@ -5953,7 +6172,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
@@ -6008,8 +6227,11 @@
       <c r="R4">
         <v>3206</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -6064,8 +6286,11 @@
       <c r="R5">
         <v>443</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -6120,8 +6345,11 @@
       <c r="R6">
         <v>587</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -6176,8 +6404,11 @@
       <c r="R7">
         <v>1595</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
@@ -6232,8 +6463,11 @@
       <c r="R8">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>45</v>
       </c>
@@ -6288,8 +6522,11 @@
       <c r="R9">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>55</v>
       </c>
@@ -6340,8 +6577,11 @@
       <c r="R10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
@@ -6396,8 +6636,11 @@
       <c r="R11">
         <v>481</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
@@ -6452,8 +6695,11 @@
       <c r="R12">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -6464,7 +6710,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
@@ -6519,8 +6765,11 @@
       <c r="R14">
         <v>601</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
@@ -6575,8 +6824,11 @@
       <c r="R15">
         <v>589</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
@@ -6631,8 +6883,11 @@
       <c r="R16">
         <v>2002</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>47</v>
       </c>
@@ -6685,6 +6940,9 @@
         <v>14</v>
       </c>
       <c r="R17">
+        <v>14</v>
+      </c>
+      <c r="S17">
         <v>14</v>
       </c>
     </row>
@@ -6696,10 +6954,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6708,7 +6966,7 @@
     <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -6760,14 +7018,17 @@
       <c r="R1" s="9">
         <v>43942</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" s="9">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>54</v>
       </c>
@@ -6823,8 +7084,11 @@
       <c r="R3">
         <v>127</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
@@ -6879,8 +7143,11 @@
       <c r="R4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -6935,8 +7202,11 @@
       <c r="R5">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>51</v>
       </c>
@@ -6991,8 +7261,11 @@
       <c r="R6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -7047,8 +7320,11 @@
       <c r="R7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
@@ -7101,6 +7377,9 @@
         <v>0</v>
       </c>
       <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
         <v>0</v>
       </c>
     </row>
@@ -7111,10 +7390,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DE713F-971D-4CE1-B1A8-BE60A2507C58}">
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7122,7 +7401,7 @@
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -7135,8 +7414,11 @@
       <c r="D2" s="9">
         <v>43942</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="9">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>54</v>
       </c>
@@ -7149,8 +7431,11 @@
       <c r="D3">
         <v>127</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -7163,8 +7448,11 @@
       <c r="D4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -7177,8 +7465,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -7191,8 +7482,11 @@
       <c r="D6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -7205,8 +7499,11 @@
       <c r="D7">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -7219,8 +7516,11 @@
       <c r="D8">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -7233,8 +7533,11 @@
       <c r="D9">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -7247,8 +7550,11 @@
       <c r="D10">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -7261,8 +7567,11 @@
       <c r="D11">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>76</v>
       </c>
@@ -7275,8 +7584,11 @@
       <c r="D12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>39</v>
       </c>
@@ -7287,6 +7599,9 @@
         <v>0</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>0</v>
       </c>
     </row>
@@ -7296,6 +7611,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -7498,12 +7819,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7514,6 +7829,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7532,23 +7864,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
13 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1240" documentId="8_{374341DD-C3B3-4BF1-BB9D-EFA90D251024}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D60B2329-C4D7-4EC1-B4DF-762F3DD0F666}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="20730" windowHeight="6945"/>
+    <workbookView xWindow="-24" yWindow="0" windowWidth="23040" windowHeight="6948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="Lives Lost by Race" sheetId="4" r:id="rId4"/>
     <sheet name="Lives Lost by Ward" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="87">
   <si>
     <t>Testing</t>
   </si>
@@ -288,11 +294,14 @@
   <si>
     <t>Percentage of pre-COVID Hospital Bed Capacity</t>
   </si>
+  <si>
+    <t>Number of Lives Lost Among Personnel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -708,30 +717,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BQ104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" topLeftCell="BI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="BQ1" sqref="BQ1:BQ1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="69" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -930,8 +939,11 @@
       <c r="BP1" s="1">
         <v>43962</v>
       </c>
+      <c r="BQ1" s="1">
+        <v>43963</v>
+      </c>
     </row>
-    <row r="2" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -955,7 +967,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1137,10 +1149,13 @@
         <v>30261</v>
       </c>
       <c r="BP3">
-        <v>31050</v>
+        <v>30050</v>
+      </c>
+      <c r="BQ3">
+        <v>31658</v>
       </c>
     </row>
-    <row r="4" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1345,8 +1360,11 @@
       <c r="BP4">
         <v>6485</v>
       </c>
+      <c r="BQ4">
+        <v>6584</v>
+      </c>
     </row>
-    <row r="5" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1533,8 +1551,11 @@
       <c r="BP5">
         <v>336</v>
       </c>
+      <c r="BQ5">
+        <v>350</v>
+      </c>
     </row>
-    <row r="6" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1691,11 +1712,14 @@
       <c r="BP6">
         <v>886</v>
       </c>
+      <c r="BQ6">
+        <v>934</v>
+      </c>
     </row>
-    <row r="7" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1744,8 +1768,11 @@
       <c r="BP8">
         <v>345</v>
       </c>
+      <c r="BQ8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1896,8 +1923,11 @@
       <c r="BP9">
         <v>88</v>
       </c>
+      <c r="BQ9">
+        <v>73</v>
+      </c>
     </row>
-    <row r="10" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2048,8 +2078,11 @@
       <c r="BP10">
         <v>440</v>
       </c>
+      <c r="BQ10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2200,8 +2233,11 @@
       <c r="BP11">
         <v>243</v>
       </c>
+      <c r="BQ11">
+        <v>250</v>
+      </c>
     </row>
-    <row r="12" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -2352,8 +2388,11 @@
       <c r="BP12">
         <v>197</v>
       </c>
+      <c r="BQ12">
+        <v>190</v>
+      </c>
     </row>
-    <row r="13" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -2366,8 +2405,11 @@
       <c r="BP13">
         <v>435</v>
       </c>
+      <c r="BQ13">
+        <v>423</v>
+      </c>
     </row>
-    <row r="14" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2380,8 +2422,11 @@
       <c r="BP14">
         <v>1805</v>
       </c>
+      <c r="BQ14">
+        <v>1887</v>
+      </c>
     </row>
-    <row r="15" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2394,13 +2439,16 @@
       <c r="BP15" s="23">
         <v>0.73</v>
       </c>
+      <c r="BQ15" s="23">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="17" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2408,7 +2456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2562,8 +2610,11 @@
       <c r="BP19">
         <v>104</v>
       </c>
+      <c r="BQ19">
+        <v>104</v>
+      </c>
     </row>
-    <row r="20" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2663,8 +2714,11 @@
       <c r="BP20">
         <v>37</v>
       </c>
+      <c r="BQ20">
+        <v>35</v>
+      </c>
     </row>
-    <row r="21" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2764,8 +2818,11 @@
       <c r="BP21">
         <v>67</v>
       </c>
+      <c r="BQ21">
+        <v>69</v>
+      </c>
     </row>
-    <row r="22" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -2910,8 +2967,11 @@
       <c r="BP22">
         <v>172</v>
       </c>
+      <c r="BQ22">
+        <v>115</v>
+      </c>
     </row>
-    <row r="23" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3056,8 +3116,11 @@
       <c r="BP23">
         <v>209</v>
       </c>
+      <c r="BQ23">
+        <v>150</v>
+      </c>
     </row>
-    <row r="24" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3202,13 +3265,16 @@
       <c r="BP24">
         <v>1031</v>
       </c>
+      <c r="BQ24">
+        <v>1065</v>
+      </c>
     </row>
-    <row r="26" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3362,8 +3428,11 @@
       <c r="BP27">
         <v>113</v>
       </c>
+      <c r="BQ27">
+        <v>113</v>
+      </c>
     </row>
-    <row r="28" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -3463,8 +3532,11 @@
       <c r="BP28">
         <v>39</v>
       </c>
+      <c r="BQ28">
+        <v>38</v>
+      </c>
     </row>
-    <row r="29" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -3564,8 +3636,11 @@
       <c r="BP29">
         <v>74</v>
       </c>
+      <c r="BQ29">
+        <v>75</v>
+      </c>
     </row>
-    <row r="30" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -3710,8 +3785,11 @@
       <c r="BP30">
         <v>65</v>
       </c>
+      <c r="BQ30">
+        <v>51</v>
+      </c>
     </row>
-    <row r="31" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3856,8 +3934,11 @@
       <c r="BP31">
         <v>104</v>
       </c>
+      <c r="BQ31">
+        <v>89</v>
+      </c>
     </row>
-    <row r="32" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4002,13 +4083,16 @@
       <c r="BP32">
         <v>968</v>
       </c>
+      <c r="BQ32">
+        <v>1007</v>
+      </c>
     </row>
-    <row r="34" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -4150,8 +4234,11 @@
       <c r="BP35">
         <v>75</v>
       </c>
+      <c r="BQ35">
+        <v>75</v>
+      </c>
     </row>
-    <row r="36" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -4245,8 +4332,11 @@
       <c r="BP36">
         <v>35</v>
       </c>
+      <c r="BQ36">
+        <v>30</v>
+      </c>
     </row>
-    <row r="37" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -4340,8 +4430,11 @@
       <c r="BP37">
         <v>39</v>
       </c>
+      <c r="BQ37">
+        <v>44</v>
+      </c>
     </row>
-    <row r="38" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -4480,8 +4573,11 @@
       <c r="BP38">
         <v>13</v>
       </c>
+      <c r="BQ38">
+        <v>12</v>
+      </c>
     </row>
-    <row r="39" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -4617,8 +4713,11 @@
       <c r="BP39">
         <v>48</v>
       </c>
+      <c r="BQ39">
+        <v>42</v>
+      </c>
     </row>
-    <row r="40" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -4760,8 +4859,11 @@
       <c r="BP40">
         <v>230</v>
       </c>
+      <c r="BQ40">
+        <v>240</v>
+      </c>
     </row>
-    <row r="41" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -4837,16 +4939,19 @@
       <c r="BP41">
         <v>1</v>
       </c>
+      <c r="BQ41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -4994,8 +5099,11 @@
       <c r="BP44">
         <v>179</v>
       </c>
+      <c r="BQ44">
+        <v>179</v>
+      </c>
     </row>
-    <row r="45" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -5095,8 +5203,11 @@
       <c r="BP45">
         <v>44</v>
       </c>
+      <c r="BQ45">
+        <v>40</v>
+      </c>
     </row>
-    <row r="46" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -5196,8 +5307,11 @@
       <c r="BP46">
         <v>130</v>
       </c>
+      <c r="BQ46">
+        <v>134</v>
+      </c>
     </row>
-    <row r="47" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -5342,8 +5456,11 @@
       <c r="BP47">
         <v>833</v>
       </c>
+      <c r="BQ47">
+        <v>828</v>
+      </c>
     </row>
-    <row r="48" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -5443,8 +5560,11 @@
       <c r="BP48">
         <v>877</v>
       </c>
+      <c r="BQ48">
+        <v>868</v>
+      </c>
     </row>
-    <row r="49" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -5541,8 +5661,11 @@
       <c r="BP49">
         <v>471</v>
       </c>
+      <c r="BQ49">
+        <v>481</v>
+      </c>
     </row>
-    <row r="50" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -5633,16 +5756,19 @@
       <c r="BP50">
         <v>1</v>
       </c>
+      <c r="BQ50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
@@ -5775,8 +5901,11 @@
       <c r="BP53">
         <v>27</v>
       </c>
+      <c r="BQ53">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -5873,8 +6002,11 @@
       <c r="BP54">
         <v>16</v>
       </c>
+      <c r="BQ54">
+        <v>14</v>
+      </c>
     </row>
-    <row r="55" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -5971,8 +6103,11 @@
       <c r="BP55">
         <v>10</v>
       </c>
+      <c r="BQ55">
+        <v>12</v>
+      </c>
     </row>
-    <row r="56" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -6105,8 +6240,11 @@
       <c r="BP56">
         <v>22</v>
       </c>
+      <c r="BQ56">
+        <v>19</v>
+      </c>
     </row>
-    <row r="57" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -6239,8 +6377,11 @@
       <c r="BP57">
         <v>38</v>
       </c>
+      <c r="BQ57">
+        <v>33</v>
+      </c>
     </row>
-    <row r="58" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -6373,8 +6514,11 @@
       <c r="BP58">
         <v>116</v>
       </c>
+      <c r="BQ58">
+        <v>121</v>
+      </c>
     </row>
-    <row r="59" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -6465,8 +6609,11 @@
       <c r="BP59">
         <v>1</v>
       </c>
+      <c r="BQ59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>20</v>
       </c>
@@ -6599,8 +6746,11 @@
       <c r="BP61">
         <v>10</v>
       </c>
+      <c r="BQ61">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -6697,8 +6847,11 @@
       <c r="BP62">
         <v>4</v>
       </c>
+      <c r="BQ62">
+        <v>4</v>
+      </c>
     </row>
-    <row r="63" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -6795,8 +6948,11 @@
       <c r="BP63">
         <v>6</v>
       </c>
+      <c r="BQ63">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -6929,8 +7085,11 @@
       <c r="BP64">
         <v>44</v>
       </c>
+      <c r="BQ64">
+        <v>44</v>
+      </c>
     </row>
-    <row r="65" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -7063,8 +7222,11 @@
       <c r="BP65">
         <v>48</v>
       </c>
+      <c r="BQ65">
+        <v>48</v>
+      </c>
     </row>
-    <row r="66" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -7197,8 +7359,11 @@
       <c r="BP66">
         <v>0</v>
       </c>
+      <c r="BQ66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -7295,13 +7460,16 @@
       <c r="BP67">
         <v>0</v>
       </c>
+      <c r="BQ67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>22</v>
       </c>
@@ -7434,8 +7602,11 @@
       <c r="BP70">
         <v>267</v>
       </c>
+      <c r="BQ70">
+        <v>267</v>
+      </c>
     </row>
-    <row r="71" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
@@ -7568,8 +7739,11 @@
       <c r="BP71">
         <v>349</v>
       </c>
+      <c r="BQ71">
+        <v>323</v>
+      </c>
     </row>
-    <row r="72" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>22</v>
       </c>
@@ -7702,8 +7876,11 @@
       <c r="BP72">
         <v>342</v>
       </c>
+      <c r="BQ72">
+        <v>319</v>
+      </c>
     </row>
-    <row r="73" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
@@ -7794,8 +7971,11 @@
       <c r="BP73">
         <v>15</v>
       </c>
+      <c r="BQ73">
+        <v>15</v>
+      </c>
     </row>
-    <row r="75" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -7928,8 +8108,11 @@
       <c r="BP75">
         <v>81</v>
       </c>
+      <c r="BQ75">
+        <v>84</v>
+      </c>
     </row>
-    <row r="76" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -8062,8 +8245,11 @@
       <c r="BP76">
         <v>27</v>
       </c>
+      <c r="BQ76">
+        <v>19</v>
+      </c>
     </row>
-    <row r="77" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -8196,8 +8382,11 @@
       <c r="BP77">
         <v>109</v>
       </c>
+      <c r="BQ77">
+        <v>103</v>
+      </c>
     </row>
-    <row r="78" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -8330,284 +8519,167 @@
       <c r="BP78">
         <v>152</v>
       </c>
+      <c r="BQ78">
+        <v>157</v>
+      </c>
     </row>
-    <row r="80" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B80" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA80">
-        <v>1</v>
-      </c>
-      <c r="AB80">
-        <v>1</v>
-      </c>
-      <c r="AC80">
-        <v>3</v>
-      </c>
-      <c r="AD80">
-        <v>5</v>
-      </c>
-      <c r="AE80">
-        <v>6</v>
-      </c>
-      <c r="AF80">
-        <v>7</v>
-      </c>
-      <c r="AG80">
-        <v>9</v>
-      </c>
-      <c r="AH80">
-        <v>11</v>
-      </c>
-      <c r="AI80">
-        <v>14</v>
-      </c>
-      <c r="AJ80">
-        <v>15</v>
-      </c>
-      <c r="AK80">
-        <v>17</v>
-      </c>
-      <c r="AL80">
-        <v>21</v>
-      </c>
-      <c r="AM80">
-        <v>21</v>
-      </c>
-      <c r="AN80">
-        <v>28</v>
-      </c>
-      <c r="AO80">
-        <v>28</v>
-      </c>
-      <c r="AP80">
-        <v>32</v>
-      </c>
-      <c r="AQ80">
-        <v>33</v>
-      </c>
-      <c r="AR80">
-        <v>36</v>
-      </c>
-      <c r="AS80">
-        <v>36</v>
-      </c>
-      <c r="AT80">
-        <v>37</v>
-      </c>
-      <c r="AU80">
-        <v>41</v>
-      </c>
-      <c r="AV80">
-        <v>41</v>
-      </c>
-      <c r="AW80">
-        <v>42</v>
-      </c>
-      <c r="AX80">
-        <v>41</v>
-      </c>
-      <c r="AY80">
-        <v>46</v>
-      </c>
-      <c r="AZ80">
-        <v>46</v>
-      </c>
-      <c r="BA80">
-        <v>48</v>
-      </c>
-      <c r="BB80">
-        <v>48</v>
-      </c>
-      <c r="BC80">
-        <v>55</v>
-      </c>
-      <c r="BD80">
-        <v>66</v>
-      </c>
-      <c r="BE80">
-        <v>66</v>
-      </c>
-      <c r="BF80">
-        <v>68</v>
-      </c>
-      <c r="BG80">
-        <v>68</v>
-      </c>
-      <c r="BH80">
-        <v>68</v>
-      </c>
-      <c r="BI80">
-        <v>70</v>
-      </c>
-      <c r="BJ80">
-        <v>72</v>
-      </c>
-      <c r="BK80">
-        <v>72</v>
-      </c>
-      <c r="BL80">
-        <v>77</v>
-      </c>
-      <c r="BM80">
-        <v>78</v>
-      </c>
-      <c r="BN80">
-        <v>78</v>
-      </c>
-      <c r="BO80">
-        <v>78</v>
-      </c>
-      <c r="BP80">
-        <v>79</v>
+    <row r="79" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" t="s">
+        <v>86</v>
+      </c>
+      <c r="BQ79">
+        <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B81" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA81">
+        <v>1</v>
+      </c>
+      <c r="AB81">
+        <v>1</v>
+      </c>
+      <c r="AC81">
+        <v>3</v>
+      </c>
+      <c r="AD81">
+        <v>5</v>
+      </c>
+      <c r="AE81">
+        <v>6</v>
+      </c>
+      <c r="AF81">
+        <v>7</v>
+      </c>
+      <c r="AG81">
+        <v>9</v>
+      </c>
+      <c r="AH81">
+        <v>11</v>
+      </c>
+      <c r="AI81">
+        <v>14</v>
+      </c>
+      <c r="AJ81">
+        <v>15</v>
+      </c>
+      <c r="AK81">
+        <v>17</v>
+      </c>
+      <c r="AL81">
+        <v>21</v>
+      </c>
+      <c r="AM81">
+        <v>21</v>
+      </c>
+      <c r="AN81">
+        <v>28</v>
+      </c>
+      <c r="AO81">
+        <v>28</v>
+      </c>
+      <c r="AP81">
+        <v>32</v>
+      </c>
+      <c r="AQ81">
         <v>33</v>
       </c>
-      <c r="AA81">
-        <v>17</v>
-      </c>
-      <c r="AB81">
-        <v>18</v>
-      </c>
-      <c r="AC81">
-        <v>81</v>
-      </c>
-      <c r="AD81">
-        <v>124</v>
-      </c>
-      <c r="AE81">
-        <v>95</v>
-      </c>
-      <c r="AF81">
-        <v>95</v>
-      </c>
-      <c r="AG81">
-        <v>119</v>
-      </c>
-      <c r="AH81">
-        <v>142</v>
-      </c>
-      <c r="AI81">
-        <v>142</v>
-      </c>
-      <c r="AJ81">
-        <v>142</v>
-      </c>
-      <c r="AK81">
-        <v>144</v>
-      </c>
-      <c r="AL81">
-        <v>123</v>
-      </c>
-      <c r="AM81">
-        <v>144</v>
-      </c>
-      <c r="AN81">
-        <v>105</v>
-      </c>
-      <c r="AO81">
-        <v>105</v>
-      </c>
-      <c r="AP81">
-        <v>105</v>
-      </c>
-      <c r="AQ81">
-        <v>74</v>
-      </c>
       <c r="AR81">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="AS81">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="AT81">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AU81">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="AV81">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="AW81">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="AX81">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="AY81">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="AZ81">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="BA81">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="BB81">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="BC81">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="BD81">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="BE81">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="BF81">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="BG81">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="BH81">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="BI81">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BJ81">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="BK81">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="BL81">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="BM81">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="BN81">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="BO81">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="BP81">
-        <v>56</v>
+        <v>79</v>
+      </c>
+      <c r="BQ81">
+        <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B82" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA82">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AB82">
         <v>18</v>
@@ -8627,8 +8699,20 @@
       <c r="AG82">
         <v>119</v>
       </c>
+      <c r="AH82">
+        <v>142</v>
+      </c>
+      <c r="AI82">
+        <v>142</v>
+      </c>
+      <c r="AJ82">
+        <v>142</v>
+      </c>
+      <c r="AK82">
+        <v>144</v>
+      </c>
       <c r="AL82">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="AM82">
         <v>144</v>
@@ -8670,444 +8754,587 @@
         <v>29</v>
       </c>
       <c r="AZ82">
-        <v>34</v>
-      </c>
-      <c r="BA82" t="s">
-        <v>77</v>
-      </c>
-      <c r="BB82" t="s">
-        <v>77</v>
+        <v>29</v>
+      </c>
+      <c r="BA82">
+        <v>29</v>
+      </c>
+      <c r="BB82">
+        <v>29</v>
       </c>
       <c r="BC82">
-        <v>17</v>
-      </c>
-      <c r="BD82" t="s">
-        <v>77</v>
+        <v>43</v>
+      </c>
+      <c r="BD82">
+        <v>50</v>
       </c>
       <c r="BE82">
-        <v>127</v>
-      </c>
-      <c r="BF82" t="s">
-        <v>77</v>
-      </c>
-      <c r="BG82" t="s">
-        <v>77</v>
-      </c>
-      <c r="BH82" t="s">
-        <v>77</v>
-      </c>
-      <c r="BI82" t="s">
-        <v>77</v>
+        <v>50</v>
+      </c>
+      <c r="BF82">
+        <v>50</v>
+      </c>
+      <c r="BG82">
+        <v>50</v>
+      </c>
+      <c r="BH82">
+        <v>50</v>
+      </c>
+      <c r="BI82">
+        <v>50</v>
       </c>
       <c r="BJ82">
-        <v>152</v>
+        <v>51</v>
       </c>
       <c r="BK82">
-        <v>152</v>
+        <v>51</v>
       </c>
       <c r="BL82">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="BM82">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="BN82">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="BO82">
-        <v>147</v>
+        <v>55</v>
       </c>
       <c r="BP82">
-        <v>142</v>
+        <v>56</v>
+      </c>
+      <c r="BQ82">
+        <v>56</v>
       </c>
     </row>
-    <row r="83" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="AA83">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AB83">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="AC83">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="AD83">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="AE83">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="AF83">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="AG83">
-        <v>1</v>
-      </c>
-      <c r="AH83">
-        <v>1</v>
-      </c>
-      <c r="AI83">
-        <v>1</v>
-      </c>
-      <c r="AJ83">
-        <v>1</v>
-      </c>
-      <c r="AK83">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="AL83">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="AM83">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="AN83">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="AO83">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="AP83">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="AQ83">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="AR83">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="AS83">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="AT83">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="AU83">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="AV83">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="AW83">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="AX83">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="AY83">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="AZ83">
-        <v>2</v>
-      </c>
-      <c r="BA83">
-        <v>2</v>
-      </c>
-      <c r="BB83">
-        <v>2</v>
+        <v>34</v>
+      </c>
+      <c r="BA83" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB83" t="s">
+        <v>77</v>
       </c>
       <c r="BC83">
-        <v>2</v>
-      </c>
-      <c r="BD83">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="BD83" t="s">
+        <v>77</v>
       </c>
       <c r="BE83">
-        <v>2</v>
-      </c>
-      <c r="BF83">
-        <v>2</v>
-      </c>
-      <c r="BG83">
-        <v>5</v>
-      </c>
-      <c r="BH83">
-        <v>5</v>
-      </c>
-      <c r="BI83">
-        <v>5</v>
+        <v>127</v>
+      </c>
+      <c r="BF83" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG83" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH83" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI83" t="s">
+        <v>77</v>
       </c>
       <c r="BJ83">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="BK83">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="BL83">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="BM83">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="BN83">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="BO83">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="BP83">
-        <v>5</v>
+        <v>142</v>
+      </c>
+      <c r="BQ83">
+        <v>142</v>
       </c>
     </row>
-    <row r="84" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B84" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA84">
+        <v>0</v>
+      </c>
+      <c r="AB84">
+        <v>1</v>
+      </c>
+      <c r="AC84">
+        <v>1</v>
+      </c>
+      <c r="AD84">
+        <v>1</v>
+      </c>
+      <c r="AE84">
+        <v>1</v>
+      </c>
+      <c r="AF84">
+        <v>1</v>
+      </c>
+      <c r="AG84">
+        <v>1</v>
+      </c>
+      <c r="AH84">
+        <v>1</v>
+      </c>
+      <c r="AI84">
+        <v>1</v>
+      </c>
+      <c r="AJ84">
+        <v>1</v>
+      </c>
+      <c r="AK84">
+        <v>2</v>
+      </c>
+      <c r="AL84">
+        <v>2</v>
+      </c>
+      <c r="AM84">
+        <v>2</v>
+      </c>
+      <c r="AN84">
+        <v>2</v>
+      </c>
+      <c r="AO84">
+        <v>2</v>
+      </c>
+      <c r="AP84">
+        <v>2</v>
+      </c>
+      <c r="AQ84">
+        <v>2</v>
+      </c>
+      <c r="AR84">
+        <v>2</v>
+      </c>
+      <c r="AS84">
+        <v>2</v>
+      </c>
+      <c r="AT84">
+        <v>2</v>
+      </c>
+      <c r="AU84">
+        <v>2</v>
+      </c>
+      <c r="AV84">
+        <v>2</v>
+      </c>
+      <c r="AW84">
+        <v>2</v>
+      </c>
+      <c r="AX84">
+        <v>2</v>
+      </c>
+      <c r="AY84">
+        <v>2</v>
+      </c>
+      <c r="AZ84">
+        <v>2</v>
+      </c>
+      <c r="BA84">
+        <v>2</v>
+      </c>
+      <c r="BB84">
+        <v>2</v>
+      </c>
+      <c r="BC84">
+        <v>2</v>
+      </c>
+      <c r="BD84">
+        <v>2</v>
+      </c>
+      <c r="BE84">
+        <v>2</v>
+      </c>
+      <c r="BF84">
+        <v>2</v>
+      </c>
+      <c r="BG84">
+        <v>5</v>
+      </c>
+      <c r="BH84">
+        <v>5</v>
+      </c>
+      <c r="BI84">
+        <v>5</v>
+      </c>
+      <c r="BJ84">
+        <v>5</v>
+      </c>
+      <c r="BK84">
+        <v>5</v>
+      </c>
+      <c r="BL84">
+        <v>5</v>
+      </c>
+      <c r="BM84">
+        <v>5</v>
+      </c>
+      <c r="BN84">
+        <v>5</v>
+      </c>
+      <c r="BO84">
+        <v>5</v>
+      </c>
+      <c r="BP84">
+        <v>5</v>
+      </c>
+      <c r="BQ84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" t="s">
         <v>70</v>
       </c>
-      <c r="AO84">
+      <c r="AO85">
         <v>4</v>
       </c>
-      <c r="AP84">
+      <c r="AP85">
         <v>4</v>
       </c>
-      <c r="AQ84">
+      <c r="AQ85">
         <v>4</v>
       </c>
-      <c r="AR84">
+      <c r="AR85">
         <v>4</v>
       </c>
-      <c r="AS84">
+      <c r="AS85">
         <v>4</v>
       </c>
-      <c r="AT84">
+      <c r="AT85">
         <v>4</v>
       </c>
-      <c r="AU84">
+      <c r="AU85">
         <v>5</v>
       </c>
-      <c r="AV84">
+      <c r="AV85">
         <v>6</v>
       </c>
-      <c r="AW84">
+      <c r="AW85">
         <v>6</v>
       </c>
-      <c r="AX84">
+      <c r="AX85">
         <v>6</v>
       </c>
-      <c r="AY84">
+      <c r="AY85">
         <v>6</v>
       </c>
-      <c r="AZ84">
+      <c r="AZ85">
         <v>8</v>
       </c>
-      <c r="BA84">
+      <c r="BA85">
         <v>9</v>
       </c>
-      <c r="BB84">
+      <c r="BB85">
         <v>9</v>
       </c>
-      <c r="BC84">
+      <c r="BC85">
         <v>9</v>
       </c>
-      <c r="BD84">
+      <c r="BD85">
         <v>9</v>
       </c>
-      <c r="BE84">
+      <c r="BE85">
         <v>10</v>
       </c>
-      <c r="BF84">
+      <c r="BF85">
         <v>10</v>
       </c>
-      <c r="BG84">
+      <c r="BG85">
         <v>11</v>
       </c>
-      <c r="BH84">
+      <c r="BH85">
         <v>11</v>
       </c>
-      <c r="BI84">
+      <c r="BI85">
         <v>13</v>
       </c>
-      <c r="BJ84">
+      <c r="BJ85">
         <v>13</v>
       </c>
-      <c r="BK84">
+      <c r="BK85">
         <v>13</v>
       </c>
-      <c r="BL84">
+      <c r="BL85">
         <v>13</v>
       </c>
-      <c r="BM84">
+      <c r="BM85">
         <v>13</v>
       </c>
-      <c r="BN84">
+      <c r="BN85">
         <v>13</v>
       </c>
-      <c r="BO84">
+      <c r="BO85">
         <v>14</v>
       </c>
-      <c r="BP84">
+      <c r="BP85">
         <v>14</v>
       </c>
+      <c r="BQ85">
+        <v>13</v>
+      </c>
     </row>
-    <row r="86" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B86" t="s">
-        <v>78</v>
-      </c>
-      <c r="BB86">
-        <v>112</v>
-      </c>
-      <c r="BC86">
-        <v>121</v>
-      </c>
-      <c r="BD86">
-        <v>130</v>
-      </c>
-      <c r="BE86">
-        <v>135</v>
-      </c>
-      <c r="BF86">
-        <v>137</v>
-      </c>
-      <c r="BG86">
-        <v>137</v>
-      </c>
-      <c r="BH86">
-        <v>137</v>
-      </c>
-      <c r="BI86">
-        <v>137</v>
-      </c>
-      <c r="BJ86">
-        <v>142</v>
-      </c>
-      <c r="BK86">
-        <v>144</v>
-      </c>
-      <c r="BL86">
-        <v>145</v>
-      </c>
-      <c r="BM86">
-        <v>147</v>
-      </c>
-      <c r="BN86">
-        <v>147</v>
-      </c>
-      <c r="BO86">
-        <v>150</v>
-      </c>
-      <c r="BP86">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="87" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="BB87">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="BC87">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="BD87">
-        <v>10</v>
+        <v>130</v>
       </c>
       <c r="BE87">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="BF87">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="BG87">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="BH87">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="BI87">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="BJ87">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="BK87">
-        <v>22</v>
+        <v>144</v>
       </c>
       <c r="BL87">
-        <v>22</v>
+        <v>145</v>
       </c>
       <c r="BM87">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="BN87">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="BO87">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="BP87">
-        <v>24</v>
+        <v>155</v>
+      </c>
+      <c r="BQ87">
+        <v>156</v>
       </c>
     </row>
-    <row r="88" spans="1:68" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B88" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BB88">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="BC88">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="BD88">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="BE88">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="BF88">
+        <v>14</v>
+      </c>
+      <c r="BG88">
+        <v>15</v>
+      </c>
+      <c r="BH88">
+        <v>15</v>
+      </c>
+      <c r="BI88">
         <v>18</v>
-      </c>
-      <c r="BG88">
-        <v>18</v>
-      </c>
-      <c r="BH88">
-        <v>19</v>
-      </c>
-      <c r="BI88">
-        <v>19</v>
       </c>
       <c r="BJ88">
         <v>19</v>
       </c>
       <c r="BK88">
+        <v>22</v>
+      </c>
+      <c r="BL88">
+        <v>22</v>
+      </c>
+      <c r="BM88">
+        <v>24</v>
+      </c>
+      <c r="BN88">
+        <v>24</v>
+      </c>
+      <c r="BO88">
+        <v>24</v>
+      </c>
+      <c r="BP88">
+        <v>24</v>
+      </c>
+      <c r="BQ88">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB89">
+        <v>16</v>
+      </c>
+      <c r="BC89">
+        <v>16</v>
+      </c>
+      <c r="BD89">
+        <v>17</v>
+      </c>
+      <c r="BE89">
+        <v>17</v>
+      </c>
+      <c r="BF89">
+        <v>18</v>
+      </c>
+      <c r="BG89">
+        <v>18</v>
+      </c>
+      <c r="BH89">
         <v>19</v>
       </c>
-      <c r="BL88">
+      <c r="BI89">
+        <v>19</v>
+      </c>
+      <c r="BJ89">
+        <v>19</v>
+      </c>
+      <c r="BK89">
+        <v>19</v>
+      </c>
+      <c r="BL89">
         <v>20</v>
       </c>
-      <c r="BM88">
+      <c r="BM89">
         <v>20</v>
       </c>
-      <c r="BN88">
+      <c r="BN89">
         <v>20</v>
       </c>
-      <c r="BO88">
+      <c r="BO89">
         <v>20</v>
       </c>
-      <c r="BP88">
+      <c r="BP89">
         <v>20</v>
       </c>
+      <c r="BQ89">
+        <v>21</v>
+      </c>
     </row>
-    <row r="103" spans="52:52" x14ac:dyDescent="0.25">
-      <c r="AZ103">
+    <row r="104" spans="52:52" x14ac:dyDescent="0.3">
+      <c r="AZ104">
         <v>9</v>
       </c>
     </row>
@@ -9118,21 +9345,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AQ11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:AR11"/>
   <sheetViews>
-    <sheetView topLeftCell="AB2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ11" sqref="AQ11"/>
+    <sheetView topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR1" sqref="AR1:AR1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -9262,8 +9489,11 @@
       <c r="AQ2" s="9">
         <v>43962</v>
       </c>
+      <c r="AR2" s="9">
+        <v>43963</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -9393,8 +9623,11 @@
       <c r="AQ3">
         <v>872</v>
       </c>
+      <c r="AR3">
+        <v>880</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -9524,8 +9757,11 @@
       <c r="AQ4">
         <v>400</v>
       </c>
+      <c r="AR4">
+        <v>403</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -9655,8 +9891,11 @@
       <c r="AQ5">
         <v>353</v>
       </c>
+      <c r="AR5">
+        <v>357</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -9786,8 +10025,11 @@
       <c r="AQ6">
         <v>1298</v>
       </c>
+      <c r="AR6">
+        <v>1328</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -9917,8 +10159,11 @@
       <c r="AQ7">
         <v>1017</v>
       </c>
+      <c r="AR7">
+        <v>1032</v>
+      </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -10048,8 +10293,11 @@
       <c r="AQ8">
         <v>610</v>
       </c>
+      <c r="AR8">
+        <v>616</v>
+      </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -10179,8 +10427,11 @@
       <c r="AQ9">
         <v>943</v>
       </c>
+      <c r="AR9">
+        <v>960</v>
+      </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -10310,8 +10561,11 @@
       <c r="AQ10">
         <v>909</v>
       </c>
+      <c r="AR10">
+        <v>925</v>
+      </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
@@ -10439,6 +10693,9 @@
         <v>82</v>
       </c>
       <c r="AQ11">
+        <v>83</v>
+      </c>
+      <c r="AR11">
         <v>83</v>
       </c>
     </row>
@@ -10449,21 +10706,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AL17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:AM17"/>
   <sheetViews>
-    <sheetView topLeftCell="O12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AL17" sqref="AL17"/>
+    <sheetView topLeftCell="V1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:38" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -10576,8 +10833,11 @@
       <c r="AL2" s="9">
         <v>43962</v>
       </c>
+      <c r="AM2" s="9">
+        <v>43963</v>
+      </c>
     </row>
-    <row r="3" spans="1:38" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>38</v>
       </c>
@@ -10585,7 +10845,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>51</v>
       </c>
@@ -10700,8 +10960,11 @@
       <c r="AL4">
         <v>6485</v>
       </c>
+      <c r="AM4">
+        <v>6584</v>
+      </c>
     </row>
-    <row r="5" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>36</v>
       </c>
@@ -10816,8 +11079,11 @@
       <c r="AL5">
         <v>905</v>
       </c>
+      <c r="AM5">
+        <v>882</v>
+      </c>
     </row>
-    <row r="6" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -10932,8 +11198,11 @@
       <c r="AL6">
         <v>988</v>
       </c>
+      <c r="AM6">
+        <v>1013</v>
+      </c>
     </row>
-    <row r="7" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -11048,8 +11317,11 @@
       <c r="AL7">
         <v>3022</v>
       </c>
+      <c r="AM7">
+        <v>3071</v>
+      </c>
     </row>
-    <row r="8" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -11164,8 +11436,11 @@
       <c r="AL8">
         <v>85</v>
       </c>
+      <c r="AM8">
+        <v>88</v>
+      </c>
     </row>
-    <row r="9" spans="1:38" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -11280,8 +11555,11 @@
       <c r="AL9">
         <v>15</v>
       </c>
+      <c r="AM9">
+        <v>15</v>
+      </c>
     </row>
-    <row r="10" spans="1:38" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -11392,8 +11670,11 @@
       <c r="AL10">
         <v>16</v>
       </c>
+      <c r="AM10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="11" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -11508,8 +11789,11 @@
       <c r="AL11">
         <v>1414</v>
       </c>
+      <c r="AM11">
+        <v>1460</v>
+      </c>
     </row>
-    <row r="12" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -11624,8 +11908,11 @@
       <c r="AL12">
         <v>40</v>
       </c>
+      <c r="AM12">
+        <v>40</v>
+      </c>
     </row>
-    <row r="13" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -11636,7 +11923,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
@@ -11751,8 +12038,11 @@
       <c r="AL14">
         <v>1398</v>
       </c>
+      <c r="AM14">
+        <v>1382</v>
+      </c>
     </row>
-    <row r="15" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -11867,8 +12157,11 @@
       <c r="AL15">
         <v>1416</v>
       </c>
+      <c r="AM15">
+        <v>1472</v>
+      </c>
     </row>
-    <row r="16" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -11983,8 +12276,11 @@
       <c r="AL16">
         <v>3649</v>
       </c>
+      <c r="AM16">
+        <v>3708</v>
+      </c>
     </row>
-    <row r="17" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -12097,6 +12393,9 @@
         <v>21</v>
       </c>
       <c r="AL17">
+        <v>22</v>
+      </c>
+      <c r="AM17">
         <v>22</v>
       </c>
     </row>
@@ -12107,20 +12406,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AM8"/>
   <sheetViews>
     <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AL9" sqref="AL9"/>
+      <selection activeCell="AM2" sqref="AM1:AM1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -12232,14 +12531,17 @@
       <c r="AL1" s="9">
         <v>43962</v>
       </c>
+      <c r="AM1" s="9">
+        <v>43963</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
@@ -12355,8 +12657,11 @@
       <c r="AL3">
         <v>336</v>
       </c>
+      <c r="AM3">
+        <v>350</v>
+      </c>
     </row>
-    <row r="4" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -12471,8 +12776,11 @@
       <c r="AL4">
         <v>5</v>
       </c>
+      <c r="AM4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:38" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -12587,8 +12895,11 @@
       <c r="AL5">
         <v>259</v>
       </c>
+      <c r="AM5">
+        <v>271</v>
+      </c>
     </row>
-    <row r="6" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -12703,8 +13014,11 @@
       <c r="AL6">
         <v>32</v>
       </c>
+      <c r="AM6">
+        <v>38</v>
+      </c>
     </row>
-    <row r="7" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -12819,8 +13133,11 @@
       <c r="AL7">
         <v>38</v>
       </c>
+      <c r="AM7">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -12933,6 +13250,9 @@
         <v>2</v>
       </c>
       <c r="AL8">
+        <v>2</v>
+      </c>
+      <c r="AM8">
         <v>2</v>
       </c>
     </row>
@@ -12942,19 +13262,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DE713F-971D-4CE1-B1A8-BE60A2507C58}">
+  <dimension ref="A2:Y13"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -13027,8 +13347,11 @@
       <c r="X2" s="9">
         <v>43962</v>
       </c>
+      <c r="Y2" s="9">
+        <v>43963</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -13101,8 +13424,11 @@
       <c r="X3">
         <v>336</v>
       </c>
+      <c r="Y3">
+        <v>350</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -13175,8 +13501,11 @@
       <c r="X4">
         <v>31</v>
       </c>
+      <c r="Y4">
+        <v>32</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -13249,8 +13578,11 @@
       <c r="X5">
         <v>17</v>
       </c>
+      <c r="Y5">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -13323,8 +13655,11 @@
       <c r="X6">
         <v>22</v>
       </c>
+      <c r="Y6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -13397,8 +13732,11 @@
       <c r="X7">
         <v>43</v>
       </c>
+      <c r="Y7">
+        <v>47</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -13471,8 +13809,11 @@
       <c r="X8">
         <v>53</v>
       </c>
+      <c r="Y8">
+        <v>55</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -13545,8 +13886,11 @@
       <c r="X9">
         <v>38</v>
       </c>
+      <c r="Y9">
+        <v>38</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -13619,8 +13963,11 @@
       <c r="X10">
         <v>43</v>
       </c>
+      <c r="Y10">
+        <v>44</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -13693,8 +14040,11 @@
       <c r="X11">
         <v>74</v>
       </c>
+      <c r="Y11">
+        <v>78</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -13767,8 +14117,11 @@
       <c r="X12">
         <v>15</v>
       </c>
+      <c r="Y12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -13839,6 +14192,9 @@
         <v>0</v>
       </c>
       <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
         <v>0</v>
       </c>
     </row>
@@ -13848,12 +14204,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14060,15 +14413,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14093,18 +14458,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
14 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1240" documentId="8_{374341DD-C3B3-4BF1-BB9D-EFA90D251024}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D60B2329-C4D7-4EC1-B4DF-762F3DD0F666}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-24" yWindow="0" windowWidth="23040" windowHeight="6948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
     <sheet name="Lives Lost by Race" sheetId="4" r:id="rId4"/>
     <sheet name="Lives Lost by Ward" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -301,7 +295,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -717,30 +711,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BQ104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BR104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" topLeftCell="BI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BQ1" sqref="BQ1:BQ1048576"/>
+      <selection pane="topRight" activeCell="BP4" sqref="BP4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" customWidth="1"/>
-    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="69" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -942,8 +936,11 @@
       <c r="BQ1" s="1">
         <v>43963</v>
       </c>
+      <c r="BR1" s="1">
+        <v>43964</v>
+      </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -967,7 +964,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1149,13 +1146,16 @@
         <v>30261</v>
       </c>
       <c r="BP3">
-        <v>30050</v>
+        <v>31050</v>
       </c>
       <c r="BQ3">
         <v>31658</v>
       </c>
+      <c r="BR3">
+        <v>32999</v>
+      </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1363,8 +1363,11 @@
       <c r="BQ4">
         <v>6584</v>
       </c>
+      <c r="BR4">
+        <v>6736</v>
+      </c>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1554,8 +1557,11 @@
       <c r="BQ5">
         <v>350</v>
       </c>
+      <c r="BR5">
+        <v>358</v>
+      </c>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1715,11 +1721,14 @@
       <c r="BQ6">
         <v>934</v>
       </c>
+      <c r="BR6">
+        <v>966</v>
+      </c>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1771,8 +1780,11 @@
       <c r="BQ8">
         <v>345</v>
       </c>
+      <c r="BR8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1926,8 +1938,11 @@
       <c r="BQ9">
         <v>73</v>
       </c>
+      <c r="BR9">
+        <v>74</v>
+      </c>
     </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2081,8 +2096,11 @@
       <c r="BQ10">
         <v>440</v>
       </c>
+      <c r="BR10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2236,8 +2254,11 @@
       <c r="BQ11">
         <v>250</v>
       </c>
+      <c r="BR11">
+        <v>264</v>
+      </c>
     </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -2391,8 +2412,11 @@
       <c r="BQ12">
         <v>190</v>
       </c>
+      <c r="BR12">
+        <v>176</v>
+      </c>
     </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -2408,8 +2432,11 @@
       <c r="BQ13">
         <v>423</v>
       </c>
+      <c r="BR13">
+        <v>397</v>
+      </c>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2425,8 +2452,11 @@
       <c r="BQ14">
         <v>1887</v>
       </c>
+      <c r="BR14">
+        <v>1895</v>
+      </c>
     </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2442,13 +2472,16 @@
       <c r="BQ15" s="23">
         <v>0.76</v>
       </c>
+      <c r="BR15" s="23">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="17" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2456,7 +2489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2613,8 +2646,11 @@
       <c r="BQ19">
         <v>104</v>
       </c>
+      <c r="BR19">
+        <v>104</v>
+      </c>
     </row>
-    <row r="20" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2717,8 +2753,11 @@
       <c r="BQ20">
         <v>35</v>
       </c>
+      <c r="BR20">
+        <v>32</v>
+      </c>
     </row>
-    <row r="21" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2821,8 +2860,11 @@
       <c r="BQ21">
         <v>69</v>
       </c>
+      <c r="BR21">
+        <v>72</v>
+      </c>
     </row>
-    <row r="22" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -2970,8 +3012,11 @@
       <c r="BQ22">
         <v>115</v>
       </c>
+      <c r="BR22">
+        <v>108</v>
+      </c>
     </row>
-    <row r="23" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3119,8 +3164,11 @@
       <c r="BQ23">
         <v>150</v>
       </c>
+      <c r="BR23">
+        <v>140</v>
+      </c>
     </row>
-    <row r="24" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3268,13 +3316,16 @@
       <c r="BQ24">
         <v>1065</v>
       </c>
+      <c r="BR24">
+        <v>1075</v>
+      </c>
     </row>
-    <row r="26" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3431,8 +3482,11 @@
       <c r="BQ27">
         <v>113</v>
       </c>
+      <c r="BR27">
+        <v>113</v>
+      </c>
     </row>
-    <row r="28" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -3535,8 +3589,11 @@
       <c r="BQ28">
         <v>38</v>
       </c>
+      <c r="BR28">
+        <v>35</v>
+      </c>
     </row>
-    <row r="29" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -3639,8 +3696,11 @@
       <c r="BQ29">
         <v>75</v>
       </c>
+      <c r="BR29">
+        <v>78</v>
+      </c>
     </row>
-    <row r="30" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -3788,8 +3848,11 @@
       <c r="BQ30">
         <v>51</v>
       </c>
+      <c r="BR30">
+        <v>56</v>
+      </c>
     </row>
-    <row r="31" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3937,8 +4000,11 @@
       <c r="BQ31">
         <v>89</v>
       </c>
+      <c r="BR31">
+        <v>91</v>
+      </c>
     </row>
-    <row r="32" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4086,13 +4152,16 @@
       <c r="BQ32">
         <v>1007</v>
       </c>
+      <c r="BR32">
+        <v>1036</v>
+      </c>
     </row>
-    <row r="34" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -4237,8 +4306,11 @@
       <c r="BQ35">
         <v>75</v>
       </c>
+      <c r="BR35">
+        <v>76</v>
+      </c>
     </row>
-    <row r="36" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -4335,8 +4407,11 @@
       <c r="BQ36">
         <v>30</v>
       </c>
+      <c r="BR36">
+        <v>26</v>
+      </c>
     </row>
-    <row r="37" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -4433,8 +4508,11 @@
       <c r="BQ37">
         <v>44</v>
       </c>
+      <c r="BR37">
+        <v>49</v>
+      </c>
     </row>
-    <row r="38" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -4576,8 +4654,11 @@
       <c r="BQ38">
         <v>12</v>
       </c>
+      <c r="BR38">
+        <v>12</v>
+      </c>
     </row>
-    <row r="39" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -4716,8 +4797,11 @@
       <c r="BQ39">
         <v>42</v>
       </c>
+      <c r="BR39">
+        <v>38</v>
+      </c>
     </row>
-    <row r="40" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -4862,8 +4946,11 @@
       <c r="BQ40">
         <v>240</v>
       </c>
+      <c r="BR40">
+        <v>245</v>
+      </c>
     </row>
-    <row r="41" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -4942,16 +5029,19 @@
       <c r="BQ41">
         <v>1</v>
       </c>
+      <c r="BR41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -5102,8 +5192,11 @@
       <c r="BQ44">
         <v>179</v>
       </c>
+      <c r="BR44">
+        <v>182</v>
+      </c>
     </row>
-    <row r="45" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -5206,8 +5299,11 @@
       <c r="BQ45">
         <v>40</v>
       </c>
+      <c r="BR45">
+        <v>38</v>
+      </c>
     </row>
-    <row r="46" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -5310,8 +5406,11 @@
       <c r="BQ46">
         <v>134</v>
       </c>
+      <c r="BR46">
+        <v>138</v>
+      </c>
     </row>
-    <row r="47" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -5459,8 +5558,11 @@
       <c r="BQ47">
         <v>828</v>
       </c>
+      <c r="BR47">
+        <v>755</v>
+      </c>
     </row>
-    <row r="48" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -5563,8 +5665,11 @@
       <c r="BQ48">
         <v>868</v>
       </c>
+      <c r="BR48">
+        <v>793</v>
+      </c>
     </row>
-    <row r="49" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -5664,8 +5769,11 @@
       <c r="BQ49">
         <v>481</v>
       </c>
+      <c r="BR49">
+        <v>534</v>
+      </c>
     </row>
-    <row r="50" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -5759,16 +5867,19 @@
       <c r="BQ50">
         <v>1</v>
       </c>
+      <c r="BR50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
@@ -5904,8 +6015,11 @@
       <c r="BQ53">
         <v>27</v>
       </c>
+      <c r="BR53">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -6005,8 +6119,11 @@
       <c r="BQ54">
         <v>14</v>
       </c>
+      <c r="BR54">
+        <v>14</v>
+      </c>
     </row>
-    <row r="55" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -6106,8 +6223,11 @@
       <c r="BQ55">
         <v>12</v>
       </c>
+      <c r="BR55">
+        <v>12</v>
+      </c>
     </row>
-    <row r="56" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -6243,8 +6363,11 @@
       <c r="BQ56">
         <v>19</v>
       </c>
+      <c r="BR56">
+        <v>17</v>
+      </c>
     </row>
-    <row r="57" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -6380,8 +6503,11 @@
       <c r="BQ57">
         <v>33</v>
       </c>
+      <c r="BR57">
+        <v>31</v>
+      </c>
     </row>
-    <row r="58" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -6517,8 +6643,11 @@
       <c r="BQ58">
         <v>121</v>
       </c>
+      <c r="BR58">
+        <v>122</v>
+      </c>
     </row>
-    <row r="59" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -6612,8 +6741,11 @@
       <c r="BQ59">
         <v>1</v>
       </c>
+      <c r="BR59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>20</v>
       </c>
@@ -6749,8 +6881,11 @@
       <c r="BQ61">
         <v>10</v>
       </c>
+      <c r="BR61">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -6850,8 +6985,11 @@
       <c r="BQ62">
         <v>4</v>
       </c>
+      <c r="BR62">
+        <v>4</v>
+      </c>
     </row>
-    <row r="63" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -6951,8 +7089,11 @@
       <c r="BQ63">
         <v>6</v>
       </c>
+      <c r="BR63">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -7088,8 +7229,11 @@
       <c r="BQ64">
         <v>44</v>
       </c>
+      <c r="BR64">
+        <v>45</v>
+      </c>
     </row>
-    <row r="65" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -7225,8 +7369,11 @@
       <c r="BQ65">
         <v>48</v>
       </c>
+      <c r="BR65">
+        <v>49</v>
+      </c>
     </row>
-    <row r="66" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -7362,8 +7509,11 @@
       <c r="BQ66">
         <v>0</v>
       </c>
+      <c r="BR66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -7463,13 +7613,16 @@
       <c r="BQ67">
         <v>0</v>
       </c>
+      <c r="BR67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>22</v>
       </c>
@@ -7605,8 +7758,11 @@
       <c r="BQ70">
         <v>267</v>
       </c>
+      <c r="BR70">
+        <v>269</v>
+      </c>
     </row>
-    <row r="71" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
@@ -7742,8 +7898,11 @@
       <c r="BQ71">
         <v>323</v>
       </c>
+      <c r="BR71">
+        <v>330</v>
+      </c>
     </row>
-    <row r="72" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>22</v>
       </c>
@@ -7879,8 +8038,11 @@
       <c r="BQ72">
         <v>319</v>
       </c>
+      <c r="BR72">
+        <v>312</v>
+      </c>
     </row>
-    <row r="73" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
@@ -7974,8 +8136,11 @@
       <c r="BQ73">
         <v>15</v>
       </c>
+      <c r="BR73">
+        <v>15</v>
+      </c>
     </row>
-    <row r="75" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -8111,8 +8276,11 @@
       <c r="BQ75">
         <v>84</v>
       </c>
+      <c r="BR75">
+        <v>84</v>
+      </c>
     </row>
-    <row r="76" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -8248,8 +8416,11 @@
       <c r="BQ76">
         <v>19</v>
       </c>
+      <c r="BR76">
+        <v>19</v>
+      </c>
     </row>
-    <row r="77" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -8385,8 +8556,11 @@
       <c r="BQ77">
         <v>103</v>
       </c>
+      <c r="BR77">
+        <v>103</v>
+      </c>
     </row>
-    <row r="78" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -8522,8 +8696,11 @@
       <c r="BQ78">
         <v>157</v>
       </c>
+      <c r="BR78">
+        <v>157</v>
+      </c>
     </row>
-    <row r="79" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -8533,8 +8710,11 @@
       <c r="BQ79">
         <v>1</v>
       </c>
+      <c r="BR79">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
@@ -8670,8 +8850,11 @@
       <c r="BQ81">
         <v>79</v>
       </c>
+      <c r="BR81">
+        <v>79</v>
+      </c>
     </row>
-    <row r="82" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>31</v>
       </c>
@@ -8807,8 +8990,11 @@
       <c r="BQ82">
         <v>56</v>
       </c>
+      <c r="BR82">
+        <v>56</v>
+      </c>
     </row>
-    <row r="83" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>31</v>
       </c>
@@ -8932,8 +9118,11 @@
       <c r="BQ83">
         <v>142</v>
       </c>
+      <c r="BR83">
+        <v>142</v>
+      </c>
     </row>
-    <row r="84" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>31</v>
       </c>
@@ -9069,8 +9258,11 @@
       <c r="BQ84">
         <v>5</v>
       </c>
+      <c r="BR84">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>31</v>
       </c>
@@ -9164,8 +9356,11 @@
       <c r="BQ85">
         <v>13</v>
       </c>
+      <c r="BR85">
+        <v>13</v>
+      </c>
     </row>
-    <row r="87" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>81</v>
       </c>
@@ -9220,8 +9415,11 @@
       <c r="BQ87">
         <v>156</v>
       </c>
+      <c r="BR87">
+        <v>158</v>
+      </c>
     </row>
-    <row r="88" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>81</v>
       </c>
@@ -9276,8 +9474,11 @@
       <c r="BQ88">
         <v>27</v>
       </c>
+      <c r="BR88">
+        <v>27</v>
+      </c>
     </row>
-    <row r="89" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>81</v>
       </c>
@@ -9332,8 +9533,11 @@
       <c r="BQ89">
         <v>21</v>
       </c>
+      <c r="BR89">
+        <v>22</v>
+      </c>
     </row>
-    <row r="104" spans="52:52" x14ac:dyDescent="0.3">
+    <row r="104" spans="52:52" x14ac:dyDescent="0.25">
       <c r="AZ104">
         <v>9</v>
       </c>
@@ -9345,21 +9549,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:AR11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AS11"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR1" sqref="AR1:AR1048576"/>
+    <sheetView topLeftCell="V2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="15" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -9492,8 +9696,11 @@
       <c r="AR2" s="9">
         <v>43963</v>
       </c>
+      <c r="AS2" s="9">
+        <v>43964</v>
+      </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -9588,7 +9795,7 @@
         <v>543</v>
       </c>
       <c r="AF3">
-        <v>543</v>
+        <v>593</v>
       </c>
       <c r="AG3">
         <v>621</v>
@@ -9626,8 +9833,11 @@
       <c r="AR3">
         <v>880</v>
       </c>
+      <c r="AS3">
+        <v>908</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -9722,7 +9932,7 @@
         <v>291</v>
       </c>
       <c r="AF4">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="AG4">
         <v>318</v>
@@ -9760,8 +9970,11 @@
       <c r="AR4">
         <v>403</v>
       </c>
+      <c r="AS4">
+        <v>400</v>
+      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -9856,7 +10069,7 @@
         <v>282</v>
       </c>
       <c r="AF5">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="AG5">
         <v>302</v>
@@ -9894,8 +10107,11 @@
       <c r="AR5">
         <v>357</v>
       </c>
+      <c r="AS5">
+        <v>362</v>
+      </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -9990,7 +10206,7 @@
         <v>774</v>
       </c>
       <c r="AF6">
-        <v>774</v>
+        <v>849</v>
       </c>
       <c r="AG6">
         <v>889</v>
@@ -10028,8 +10244,11 @@
       <c r="AR6">
         <v>1328</v>
       </c>
+      <c r="AS6">
+        <v>1377</v>
+      </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -10124,7 +10343,7 @@
         <v>646</v>
       </c>
       <c r="AF7">
-        <v>646</v>
+        <v>699</v>
       </c>
       <c r="AG7">
         <v>722</v>
@@ -10162,8 +10381,11 @@
       <c r="AR7">
         <v>1032</v>
       </c>
+      <c r="AS7">
+        <v>1054</v>
+      </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -10258,7 +10480,7 @@
         <v>450</v>
       </c>
       <c r="AF8">
-        <v>450</v>
+        <v>468</v>
       </c>
       <c r="AG8">
         <v>476</v>
@@ -10296,8 +10518,11 @@
       <c r="AR8">
         <v>616</v>
       </c>
+      <c r="AS8">
+        <v>624</v>
+      </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -10392,7 +10617,7 @@
         <v>659</v>
       </c>
       <c r="AF9">
-        <v>659</v>
+        <v>701</v>
       </c>
       <c r="AG9">
         <v>711</v>
@@ -10430,8 +10655,11 @@
       <c r="AR9">
         <v>960</v>
       </c>
+      <c r="AS9">
+        <v>979</v>
+      </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -10526,7 +10754,7 @@
         <v>632</v>
       </c>
       <c r="AF10">
-        <v>632</v>
+        <v>677</v>
       </c>
       <c r="AG10">
         <v>692</v>
@@ -10564,8 +10792,11 @@
       <c r="AR10">
         <v>925</v>
       </c>
+      <c r="AS10">
+        <v>937</v>
+      </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
@@ -10660,7 +10891,7 @@
         <v>46</v>
       </c>
       <c r="AF11">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="AG11">
         <v>66</v>
@@ -10697,6 +10928,9 @@
       </c>
       <c r="AR11">
         <v>83</v>
+      </c>
+      <c r="AS11">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -10706,21 +10940,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:AM17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AN17"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AM4" sqref="AM4"/>
+    <sheetView topLeftCell="T10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AN17" sqref="AN17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -10836,8 +11070,11 @@
       <c r="AM2" s="9">
         <v>43963</v>
       </c>
+      <c r="AN2" s="9">
+        <v>43964</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>38</v>
       </c>
@@ -10845,7 +11082,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>51</v>
       </c>
@@ -10963,8 +11200,11 @@
       <c r="AM4">
         <v>6584</v>
       </c>
+      <c r="AN4">
+        <v>6736</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>36</v>
       </c>
@@ -11082,8 +11322,11 @@
       <c r="AM5">
         <v>882</v>
       </c>
+      <c r="AN5">
+        <v>795</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -11201,8 +11444,11 @@
       <c r="AM6">
         <v>1013</v>
       </c>
+      <c r="AN6">
+        <v>1076</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -11320,8 +11566,11 @@
       <c r="AM7">
         <v>3071</v>
       </c>
+      <c r="AN7">
+        <v>3179</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -11439,8 +11688,11 @@
       <c r="AM8">
         <v>88</v>
       </c>
+      <c r="AN8">
+        <v>93</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -11558,8 +11810,11 @@
       <c r="AM9">
         <v>15</v>
       </c>
+      <c r="AN9">
+        <v>18</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -11673,8 +11928,11 @@
       <c r="AM10">
         <v>15</v>
       </c>
+      <c r="AN10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -11792,8 +12050,11 @@
       <c r="AM11">
         <v>1460</v>
       </c>
+      <c r="AN11">
+        <v>1499</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -11911,8 +12172,11 @@
       <c r="AM12">
         <v>40</v>
       </c>
+      <c r="AN12">
+        <v>42</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -11923,7 +12187,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
@@ -12041,8 +12305,11 @@
       <c r="AM14">
         <v>1382</v>
       </c>
+      <c r="AN14">
+        <v>1259</v>
+      </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -12160,8 +12427,11 @@
       <c r="AM15">
         <v>1472</v>
       </c>
+      <c r="AN15">
+        <v>1573</v>
+      </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -12279,8 +12549,11 @@
       <c r="AM16">
         <v>3708</v>
       </c>
+      <c r="AN16">
+        <v>3881</v>
+      </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -12397,6 +12670,9 @@
       </c>
       <c r="AM17">
         <v>22</v>
+      </c>
+      <c r="AN17">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -12406,20 +12682,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AM8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN8"/>
   <sheetViews>
     <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM1:AM1048576"/>
+      <selection activeCell="AN9" sqref="AN9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -12534,14 +12810,17 @@
       <c r="AM1" s="9">
         <v>43963</v>
       </c>
+      <c r="AN1" s="9">
+        <v>43964</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
@@ -12660,8 +12939,11 @@
       <c r="AM3">
         <v>350</v>
       </c>
+      <c r="AN3">
+        <v>358</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -12779,8 +13061,11 @@
       <c r="AM4">
         <v>5</v>
       </c>
+      <c r="AN4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -12898,8 +13183,11 @@
       <c r="AM5">
         <v>271</v>
       </c>
+      <c r="AN5">
+        <v>277</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -13017,8 +13305,11 @@
       <c r="AM6">
         <v>38</v>
       </c>
+      <c r="AN6">
+        <v>36</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -13136,8 +13427,11 @@
       <c r="AM7">
         <v>34</v>
       </c>
+      <c r="AN7">
+        <v>38</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -13253,6 +13547,9 @@
         <v>2</v>
       </c>
       <c r="AM8">
+        <v>2</v>
+      </c>
+      <c r="AN8">
         <v>2</v>
       </c>
     </row>
@@ -13262,19 +13559,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DE713F-971D-4CE1-B1A8-BE60A2507C58}">
-  <dimension ref="A2:Y13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Z13"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
+    <sheetView topLeftCell="K5" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -13350,8 +13647,11 @@
       <c r="Y2" s="9">
         <v>43963</v>
       </c>
+      <c r="Z2" s="9">
+        <v>43964</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -13427,8 +13727,11 @@
       <c r="Y3">
         <v>350</v>
       </c>
+      <c r="Z3">
+        <v>358</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -13504,8 +13807,11 @@
       <c r="Y4">
         <v>32</v>
       </c>
+      <c r="Z4">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -13581,8 +13887,11 @@
       <c r="Y5">
         <v>18</v>
       </c>
+      <c r="Z5">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -13658,8 +13967,11 @@
       <c r="Y6">
         <v>23</v>
       </c>
+      <c r="Z6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -13735,8 +14047,11 @@
       <c r="Y7">
         <v>47</v>
       </c>
+      <c r="Z7">
+        <v>48</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -13812,8 +14127,11 @@
       <c r="Y8">
         <v>55</v>
       </c>
+      <c r="Z8">
+        <v>56</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -13889,8 +14207,11 @@
       <c r="Y9">
         <v>38</v>
       </c>
+      <c r="Z9">
+        <v>38</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -13966,8 +14287,11 @@
       <c r="Y10">
         <v>44</v>
       </c>
+      <c r="Z10">
+        <v>47</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -14043,8 +14367,11 @@
       <c r="Y11">
         <v>78</v>
       </c>
+      <c r="Z11">
+        <v>80</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -14120,8 +14447,11 @@
       <c r="Y12">
         <v>15</v>
       </c>
+      <c r="Z12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -14195,6 +14525,9 @@
         <v>0</v>
       </c>
       <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
         <v>0</v>
       </c>
     </row>
@@ -14204,12 +14537,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -14412,33 +14754,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14455,12 +14796,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
15 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Total Cases by Race" sheetId="3" r:id="rId3"/>
     <sheet name="Lives Lost by Race" sheetId="4" r:id="rId4"/>
     <sheet name="Lives Lost by Ward" sheetId="5" r:id="rId5"/>
+    <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="156">
   <si>
     <t>Testing</t>
   </si>
@@ -291,12 +292,219 @@
   <si>
     <t>Number of Lives Lost Among Personnel</t>
   </si>
+  <si>
+    <t>Skilled Nursing Facility</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Cases;</t>
+  </si>
+  <si>
+    <t>(Symptomatic</t>
+  </si>
+  <si>
+    <t>Loss of</t>
+  </si>
+  <si>
+    <t>Life:</t>
+  </si>
+  <si>
+    <t>Recovered:</t>
+  </si>
+  <si>
+    <t>Personnel</t>
+  </si>
+  <si>
+    <t>Personnel):</t>
+  </si>
+  <si>
+    <t>BridgePoint Capitol Hill (Bed Capacity: 117)</t>
+  </si>
+  <si>
+    <t>6; (2)</t>
+  </si>
+  <si>
+    <t>8; (4)</t>
+  </si>
+  <si>
+    <t>BridgePoint National Harbor (Bed Capacity: 92)</t>
+  </si>
+  <si>
+    <t>3; (0)</t>
+  </si>
+  <si>
+    <t>0; (0)</t>
+  </si>
+  <si>
+    <t>Carroll Manor (Bed Capacity: 240)</t>
+  </si>
+  <si>
+    <t>9; (7)</t>
+  </si>
+  <si>
+    <t>10; (3)</t>
+  </si>
+  <si>
+    <t>Deanwood (Bed Capacity: 296)</t>
+  </si>
+  <si>
+    <t>51; (44)</t>
+  </si>
+  <si>
+    <t>10; (1)</t>
+  </si>
+  <si>
+    <t>Forest Hills (Bed Capacity: 50)</t>
+  </si>
+  <si>
+    <t>1; (1)</t>
+  </si>
+  <si>
+    <t>1; (0)</t>
+  </si>
+  <si>
+    <t>Ingleside (Bed Capacity: 60)</t>
+  </si>
+  <si>
+    <t>2; (1)</t>
+  </si>
+  <si>
+    <t>Inspire (Bed Capacity: 180)</t>
+  </si>
+  <si>
+    <t>45; (18)</t>
+  </si>
+  <si>
+    <t>17; (14)</t>
+  </si>
+  <si>
+    <t>Jeanne Jugan Little Sisters of the Poor (Bed</t>
+  </si>
+  <si>
+    <t>Capacity: 40)</t>
+  </si>
+  <si>
+    <t>20; (11)</t>
+  </si>
+  <si>
+    <t>9; (1)</t>
+  </si>
+  <si>
+    <t>Knollwood (Bed Capacity: 73)</t>
+  </si>
+  <si>
+    <t>26; (6)</t>
+  </si>
+  <si>
+    <t>22; (14)</t>
+  </si>
+  <si>
+    <t>Lisner Home (Bed Capacity: 60)</t>
+  </si>
+  <si>
+    <t>42; (28)</t>
+  </si>
+  <si>
+    <t>9; (6)</t>
+  </si>
+  <si>
+    <t>Serenity (Bed Capacity: 183)</t>
+  </si>
+  <si>
+    <t>34; (24)</t>
+  </si>
+  <si>
+    <t>20; (15)</t>
+  </si>
+  <si>
+    <t>Stoddard Baptist (Bed Capacity: 164)</t>
+  </si>
+  <si>
+    <t>42; (18)</t>
+  </si>
+  <si>
+    <t>Thomas Circle (Bed Capacity: 57)</t>
+  </si>
+  <si>
+    <t>3; (1)</t>
+  </si>
+  <si>
+    <t>2; (2)</t>
+  </si>
+  <si>
+    <t>Transitions (Bed Capacity: 360)</t>
+  </si>
+  <si>
+    <t>102; (41)</t>
+  </si>
+  <si>
+    <t>26; (0)</t>
+  </si>
+  <si>
+    <t>UMNC (Bed Capacity: 120)</t>
+  </si>
+  <si>
+    <t>23; (7)</t>
+  </si>
+  <si>
+    <t>Unique (Bed Capacity: 230)</t>
+  </si>
+  <si>
+    <t>12; (8)</t>
+  </si>
+  <si>
+    <t>Washington Center for Aging Services</t>
+  </si>
+  <si>
+    <t>(Stoddard Global) (Bed Capacity: 259)</t>
+  </si>
+  <si>
+    <t>80; (50)</t>
+  </si>
+  <si>
+    <t>13; (3)</t>
+  </si>
+  <si>
+    <t>501; (267)</t>
+  </si>
+  <si>
+    <t>150; (64)</t>
+  </si>
+  <si>
+    <t>Grand Total All (Resident/Personnel)</t>
+  </si>
+  <si>
+    <t>651; (331)</t>
+  </si>
+  <si>
+    <t>Resident Loss of Life:</t>
+  </si>
+  <si>
+    <t>Total Resident Positive Cases; (Symptomatic Residents):</t>
+  </si>
+  <si>
+    <t>Total Personnel Positive Cases; (Symptomatic Personnel):</t>
+  </si>
+  <si>
+    <t>Residents Recovered:</t>
+  </si>
+  <si>
+    <t>Personnel Loss of Life:</t>
+  </si>
+  <si>
+    <t>These data show the number of skilled nursing facility residents and employees who were reported to DC Health as having any type of symptom or COVID-19 exposure that prompted a healthcare provider to order a test to determine if they had COVID-19; many of these people were tested when DC Health approval was required for ordering a test through the DC Public Health Laboratory.Resident and personnel loss of life that was associated with a positive SARS-CoV-2 test has been documented since mid-March 2020; DC Health replies on skilled nursing facilities to be forthcoming about this information in order for it to be properly documented in public reports.DC Health started documenting 'Recovered' for residents and personnel starting on May 5, 2020; retrospective data collection is required to gain a more complete picture for this metric.</t>
+  </si>
+  <si>
+    <t>As of May 14, 2020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,13 +539,73 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF112277"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF112277"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDF2F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -352,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -405,6 +673,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,11 +1035,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR104"/>
+  <dimension ref="A1:BS104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" topLeftCell="BI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BP4" sqref="BP4"/>
+      <selection pane="topRight" activeCell="BT3" sqref="BT3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +1050,7 @@
     <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -939,8 +1255,11 @@
       <c r="BR1" s="1">
         <v>43964</v>
       </c>
+      <c r="BS1" s="1">
+        <v>43965</v>
+      </c>
     </row>
-    <row r="2" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -964,7 +1283,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1154,8 +1473,11 @@
       <c r="BR3">
         <v>32999</v>
       </c>
+      <c r="BS3">
+        <v>34339</v>
+      </c>
     </row>
-    <row r="4" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1366,8 +1688,11 @@
       <c r="BR4">
         <v>6736</v>
       </c>
+      <c r="BS4">
+        <v>6871</v>
+      </c>
     </row>
-    <row r="5" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1560,8 +1885,11 @@
       <c r="BR5">
         <v>358</v>
       </c>
+      <c r="BS5">
+        <v>368</v>
+      </c>
     </row>
-    <row r="6" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1724,11 +2052,14 @@
       <c r="BR6">
         <v>966</v>
       </c>
+      <c r="BS6">
+        <v>975</v>
+      </c>
     </row>
-    <row r="7" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1783,8 +2114,11 @@
       <c r="BR8">
         <v>345</v>
       </c>
+      <c r="BS8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1941,8 +2275,11 @@
       <c r="BR9">
         <v>74</v>
       </c>
+      <c r="BS9">
+        <v>88</v>
+      </c>
     </row>
-    <row r="10" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2099,8 +2436,11 @@
       <c r="BR10">
         <v>440</v>
       </c>
+      <c r="BS10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2257,8 +2597,11 @@
       <c r="BR11">
         <v>264</v>
       </c>
+      <c r="BS11">
+        <v>249</v>
+      </c>
     </row>
-    <row r="12" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -2415,8 +2758,11 @@
       <c r="BR12">
         <v>176</v>
       </c>
+      <c r="BS12">
+        <v>191</v>
+      </c>
     </row>
-    <row r="13" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -2435,8 +2781,11 @@
       <c r="BR13">
         <v>397</v>
       </c>
+      <c r="BS13">
+        <v>393</v>
+      </c>
     </row>
-    <row r="14" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2455,8 +2804,11 @@
       <c r="BR14">
         <v>1895</v>
       </c>
+      <c r="BS14">
+        <v>1874</v>
+      </c>
     </row>
-    <row r="15" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2475,13 +2827,16 @@
       <c r="BR15" s="23">
         <v>0.76</v>
       </c>
+      <c r="BS15" s="23">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="17" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2489,7 +2844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2649,8 +3004,11 @@
       <c r="BR19">
         <v>104</v>
       </c>
+      <c r="BS19">
+        <v>104</v>
+      </c>
     </row>
-    <row r="20" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2756,8 +3114,11 @@
       <c r="BR20">
         <v>32</v>
       </c>
+      <c r="BS20">
+        <v>32</v>
+      </c>
     </row>
-    <row r="21" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2863,8 +3224,11 @@
       <c r="BR21">
         <v>72</v>
       </c>
+      <c r="BS21">
+        <v>72</v>
+      </c>
     </row>
-    <row r="22" spans="1:70" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3015,8 +3379,11 @@
       <c r="BR22">
         <v>108</v>
       </c>
+      <c r="BS22">
+        <v>100</v>
+      </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3167,8 +3534,11 @@
       <c r="BR23">
         <v>140</v>
       </c>
+      <c r="BS23">
+        <v>132</v>
+      </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3319,13 +3689,16 @@
       <c r="BR24">
         <v>1075</v>
       </c>
+      <c r="BS24">
+        <v>1102</v>
+      </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3485,8 +3858,11 @@
       <c r="BR27">
         <v>113</v>
       </c>
+      <c r="BS27">
+        <v>114</v>
+      </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -3592,8 +3968,11 @@
       <c r="BR28">
         <v>35</v>
       </c>
+      <c r="BS28">
+        <v>36</v>
+      </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -3699,8 +4078,11 @@
       <c r="BR29">
         <v>78</v>
       </c>
+      <c r="BS29">
+        <v>78</v>
+      </c>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -3851,8 +4233,11 @@
       <c r="BR30">
         <v>56</v>
       </c>
+      <c r="BS30">
+        <v>51</v>
+      </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4003,8 +4388,11 @@
       <c r="BR31">
         <v>91</v>
       </c>
+      <c r="BS31">
+        <v>87</v>
+      </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4155,13 +4543,16 @@
       <c r="BR32">
         <v>1036</v>
       </c>
+      <c r="BS32">
+        <v>1052</v>
+      </c>
     </row>
-    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -4309,8 +4700,11 @@
       <c r="BR35">
         <v>76</v>
       </c>
+      <c r="BS35">
+        <v>76</v>
+      </c>
     </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -4410,8 +4804,11 @@
       <c r="BR36">
         <v>26</v>
       </c>
+      <c r="BS36">
+        <v>20</v>
+      </c>
     </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -4511,8 +4908,11 @@
       <c r="BR37">
         <v>49</v>
       </c>
+      <c r="BS37">
+        <v>55</v>
+      </c>
     </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -4657,8 +5057,11 @@
       <c r="BR38">
         <v>12</v>
       </c>
+      <c r="BS38">
+        <v>9</v>
+      </c>
     </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -4800,8 +5203,11 @@
       <c r="BR39">
         <v>38</v>
       </c>
+      <c r="BS39">
+        <v>29</v>
+      </c>
     </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -4949,8 +5355,11 @@
       <c r="BR40">
         <v>245</v>
       </c>
+      <c r="BS40">
+        <v>255</v>
+      </c>
     </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -5032,16 +5441,19 @@
       <c r="BR41">
         <v>1</v>
       </c>
+      <c r="BS41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -5195,8 +5607,11 @@
       <c r="BR44">
         <v>182</v>
       </c>
+      <c r="BS44">
+        <v>180</v>
+      </c>
     </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -5302,8 +5717,11 @@
       <c r="BR45">
         <v>38</v>
       </c>
+      <c r="BS45">
+        <v>32</v>
+      </c>
     </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -5409,8 +5827,11 @@
       <c r="BR46">
         <v>138</v>
       </c>
+      <c r="BS46">
+        <v>142</v>
+      </c>
     </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -5561,8 +5982,11 @@
       <c r="BR47">
         <v>755</v>
       </c>
+      <c r="BS47">
+        <v>756</v>
+      </c>
     </row>
-    <row r="48" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -5668,8 +6092,11 @@
       <c r="BR48">
         <v>793</v>
       </c>
+      <c r="BS48">
+        <v>788</v>
+      </c>
     </row>
-    <row r="49" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -5772,8 +6199,11 @@
       <c r="BR49">
         <v>534</v>
       </c>
+      <c r="BS49">
+        <v>538</v>
+      </c>
     </row>
-    <row r="50" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -5870,16 +6300,19 @@
       <c r="BR50">
         <v>1</v>
       </c>
+      <c r="BS50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
@@ -6018,8 +6451,11 @@
       <c r="BR53">
         <v>27</v>
       </c>
+      <c r="BS53">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -6122,8 +6558,11 @@
       <c r="BR54">
         <v>14</v>
       </c>
+      <c r="BS54">
+        <v>13</v>
+      </c>
     </row>
-    <row r="55" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -6226,8 +6665,11 @@
       <c r="BR55">
         <v>12</v>
       </c>
+      <c r="BS55">
+        <v>13</v>
+      </c>
     </row>
-    <row r="56" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -6366,8 +6808,11 @@
       <c r="BR56">
         <v>17</v>
       </c>
+      <c r="BS56">
+        <v>18</v>
+      </c>
     </row>
-    <row r="57" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -6506,8 +6951,11 @@
       <c r="BR57">
         <v>31</v>
       </c>
+      <c r="BS57">
+        <v>31</v>
+      </c>
     </row>
-    <row r="58" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -6646,8 +7094,11 @@
       <c r="BR58">
         <v>122</v>
       </c>
+      <c r="BS58">
+        <v>125</v>
+      </c>
     </row>
-    <row r="59" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -6744,8 +7195,11 @@
       <c r="BR59">
         <v>1</v>
       </c>
+      <c r="BS59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>20</v>
       </c>
@@ -6884,8 +7338,11 @@
       <c r="BR61">
         <v>10</v>
       </c>
+      <c r="BS61">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -6988,8 +7445,11 @@
       <c r="BR62">
         <v>4</v>
       </c>
+      <c r="BS62">
+        <v>4</v>
+      </c>
     </row>
-    <row r="63" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -7092,8 +7552,11 @@
       <c r="BR63">
         <v>6</v>
       </c>
+      <c r="BS63">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -7232,8 +7695,11 @@
       <c r="BR64">
         <v>45</v>
       </c>
+      <c r="BS64">
+        <v>43</v>
+      </c>
     </row>
-    <row r="65" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -7372,8 +7838,11 @@
       <c r="BR65">
         <v>49</v>
       </c>
+      <c r="BS65">
+        <v>47</v>
+      </c>
     </row>
-    <row r="66" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -7512,8 +7981,11 @@
       <c r="BR66">
         <v>0</v>
       </c>
+      <c r="BS66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -7616,13 +8088,16 @@
       <c r="BR67">
         <v>0</v>
       </c>
+      <c r="BS67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:71" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>22</v>
       </c>
@@ -7761,8 +8236,11 @@
       <c r="BR70">
         <v>269</v>
       </c>
+      <c r="BS70">
+        <v>272</v>
+      </c>
     </row>
-    <row r="71" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
@@ -7901,8 +8379,11 @@
       <c r="BR71">
         <v>330</v>
       </c>
+      <c r="BS71">
+        <v>327</v>
+      </c>
     </row>
-    <row r="72" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>22</v>
       </c>
@@ -8041,8 +8522,11 @@
       <c r="BR72">
         <v>312</v>
       </c>
+      <c r="BS72">
+        <v>326</v>
+      </c>
     </row>
-    <row r="73" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
@@ -8139,8 +8623,11 @@
       <c r="BR73">
         <v>15</v>
       </c>
+      <c r="BS73">
+        <v>15</v>
+      </c>
     </row>
-    <row r="75" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -8279,8 +8766,11 @@
       <c r="BR75">
         <v>84</v>
       </c>
+      <c r="BS75">
+        <v>87</v>
+      </c>
     </row>
-    <row r="76" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -8419,8 +8909,11 @@
       <c r="BR76">
         <v>19</v>
       </c>
+      <c r="BS76">
+        <v>13</v>
+      </c>
     </row>
-    <row r="77" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -8559,8 +9052,11 @@
       <c r="BR77">
         <v>103</v>
       </c>
+      <c r="BS77">
+        <v>100</v>
+      </c>
     </row>
-    <row r="78" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -8699,8 +9195,11 @@
       <c r="BR78">
         <v>157</v>
       </c>
+      <c r="BS78">
+        <v>163</v>
+      </c>
     </row>
-    <row r="79" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -8713,8 +9212,11 @@
       <c r="BR79">
         <v>1</v>
       </c>
+      <c r="BS79">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
@@ -8853,8 +9355,11 @@
       <c r="BR81">
         <v>79</v>
       </c>
+      <c r="BS81">
+        <v>79</v>
+      </c>
     </row>
-    <row r="82" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>31</v>
       </c>
@@ -8993,8 +9498,11 @@
       <c r="BR82">
         <v>56</v>
       </c>
+      <c r="BS82">
+        <v>56</v>
+      </c>
     </row>
-    <row r="83" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>31</v>
       </c>
@@ -9121,8 +9629,11 @@
       <c r="BR83">
         <v>142</v>
       </c>
+      <c r="BS83">
+        <v>142</v>
+      </c>
     </row>
-    <row r="84" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>31</v>
       </c>
@@ -9261,8 +9772,11 @@
       <c r="BR84">
         <v>5</v>
       </c>
+      <c r="BS84">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>31</v>
       </c>
@@ -9359,8 +9873,11 @@
       <c r="BR85">
         <v>13</v>
       </c>
+      <c r="BS85">
+        <v>13</v>
+      </c>
     </row>
-    <row r="87" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>81</v>
       </c>
@@ -9418,8 +9935,11 @@
       <c r="BR87">
         <v>158</v>
       </c>
+      <c r="BS87">
+        <v>158</v>
+      </c>
     </row>
-    <row r="88" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>81</v>
       </c>
@@ -9477,8 +9997,11 @@
       <c r="BR88">
         <v>27</v>
       </c>
+      <c r="BS88">
+        <v>38</v>
+      </c>
     </row>
-    <row r="89" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>81</v>
       </c>
@@ -9535,6 +10058,9 @@
       </c>
       <c r="BR89">
         <v>22</v>
+      </c>
+      <c r="BS89">
+        <v>23</v>
       </c>
     </row>
     <row r="104" spans="52:52" x14ac:dyDescent="0.25">
@@ -9550,10 +10076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AS11"/>
+  <dimension ref="A2:AT11"/>
   <sheetViews>
-    <sheetView topLeftCell="V2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI16" sqref="AI16"/>
+    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT2" sqref="AT2:AT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9563,7 +10089,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:45" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -9699,8 +10225,11 @@
       <c r="AS2" s="9">
         <v>43964</v>
       </c>
+      <c r="AT2" s="9">
+        <v>43965</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -9836,8 +10365,11 @@
       <c r="AS3">
         <v>908</v>
       </c>
+      <c r="AT3">
+        <v>924</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -9973,8 +10505,11 @@
       <c r="AS4">
         <v>400</v>
       </c>
+      <c r="AT4">
+        <v>408</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -10110,8 +10645,11 @@
       <c r="AS5">
         <v>362</v>
       </c>
+      <c r="AT5">
+        <v>364</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -10247,8 +10785,11 @@
       <c r="AS6">
         <v>1377</v>
       </c>
+      <c r="AT6">
+        <v>1409</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -10384,8 +10925,11 @@
       <c r="AS7">
         <v>1054</v>
       </c>
+      <c r="AT7">
+        <v>1070</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -10521,8 +11065,11 @@
       <c r="AS8">
         <v>624</v>
       </c>
+      <c r="AT8">
+        <v>635</v>
+      </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -10658,8 +11205,11 @@
       <c r="AS9">
         <v>979</v>
       </c>
+      <c r="AT9">
+        <v>989</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -10795,8 +11345,11 @@
       <c r="AS10">
         <v>937</v>
       </c>
+      <c r="AT10">
+        <v>977</v>
+      </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
@@ -10930,6 +11483,9 @@
         <v>83</v>
       </c>
       <c r="AS11">
+        <v>95</v>
+      </c>
+      <c r="AT11">
         <v>95</v>
       </c>
     </row>
@@ -10941,10 +11497,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AN17"/>
+  <dimension ref="A2:AO17"/>
   <sheetViews>
-    <sheetView topLeftCell="T10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AN17" sqref="AN17"/>
+    <sheetView topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2:AO17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10954,7 +11510,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:40" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -11073,8 +11629,11 @@
       <c r="AN2" s="9">
         <v>43964</v>
       </c>
+      <c r="AO2" s="9">
+        <v>43965</v>
+      </c>
     </row>
-    <row r="3" spans="1:40" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>38</v>
       </c>
@@ -11082,7 +11641,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>51</v>
       </c>
@@ -11203,8 +11762,11 @@
       <c r="AN4">
         <v>6736</v>
       </c>
+      <c r="AO4">
+        <v>6871</v>
+      </c>
     </row>
-    <row r="5" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>36</v>
       </c>
@@ -11325,8 +11887,11 @@
       <c r="AN5">
         <v>795</v>
       </c>
+      <c r="AO5">
+        <v>807</v>
+      </c>
     </row>
-    <row r="6" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -11447,8 +12012,11 @@
       <c r="AN6">
         <v>1076</v>
       </c>
+      <c r="AO6">
+        <v>1097</v>
+      </c>
     </row>
-    <row r="7" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -11569,8 +12137,11 @@
       <c r="AN7">
         <v>3179</v>
       </c>
+      <c r="AO7">
+        <v>3258</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -11691,8 +12262,11 @@
       <c r="AN8">
         <v>93</v>
       </c>
+      <c r="AO8">
+        <v>95</v>
+      </c>
     </row>
-    <row r="9" spans="1:40" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -11813,8 +12387,11 @@
       <c r="AN9">
         <v>18</v>
       </c>
+      <c r="AO9">
+        <v>19</v>
+      </c>
     </row>
-    <row r="10" spans="1:40" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -11931,8 +12508,11 @@
       <c r="AN10">
         <v>16</v>
       </c>
+      <c r="AO10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="11" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -12053,8 +12633,11 @@
       <c r="AN11">
         <v>1499</v>
       </c>
+      <c r="AO11">
+        <v>1538</v>
+      </c>
     </row>
-    <row r="12" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -12175,8 +12758,11 @@
       <c r="AN12">
         <v>42</v>
       </c>
+      <c r="AO12">
+        <v>42</v>
+      </c>
     </row>
-    <row r="13" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -12187,7 +12773,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
@@ -12308,8 +12894,11 @@
       <c r="AN14">
         <v>1259</v>
       </c>
+      <c r="AO14">
+        <v>1286</v>
+      </c>
     </row>
-    <row r="15" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -12430,8 +13019,11 @@
       <c r="AN15">
         <v>1573</v>
       </c>
+      <c r="AO15">
+        <v>1624</v>
+      </c>
     </row>
-    <row r="16" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -12552,8 +13144,11 @@
       <c r="AN16">
         <v>3881</v>
       </c>
+      <c r="AO16">
+        <v>3938</v>
+      </c>
     </row>
-    <row r="17" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -12672,6 +13267,9 @@
         <v>22</v>
       </c>
       <c r="AN17">
+        <v>23</v>
+      </c>
+      <c r="AO17">
         <v>23</v>
       </c>
     </row>
@@ -12683,10 +13281,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN8"/>
+  <dimension ref="A1:AO8"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AN9" sqref="AN9"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AO1" sqref="AO1:AO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12695,7 +13293,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -12813,14 +13411,17 @@
       <c r="AN1" s="9">
         <v>43964</v>
       </c>
+      <c r="AO1" s="9">
+        <v>43965</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
@@ -12942,8 +13543,11 @@
       <c r="AN3">
         <v>358</v>
       </c>
+      <c r="AO3">
+        <v>368</v>
+      </c>
     </row>
-    <row r="4" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -13064,8 +13668,11 @@
       <c r="AN4">
         <v>5</v>
       </c>
+      <c r="AO4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:40" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -13186,8 +13793,11 @@
       <c r="AN5">
         <v>277</v>
       </c>
+      <c r="AO5">
+        <v>283</v>
+      </c>
     </row>
-    <row r="6" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -13308,8 +13918,11 @@
       <c r="AN6">
         <v>36</v>
       </c>
+      <c r="AO6">
+        <v>37</v>
+      </c>
     </row>
-    <row r="7" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -13430,8 +14043,11 @@
       <c r="AN7">
         <v>38</v>
       </c>
+      <c r="AO7">
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -13550,6 +14166,9 @@
         <v>2</v>
       </c>
       <c r="AN8">
+        <v>2</v>
+      </c>
+      <c r="AO8">
         <v>2</v>
       </c>
     </row>
@@ -13560,10 +14179,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Z13"/>
+  <dimension ref="A2:AA13"/>
   <sheetViews>
-    <sheetView topLeftCell="K5" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2:AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13571,7 +14190,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -13650,8 +14269,11 @@
       <c r="Z2" s="9">
         <v>43964</v>
       </c>
+      <c r="AA2" s="9">
+        <v>43965</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -13730,8 +14352,11 @@
       <c r="Z3">
         <v>358</v>
       </c>
+      <c r="AA3">
+        <v>368</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -13810,8 +14435,11 @@
       <c r="Z4">
         <v>33</v>
       </c>
+      <c r="AA4">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -13890,8 +14518,11 @@
       <c r="Z5">
         <v>18</v>
       </c>
+      <c r="AA5">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -13970,8 +14601,11 @@
       <c r="Z6">
         <v>23</v>
       </c>
+      <c r="AA6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -14050,8 +14684,11 @@
       <c r="Z7">
         <v>48</v>
       </c>
+      <c r="AA7">
+        <v>49</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -14130,8 +14767,11 @@
       <c r="Z8">
         <v>56</v>
       </c>
+      <c r="AA8">
+        <v>57</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -14210,8 +14850,11 @@
       <c r="Z9">
         <v>38</v>
       </c>
+      <c r="AA9">
+        <v>39</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -14290,8 +14933,11 @@
       <c r="Z10">
         <v>47</v>
       </c>
+      <c r="AA10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -14370,8 +15016,11 @@
       <c r="Z11">
         <v>80</v>
       </c>
+      <c r="AA11">
+        <v>82</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -14450,8 +15099,11 @@
       <c r="Z12">
         <v>15</v>
       </c>
+      <c r="AA12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -14528,11 +15180,610 @@
         <v>0</v>
       </c>
       <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="28"/>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="29">
+        <v>0</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="29">
+        <v>0</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="29">
+        <v>3</v>
+      </c>
+      <c r="D9" s="29">
+        <v>0</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="29">
+        <v>4</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="29">
+        <v>0</v>
+      </c>
+      <c r="G10" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="29">
+        <v>9</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="29">
+        <v>0</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="29">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="29">
+        <v>0</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="29">
+        <v>1</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="29">
+        <v>10</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="29">
+        <v>1</v>
+      </c>
+      <c r="G14" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="36">
+        <v>3</v>
+      </c>
+      <c r="D15" s="36">
+        <v>0</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="36">
+        <v>0</v>
+      </c>
+      <c r="G15" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="29">
+        <v>6</v>
+      </c>
+      <c r="D17" s="29">
+        <v>0</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="29">
+        <v>1</v>
+      </c>
+      <c r="G17" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="29">
+        <v>9</v>
+      </c>
+      <c r="D18" s="29">
+        <v>0</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="29">
+        <v>0</v>
+      </c>
+      <c r="G18" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="29">
+        <v>8</v>
+      </c>
+      <c r="D19" s="29">
+        <v>0</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="29">
+        <v>0</v>
+      </c>
+      <c r="G19" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="29">
+        <v>14</v>
+      </c>
+      <c r="D20" s="29">
+        <v>0</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="29">
+        <v>0</v>
+      </c>
+      <c r="G20" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="29">
+        <v>1</v>
+      </c>
+      <c r="D21" s="29">
+        <v>0</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="29">
+        <v>0</v>
+      </c>
+      <c r="G21" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="29">
+        <v>21</v>
+      </c>
+      <c r="D22" s="29">
+        <v>0</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="29">
+        <v>0</v>
+      </c>
+      <c r="G22" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="29">
+        <v>6</v>
+      </c>
+      <c r="D23" s="29">
+        <v>0</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="29">
+        <v>0</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="29">
+        <v>7</v>
+      </c>
+      <c r="D24" s="29">
+        <v>0</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="29">
+        <v>0</v>
+      </c>
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="36">
+        <v>17</v>
+      </c>
+      <c r="D25" s="36">
+        <v>0</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="36">
+        <v>1</v>
+      </c>
+      <c r="G25" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="29">
+        <v>119</v>
+      </c>
+      <c r="D27" s="29">
+        <v>0</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="29">
+        <v>3</v>
+      </c>
+      <c r="G27" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+    </row>
+    <row r="31" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="D2:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14767,13 +16018,13 @@
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
16 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="155">
   <si>
     <t>Testing</t>
   </si>
@@ -332,9 +332,6 @@
     <t>BridgePoint National Harbor (Bed Capacity: 92)</t>
   </si>
   <si>
-    <t>3; (0)</t>
-  </si>
-  <si>
     <t>0; (0)</t>
   </si>
   <si>
@@ -350,12 +347,6 @@
     <t>Deanwood (Bed Capacity: 296)</t>
   </si>
   <si>
-    <t>51; (44)</t>
-  </si>
-  <si>
-    <t>10; (1)</t>
-  </si>
-  <si>
     <t>Forest Hills (Bed Capacity: 50)</t>
   </si>
   <si>
@@ -368,22 +359,10 @@
     <t>Ingleside (Bed Capacity: 60)</t>
   </si>
   <si>
-    <t>2; (1)</t>
-  </si>
-  <si>
     <t>Inspire (Bed Capacity: 180)</t>
   </si>
   <si>
-    <t>45; (18)</t>
-  </si>
-  <si>
     <t>17; (14)</t>
-  </si>
-  <si>
-    <t>Jeanne Jugan Little Sisters of the Poor (Bed</t>
-  </si>
-  <si>
-    <t>Capacity: 40)</t>
   </si>
   <si>
     <t>20; (11)</t>
@@ -413,16 +392,10 @@
     <t>Serenity (Bed Capacity: 183)</t>
   </si>
   <si>
-    <t>34; (24)</t>
-  </si>
-  <si>
     <t>20; (15)</t>
   </si>
   <si>
     <t>Stoddard Baptist (Bed Capacity: 164)</t>
-  </si>
-  <si>
-    <t>42; (18)</t>
   </si>
   <si>
     <t>Thomas Circle (Bed Capacity: 57)</t>
@@ -455,28 +428,13 @@
     <t>12; (8)</t>
   </si>
   <si>
-    <t>Washington Center for Aging Services</t>
-  </si>
-  <si>
-    <t>(Stoddard Global) (Bed Capacity: 259)</t>
-  </si>
-  <si>
     <t>80; (50)</t>
   </si>
   <si>
     <t>13; (3)</t>
   </si>
   <si>
-    <t>501; (267)</t>
-  </si>
-  <si>
-    <t>150; (64)</t>
-  </si>
-  <si>
     <t>Grand Total All (Resident/Personnel)</t>
-  </si>
-  <si>
-    <t>651; (331)</t>
   </si>
   <si>
     <t>Resident Loss of Life:</t>
@@ -497,7 +455,46 @@
     <t>These data show the number of skilled nursing facility residents and employees who were reported to DC Health as having any type of symptom or COVID-19 exposure that prompted a healthcare provider to order a test to determine if they had COVID-19; many of these people were tested when DC Health approval was required for ordering a test through the DC Public Health Laboratory.Resident and personnel loss of life that was associated with a positive SARS-CoV-2 test has been documented since mid-March 2020; DC Health replies on skilled nursing facilities to be forthcoming about this information in order for it to be properly documented in public reports.DC Health started documenting 'Recovered' for residents and personnel starting on May 5, 2020; retrospective data collection is required to gain a more complete picture for this metric.</t>
   </si>
   <si>
-    <t>As of May 14, 2020</t>
+    <t>4; (0)</t>
+  </si>
+  <si>
+    <t>55; (46)</t>
+  </si>
+  <si>
+    <t>4; (1)</t>
+  </si>
+  <si>
+    <t>47; (19)</t>
+  </si>
+  <si>
+    <t>39; (27)</t>
+  </si>
+  <si>
+    <t>43; (18)</t>
+  </si>
+  <si>
+    <t>516; (273)</t>
+  </si>
+  <si>
+    <t>668; (338)</t>
+  </si>
+  <si>
+    <t>Jeanne Jugan Little Sisters of the Poor (Bed Capacity: 40)</t>
+  </si>
+  <si>
+    <t>Washington Center for Aging Services (Stoddard Global) (Bed Capacity: 259)</t>
+  </si>
+  <si>
+    <t>11; (1)</t>
+  </si>
+  <si>
+    <t>152; (65)</t>
+  </si>
+  <si>
+    <t>As of May 15, 2020</t>
+  </si>
+  <si>
+    <t>Personnel Recovered:</t>
   </si>
 </sst>
 </file>
@@ -608,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -616,11 +613,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,9 +713,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -694,26 +725,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1035,11 +1072,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BS104"/>
+  <dimension ref="A1:BT104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BT3" sqref="BT3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="BR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BU1" sqref="BU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1087,7 @@
     <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1258,8 +1295,11 @@
       <c r="BS1" s="1">
         <v>43965</v>
       </c>
+      <c r="BT1" s="1">
+        <v>43966</v>
+      </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1323,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1476,8 +1516,11 @@
       <c r="BS3">
         <v>34339</v>
       </c>
+      <c r="BT3">
+        <v>35532</v>
+      </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1691,8 +1734,11 @@
       <c r="BS4">
         <v>6871</v>
       </c>
+      <c r="BT4">
+        <v>7042</v>
+      </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1888,8 +1934,11 @@
       <c r="BS5">
         <v>368</v>
       </c>
+      <c r="BT5">
+        <v>375</v>
+      </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2055,11 +2104,14 @@
       <c r="BS6">
         <v>975</v>
       </c>
+      <c r="BT6">
+        <v>998</v>
+      </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -2117,8 +2169,11 @@
       <c r="BS8">
         <v>345</v>
       </c>
+      <c r="BT8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2278,8 +2333,11 @@
       <c r="BS9">
         <v>88</v>
       </c>
+      <c r="BT9">
+        <v>86</v>
+      </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2439,8 +2497,11 @@
       <c r="BS10">
         <v>440</v>
       </c>
+      <c r="BT10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2600,8 +2661,11 @@
       <c r="BS11">
         <v>249</v>
       </c>
+      <c r="BT11">
+        <v>251</v>
+      </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -2761,8 +2825,11 @@
       <c r="BS12">
         <v>191</v>
       </c>
+      <c r="BT12">
+        <v>189</v>
+      </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -2784,8 +2851,11 @@
       <c r="BS13">
         <v>393</v>
       </c>
+      <c r="BT13">
+        <v>382</v>
+      </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2807,8 +2877,11 @@
       <c r="BS14">
         <v>1874</v>
       </c>
+      <c r="BT14">
+        <v>1862</v>
+      </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2830,13 +2903,16 @@
       <c r="BS15" s="23">
         <v>0.75</v>
       </c>
+      <c r="BT15" s="23">
+        <v>0.74</v>
+      </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2844,7 +2920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3007,8 +3083,11 @@
       <c r="BS19">
         <v>104</v>
       </c>
+      <c r="BT19">
+        <v>104</v>
+      </c>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3117,8 +3196,11 @@
       <c r="BS20">
         <v>32</v>
       </c>
+      <c r="BT20">
+        <v>32</v>
+      </c>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3227,8 +3309,11 @@
       <c r="BS21">
         <v>72</v>
       </c>
+      <c r="BT21">
+        <v>72</v>
+      </c>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3382,8 +3467,11 @@
       <c r="BS22">
         <v>100</v>
       </c>
+      <c r="BT22">
+        <v>88</v>
+      </c>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3537,8 +3625,11 @@
       <c r="BS23">
         <v>132</v>
       </c>
+      <c r="BT23">
+        <v>120</v>
+      </c>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3692,13 +3783,16 @@
       <c r="BS24">
         <v>1102</v>
       </c>
+      <c r="BT24">
+        <v>1125</v>
+      </c>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3861,8 +3955,11 @@
       <c r="BS27">
         <v>114</v>
       </c>
+      <c r="BT27">
+        <v>116</v>
+      </c>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -3971,8 +4068,11 @@
       <c r="BS28">
         <v>36</v>
       </c>
+      <c r="BT28">
+        <v>38</v>
+      </c>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4081,8 +4181,11 @@
       <c r="BS29">
         <v>78</v>
       </c>
+      <c r="BT29">
+        <v>78</v>
+      </c>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4236,8 +4339,11 @@
       <c r="BS30">
         <v>51</v>
       </c>
+      <c r="BT30">
+        <v>43</v>
+      </c>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4391,8 +4497,11 @@
       <c r="BS31">
         <v>87</v>
       </c>
+      <c r="BT31">
+        <v>81</v>
+      </c>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4546,13 +4655,16 @@
       <c r="BS32">
         <v>1052</v>
       </c>
+      <c r="BT32">
+        <v>1068</v>
+      </c>
     </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -4703,8 +4815,11 @@
       <c r="BS35">
         <v>76</v>
       </c>
+      <c r="BT35">
+        <v>76</v>
+      </c>
     </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -4807,8 +4922,11 @@
       <c r="BS36">
         <v>20</v>
       </c>
+      <c r="BT36">
+        <v>20</v>
+      </c>
     </row>
-    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -4911,8 +5029,11 @@
       <c r="BS37">
         <v>55</v>
       </c>
+      <c r="BT37">
+        <v>55</v>
+      </c>
     </row>
-    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -5060,8 +5181,11 @@
       <c r="BS38">
         <v>9</v>
       </c>
+      <c r="BT38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -5206,8 +5330,11 @@
       <c r="BS39">
         <v>29</v>
       </c>
+      <c r="BT39">
+        <v>26</v>
+      </c>
     </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -5358,8 +5485,11 @@
       <c r="BS40">
         <v>255</v>
       </c>
+      <c r="BT40">
+        <v>258</v>
+      </c>
     </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -5444,16 +5574,19 @@
       <c r="BS41">
         <v>1</v>
       </c>
+      <c r="BT41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -5610,8 +5743,11 @@
       <c r="BS44">
         <v>180</v>
       </c>
+      <c r="BT44">
+        <v>184</v>
+      </c>
     </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -5720,8 +5856,11 @@
       <c r="BS45">
         <v>32</v>
       </c>
+      <c r="BT45">
+        <v>31</v>
+      </c>
     </row>
-    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -5830,8 +5969,11 @@
       <c r="BS46">
         <v>142</v>
       </c>
+      <c r="BT46">
+        <v>147</v>
+      </c>
     </row>
-    <row r="47" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -5985,8 +6127,11 @@
       <c r="BS47">
         <v>756</v>
       </c>
+      <c r="BT47">
+        <v>761</v>
+      </c>
     </row>
-    <row r="48" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -6095,8 +6240,11 @@
       <c r="BS48">
         <v>788</v>
       </c>
+      <c r="BT48">
+        <v>792</v>
+      </c>
     </row>
-    <row r="49" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -6202,8 +6350,11 @@
       <c r="BS49">
         <v>538</v>
       </c>
+      <c r="BT49">
+        <v>535</v>
+      </c>
     </row>
-    <row r="50" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -6303,16 +6454,19 @@
       <c r="BS50">
         <v>1</v>
       </c>
+      <c r="BT50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
@@ -6454,8 +6608,11 @@
       <c r="BS53">
         <v>27</v>
       </c>
+      <c r="BT53">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -6561,8 +6718,11 @@
       <c r="BS54">
         <v>13</v>
       </c>
+      <c r="BT54">
+        <v>13</v>
+      </c>
     </row>
-    <row r="55" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -6668,8 +6828,11 @@
       <c r="BS55">
         <v>13</v>
       </c>
+      <c r="BT55">
+        <v>13</v>
+      </c>
     </row>
-    <row r="56" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -6811,8 +6974,11 @@
       <c r="BS56">
         <v>18</v>
       </c>
+      <c r="BT56">
+        <v>18</v>
+      </c>
     </row>
-    <row r="57" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -6954,8 +7120,11 @@
       <c r="BS57">
         <v>31</v>
       </c>
+      <c r="BT57">
+        <v>31</v>
+      </c>
     </row>
-    <row r="58" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -7097,8 +7266,11 @@
       <c r="BS58">
         <v>125</v>
       </c>
+      <c r="BT58">
+        <v>125</v>
+      </c>
     </row>
-    <row r="59" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -7198,8 +7370,11 @@
       <c r="BS59">
         <v>1</v>
       </c>
+      <c r="BT59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>20</v>
       </c>
@@ -7341,8 +7516,11 @@
       <c r="BS61">
         <v>10</v>
       </c>
+      <c r="BT61">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -7448,8 +7626,11 @@
       <c r="BS62">
         <v>4</v>
       </c>
+      <c r="BT62">
+        <v>4</v>
+      </c>
     </row>
-    <row r="63" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -7555,8 +7736,11 @@
       <c r="BS63">
         <v>6</v>
       </c>
+      <c r="BT63">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -7698,8 +7882,11 @@
       <c r="BS64">
         <v>43</v>
       </c>
+      <c r="BT64">
+        <v>42</v>
+      </c>
     </row>
-    <row r="65" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -7841,8 +8028,11 @@
       <c r="BS65">
         <v>47</v>
       </c>
+      <c r="BT65">
+        <v>46</v>
+      </c>
     </row>
-    <row r="66" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -7984,8 +8174,11 @@
       <c r="BS66">
         <v>0</v>
       </c>
+      <c r="BT66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -8091,13 +8284,16 @@
       <c r="BS67">
         <v>0</v>
       </c>
+      <c r="BT67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>22</v>
       </c>
@@ -8239,8 +8435,11 @@
       <c r="BS70">
         <v>272</v>
       </c>
+      <c r="BT70">
+        <v>277</v>
+      </c>
     </row>
-    <row r="71" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
@@ -8382,8 +8581,11 @@
       <c r="BS71">
         <v>327</v>
       </c>
+      <c r="BT71">
+        <v>321</v>
+      </c>
     </row>
-    <row r="72" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>22</v>
       </c>
@@ -8525,8 +8727,11 @@
       <c r="BS72">
         <v>326</v>
       </c>
+      <c r="BT72">
+        <v>312</v>
+      </c>
     </row>
-    <row r="73" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
@@ -8626,8 +8831,11 @@
       <c r="BS73">
         <v>15</v>
       </c>
+      <c r="BT73">
+        <v>15</v>
+      </c>
     </row>
-    <row r="75" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -8769,8 +8977,11 @@
       <c r="BS75">
         <v>87</v>
       </c>
+      <c r="BT75">
+        <v>95</v>
+      </c>
     </row>
-    <row r="76" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -8912,8 +9123,11 @@
       <c r="BS76">
         <v>13</v>
       </c>
+      <c r="BT76">
+        <v>15</v>
+      </c>
     </row>
-    <row r="77" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -9055,8 +9269,11 @@
       <c r="BS77">
         <v>100</v>
       </c>
+      <c r="BT77">
+        <v>108</v>
+      </c>
     </row>
-    <row r="78" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -9198,8 +9415,11 @@
       <c r="BS78">
         <v>163</v>
       </c>
+      <c r="BT78">
+        <v>163</v>
+      </c>
     </row>
-    <row r="79" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -9215,8 +9435,11 @@
       <c r="BS79">
         <v>1</v>
       </c>
+      <c r="BT79">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
@@ -9358,8 +9581,11 @@
       <c r="BS81">
         <v>79</v>
       </c>
+      <c r="BT81">
+        <v>79</v>
+      </c>
     </row>
-    <row r="82" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>31</v>
       </c>
@@ -9501,8 +9727,11 @@
       <c r="BS82">
         <v>56</v>
       </c>
+      <c r="BT82">
+        <v>56</v>
+      </c>
     </row>
-    <row r="83" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>31</v>
       </c>
@@ -9632,8 +9861,11 @@
       <c r="BS83">
         <v>142</v>
       </c>
+      <c r="BT83">
+        <v>142</v>
+      </c>
     </row>
-    <row r="84" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>31</v>
       </c>
@@ -9775,8 +10007,11 @@
       <c r="BS84">
         <v>5</v>
       </c>
+      <c r="BT84">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>31</v>
       </c>
@@ -9876,8 +10111,11 @@
       <c r="BS85">
         <v>13</v>
       </c>
+      <c r="BT85">
+        <v>13</v>
+      </c>
     </row>
-    <row r="87" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>81</v>
       </c>
@@ -9938,8 +10176,11 @@
       <c r="BS87">
         <v>158</v>
       </c>
+      <c r="BT87">
+        <v>168</v>
+      </c>
     </row>
-    <row r="88" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>81</v>
       </c>
@@ -10000,8 +10241,11 @@
       <c r="BS88">
         <v>38</v>
       </c>
+      <c r="BT88">
+        <v>38</v>
+      </c>
     </row>
-    <row r="89" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>81</v>
       </c>
@@ -10061,6 +10305,9 @@
       </c>
       <c r="BS89">
         <v>23</v>
+      </c>
+      <c r="BT89">
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="52:52" x14ac:dyDescent="0.25">
@@ -10076,10 +10323,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AT11"/>
+  <dimension ref="A2:AU11"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT2" sqref="AT2:AT11"/>
+    <sheetView topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU3" sqref="AU3:AU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10089,7 +10336,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -10228,8 +10475,11 @@
       <c r="AT2" s="9">
         <v>43965</v>
       </c>
+      <c r="AU2" s="9">
+        <v>43966</v>
+      </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -10368,8 +10618,11 @@
       <c r="AT3">
         <v>924</v>
       </c>
+      <c r="AU3">
+        <v>951</v>
+      </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -10508,8 +10761,11 @@
       <c r="AT4">
         <v>408</v>
       </c>
+      <c r="AU4">
+        <v>415</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -10648,8 +10904,11 @@
       <c r="AT5">
         <v>364</v>
       </c>
+      <c r="AU5">
+        <v>368</v>
+      </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -10788,8 +11047,11 @@
       <c r="AT6">
         <v>1409</v>
       </c>
+      <c r="AU6">
+        <v>1450</v>
+      </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -10928,8 +11190,11 @@
       <c r="AT7">
         <v>1070</v>
       </c>
+      <c r="AU7">
+        <v>1087</v>
+      </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -11068,8 +11333,11 @@
       <c r="AT8">
         <v>635</v>
       </c>
+      <c r="AU8">
+        <v>644</v>
+      </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -11208,8 +11476,11 @@
       <c r="AT9">
         <v>989</v>
       </c>
+      <c r="AU9">
+        <v>1016</v>
+      </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -11348,8 +11619,11 @@
       <c r="AT10">
         <v>977</v>
       </c>
+      <c r="AU10">
+        <v>1010</v>
+      </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
@@ -11487,6 +11761,9 @@
       </c>
       <c r="AT11">
         <v>95</v>
+      </c>
+      <c r="AU11">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -11497,10 +11774,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AO17"/>
+  <dimension ref="A2:AP17"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2:AO17"/>
+      <selection activeCell="AP4" sqref="AP4:AP17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11510,7 +11787,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -11632,8 +11909,11 @@
       <c r="AO2" s="9">
         <v>43965</v>
       </c>
+      <c r="AP2" s="9">
+        <v>43966</v>
+      </c>
     </row>
-    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>38</v>
       </c>
@@ -11641,7 +11921,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>51</v>
       </c>
@@ -11765,8 +12045,11 @@
       <c r="AO4">
         <v>6871</v>
       </c>
+      <c r="AP4">
+        <v>7042</v>
+      </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>36</v>
       </c>
@@ -11890,8 +12173,11 @@
       <c r="AO5">
         <v>807</v>
       </c>
+      <c r="AP5">
+        <v>838</v>
+      </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -12015,8 +12301,11 @@
       <c r="AO6">
         <v>1097</v>
       </c>
+      <c r="AP6">
+        <v>1105</v>
+      </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -12140,8 +12429,11 @@
       <c r="AO7">
         <v>3258</v>
       </c>
+      <c r="AP7">
+        <v>3325</v>
+      </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -12265,8 +12557,11 @@
       <c r="AO8">
         <v>95</v>
       </c>
+      <c r="AP8">
+        <v>96</v>
+      </c>
     </row>
-    <row r="9" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -12390,8 +12685,11 @@
       <c r="AO9">
         <v>19</v>
       </c>
+      <c r="AP9">
+        <v>19</v>
+      </c>
     </row>
-    <row r="10" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -12511,8 +12809,11 @@
       <c r="AO10">
         <v>15</v>
       </c>
+      <c r="AP10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -12636,8 +12937,11 @@
       <c r="AO11">
         <v>1538</v>
       </c>
+      <c r="AP11">
+        <v>1602</v>
+      </c>
     </row>
-    <row r="12" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -12761,8 +13065,11 @@
       <c r="AO12">
         <v>42</v>
       </c>
+      <c r="AP12">
+        <v>42</v>
+      </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -12773,7 +13080,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
@@ -12897,8 +13204,11 @@
       <c r="AO14">
         <v>1286</v>
       </c>
+      <c r="AP14">
+        <v>1363</v>
+      </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -13022,8 +13332,11 @@
       <c r="AO15">
         <v>1624</v>
       </c>
+      <c r="AP15">
+        <v>1659</v>
+      </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -13147,8 +13460,11 @@
       <c r="AO16">
         <v>3938</v>
       </c>
+      <c r="AP16">
+        <v>3997</v>
+      </c>
     </row>
-    <row r="17" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -13270,6 +13586,9 @@
         <v>23</v>
       </c>
       <c r="AO17">
+        <v>23</v>
+      </c>
+      <c r="AP17">
         <v>23</v>
       </c>
     </row>
@@ -13281,10 +13600,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO8"/>
+  <dimension ref="A1:AP8"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1:AO8"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13293,7 +13612,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -13414,14 +13733,17 @@
       <c r="AO1" s="9">
         <v>43965</v>
       </c>
+      <c r="AP1" s="9">
+        <v>43966</v>
+      </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
@@ -13546,8 +13868,11 @@
       <c r="AO3">
         <v>368</v>
       </c>
+      <c r="AP3">
+        <v>375</v>
+      </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -13671,8 +13996,11 @@
       <c r="AO4">
         <v>6</v>
       </c>
+      <c r="AP4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -13796,8 +14124,11 @@
       <c r="AO5">
         <v>283</v>
       </c>
+      <c r="AP5">
+        <v>288</v>
+      </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -13921,8 +14252,11 @@
       <c r="AO6">
         <v>37</v>
       </c>
+      <c r="AP6">
+        <v>37</v>
+      </c>
     </row>
-    <row r="7" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -14046,8 +14380,11 @@
       <c r="AO7">
         <v>40</v>
       </c>
+      <c r="AP7">
+        <v>41</v>
+      </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -14169,6 +14506,9 @@
         <v>2</v>
       </c>
       <c r="AO8">
+        <v>2</v>
+      </c>
+      <c r="AP8">
         <v>2</v>
       </c>
     </row>
@@ -14179,10 +14519,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AA13"/>
+  <dimension ref="A2:AB13"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2:AA13"/>
+      <selection activeCell="AB3" sqref="AB3:AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14190,7 +14530,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -14272,8 +14612,11 @@
       <c r="AA2" s="9">
         <v>43965</v>
       </c>
+      <c r="AB2" s="9">
+        <v>43966</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -14355,8 +14698,11 @@
       <c r="AA3">
         <v>368</v>
       </c>
+      <c r="AB3">
+        <v>375</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -14438,8 +14784,11 @@
       <c r="AA4">
         <v>33</v>
       </c>
+      <c r="AB4">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -14521,8 +14870,11 @@
       <c r="AA5">
         <v>20</v>
       </c>
+      <c r="AB5">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -14604,8 +14956,11 @@
       <c r="AA6">
         <v>24</v>
       </c>
+      <c r="AB6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -14687,8 +15042,11 @@
       <c r="AA7">
         <v>49</v>
       </c>
+      <c r="AB7">
+        <v>50</v>
+      </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -14770,8 +15128,11 @@
       <c r="AA8">
         <v>57</v>
       </c>
+      <c r="AB8">
+        <v>57</v>
+      </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -14853,8 +15214,11 @@
       <c r="AA9">
         <v>39</v>
       </c>
+      <c r="AB9">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -14936,8 +15300,11 @@
       <c r="AA10">
         <v>49</v>
       </c>
+      <c r="AB10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -15019,8 +15386,11 @@
       <c r="AA11">
         <v>82</v>
       </c>
+      <c r="AB11">
+        <v>83</v>
+      </c>
     </row>
-    <row r="12" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -15102,8 +15472,11 @@
       <c r="AA12">
         <v>15</v>
       </c>
+      <c r="AB12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -15183,6 +15556,9 @@
         <v>0</v>
       </c>
       <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
         <v>0</v>
       </c>
     </row>
@@ -15193,10 +15569,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15205,581 +15581,556 @@
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="A1" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>94</v>
+      <c r="B2" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="27" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="27" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="27" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="27" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="27" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="29">
-        <v>0</v>
-      </c>
-      <c r="D8" s="29">
-        <v>0</v>
-      </c>
-      <c r="E8" s="31" t="s">
+      <c r="C8" s="32">
+        <v>0</v>
+      </c>
+      <c r="D8" s="32">
+        <v>0</v>
+      </c>
+      <c r="E8" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="29">
-        <v>0</v>
-      </c>
-      <c r="G8" s="29">
+      <c r="F8" s="32">
+        <v>0</v>
+      </c>
+      <c r="G8" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="32">
+        <v>4</v>
+      </c>
+      <c r="D9" s="32">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="29">
-        <v>3</v>
-      </c>
-      <c r="D9" s="29">
-        <v>0</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" s="29">
-        <v>0</v>
-      </c>
-      <c r="G9" s="29">
+      <c r="F9" s="32">
+        <v>0</v>
+      </c>
+      <c r="G9" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="C10" s="32">
+        <v>4</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="29">
-        <v>4</v>
-      </c>
-      <c r="D10" s="29">
-        <v>0</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="29">
-        <v>0</v>
-      </c>
-      <c r="G10" s="29">
+      <c r="F10" s="32">
+        <v>0</v>
+      </c>
+      <c r="G10" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="29">
+      <c r="A11" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="32">
         <v>9</v>
       </c>
-      <c r="D11" s="29">
-        <v>0</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" s="29">
-        <v>0</v>
-      </c>
-      <c r="G11" s="29">
+      <c r="D11" s="32">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" s="32">
+        <v>0</v>
+      </c>
+      <c r="G11" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="29">
-        <v>0</v>
-      </c>
-      <c r="D12" s="29">
-        <v>0</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12" s="29">
-        <v>0</v>
-      </c>
-      <c r="G12" s="29">
+      <c r="A12" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="32">
+        <v>0</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0</v>
+      </c>
+      <c r="G12" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="29">
-        <v>1</v>
-      </c>
-      <c r="D13" s="29">
-        <v>0</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" s="29">
-        <v>0</v>
-      </c>
-      <c r="G13" s="29">
+      <c r="A13" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="32">
+        <v>3</v>
+      </c>
+      <c r="D13" s="32">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="32">
+        <v>0</v>
+      </c>
+      <c r="G13" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" s="29">
-        <v>10</v>
-      </c>
-      <c r="D14" s="29">
-        <v>0</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="29">
-        <v>1</v>
-      </c>
-      <c r="G14" s="29">
+      <c r="A14" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="32">
+        <v>12</v>
+      </c>
+      <c r="D14" s="32">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="32">
+        <v>1</v>
+      </c>
+      <c r="G14" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="36">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="32">
         <v>3</v>
       </c>
-      <c r="D15" s="36">
-        <v>0</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="F15" s="36">
-        <v>0</v>
-      </c>
-      <c r="G15" s="36">
+      <c r="D15" s="32">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="32">
+        <v>0</v>
+      </c>
+      <c r="G15" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
+      <c r="A16" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="32">
+        <v>7</v>
+      </c>
+      <c r="D16" s="32">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="32">
+        <v>1</v>
+      </c>
+      <c r="G16" s="32">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="29">
-        <v>6</v>
-      </c>
-      <c r="D17" s="29">
-        <v>0</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="F17" s="29">
-        <v>1</v>
-      </c>
-      <c r="G17" s="29">
-        <v>0</v>
+      <c r="A17" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="32">
+        <v>9</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="32">
+        <v>0</v>
+      </c>
+      <c r="G17" s="32">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="29">
-        <v>9</v>
-      </c>
-      <c r="D18" s="29">
-        <v>0</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="29">
-        <v>0</v>
-      </c>
-      <c r="G18" s="29">
-        <v>2</v>
+      <c r="A18" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="32">
+        <v>8</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" s="32">
+        <v>0</v>
+      </c>
+      <c r="G18" s="32">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" s="29">
-        <v>8</v>
-      </c>
-      <c r="D19" s="29">
-        <v>0</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="F19" s="29">
-        <v>0</v>
-      </c>
-      <c r="G19" s="29">
+      <c r="A19" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="32">
+        <v>15</v>
+      </c>
+      <c r="D19" s="32">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="32">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="29">
-        <v>14</v>
-      </c>
-      <c r="D20" s="29">
-        <v>0</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="29">
-        <v>0</v>
-      </c>
-      <c r="G20" s="29">
+      <c r="A20" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="32">
+        <v>1</v>
+      </c>
+      <c r="D20" s="32">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="F20" s="32">
+        <v>0</v>
+      </c>
+      <c r="G20" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="29">
-        <v>1</v>
-      </c>
-      <c r="D21" s="29">
-        <v>0</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="29">
-        <v>0</v>
-      </c>
-      <c r="G21" s="29">
+      <c r="A21" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="32">
+        <v>21</v>
+      </c>
+      <c r="D21" s="32">
+        <v>0</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="32">
+        <v>0</v>
+      </c>
+      <c r="G21" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="29">
-        <v>21</v>
-      </c>
-      <c r="D22" s="29">
-        <v>0</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="F22" s="29">
-        <v>0</v>
-      </c>
-      <c r="G22" s="29">
+      <c r="A22" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="32">
+        <v>6</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="32">
+        <v>0</v>
+      </c>
+      <c r="G22" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" s="29">
-        <v>6</v>
-      </c>
-      <c r="D23" s="29">
-        <v>0</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F23" s="29">
-        <v>0</v>
-      </c>
-      <c r="G23" s="29">
+      <c r="A23" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="32">
+        <v>7</v>
+      </c>
+      <c r="D23" s="32">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="32">
+        <v>0</v>
+      </c>
+      <c r="G23" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="C24" s="29">
-        <v>7</v>
-      </c>
-      <c r="D24" s="29">
-        <v>0</v>
-      </c>
-      <c r="E24" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="29">
-        <v>0</v>
-      </c>
-      <c r="G24" s="29">
+      <c r="C24" s="32">
+        <v>17</v>
+      </c>
+      <c r="D24" s="32">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" s="32">
+        <v>1</v>
+      </c>
+      <c r="G24" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="36">
-        <v>17</v>
-      </c>
-      <c r="D25" s="36">
-        <v>0</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="36">
-        <v>1</v>
-      </c>
-      <c r="G25" s="36">
-        <v>0</v>
+      <c r="A25" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="32">
+        <v>126</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" s="32">
+        <v>3</v>
+      </c>
+      <c r="G25" s="32">
+        <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" s="29">
-        <v>119</v>
-      </c>
-      <c r="D27" s="29">
-        <v>0</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="F27" s="29">
-        <v>3</v>
-      </c>
-      <c r="G27" s="29">
-        <v>2</v>
-      </c>
+      <c r="A27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-    </row>
-    <row r="31" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
+    <row r="29" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A31:E31"/>
+  <mergeCells count="4">
+    <mergeCell ref="A29:E29"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
     <mergeCell ref="D2:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16016,16 +16367,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
17 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="156">
   <si>
     <t>Testing</t>
   </si>
@@ -377,16 +377,10 @@
     <t>26; (6)</t>
   </si>
   <si>
-    <t>22; (14)</t>
-  </si>
-  <si>
     <t>Lisner Home (Bed Capacity: 60)</t>
   </si>
   <si>
     <t>42; (28)</t>
-  </si>
-  <si>
-    <t>9; (6)</t>
   </si>
   <si>
     <t>Serenity (Bed Capacity: 183)</t>
@@ -410,9 +404,6 @@
     <t>Transitions (Bed Capacity: 360)</t>
   </si>
   <si>
-    <t>102; (41)</t>
-  </si>
-  <si>
     <t>26; (0)</t>
   </si>
   <si>
@@ -426,9 +417,6 @@
   </si>
   <si>
     <t>12; (8)</t>
-  </si>
-  <si>
-    <t>80; (50)</t>
   </si>
   <si>
     <t>13; (3)</t>
@@ -458,9 +446,6 @@
     <t>4; (0)</t>
   </si>
   <si>
-    <t>55; (46)</t>
-  </si>
-  <si>
     <t>4; (1)</t>
   </si>
   <si>
@@ -468,15 +453,6 @@
   </si>
   <si>
     <t>39; (27)</t>
-  </si>
-  <si>
-    <t>43; (18)</t>
-  </si>
-  <si>
-    <t>516; (273)</t>
-  </si>
-  <si>
-    <t>668; (338)</t>
   </si>
   <si>
     <t>Jeanne Jugan Little Sisters of the Poor (Bed Capacity: 40)</t>
@@ -488,13 +464,40 @@
     <t>11; (1)</t>
   </si>
   <si>
-    <t>152; (65)</t>
+    <t>Personnel Recovered:</t>
   </si>
   <si>
-    <t>As of May 15, 2020</t>
+    <t>As of May 16, 2020</t>
   </si>
   <si>
-    <t>Personnel Recovered:</t>
+    <t>54; (46)</t>
+  </si>
+  <si>
+    <t>St. Elizabeths</t>
+  </si>
+  <si>
+    <t>41; (16)</t>
+  </si>
+  <si>
+    <t>139; (41)</t>
+  </si>
+  <si>
+    <t>79; (49)</t>
+  </si>
+  <si>
+    <t>551; (272)</t>
+  </si>
+  <si>
+    <t>707; (337)</t>
+  </si>
+  <si>
+    <t>25; (14)</t>
+  </si>
+  <si>
+    <t>10; (6)</t>
+  </si>
+  <si>
+    <t>156; (65)</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1067,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1072,11 +1075,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BT104"/>
+  <dimension ref="A1:BU104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BR1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BU1" sqref="BU1"/>
+      <pane xSplit="2" topLeftCell="BQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BV3" sqref="BV3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1090,7 @@
     <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1298,8 +1301,11 @@
       <c r="BT1" s="1">
         <v>43966</v>
       </c>
+      <c r="BU1" s="1">
+        <v>43967</v>
+      </c>
     </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1329,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1519,8 +1525,11 @@
       <c r="BT3">
         <v>35532</v>
       </c>
+      <c r="BU3">
+        <v>36526</v>
+      </c>
     </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1737,8 +1746,11 @@
       <c r="BT4">
         <v>7042</v>
       </c>
+      <c r="BU4">
+        <v>7123</v>
+      </c>
     </row>
-    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1937,8 +1949,11 @@
       <c r="BT5">
         <v>375</v>
       </c>
+      <c r="BU5">
+        <v>383</v>
+      </c>
     </row>
-    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2107,11 +2122,14 @@
       <c r="BT6">
         <v>998</v>
       </c>
+      <c r="BU6">
+        <v>1023</v>
+      </c>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -2172,8 +2190,11 @@
       <c r="BT8">
         <v>345</v>
       </c>
+      <c r="BU8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2336,8 +2357,11 @@
       <c r="BT9">
         <v>86</v>
       </c>
+      <c r="BU9">
+        <v>83</v>
+      </c>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2500,8 +2524,11 @@
       <c r="BT10">
         <v>440</v>
       </c>
+      <c r="BU10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2664,8 +2691,11 @@
       <c r="BT11">
         <v>251</v>
       </c>
+      <c r="BU11">
+        <v>232</v>
+      </c>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -2828,8 +2858,11 @@
       <c r="BT12">
         <v>189</v>
       </c>
+      <c r="BU12">
+        <v>208</v>
+      </c>
     </row>
-    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -2854,8 +2887,11 @@
       <c r="BT13">
         <v>382</v>
       </c>
+      <c r="BU13">
+        <v>369</v>
+      </c>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2880,8 +2916,11 @@
       <c r="BT14">
         <v>1862</v>
       </c>
+      <c r="BU14">
+        <v>1813</v>
+      </c>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2906,13 +2945,16 @@
       <c r="BT15" s="23">
         <v>0.74</v>
       </c>
+      <c r="BU15" s="23">
+        <v>0.73</v>
+      </c>
     </row>
-    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2920,7 +2962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3086,8 +3128,11 @@
       <c r="BT19">
         <v>104</v>
       </c>
+      <c r="BU19">
+        <v>105</v>
+      </c>
     </row>
-    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3199,8 +3244,11 @@
       <c r="BT20">
         <v>32</v>
       </c>
+      <c r="BU20">
+        <v>32</v>
+      </c>
     </row>
-    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3312,8 +3360,11 @@
       <c r="BT21">
         <v>72</v>
       </c>
+      <c r="BU21">
+        <v>73</v>
+      </c>
     </row>
-    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3470,8 +3521,11 @@
       <c r="BT22">
         <v>88</v>
       </c>
+      <c r="BU22">
+        <v>88</v>
+      </c>
     </row>
-    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3628,8 +3682,11 @@
       <c r="BT23">
         <v>120</v>
       </c>
+      <c r="BU23">
+        <v>120</v>
+      </c>
     </row>
-    <row r="24" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3786,13 +3843,16 @@
       <c r="BT24">
         <v>1125</v>
       </c>
+      <c r="BU24">
+        <v>1147</v>
+      </c>
     </row>
-    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3958,8 +4018,11 @@
       <c r="BT27">
         <v>116</v>
       </c>
+      <c r="BU27">
+        <v>117</v>
+      </c>
     </row>
-    <row r="28" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -4071,8 +4134,11 @@
       <c r="BT28">
         <v>38</v>
       </c>
+      <c r="BU28">
+        <v>39</v>
+      </c>
     </row>
-    <row r="29" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4184,8 +4250,11 @@
       <c r="BT29">
         <v>78</v>
       </c>
+      <c r="BU29">
+        <v>78</v>
+      </c>
     </row>
-    <row r="30" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4342,8 +4411,11 @@
       <c r="BT30">
         <v>43</v>
       </c>
+      <c r="BU30">
+        <v>44</v>
+      </c>
     </row>
-    <row r="31" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4500,8 +4572,11 @@
       <c r="BT31">
         <v>81</v>
       </c>
+      <c r="BU31">
+        <v>83</v>
+      </c>
     </row>
-    <row r="32" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4658,13 +4733,16 @@
       <c r="BT32">
         <v>1068</v>
       </c>
+      <c r="BU32">
+        <v>1067</v>
+      </c>
     </row>
-    <row r="34" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -4818,8 +4896,11 @@
       <c r="BT35">
         <v>76</v>
       </c>
+      <c r="BU35">
+        <v>76</v>
+      </c>
     </row>
-    <row r="36" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -4925,8 +5006,11 @@
       <c r="BT36">
         <v>20</v>
       </c>
+      <c r="BU36">
+        <v>20</v>
+      </c>
     </row>
-    <row r="37" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5032,8 +5116,11 @@
       <c r="BT37">
         <v>55</v>
       </c>
+      <c r="BU37">
+        <v>55</v>
+      </c>
     </row>
-    <row r="38" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -5184,8 +5271,11 @@
       <c r="BT38">
         <v>6</v>
       </c>
+      <c r="BU38">
+        <v>88</v>
+      </c>
     </row>
-    <row r="39" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -5333,8 +5423,11 @@
       <c r="BT39">
         <v>26</v>
       </c>
+      <c r="BU39">
+        <v>208</v>
+      </c>
     </row>
-    <row r="40" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -5488,8 +5581,11 @@
       <c r="BT40">
         <v>258</v>
       </c>
+      <c r="BU40">
+        <v>258</v>
+      </c>
     </row>
-    <row r="41" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -5577,16 +5673,19 @@
       <c r="BT41">
         <v>1</v>
       </c>
+      <c r="BU41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -5746,8 +5845,11 @@
       <c r="BT44">
         <v>184</v>
       </c>
+      <c r="BU44">
+        <v>186</v>
+      </c>
     </row>
-    <row r="45" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -5859,8 +5961,11 @@
       <c r="BT45">
         <v>31</v>
       </c>
+      <c r="BU45">
+        <v>32</v>
+      </c>
     </row>
-    <row r="46" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -5972,8 +6077,11 @@
       <c r="BT46">
         <v>147</v>
       </c>
+      <c r="BU46">
+        <v>148</v>
+      </c>
     </row>
-    <row r="47" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -6130,8 +6238,11 @@
       <c r="BT47">
         <v>761</v>
       </c>
+      <c r="BU47">
+        <v>768</v>
+      </c>
     </row>
-    <row r="48" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -6243,8 +6354,11 @@
       <c r="BT48">
         <v>792</v>
       </c>
+      <c r="BU48">
+        <v>800</v>
+      </c>
     </row>
-    <row r="49" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -6353,8 +6467,11 @@
       <c r="BT49">
         <v>535</v>
       </c>
+      <c r="BU49">
+        <v>527</v>
+      </c>
     </row>
-    <row r="50" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -6457,16 +6574,19 @@
       <c r="BT50">
         <v>1</v>
       </c>
+      <c r="BU50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
@@ -6611,8 +6731,11 @@
       <c r="BT53">
         <v>27</v>
       </c>
+      <c r="BU53">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -6721,8 +6844,11 @@
       <c r="BT54">
         <v>13</v>
       </c>
+      <c r="BU54">
+        <v>13</v>
+      </c>
     </row>
-    <row r="55" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -6831,8 +6957,11 @@
       <c r="BT55">
         <v>13</v>
       </c>
+      <c r="BU55">
+        <v>13</v>
+      </c>
     </row>
-    <row r="56" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -6977,8 +7106,11 @@
       <c r="BT56">
         <v>18</v>
       </c>
+      <c r="BU56">
+        <v>18</v>
+      </c>
     </row>
-    <row r="57" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -7123,8 +7255,11 @@
       <c r="BT57">
         <v>31</v>
       </c>
+      <c r="BU57">
+        <v>31</v>
+      </c>
     </row>
-    <row r="58" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -7269,8 +7404,11 @@
       <c r="BT58">
         <v>125</v>
       </c>
+      <c r="BU58">
+        <v>125</v>
+      </c>
     </row>
-    <row r="59" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -7373,8 +7511,11 @@
       <c r="BT59">
         <v>1</v>
       </c>
+      <c r="BU59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>20</v>
       </c>
@@ -7519,8 +7660,11 @@
       <c r="BT61">
         <v>10</v>
       </c>
+      <c r="BU61">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -7629,8 +7773,11 @@
       <c r="BT62">
         <v>4</v>
       </c>
+      <c r="BU62">
+        <v>4</v>
+      </c>
     </row>
-    <row r="63" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -7739,8 +7886,11 @@
       <c r="BT63">
         <v>6</v>
       </c>
+      <c r="BU63">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -7885,8 +8035,11 @@
       <c r="BT64">
         <v>42</v>
       </c>
+      <c r="BU64">
+        <v>44</v>
+      </c>
     </row>
-    <row r="65" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -8031,8 +8184,11 @@
       <c r="BT65">
         <v>46</v>
       </c>
+      <c r="BU65">
+        <v>48</v>
+      </c>
     </row>
-    <row r="66" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -8177,8 +8333,11 @@
       <c r="BT66">
         <v>0</v>
       </c>
+      <c r="BU66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -8287,13 +8446,16 @@
       <c r="BT67">
         <v>0</v>
       </c>
+      <c r="BU67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:73" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>22</v>
       </c>
@@ -8438,8 +8600,11 @@
       <c r="BT70">
         <v>277</v>
       </c>
+      <c r="BU70">
+        <v>277</v>
+      </c>
     </row>
-    <row r="71" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
@@ -8584,8 +8749,11 @@
       <c r="BT71">
         <v>321</v>
       </c>
+      <c r="BU71">
+        <v>326</v>
+      </c>
     </row>
-    <row r="72" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>22</v>
       </c>
@@ -8730,8 +8898,11 @@
       <c r="BT72">
         <v>312</v>
       </c>
+      <c r="BU72">
+        <v>312</v>
+      </c>
     </row>
-    <row r="73" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
@@ -8834,8 +9005,11 @@
       <c r="BT73">
         <v>15</v>
       </c>
+      <c r="BU73">
+        <v>15</v>
+      </c>
     </row>
-    <row r="75" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -8980,8 +9154,11 @@
       <c r="BT75">
         <v>95</v>
       </c>
+      <c r="BU75">
+        <v>102</v>
+      </c>
     </row>
-    <row r="76" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -9126,8 +9303,11 @@
       <c r="BT76">
         <v>15</v>
       </c>
+      <c r="BU76">
+        <v>11</v>
+      </c>
     </row>
-    <row r="77" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -9272,8 +9452,11 @@
       <c r="BT77">
         <v>108</v>
       </c>
+      <c r="BU77">
+        <v>113</v>
+      </c>
     </row>
-    <row r="78" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -9418,8 +9601,11 @@
       <c r="BT78">
         <v>163</v>
       </c>
+      <c r="BU78">
+        <v>163</v>
+      </c>
     </row>
-    <row r="79" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -9438,8 +9624,11 @@
       <c r="BT79">
         <v>1</v>
       </c>
+      <c r="BU79">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
@@ -9584,8 +9773,11 @@
       <c r="BT81">
         <v>79</v>
       </c>
+      <c r="BU81">
+        <v>79</v>
+      </c>
     </row>
-    <row r="82" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>31</v>
       </c>
@@ -9730,8 +9922,11 @@
       <c r="BT82">
         <v>56</v>
       </c>
+      <c r="BU82">
+        <v>56</v>
+      </c>
     </row>
-    <row r="83" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>31</v>
       </c>
@@ -9864,8 +10059,11 @@
       <c r="BT83">
         <v>142</v>
       </c>
+      <c r="BU83">
+        <v>142</v>
+      </c>
     </row>
-    <row r="84" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>31</v>
       </c>
@@ -10010,8 +10208,11 @@
       <c r="BT84">
         <v>5</v>
       </c>
+      <c r="BU84">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>31</v>
       </c>
@@ -10114,8 +10315,11 @@
       <c r="BT85">
         <v>13</v>
       </c>
+      <c r="BU85">
+        <v>13</v>
+      </c>
     </row>
-    <row r="87" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>81</v>
       </c>
@@ -10179,8 +10383,11 @@
       <c r="BT87">
         <v>168</v>
       </c>
+      <c r="BU87">
+        <v>169</v>
+      </c>
     </row>
-    <row r="88" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>81</v>
       </c>
@@ -10244,8 +10451,11 @@
       <c r="BT88">
         <v>38</v>
       </c>
+      <c r="BU88">
+        <v>40</v>
+      </c>
     </row>
-    <row r="89" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>81</v>
       </c>
@@ -10307,6 +10517,9 @@
         <v>23</v>
       </c>
       <c r="BT89">
+        <v>24</v>
+      </c>
+      <c r="BU89">
         <v>24</v>
       </c>
     </row>
@@ -10323,10 +10536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AU11"/>
+  <dimension ref="A2:AV11"/>
   <sheetViews>
     <sheetView topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU3" sqref="AU3:AU11"/>
+      <selection activeCell="AW4" sqref="AW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10336,7 +10549,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -10478,8 +10691,11 @@
       <c r="AU2" s="9">
         <v>43966</v>
       </c>
+      <c r="AV2" s="9">
+        <v>43967</v>
+      </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -10621,8 +10837,11 @@
       <c r="AU3">
         <v>951</v>
       </c>
+      <c r="AV3">
+        <v>962</v>
+      </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -10764,8 +10983,11 @@
       <c r="AU4">
         <v>415</v>
       </c>
+      <c r="AV4">
+        <v>419</v>
+      </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -10907,8 +11129,11 @@
       <c r="AU5">
         <v>368</v>
       </c>
+      <c r="AV5">
+        <v>374</v>
+      </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -11050,8 +11275,11 @@
       <c r="AU6">
         <v>1450</v>
       </c>
+      <c r="AV6">
+        <v>1463</v>
+      </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -11193,8 +11421,11 @@
       <c r="AU7">
         <v>1087</v>
       </c>
+      <c r="AV7">
+        <v>1111</v>
+      </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -11336,8 +11567,11 @@
       <c r="AU8">
         <v>644</v>
       </c>
+      <c r="AV8">
+        <v>646</v>
+      </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -11479,8 +11713,11 @@
       <c r="AU9">
         <v>1016</v>
       </c>
+      <c r="AV9">
+        <v>1030</v>
+      </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -11622,8 +11859,11 @@
       <c r="AU10">
         <v>1010</v>
       </c>
+      <c r="AV10">
+        <v>1015</v>
+      </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
@@ -11764,6 +12004,9 @@
       </c>
       <c r="AU11">
         <v>101</v>
+      </c>
+      <c r="AV11">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -11774,10 +12017,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AP17"/>
+  <dimension ref="A2:AQ17"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AP4" sqref="AP4:AP17"/>
+      <selection activeCell="AJ21" sqref="AJ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11787,7 +12030,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -11912,8 +12155,11 @@
       <c r="AP2" s="9">
         <v>43966</v>
       </c>
+      <c r="AQ2" s="9">
+        <v>43967</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>38</v>
       </c>
@@ -11921,7 +12167,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>51</v>
       </c>
@@ -12048,8 +12294,11 @@
       <c r="AP4">
         <v>7042</v>
       </c>
+      <c r="AQ4">
+        <v>7123</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>36</v>
       </c>
@@ -12176,8 +12425,11 @@
       <c r="AP5">
         <v>838</v>
       </c>
+      <c r="AQ5">
+        <v>825</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -12304,8 +12556,11 @@
       <c r="AP6">
         <v>1105</v>
       </c>
+      <c r="AQ6">
+        <v>1122</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -12432,8 +12687,11 @@
       <c r="AP7">
         <v>3325</v>
       </c>
+      <c r="AQ7">
+        <v>3366</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -12560,8 +12818,11 @@
       <c r="AP8">
         <v>96</v>
       </c>
+      <c r="AQ8">
+        <v>96</v>
+      </c>
     </row>
-    <row r="9" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -12688,8 +12949,11 @@
       <c r="AP9">
         <v>19</v>
       </c>
+      <c r="AQ9">
+        <v>19</v>
+      </c>
     </row>
-    <row r="10" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -12812,8 +13076,11 @@
       <c r="AP10">
         <v>15</v>
       </c>
+      <c r="AQ10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -12940,8 +13207,11 @@
       <c r="AP11">
         <v>1602</v>
       </c>
+      <c r="AQ11">
+        <v>1637</v>
+      </c>
     </row>
-    <row r="12" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -13068,8 +13338,11 @@
       <c r="AP12">
         <v>42</v>
       </c>
+      <c r="AQ12">
+        <v>42</v>
+      </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -13080,7 +13353,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
@@ -13207,8 +13480,11 @@
       <c r="AP14">
         <v>1363</v>
       </c>
+      <c r="AQ14">
+        <v>1346</v>
+      </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -13335,8 +13611,11 @@
       <c r="AP15">
         <v>1659</v>
       </c>
+      <c r="AQ15">
+        <v>1700</v>
+      </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -13463,8 +13742,11 @@
       <c r="AP16">
         <v>3997</v>
       </c>
+      <c r="AQ16">
+        <v>4054</v>
+      </c>
     </row>
-    <row r="17" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -13589,6 +13871,9 @@
         <v>23</v>
       </c>
       <c r="AP17">
+        <v>23</v>
+      </c>
+      <c r="AQ17">
         <v>23</v>
       </c>
     </row>
@@ -13600,10 +13885,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP8"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AG24" sqref="AG24"/>
+      <selection activeCell="AQ1" sqref="AQ1:AQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13612,7 +13897,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -13736,14 +14021,17 @@
       <c r="AP1" s="9">
         <v>43966</v>
       </c>
+      <c r="AQ1" s="9">
+        <v>43967</v>
+      </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
@@ -13871,8 +14159,11 @@
       <c r="AP3">
         <v>375</v>
       </c>
+      <c r="AQ3">
+        <v>383</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -13999,8 +14290,11 @@
       <c r="AP4">
         <v>7</v>
       </c>
+      <c r="AQ4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -14127,8 +14421,11 @@
       <c r="AP5">
         <v>288</v>
       </c>
+      <c r="AQ5">
+        <v>294</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -14255,8 +14552,11 @@
       <c r="AP6">
         <v>37</v>
       </c>
+      <c r="AQ6">
+        <v>37</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -14383,8 +14683,11 @@
       <c r="AP7">
         <v>41</v>
       </c>
+      <c r="AQ7">
+        <v>43</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -14509,6 +14812,9 @@
         <v>2</v>
       </c>
       <c r="AP8">
+        <v>2</v>
+      </c>
+      <c r="AQ8">
         <v>2</v>
       </c>
     </row>
@@ -14519,10 +14825,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AB13"/>
+  <dimension ref="A2:AC13"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3:AB13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14530,7 +14836,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -14615,8 +14921,11 @@
       <c r="AB2" s="9">
         <v>43966</v>
       </c>
+      <c r="AC2" s="9">
+        <v>43967</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -14701,8 +15010,11 @@
       <c r="AB3">
         <v>375</v>
       </c>
+      <c r="AC3">
+        <v>383</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -14787,8 +15099,11 @@
       <c r="AB4">
         <v>35</v>
       </c>
+      <c r="AC4">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -14873,8 +15188,11 @@
       <c r="AB5">
         <v>22</v>
       </c>
+      <c r="AC5">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -14959,8 +15277,11 @@
       <c r="AB6">
         <v>24</v>
       </c>
+      <c r="AC6">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -15045,8 +15366,11 @@
       <c r="AB7">
         <v>50</v>
       </c>
+      <c r="AC7">
+        <v>50</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -15131,8 +15455,11 @@
       <c r="AB8">
         <v>57</v>
       </c>
+      <c r="AC8">
+        <v>60</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -15217,8 +15544,11 @@
       <c r="AB9">
         <v>40</v>
       </c>
+      <c r="AC9">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -15303,8 +15633,11 @@
       <c r="AB10">
         <v>49</v>
       </c>
+      <c r="AC10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -15389,8 +15722,11 @@
       <c r="AB11">
         <v>83</v>
       </c>
+      <c r="AC11">
+        <v>84</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -15475,8 +15811,11 @@
       <c r="AB12">
         <v>15</v>
       </c>
+      <c r="AC12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -15559,6 +15898,9 @@
         <v>0</v>
       </c>
       <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
         <v>0</v>
       </c>
     </row>
@@ -15569,10 +15911,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15588,7 +15930,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -15602,22 +15944,22 @@
         <v>87</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C2" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="G2" s="30" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15709,7 +16051,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C9" s="32">
         <v>4</v>
@@ -15755,16 +16097,16 @@
         <v>104</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C11" s="32">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" s="32">
         <v>0</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F11" s="32">
         <v>0</v>
@@ -15801,7 +16143,7 @@
         <v>108</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C13" s="32">
         <v>3</v>
@@ -15824,7 +16166,7 @@
         <v>109</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C14" s="32">
         <v>12</v>
@@ -15844,13 +16186,13 @@
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>111</v>
       </c>
       <c r="C15" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="32">
         <v>0</v>
@@ -15879,7 +16221,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="F16" s="32">
         <v>1</v>
@@ -15890,10 +16232,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="32" t="s">
         <v>116</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>117</v>
       </c>
       <c r="C17" s="32">
         <v>9</v>
@@ -15902,7 +16244,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="F17" s="32">
         <v>0</v>
@@ -15913,10 +16255,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C18" s="32">
         <v>8</v>
@@ -15925,7 +16267,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F18" s="32">
         <v>0</v>
@@ -15935,14 +16277,14 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>121</v>
+      <c r="A19" s="31" t="s">
+        <v>147</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="C19" s="32">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D19" s="32">
         <v>0</v>
@@ -15959,19 +16301,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="C20" s="32">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D20" s="32">
         <v>0</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="F20" s="32">
         <v>0</v>
@@ -15982,19 +16324,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C21" s="32">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D21" s="32">
         <v>0</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F21" s="32">
         <v>0</v>
@@ -16005,19 +16347,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="C22" s="32">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D22" s="32">
         <v>0</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="F22" s="32">
         <v>0</v>
@@ -16028,107 +16370,130 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="32">
+        <v>6</v>
+      </c>
+      <c r="D23" s="32">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="32">
+        <v>0</v>
+      </c>
+      <c r="G23" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="32">
+        <v>7</v>
+      </c>
+      <c r="D24" s="32">
+        <v>0</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="32">
+        <v>0</v>
+      </c>
+      <c r="G24" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="32">
+        <v>17</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="32">
+        <v>1</v>
+      </c>
+      <c r="G25" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="32">
+        <v>128</v>
+      </c>
+      <c r="D26" s="32">
+        <v>0</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" s="32">
+        <v>3</v>
+      </c>
+      <c r="G26" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B23" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="32">
-        <v>7</v>
-      </c>
-      <c r="D23" s="32">
-        <v>0</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" s="32">
-        <v>0</v>
-      </c>
-      <c r="G23" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="C24" s="32">
-        <v>17</v>
-      </c>
-      <c r="D24" s="32">
-        <v>0</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" s="32">
-        <v>1</v>
-      </c>
-      <c r="G24" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" s="32">
-        <v>126</v>
-      </c>
-      <c r="D25" s="32">
-        <v>0</v>
-      </c>
-      <c r="E25" s="33" t="s">
+      <c r="B27" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="F25" s="32">
-        <v>3</v>
-      </c>
-      <c r="G25" s="32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
       <c r="C27" s="32"/>
       <c r="D27" s="32"/>
       <c r="E27" s="33"/>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
     </row>
-    <row r="29" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="36"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+    </row>
+    <row r="30" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:E30"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="D2:D7"/>
@@ -16139,21 +16504,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -16356,32 +16706,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16398,4 +16738,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
18 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{A5B6B11A-29FC-4452-9C12-302E5F9EB695}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BF1A4A98-642C-4133-957A-1DF627A813DE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="6945"/>
+    <workbookView xWindow="-60" yWindow="156" windowWidth="22836" windowHeight="6948" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="Lives Lost by Ward" sheetId="5" r:id="rId5"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="155">
   <si>
     <t>Testing</t>
   </si>
@@ -440,9 +446,6 @@
     <t>Personnel Loss of Life:</t>
   </si>
   <si>
-    <t>These data show the number of skilled nursing facility residents and employees who were reported to DC Health as having any type of symptom or COVID-19 exposure that prompted a healthcare provider to order a test to determine if they had COVID-19; many of these people were tested when DC Health approval was required for ordering a test through the DC Public Health Laboratory.Resident and personnel loss of life that was associated with a positive SARS-CoV-2 test has been documented since mid-March 2020; DC Health replies on skilled nursing facilities to be forthcoming about this information in order for it to be properly documented in public reports.DC Health started documenting 'Recovered' for residents and personnel starting on May 5, 2020; retrospective data collection is required to gain a more complete picture for this metric.</t>
-  </si>
-  <si>
     <t>4; (0)</t>
   </si>
   <si>
@@ -467,12 +470,6 @@
     <t>Personnel Recovered:</t>
   </si>
   <si>
-    <t>As of May 16, 2020</t>
-  </si>
-  <si>
-    <t>54; (46)</t>
-  </si>
-  <si>
     <t>St. Elizabeths</t>
   </si>
   <si>
@@ -485,12 +482,6 @@
     <t>79; (49)</t>
   </si>
   <si>
-    <t>551; (272)</t>
-  </si>
-  <si>
-    <t>707; (337)</t>
-  </si>
-  <si>
     <t>25; (14)</t>
   </si>
   <si>
@@ -499,12 +490,24 @@
   <si>
     <t>156; (65)</t>
   </si>
+  <si>
+    <t>50; (42)</t>
+  </si>
+  <si>
+    <t>547; (268)</t>
+  </si>
+  <si>
+    <t>703; (333)</t>
+  </si>
+  <si>
+    <t>As of May 17, 2020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,13 +571,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color rgb="FF112277"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -582,7 +578,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,14 +597,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -616,48 +606,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -725,31 +678,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -760,6 +698,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,6 +717,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>394</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4838700"/>
+          <a:ext cx="249288300" cy="929640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1067,30 +1074,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BU104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BV104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BV3" sqref="BV3"/>
+    <sheetView topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="BL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BV1" sqref="BV1:BV1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1304,8 +1312,11 @@
       <c r="BU1" s="1">
         <v>43967</v>
       </c>
+      <c r="BV1" s="1">
+        <v>43968</v>
+      </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1329,7 +1340,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1528,8 +1539,11 @@
       <c r="BU3">
         <v>36526</v>
       </c>
+      <c r="BV3">
+        <v>37825</v>
+      </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1749,8 +1763,11 @@
       <c r="BU4">
         <v>7123</v>
       </c>
+      <c r="BV4">
+        <v>7270</v>
+      </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1952,8 +1969,11 @@
       <c r="BU5">
         <v>383</v>
       </c>
+      <c r="BV5">
+        <v>392</v>
+      </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2125,11 +2145,14 @@
       <c r="BU6">
         <v>1023</v>
       </c>
+      <c r="BV6">
+        <v>1028</v>
+      </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -2193,8 +2216,11 @@
       <c r="BU8">
         <v>345</v>
       </c>
+      <c r="BV8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2360,8 +2386,11 @@
       <c r="BU9">
         <v>83</v>
       </c>
+      <c r="BV9">
+        <v>104</v>
+      </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2527,8 +2556,11 @@
       <c r="BU10">
         <v>440</v>
       </c>
+      <c r="BV10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2694,8 +2726,11 @@
       <c r="BU11">
         <v>232</v>
       </c>
+      <c r="BV11">
+        <v>228</v>
+      </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -2861,8 +2896,11 @@
       <c r="BU12">
         <v>208</v>
       </c>
+      <c r="BV12">
+        <v>212</v>
+      </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -2890,8 +2928,11 @@
       <c r="BU13">
         <v>369</v>
       </c>
+      <c r="BV13">
+        <v>374</v>
+      </c>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -2919,8 +2960,11 @@
       <c r="BU14">
         <v>1813</v>
       </c>
+      <c r="BV14">
+        <v>1803</v>
+      </c>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -2948,13 +2992,16 @@
       <c r="BU15" s="23">
         <v>0.73</v>
       </c>
+      <c r="BV15" s="23">
+        <v>0.72</v>
+      </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2962,7 +3009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3131,8 +3178,11 @@
       <c r="BU19">
         <v>105</v>
       </c>
+      <c r="BV19">
+        <v>105</v>
+      </c>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3247,8 +3297,11 @@
       <c r="BU20">
         <v>32</v>
       </c>
+      <c r="BV20">
+        <v>25</v>
+      </c>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3363,8 +3416,11 @@
       <c r="BU21">
         <v>73</v>
       </c>
+      <c r="BV21">
+        <v>80</v>
+      </c>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3524,8 +3580,11 @@
       <c r="BU22">
         <v>88</v>
       </c>
+      <c r="BV22">
+        <v>100</v>
+      </c>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3685,8 +3744,11 @@
       <c r="BU23">
         <v>120</v>
       </c>
+      <c r="BV23">
+        <v>125</v>
+      </c>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3846,13 +3908,16 @@
       <c r="BU24">
         <v>1147</v>
       </c>
+      <c r="BV24">
+        <v>1163</v>
+      </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:74" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -4021,8 +4086,11 @@
       <c r="BU27">
         <v>117</v>
       </c>
+      <c r="BV27">
+        <v>117</v>
+      </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -4137,8 +4205,11 @@
       <c r="BU28">
         <v>39</v>
       </c>
+      <c r="BV28">
+        <v>39</v>
+      </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4253,8 +4324,11 @@
       <c r="BU29">
         <v>78</v>
       </c>
+      <c r="BV29">
+        <v>78</v>
+      </c>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4414,8 +4488,11 @@
       <c r="BU30">
         <v>44</v>
       </c>
+      <c r="BV30">
+        <v>44</v>
+      </c>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4575,8 +4652,11 @@
       <c r="BU31">
         <v>83</v>
       </c>
+      <c r="BV31">
+        <v>83</v>
+      </c>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4736,13 +4816,16 @@
       <c r="BU32">
         <v>1067</v>
       </c>
+      <c r="BV32">
+        <v>1067</v>
+      </c>
     </row>
-    <row r="34" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:74" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -4899,8 +4982,11 @@
       <c r="BU35">
         <v>76</v>
       </c>
+      <c r="BV35">
+        <v>76</v>
+      </c>
     </row>
-    <row r="36" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -5009,8 +5095,11 @@
       <c r="BU36">
         <v>20</v>
       </c>
+      <c r="BV36">
+        <v>20</v>
+      </c>
     </row>
-    <row r="37" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5119,8 +5208,11 @@
       <c r="BU37">
         <v>55</v>
       </c>
+      <c r="BV37">
+        <v>55</v>
+      </c>
     </row>
-    <row r="38" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -5274,8 +5366,11 @@
       <c r="BU38">
         <v>88</v>
       </c>
+      <c r="BV38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -5426,8 +5521,11 @@
       <c r="BU39">
         <v>208</v>
       </c>
+      <c r="BV39">
+        <v>26</v>
+      </c>
     </row>
-    <row r="40" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -5584,8 +5682,11 @@
       <c r="BU40">
         <v>258</v>
       </c>
+      <c r="BV40">
+        <v>258</v>
+      </c>
     </row>
-    <row r="41" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -5676,16 +5777,19 @@
       <c r="BU41">
         <v>1</v>
       </c>
+      <c r="BV41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:74" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -5848,8 +5952,11 @@
       <c r="BU44">
         <v>186</v>
       </c>
+      <c r="BV44">
+        <v>186</v>
+      </c>
     </row>
-    <row r="45" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -5964,8 +6071,11 @@
       <c r="BU45">
         <v>32</v>
       </c>
+      <c r="BV45">
+        <v>30</v>
+      </c>
     </row>
-    <row r="46" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -6080,8 +6190,11 @@
       <c r="BU46">
         <v>148</v>
       </c>
+      <c r="BV46">
+        <v>150</v>
+      </c>
     </row>
-    <row r="47" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -6241,8 +6354,11 @@
       <c r="BU47">
         <v>768</v>
       </c>
+      <c r="BV47">
+        <v>791</v>
+      </c>
     </row>
-    <row r="48" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -6357,8 +6473,11 @@
       <c r="BU48">
         <v>800</v>
       </c>
+      <c r="BV48">
+        <v>821</v>
+      </c>
     </row>
-    <row r="49" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -6470,8 +6589,11 @@
       <c r="BU49">
         <v>527</v>
       </c>
+      <c r="BV49">
+        <v>509</v>
+      </c>
     </row>
-    <row r="50" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -6577,16 +6699,19 @@
       <c r="BU50">
         <v>1</v>
       </c>
+      <c r="BV50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:74" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
@@ -6734,8 +6859,11 @@
       <c r="BU53">
         <v>27</v>
       </c>
+      <c r="BV53">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -6847,8 +6975,11 @@
       <c r="BU54">
         <v>13</v>
       </c>
+      <c r="BV54">
+        <v>13</v>
+      </c>
     </row>
-    <row r="55" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -6960,8 +7091,11 @@
       <c r="BU55">
         <v>13</v>
       </c>
+      <c r="BV55">
+        <v>13</v>
+      </c>
     </row>
-    <row r="56" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -7109,8 +7243,11 @@
       <c r="BU56">
         <v>18</v>
       </c>
+      <c r="BV56">
+        <v>18</v>
+      </c>
     </row>
-    <row r="57" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -7258,8 +7395,11 @@
       <c r="BU57">
         <v>31</v>
       </c>
+      <c r="BV57">
+        <v>31</v>
+      </c>
     </row>
-    <row r="58" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -7407,8 +7547,11 @@
       <c r="BU58">
         <v>125</v>
       </c>
+      <c r="BV58">
+        <v>125</v>
+      </c>
     </row>
-    <row r="59" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -7514,8 +7657,11 @@
       <c r="BU59">
         <v>1</v>
       </c>
+      <c r="BV59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>20</v>
       </c>
@@ -7663,8 +7809,11 @@
       <c r="BU61">
         <v>10</v>
       </c>
+      <c r="BV61">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -7776,8 +7925,11 @@
       <c r="BU62">
         <v>4</v>
       </c>
+      <c r="BV62">
+        <v>4</v>
+      </c>
     </row>
-    <row r="63" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -7889,8 +8041,11 @@
       <c r="BU63">
         <v>6</v>
       </c>
+      <c r="BV63">
+        <v>6</v>
+      </c>
     </row>
-    <row r="64" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -8038,8 +8193,11 @@
       <c r="BU64">
         <v>44</v>
       </c>
+      <c r="BV64">
+        <v>44</v>
+      </c>
     </row>
-    <row r="65" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -8187,8 +8345,11 @@
       <c r="BU65">
         <v>48</v>
       </c>
+      <c r="BV65">
+        <v>48</v>
+      </c>
     </row>
-    <row r="66" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -8336,8 +8497,11 @@
       <c r="BU66">
         <v>0</v>
       </c>
+      <c r="BV66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -8449,13 +8613,16 @@
       <c r="BU67">
         <v>0</v>
       </c>
+      <c r="BV67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:74" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>22</v>
       </c>
@@ -8603,8 +8770,11 @@
       <c r="BU70">
         <v>277</v>
       </c>
+      <c r="BV70">
+        <v>283</v>
+      </c>
     </row>
-    <row r="71" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
@@ -8752,8 +8922,11 @@
       <c r="BU71">
         <v>326</v>
       </c>
+      <c r="BV71">
+        <v>312</v>
+      </c>
     </row>
-    <row r="72" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>22</v>
       </c>
@@ -8901,8 +9074,11 @@
       <c r="BU72">
         <v>312</v>
       </c>
+      <c r="BV72">
+        <v>275</v>
+      </c>
     </row>
-    <row r="73" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
@@ -9008,8 +9184,11 @@
       <c r="BU73">
         <v>15</v>
       </c>
+      <c r="BV73">
+        <v>15</v>
+      </c>
     </row>
-    <row r="75" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -9157,8 +9336,11 @@
       <c r="BU75">
         <v>102</v>
       </c>
+      <c r="BV75">
+        <v>108</v>
+      </c>
     </row>
-    <row r="76" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -9306,8 +9488,11 @@
       <c r="BU76">
         <v>11</v>
       </c>
+      <c r="BV76">
+        <v>13</v>
+      </c>
     </row>
-    <row r="77" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -9455,8 +9640,11 @@
       <c r="BU77">
         <v>113</v>
       </c>
+      <c r="BV77">
+        <v>121</v>
+      </c>
     </row>
-    <row r="78" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -9604,8 +9792,11 @@
       <c r="BU78">
         <v>163</v>
       </c>
+      <c r="BV78">
+        <v>168</v>
+      </c>
     </row>
-    <row r="79" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -9627,8 +9818,11 @@
       <c r="BU79">
         <v>1</v>
       </c>
+      <c r="BV79">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
@@ -9776,8 +9970,11 @@
       <c r="BU81">
         <v>79</v>
       </c>
+      <c r="BV81">
+        <v>79</v>
+      </c>
     </row>
-    <row r="82" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>31</v>
       </c>
@@ -9925,8 +10122,11 @@
       <c r="BU82">
         <v>56</v>
       </c>
+      <c r="BV82">
+        <v>56</v>
+      </c>
     </row>
-    <row r="83" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>31</v>
       </c>
@@ -10062,8 +10262,11 @@
       <c r="BU83">
         <v>142</v>
       </c>
+      <c r="BV83">
+        <v>142</v>
+      </c>
     </row>
-    <row r="84" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>31</v>
       </c>
@@ -10211,8 +10414,11 @@
       <c r="BU84">
         <v>5</v>
       </c>
+      <c r="BV84">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>31</v>
       </c>
@@ -10318,8 +10524,11 @@
       <c r="BU85">
         <v>13</v>
       </c>
+      <c r="BV85">
+        <v>13</v>
+      </c>
     </row>
-    <row r="87" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>81</v>
       </c>
@@ -10386,8 +10595,11 @@
       <c r="BU87">
         <v>169</v>
       </c>
+      <c r="BV87">
+        <v>169</v>
+      </c>
     </row>
-    <row r="88" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>81</v>
       </c>
@@ -10454,8 +10666,11 @@
       <c r="BU88">
         <v>40</v>
       </c>
+      <c r="BV88">
+        <v>40</v>
+      </c>
     </row>
-    <row r="89" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>81</v>
       </c>
@@ -10522,8 +10737,11 @@
       <c r="BU89">
         <v>24</v>
       </c>
+      <c r="BV89">
+        <v>24</v>
+      </c>
     </row>
-    <row r="104" spans="52:52" x14ac:dyDescent="0.25">
+    <row r="104" spans="52:52" x14ac:dyDescent="0.3">
       <c r="AZ104">
         <v>9</v>
       </c>
@@ -10535,21 +10753,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AV11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:AW11"/>
   <sheetViews>
-    <sheetView topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW4" sqref="AW4"/>
+    <sheetView topLeftCell="AR4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AW11" sqref="AW11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -10694,8 +10912,11 @@
       <c r="AV2" s="9">
         <v>43967</v>
       </c>
+      <c r="AW2" s="9">
+        <v>43968</v>
+      </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -10840,8 +11061,11 @@
       <c r="AV3">
         <v>962</v>
       </c>
+      <c r="AW3">
+        <v>985</v>
+      </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -10986,8 +11210,11 @@
       <c r="AV4">
         <v>419</v>
       </c>
+      <c r="AW4">
+        <v>426</v>
+      </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -11132,8 +11359,11 @@
       <c r="AV5">
         <v>374</v>
       </c>
+      <c r="AW5">
+        <v>377</v>
+      </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -11278,8 +11508,11 @@
       <c r="AV6">
         <v>1463</v>
       </c>
+      <c r="AW6">
+        <v>1497</v>
+      </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -11424,8 +11657,11 @@
       <c r="AV7">
         <v>1111</v>
       </c>
+      <c r="AW7">
+        <v>1133</v>
+      </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -11570,8 +11806,11 @@
       <c r="AV8">
         <v>646</v>
       </c>
+      <c r="AW8">
+        <v>652</v>
+      </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -11716,8 +11955,11 @@
       <c r="AV9">
         <v>1030</v>
       </c>
+      <c r="AW9">
+        <v>1058</v>
+      </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -11862,8 +12104,11 @@
       <c r="AV10">
         <v>1015</v>
       </c>
+      <c r="AW10">
+        <v>1040</v>
+      </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
@@ -12007,6 +12252,9 @@
       </c>
       <c r="AV11">
         <v>103</v>
+      </c>
+      <c r="AW11">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -12016,21 +12264,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AQ17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:AR17"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AJ21" sqref="AJ21"/>
+    <sheetView topLeftCell="Y10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AR17" sqref="AR17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -12158,8 +12406,11 @@
       <c r="AQ2" s="9">
         <v>43967</v>
       </c>
+      <c r="AR2" s="9">
+        <v>43968</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>38</v>
       </c>
@@ -12167,7 +12418,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>51</v>
       </c>
@@ -12297,8 +12548,11 @@
       <c r="AQ4">
         <v>7123</v>
       </c>
+      <c r="AR4">
+        <v>7270</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>36</v>
       </c>
@@ -12428,8 +12682,11 @@
       <c r="AQ5">
         <v>825</v>
       </c>
+      <c r="AR5">
+        <v>902</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -12559,8 +12816,11 @@
       <c r="AQ6">
         <v>1122</v>
       </c>
+      <c r="AR6">
+        <v>1132</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -12690,8 +12950,11 @@
       <c r="AQ7">
         <v>3366</v>
       </c>
+      <c r="AR7">
+        <v>3412</v>
+      </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -12821,8 +13084,11 @@
       <c r="AQ8">
         <v>96</v>
       </c>
+      <c r="AR8">
+        <v>97</v>
+      </c>
     </row>
-    <row r="9" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -12952,8 +13218,11 @@
       <c r="AQ9">
         <v>19</v>
       </c>
+      <c r="AR9">
+        <v>20</v>
+      </c>
     </row>
-    <row r="10" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -13079,8 +13348,11 @@
       <c r="AQ10">
         <v>16</v>
       </c>
+      <c r="AR10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -13210,8 +13482,11 @@
       <c r="AQ11">
         <v>1637</v>
       </c>
+      <c r="AR11">
+        <v>1649</v>
+      </c>
     </row>
-    <row r="12" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -13341,8 +13616,11 @@
       <c r="AQ12">
         <v>42</v>
       </c>
+      <c r="AR12">
+        <v>42</v>
+      </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -13353,7 +13631,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
@@ -13483,8 +13761,11 @@
       <c r="AQ14">
         <v>1346</v>
       </c>
+      <c r="AR14">
+        <v>1423</v>
+      </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -13614,8 +13895,11 @@
       <c r="AQ15">
         <v>1700</v>
       </c>
+      <c r="AR15">
+        <v>1728</v>
+      </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -13745,8 +14029,11 @@
       <c r="AQ16">
         <v>4054</v>
       </c>
+      <c r="AR16">
+        <v>4096</v>
+      </c>
     </row>
-    <row r="17" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -13874,6 +14161,9 @@
         <v>23</v>
       </c>
       <c r="AQ17">
+        <v>23</v>
+      </c>
+      <c r="AR17">
         <v>23</v>
       </c>
     </row>
@@ -13884,20 +14174,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AR8"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1:AQ8"/>
+      <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -14024,20 +14314,23 @@
       <c r="AQ1" s="9">
         <v>43967</v>
       </c>
+      <c r="AR1" s="9">
+        <v>43968</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B3">
         <f ca="1">SUM(B3:B8)</f>
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="C3">
         <v>22</v>
@@ -14162,8 +14455,11 @@
       <c r="AQ3">
         <v>383</v>
       </c>
+      <c r="AR3">
+        <v>392</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -14293,8 +14589,11 @@
       <c r="AQ4">
         <v>7</v>
       </c>
+      <c r="AR4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -14424,8 +14723,11 @@
       <c r="AQ5">
         <v>294</v>
       </c>
+      <c r="AR5">
+        <v>301</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -14555,8 +14857,11 @@
       <c r="AQ6">
         <v>37</v>
       </c>
+      <c r="AR6">
+        <v>38</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -14686,8 +14991,11 @@
       <c r="AQ7">
         <v>43</v>
       </c>
+      <c r="AR7">
+        <v>44</v>
+      </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -14815,6 +15123,9 @@
         <v>2</v>
       </c>
       <c r="AQ8">
+        <v>2</v>
+      </c>
+      <c r="AR8">
         <v>2</v>
       </c>
     </row>
@@ -14824,19 +15135,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A2:AD13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1:AD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -14924,8 +15235,11 @@
       <c r="AC2" s="9">
         <v>43967</v>
       </c>
+      <c r="AD2" s="9">
+        <v>43968</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -15013,8 +15327,11 @@
       <c r="AC3">
         <v>383</v>
       </c>
+      <c r="AD3">
+        <v>392</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -15102,8 +15419,11 @@
       <c r="AC4">
         <v>35</v>
       </c>
+      <c r="AD4">
+        <v>36</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -15191,8 +15511,11 @@
       <c r="AC5">
         <v>23</v>
       </c>
+      <c r="AD5">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -15280,8 +15603,11 @@
       <c r="AC6">
         <v>25</v>
       </c>
+      <c r="AD6">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -15369,8 +15695,11 @@
       <c r="AC7">
         <v>50</v>
       </c>
+      <c r="AD7">
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -15458,8 +15787,11 @@
       <c r="AC8">
         <v>60</v>
       </c>
+      <c r="AD8">
+        <v>62</v>
+      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -15547,8 +15879,11 @@
       <c r="AC9">
         <v>40</v>
       </c>
+      <c r="AD9">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -15636,8 +15971,11 @@
       <c r="AC10">
         <v>51</v>
       </c>
+      <c r="AD10">
+        <v>54</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -15725,8 +16063,11 @@
       <c r="AC11">
         <v>84</v>
       </c>
+      <c r="AD11">
+        <v>84</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -15814,8 +16155,11 @@
       <c r="AC12">
         <v>15</v>
       </c>
+      <c r="AD12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -15901,6 +16245,9 @@
         <v>0</v>
       </c>
       <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
         <v>0</v>
       </c>
     </row>
@@ -15910,63 +16257,63 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+    <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
-    <row r="2" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
         <v>87</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="G2" s="30" t="s">
-        <v>144</v>
+      <c r="G2" s="31" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
+    <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34"/>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
-      <c r="D3" s="40"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="26" t="s">
         <v>94</v>
       </c>
@@ -15977,11 +16324,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34"/>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
-      <c r="D4" s="40"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="26" t="s">
         <v>88</v>
       </c>
@@ -15990,520 +16337,525 @@
       </c>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34"/>
       <c r="B5" s="26"/>
       <c r="C5" s="27"/>
-      <c r="D5" s="40"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="26" t="s">
         <v>89</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
       <c r="B6" s="26"/>
       <c r="C6" s="27"/>
-      <c r="D6" s="40"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="26" t="s">
         <v>90</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34"/>
       <c r="B7" s="26"/>
       <c r="C7" s="27"/>
-      <c r="D7" s="40"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="26" t="s">
         <v>95</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="32">
-        <v>0</v>
-      </c>
-      <c r="D8" s="32">
-        <v>0</v>
-      </c>
-      <c r="E8" s="33" t="s">
+      <c r="C8" s="29">
+        <v>0</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0</v>
+      </c>
+      <c r="E8" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="32">
-        <v>0</v>
-      </c>
-      <c r="G8" s="32">
+      <c r="F8" s="29">
+        <v>0</v>
+      </c>
+      <c r="G8" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="29">
+        <v>4</v>
+      </c>
+      <c r="D9" s="29">
+        <v>0</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="29">
+        <v>4</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="29">
+        <v>0</v>
+      </c>
+      <c r="G10" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="29">
+        <v>10</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="29">
+        <v>0</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="29">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="29">
+        <v>0</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C13" s="29">
+        <v>3</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="29">
+        <v>12</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="29">
+        <v>1</v>
+      </c>
+      <c r="G14" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="29">
         <v>4</v>
       </c>
-      <c r="D9" s="32">
-        <v>0</v>
-      </c>
-      <c r="E9" s="33" t="s">
+      <c r="D15" s="29">
+        <v>0</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="29">
+        <v>8</v>
+      </c>
+      <c r="D16" s="29">
+        <v>0</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="29">
+        <v>1</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="29">
+        <v>9</v>
+      </c>
+      <c r="D17" s="29">
+        <v>0</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" s="29">
+        <v>0</v>
+      </c>
+      <c r="G17" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="29">
+        <v>8</v>
+      </c>
+      <c r="D18" s="29">
+        <v>0</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="29">
+        <v>0</v>
+      </c>
+      <c r="G18" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="29">
+        <v>0</v>
+      </c>
+      <c r="D19" s="29">
+        <v>0</v>
+      </c>
+      <c r="E19" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="32">
-        <v>0</v>
-      </c>
-      <c r="G9" s="32">
+      <c r="F19" s="29">
+        <v>0</v>
+      </c>
+      <c r="G19" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="32">
-        <v>4</v>
-      </c>
-      <c r="D10" s="32">
-        <v>0</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" s="32">
-        <v>0</v>
-      </c>
-      <c r="G10" s="32">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="29">
+        <v>15</v>
+      </c>
+      <c r="D20" s="29">
+        <v>0</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="29">
+        <v>0</v>
+      </c>
+      <c r="G20" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="32" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="29">
+        <v>1</v>
+      </c>
+      <c r="D21" s="29">
+        <v>0</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="29">
+        <v>0</v>
+      </c>
+      <c r="G21" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="32">
-        <v>10</v>
-      </c>
-      <c r="D11" s="32">
-        <v>0</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="F11" s="32">
-        <v>0</v>
-      </c>
-      <c r="G11" s="32">
+      <c r="C22" s="29">
+        <v>21</v>
+      </c>
+      <c r="D22" s="29">
+        <v>0</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="29">
+        <v>0</v>
+      </c>
+      <c r="G22" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="32">
-        <v>0</v>
-      </c>
-      <c r="D12" s="32">
-        <v>0</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="32">
-        <v>0</v>
-      </c>
-      <c r="G12" s="32">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="29">
+        <v>6</v>
+      </c>
+      <c r="D23" s="29">
+        <v>0</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="29">
+        <v>0</v>
+      </c>
+      <c r="G23" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" s="32">
-        <v>3</v>
-      </c>
-      <c r="D13" s="32">
-        <v>0</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="32">
-        <v>0</v>
-      </c>
-      <c r="G13" s="32">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="29">
+        <v>7</v>
+      </c>
+      <c r="D24" s="29">
+        <v>0</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="29">
+        <v>0</v>
+      </c>
+      <c r="G24" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" s="32">
-        <v>12</v>
-      </c>
-      <c r="D14" s="32">
-        <v>0</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="F14" s="32">
-        <v>1</v>
-      </c>
-      <c r="G14" s="32">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="29">
+        <v>18</v>
+      </c>
+      <c r="D25" s="29">
+        <v>0</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="29">
+        <v>1</v>
+      </c>
+      <c r="G25" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="32">
-        <v>4</v>
-      </c>
-      <c r="D15" s="32">
-        <v>0</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" s="32">
-        <v>0</v>
-      </c>
-      <c r="G15" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="32">
-        <v>7</v>
-      </c>
-      <c r="D16" s="32">
-        <v>0</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="F16" s="32">
-        <v>1</v>
-      </c>
-      <c r="G16" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="32">
-        <v>9</v>
-      </c>
-      <c r="D17" s="32">
-        <v>0</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="F17" s="32">
-        <v>0</v>
-      </c>
-      <c r="G17" s="32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="32">
-        <v>8</v>
-      </c>
-      <c r="D18" s="32">
-        <v>0</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="32">
-        <v>0</v>
-      </c>
-      <c r="G18" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="32">
-        <v>0</v>
-      </c>
-      <c r="D19" s="32">
-        <v>0</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="32">
-        <v>0</v>
-      </c>
-      <c r="G19" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="32">
-        <v>15</v>
-      </c>
-      <c r="D20" s="32">
-        <v>0</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="32">
-        <v>0</v>
-      </c>
-      <c r="G20" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="32">
-        <v>1</v>
-      </c>
-      <c r="D21" s="32">
-        <v>0</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="32">
-        <v>0</v>
-      </c>
-      <c r="G21" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="32">
-        <v>21</v>
-      </c>
-      <c r="D22" s="32">
-        <v>0</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" s="32">
-        <v>0</v>
-      </c>
-      <c r="G22" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="32">
-        <v>6</v>
-      </c>
-      <c r="D23" s="32">
-        <v>0</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="32">
-        <v>0</v>
-      </c>
-      <c r="G23" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" s="32">
-        <v>7</v>
-      </c>
-      <c r="D24" s="32">
-        <v>0</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24" s="32">
-        <v>0</v>
-      </c>
-      <c r="G24" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="C25" s="32">
-        <v>17</v>
-      </c>
-      <c r="D25" s="32">
-        <v>0</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" s="32">
-        <v>1</v>
-      </c>
-      <c r="G25" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" s="32">
-        <v>128</v>
-      </c>
-      <c r="D26" s="32">
-        <v>0</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="F26" s="32">
+      <c r="B26" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="29">
+        <v>130</v>
+      </c>
+      <c r="D26" s="29">
+        <v>0</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" s="29">
         <v>3</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="29">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>130</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
+        <v>153</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-    </row>
-    <row r="30" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="36"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A30:E30"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="D2:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -16706,22 +17058,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16738,29 +17100,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
20 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="8_{A5B6B11A-29FC-4452-9C12-302E5F9EB695}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BD81FD7F-C637-4113-9984-4F21718C6B50}"/>
+  <xr:revisionPtr revIDLastSave="333" documentId="8_{A5B6B11A-29FC-4452-9C12-302E5F9EB695}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{DBB51F8B-303D-46DC-8565-9A64FA67AADE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="156" windowWidth="22836" windowHeight="6948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,9 +485,6 @@
     <t>156; (65)</t>
   </si>
   <si>
-    <t>As of May 18, 2020</t>
-  </si>
-  <si>
     <t>54; (46)</t>
   </si>
   <si>
@@ -501,6 +498,9 @@
   </si>
   <si>
     <t>709; (337)</t>
+  </si>
+  <si>
+    <t>As of May 19, 2020</t>
   </si>
 </sst>
 </file>
@@ -1082,11 +1082,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BW104"/>
+  <dimension ref="A1:BX104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="106" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BW1" sqref="BW1:BW1048576"/>
+      <pane xSplit="2" topLeftCell="BQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BX1" sqref="BX1:BX1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,9 +1097,10 @@
     <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1319,8 +1320,11 @@
       <c r="BW1" s="1">
         <v>43969</v>
       </c>
+      <c r="BX1" s="1">
+        <v>43970</v>
+      </c>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1348,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1549,8 +1553,11 @@
       <c r="BW3">
         <v>39374</v>
       </c>
+      <c r="BX3">
+        <v>40419</v>
+      </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1776,8 +1783,11 @@
       <c r="BW4">
         <v>7434</v>
       </c>
+      <c r="BX4">
+        <v>7551</v>
+      </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1985,8 +1995,11 @@
       <c r="BW5">
         <v>400</v>
       </c>
+      <c r="BX5">
+        <v>407</v>
+      </c>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2164,11 +2177,14 @@
       <c r="BW6">
         <v>1040</v>
       </c>
+      <c r="BX6">
+        <v>1059</v>
+      </c>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -2238,8 +2254,11 @@
       <c r="BW8">
         <v>345</v>
       </c>
+      <c r="BX8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2411,8 +2430,11 @@
       <c r="BW9">
         <v>74</v>
       </c>
+      <c r="BX9">
+        <v>102</v>
+      </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2584,8 +2606,11 @@
       <c r="BW10">
         <v>440</v>
       </c>
+      <c r="BX10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2757,8 +2782,11 @@
       <c r="BW11">
         <v>232</v>
       </c>
+      <c r="BX11">
+        <v>219</v>
+      </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -2930,8 +2958,11 @@
       <c r="BW12">
         <v>208</v>
       </c>
+      <c r="BX12">
+        <v>221</v>
+      </c>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -2965,8 +2996,11 @@
       <c r="BW13">
         <v>375</v>
       </c>
+      <c r="BX13">
+        <v>336</v>
+      </c>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3000,8 +3034,11 @@
       <c r="BW14">
         <v>1803</v>
       </c>
+      <c r="BX14">
+        <v>1820</v>
+      </c>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3035,13 +3072,16 @@
       <c r="BW15" s="23">
         <v>0.72</v>
       </c>
+      <c r="BX15" s="23">
+        <v>0.73</v>
+      </c>
     </row>
-    <row r="17" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:76" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -3049,7 +3089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3224,8 +3264,11 @@
       <c r="BW19">
         <v>105</v>
       </c>
+      <c r="BX19">
+        <v>105</v>
+      </c>
     </row>
-    <row r="20" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3346,8 +3389,11 @@
       <c r="BW20">
         <v>25</v>
       </c>
+      <c r="BX20">
+        <v>25</v>
+      </c>
     </row>
-    <row r="21" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3468,8 +3514,11 @@
       <c r="BW21">
         <v>80</v>
       </c>
+      <c r="BX21">
+        <v>80</v>
+      </c>
     </row>
-    <row r="22" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3635,8 +3684,11 @@
       <c r="BW22">
         <v>84</v>
       </c>
+      <c r="BX22">
+        <v>80</v>
+      </c>
     </row>
-    <row r="23" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3802,8 +3854,11 @@
       <c r="BW23">
         <v>109</v>
       </c>
+      <c r="BX23">
+        <v>105</v>
+      </c>
     </row>
-    <row r="24" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3969,13 +4024,16 @@
       <c r="BW24">
         <v>1175</v>
       </c>
+      <c r="BX24">
+        <v>1204</v>
+      </c>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:76" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -4150,8 +4208,11 @@
       <c r="BW27">
         <v>120</v>
       </c>
+      <c r="BX27">
+        <v>121</v>
+      </c>
     </row>
-    <row r="28" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -4272,8 +4333,11 @@
       <c r="BW28">
         <v>38</v>
       </c>
+      <c r="BX28">
+        <v>39</v>
+      </c>
     </row>
-    <row r="29" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4394,8 +4458,11 @@
       <c r="BW29">
         <v>82</v>
       </c>
+      <c r="BX29">
+        <v>82</v>
+      </c>
     </row>
-    <row r="30" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4561,8 +4628,11 @@
       <c r="BW30">
         <v>47</v>
       </c>
+      <c r="BX30">
+        <v>46</v>
+      </c>
     </row>
-    <row r="31" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4728,8 +4798,11 @@
       <c r="BW31">
         <v>85</v>
       </c>
+      <c r="BX31">
+        <v>85</v>
+      </c>
     </row>
-    <row r="32" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4895,13 +4968,16 @@
       <c r="BW32">
         <v>1082</v>
       </c>
+      <c r="BX32">
+        <v>1097</v>
+      </c>
     </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:76" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -5064,8 +5140,11 @@
       <c r="BW35">
         <v>76</v>
       </c>
+      <c r="BX35">
+        <v>78</v>
+      </c>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -5180,8 +5259,11 @@
       <c r="BW36">
         <v>20</v>
       </c>
+      <c r="BX36">
+        <v>20</v>
+      </c>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5296,8 +5378,11 @@
       <c r="BW37">
         <v>55</v>
       </c>
+      <c r="BX37">
+        <v>57</v>
+      </c>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -5457,8 +5542,11 @@
       <c r="BW38">
         <v>5</v>
       </c>
+      <c r="BX38">
+        <v>5</v>
+      </c>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -5615,8 +5703,11 @@
       <c r="BW39">
         <v>25</v>
       </c>
+      <c r="BX39">
+        <v>25</v>
+      </c>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -5779,8 +5870,11 @@
       <c r="BW40">
         <v>259</v>
       </c>
+      <c r="BX40">
+        <v>261</v>
+      </c>
     </row>
-    <row r="41" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -5877,16 +5971,19 @@
       <c r="BW41">
         <v>1</v>
       </c>
+      <c r="BX41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:76" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -6055,8 +6152,11 @@
       <c r="BW44">
         <v>186</v>
       </c>
+      <c r="BX44">
+        <v>187</v>
+      </c>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -6177,8 +6277,11 @@
       <c r="BW45">
         <v>30</v>
       </c>
+      <c r="BX45">
+        <v>16</v>
+      </c>
     </row>
-    <row r="46" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -6299,8 +6402,11 @@
       <c r="BW46">
         <v>150</v>
       </c>
+      <c r="BX46">
+        <v>165</v>
+      </c>
     </row>
-    <row r="47" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -6466,8 +6572,11 @@
       <c r="BW47">
         <v>802</v>
       </c>
+      <c r="BX47">
+        <v>587</v>
+      </c>
     </row>
-    <row r="48" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -6588,8 +6697,11 @@
       <c r="BW48">
         <v>832</v>
       </c>
+      <c r="BX48">
+        <v>603</v>
+      </c>
     </row>
-    <row r="49" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -6707,8 +6819,11 @@
       <c r="BW49">
         <v>498</v>
       </c>
+      <c r="BX49">
+        <v>729</v>
+      </c>
     </row>
-    <row r="50" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -6820,16 +6935,19 @@
       <c r="BW50">
         <v>1</v>
       </c>
+      <c r="BX50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:76" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
@@ -6983,8 +7101,11 @@
       <c r="BW53">
         <v>27</v>
       </c>
+      <c r="BX53">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -7102,8 +7223,11 @@
       <c r="BW54">
         <v>11</v>
       </c>
+      <c r="BX54">
+        <v>12</v>
+      </c>
     </row>
-    <row r="55" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -7221,8 +7345,11 @@
       <c r="BW55">
         <v>15</v>
       </c>
+      <c r="BX55">
+        <v>15</v>
+      </c>
     </row>
-    <row r="56" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -7376,8 +7503,11 @@
       <c r="BW56">
         <v>16</v>
       </c>
+      <c r="BX56">
+        <v>16</v>
+      </c>
     </row>
-    <row r="57" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -7531,8 +7661,11 @@
       <c r="BW57">
         <v>27</v>
       </c>
+      <c r="BX57">
+        <v>28</v>
+      </c>
     </row>
-    <row r="58" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -7686,8 +7819,11 @@
       <c r="BW58">
         <v>130</v>
       </c>
+      <c r="BX58">
+        <v>130</v>
+      </c>
     </row>
-    <row r="59" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -7799,8 +7935,11 @@
       <c r="BW59">
         <v>1</v>
       </c>
+      <c r="BX59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>20</v>
       </c>
@@ -7954,8 +8093,11 @@
       <c r="BW61">
         <v>10</v>
       </c>
+      <c r="BX61">
+        <v>10</v>
+      </c>
     </row>
-    <row r="62" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -8073,8 +8215,11 @@
       <c r="BW62">
         <v>3</v>
       </c>
+      <c r="BX62">
+        <v>3</v>
+      </c>
     </row>
-    <row r="63" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -8192,8 +8337,11 @@
       <c r="BW63">
         <v>7</v>
       </c>
+      <c r="BX63">
+        <v>7</v>
+      </c>
     </row>
-    <row r="64" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -8347,8 +8495,11 @@
       <c r="BW64">
         <v>45</v>
       </c>
+      <c r="BX64">
+        <v>42</v>
+      </c>
     </row>
-    <row r="65" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -8502,8 +8653,11 @@
       <c r="BW65">
         <v>48</v>
       </c>
+      <c r="BX65">
+        <v>45</v>
+      </c>
     </row>
-    <row r="66" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -8657,8 +8811,11 @@
       <c r="BW66">
         <v>0</v>
       </c>
+      <c r="BX66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -8776,13 +8933,16 @@
       <c r="BW67">
         <v>0</v>
       </c>
+      <c r="BX67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:76" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>22</v>
       </c>
@@ -8936,8 +9096,11 @@
       <c r="BW70">
         <v>285</v>
       </c>
+      <c r="BX70">
+        <v>285</v>
+      </c>
     </row>
-    <row r="71" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
@@ -9091,8 +9254,11 @@
       <c r="BW71">
         <v>306</v>
       </c>
+      <c r="BX71">
+        <v>286</v>
+      </c>
     </row>
-    <row r="72" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>22</v>
       </c>
@@ -9246,8 +9412,11 @@
       <c r="BW72">
         <v>268</v>
       </c>
+      <c r="BX72">
+        <v>241</v>
+      </c>
     </row>
-    <row r="73" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
@@ -9359,8 +9528,11 @@
       <c r="BW73">
         <v>15</v>
       </c>
+      <c r="BX73">
+        <v>15</v>
+      </c>
     </row>
-    <row r="75" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -9514,8 +9686,11 @@
       <c r="BW75">
         <v>108</v>
       </c>
+      <c r="BX75">
+        <v>108</v>
+      </c>
     </row>
-    <row r="76" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -9669,8 +9844,11 @@
       <c r="BW76">
         <v>11</v>
       </c>
+      <c r="BX76">
+        <v>8</v>
+      </c>
     </row>
-    <row r="77" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -9824,8 +10002,11 @@
       <c r="BW77">
         <v>108</v>
       </c>
+      <c r="BX77">
+        <v>116</v>
+      </c>
     </row>
-    <row r="78" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -9979,8 +10160,11 @@
       <c r="BW78">
         <v>170</v>
       </c>
+      <c r="BX78">
+        <v>176</v>
+      </c>
     </row>
-    <row r="79" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -10008,8 +10192,11 @@
       <c r="BW79">
         <v>1</v>
       </c>
+      <c r="BX79">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
@@ -10163,8 +10350,11 @@
       <c r="BW81">
         <v>79</v>
       </c>
+      <c r="BX81">
+        <v>79</v>
+      </c>
     </row>
-    <row r="82" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>31</v>
       </c>
@@ -10318,8 +10508,11 @@
       <c r="BW82">
         <v>56</v>
       </c>
+      <c r="BX82">
+        <v>56</v>
+      </c>
     </row>
-    <row r="83" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>31</v>
       </c>
@@ -10461,8 +10654,11 @@
       <c r="BW83">
         <v>142</v>
       </c>
+      <c r="BX83">
+        <v>142</v>
+      </c>
     </row>
-    <row r="84" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>31</v>
       </c>
@@ -10616,8 +10812,11 @@
       <c r="BW84">
         <v>5</v>
       </c>
+      <c r="BX84">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>31</v>
       </c>
@@ -10729,8 +10928,11 @@
       <c r="BW85">
         <v>13</v>
       </c>
+      <c r="BX85">
+        <v>13</v>
+      </c>
     </row>
-    <row r="87" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>81</v>
       </c>
@@ -10803,8 +11005,11 @@
       <c r="BW87">
         <v>172</v>
       </c>
+      <c r="BX87">
+        <v>175</v>
+      </c>
     </row>
-    <row r="88" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>81</v>
       </c>
@@ -10877,8 +11082,11 @@
       <c r="BW88">
         <v>40</v>
       </c>
+      <c r="BX88">
+        <v>40</v>
+      </c>
     </row>
-    <row r="89" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>81</v>
       </c>
@@ -10950,6 +11158,9 @@
       </c>
       <c r="BW89">
         <v>24</v>
+      </c>
+      <c r="BX89">
+        <v>25</v>
       </c>
     </row>
     <row r="104" spans="52:52" x14ac:dyDescent="0.3">
@@ -10965,10 +11176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:AX11"/>
+  <dimension ref="A2:AY11"/>
   <sheetViews>
-    <sheetView topLeftCell="AR8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX11" sqref="AX11"/>
+    <sheetView topLeftCell="AT3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AY11" sqref="AY11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10978,7 +11189,7 @@
     <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -11129,8 +11340,11 @@
       <c r="AX2" s="9">
         <v>43969</v>
       </c>
+      <c r="AY2" s="9">
+        <v>43970</v>
+      </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -11281,8 +11495,11 @@
       <c r="AX3">
         <v>1023</v>
       </c>
+      <c r="AY3">
+        <v>1032</v>
+      </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -11433,8 +11650,11 @@
       <c r="AX4">
         <v>439</v>
       </c>
+      <c r="AY4">
+        <v>442</v>
+      </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -11585,8 +11805,11 @@
       <c r="AX5">
         <v>380</v>
       </c>
+      <c r="AY5">
+        <v>382</v>
+      </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -11737,8 +11960,11 @@
       <c r="AX6">
         <v>1528</v>
       </c>
+      <c r="AY6">
+        <v>1569</v>
+      </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -11889,8 +12115,11 @@
       <c r="AX7">
         <v>1157</v>
       </c>
+      <c r="AY7">
+        <v>1177</v>
+      </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -12041,8 +12270,11 @@
       <c r="AX8">
         <v>657</v>
       </c>
+      <c r="AY8">
+        <v>662</v>
+      </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -12193,8 +12425,11 @@
       <c r="AX9">
         <v>1080</v>
       </c>
+      <c r="AY9">
+        <v>1091</v>
+      </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -12345,8 +12580,11 @@
       <c r="AX10">
         <v>1054</v>
       </c>
+      <c r="AY10">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
@@ -12496,6 +12734,9 @@
       </c>
       <c r="AX11">
         <v>116</v>
+      </c>
+      <c r="AY11">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -12506,10 +12747,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:AS17"/>
+  <dimension ref="A2:AT17"/>
   <sheetViews>
-    <sheetView topLeftCell="X11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AS17" sqref="AS17"/>
+    <sheetView topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AT17" sqref="AT17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12519,7 +12760,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -12653,8 +12894,11 @@
       <c r="AS2" s="9">
         <v>43969</v>
       </c>
+      <c r="AT2" s="9">
+        <v>43970</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>38</v>
       </c>
@@ -12662,7 +12906,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>51</v>
       </c>
@@ -12798,8 +13042,11 @@
       <c r="AS4">
         <v>7434</v>
       </c>
+      <c r="AT4">
+        <v>7551</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>36</v>
       </c>
@@ -12935,8 +13182,11 @@
       <c r="AS5">
         <v>964</v>
       </c>
+      <c r="AT5">
+        <v>950</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -13072,8 +13322,11 @@
       <c r="AS6">
         <v>1145</v>
       </c>
+      <c r="AT6">
+        <v>1158</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -13209,8 +13462,11 @@
       <c r="AS7">
         <v>3470</v>
       </c>
+      <c r="AT7">
+        <v>3521</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -13346,8 +13602,11 @@
       <c r="AS8">
         <v>97</v>
       </c>
+      <c r="AT8">
+        <v>97</v>
+      </c>
     </row>
-    <row r="9" spans="1:45" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -13483,8 +13742,11 @@
       <c r="AS9">
         <v>19</v>
       </c>
+      <c r="AT9">
+        <v>20</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -13616,8 +13878,11 @@
       <c r="AS10">
         <v>16</v>
       </c>
+      <c r="AT10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -13753,8 +14018,11 @@
       <c r="AS11">
         <v>1681</v>
       </c>
+      <c r="AT11">
+        <v>1747</v>
+      </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -13890,8 +14158,11 @@
       <c r="AS12">
         <v>42</v>
       </c>
+      <c r="AT12">
+        <v>42</v>
+      </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -13902,7 +14173,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
@@ -14038,8 +14309,11 @@
       <c r="AS14">
         <v>1495</v>
       </c>
+      <c r="AT14">
+        <v>1497</v>
+      </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -14175,8 +14449,11 @@
       <c r="AS15">
         <v>1758</v>
       </c>
+      <c r="AT15">
+        <v>1812</v>
+      </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -14312,8 +14589,11 @@
       <c r="AS16">
         <v>4158</v>
       </c>
+      <c r="AT16">
+        <v>4218</v>
+      </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -14448,6 +14728,9 @@
       </c>
       <c r="AS17">
         <v>23</v>
+      </c>
+      <c r="AT17">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -14458,10 +14741,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AS8"/>
+  <dimension ref="A1:AT8"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AS8" sqref="AS8"/>
+      <selection activeCell="AT8" sqref="AT8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14470,7 +14753,7 @@
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -14603,14 +14886,17 @@
       <c r="AS1" s="9">
         <v>43969</v>
       </c>
+      <c r="AT1" s="9">
+        <v>43970</v>
+      </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
@@ -14747,8 +15033,11 @@
       <c r="AS3">
         <v>400</v>
       </c>
+      <c r="AT3">
+        <v>407</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -14884,8 +15173,11 @@
       <c r="AS4">
         <v>7</v>
       </c>
+      <c r="AT4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -15021,8 +15313,11 @@
       <c r="AS5">
         <v>309</v>
       </c>
+      <c r="AT5">
+        <v>313</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -15158,8 +15453,11 @@
       <c r="AS6">
         <v>38</v>
       </c>
+      <c r="AT6">
+        <v>41</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -15295,8 +15593,11 @@
       <c r="AS7">
         <v>44</v>
       </c>
+      <c r="AT7">
+        <v>44</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -15430,6 +15731,9 @@
         <v>2</v>
       </c>
       <c r="AS8">
+        <v>2</v>
+      </c>
+      <c r="AT8">
         <v>2</v>
       </c>
     </row>
@@ -15440,10 +15744,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AE13"/>
+  <dimension ref="A2:AF13"/>
   <sheetViews>
-    <sheetView topLeftCell="M10" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView topLeftCell="M4" workbookViewId="0">
+      <selection activeCell="AF4" sqref="AF3:AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15451,7 +15755,7 @@
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -15545,8 +15849,11 @@
       <c r="AE2" s="9">
         <v>43969</v>
       </c>
+      <c r="AF2" s="9">
+        <v>43970</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -15640,8 +15947,11 @@
       <c r="AE3">
         <v>400</v>
       </c>
+      <c r="AF3">
+        <v>407</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -15735,8 +16045,11 @@
       <c r="AE4">
         <v>36</v>
       </c>
+      <c r="AF4">
+        <v>36</v>
+      </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -15830,8 +16143,11 @@
       <c r="AE5">
         <v>25</v>
       </c>
+      <c r="AF5">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -15925,8 +16241,11 @@
       <c r="AE6">
         <v>25</v>
       </c>
+      <c r="AF6">
+        <v>26</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -16020,8 +16339,11 @@
       <c r="AE7">
         <v>54</v>
       </c>
+      <c r="AF7">
+        <v>57</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -16115,8 +16437,11 @@
       <c r="AE8">
         <v>63</v>
       </c>
+      <c r="AF8">
+        <v>63</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -16210,8 +16535,11 @@
       <c r="AE9">
         <v>40</v>
       </c>
+      <c r="AF9">
+        <v>41</v>
+      </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -16305,8 +16633,11 @@
       <c r="AE10">
         <v>56</v>
       </c>
+      <c r="AF10">
+        <v>57</v>
+      </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -16400,8 +16731,11 @@
       <c r="AE11">
         <v>86</v>
       </c>
+      <c r="AF11">
+        <v>87</v>
+      </c>
     </row>
-    <row r="12" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -16495,8 +16829,11 @@
       <c r="AE12">
         <v>15</v>
       </c>
+      <c r="AF12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -16588,6 +16925,9 @@
         <v>0</v>
       </c>
       <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
         <v>0</v>
       </c>
     </row>
@@ -16600,8 +16940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16617,7 +16957,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -16784,7 +17124,7 @@
         <v>104</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="29">
         <v>12</v>
@@ -16853,7 +17193,7 @@
         <v>109</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C14" s="29">
         <v>13</v>
@@ -16922,7 +17262,7 @@
         <v>115</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" s="29">
         <v>10</v>
@@ -17129,7 +17469,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C26" s="29">
         <v>136</v>
@@ -17152,7 +17492,7 @@
         <v>129</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
@@ -17181,6 +17521,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -17383,22 +17738,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17415,29 +17780,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
22 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="683" documentId="8_{A5B6B11A-29FC-4452-9C12-302E5F9EB695}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B5CEB2D6-C59C-439D-B0F8-7AFA526757C5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="20730" windowHeight="6945" tabRatio="818"/>
+    <workbookView xWindow="0" yWindow="156" windowWidth="23112" windowHeight="7296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -12,10 +18,10 @@
     <sheet name="Total Cases by Race" sheetId="3" r:id="rId3"/>
     <sheet name="Lives Lost by Race" sheetId="4" r:id="rId4"/>
     <sheet name="Lives Lost by Ward" sheetId="5" r:id="rId5"/>
-    <sheet name="Community Cases Tested by OCME" sheetId="7" r:id="rId6"/>
+    <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId6"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="161">
   <si>
     <t>Testing</t>
   </si>
@@ -336,9 +342,6 @@
     <t>Carroll Manor (Bed Capacity: 240)</t>
   </si>
   <si>
-    <t>10; (3)</t>
-  </si>
-  <si>
     <t>Deanwood (Bed Capacity: 296)</t>
   </si>
   <si>
@@ -357,9 +360,6 @@
     <t>Inspire (Bed Capacity: 180)</t>
   </si>
   <si>
-    <t>17; (14)</t>
-  </si>
-  <si>
     <t>20; (11)</t>
   </si>
   <si>
@@ -376,9 +376,6 @@
   </si>
   <si>
     <t>Serenity (Bed Capacity: 183)</t>
-  </si>
-  <si>
-    <t>20; (15)</t>
   </si>
   <si>
     <t>Stoddard Baptist (Bed Capacity: 164)</t>
@@ -462,12 +459,6 @@
     <t>10; (6)</t>
   </si>
   <si>
-    <t>156; (65)</t>
-  </si>
-  <si>
-    <t>As of May 20, 2020</t>
-  </si>
-  <si>
     <t>Public Safety - OUC -Personnel</t>
   </si>
   <si>
@@ -486,32 +477,47 @@
     <t>44; (28)</t>
   </si>
   <si>
-    <t>41; (29)</t>
-  </si>
-  <si>
     <t>46; (18)</t>
   </si>
   <si>
-    <t>580; (276)</t>
+    <t>16; (3)</t>
   </si>
   <si>
-    <t>751; (349)</t>
+    <t>26; (22)</t>
+  </si>
+  <si>
+    <t>As of May 21, 2020</t>
+  </si>
+  <si>
+    <t>45; (33)</t>
+  </si>
+  <si>
+    <t>584; (280)</t>
+  </si>
+  <si>
+    <t>756; (355)</t>
+  </si>
+  <si>
+    <t>21; (17)</t>
+  </si>
+  <si>
+    <t>172; (75)</t>
+  </si>
+  <si>
+    <t>Total Submitted for Testing</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
   </si>
   <si>
     <t>Other Jurisdiction</t>
   </si>
   <si>
-    <t>Hispanic</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Total Submitted for Testing</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">As of May 20, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of May 21, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -542,7 +548,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,13 +641,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -756,20 +762,19 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -812,7 +817,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1147,33 +1152,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BY112"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BZ112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="106" workbookViewId="0">
       <pane xSplit="2" topLeftCell="BV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="CC15" sqref="CC15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1399,8 +1404,11 @@
       <c r="BY1" s="1">
         <v>43971</v>
       </c>
+      <c r="BZ1" s="1">
+        <v>43972</v>
+      </c>
     </row>
-    <row r="2" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1432,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1635,8 +1643,11 @@
       <c r="BY3">
         <v>41756</v>
       </c>
+      <c r="BZ3">
+        <v>42993</v>
+      </c>
     </row>
-    <row r="4" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1868,8 +1879,11 @@
       <c r="BY4">
         <v>7788</v>
       </c>
+      <c r="BZ4">
+        <v>7893</v>
+      </c>
     </row>
-    <row r="5" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2083,8 +2097,11 @@
       <c r="BY5">
         <v>412</v>
       </c>
+      <c r="BZ5">
+        <v>418</v>
+      </c>
     </row>
-    <row r="6" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2268,11 +2285,14 @@
       <c r="BY6">
         <v>1061</v>
       </c>
+      <c r="BZ6">
+        <v>1069</v>
+      </c>
     </row>
-    <row r="7" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -2348,8 +2368,11 @@
       <c r="BY8">
         <v>345</v>
       </c>
+      <c r="BZ8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2527,8 +2550,11 @@
       <c r="BY9">
         <v>54</v>
       </c>
+      <c r="BZ9">
+        <v>46</v>
+      </c>
     </row>
-    <row r="10" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2706,8 +2732,11 @@
       <c r="BY10">
         <v>440</v>
       </c>
+      <c r="BZ10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2885,8 +2914,11 @@
       <c r="BY11">
         <v>221</v>
       </c>
+      <c r="BZ11">
+        <v>228</v>
+      </c>
     </row>
-    <row r="12" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3064,8 +3096,11 @@
       <c r="BY12">
         <v>219</v>
       </c>
+      <c r="BZ12">
+        <v>212</v>
+      </c>
     </row>
-    <row r="13" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3105,8 +3140,11 @@
       <c r="BY13">
         <v>342</v>
       </c>
+      <c r="BZ13">
+        <v>342</v>
+      </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3116,8 +3154,11 @@
       <c r="BY14">
         <v>110</v>
       </c>
+      <c r="BZ14">
+        <v>112</v>
+      </c>
     </row>
-    <row r="15" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3157,8 +3198,11 @@
       <c r="BY15">
         <v>1926</v>
       </c>
+      <c r="BZ15">
+        <v>1896</v>
+      </c>
     </row>
-    <row r="16" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3198,13 +3242,16 @@
       <c r="BY16" s="23">
         <v>0.77</v>
       </c>
+      <c r="BZ16" s="23">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="18" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:78" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3212,7 +3259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3393,8 +3440,11 @@
       <c r="BY20">
         <v>105</v>
       </c>
+      <c r="BZ20">
+        <v>105</v>
+      </c>
     </row>
-    <row r="21" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3521,8 +3571,11 @@
       <c r="BY21">
         <v>25</v>
       </c>
+      <c r="BZ21">
+        <v>25</v>
+      </c>
     </row>
-    <row r="22" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3649,8 +3702,11 @@
       <c r="BY22">
         <v>80</v>
       </c>
+      <c r="BZ22">
+        <v>80</v>
+      </c>
     </row>
-    <row r="23" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3822,8 +3878,11 @@
       <c r="BY23">
         <v>70</v>
       </c>
+      <c r="BZ23">
+        <v>70</v>
+      </c>
     </row>
-    <row r="24" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3995,8 +4054,11 @@
       <c r="BY24">
         <v>95</v>
       </c>
+      <c r="BZ24">
+        <v>95</v>
+      </c>
     </row>
-    <row r="25" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4168,13 +4230,16 @@
       <c r="BY25">
         <v>1222</v>
       </c>
+      <c r="BZ25">
+        <v>1237</v>
+      </c>
     </row>
-    <row r="27" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:78" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -4355,8 +4420,11 @@
       <c r="BY28">
         <v>125</v>
       </c>
+      <c r="BZ28">
+        <v>126</v>
+      </c>
     </row>
-    <row r="29" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4483,8 +4551,11 @@
       <c r="BY29">
         <v>43</v>
       </c>
+      <c r="BZ29">
+        <v>40</v>
+      </c>
     </row>
-    <row r="30" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4611,8 +4682,11 @@
       <c r="BY30">
         <v>82</v>
       </c>
+      <c r="BZ30">
+        <v>86</v>
+      </c>
     </row>
-    <row r="31" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4784,8 +4858,11 @@
       <c r="BY31">
         <v>57</v>
       </c>
+      <c r="BZ31">
+        <v>56</v>
+      </c>
     </row>
-    <row r="32" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -4957,8 +5034,11 @@
       <c r="BY32">
         <v>100</v>
       </c>
+      <c r="BZ32">
+        <v>96</v>
+      </c>
     </row>
-    <row r="33" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5130,13 +5210,16 @@
       <c r="BY33">
         <v>1092</v>
       </c>
+      <c r="BZ33">
+        <v>1116</v>
+      </c>
     </row>
-    <row r="35" spans="1:77" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:78" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -5305,8 +5388,11 @@
       <c r="BY36">
         <v>78</v>
       </c>
+      <c r="BZ36">
+        <v>78</v>
+      </c>
     </row>
-    <row r="37" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5427,8 +5513,11 @@
       <c r="BY37">
         <v>19</v>
       </c>
+      <c r="BZ37">
+        <v>19</v>
+      </c>
     </row>
-    <row r="38" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -5549,8 +5638,11 @@
       <c r="BY38">
         <v>58</v>
       </c>
+      <c r="BZ38">
+        <v>58</v>
+      </c>
     </row>
-    <row r="39" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -5716,8 +5808,11 @@
       <c r="BY39">
         <v>4</v>
       </c>
+      <c r="BZ39">
+        <v>4</v>
+      </c>
     </row>
-    <row r="40" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -5880,8 +5975,11 @@
       <c r="BY40">
         <v>23</v>
       </c>
+      <c r="BZ40">
+        <v>23</v>
+      </c>
     </row>
-    <row r="41" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6050,8 +6148,11 @@
       <c r="BY41">
         <v>263</v>
       </c>
+      <c r="BZ41">
+        <v>263</v>
+      </c>
     </row>
-    <row r="42" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -6154,16 +6255,19 @@
       <c r="BY42">
         <v>1</v>
       </c>
+      <c r="BZ42">
+        <v>1</v>
+      </c>
     </row>
-    <row r="43" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:78" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -6338,8 +6442,11 @@
       <c r="BY45">
         <v>187</v>
       </c>
+      <c r="BZ45">
+        <v>193</v>
+      </c>
     </row>
-    <row r="46" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -6466,8 +6573,11 @@
       <c r="BY46">
         <v>16</v>
       </c>
+      <c r="BZ46">
+        <v>21</v>
+      </c>
     </row>
-    <row r="47" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -6594,8 +6704,11 @@
       <c r="BY47">
         <v>165</v>
       </c>
+      <c r="BZ47">
+        <v>166</v>
+      </c>
     </row>
-    <row r="48" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -6767,8 +6880,11 @@
       <c r="BY48">
         <v>589</v>
       </c>
+      <c r="BZ48">
+        <v>580</v>
+      </c>
     </row>
-    <row r="49" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -6895,8 +7011,11 @@
       <c r="BY49">
         <v>605</v>
       </c>
+      <c r="BZ49">
+        <v>601</v>
+      </c>
     </row>
-    <row r="50" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -7020,8 +7139,11 @@
       <c r="BY50">
         <v>730</v>
       </c>
+      <c r="BZ50">
+        <v>732</v>
+      </c>
     </row>
-    <row r="51" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -7139,16 +7261,19 @@
       <c r="BY51">
         <v>1</v>
       </c>
+      <c r="BZ51">
+        <v>1</v>
+      </c>
     </row>
-    <row r="52" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:78" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -7308,8 +7433,11 @@
       <c r="BY54">
         <v>27</v>
       </c>
+      <c r="BZ54">
+        <v>27</v>
+      </c>
     </row>
-    <row r="55" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -7433,8 +7561,11 @@
       <c r="BY55">
         <v>10</v>
       </c>
+      <c r="BZ55">
+        <v>10</v>
+      </c>
     </row>
-    <row r="56" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -7558,8 +7689,11 @@
       <c r="BY56">
         <v>16</v>
       </c>
+      <c r="BZ56">
+        <v>16</v>
+      </c>
     </row>
-    <row r="57" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -7719,8 +7853,11 @@
       <c r="BY57">
         <v>15</v>
       </c>
+      <c r="BZ57">
+        <v>15</v>
+      </c>
     </row>
-    <row r="58" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -7880,8 +8017,11 @@
       <c r="BY58">
         <v>25</v>
       </c>
+      <c r="BZ58">
+        <v>25</v>
+      </c>
     </row>
-    <row r="59" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -8041,8 +8181,11 @@
       <c r="BY59">
         <v>132</v>
       </c>
+      <c r="BZ59">
+        <v>132</v>
+      </c>
     </row>
-    <row r="60" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -8160,8 +8303,11 @@
       <c r="BY60">
         <v>1</v>
       </c>
+      <c r="BZ60">
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -8321,8 +8467,11 @@
       <c r="BY62">
         <v>10</v>
       </c>
+      <c r="BZ62">
+        <v>11</v>
+      </c>
     </row>
-    <row r="63" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -8446,8 +8595,11 @@
       <c r="BY63">
         <v>3</v>
       </c>
+      <c r="BZ63">
+        <v>4</v>
+      </c>
     </row>
-    <row r="64" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -8571,8 +8723,11 @@
       <c r="BY64">
         <v>7</v>
       </c>
+      <c r="BZ64">
+        <v>7</v>
+      </c>
     </row>
-    <row r="65" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -8732,8 +8887,11 @@
       <c r="BY65">
         <v>43</v>
       </c>
+      <c r="BZ65">
+        <v>42</v>
+      </c>
     </row>
-    <row r="66" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -8894,8 +9052,11 @@
       <c r="BY66">
         <v>46</v>
       </c>
+      <c r="BZ66">
+        <v>46</v>
+      </c>
     </row>
-    <row r="67" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -9055,8 +9216,11 @@
       <c r="BY67">
         <v>0</v>
       </c>
+      <c r="BZ67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -9180,13 +9344,16 @@
       <c r="BY68">
         <v>0</v>
       </c>
+      <c r="BZ68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
@@ -9194,10 +9361,13 @@
       <c r="BY70">
         <v>8</v>
       </c>
+      <c r="BZ70">
+        <v>9</v>
+      </c>
     </row>
-    <row r="71" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B71" t="s">
         <v>62</v>
@@ -9205,10 +9375,13 @@
       <c r="BY71">
         <v>7</v>
       </c>
+      <c r="BZ71">
+        <v>8</v>
+      </c>
     </row>
-    <row r="72" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
@@ -9216,10 +9389,13 @@
       <c r="BY72">
         <v>1</v>
       </c>
+      <c r="BZ72">
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
@@ -9227,10 +9403,13 @@
       <c r="BY73">
         <v>15</v>
       </c>
+      <c r="BZ73">
+        <v>15</v>
+      </c>
     </row>
-    <row r="74" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
@@ -9238,10 +9417,13 @@
       <c r="BY74">
         <v>22</v>
       </c>
+      <c r="BZ74">
+        <v>23</v>
+      </c>
     </row>
-    <row r="75" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
@@ -9249,13 +9431,16 @@
       <c r="BY75">
         <v>19</v>
       </c>
+      <c r="BZ75">
+        <v>19</v>
+      </c>
     </row>
-    <row r="77" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:78" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>22</v>
       </c>
@@ -9415,8 +9600,11 @@
       <c r="BY78">
         <v>286</v>
       </c>
+      <c r="BZ78">
+        <v>286</v>
+      </c>
     </row>
-    <row r="79" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -9576,8 +9764,11 @@
       <c r="BY79">
         <v>291</v>
       </c>
+      <c r="BZ79">
+        <v>246</v>
+      </c>
     </row>
-    <row r="80" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -9737,8 +9928,11 @@
       <c r="BY80">
         <v>242</v>
       </c>
+      <c r="BZ80">
+        <v>214</v>
+      </c>
     </row>
-    <row r="81" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -9856,8 +10050,11 @@
       <c r="BY81">
         <v>15</v>
       </c>
+      <c r="BZ81">
+        <v>15</v>
+      </c>
     </row>
-    <row r="83" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>30</v>
       </c>
@@ -10017,8 +10214,11 @@
       <c r="BY83">
         <v>108</v>
       </c>
+      <c r="BZ83">
+        <v>108</v>
+      </c>
     </row>
-    <row r="84" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>30</v>
       </c>
@@ -10178,8 +10378,11 @@
       <c r="BY84">
         <v>18</v>
       </c>
+      <c r="BZ84">
+        <v>4</v>
+      </c>
     </row>
-    <row r="85" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>30</v>
       </c>
@@ -10339,8 +10542,11 @@
       <c r="BY85">
         <v>116</v>
       </c>
+      <c r="BZ85">
+        <v>112</v>
+      </c>
     </row>
-    <row r="86" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>30</v>
       </c>
@@ -10500,8 +10706,11 @@
       <c r="BY86">
         <v>176</v>
       </c>
+      <c r="BZ86">
+        <v>180</v>
+      </c>
     </row>
-    <row r="87" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>30</v>
       </c>
@@ -10535,8 +10744,11 @@
       <c r="BY87">
         <v>1</v>
       </c>
+      <c r="BZ87">
+        <v>1</v>
+      </c>
     </row>
-    <row r="89" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>31</v>
       </c>
@@ -10696,8 +10908,11 @@
       <c r="BY89">
         <v>79</v>
       </c>
+      <c r="BZ89">
+        <v>79</v>
+      </c>
     </row>
-    <row r="90" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>31</v>
       </c>
@@ -10857,8 +11072,11 @@
       <c r="BY90">
         <v>56</v>
       </c>
+      <c r="BZ90">
+        <v>56</v>
+      </c>
     </row>
-    <row r="91" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>31</v>
       </c>
@@ -11006,8 +11224,11 @@
       <c r="BY91">
         <v>142</v>
       </c>
+      <c r="BZ91">
+        <v>142</v>
+      </c>
     </row>
-    <row r="92" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>31</v>
       </c>
@@ -11167,8 +11388,11 @@
       <c r="BY92">
         <v>5</v>
       </c>
+      <c r="BZ92">
+        <v>12</v>
+      </c>
     </row>
-    <row r="93" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>31</v>
       </c>
@@ -11286,8 +11510,11 @@
       <c r="BY93">
         <v>13</v>
       </c>
+      <c r="BZ93">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>81</v>
       </c>
@@ -11366,8 +11593,11 @@
       <c r="BY95">
         <v>176</v>
       </c>
+      <c r="BZ95">
+        <v>178</v>
+      </c>
     </row>
-    <row r="96" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>81</v>
       </c>
@@ -11446,8 +11676,11 @@
       <c r="BY96">
         <v>40</v>
       </c>
+      <c r="BZ96">
+        <v>41</v>
+      </c>
     </row>
-    <row r="97" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>81</v>
       </c>
@@ -11526,8 +11759,11 @@
       <c r="BY97">
         <v>25</v>
       </c>
+      <c r="BZ97">
+        <v>25</v>
+      </c>
     </row>
-    <row r="112" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:78" x14ac:dyDescent="0.3">
       <c r="AZ112">
         <v>9</v>
       </c>
@@ -11539,21 +11775,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AZ11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:BA11"/>
   <sheetViews>
-    <sheetView topLeftCell="AT1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AZ11" sqref="AZ11"/>
+    <sheetView topLeftCell="AT2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BA11" sqref="BA11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -11710,8 +11946,11 @@
       <c r="AZ2" s="9">
         <v>43971</v>
       </c>
+      <c r="BA2" s="9">
+        <v>43972</v>
+      </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -11868,8 +12107,11 @@
       <c r="AZ3">
         <v>1071</v>
       </c>
+      <c r="BA3">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -12026,8 +12268,11 @@
       <c r="AZ4">
         <v>451</v>
       </c>
+      <c r="BA4">
+        <v>460</v>
+      </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -12184,8 +12429,11 @@
       <c r="AZ5">
         <v>385</v>
       </c>
+      <c r="BA5">
+        <v>393</v>
+      </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -12342,8 +12590,11 @@
       <c r="AZ6">
         <v>1642</v>
       </c>
+      <c r="BA6">
+        <v>1657</v>
+      </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -12500,8 +12751,11 @@
       <c r="AZ7">
         <v>1204</v>
       </c>
+      <c r="BA7">
+        <v>1225</v>
+      </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -12658,8 +12912,11 @@
       <c r="AZ8">
         <v>680</v>
       </c>
+      <c r="BA8">
+        <v>682</v>
+      </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -12816,8 +13073,11 @@
       <c r="AZ9">
         <v>1134</v>
       </c>
+      <c r="BA9">
+        <v>1147</v>
+      </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -12974,8 +13234,11 @@
       <c r="AZ10">
         <v>1101</v>
       </c>
+      <c r="BA10">
+        <v>1112</v>
+      </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
@@ -13131,6 +13394,9 @@
       </c>
       <c r="AZ11">
         <v>120</v>
+      </c>
+      <c r="BA11">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -13140,21 +13406,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AU17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:AV17"/>
   <sheetViews>
-    <sheetView topLeftCell="X5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AU17" sqref="AU17"/>
+    <sheetView topLeftCell="AE9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AV17" sqref="AV17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:47" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -13294,8 +13560,11 @@
       <c r="AU2" s="9">
         <v>43971</v>
       </c>
+      <c r="AV2" s="9">
+        <v>43972</v>
+      </c>
     </row>
-    <row r="3" spans="1:47" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>38</v>
       </c>
@@ -13303,7 +13572,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>51</v>
       </c>
@@ -13445,8 +13714,11 @@
       <c r="AU4">
         <v>7788</v>
       </c>
+      <c r="AV4">
+        <v>7893</v>
+      </c>
     </row>
-    <row r="5" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>36</v>
       </c>
@@ -13588,8 +13860,11 @@
       <c r="AU5">
         <v>1069</v>
       </c>
+      <c r="AV5">
+        <v>926</v>
+      </c>
     </row>
-    <row r="6" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -13731,8 +14006,11 @@
       <c r="AU6">
         <v>1178</v>
       </c>
+      <c r="AV6">
+        <v>1232</v>
+      </c>
     </row>
-    <row r="7" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -13874,8 +14152,11 @@
       <c r="AU7">
         <v>3570</v>
       </c>
+      <c r="AV7">
+        <v>3683</v>
+      </c>
     </row>
-    <row r="8" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
@@ -14017,8 +14298,11 @@
       <c r="AU8">
         <v>98</v>
       </c>
+      <c r="AV8">
+        <v>101</v>
+      </c>
     </row>
-    <row r="9" spans="1:47" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -14160,8 +14444,11 @@
       <c r="AU9">
         <v>21</v>
       </c>
+      <c r="AV9">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:47" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -14299,8 +14586,11 @@
       <c r="AU10">
         <v>16</v>
       </c>
+      <c r="AV10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
@@ -14442,8 +14732,11 @@
       <c r="AU11">
         <v>1794</v>
       </c>
+      <c r="AV11">
+        <v>1869</v>
+      </c>
     </row>
-    <row r="12" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -14585,8 +14878,11 @@
       <c r="AU12">
         <v>42</v>
       </c>
+      <c r="AV12">
+        <v>44</v>
+      </c>
     </row>
-    <row r="13" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -14597,7 +14893,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
@@ -14739,8 +15035,11 @@
       <c r="AU14">
         <v>1650</v>
       </c>
+      <c r="AV14">
+        <v>1447</v>
+      </c>
     </row>
-    <row r="15" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
@@ -14882,8 +15181,11 @@
       <c r="AU15">
         <v>1863</v>
       </c>
+      <c r="AV15">
+        <v>1975</v>
+      </c>
     </row>
-    <row r="16" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -15025,8 +15327,11 @@
       <c r="AU16">
         <v>4281</v>
       </c>
+      <c r="AV16">
+        <v>4447</v>
+      </c>
     </row>
-    <row r="17" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -15166,6 +15471,9 @@
         <v>24</v>
       </c>
       <c r="AU17">
+        <v>24</v>
+      </c>
+      <c r="AV17">
         <v>24</v>
       </c>
     </row>
@@ -15176,20 +15484,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AV9"/>
   <sheetViews>
-    <sheetView topLeftCell="Z3" workbookViewId="0">
-      <selection activeCell="AU9" sqref="AU9"/>
+    <sheetView topLeftCell="AK10" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -15328,14 +15636,17 @@
       <c r="AU1" s="9">
         <v>43971</v>
       </c>
+      <c r="AV1" s="9">
+        <v>43972</v>
+      </c>
     </row>
-    <row r="2" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
@@ -15478,8 +15789,11 @@
       <c r="AU3">
         <v>412</v>
       </c>
+      <c r="AV3">
+        <v>418</v>
+      </c>
     </row>
-    <row r="4" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -15621,8 +15935,11 @@
       <c r="AU4">
         <v>7</v>
       </c>
+      <c r="AV4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:47" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
@@ -15764,8 +16081,11 @@
       <c r="AU5">
         <v>316</v>
       </c>
+      <c r="AV5">
+        <v>320</v>
+      </c>
     </row>
-    <row r="6" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>48</v>
       </c>
@@ -15907,8 +16227,11 @@
       <c r="AU6">
         <v>42</v>
       </c>
+      <c r="AV6">
+        <v>42</v>
+      </c>
     </row>
-    <row r="7" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -16050,8 +16373,11 @@
       <c r="AU7">
         <v>45</v>
       </c>
+      <c r="AV7">
+        <v>46</v>
+      </c>
     </row>
-    <row r="8" spans="1:47" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>50</v>
       </c>
@@ -16191,6 +16517,17 @@
         <v>2</v>
       </c>
       <c r="AU8">
+        <v>2</v>
+      </c>
+      <c r="AV8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A9" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV9">
         <v>2</v>
       </c>
     </row>
@@ -16200,19 +16537,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AG13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A2:AH13"/>
   <sheetViews>
-    <sheetView topLeftCell="M6" workbookViewId="0">
-      <selection activeCell="AG14" sqref="AG14"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -16312,8 +16649,11 @@
       <c r="AG2" s="9">
         <v>43971</v>
       </c>
+      <c r="AH2" s="9">
+        <v>43972</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -16413,8 +16753,11 @@
       <c r="AG3">
         <v>412</v>
       </c>
+      <c r="AH3">
+        <v>418</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -16514,8 +16857,11 @@
       <c r="AG4">
         <v>37</v>
       </c>
+      <c r="AH4">
+        <v>37</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -16615,8 +16961,11 @@
       <c r="AG5">
         <v>25</v>
       </c>
+      <c r="AH5">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -16716,8 +17065,11 @@
       <c r="AG6">
         <v>27</v>
       </c>
+      <c r="AH6">
+        <v>27</v>
+      </c>
     </row>
-    <row r="7" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -16817,8 +17169,11 @@
       <c r="AG7">
         <v>57</v>
       </c>
+      <c r="AH7">
+        <v>58</v>
+      </c>
     </row>
-    <row r="8" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -16918,8 +17273,11 @@
       <c r="AG8">
         <v>64</v>
       </c>
+      <c r="AH8">
+        <v>65</v>
+      </c>
     </row>
-    <row r="9" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -17019,8 +17377,11 @@
       <c r="AG9">
         <v>41</v>
       </c>
+      <c r="AH9">
+        <v>41</v>
+      </c>
     </row>
-    <row r="10" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -17120,8 +17481,11 @@
       <c r="AG10">
         <v>59</v>
       </c>
+      <c r="AH10">
+        <v>60</v>
+      </c>
     </row>
-    <row r="11" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -17221,8 +17585,11 @@
       <c r="AG11">
         <v>87</v>
       </c>
+      <c r="AH11">
+        <v>89</v>
+      </c>
     </row>
-    <row r="12" spans="1:33" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -17322,8 +17689,11 @@
       <c r="AG12">
         <v>15</v>
       </c>
+      <c r="AH12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -17421,6 +17791,9 @@
         <v>0</v>
       </c>
       <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
         <v>0</v>
       </c>
     </row>
@@ -17430,221 +17803,268 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80E935D-0DE1-4E26-AC60-89F6B9B8891F}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="41" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C1" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
+      <c r="D5" s="9">
+        <v>43972</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="39">
+        <v>155</v>
+      </c>
+      <c r="C6">
         <v>103</v>
       </c>
+      <c r="D6">
+        <v>103</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7">
         <v>26</v>
       </c>
+      <c r="D7">
+        <v>26</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="33" t="s">
         <v>41</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10">
         <v>18</v>
       </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="33">
         <v>1</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="33">
         <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="33">
         <v>3</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="33">
         <v>4</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="33">
         <v>5</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="33">
         <v>6</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="33">
         <v>7</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="33">
         <v>8</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+    <row r="22" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="44" t="s">
         <v>73</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
         <v>1</v>
       </c>
     </row>
@@ -17657,27 +18077,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -17686,27 +18106,27 @@
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
     </row>
-    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>87</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>132</v>
-      </c>
       <c r="G2" s="31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -17724,7 +18144,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37"/>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -17737,7 +18157,7 @@
       </c>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37"/>
       <c r="B5" s="26"/>
       <c r="C5" s="27"/>
@@ -17748,7 +18168,7 @@
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37"/>
       <c r="B6" s="26"/>
       <c r="C6" s="27"/>
@@ -17759,7 +18179,7 @@
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="37"/>
       <c r="B7" s="26"/>
       <c r="C7" s="27"/>
@@ -17770,12 +18190,12 @@
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
     </row>
-    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>96</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C8" s="29">
         <v>3</v>
@@ -17786,19 +18206,19 @@
       <c r="E8" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="29">
-        <v>0</v>
-      </c>
-      <c r="G8" s="29">
+      <c r="F8" s="30">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>98</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C9" s="29">
         <v>4</v>
@@ -17809,19 +18229,19 @@
       <c r="E9" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="29">
-        <v>0</v>
-      </c>
-      <c r="G9" s="29">
+      <c r="F9" s="30">
+        <v>0</v>
+      </c>
+      <c r="G9" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C10" s="29">
         <v>4</v>
@@ -17830,21 +18250,21 @@
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="30">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="29">
-        <v>0</v>
-      </c>
-      <c r="G10" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>102</v>
-      </c>
       <c r="B11" s="29" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C11" s="29">
         <v>12</v>
@@ -17853,44 +18273,44 @@
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="F11" s="29">
-        <v>0</v>
-      </c>
-      <c r="G11" s="29">
+        <v>134</v>
+      </c>
+      <c r="F11" s="30">
+        <v>0</v>
+      </c>
+      <c r="G11" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="C12" s="29">
+        <v>0</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="29">
-        <v>0</v>
-      </c>
-      <c r="D12" s="29">
-        <v>0</v>
-      </c>
-      <c r="E12" s="30" t="s">
+      <c r="F12" s="30">
+        <v>0</v>
+      </c>
+      <c r="G12" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="F12" s="29">
-        <v>0</v>
-      </c>
-      <c r="G12" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
-        <v>106</v>
-      </c>
       <c r="B13" s="29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" s="29">
         <v>3</v>
@@ -17899,21 +18319,21 @@
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="29">
-        <v>0</v>
-      </c>
-      <c r="G13" s="29">
+        <v>103</v>
+      </c>
+      <c r="F13" s="30">
+        <v>0</v>
+      </c>
+      <c r="G13" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C14" s="29">
         <v>14</v>
@@ -17922,21 +18342,21 @@
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="29">
-        <v>1</v>
-      </c>
-      <c r="G14" s="29">
+        <v>148</v>
+      </c>
+      <c r="F14" s="30">
+        <v>1</v>
+      </c>
+      <c r="G14" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C15" s="29">
         <v>4</v>
@@ -17945,21 +18365,21 @@
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="30">
+        <v>0</v>
+      </c>
+      <c r="G15" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="29" t="s">
         <v>110</v>
-      </c>
-      <c r="F15" s="29">
-        <v>0</v>
-      </c>
-      <c r="G15" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>112</v>
       </c>
       <c r="C16" s="29">
         <v>8</v>
@@ -17968,21 +18388,21 @@
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" s="29">
-        <v>1</v>
-      </c>
-      <c r="G16" s="29">
+        <v>138</v>
+      </c>
+      <c r="F16" s="30">
+        <v>1</v>
+      </c>
+      <c r="G16" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C17" s="29">
         <v>11</v>
@@ -17991,44 +18411,44 @@
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="F17" s="29">
-        <v>0</v>
-      </c>
-      <c r="G17" s="29">
+        <v>139</v>
+      </c>
+      <c r="F17" s="30">
+        <v>0</v>
+      </c>
+      <c r="G17" s="30">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" s="29">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D18" s="29">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="29">
-        <v>0</v>
-      </c>
-      <c r="G18" s="29">
+        <v>153</v>
+      </c>
+      <c r="F18" s="30">
+        <v>0</v>
+      </c>
+      <c r="G18" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C19" s="29">
         <v>15</v>
@@ -18039,42 +18459,42 @@
       <c r="E19" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="29">
-        <v>0</v>
-      </c>
-      <c r="G19" s="29">
+      <c r="F19" s="30">
+        <v>0</v>
+      </c>
+      <c r="G19" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="29">
+        <v>1</v>
+      </c>
+      <c r="D20" s="29">
+        <v>0</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="30">
+        <v>0</v>
+      </c>
+      <c r="G20" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="29">
-        <v>1</v>
-      </c>
-      <c r="D20" s="29">
-        <v>0</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="F20" s="29">
-        <v>0</v>
-      </c>
-      <c r="G20" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>120</v>
-      </c>
       <c r="B21" s="29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C21" s="29">
         <v>24</v>
@@ -18083,21 +18503,21 @@
         <v>0</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="F21" s="29">
-        <v>0</v>
-      </c>
-      <c r="G21" s="29">
+        <v>118</v>
+      </c>
+      <c r="F21" s="30">
+        <v>1</v>
+      </c>
+      <c r="G21" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C22" s="29">
         <v>6</v>
@@ -18108,19 +18528,19 @@
       <c r="E22" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="29">
-        <v>0</v>
-      </c>
-      <c r="G22" s="29">
+      <c r="F22" s="30">
+        <v>0</v>
+      </c>
+      <c r="G22" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C23" s="29">
         <v>7</v>
@@ -18129,21 +18549,21 @@
         <v>0</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="F23" s="29">
-        <v>0</v>
-      </c>
-      <c r="G23" s="29">
+        <v>115</v>
+      </c>
+      <c r="F23" s="30">
+        <v>0</v>
+      </c>
+      <c r="G23" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="32" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C24" s="29">
         <v>18</v>
@@ -18152,44 +18572,44 @@
         <v>0</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" s="29">
-        <v>1</v>
-      </c>
-      <c r="G24" s="29">
+        <v>123</v>
+      </c>
+      <c r="F24" s="30">
+        <v>1</v>
+      </c>
+      <c r="G24" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C25" s="29">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D25" s="29">
         <v>0</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="F25" s="29">
-        <v>3</v>
-      </c>
-      <c r="G25" s="29">
+        <v>154</v>
+      </c>
+      <c r="F25" s="30">
+        <v>4</v>
+      </c>
+      <c r="G25" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
@@ -18197,7 +18617,7 @@
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
     </row>
-    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
@@ -18446,15 +18866,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
23 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="8_{A5B6B11A-29FC-4452-9C12-302E5F9EB695}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B5CEB2D6-C59C-439D-B0F8-7AFA526757C5}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="23112" windowHeight="7296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="20730" windowHeight="7290" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId6"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="162">
   <si>
     <t>Testing</t>
   </si>
@@ -115,9 +109,6 @@
   </si>
   <si>
     <t>Number of Deaths</t>
-  </si>
-  <si>
-    <t>People Recovered</t>
   </si>
   <si>
     <t>Of People in Remote Quarantine, Total Number from Shelters</t>
@@ -441,9 +432,6 @@
     <t>Washington Center for Aging Services (Stoddard Global) (Bed Capacity: 259)</t>
   </si>
   <si>
-    <t>11; (1)</t>
-  </si>
-  <si>
     <t>Personnel Recovered:</t>
   </si>
   <si>
@@ -471,37 +459,16 @@
     <t>56; (47)</t>
   </si>
   <si>
-    <t>50; (19)</t>
-  </si>
-  <si>
     <t>44; (28)</t>
   </si>
   <si>
     <t>46; (18)</t>
   </si>
   <si>
-    <t>16; (3)</t>
-  </si>
-  <si>
-    <t>26; (22)</t>
-  </si>
-  <si>
-    <t>As of May 21, 2020</t>
-  </si>
-  <si>
     <t>45; (33)</t>
   </si>
   <si>
-    <t>584; (280)</t>
-  </si>
-  <si>
-    <t>756; (355)</t>
-  </si>
-  <si>
     <t>21; (17)</t>
-  </si>
-  <si>
-    <t>172; (75)</t>
   </si>
   <si>
     <t>Total Submitted for Testing</t>
@@ -544,11 +511,41 @@
   <si>
     <t>Total COVID-19 Patients in ICU</t>
   </si>
+  <si>
+    <t>Cleared From Isolation</t>
+  </si>
+  <si>
+    <t>55; (20)</t>
+  </si>
+  <si>
+    <t>Hospital for Sick Children LTC</t>
+  </si>
+  <si>
+    <t>589; (281)</t>
+  </si>
+  <si>
+    <t>17; (3)</t>
+  </si>
+  <si>
+    <t>20; (1)</t>
+  </si>
+  <si>
+    <t>31; (24)</t>
+  </si>
+  <si>
+    <t>188; (78)</t>
+  </si>
+  <si>
+    <t>777; (359)</t>
+  </si>
+  <si>
+    <t>As of May 22, 2020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -720,9 +717,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -750,23 +744,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -780,6 +759,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,13 +798,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>394</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -817,7 +812,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1152,33 +1147,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BZ112"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CA112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="106" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CC15" sqref="CC15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="BZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CA81" sqref="CA81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" customWidth="1"/>
-    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1407,8 +1402,11 @@
       <c r="BZ1" s="1">
         <v>43972</v>
       </c>
+      <c r="CA1" s="1">
+        <v>43973</v>
+      </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1430,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1646,13 +1644,16 @@
       <c r="BZ3">
         <v>42993</v>
       </c>
+      <c r="CA3">
+        <v>51991</v>
+      </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1882,8 +1883,11 @@
       <c r="BZ4">
         <v>7893</v>
       </c>
+      <c r="CA4">
+        <v>7966</v>
+      </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2100,13 +2104,16 @@
       <c r="BZ5">
         <v>418</v>
       </c>
+      <c r="CA5">
+        <v>427</v>
+      </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
       <c r="S6">
         <v>17</v>
@@ -2288,16 +2295,19 @@
       <c r="BZ6">
         <v>1069</v>
       </c>
+      <c r="CA6">
+        <v>1075</v>
+      </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BC8">
         <v>345</v>
@@ -2371,8 +2381,11 @@
       <c r="BZ8">
         <v>345</v>
       </c>
+      <c r="CA8">
+        <v>345</v>
+      </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2553,13 +2566,16 @@
       <c r="BZ9">
         <v>46</v>
       </c>
+      <c r="CA9">
+        <v>75</v>
+      </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U10">
         <v>405</v>
@@ -2735,13 +2751,16 @@
       <c r="BZ10">
         <v>440</v>
       </c>
+      <c r="CA10">
+        <v>440</v>
+      </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U11">
         <v>147</v>
@@ -2917,13 +2936,16 @@
       <c r="BZ11">
         <v>228</v>
       </c>
+      <c r="CA11">
+        <v>218</v>
+      </c>
     </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U12">
         <v>258</v>
@@ -3099,13 +3121,16 @@
       <c r="BZ12">
         <v>212</v>
       </c>
+      <c r="CA12">
+        <v>222</v>
+      </c>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BO13">
         <v>416</v>
@@ -3143,13 +3168,16 @@
       <c r="BZ13">
         <v>342</v>
       </c>
+      <c r="CA13">
+        <v>324</v>
+      </c>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="BY14">
         <v>110</v>
@@ -3157,13 +3185,16 @@
       <c r="BZ14">
         <v>112</v>
       </c>
+      <c r="CA14">
+        <v>110</v>
+      </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BO15">
         <v>1775</v>
@@ -3201,13 +3232,16 @@
       <c r="BZ15">
         <v>1896</v>
       </c>
+      <c r="CA15">
+        <v>1883</v>
+      </c>
     </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BO16" s="23">
         <v>0.71</v>
@@ -3245,13 +3279,16 @@
       <c r="BZ16" s="23">
         <v>0.76</v>
       </c>
+      <c r="CA16" s="23">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="18" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3259,12 +3296,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S20">
         <v>8</v>
@@ -3443,13 +3480,16 @@
       <c r="BZ20">
         <v>105</v>
       </c>
+      <c r="CA20">
+        <v>106</v>
+      </c>
     </row>
-    <row r="21" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AK21">
         <v>44</v>
@@ -3574,13 +3614,16 @@
       <c r="BZ21">
         <v>25</v>
       </c>
+      <c r="CA21">
+        <v>26</v>
+      </c>
     </row>
-    <row r="22" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AK22">
         <v>12</v>
@@ -3705,8 +3748,11 @@
       <c r="BZ22">
         <v>80</v>
       </c>
+      <c r="CA22">
+        <v>80</v>
+      </c>
     </row>
-    <row r="23" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3881,8 +3927,11 @@
       <c r="BZ23">
         <v>70</v>
       </c>
+      <c r="CA23">
+        <v>99</v>
+      </c>
     </row>
-    <row r="24" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4057,8 +4106,11 @@
       <c r="BZ24">
         <v>95</v>
       </c>
+      <c r="CA24">
+        <v>125</v>
+      </c>
     </row>
-    <row r="25" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:79" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4233,18 +4285,21 @@
       <c r="BZ25">
         <v>1237</v>
       </c>
+      <c r="CA25">
+        <v>1248</v>
+      </c>
     </row>
-    <row r="27" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S28">
         <v>2</v>
@@ -4423,13 +4478,16 @@
       <c r="BZ28">
         <v>126</v>
       </c>
+      <c r="CA28">
+        <v>128</v>
+      </c>
     </row>
-    <row r="29" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AK29">
         <v>47</v>
@@ -4554,13 +4612,16 @@
       <c r="BZ29">
         <v>40</v>
       </c>
+      <c r="CA29">
+        <v>30</v>
+      </c>
     </row>
-    <row r="30" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AK30">
         <v>4</v>
@@ -4685,8 +4746,11 @@
       <c r="BZ30">
         <v>86</v>
       </c>
+      <c r="CA30">
+        <v>98</v>
+      </c>
     </row>
-    <row r="31" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4861,8 +4925,11 @@
       <c r="BZ31">
         <v>56</v>
       </c>
+      <c r="CA31">
+        <v>67</v>
+      </c>
     </row>
-    <row r="32" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5037,8 +5104,11 @@
       <c r="BZ32">
         <v>96</v>
       </c>
+      <c r="CA32">
+        <v>97</v>
+      </c>
     </row>
-    <row r="33" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5213,18 +5283,21 @@
       <c r="BZ33">
         <v>1116</v>
       </c>
+      <c r="CA33">
+        <v>1127</v>
+      </c>
     </row>
-    <row r="35" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V36">
         <v>1</v>
@@ -5391,13 +5464,16 @@
       <c r="BZ36">
         <v>78</v>
       </c>
+      <c r="CA36">
+        <v>78</v>
+      </c>
     </row>
-    <row r="37" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AL37">
         <v>15</v>
@@ -5516,13 +5592,16 @@
       <c r="BZ37">
         <v>19</v>
       </c>
+      <c r="CA37">
+        <v>20</v>
+      </c>
     </row>
-    <row r="38" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL38">
         <v>0</v>
@@ -5641,8 +5720,11 @@
       <c r="BZ38">
         <v>58</v>
       </c>
+      <c r="CA38">
+        <v>58</v>
+      </c>
     </row>
-    <row r="39" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -5811,8 +5893,11 @@
       <c r="BZ39">
         <v>4</v>
       </c>
+      <c r="CA39">
+        <v>2</v>
+      </c>
     </row>
-    <row r="40" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -5978,8 +6063,11 @@
       <c r="BZ40">
         <v>23</v>
       </c>
+      <c r="CA40">
+        <v>22</v>
+      </c>
     </row>
-    <row r="41" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6151,13 +6239,16 @@
       <c r="BZ41">
         <v>263</v>
       </c>
+      <c r="CA41">
+        <v>265</v>
+      </c>
     </row>
-    <row r="42" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AS42">
         <v>1</v>
@@ -6258,21 +6349,24 @@
       <c r="BZ42">
         <v>1</v>
       </c>
+      <c r="CA42">
+        <v>1</v>
+      </c>
     </row>
-    <row r="43" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U45">
         <v>0</v>
@@ -6445,13 +6539,16 @@
       <c r="BZ45">
         <v>193</v>
       </c>
+      <c r="CA45">
+        <v>193</v>
+      </c>
     </row>
-    <row r="46" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AK46">
         <v>38</v>
@@ -6576,13 +6673,16 @@
       <c r="BZ46">
         <v>21</v>
       </c>
+      <c r="CA46">
+        <v>20</v>
+      </c>
     </row>
-    <row r="47" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK47">
         <v>9</v>
@@ -6707,8 +6807,11 @@
       <c r="BZ47">
         <v>166</v>
       </c>
+      <c r="CA47">
+        <v>167</v>
+      </c>
     </row>
-    <row r="48" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -6883,13 +6986,16 @@
       <c r="BZ48">
         <v>580</v>
       </c>
+      <c r="CA48">
+        <v>515</v>
+      </c>
     </row>
-    <row r="49" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AK49">
         <v>262</v>
@@ -7014,13 +7120,16 @@
       <c r="BZ49">
         <v>601</v>
       </c>
+      <c r="CA49">
+        <v>535</v>
+      </c>
     </row>
-    <row r="50" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AL50">
         <v>9</v>
@@ -7142,13 +7251,16 @@
       <c r="BZ50">
         <v>732</v>
       </c>
+      <c r="CA50">
+        <v>796</v>
+      </c>
     </row>
-    <row r="51" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AO51">
         <v>1</v>
@@ -7264,16 +7376,19 @@
       <c r="BZ51">
         <v>1</v>
       </c>
+      <c r="CA51">
+        <v>1</v>
+      </c>
     </row>
-    <row r="52" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -7436,13 +7551,16 @@
       <c r="BZ54">
         <v>27</v>
       </c>
+      <c r="CA54">
+        <v>29</v>
+      </c>
     </row>
-    <row r="55" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AL55">
         <v>5</v>
@@ -7564,8 +7682,11 @@
       <c r="BZ55">
         <v>10</v>
       </c>
+      <c r="CA55">
+        <v>12</v>
+      </c>
     </row>
-    <row r="56" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -7692,8 +7813,11 @@
       <c r="BZ56">
         <v>16</v>
       </c>
+      <c r="CA56">
+        <v>16</v>
+      </c>
     </row>
-    <row r="57" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -7856,8 +7980,11 @@
       <c r="BZ57">
         <v>15</v>
       </c>
+      <c r="CA57">
+        <v>19</v>
+      </c>
     </row>
-    <row r="58" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -8020,8 +8147,11 @@
       <c r="BZ58">
         <v>25</v>
       </c>
+      <c r="CA58">
+        <v>31</v>
+      </c>
     </row>
-    <row r="59" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -8184,13 +8314,16 @@
       <c r="BZ59">
         <v>132</v>
       </c>
+      <c r="CA59">
+        <v>132</v>
+      </c>
     </row>
-    <row r="60" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AO60">
         <v>1</v>
@@ -8306,8 +8439,11 @@
       <c r="BZ60">
         <v>1</v>
       </c>
+      <c r="CA60">
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>20</v>
       </c>
@@ -8470,13 +8606,16 @@
       <c r="BZ62">
         <v>11</v>
       </c>
+      <c r="CA62">
+        <v>11</v>
+      </c>
     </row>
-    <row r="63" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AL63">
         <v>4</v>
@@ -8598,13 +8737,16 @@
       <c r="BZ63">
         <v>4</v>
       </c>
+      <c r="CA63">
+        <v>4</v>
+      </c>
     </row>
-    <row r="64" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AL64">
         <v>0</v>
@@ -8726,8 +8868,11 @@
       <c r="BZ64">
         <v>7</v>
       </c>
+      <c r="CA64">
+        <v>7</v>
+      </c>
     </row>
-    <row r="65" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -8890,15 +9035,18 @@
       <c r="BZ65">
         <v>42</v>
       </c>
+      <c r="CA65">
+        <v>42</v>
+      </c>
     </row>
-    <row r="66" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C66" s="34"/>
+        <v>66</v>
+      </c>
+      <c r="C66" s="33"/>
       <c r="Z66">
         <v>8</v>
       </c>
@@ -9055,8 +9203,11 @@
       <c r="BZ66">
         <v>46</v>
       </c>
+      <c r="CA66">
+        <v>46</v>
+      </c>
     </row>
-    <row r="67" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -9219,13 +9370,16 @@
       <c r="BZ67">
         <v>0</v>
       </c>
+      <c r="CA67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AL68">
         <v>0</v>
@@ -9347,13 +9501,16 @@
       <c r="BZ68">
         <v>0</v>
       </c>
+      <c r="CA68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
@@ -9364,13 +9521,16 @@
       <c r="BZ70">
         <v>9</v>
       </c>
+      <c r="CA70">
+        <v>9</v>
+      </c>
     </row>
-    <row r="71" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BY71">
         <v>7</v>
@@ -9378,10 +9538,13 @@
       <c r="BZ71">
         <v>8</v>
       </c>
+      <c r="CA71">
+        <v>7</v>
+      </c>
     </row>
-    <row r="72" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
@@ -9392,10 +9555,13 @@
       <c r="BZ72">
         <v>1</v>
       </c>
+      <c r="CA72">
+        <v>2</v>
+      </c>
     </row>
-    <row r="73" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
@@ -9406,10 +9572,13 @@
       <c r="BZ73">
         <v>15</v>
       </c>
+      <c r="CA73">
+        <v>17</v>
+      </c>
     </row>
-    <row r="74" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
@@ -9420,10 +9589,13 @@
       <c r="BZ74">
         <v>23</v>
       </c>
+      <c r="CA74">
+        <v>24</v>
+      </c>
     </row>
-    <row r="75" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
@@ -9434,18 +9606,21 @@
       <c r="BZ75">
         <v>19</v>
       </c>
+      <c r="CA75">
+        <v>21</v>
+      </c>
     </row>
-    <row r="77" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:79" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA78">
         <v>5</v>
@@ -9603,8 +9778,11 @@
       <c r="BZ78">
         <v>286</v>
       </c>
+      <c r="CA78">
+        <v>287</v>
+      </c>
     </row>
-    <row r="79" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -9767,13 +9945,16 @@
       <c r="BZ79">
         <v>246</v>
       </c>
+      <c r="CA79">
+        <v>228</v>
+      </c>
     </row>
-    <row r="80" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA80">
         <v>35</v>
@@ -9931,13 +10112,16 @@
       <c r="BZ80">
         <v>214</v>
       </c>
+      <c r="CA80">
+        <v>208</v>
+      </c>
     </row>
-    <row r="81" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AO81">
         <v>4</v>
@@ -10053,10 +10237,13 @@
       <c r="BZ81">
         <v>15</v>
       </c>
+      <c r="CA81">
+        <v>15</v>
+      </c>
     </row>
-    <row r="83" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -10217,10 +10404,13 @@
       <c r="BZ83">
         <v>108</v>
       </c>
+      <c r="CA83">
+        <v>110</v>
+      </c>
     </row>
-    <row r="84" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B84" t="s">
         <v>10</v>
@@ -10381,10 +10571,13 @@
       <c r="BZ84">
         <v>4</v>
       </c>
+      <c r="CA84">
+        <v>4</v>
+      </c>
     </row>
-    <row r="85" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s">
         <v>11</v>
@@ -10545,10 +10738,13 @@
       <c r="BZ85">
         <v>112</v>
       </c>
+      <c r="CA85">
+        <v>114</v>
+      </c>
     </row>
-    <row r="86" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B86" t="s">
         <v>12</v>
@@ -10563,16 +10759,16 @@
         <v>0</v>
       </c>
       <c r="AD86" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AE86" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF86" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AG86" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH86">
         <v>1</v>
@@ -10709,51 +10905,57 @@
       <c r="BZ86">
         <v>180</v>
       </c>
+      <c r="CA86">
+        <v>180</v>
+      </c>
     </row>
-    <row r="87" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87" t="s">
+        <v>85</v>
+      </c>
+      <c r="BQ87">
+        <v>1</v>
+      </c>
+      <c r="BR87">
+        <v>1</v>
+      </c>
+      <c r="BS87">
+        <v>1</v>
+      </c>
+      <c r="BT87">
+        <v>1</v>
+      </c>
+      <c r="BU87">
+        <v>1</v>
+      </c>
+      <c r="BV87">
+        <v>1</v>
+      </c>
+      <c r="BW87">
+        <v>1</v>
+      </c>
+      <c r="BX87">
+        <v>1</v>
+      </c>
+      <c r="BY87">
+        <v>1</v>
+      </c>
+      <c r="BZ87">
+        <v>1</v>
+      </c>
+      <c r="CA87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B87" t="s">
-        <v>86</v>
-      </c>
-      <c r="BQ87">
-        <v>1</v>
-      </c>
-      <c r="BR87">
-        <v>1</v>
-      </c>
-      <c r="BS87">
-        <v>1</v>
-      </c>
-      <c r="BT87">
-        <v>1</v>
-      </c>
-      <c r="BU87">
-        <v>1</v>
-      </c>
-      <c r="BV87">
-        <v>1</v>
-      </c>
-      <c r="BW87">
-        <v>1</v>
-      </c>
-      <c r="BX87">
-        <v>1</v>
-      </c>
-      <c r="BY87">
-        <v>1</v>
-      </c>
-      <c r="BZ87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
+      <c r="B89" t="s">
         <v>31</v>
-      </c>
-      <c r="B89" t="s">
-        <v>32</v>
       </c>
       <c r="AA89">
         <v>1</v>
@@ -10911,13 +11113,16 @@
       <c r="BZ89">
         <v>79</v>
       </c>
+      <c r="CA89">
+        <v>79</v>
+      </c>
     </row>
-    <row r="90" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B90" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA90">
         <v>17</v>
@@ -11075,13 +11280,16 @@
       <c r="BZ90">
         <v>56</v>
       </c>
+      <c r="CA90">
+        <v>49</v>
+      </c>
     </row>
-    <row r="91" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B91" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA91">
         <v>18</v>
@@ -11150,31 +11358,31 @@
         <v>34</v>
       </c>
       <c r="BA91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BB91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BC91">
         <v>17</v>
       </c>
       <c r="BD91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BE91">
         <v>127</v>
       </c>
       <c r="BF91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BG91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BH91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BI91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BJ91">
         <v>152</v>
@@ -11227,10 +11435,13 @@
       <c r="BZ91">
         <v>142</v>
       </c>
+      <c r="CA91">
+        <v>130</v>
+      </c>
     </row>
-    <row r="92" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B92" t="s">
         <v>15</v>
@@ -11391,13 +11602,16 @@
       <c r="BZ92">
         <v>12</v>
       </c>
+      <c r="CA92">
+        <v>13</v>
+      </c>
     </row>
-    <row r="93" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AO93">
         <v>4</v>
@@ -11513,13 +11727,16 @@
       <c r="BZ93">
         <v>13</v>
       </c>
+      <c r="CA93">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B95" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BB95">
         <v>112</v>
@@ -11597,12 +11814,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="96" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B96" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="BB96">
         <v>5</v>
@@ -11680,12 +11897,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="97" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BB97">
         <v>16</v>
@@ -11763,7 +11980,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:78" x14ac:dyDescent="0.25">
       <c r="AZ112">
         <v>9</v>
       </c>
@@ -11775,23 +11992,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BA11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:BB11"/>
   <sheetViews>
     <sheetView topLeftCell="AT2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BA11" sqref="BA11"/>
+      <selection activeCell="BB4" sqref="BB4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="9">
         <v>43921</v>
@@ -11949,8 +12166,11 @@
       <c r="BA2" s="9">
         <v>43972</v>
       </c>
+      <c r="BB2" s="9">
+        <v>43973</v>
+      </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -12110,8 +12330,11 @@
       <c r="BA3">
         <v>1095</v>
       </c>
+      <c r="BB3">
+        <v>1105</v>
+      </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -12271,8 +12494,11 @@
       <c r="BA4">
         <v>460</v>
       </c>
+      <c r="BB4">
+        <v>468</v>
+      </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -12432,8 +12658,11 @@
       <c r="BA5">
         <v>393</v>
       </c>
+      <c r="BB5">
+        <v>396</v>
+      </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -12593,8 +12822,11 @@
       <c r="BA6">
         <v>1657</v>
       </c>
+      <c r="BB6">
+        <v>1666</v>
+      </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -12754,8 +12986,11 @@
       <c r="BA7">
         <v>1225</v>
       </c>
+      <c r="BB7">
+        <v>1242</v>
+      </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -12915,8 +13150,11 @@
       <c r="BA8">
         <v>682</v>
       </c>
+      <c r="BB8">
+        <v>687</v>
+      </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -13076,8 +13314,11 @@
       <c r="BA9">
         <v>1147</v>
       </c>
+      <c r="BB9">
+        <v>1159</v>
+      </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -13237,10 +13478,13 @@
       <c r="BA10">
         <v>1112</v>
       </c>
+      <c r="BB10">
+        <v>1120</v>
+      </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6">
         <v>25</v>
@@ -13397,6 +13641,9 @@
       </c>
       <c r="BA11">
         <v>122</v>
+      </c>
+      <c r="BB11">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -13406,21 +13653,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:AV17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AW17"/>
   <sheetViews>
-    <sheetView topLeftCell="AE9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AV17" sqref="AV17"/>
+    <sheetView topLeftCell="AL1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AW18" sqref="AW18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -13563,18 +13810,21 @@
       <c r="AV2" s="9">
         <v>43972</v>
       </c>
+      <c r="AW2" s="9">
+        <v>43973</v>
+      </c>
     </row>
-    <row r="3" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="14">
         <v>1097</v>
@@ -13717,10 +13967,13 @@
       <c r="AV4">
         <v>7893</v>
       </c>
+      <c r="AW4">
+        <v>7966</v>
+      </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="14">
         <v>349</v>
@@ -13863,10 +14116,13 @@
       <c r="AV5">
         <v>926</v>
       </c>
+      <c r="AW5">
+        <v>904</v>
+      </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="14">
         <v>135</v>
@@ -14009,10 +14265,13 @@
       <c r="AV6">
         <v>1232</v>
       </c>
+      <c r="AW6">
+        <v>1237</v>
+      </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="14">
         <v>303</v>
@@ -14155,10 +14414,13 @@
       <c r="AV7">
         <v>3683</v>
       </c>
+      <c r="AW7">
+        <v>3729</v>
+      </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="14">
         <v>12</v>
@@ -14301,10 +14563,13 @@
       <c r="AV8">
         <v>101</v>
       </c>
+      <c r="AW8">
+        <v>102</v>
+      </c>
     </row>
-    <row r="9" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="14">
         <v>1</v>
@@ -14447,10 +14712,13 @@
       <c r="AV9">
         <v>22</v>
       </c>
+      <c r="AW9">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="16"/>
@@ -14589,10 +14857,13 @@
       <c r="AV10">
         <v>16</v>
       </c>
+      <c r="AW10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="14">
         <v>78</v>
@@ -14735,10 +15006,13 @@
       <c r="AV11">
         <v>1869</v>
       </c>
+      <c r="AW11">
+        <v>1909</v>
+      </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="14">
         <v>9</v>
@@ -14881,10 +15155,13 @@
       <c r="AV12">
         <v>44</v>
       </c>
+      <c r="AW12">
+        <v>45</v>
+      </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="16"/>
@@ -14893,9 +15170,9 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="14">
         <v>341</v>
@@ -15038,10 +15315,13 @@
       <c r="AV14">
         <v>1447</v>
       </c>
+      <c r="AW14">
+        <v>1428</v>
+      </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="14">
         <v>98</v>
@@ -15184,10 +15464,13 @@
       <c r="AV15">
         <v>1975</v>
       </c>
+      <c r="AW15">
+        <v>2017</v>
+      </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="14">
         <v>517</v>
@@ -15330,10 +15613,13 @@
       <c r="AV16">
         <v>4447</v>
       </c>
+      <c r="AW16">
+        <v>4496</v>
+      </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="14">
         <v>2</v>
@@ -15475,6 +15761,9 @@
       </c>
       <c r="AV17">
         <v>24</v>
+      </c>
+      <c r="AW17">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -15484,20 +15773,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AV9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AW9"/>
   <sheetViews>
-    <sheetView topLeftCell="AK10" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -15639,16 +15928,19 @@
       <c r="AV1" s="9">
         <v>43972</v>
       </c>
+      <c r="AW1" s="9">
+        <v>43973</v>
+      </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <f ca="1">SUM(B3:B8)</f>
@@ -15792,10 +16084,13 @@
       <c r="AV3">
         <v>418</v>
       </c>
+      <c r="AW3">
+        <v>427</v>
+      </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="11">
         <v>2</v>
@@ -15938,10 +16233,13 @@
       <c r="AV4">
         <v>7</v>
       </c>
+      <c r="AW4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:49" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="11">
         <v>14</v>
@@ -16084,10 +16382,13 @@
       <c r="AV5">
         <v>320</v>
       </c>
+      <c r="AW5">
+        <v>323</v>
+      </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="11">
         <v>2</v>
@@ -16230,10 +16531,13 @@
       <c r="AV6">
         <v>42</v>
       </c>
+      <c r="AW6">
+        <v>46</v>
+      </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="11">
         <v>4</v>
@@ -16376,10 +16680,13 @@
       <c r="AV7">
         <v>46</v>
       </c>
+      <c r="AW7">
+        <v>47</v>
+      </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="11">
         <v>2</v>
@@ -16520,16 +16827,14 @@
         <v>2</v>
       </c>
       <c r="AV8">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="AW8">
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV9">
-        <v>2</v>
-      </c>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16537,21 +16842,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AH13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AI13"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="9">
         <v>43940</v>
@@ -16652,10 +16957,13 @@
       <c r="AH2" s="9">
         <v>43972</v>
       </c>
+      <c r="AI2" s="9">
+        <v>43973</v>
+      </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="21">
         <v>105</v>
@@ -16756,8 +17064,11 @@
       <c r="AH3">
         <v>418</v>
       </c>
+      <c r="AI3">
+        <v>427</v>
+      </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -16860,8 +17171,11 @@
       <c r="AH4">
         <v>37</v>
       </c>
+      <c r="AI4">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -16964,8 +17278,11 @@
       <c r="AH5">
         <v>26</v>
       </c>
+      <c r="AI5">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -17068,8 +17385,11 @@
       <c r="AH6">
         <v>27</v>
       </c>
+      <c r="AI6">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -17172,8 +17492,11 @@
       <c r="AH7">
         <v>58</v>
       </c>
+      <c r="AI7">
+        <v>60</v>
+      </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -17276,8 +17599,11 @@
       <c r="AH8">
         <v>65</v>
       </c>
+      <c r="AI8">
+        <v>65</v>
+      </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -17380,8 +17706,11 @@
       <c r="AH9">
         <v>41</v>
       </c>
+      <c r="AI9">
+        <v>41</v>
+      </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -17484,8 +17813,11 @@
       <c r="AH10">
         <v>60</v>
       </c>
+      <c r="AI10">
+        <v>61</v>
+      </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -17588,10 +17920,13 @@
       <c r="AH11">
         <v>89</v>
       </c>
+      <c r="AI11">
+        <v>91</v>
+      </c>
     </row>
-    <row r="12" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="22">
         <v>7</v>
@@ -17692,10 +18027,13 @@
       <c r="AH12">
         <v>15</v>
       </c>
+      <c r="AI12">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="22">
         <v>0</v>
@@ -17794,6 +18132,9 @@
         <v>0</v>
       </c>
       <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
         <v>0</v>
       </c>
     </row>
@@ -17803,88 +18144,91 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80E935D-0DE1-4E26-AC60-89F6B9B8891F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O3"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C1" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
+    <row r="4" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
       <c r="D5" s="9">
         <v>43972</v>
       </c>
+      <c r="E5" s="9">
+        <v>43973</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C6">
         <v>103</v>
@@ -17892,10 +18236,13 @@
       <c r="D6">
         <v>103</v>
       </c>
+      <c r="E6">
+        <v>107</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>26</v>
@@ -17903,15 +18250,18 @@
       <c r="D7">
         <v>26</v>
       </c>
+      <c r="E7">
+        <v>26</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
-        <v>38</v>
+    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
-        <v>41</v>
+    <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>40</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -17919,10 +18269,13 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
-        <v>156</v>
+    <row r="10" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>147</v>
       </c>
       <c r="C10">
         <v>18</v>
@@ -17930,10 +18283,13 @@
       <c r="D10">
         <v>18</v>
       </c>
+      <c r="E10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
-        <v>157</v>
+    <row r="11" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>148</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -17941,10 +18297,13 @@
       <c r="D11">
         <v>5</v>
       </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
-        <v>39</v>
+    <row r="12" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>38</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -17952,14 +18311,17 @@
       <c r="D12">
         <v>2</v>
       </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
-        <v>29</v>
+    <row r="13" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A13" s="37" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="33">
+    <row r="14" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="32">
         <v>1</v>
       </c>
       <c r="C14">
@@ -17968,9 +18330,12 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="33">
+    <row r="15" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A15" s="32">
         <v>2</v>
       </c>
       <c r="C15">
@@ -17979,9 +18344,12 @@
       <c r="D15">
         <v>0</v>
       </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="33">
+    <row r="16" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A16" s="32">
         <v>3</v>
       </c>
       <c r="C16">
@@ -17990,9 +18358,12 @@
       <c r="D16">
         <v>2</v>
       </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="33">
+    <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A17" s="32">
         <v>4</v>
       </c>
       <c r="C17">
@@ -18001,9 +18372,12 @@
       <c r="D17">
         <v>7</v>
       </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="33">
+    <row r="18" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A18" s="32">
         <v>5</v>
       </c>
       <c r="C18">
@@ -18012,9 +18386,12 @@
       <c r="D18">
         <v>2</v>
       </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="33">
+    <row r="19" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A19" s="32">
         <v>6</v>
       </c>
       <c r="C19">
@@ -18023,9 +18400,12 @@
       <c r="D19">
         <v>2</v>
       </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="33">
+    <row r="20" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A20" s="32">
         <v>7</v>
       </c>
       <c r="C20">
@@ -18034,9 +18414,12 @@
       <c r="D20">
         <v>3</v>
       </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="33">
+    <row r="21" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" s="32">
         <v>8</v>
       </c>
       <c r="C21">
@@ -18045,10 +18428,13 @@
       <c r="D21">
         <v>4</v>
       </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
     </row>
-    <row r="22" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="44" t="s">
-        <v>73</v>
+    <row r="22" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="38" t="s">
+        <v>72</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -18056,15 +18442,21 @@
       <c r="D22">
         <v>4</v>
       </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
-        <v>158</v>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>149</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
         <v>1</v>
       </c>
     </row>
@@ -18077,553 +18469,576 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="A1" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
-    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="38" t="s">
+      <c r="F2" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>135</v>
+      <c r="G2" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="26" t="s">
+      <c r="A3" s="42"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="42"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="42"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>93</v>
-      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
     </row>
-    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="27"/>
+    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3</v>
+      </c>
+      <c r="D8" s="28">
+        <v>0</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="29">
+        <v>0</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+    <row r="9" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="28">
+        <v>4</v>
+      </c>
+      <c r="D9" s="28">
+        <v>0</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+    <row r="10" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="28">
+        <v>4</v>
+      </c>
+      <c r="D10" s="28">
+        <v>0</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" s="29">
+        <v>0</v>
+      </c>
+      <c r="G10" s="29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
+    <row r="11" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="28">
+        <v>12</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="29">
+        <v>0</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="29">
+    <row r="12" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="29">
+        <v>0</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0</v>
+      </c>
+      <c r="G13" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="28">
         <v>3</v>
       </c>
-      <c r="D8" s="29">
-        <v>0</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" s="30">
-        <v>0</v>
-      </c>
-      <c r="G8" s="30">
+      <c r="D14" s="28">
+        <v>0</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="29">
+        <v>0</v>
+      </c>
+      <c r="G14" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+    <row r="15" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="28">
+        <v>14</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="29">
+        <v>1</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="28">
+        <v>4</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="29">
+        <v>0</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="28">
+        <v>8</v>
+      </c>
+      <c r="D17" s="28">
+        <v>0</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="29">
+        <v>1</v>
+      </c>
+      <c r="G17" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="28">
+        <v>12</v>
+      </c>
+      <c r="D18" s="28">
+        <v>0</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="29">
+        <v>0</v>
+      </c>
+      <c r="G18" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="28">
+        <v>10</v>
+      </c>
+      <c r="D19" s="28">
+        <v>0</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="29">
+        <v>0</v>
+      </c>
+      <c r="G19" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="28">
+        <v>15</v>
+      </c>
+      <c r="D20" s="28">
+        <v>0</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="29">
+      <c r="F20" s="29">
+        <v>0</v>
+      </c>
+      <c r="G20" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="28">
+        <v>1</v>
+      </c>
+      <c r="D21" s="28">
+        <v>0</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="29">
+        <v>0</v>
+      </c>
+      <c r="G21" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="28">
+        <v>24</v>
+      </c>
+      <c r="D22" s="28">
+        <v>0</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="29">
+        <v>1</v>
+      </c>
+      <c r="G22" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="28">
+        <v>6</v>
+      </c>
+      <c r="D23" s="28">
+        <v>0</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="29">
+        <v>0</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="28">
+        <v>7</v>
+      </c>
+      <c r="D24" s="28">
+        <v>0</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="29">
+        <v>0</v>
+      </c>
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="28">
+        <v>18</v>
+      </c>
+      <c r="D25" s="28">
+        <v>0</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="29">
+        <v>1</v>
+      </c>
+      <c r="G25" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="28">
+        <v>145</v>
+      </c>
+      <c r="D26" s="28">
+        <v>0</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" s="29">
         <v>4</v>
       </c>
-      <c r="D9" s="29">
-        <v>0</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="30">
-        <v>0</v>
-      </c>
-      <c r="G9" s="30">
-        <v>0</v>
+      <c r="G26" s="29">
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" s="29">
-        <v>4</v>
-      </c>
-      <c r="D10" s="29">
-        <v>0</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="F10" s="30">
-        <v>0</v>
-      </c>
-      <c r="G10" s="30">
-        <v>0</v>
-      </c>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="C11" s="29">
-        <v>12</v>
-      </c>
-      <c r="D11" s="29">
-        <v>0</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" s="30">
-        <v>0</v>
-      </c>
-      <c r="G11" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="29">
-        <v>0</v>
-      </c>
-      <c r="D12" s="29">
-        <v>0</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="30">
-        <v>0</v>
-      </c>
-      <c r="G12" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="29">
-        <v>3</v>
-      </c>
-      <c r="D13" s="29">
-        <v>0</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="30">
-        <v>0</v>
-      </c>
-      <c r="G13" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="C14" s="29">
-        <v>14</v>
-      </c>
-      <c r="D14" s="29">
-        <v>0</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="F14" s="30">
-        <v>1</v>
-      </c>
-      <c r="G14" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="29">
-        <v>4</v>
-      </c>
-      <c r="D15" s="29">
-        <v>0</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="30">
-        <v>0</v>
-      </c>
-      <c r="G15" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C16" s="29">
-        <v>8</v>
-      </c>
-      <c r="D16" s="29">
-        <v>0</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="F16" s="30">
-        <v>1</v>
-      </c>
-      <c r="G16" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" s="29">
-        <v>11</v>
-      </c>
-      <c r="D17" s="29">
-        <v>0</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="30">
-        <v>0</v>
-      </c>
-      <c r="G17" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="29">
-        <v>10</v>
-      </c>
-      <c r="D18" s="29">
-        <v>0</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="F18" s="30">
-        <v>0</v>
-      </c>
-      <c r="G18" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" s="29">
-        <v>15</v>
-      </c>
-      <c r="D19" s="29">
-        <v>0</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="30">
-        <v>0</v>
-      </c>
-      <c r="G19" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="29">
-        <v>1</v>
-      </c>
-      <c r="D20" s="29">
-        <v>0</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="30">
-        <v>0</v>
-      </c>
-      <c r="G20" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="29">
-        <v>24</v>
-      </c>
-      <c r="D21" s="29">
-        <v>0</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" s="30">
-        <v>1</v>
-      </c>
-      <c r="G21" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="29">
-        <v>6</v>
-      </c>
-      <c r="D22" s="29">
-        <v>0</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="F22" s="30">
-        <v>0</v>
-      </c>
-      <c r="G22" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="29">
-        <v>7</v>
-      </c>
-      <c r="D23" s="29">
-        <v>0</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="F23" s="30">
-        <v>0</v>
-      </c>
-      <c r="G23" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="29">
-        <v>18</v>
-      </c>
-      <c r="D24" s="29">
-        <v>0</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="F24" s="30">
-        <v>1</v>
-      </c>
-      <c r="G24" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25" s="29">
-        <v>144</v>
-      </c>
-      <c r="D25" s="29">
-        <v>0</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="F25" s="30">
-        <v>4</v>
-      </c>
-      <c r="G25" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -18638,18 +19053,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18856,26 +19271,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
26 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DB1400-773B-4A4A-8C06-D922DB915048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C0BF63-309E-458C-9DAE-ED47D5352DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="945" windowWidth="21600" windowHeight="12855" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="163">
   <si>
     <t>Testing</t>
   </si>
@@ -512,20 +512,23 @@
     <t>45; (18)</t>
   </si>
   <si>
-    <t>Under Review</t>
-  </si>
-  <si>
-    <t>Total Number of Tests</t>
-  </si>
-  <si>
     <t>Total Number of DC Residents Tested</t>
   </si>
   <si>
-    <t>As of May 24, 2020</t>
+    <t>588; (281)</t>
+  </si>
+  <si>
+    <t>187; (78)</t>
+  </si>
+  <si>
+    <t>Total Overall Tested</t>
+  </si>
+  <si>
+    <t>As of May 25, 2020</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of May 24, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of May 25, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -548,12 +551,6 @@
       </rPr>
       <t xml:space="preserve"> for COVID-19 testing,  and 28 (26.2%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
-  </si>
-  <si>
-    <t>588; (281)</t>
-  </si>
-  <si>
-    <t>187; (78)</t>
   </si>
 </sst>
 </file>
@@ -1172,11 +1169,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC113"/>
+  <dimension ref="A1:CD113"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="BV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CC73" sqref="CC1:CC1048576"/>
+      <selection pane="topRight" activeCell="CD85" sqref="CD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,10 +1185,10 @@
     <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="81" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="82" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1429,8 +1426,11 @@
       <c r="CC1" s="1">
         <v>43975</v>
       </c>
+      <c r="CD1" s="1">
+        <v>43976</v>
+      </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1454,12 +1454,12 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>69</v>
@@ -1668,32 +1668,42 @@
       <c r="BZ3">
         <v>42993</v>
       </c>
-      <c r="CA3" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="CB3" s="39" t="s">
-        <v>157</v>
+      <c r="CA3" s="20">
+        <v>38928</v>
+      </c>
+      <c r="CB3" s="39">
+        <v>40003</v>
       </c>
       <c r="CC3">
         <v>40803</v>
       </c>
+      <c r="CD3">
+        <v>42055</v>
+      </c>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AN4" s="19"/>
       <c r="AO4" s="20"/>
-      <c r="CA4" s="20"/>
-      <c r="CB4" s="39"/>
+      <c r="CA4" s="20">
+        <v>32735</v>
+      </c>
+      <c r="CB4" s="39">
+        <v>33576</v>
+      </c>
       <c r="CC4">
         <v>34194</v>
       </c>
+      <c r="CD4">
+        <v>35262</v>
+      </c>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1937,8 +1947,11 @@
       <c r="CC5">
         <v>8225</v>
       </c>
+      <c r="CD5">
+        <v>8334</v>
+      </c>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2164,8 +2177,11 @@
       <c r="CC6">
         <v>440</v>
       </c>
+      <c r="CD6">
+        <v>440</v>
+      </c>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2361,11 +2377,14 @@
       <c r="CC7">
         <v>1080</v>
       </c>
+      <c r="CD7">
+        <v>1080</v>
+      </c>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2453,8 +2472,11 @@
       <c r="CC9">
         <v>345</v>
       </c>
+      <c r="CD9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2644,8 +2666,11 @@
       <c r="CC10">
         <v>114</v>
       </c>
+      <c r="CD10">
+        <v>102</v>
+      </c>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2835,8 +2860,11 @@
       <c r="CC11">
         <v>440</v>
       </c>
+      <c r="CD11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3026,8 +3054,11 @@
       <c r="CC12">
         <v>203</v>
       </c>
+      <c r="CD12">
+        <v>217</v>
+      </c>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3217,8 +3248,11 @@
       <c r="CC13">
         <v>237</v>
       </c>
+      <c r="CD13">
+        <v>223</v>
+      </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3270,8 +3304,11 @@
       <c r="CC14">
         <v>331</v>
       </c>
+      <c r="CD14">
+        <v>353</v>
+      </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3293,8 +3330,11 @@
       <c r="CC15">
         <v>106</v>
       </c>
+      <c r="CD15">
+        <v>113</v>
+      </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3346,8 +3386,11 @@
       <c r="CC16">
         <v>1838</v>
       </c>
+      <c r="CD16">
+        <v>1842</v>
+      </c>
     </row>
-    <row r="17" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3399,13 +3442,16 @@
       <c r="CC17" s="23">
         <v>0.74</v>
       </c>
+      <c r="CD17" s="23">
+        <v>0.74</v>
+      </c>
     </row>
-    <row r="19" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:82" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3413,7 +3459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3606,8 +3652,11 @@
       <c r="CC21">
         <v>106</v>
       </c>
+      <c r="CD21">
+        <v>107</v>
+      </c>
     </row>
-    <row r="22" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3746,8 +3795,11 @@
       <c r="CC22">
         <v>26</v>
       </c>
+      <c r="CD22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3886,8 +3938,11 @@
       <c r="CC23">
         <v>80</v>
       </c>
+      <c r="CD23">
+        <v>89</v>
+      </c>
     </row>
-    <row r="24" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4071,8 +4126,11 @@
       <c r="CC24">
         <v>66</v>
       </c>
+      <c r="CD24">
+        <v>157</v>
+      </c>
     </row>
-    <row r="25" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4256,8 +4314,11 @@
       <c r="CC25">
         <v>91</v>
       </c>
+      <c r="CD25">
+        <v>175</v>
+      </c>
     </row>
-    <row r="26" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4441,13 +4502,16 @@
       <c r="CC26">
         <v>1281</v>
       </c>
+      <c r="CD26">
+        <v>1296</v>
+      </c>
     </row>
-    <row r="28" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:82" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4640,8 +4704,11 @@
       <c r="CC29">
         <v>130</v>
       </c>
+      <c r="CD29">
+        <v>131</v>
+      </c>
     </row>
-    <row r="30" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4780,8 +4847,11 @@
       <c r="CC30">
         <v>33</v>
       </c>
+      <c r="CD30">
+        <v>33</v>
+      </c>
     </row>
-    <row r="31" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4920,8 +4990,11 @@
       <c r="CC31">
         <v>97</v>
       </c>
+      <c r="CD31">
+        <v>98</v>
+      </c>
     </row>
-    <row r="32" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5105,8 +5178,11 @@
       <c r="CC32">
         <v>58</v>
       </c>
+      <c r="CD32">
+        <v>78</v>
+      </c>
     </row>
-    <row r="33" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5290,8 +5366,11 @@
       <c r="CC33">
         <v>91</v>
       </c>
+      <c r="CD33">
+        <v>111</v>
+      </c>
     </row>
-    <row r="34" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -5475,13 +5554,16 @@
       <c r="CC34">
         <v>1132</v>
       </c>
+      <c r="CD34">
+        <v>1124</v>
+      </c>
     </row>
-    <row r="36" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:82" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5662,8 +5744,11 @@
       <c r="CC37">
         <v>79</v>
       </c>
+      <c r="CD37">
+        <v>79</v>
+      </c>
     </row>
-    <row r="38" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -5796,8 +5881,11 @@
       <c r="CC38">
         <v>17</v>
       </c>
+      <c r="CD38">
+        <v>20</v>
+      </c>
     </row>
-    <row r="39" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -5930,8 +6018,11 @@
       <c r="CC39">
         <v>170</v>
       </c>
+      <c r="CD39">
+        <v>58</v>
+      </c>
     </row>
-    <row r="40" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6109,8 +6200,11 @@
       <c r="CC40">
         <v>519</v>
       </c>
+      <c r="CD40">
+        <v>2</v>
+      </c>
     </row>
-    <row r="41" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6285,8 +6379,11 @@
       <c r="CC41">
         <v>536</v>
       </c>
+      <c r="CD41">
+        <v>22</v>
+      </c>
     </row>
-    <row r="42" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -6467,8 +6564,11 @@
       <c r="CC42">
         <v>804</v>
       </c>
+      <c r="CD42">
+        <v>265</v>
+      </c>
     </row>
-    <row r="43" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -6583,16 +6683,19 @@
       <c r="CC43">
         <v>1</v>
       </c>
+      <c r="CD43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:82" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -6779,8 +6882,11 @@
       <c r="CC46">
         <v>193</v>
       </c>
+      <c r="CD46">
+        <v>193</v>
+      </c>
     </row>
-    <row r="47" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -6919,8 +7025,11 @@
       <c r="CC47">
         <v>17</v>
       </c>
+      <c r="CD47">
+        <v>17</v>
+      </c>
     </row>
-    <row r="48" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7059,8 +7168,11 @@
       <c r="CC48">
         <v>170</v>
       </c>
+      <c r="CD48">
+        <v>170</v>
+      </c>
     </row>
-    <row r="49" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -7244,8 +7356,11 @@
       <c r="CC49">
         <v>519</v>
       </c>
+      <c r="CD49">
+        <v>518</v>
+      </c>
     </row>
-    <row r="50" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -7384,8 +7499,11 @@
       <c r="CC50">
         <v>536</v>
       </c>
+      <c r="CD50">
+        <v>535</v>
+      </c>
     </row>
-    <row r="51" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -7521,8 +7639,11 @@
       <c r="CC51">
         <v>804</v>
       </c>
+      <c r="CD51">
+        <v>805</v>
+      </c>
     </row>
-    <row r="52" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -7652,16 +7773,19 @@
       <c r="CC52">
         <v>1</v>
       </c>
+      <c r="CD52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:82" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -7833,8 +7957,11 @@
       <c r="CC55">
         <v>29</v>
       </c>
+      <c r="CD55">
+        <v>29</v>
+      </c>
     </row>
-    <row r="56" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -7970,8 +8097,11 @@
       <c r="CC56">
         <v>12</v>
       </c>
+      <c r="CD56">
+        <v>12</v>
+      </c>
     </row>
-    <row r="57" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -8107,8 +8237,11 @@
       <c r="CC57">
         <v>16</v>
       </c>
+      <c r="CD57">
+        <v>16</v>
+      </c>
     </row>
-    <row r="58" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -8280,8 +8413,11 @@
       <c r="CC58">
         <v>19</v>
       </c>
+      <c r="CD58">
+        <v>19</v>
+      </c>
     </row>
-    <row r="59" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -8453,8 +8589,11 @@
       <c r="CC59">
         <v>31</v>
       </c>
+      <c r="CD59">
+        <v>31</v>
+      </c>
     </row>
-    <row r="60" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -8626,8 +8765,11 @@
       <c r="CC60">
         <v>132</v>
       </c>
+      <c r="CD60">
+        <v>132</v>
+      </c>
     </row>
-    <row r="61" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -8757,8 +8899,11 @@
       <c r="CC61">
         <v>1</v>
       </c>
+      <c r="CD61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -8930,8 +9075,11 @@
       <c r="CC63">
         <v>11</v>
       </c>
+      <c r="CD63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -9067,8 +9215,11 @@
       <c r="CC64">
         <v>4</v>
       </c>
+      <c r="CD64">
+        <v>4</v>
+      </c>
     </row>
-    <row r="65" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -9204,8 +9355,11 @@
       <c r="CC65">
         <v>7</v>
       </c>
+      <c r="CD65">
+        <v>7</v>
+      </c>
     </row>
-    <row r="66" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -9377,8 +9531,11 @@
       <c r="CC66">
         <v>42</v>
       </c>
+      <c r="CD66">
+        <v>43</v>
+      </c>
     </row>
-    <row r="67" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -9551,8 +9708,11 @@
       <c r="CC67">
         <v>46</v>
       </c>
+      <c r="CD67">
+        <v>47</v>
+      </c>
     </row>
-    <row r="68" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -9724,8 +9884,11 @@
       <c r="CC68">
         <v>0</v>
       </c>
+      <c r="CD68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -9861,11 +10024,14 @@
       <c r="CC69">
         <v>0</v>
       </c>
+      <c r="CD69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>137</v>
       </c>
@@ -9887,8 +10053,11 @@
       <c r="CC71">
         <v>9</v>
       </c>
+      <c r="CD71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>137</v>
       </c>
@@ -9910,8 +10079,11 @@
       <c r="CC72">
         <v>6</v>
       </c>
+      <c r="CD72">
+        <v>7</v>
+      </c>
     </row>
-    <row r="73" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>137</v>
       </c>
@@ -9933,8 +10105,11 @@
       <c r="CC73">
         <v>3</v>
       </c>
+      <c r="CD73">
+        <v>3</v>
+      </c>
     </row>
-    <row r="74" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>137</v>
       </c>
@@ -9956,8 +10131,11 @@
       <c r="CC74">
         <v>18</v>
       </c>
+      <c r="CD74">
+        <v>15</v>
+      </c>
     </row>
-    <row r="75" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>137</v>
       </c>
@@ -9979,8 +10157,11 @@
       <c r="CC75">
         <v>24</v>
       </c>
+      <c r="CD75">
+        <v>22</v>
+      </c>
     </row>
-    <row r="76" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>137</v>
       </c>
@@ -10002,13 +10183,16 @@
       <c r="CC76">
         <v>21</v>
       </c>
+      <c r="CD76">
+        <v>23</v>
+      </c>
     </row>
-    <row r="78" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:82" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -10180,8 +10364,11 @@
       <c r="CC79">
         <v>292</v>
       </c>
+      <c r="CD79">
+        <v>292</v>
+      </c>
     </row>
-    <row r="80" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -10353,8 +10540,11 @@
       <c r="CC80">
         <v>205</v>
       </c>
+      <c r="CD80">
+        <v>190</v>
+      </c>
     </row>
-    <row r="81" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -10526,8 +10716,11 @@
       <c r="CC81">
         <v>176</v>
       </c>
+      <c r="CD81">
+        <v>154</v>
+      </c>
     </row>
-    <row r="82" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -10657,8 +10850,11 @@
       <c r="CC82">
         <v>16</v>
       </c>
+      <c r="CD82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -10830,8 +11026,11 @@
       <c r="CC84">
         <v>110</v>
       </c>
+      <c r="CD84">
+        <v>110</v>
+      </c>
     </row>
-    <row r="85" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -11003,8 +11202,11 @@
       <c r="CC85">
         <v>4</v>
       </c>
+      <c r="CD85">
+        <v>4</v>
+      </c>
     </row>
-    <row r="86" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -11176,8 +11378,11 @@
       <c r="CC86">
         <v>114</v>
       </c>
+      <c r="CD86">
+        <v>114</v>
+      </c>
     </row>
-    <row r="87" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -11349,8 +11554,11 @@
       <c r="CC87">
         <v>180</v>
       </c>
+      <c r="CD87">
+        <v>180</v>
+      </c>
     </row>
-    <row r="88" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -11396,8 +11604,11 @@
       <c r="CC88">
         <v>1</v>
       </c>
+      <c r="CD88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -11569,8 +11780,11 @@
       <c r="CC90">
         <v>79</v>
       </c>
+      <c r="CD90">
+        <v>79</v>
+      </c>
     </row>
-    <row r="91" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -11742,8 +11956,11 @@
       <c r="CC91">
         <v>49</v>
       </c>
+      <c r="CD91">
+        <v>49</v>
+      </c>
     </row>
-    <row r="92" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -11903,8 +12120,11 @@
       <c r="CC92">
         <v>130</v>
       </c>
+      <c r="CD92">
+        <v>130</v>
+      </c>
     </row>
-    <row r="93" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -12076,8 +12296,11 @@
       <c r="CC93">
         <v>13</v>
       </c>
+      <c r="CD93">
+        <v>13</v>
+      </c>
     </row>
-    <row r="94" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -12207,8 +12430,11 @@
       <c r="CC94">
         <v>13</v>
       </c>
+      <c r="CD94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>79</v>
       </c>
@@ -12299,8 +12525,11 @@
       <c r="CC96">
         <v>179</v>
       </c>
+      <c r="CD96">
+        <v>179</v>
+      </c>
     </row>
-    <row r="97" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>79</v>
       </c>
@@ -12391,8 +12620,11 @@
       <c r="CC97">
         <v>41</v>
       </c>
+      <c r="CD97">
+        <v>41</v>
+      </c>
     </row>
-    <row r="98" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>79</v>
       </c>
@@ -12481,6 +12713,9 @@
         <v>25</v>
       </c>
       <c r="CC98">
+        <v>25</v>
+      </c>
+      <c r="CD98">
         <v>25</v>
       </c>
     </row>
@@ -12497,10 +12732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BD11"/>
+  <dimension ref="A2:BE11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC3" sqref="BC3:BD11"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BE3" sqref="BE3:BE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12510,7 +12745,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -12679,8 +12914,11 @@
       <c r="BD2" s="9">
         <v>43975</v>
       </c>
+      <c r="BE2" s="9">
+        <v>43976</v>
+      </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -12849,8 +13087,11 @@
       <c r="BD3">
         <v>1144</v>
       </c>
+      <c r="BE3">
+        <v>1166</v>
+      </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -13019,8 +13260,11 @@
       <c r="BD4">
         <v>490</v>
       </c>
+      <c r="BE4">
+        <v>508</v>
+      </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -13189,8 +13433,11 @@
       <c r="BD5">
         <v>408</v>
       </c>
+      <c r="BE5">
+        <v>410</v>
+      </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -13359,8 +13606,11 @@
       <c r="BD6">
         <v>1737</v>
       </c>
+      <c r="BE6">
+        <v>1759</v>
+      </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -13529,8 +13779,11 @@
       <c r="BD7">
         <v>1286</v>
       </c>
+      <c r="BE7">
+        <v>1303</v>
+      </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -13699,8 +13952,11 @@
       <c r="BD8">
         <v>705</v>
       </c>
+      <c r="BE8">
+        <v>709</v>
+      </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -13869,8 +14125,11 @@
       <c r="BD9">
         <v>1180</v>
       </c>
+      <c r="BE9">
+        <v>1194</v>
+      </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -14039,8 +14298,11 @@
       <c r="BD10">
         <v>1147</v>
       </c>
+      <c r="BE10">
+        <v>1156</v>
+      </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -14208,6 +14470,9 @@
       </c>
       <c r="BD11">
         <v>128</v>
+      </c>
+      <c r="BE11">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -14218,10 +14483,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:AY17"/>
+  <dimension ref="A2:AZ17"/>
   <sheetViews>
-    <sheetView topLeftCell="AL8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AY17" sqref="AY17"/>
+    <sheetView topLeftCell="AQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AZ13" sqref="AZ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14231,7 +14496,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -14383,8 +14648,11 @@
       <c r="AY2" s="9">
         <v>43975</v>
       </c>
+      <c r="AZ2" s="9">
+        <v>43976</v>
+      </c>
     </row>
-    <row r="3" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -14392,7 +14660,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -14546,8 +14814,11 @@
       <c r="AY4">
         <v>8225</v>
       </c>
+      <c r="AZ4">
+        <v>8334</v>
+      </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -14701,8 +14972,11 @@
       <c r="AY5">
         <v>983</v>
       </c>
+      <c r="AZ5">
+        <v>1010</v>
+      </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -14856,8 +15130,11 @@
       <c r="AY6">
         <v>1271</v>
       </c>
+      <c r="AZ6">
+        <v>1282</v>
+      </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -15011,8 +15288,11 @@
       <c r="AY7">
         <v>3792</v>
       </c>
+      <c r="AZ7">
+        <v>3822</v>
+      </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -15166,8 +15446,11 @@
       <c r="AY8">
         <v>104</v>
       </c>
+      <c r="AZ8">
+        <v>104</v>
+      </c>
     </row>
-    <row r="9" spans="1:51" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -15321,8 +15604,11 @@
       <c r="AY9">
         <v>23</v>
       </c>
+      <c r="AZ9">
+        <v>23</v>
+      </c>
     </row>
-    <row r="10" spans="1:51" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -15472,8 +15758,11 @@
       <c r="AY10">
         <v>20</v>
       </c>
+      <c r="AZ10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -15627,8 +15916,11 @@
       <c r="AY11">
         <v>1986</v>
       </c>
+      <c r="AZ11">
+        <v>2027</v>
+      </c>
     </row>
-    <row r="12" spans="1:51" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -15782,8 +16074,11 @@
       <c r="AY12">
         <v>46</v>
       </c>
+      <c r="AZ12">
+        <v>46</v>
+      </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -15794,7 +16089,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -15948,8 +16243,11 @@
       <c r="AY14">
         <v>1545</v>
       </c>
+      <c r="AZ14">
+        <v>1593</v>
+      </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -16103,8 +16401,11 @@
       <c r="AY15">
         <v>2086</v>
       </c>
+      <c r="AZ15">
+        <v>2115</v>
+      </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -16258,8 +16559,11 @@
       <c r="AY16">
         <v>4566</v>
       </c>
+      <c r="AZ16">
+        <v>4600</v>
+      </c>
     </row>
-    <row r="17" spans="1:51" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -16411,6 +16715,9 @@
         <v>26</v>
       </c>
       <c r="AY17">
+        <v>26</v>
+      </c>
+      <c r="AZ17">
         <v>26</v>
       </c>
     </row>
@@ -16422,10 +16729,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AY9"/>
+  <dimension ref="A1:AZ9"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AY8" sqref="AY8"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AZ3" sqref="AZ3:AZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16434,7 +16741,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -16585,14 +16892,17 @@
       <c r="AY1" s="9">
         <v>43975</v>
       </c>
+      <c r="AZ1" s="9">
+        <v>43976</v>
+      </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -16747,8 +17057,11 @@
       <c r="AY3">
         <v>440</v>
       </c>
+      <c r="AZ3">
+        <v>440</v>
+      </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -16902,8 +17215,11 @@
       <c r="AY4">
         <v>7</v>
       </c>
+      <c r="AZ4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:51" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -17057,8 +17373,11 @@
       <c r="AY5">
         <v>333</v>
       </c>
+      <c r="AZ5">
+        <v>333</v>
+      </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -17212,8 +17531,11 @@
       <c r="AY6">
         <v>47</v>
       </c>
+      <c r="AZ6">
+        <v>47</v>
+      </c>
     </row>
-    <row r="7" spans="1:51" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -17367,8 +17689,11 @@
       <c r="AY7">
         <v>49</v>
       </c>
+      <c r="AZ7">
+        <v>49</v>
+      </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -17522,8 +17847,11 @@
       <c r="AY8">
         <v>4</v>
       </c>
+      <c r="AZ8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -17535,10 +17863,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AK13"/>
+  <dimension ref="A2:AL13"/>
   <sheetViews>
-    <sheetView topLeftCell="Y3" workbookViewId="0">
-      <selection activeCell="AK12" sqref="AK12"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AL13" sqref="AL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17546,7 +17874,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -17658,8 +17986,11 @@
       <c r="AK2" s="9">
         <v>43975</v>
       </c>
+      <c r="AL2" s="9">
+        <v>43976</v>
+      </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -17771,8 +18102,11 @@
       <c r="AK3">
         <v>440</v>
       </c>
+      <c r="AL3">
+        <v>440</v>
+      </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -17884,8 +18218,11 @@
       <c r="AK4">
         <v>43</v>
       </c>
+      <c r="AL4">
+        <v>43</v>
+      </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -17997,8 +18334,11 @@
       <c r="AK5">
         <v>27</v>
       </c>
+      <c r="AL5">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -18110,8 +18450,11 @@
       <c r="AK6">
         <v>30</v>
       </c>
+      <c r="AL6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -18223,8 +18566,11 @@
       <c r="AK7">
         <v>62</v>
       </c>
+      <c r="AL7">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -18336,8 +18682,11 @@
       <c r="AK8">
         <v>68</v>
       </c>
+      <c r="AL8">
+        <v>68</v>
+      </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -18449,8 +18798,11 @@
       <c r="AK9">
         <v>41</v>
       </c>
+      <c r="AL9">
+        <v>41</v>
+      </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -18562,8 +18914,11 @@
       <c r="AK10">
         <v>62</v>
       </c>
+      <c r="AL10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -18675,8 +19030,11 @@
       <c r="AK11">
         <v>91</v>
       </c>
+      <c r="AL11">
+        <v>91</v>
+      </c>
     </row>
-    <row r="12" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -18788,8 +19146,11 @@
       <c r="AK12">
         <v>16</v>
       </c>
+      <c r="AL12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -18896,6 +19257,12 @@
         <v>0</v>
       </c>
       <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
         <v>0</v>
       </c>
     </row>
@@ -18909,8 +19276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="D1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18920,7 +19287,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C1" s="41" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D1" s="41"/>
       <c r="E1" s="41"/>
@@ -18996,6 +19363,9 @@
       <c r="G5" s="9">
         <v>43975</v>
       </c>
+      <c r="H5" s="9">
+        <v>43976</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -19016,6 +19386,9 @@
       <c r="G6">
         <v>107</v>
       </c>
+      <c r="H6">
+        <v>107</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -19036,6 +19409,9 @@
       <c r="G7">
         <v>28</v>
       </c>
+      <c r="H7">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
@@ -19061,6 +19437,9 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
@@ -19081,6 +19460,9 @@
       <c r="G10">
         <v>20</v>
       </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
@@ -19101,6 +19483,9 @@
       <c r="G11">
         <v>5</v>
       </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
@@ -19121,6 +19506,9 @@
       <c r="G12">
         <v>2</v>
       </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
@@ -19146,6 +19534,9 @@
       <c r="G14">
         <v>1</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
@@ -19166,6 +19557,9 @@
       <c r="G15">
         <v>0</v>
       </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
@@ -19186,8 +19580,11 @@
       <c r="G16">
         <v>2</v>
       </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -19206,8 +19603,11 @@
       <c r="G17">
         <v>8</v>
       </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -19226,8 +19626,11 @@
       <c r="G18">
         <v>2</v>
       </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -19246,8 +19649,11 @@
       <c r="G19">
         <v>2</v>
       </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -19266,8 +19672,11 @@
       <c r="G20">
         <v>3</v>
       </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -19286,8 +19695,11 @@
       <c r="G21">
         <v>5</v>
       </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -19306,8 +19718,11 @@
       <c r="G22">
         <v>4</v>
       </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
         <v>147</v>
       </c>
@@ -19324,6 +19739,9 @@
         <v>1</v>
       </c>
       <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>1</v>
       </c>
     </row>
@@ -19340,7 +19758,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19356,7 +19774,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -19868,7 +20286,7 @@
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C26" s="27">
         <v>149</v>
@@ -19877,7 +20295,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F26" s="28">
         <v>4</v>
@@ -19920,15 +20338,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -20131,21 +20540,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20164,19 +20574,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
27 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C0BF63-309E-458C-9DAE-ED47D5352DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{C5E88C75-E440-43B4-B034-AA36176F93AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4A528D01-D78E-4B25-B78E-AAD36C8A6AEC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="156" windowWidth="23040" windowHeight="7296" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -389,9 +387,6 @@
     <t>Transitions (Bed Capacity: 360)</t>
   </si>
   <si>
-    <t>26; (0)</t>
-  </si>
-  <si>
     <t>UMNC (Bed Capacity: 120)</t>
   </si>
   <si>
@@ -399,9 +394,6 @@
   </si>
   <si>
     <t>Unique (Bed Capacity: 230)</t>
-  </si>
-  <si>
-    <t>12; (8)</t>
   </si>
   <si>
     <t>13; (3)</t>
@@ -438,9 +430,6 @@
   </si>
   <si>
     <t>Personnel Recovered:</t>
-  </si>
-  <si>
-    <t>139; (41)</t>
   </si>
   <si>
     <t>79; (49)</t>
@@ -503,32 +492,20 @@
     <t>31; (24)</t>
   </si>
   <si>
-    <t>775; (359)</t>
-  </si>
-  <si>
-    <t>16; (3)</t>
-  </si>
-  <si>
     <t>45; (18)</t>
   </si>
   <si>
     <t>Total Number of DC Residents Tested</t>
   </si>
   <si>
-    <t>588; (281)</t>
-  </si>
-  <si>
-    <t>187; (78)</t>
-  </si>
-  <si>
     <t>Total Overall Tested</t>
   </si>
   <si>
-    <t>As of May 25, 2020</t>
+    <t>As of May 26, 2020</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of May 25, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of May 26, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -552,12 +529,33 @@
       <t xml:space="preserve"> for COVID-19 testing,  and 28 (26.2%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
   </si>
+  <si>
+    <t>20; (3)</t>
+  </si>
+  <si>
+    <t>141; (43)</t>
+  </si>
+  <si>
+    <t>29; (0)</t>
+  </si>
+  <si>
+    <t>21; (8)</t>
+  </si>
+  <si>
+    <t>599; (283)</t>
+  </si>
+  <si>
+    <t>194; (78)</t>
+  </si>
+  <si>
+    <t>793; (361)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,13 +591,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF112277"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -626,6 +617,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF112277"/>
+      <name val="Albany AMT"/>
     </font>
   </fonts>
   <fills count="6">
@@ -725,25 +722,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -767,9 +764,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -777,17 +771,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,26 +1166,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD113"/>
+  <dimension ref="A1:CE113"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CD85" sqref="CD85"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="BU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CE93" sqref="CE1:CE1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="82" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="83" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1429,8 +1426,11 @@
       <c r="CD1" s="1">
         <v>43976</v>
       </c>
+      <c r="CE1" s="1">
+        <v>43977</v>
+      </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1454,12 +1454,12 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="I3">
         <v>69</v>
@@ -1671,7 +1671,7 @@
       <c r="CA3" s="20">
         <v>38928</v>
       </c>
-      <c r="CB3" s="39">
+      <c r="CB3" s="38">
         <v>40003</v>
       </c>
       <c r="CC3">
@@ -1680,20 +1680,23 @@
       <c r="CD3">
         <v>42055</v>
       </c>
+      <c r="CE3">
+        <v>42697</v>
+      </c>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:83">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="AN4" s="19"/>
       <c r="AO4" s="20"/>
       <c r="CA4" s="20">
         <v>32735</v>
       </c>
-      <c r="CB4" s="39">
+      <c r="CB4" s="38">
         <v>33576</v>
       </c>
       <c r="CC4">
@@ -1702,8 +1705,11 @@
       <c r="CD4">
         <v>35262</v>
       </c>
+      <c r="CE4">
+        <v>35682</v>
+      </c>
     </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:83">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1950,8 +1956,11 @@
       <c r="CD5">
         <v>8334</v>
       </c>
+      <c r="CE5">
+        <v>8406</v>
+      </c>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:83">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2180,13 +2189,16 @@
       <c r="CD6">
         <v>440</v>
       </c>
+      <c r="CE6">
+        <v>445</v>
+      </c>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:83">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="S7">
         <v>17</v>
@@ -2380,11 +2392,14 @@
       <c r="CD7">
         <v>1080</v>
       </c>
+      <c r="CE7">
+        <v>1082</v>
+      </c>
     </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:83">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2475,8 +2490,11 @@
       <c r="CD9">
         <v>345</v>
       </c>
+      <c r="CE9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:83">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2669,8 +2687,11 @@
       <c r="CD10">
         <v>102</v>
       </c>
+      <c r="CE10">
+        <v>80</v>
+      </c>
     </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:83">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2863,8 +2884,11 @@
       <c r="CD11">
         <v>440</v>
       </c>
+      <c r="CE11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3057,8 +3081,11 @@
       <c r="CD12">
         <v>217</v>
       </c>
+      <c r="CE12">
+        <v>214</v>
+      </c>
     </row>
-    <row r="13" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:83">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3251,8 +3278,11 @@
       <c r="CD13">
         <v>223</v>
       </c>
+      <c r="CE13">
+        <v>226</v>
+      </c>
     </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:83">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3307,13 +3337,16 @@
       <c r="CD14">
         <v>353</v>
       </c>
+      <c r="CE14">
+        <v>349</v>
+      </c>
     </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:83">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="BY15">
         <v>110</v>
@@ -3333,8 +3366,11 @@
       <c r="CD15">
         <v>113</v>
       </c>
+      <c r="CE15">
+        <v>113</v>
+      </c>
     </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:83">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3389,8 +3425,11 @@
       <c r="CD16">
         <v>1842</v>
       </c>
+      <c r="CE16">
+        <v>1851</v>
+      </c>
     </row>
-    <row r="17" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:83">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3445,13 +3484,16 @@
       <c r="CD17" s="23">
         <v>0.74</v>
       </c>
+      <c r="CE17" s="23">
+        <v>0.74</v>
+      </c>
     </row>
-    <row r="19" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:83">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:83">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3459,7 +3501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:83">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3655,8 +3697,11 @@
       <c r="CD21">
         <v>107</v>
       </c>
+      <c r="CE21">
+        <v>107</v>
+      </c>
     </row>
-    <row r="22" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:83">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3798,8 +3843,11 @@
       <c r="CD22">
         <v>18</v>
       </c>
+      <c r="CE22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:83">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3941,8 +3989,11 @@
       <c r="CD23">
         <v>89</v>
       </c>
+      <c r="CE23">
+        <v>89</v>
+      </c>
     </row>
-    <row r="24" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:83">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4129,8 +4180,11 @@
       <c r="CD24">
         <v>157</v>
       </c>
+      <c r="CE24">
+        <v>161</v>
+      </c>
     </row>
-    <row r="25" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:83">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4317,8 +4371,11 @@
       <c r="CD25">
         <v>175</v>
       </c>
+      <c r="CE25">
+        <v>179</v>
+      </c>
     </row>
-    <row r="26" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:83">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4505,13 +4562,16 @@
       <c r="CD26">
         <v>1296</v>
       </c>
+      <c r="CE26">
+        <v>1312</v>
+      </c>
     </row>
-    <row r="28" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:83">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:83">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4707,8 +4767,11 @@
       <c r="CD29">
         <v>131</v>
       </c>
+      <c r="CE29">
+        <v>131</v>
+      </c>
     </row>
-    <row r="30" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:83">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4850,8 +4913,11 @@
       <c r="CD30">
         <v>33</v>
       </c>
+      <c r="CE30">
+        <v>33</v>
+      </c>
     </row>
-    <row r="31" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:83">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4993,8 +5059,11 @@
       <c r="CD31">
         <v>98</v>
       </c>
+      <c r="CE31">
+        <v>98</v>
+      </c>
     </row>
-    <row r="32" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:83">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5181,8 +5250,11 @@
       <c r="CD32">
         <v>78</v>
       </c>
+      <c r="CE32">
+        <v>63</v>
+      </c>
     </row>
-    <row r="33" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:83">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5369,8 +5441,11 @@
       <c r="CD33">
         <v>111</v>
       </c>
+      <c r="CE33">
+        <v>96</v>
+      </c>
     </row>
-    <row r="34" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:83">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -5557,13 +5632,16 @@
       <c r="CD34">
         <v>1124</v>
       </c>
+      <c r="CE34">
+        <v>1156</v>
+      </c>
     </row>
-    <row r="36" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:83">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:83">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5747,8 +5825,11 @@
       <c r="CD37">
         <v>79</v>
       </c>
+      <c r="CE37">
+        <v>80</v>
+      </c>
     </row>
-    <row r="38" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:83">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -5884,8 +5965,11 @@
       <c r="CD38">
         <v>20</v>
       </c>
+      <c r="CE38">
+        <v>17</v>
+      </c>
     </row>
-    <row r="39" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:83">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6021,8 +6105,11 @@
       <c r="CD39">
         <v>58</v>
       </c>
+      <c r="CE39">
+        <v>62</v>
+      </c>
     </row>
-    <row r="40" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:83">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6203,8 +6290,11 @@
       <c r="CD40">
         <v>2</v>
       </c>
+      <c r="CE40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:83">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6382,8 +6472,11 @@
       <c r="CD41">
         <v>22</v>
       </c>
+      <c r="CE41">
+        <v>18</v>
+      </c>
     </row>
-    <row r="42" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:83">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -6567,8 +6660,11 @@
       <c r="CD42">
         <v>265</v>
       </c>
+      <c r="CE42">
+        <v>270</v>
+      </c>
     </row>
-    <row r="43" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:83">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -6686,16 +6782,19 @@
       <c r="CD43">
         <v>1</v>
       </c>
+      <c r="CE43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:83">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:83">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:83">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -6885,8 +6984,11 @@
       <c r="CD46">
         <v>193</v>
       </c>
+      <c r="CE46">
+        <v>193</v>
+      </c>
     </row>
-    <row r="47" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:83">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7028,8 +7130,11 @@
       <c r="CD47">
         <v>17</v>
       </c>
+      <c r="CE47">
+        <v>17</v>
+      </c>
     </row>
-    <row r="48" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:83">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7171,8 +7276,11 @@
       <c r="CD48">
         <v>170</v>
       </c>
+      <c r="CE48">
+        <v>170</v>
+      </c>
     </row>
-    <row r="49" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:83">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -7359,8 +7467,11 @@
       <c r="CD49">
         <v>518</v>
       </c>
+      <c r="CE49">
+        <v>517</v>
+      </c>
     </row>
-    <row r="50" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:83">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -7502,8 +7613,11 @@
       <c r="CD50">
         <v>535</v>
       </c>
+      <c r="CE50">
+        <v>534</v>
+      </c>
     </row>
-    <row r="51" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:83">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -7642,8 +7756,11 @@
       <c r="CD51">
         <v>805</v>
       </c>
+      <c r="CE51">
+        <v>813</v>
+      </c>
     </row>
-    <row r="52" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:83">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -7776,16 +7893,19 @@
       <c r="CD52">
         <v>1</v>
       </c>
+      <c r="CE52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:83">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:83">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:83">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -7960,8 +8080,11 @@
       <c r="CD55">
         <v>29</v>
       </c>
+      <c r="CE55">
+        <v>30</v>
+      </c>
     </row>
-    <row r="56" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:83">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -8100,8 +8223,11 @@
       <c r="CD56">
         <v>12</v>
       </c>
+      <c r="CE56">
+        <v>11</v>
+      </c>
     </row>
-    <row r="57" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:83">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -8240,8 +8366,11 @@
       <c r="CD57">
         <v>16</v>
       </c>
+      <c r="CE57">
+        <v>19</v>
+      </c>
     </row>
-    <row r="58" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:83">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -8416,8 +8545,11 @@
       <c r="CD58">
         <v>19</v>
       </c>
+      <c r="CE58">
+        <v>20</v>
+      </c>
     </row>
-    <row r="59" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:83">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -8592,8 +8724,11 @@
       <c r="CD59">
         <v>31</v>
       </c>
+      <c r="CE59">
+        <v>31</v>
+      </c>
     </row>
-    <row r="60" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:83">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -8768,8 +8903,11 @@
       <c r="CD60">
         <v>132</v>
       </c>
+      <c r="CE60">
+        <v>138</v>
+      </c>
     </row>
-    <row r="61" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:83">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -8902,8 +9040,11 @@
       <c r="CD61">
         <v>1</v>
       </c>
+      <c r="CE61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:83">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -9078,8 +9219,11 @@
       <c r="CD63">
         <v>11</v>
       </c>
+      <c r="CE63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:83">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -9218,8 +9362,11 @@
       <c r="CD64">
         <v>4</v>
       </c>
+      <c r="CE64">
+        <v>4</v>
+      </c>
     </row>
-    <row r="65" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:83">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -9358,8 +9505,11 @@
       <c r="CD65">
         <v>7</v>
       </c>
+      <c r="CE65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:83">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -9534,8 +9684,11 @@
       <c r="CD66">
         <v>43</v>
       </c>
+      <c r="CE66">
+        <v>46</v>
+      </c>
     </row>
-    <row r="67" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:83">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -9711,8 +9864,11 @@
       <c r="CD67">
         <v>47</v>
       </c>
+      <c r="CE67">
+        <v>50</v>
+      </c>
     </row>
-    <row r="68" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:83">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -9887,8 +10043,11 @@
       <c r="CD68">
         <v>0</v>
       </c>
+      <c r="CE68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:83">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -10027,13 +10186,16 @@
       <c r="CD69">
         <v>0</v>
       </c>
+      <c r="CE69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:83">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:83">
       <c r="A71" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -10056,10 +10218,13 @@
       <c r="CD71">
         <v>10</v>
       </c>
+      <c r="CE71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:83">
       <c r="A72" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
@@ -10082,10 +10247,13 @@
       <c r="CD72">
         <v>7</v>
       </c>
+      <c r="CE72">
+        <v>7</v>
+      </c>
     </row>
-    <row r="73" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:83">
       <c r="A73" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -10108,10 +10276,13 @@
       <c r="CD73">
         <v>3</v>
       </c>
+      <c r="CE73">
+        <v>3</v>
+      </c>
     </row>
-    <row r="74" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:83">
       <c r="A74" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
@@ -10134,10 +10305,13 @@
       <c r="CD74">
         <v>15</v>
       </c>
+      <c r="CE74">
+        <v>13</v>
+      </c>
     </row>
-    <row r="75" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:83">
       <c r="A75" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
@@ -10160,10 +10334,13 @@
       <c r="CD75">
         <v>22</v>
       </c>
+      <c r="CE75">
+        <v>20</v>
+      </c>
     </row>
-    <row r="76" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:83">
       <c r="A76" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
@@ -10186,13 +10363,16 @@
       <c r="CD76">
         <v>23</v>
       </c>
+      <c r="CE76">
+        <v>25</v>
+      </c>
     </row>
-    <row r="78" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:83">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:83">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -10367,8 +10547,11 @@
       <c r="CD79">
         <v>292</v>
       </c>
+      <c r="CE79">
+        <v>294</v>
+      </c>
     </row>
-    <row r="80" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:83">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -10543,8 +10726,11 @@
       <c r="CD80">
         <v>190</v>
       </c>
+      <c r="CE80">
+        <v>179</v>
+      </c>
     </row>
-    <row r="81" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:83">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -10719,8 +10905,11 @@
       <c r="CD81">
         <v>154</v>
       </c>
+      <c r="CE81">
+        <v>150</v>
+      </c>
     </row>
-    <row r="82" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:83">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -10853,8 +11042,11 @@
       <c r="CD82">
         <v>16</v>
       </c>
+      <c r="CE82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:83">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -11029,8 +11221,11 @@
       <c r="CD84">
         <v>110</v>
       </c>
+      <c r="CE84">
+        <v>115</v>
+      </c>
     </row>
-    <row r="85" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:83">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -11205,8 +11400,11 @@
       <c r="CD85">
         <v>4</v>
       </c>
+      <c r="CE85">
+        <v>3</v>
+      </c>
     </row>
-    <row r="86" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:83">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -11381,8 +11579,11 @@
       <c r="CD86">
         <v>114</v>
       </c>
+      <c r="CE86">
+        <v>118</v>
+      </c>
     </row>
-    <row r="87" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:83">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -11557,8 +11758,11 @@
       <c r="CD87">
         <v>180</v>
       </c>
+      <c r="CE87">
+        <v>180</v>
+      </c>
     </row>
-    <row r="88" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:83">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -11607,8 +11811,11 @@
       <c r="CD88">
         <v>1</v>
       </c>
+      <c r="CE88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:83">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -11783,8 +11990,11 @@
       <c r="CD90">
         <v>79</v>
       </c>
+      <c r="CE90">
+        <v>79</v>
+      </c>
     </row>
-    <row r="91" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:83">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -11959,8 +12169,11 @@
       <c r="CD91">
         <v>49</v>
       </c>
+      <c r="CE91">
+        <v>49</v>
+      </c>
     </row>
-    <row r="92" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:83">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -12123,8 +12336,11 @@
       <c r="CD92">
         <v>130</v>
       </c>
+      <c r="CE92">
+        <v>130</v>
+      </c>
     </row>
-    <row r="93" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:83">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -12299,8 +12515,11 @@
       <c r="CD93">
         <v>13</v>
       </c>
+      <c r="CE93">
+        <v>13</v>
+      </c>
     </row>
-    <row r="94" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:83">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -12433,8 +12652,11 @@
       <c r="CD94">
         <v>13</v>
       </c>
+      <c r="CE94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:83">
       <c r="A96" s="2" t="s">
         <v>79</v>
       </c>
@@ -12528,8 +12750,11 @@
       <c r="CD96">
         <v>179</v>
       </c>
+      <c r="CE96">
+        <v>182</v>
+      </c>
     </row>
-    <row r="97" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:83">
       <c r="A97" s="2" t="s">
         <v>79</v>
       </c>
@@ -12623,8 +12848,11 @@
       <c r="CD97">
         <v>41</v>
       </c>
+      <c r="CE97">
+        <v>47</v>
+      </c>
     </row>
-    <row r="98" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:83">
       <c r="A98" s="2" t="s">
         <v>79</v>
       </c>
@@ -12718,8 +12946,11 @@
       <c r="CD98">
         <v>25</v>
       </c>
+      <c r="CE98">
+        <v>25</v>
+      </c>
     </row>
-    <row r="113" spans="52:52" x14ac:dyDescent="0.25">
+    <row r="113" spans="52:52">
       <c r="AZ113">
         <v>9</v>
       </c>
@@ -12732,20 +12963,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BE11"/>
+  <dimension ref="A2:BF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BE3" sqref="BE3:BE11"/>
+    <sheetView topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BF11" sqref="BF11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -12917,8 +13148,11 @@
       <c r="BE2" s="9">
         <v>43976</v>
       </c>
+      <c r="BF2" s="9">
+        <v>43977</v>
+      </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -13090,8 +13324,11 @@
       <c r="BE3">
         <v>1166</v>
       </c>
+      <c r="BF3">
+        <v>1178</v>
+      </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -13263,8 +13500,11 @@
       <c r="BE4">
         <v>508</v>
       </c>
+      <c r="BF4">
+        <v>509</v>
+      </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -13436,8 +13676,11 @@
       <c r="BE5">
         <v>410</v>
       </c>
+      <c r="BF5">
+        <v>411</v>
+      </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -13609,8 +13852,11 @@
       <c r="BE6">
         <v>1759</v>
       </c>
+      <c r="BF6">
+        <v>1771</v>
+      </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -13782,8 +14028,11 @@
       <c r="BE7">
         <v>1303</v>
       </c>
+      <c r="BF7">
+        <v>1315</v>
+      </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -13955,8 +14204,11 @@
       <c r="BE8">
         <v>709</v>
       </c>
+      <c r="BF8">
+        <v>713</v>
+      </c>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -14128,8 +14380,11 @@
       <c r="BE9">
         <v>1194</v>
       </c>
+      <c r="BF9">
+        <v>1204</v>
+      </c>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -14301,8 +14556,11 @@
       <c r="BE10">
         <v>1156</v>
       </c>
+      <c r="BF10">
+        <v>1174</v>
+      </c>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -14473,6 +14731,9 @@
       </c>
       <c r="BE11">
         <v>129</v>
+      </c>
+      <c r="BF11">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -14483,20 +14744,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:AZ17"/>
+  <dimension ref="A2:BA17"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AZ13" sqref="AZ13"/>
+    <sheetView topLeftCell="AQ9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BA17" sqref="BA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -14651,8 +14912,11 @@
       <c r="AZ2" s="9">
         <v>43976</v>
       </c>
+      <c r="BA2" s="9">
+        <v>43977</v>
+      </c>
     </row>
-    <row r="3" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -14660,7 +14924,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -14817,8 +15081,11 @@
       <c r="AZ4">
         <v>8334</v>
       </c>
+      <c r="BA4">
+        <v>8406</v>
+      </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -14975,8 +15242,11 @@
       <c r="AZ5">
         <v>1010</v>
       </c>
+      <c r="BA5">
+        <v>1028</v>
+      </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -15133,8 +15403,11 @@
       <c r="AZ6">
         <v>1282</v>
       </c>
+      <c r="BA6">
+        <v>1293</v>
+      </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -15291,8 +15564,11 @@
       <c r="AZ7">
         <v>3822</v>
       </c>
+      <c r="BA7">
+        <v>3839</v>
+      </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -15449,8 +15725,11 @@
       <c r="AZ8">
         <v>104</v>
       </c>
+      <c r="BA8">
+        <v>104</v>
+      </c>
     </row>
-    <row r="9" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" ht="28.8">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -15607,8 +15886,11 @@
       <c r="AZ9">
         <v>23</v>
       </c>
+      <c r="BA9">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" ht="28.8">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -15761,8 +16043,11 @@
       <c r="AZ10">
         <v>20</v>
       </c>
+      <c r="BA10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -15919,8 +16204,11 @@
       <c r="AZ11">
         <v>2027</v>
       </c>
+      <c r="BA11">
+        <v>2051</v>
+      </c>
     </row>
-    <row r="12" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -16077,8 +16365,11 @@
       <c r="AZ12">
         <v>46</v>
       </c>
+      <c r="BA12">
+        <v>47</v>
+      </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -16089,7 +16380,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -16246,8 +16537,11 @@
       <c r="AZ14">
         <v>1593</v>
       </c>
+      <c r="BA14">
+        <v>1612</v>
+      </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -16404,8 +16698,11 @@
       <c r="AZ15">
         <v>2115</v>
       </c>
+      <c r="BA15">
+        <v>2138</v>
+      </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -16562,8 +16859,11 @@
       <c r="AZ16">
         <v>4600</v>
       </c>
+      <c r="BA16">
+        <v>4630</v>
+      </c>
     </row>
-    <row r="17" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -16718,6 +17018,9 @@
         <v>26</v>
       </c>
       <c r="AZ17">
+        <v>26</v>
+      </c>
+      <c r="BA17">
         <v>26</v>
       </c>
     </row>
@@ -16729,19 +17032,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AZ9"/>
+  <dimension ref="A1:BA9"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AZ3" sqref="AZ3:AZ8"/>
+      <selection activeCell="BA8" sqref="BA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -16895,14 +17198,17 @@
       <c r="AZ1" s="9">
         <v>43976</v>
       </c>
+      <c r="BA1" s="9">
+        <v>43977</v>
+      </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -17060,8 +17366,11 @@
       <c r="AZ3">
         <v>440</v>
       </c>
+      <c r="BA3">
+        <v>445</v>
+      </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -17218,8 +17527,11 @@
       <c r="AZ4">
         <v>7</v>
       </c>
+      <c r="BA4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" ht="28.8">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -17376,8 +17688,11 @@
       <c r="AZ5">
         <v>333</v>
       </c>
+      <c r="BA5">
+        <v>335</v>
+      </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -17534,8 +17849,11 @@
       <c r="AZ6">
         <v>47</v>
       </c>
+      <c r="BA6">
+        <v>49</v>
+      </c>
     </row>
-    <row r="7" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -17692,8 +18010,11 @@
       <c r="AZ7">
         <v>49</v>
       </c>
+      <c r="BA7">
+        <v>50</v>
+      </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -17850,8 +18171,11 @@
       <c r="AZ8">
         <v>4</v>
       </c>
+      <c r="BA8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -17863,18 +18187,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AL13"/>
+  <dimension ref="A2:AM13"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AL13" sqref="AL13"/>
+    <sheetView topLeftCell="AE4" workbookViewId="0">
+      <selection activeCell="AM13" sqref="AM13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -17989,8 +18313,11 @@
       <c r="AL2" s="9">
         <v>43976</v>
       </c>
+      <c r="AM2" s="9">
+        <v>43977</v>
+      </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -18105,8 +18432,11 @@
       <c r="AL3">
         <v>440</v>
       </c>
+      <c r="AM3">
+        <v>445</v>
+      </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -18221,8 +18551,11 @@
       <c r="AL4">
         <v>43</v>
       </c>
+      <c r="AM4">
+        <v>45</v>
+      </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -18337,8 +18670,11 @@
       <c r="AL5">
         <v>27</v>
       </c>
+      <c r="AM5">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -18453,8 +18789,11 @@
       <c r="AL6">
         <v>30</v>
       </c>
+      <c r="AM6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -18569,8 +18908,11 @@
       <c r="AL7">
         <v>62</v>
       </c>
+      <c r="AM7">
+        <v>63</v>
+      </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -18685,8 +19027,11 @@
       <c r="AL8">
         <v>68</v>
       </c>
+      <c r="AM8">
+        <v>69</v>
+      </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -18801,8 +19146,11 @@
       <c r="AL9">
         <v>41</v>
       </c>
+      <c r="AM9">
+        <v>41</v>
+      </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -18917,8 +19265,11 @@
       <c r="AL10">
         <v>62</v>
       </c>
+      <c r="AM10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -19033,8 +19384,11 @@
       <c r="AL11">
         <v>91</v>
       </c>
+      <c r="AM11">
+        <v>92</v>
+      </c>
     </row>
-    <row r="12" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" ht="28.8">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -19149,8 +19503,11 @@
       <c r="AL12">
         <v>16</v>
       </c>
+      <c r="AM12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -19263,6 +19620,9 @@
         <v>0</v>
       </c>
       <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
         <v>0</v>
       </c>
     </row>
@@ -19276,63 +19636,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C1" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+    <row r="1" spans="1:15">
+      <c r="C1" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+    <row r="2" spans="1:15">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+    <row r="3" spans="1:15">
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -19347,7 +19707,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -19366,10 +19726,13 @@
       <c r="H5" s="9">
         <v>43976</v>
       </c>
+      <c r="I5" s="9">
+        <v>43977</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C6">
         <v>103</v>
@@ -19389,8 +19752,11 @@
       <c r="H6">
         <v>107</v>
       </c>
+      <c r="I6">
+        <v>107</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -19412,13 +19778,16 @@
       <c r="H7">
         <v>28</v>
       </c>
+      <c r="I7">
+        <v>28</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -19440,10 +19809,13 @@
       <c r="H9">
         <v>1</v>
       </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C10">
         <v>18</v>
@@ -19463,10 +19835,13 @@
       <c r="H10">
         <v>20</v>
       </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -19486,8 +19861,11 @@
       <c r="H11">
         <v>5</v>
       </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -19509,13 +19887,16 @@
       <c r="H12">
         <v>2</v>
       </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -19537,8 +19918,11 @@
       <c r="H14">
         <v>1</v>
       </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -19560,8 +19944,11 @@
       <c r="H15">
         <v>0</v>
       </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -19583,8 +19970,11 @@
       <c r="H16">
         <v>2</v>
       </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -19606,8 +19996,11 @@
       <c r="H17">
         <v>8</v>
       </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -19629,8 +20022,11 @@
       <c r="H18">
         <v>2</v>
       </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -19652,8 +20048,11 @@
       <c r="H19">
         <v>2</v>
       </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -19675,8 +20074,11 @@
       <c r="H20">
         <v>3</v>
       </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -19698,8 +20100,11 @@
       <c r="H21">
         <v>5</v>
       </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="28.8">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -19721,10 +20126,13 @@
       <c r="H22">
         <v>4</v>
       </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
-        <v>147</v>
+    <row r="23" spans="1:9" ht="28.8">
+      <c r="A23" s="39" t="s">
+        <v>144</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -19742,6 +20150,9 @@
         <v>1</v>
       </c>
       <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
         <v>1</v>
       </c>
     </row>
@@ -19758,59 +20169,59 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+    <row r="1" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A1" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
     </row>
-    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:7" ht="36.6" customHeight="1">
+      <c r="A2" s="43" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="E2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="29" t="s">
-        <v>127</v>
-      </c>
       <c r="G2" s="29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
+    <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1">
+      <c r="A3" s="43"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="45"/>
+      <c r="D3" s="44"/>
       <c r="E3" s="25" t="s">
         <v>92</v>
       </c>
@@ -19821,11 +20232,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1">
+      <c r="A4" s="43"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="45"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="25" t="s">
         <v>86</v>
       </c>
@@ -19834,47 +20245,47 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1">
+      <c r="A5" s="43"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="45"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="25" t="s">
         <v>87</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1">
+      <c r="A6" s="43"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="45"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1">
+      <c r="A7" s="43"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="45"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="25" t="s">
         <v>93</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14.4" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="27">
+        <v>135</v>
+      </c>
+      <c r="C8" s="28">
         <v>3</v>
       </c>
       <c r="D8" s="28">
@@ -19890,14 +20301,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="14.4" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>96</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="27">
+        <v>126</v>
+      </c>
+      <c r="C9" s="28">
         <v>4</v>
       </c>
       <c r="D9" s="28">
@@ -19913,44 +20324,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="14.4" customHeight="1">
       <c r="A10" s="27" t="s">
         <v>98</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="27">
+        <v>136</v>
+      </c>
+      <c r="C10" s="28">
         <v>4</v>
       </c>
       <c r="D10" s="28">
         <v>0</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F10" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="14.4" customHeight="1">
       <c r="A11" s="27" t="s">
         <v>99</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="27">
+        <v>137</v>
+      </c>
+      <c r="C11" s="28">
         <v>13</v>
       </c>
       <c r="D11" s="28">
         <v>0</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
@@ -19959,14 +20370,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="14.4" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>100</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="28">
         <v>0</v>
       </c>
       <c r="D12" s="28">
@@ -19982,14 +20393,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="14.4" customHeight="1">
       <c r="A13" s="27" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="28">
         <v>0</v>
       </c>
       <c r="D13" s="28">
@@ -20005,14 +20416,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="14.4" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>103</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="27">
+        <v>127</v>
+      </c>
+      <c r="C14" s="28">
         <v>3</v>
       </c>
       <c r="D14" s="28">
@@ -20028,22 +20439,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="14.4" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>104</v>
       </c>
       <c r="B15" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="28">
+        <v>14</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0</v>
+      </c>
+      <c r="E15" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="27">
-        <v>14</v>
-      </c>
-      <c r="D15" s="28">
-        <v>0</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>153</v>
-      </c>
       <c r="F15" s="28">
         <v>1</v>
       </c>
@@ -20051,14 +20462,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1">
       <c r="A16" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="28">
         <v>4</v>
       </c>
       <c r="D16" s="28">
@@ -20074,21 +20485,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="14.4" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>107</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="28">
         <v>9</v>
       </c>
       <c r="D17" s="28">
         <v>0</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F17" s="28">
         <v>1</v>
@@ -20097,21 +20508,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14.4" customHeight="1">
       <c r="A18" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" s="27">
+        <v>138</v>
+      </c>
+      <c r="C18" s="28">
         <v>12</v>
       </c>
       <c r="D18" s="28">
         <v>0</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F18" s="28">
         <v>0</v>
@@ -20120,21 +20531,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14.4" customHeight="1">
       <c r="A19" s="27" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="C19" s="27">
+        <v>139</v>
+      </c>
+      <c r="C19" s="28">
         <v>10</v>
       </c>
       <c r="D19" s="28">
         <v>0</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
@@ -20143,14 +20554,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="14.4" customHeight="1">
       <c r="A20" s="27" t="s">
         <v>111</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" s="27">
+        <v>151</v>
+      </c>
+      <c r="C20" s="28">
         <v>17</v>
       </c>
       <c r="D20" s="28">
@@ -20166,14 +20577,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="14.4" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>112</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="28">
         <v>1</v>
       </c>
       <c r="D21" s="28">
@@ -20189,37 +20600,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="14.4" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>115</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="27">
-        <v>24</v>
+        <v>157</v>
+      </c>
+      <c r="C22" s="28">
+        <v>25</v>
       </c>
       <c r="D22" s="28">
         <v>0</v>
       </c>
       <c r="E22" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="28">
+        <v>1</v>
+      </c>
+      <c r="G22" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A23" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="28">
-        <v>1</v>
-      </c>
-      <c r="G22" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+      <c r="B23" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="27">
+      <c r="C23" s="28">
         <v>6</v>
       </c>
       <c r="D23" s="28">
@@ -20235,14 +20646,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="18" customHeight="1">
       <c r="A24" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" s="27">
+        <v>159</v>
+      </c>
+      <c r="C24" s="28">
         <v>7</v>
       </c>
       <c r="D24" s="28">
@@ -20258,21 +20669,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="33.6" customHeight="1">
       <c r="A25" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="27">
+      <c r="C25" s="28">
         <v>18</v>
       </c>
       <c r="D25" s="28">
         <v>0</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F25" s="28">
         <v>1</v>
@@ -20281,35 +20692,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1">
       <c r="A26" s="30" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="27">
-        <v>149</v>
+        <v>160</v>
+      </c>
+      <c r="C26" s="28">
+        <v>150</v>
       </c>
       <c r="D26" s="28">
         <v>0</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F26" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G26" s="28">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.6">
       <c r="A27" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>154</v>
+        <v>120</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>162</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -20317,7 +20728,7 @@
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
@@ -20577,16 +20988,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
28 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{C5E88C75-E440-43B4-B034-AA36176F93AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4A528D01-D78E-4B25-B78E-AAD36C8A6AEC}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="23040" windowHeight="7296" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="20730" windowHeight="7290" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId6"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -450,13 +444,7 @@
     <t>23; (8)</t>
   </si>
   <si>
-    <t>56; (47)</t>
-  </si>
-  <si>
     <t>44; (28)</t>
-  </si>
-  <si>
-    <t>45; (33)</t>
   </si>
   <si>
     <t>21; (17)</t>
@@ -501,35 +489,6 @@
     <t>Total Overall Tested</t>
   </si>
   <si>
-    <t>As of May 26, 2020</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As of May 26, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>107 cases</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for COVID-19 testing,  and 28 (26.2%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
-    </r>
-  </si>
-  <si>
     <t>20; (3)</t>
   </si>
   <si>
@@ -542,19 +501,54 @@
     <t>21; (8)</t>
   </si>
   <si>
-    <t>599; (283)</t>
-  </si>
-  <si>
     <t>194; (78)</t>
   </si>
   <si>
-    <t>793; (361)</t>
+    <t>As of May 27, 2020</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As of May 27, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>113 cases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for COVID-19 testing,  and 30 (26.5%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
+    </r>
+  </si>
+  <si>
+    <t>96; (47)</t>
+  </si>
+  <si>
+    <t>58; (33)</t>
+  </si>
+  <si>
+    <t>652; (283)</t>
+  </si>
+  <si>
+    <t>846; (361)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -768,6 +762,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -782,9 +779,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,7 +817,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1158,34 +1152,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE113"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CF113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CE93" sqref="CE1:CE1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="CA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CH3" sqref="CH3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" customWidth="1"/>
-    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="80" max="83" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="84" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83">
+    <row r="1" spans="1:84">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1429,8 +1423,11 @@
       <c r="CE1" s="1">
         <v>43977</v>
       </c>
+      <c r="CF1" s="1">
+        <v>43978</v>
+      </c>
     </row>
-    <row r="2" spans="1:83">
+    <row r="2" spans="1:84">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1454,12 +1451,12 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:83">
+    <row r="3" spans="1:84">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I3">
         <v>69</v>
@@ -1683,13 +1680,16 @@
       <c r="CE3">
         <v>42697</v>
       </c>
+      <c r="CF3">
+        <v>43514</v>
+      </c>
     </row>
-    <row r="4" spans="1:83">
+    <row r="4" spans="1:84">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AN4" s="19"/>
       <c r="AO4" s="20"/>
@@ -1708,8 +1708,11 @@
       <c r="CE4">
         <v>35682</v>
       </c>
+      <c r="CF4">
+        <v>36284</v>
+      </c>
     </row>
-    <row r="5" spans="1:83">
+    <row r="5" spans="1:84">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1959,8 +1962,11 @@
       <c r="CE5">
         <v>8406</v>
       </c>
+      <c r="CF5">
+        <v>8492</v>
+      </c>
     </row>
-    <row r="6" spans="1:83">
+    <row r="6" spans="1:84">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2192,13 +2198,16 @@
       <c r="CE6">
         <v>445</v>
       </c>
+      <c r="CF6">
+        <v>453</v>
+      </c>
     </row>
-    <row r="7" spans="1:83">
+    <row r="7" spans="1:84">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="S7">
         <v>17</v>
@@ -2395,11 +2404,14 @@
       <c r="CE7">
         <v>1082</v>
       </c>
+      <c r="CF7">
+        <v>1082</v>
+      </c>
     </row>
-    <row r="8" spans="1:83">
+    <row r="8" spans="1:84">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:83">
+    <row r="9" spans="1:84">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2493,8 +2505,11 @@
       <c r="CE9">
         <v>345</v>
       </c>
+      <c r="CF9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:83">
+    <row r="10" spans="1:84">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2690,8 +2705,11 @@
       <c r="CE10">
         <v>80</v>
       </c>
+      <c r="CF10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="11" spans="1:83">
+    <row r="11" spans="1:84">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2887,8 +2905,11 @@
       <c r="CE11">
         <v>440</v>
       </c>
+      <c r="CF11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:83">
+    <row r="12" spans="1:84">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3084,8 +3105,11 @@
       <c r="CE12">
         <v>214</v>
       </c>
+      <c r="CF12">
+        <v>218</v>
+      </c>
     </row>
-    <row r="13" spans="1:83">
+    <row r="13" spans="1:84">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3281,8 +3305,11 @@
       <c r="CE13">
         <v>226</v>
       </c>
+      <c r="CF13">
+        <v>222</v>
+      </c>
     </row>
-    <row r="14" spans="1:83">
+    <row r="14" spans="1:84">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3340,13 +3367,16 @@
       <c r="CE14">
         <v>349</v>
       </c>
+      <c r="CF14">
+        <v>343</v>
+      </c>
     </row>
-    <row r="15" spans="1:83">
+    <row r="15" spans="1:84">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="BY15">
         <v>110</v>
@@ -3369,8 +3399,11 @@
       <c r="CE15">
         <v>113</v>
       </c>
+      <c r="CF15">
+        <v>108</v>
+      </c>
     </row>
-    <row r="16" spans="1:83">
+    <row r="16" spans="1:84">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3428,8 +3461,11 @@
       <c r="CE16">
         <v>1851</v>
       </c>
+      <c r="CF16">
+        <v>1939</v>
+      </c>
     </row>
-    <row r="17" spans="1:83">
+    <row r="17" spans="1:84">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3487,13 +3523,16 @@
       <c r="CE17" s="23">
         <v>0.74</v>
       </c>
+      <c r="CF17" s="23">
+        <v>0.78</v>
+      </c>
     </row>
-    <row r="19" spans="1:83">
+    <row r="19" spans="1:84">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:83">
+    <row r="20" spans="1:84">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3501,7 +3540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:83">
+    <row r="21" spans="1:84">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3700,8 +3739,11 @@
       <c r="CE21">
         <v>107</v>
       </c>
+      <c r="CF21">
+        <v>107</v>
+      </c>
     </row>
-    <row r="22" spans="1:83">
+    <row r="22" spans="1:84">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3846,8 +3888,11 @@
       <c r="CE22">
         <v>18</v>
       </c>
+      <c r="CF22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:83">
+    <row r="23" spans="1:84">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3992,8 +4037,11 @@
       <c r="CE23">
         <v>89</v>
       </c>
+      <c r="CF23">
+        <v>89</v>
+      </c>
     </row>
-    <row r="24" spans="1:83">
+    <row r="24" spans="1:84">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4183,8 +4231,11 @@
       <c r="CE24">
         <v>161</v>
       </c>
+      <c r="CF24">
+        <v>154</v>
+      </c>
     </row>
-    <row r="25" spans="1:83">
+    <row r="25" spans="1:84">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4374,8 +4425,11 @@
       <c r="CE25">
         <v>179</v>
       </c>
+      <c r="CF25">
+        <v>172</v>
+      </c>
     </row>
-    <row r="26" spans="1:83">
+    <row r="26" spans="1:84">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4565,13 +4619,16 @@
       <c r="CE26">
         <v>1312</v>
       </c>
+      <c r="CF26">
+        <v>1324</v>
+      </c>
     </row>
-    <row r="28" spans="1:83">
+    <row r="28" spans="1:84">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:83">
+    <row r="29" spans="1:84">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4770,8 +4827,11 @@
       <c r="CE29">
         <v>131</v>
       </c>
+      <c r="CF29">
+        <v>132</v>
+      </c>
     </row>
-    <row r="30" spans="1:83">
+    <row r="30" spans="1:84">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4916,8 +4976,11 @@
       <c r="CE30">
         <v>33</v>
       </c>
+      <c r="CF30">
+        <v>31</v>
+      </c>
     </row>
-    <row r="31" spans="1:83">
+    <row r="31" spans="1:84">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5062,8 +5125,11 @@
       <c r="CE31">
         <v>98</v>
       </c>
+      <c r="CF31">
+        <v>101</v>
+      </c>
     </row>
-    <row r="32" spans="1:83">
+    <row r="32" spans="1:84">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5253,8 +5319,11 @@
       <c r="CE32">
         <v>63</v>
       </c>
+      <c r="CF32">
+        <v>59</v>
+      </c>
     </row>
-    <row r="33" spans="1:83">
+    <row r="33" spans="1:84">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5444,8 +5513,11 @@
       <c r="CE33">
         <v>96</v>
       </c>
+      <c r="CF33">
+        <v>90</v>
+      </c>
     </row>
-    <row r="34" spans="1:83">
+    <row r="34" spans="1:84">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -5635,13 +5707,16 @@
       <c r="CE34">
         <v>1156</v>
       </c>
+      <c r="CF34">
+        <v>1178</v>
+      </c>
     </row>
-    <row r="36" spans="1:83">
+    <row r="36" spans="1:84">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:83">
+    <row r="37" spans="1:84">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5828,8 +5903,11 @@
       <c r="CE37">
         <v>80</v>
       </c>
+      <c r="CF37">
+        <v>80</v>
+      </c>
     </row>
-    <row r="38" spans="1:83">
+    <row r="38" spans="1:84">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -5968,8 +6046,11 @@
       <c r="CE38">
         <v>17</v>
       </c>
+      <c r="CF38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:83">
+    <row r="39" spans="1:84">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6108,8 +6189,11 @@
       <c r="CE39">
         <v>62</v>
       </c>
+      <c r="CF39">
+        <v>73</v>
+      </c>
     </row>
-    <row r="40" spans="1:83">
+    <row r="40" spans="1:84">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6293,8 +6377,11 @@
       <c r="CE40">
         <v>1</v>
       </c>
+      <c r="CF40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:83">
+    <row r="41" spans="1:84">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6475,8 +6562,11 @@
       <c r="CE41">
         <v>18</v>
       </c>
+      <c r="CF41">
+        <v>7</v>
+      </c>
     </row>
-    <row r="42" spans="1:83">
+    <row r="42" spans="1:84">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -6663,8 +6753,11 @@
       <c r="CE42">
         <v>270</v>
       </c>
+      <c r="CF42">
+        <v>281</v>
+      </c>
     </row>
-    <row r="43" spans="1:83">
+    <row r="43" spans="1:84">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -6785,16 +6878,19 @@
       <c r="CE43">
         <v>1</v>
       </c>
+      <c r="CF43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:83">
+    <row r="44" spans="1:84">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:83">
+    <row r="45" spans="1:84">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:83">
+    <row r="46" spans="1:84">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -6987,8 +7083,11 @@
       <c r="CE46">
         <v>193</v>
       </c>
+      <c r="CF46">
+        <v>205</v>
+      </c>
     </row>
-    <row r="47" spans="1:83">
+    <row r="47" spans="1:84">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7133,8 +7232,11 @@
       <c r="CE47">
         <v>17</v>
       </c>
+      <c r="CF47">
+        <v>25</v>
+      </c>
     </row>
-    <row r="48" spans="1:83">
+    <row r="48" spans="1:84">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7279,8 +7381,11 @@
       <c r="CE48">
         <v>170</v>
       </c>
+      <c r="CF48">
+        <v>174</v>
+      </c>
     </row>
-    <row r="49" spans="1:83">
+    <row r="49" spans="1:84">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -7470,8 +7575,11 @@
       <c r="CE49">
         <v>517</v>
       </c>
+      <c r="CF49">
+        <v>619</v>
+      </c>
     </row>
-    <row r="50" spans="1:83">
+    <row r="50" spans="1:84">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -7616,8 +7724,11 @@
       <c r="CE50">
         <v>534</v>
       </c>
+      <c r="CF50">
+        <v>644</v>
+      </c>
     </row>
-    <row r="51" spans="1:83">
+    <row r="51" spans="1:84">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -7759,8 +7870,11 @@
       <c r="CE51">
         <v>813</v>
       </c>
+      <c r="CF51">
+        <v>708</v>
+      </c>
     </row>
-    <row r="52" spans="1:83">
+    <row r="52" spans="1:84">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -7896,16 +8010,19 @@
       <c r="CE52">
         <v>1</v>
       </c>
+      <c r="CF52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:83">
+    <row r="53" spans="1:84">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:83">
+    <row r="54" spans="1:84">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:83">
+    <row r="55" spans="1:84">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -8083,8 +8200,11 @@
       <c r="CE55">
         <v>30</v>
       </c>
+      <c r="CF55">
+        <v>30</v>
+      </c>
     </row>
-    <row r="56" spans="1:83">
+    <row r="56" spans="1:84">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -8226,8 +8346,11 @@
       <c r="CE56">
         <v>11</v>
       </c>
+      <c r="CF56">
+        <v>10</v>
+      </c>
     </row>
-    <row r="57" spans="1:83">
+    <row r="57" spans="1:84">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -8369,8 +8492,11 @@
       <c r="CE57">
         <v>19</v>
       </c>
+      <c r="CF57">
+        <v>19</v>
+      </c>
     </row>
-    <row r="58" spans="1:83">
+    <row r="58" spans="1:84">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -8548,8 +8674,11 @@
       <c r="CE58">
         <v>20</v>
       </c>
+      <c r="CF58">
+        <v>21</v>
+      </c>
     </row>
-    <row r="59" spans="1:83">
+    <row r="59" spans="1:84">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -8727,8 +8856,11 @@
       <c r="CE59">
         <v>31</v>
       </c>
+      <c r="CF59">
+        <v>31</v>
+      </c>
     </row>
-    <row r="60" spans="1:83">
+    <row r="60" spans="1:84">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -8906,8 +9038,11 @@
       <c r="CE60">
         <v>138</v>
       </c>
+      <c r="CF60">
+        <v>138</v>
+      </c>
     </row>
-    <row r="61" spans="1:83">
+    <row r="61" spans="1:84">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -9043,8 +9178,11 @@
       <c r="CE61">
         <v>1</v>
       </c>
+      <c r="CF61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:83">
+    <row r="63" spans="1:84">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -9222,8 +9360,11 @@
       <c r="CE63">
         <v>11</v>
       </c>
+      <c r="CF63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:83">
+    <row r="64" spans="1:84">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -9365,8 +9506,11 @@
       <c r="CE64">
         <v>4</v>
       </c>
+      <c r="CF64">
+        <v>4</v>
+      </c>
     </row>
-    <row r="65" spans="1:83">
+    <row r="65" spans="1:84">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -9508,8 +9652,11 @@
       <c r="CE65">
         <v>0</v>
       </c>
+      <c r="CF65">
+        <v>7</v>
+      </c>
     </row>
-    <row r="66" spans="1:83">
+    <row r="66" spans="1:84">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -9687,8 +9834,11 @@
       <c r="CE66">
         <v>46</v>
       </c>
+      <c r="CF66">
+        <v>46</v>
+      </c>
     </row>
-    <row r="67" spans="1:83">
+    <row r="67" spans="1:84">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -9867,8 +10017,11 @@
       <c r="CE67">
         <v>50</v>
       </c>
+      <c r="CF67">
+        <v>50</v>
+      </c>
     </row>
-    <row r="68" spans="1:83">
+    <row r="68" spans="1:84">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -10046,8 +10199,11 @@
       <c r="CE68">
         <v>0</v>
       </c>
+      <c r="CF68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:83">
+    <row r="69" spans="1:84">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -10189,11 +10345,14 @@
       <c r="CE69">
         <v>0</v>
       </c>
+      <c r="CF69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:83">
+    <row r="70" spans="1:84">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:83">
+    <row r="71" spans="1:84">
       <c r="A71" s="2" t="s">
         <v>134</v>
       </c>
@@ -10221,8 +10380,11 @@
       <c r="CE71">
         <v>10</v>
       </c>
+      <c r="CF71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:83">
+    <row r="72" spans="1:84">
       <c r="A72" s="2" t="s">
         <v>134</v>
       </c>
@@ -10250,8 +10412,11 @@
       <c r="CE72">
         <v>7</v>
       </c>
+      <c r="CF72">
+        <v>7</v>
+      </c>
     </row>
-    <row r="73" spans="1:83">
+    <row r="73" spans="1:84">
       <c r="A73" s="2" t="s">
         <v>134</v>
       </c>
@@ -10279,8 +10444,11 @@
       <c r="CE73">
         <v>3</v>
       </c>
+      <c r="CF73">
+        <v>3</v>
+      </c>
     </row>
-    <row r="74" spans="1:83">
+    <row r="74" spans="1:84">
       <c r="A74" s="2" t="s">
         <v>134</v>
       </c>
@@ -10308,8 +10476,11 @@
       <c r="CE74">
         <v>13</v>
       </c>
+      <c r="CF74">
+        <v>13</v>
+      </c>
     </row>
-    <row r="75" spans="1:83">
+    <row r="75" spans="1:84">
       <c r="A75" s="2" t="s">
         <v>134</v>
       </c>
@@ -10337,8 +10508,11 @@
       <c r="CE75">
         <v>20</v>
       </c>
+      <c r="CF75">
+        <v>20</v>
+      </c>
     </row>
-    <row r="76" spans="1:83">
+    <row r="76" spans="1:84">
       <c r="A76" s="2" t="s">
         <v>134</v>
       </c>
@@ -10366,13 +10540,16 @@
       <c r="CE76">
         <v>25</v>
       </c>
+      <c r="CF76">
+        <v>26</v>
+      </c>
     </row>
-    <row r="78" spans="1:83">
+    <row r="78" spans="1:84">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:83">
+    <row r="79" spans="1:84">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -10550,8 +10727,11 @@
       <c r="CE79">
         <v>294</v>
       </c>
+      <c r="CF79">
+        <v>295</v>
+      </c>
     </row>
-    <row r="80" spans="1:83">
+    <row r="80" spans="1:84">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -10729,8 +10909,11 @@
       <c r="CE80">
         <v>179</v>
       </c>
+      <c r="CF80">
+        <v>167</v>
+      </c>
     </row>
-    <row r="81" spans="1:83">
+    <row r="81" spans="1:84">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -10908,8 +11091,11 @@
       <c r="CE81">
         <v>150</v>
       </c>
+      <c r="CF81">
+        <v>135</v>
+      </c>
     </row>
-    <row r="82" spans="1:83">
+    <row r="82" spans="1:84">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -11045,8 +11231,11 @@
       <c r="CE82">
         <v>16</v>
       </c>
+      <c r="CF82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:83">
+    <row r="84" spans="1:84">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -11224,8 +11413,11 @@
       <c r="CE84">
         <v>115</v>
       </c>
+      <c r="CF84">
+        <v>116</v>
+      </c>
     </row>
-    <row r="85" spans="1:83">
+    <row r="85" spans="1:84">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -11403,8 +11595,11 @@
       <c r="CE85">
         <v>3</v>
       </c>
+      <c r="CF85">
+        <v>26</v>
+      </c>
     </row>
-    <row r="86" spans="1:83">
+    <row r="86" spans="1:84">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -11582,8 +11777,11 @@
       <c r="CE86">
         <v>118</v>
       </c>
+      <c r="CF86">
+        <v>142</v>
+      </c>
     </row>
-    <row r="87" spans="1:83">
+    <row r="87" spans="1:84">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -11761,8 +11959,11 @@
       <c r="CE87">
         <v>180</v>
       </c>
+      <c r="CF87">
+        <v>186</v>
+      </c>
     </row>
-    <row r="88" spans="1:83">
+    <row r="88" spans="1:84">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -11814,8 +12015,11 @@
       <c r="CE88">
         <v>1</v>
       </c>
+      <c r="CF88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:83">
+    <row r="90" spans="1:84">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -11993,8 +12197,11 @@
       <c r="CE90">
         <v>79</v>
       </c>
+      <c r="CF90">
+        <v>79</v>
+      </c>
     </row>
-    <row r="91" spans="1:83">
+    <row r="91" spans="1:84">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -12172,8 +12379,11 @@
       <c r="CE91">
         <v>49</v>
       </c>
+      <c r="CF91">
+        <v>31</v>
+      </c>
     </row>
-    <row r="92" spans="1:83">
+    <row r="92" spans="1:84">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -12339,8 +12549,11 @@
       <c r="CE92">
         <v>130</v>
       </c>
+      <c r="CF92">
+        <v>163</v>
+      </c>
     </row>
-    <row r="93" spans="1:83">
+    <row r="93" spans="1:84">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -12518,8 +12731,11 @@
       <c r="CE93">
         <v>13</v>
       </c>
+      <c r="CF93">
+        <v>32</v>
+      </c>
     </row>
-    <row r="94" spans="1:83">
+    <row r="94" spans="1:84">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -12655,8 +12871,11 @@
       <c r="CE94">
         <v>13</v>
       </c>
+      <c r="CF94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:83">
+    <row r="96" spans="1:84">
       <c r="A96" s="2" t="s">
         <v>79</v>
       </c>
@@ -12753,8 +12972,11 @@
       <c r="CE96">
         <v>182</v>
       </c>
+      <c r="CF96">
+        <v>183</v>
+      </c>
     </row>
-    <row r="97" spans="1:83">
+    <row r="97" spans="1:84">
       <c r="A97" s="2" t="s">
         <v>79</v>
       </c>
@@ -12851,8 +13073,11 @@
       <c r="CE97">
         <v>47</v>
       </c>
+      <c r="CF97">
+        <v>49</v>
+      </c>
     </row>
-    <row r="98" spans="1:83">
+    <row r="98" spans="1:84">
       <c r="A98" s="2" t="s">
         <v>79</v>
       </c>
@@ -12947,6 +13172,9 @@
         <v>25</v>
       </c>
       <c r="CE98">
+        <v>25</v>
+      </c>
+      <c r="CF98">
         <v>25</v>
       </c>
     </row>
@@ -12962,21 +13190,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BF11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:BG11"/>
   <sheetViews>
-    <sheetView topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BF11" sqref="BF11"/>
+    <sheetView topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BI5" sqref="BI5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:58" s="2" customFormat="1">
+    <row r="2" spans="1:59" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -13151,8 +13379,11 @@
       <c r="BF2" s="9">
         <v>43977</v>
       </c>
+      <c r="BG2" s="9">
+        <v>43978</v>
+      </c>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:59">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -13327,8 +13558,11 @@
       <c r="BF3">
         <v>1178</v>
       </c>
+      <c r="BG3">
+        <v>1188</v>
+      </c>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:59">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -13503,8 +13737,11 @@
       <c r="BF4">
         <v>509</v>
       </c>
+      <c r="BG4">
+        <v>511</v>
+      </c>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:59">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -13679,8 +13916,11 @@
       <c r="BF5">
         <v>411</v>
       </c>
+      <c r="BG5">
+        <v>413</v>
+      </c>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:59">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -13855,8 +14095,11 @@
       <c r="BF6">
         <v>1771</v>
       </c>
+      <c r="BG6">
+        <v>1785</v>
+      </c>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:59">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -14031,8 +14274,11 @@
       <c r="BF7">
         <v>1315</v>
       </c>
+      <c r="BG7">
+        <v>1327</v>
+      </c>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:59">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -14207,8 +14453,11 @@
       <c r="BF8">
         <v>713</v>
       </c>
+      <c r="BG8">
+        <v>722</v>
+      </c>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:59">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -14383,8 +14632,11 @@
       <c r="BF9">
         <v>1204</v>
       </c>
+      <c r="BG9">
+        <v>1219</v>
+      </c>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:59">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -14559,8 +14811,11 @@
       <c r="BF10">
         <v>1174</v>
       </c>
+      <c r="BG10">
+        <v>1191</v>
+      </c>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:59">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -14734,6 +14989,9 @@
       </c>
       <c r="BF11">
         <v>131</v>
+      </c>
+      <c r="BG11">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -14743,21 +15001,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BA17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:BB17"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BA17" sqref="BA17"/>
+    <sheetView topLeftCell="AT1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC3" sqref="BC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:53" s="2" customFormat="1">
+    <row r="2" spans="1:54" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -14915,8 +15173,11 @@
       <c r="BA2" s="9">
         <v>43977</v>
       </c>
+      <c r="BB2" s="9">
+        <v>43978</v>
+      </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1">
+    <row r="3" spans="1:54" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -14924,7 +15185,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:54">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -15084,8 +15345,11 @@
       <c r="BA4">
         <v>8406</v>
       </c>
+      <c r="BB4">
+        <v>8492</v>
+      </c>
     </row>
-    <row r="5" spans="1:53">
+    <row r="5" spans="1:54">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -15245,8 +15509,11 @@
       <c r="BA5">
         <v>1028</v>
       </c>
+      <c r="BB5">
+        <v>1006</v>
+      </c>
     </row>
-    <row r="6" spans="1:53">
+    <row r="6" spans="1:54">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -15406,8 +15673,11 @@
       <c r="BA6">
         <v>1293</v>
       </c>
+      <c r="BB6">
+        <v>1300</v>
+      </c>
     </row>
-    <row r="7" spans="1:53">
+    <row r="7" spans="1:54">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -15567,8 +15837,11 @@
       <c r="BA7">
         <v>3839</v>
       </c>
+      <c r="BB7">
+        <v>3896</v>
+      </c>
     </row>
-    <row r="8" spans="1:53">
+    <row r="8" spans="1:54">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -15728,8 +16001,11 @@
       <c r="BA8">
         <v>104</v>
       </c>
+      <c r="BB8">
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:53" ht="28.8">
+    <row r="9" spans="1:54" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -15889,8 +16165,11 @@
       <c r="BA9">
         <v>24</v>
       </c>
+      <c r="BB9">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="1:53" ht="28.8">
+    <row r="10" spans="1:54" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -16046,8 +16325,11 @@
       <c r="BA10">
         <v>20</v>
       </c>
+      <c r="BB10">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="1:53">
+    <row r="11" spans="1:54">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -16207,8 +16489,11 @@
       <c r="BA11">
         <v>2051</v>
       </c>
+      <c r="BB11">
+        <v>2092</v>
+      </c>
     </row>
-    <row r="12" spans="1:53">
+    <row r="12" spans="1:54" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -16368,8 +16653,11 @@
       <c r="BA12">
         <v>47</v>
       </c>
+      <c r="BB12">
+        <v>48</v>
+      </c>
     </row>
-    <row r="13" spans="1:53">
+    <row r="13" spans="1:54">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -16380,7 +16668,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:53">
+    <row r="14" spans="1:54">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -16540,8 +16828,11 @@
       <c r="BA14">
         <v>1612</v>
       </c>
+      <c r="BB14">
+        <v>1618</v>
+      </c>
     </row>
-    <row r="15" spans="1:53">
+    <row r="15" spans="1:54">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -16701,8 +16992,11 @@
       <c r="BA15">
         <v>2138</v>
       </c>
+      <c r="BB15">
+        <v>2173</v>
+      </c>
     </row>
-    <row r="16" spans="1:53">
+    <row r="16" spans="1:54">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -16862,8 +17156,11 @@
       <c r="BA16">
         <v>4630</v>
       </c>
+      <c r="BB16">
+        <v>4674</v>
+      </c>
     </row>
-    <row r="17" spans="1:53">
+    <row r="17" spans="1:54" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -17022,6 +17319,9 @@
       </c>
       <c r="BA17">
         <v>26</v>
+      </c>
+      <c r="BB17">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -17031,20 +17331,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BA9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BB9"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BA8" sqref="BA8"/>
+    <sheetView topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BD3" sqref="BD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="2" customFormat="1">
+    <row r="1" spans="1:54" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -17201,14 +17501,17 @@
       <c r="BA1" s="9">
         <v>43977</v>
       </c>
+      <c r="BB1" s="9">
+        <v>43978</v>
+      </c>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:54">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:54">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -17369,8 +17672,11 @@
       <c r="BA3">
         <v>445</v>
       </c>
+      <c r="BB3">
+        <v>453</v>
+      </c>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:54">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -17530,8 +17836,11 @@
       <c r="BA4">
         <v>7</v>
       </c>
+      <c r="BB4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:53" ht="28.8">
+    <row r="5" spans="1:54" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -17691,8 +18000,11 @@
       <c r="BA5">
         <v>335</v>
       </c>
+      <c r="BB5">
+        <v>339</v>
+      </c>
     </row>
-    <row r="6" spans="1:53">
+    <row r="6" spans="1:54">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -17852,8 +18164,11 @@
       <c r="BA6">
         <v>49</v>
       </c>
+      <c r="BB6">
+        <v>51</v>
+      </c>
     </row>
-    <row r="7" spans="1:53">
+    <row r="7" spans="1:54" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -18013,8 +18328,11 @@
       <c r="BA7">
         <v>50</v>
       </c>
+      <c r="BB7">
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="1:53">
+    <row r="8" spans="1:54">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -18174,10 +18492,16 @@
       <c r="BA8">
         <v>4</v>
       </c>
+      <c r="BB8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:53">
+    <row r="9" spans="1:54">
       <c r="A9" s="33" t="s">
         <v>48</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -18186,19 +18510,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AM13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AN13"/>
   <sheetViews>
-    <sheetView topLeftCell="AE4" workbookViewId="0">
-      <selection activeCell="AM13" sqref="AM13"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AP3" sqref="AP3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:39" s="2" customFormat="1">
+    <row r="2" spans="1:40" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -18316,8 +18640,11 @@
       <c r="AM2" s="9">
         <v>43977</v>
       </c>
+      <c r="AN2" s="9">
+        <v>43978</v>
+      </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:40">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -18435,8 +18762,11 @@
       <c r="AM3">
         <v>445</v>
       </c>
+      <c r="AN3">
+        <v>453</v>
+      </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:40">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -18554,8 +18884,11 @@
       <c r="AM4">
         <v>45</v>
       </c>
+      <c r="AN4">
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:40">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -18673,8 +19006,11 @@
       <c r="AM5">
         <v>27</v>
       </c>
+      <c r="AN5">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:40">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -18792,8 +19128,11 @@
       <c r="AM6">
         <v>30</v>
       </c>
+      <c r="AN6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:40">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -18911,8 +19250,11 @@
       <c r="AM7">
         <v>63</v>
       </c>
+      <c r="AN7">
+        <v>64</v>
+      </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:40">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -19030,8 +19372,11 @@
       <c r="AM8">
         <v>69</v>
       </c>
+      <c r="AN8">
+        <v>72</v>
+      </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:40">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -19149,8 +19494,11 @@
       <c r="AM9">
         <v>41</v>
       </c>
+      <c r="AN9">
+        <v>41</v>
+      </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:40">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -19268,8 +19616,11 @@
       <c r="AM10">
         <v>62</v>
       </c>
+      <c r="AN10">
+        <v>64</v>
+      </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:40">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -19387,8 +19738,11 @@
       <c r="AM11">
         <v>92</v>
       </c>
+      <c r="AN11">
+        <v>93</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" ht="28.8">
+    <row r="12" spans="1:40" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -19506,8 +19860,11 @@
       <c r="AM12">
         <v>16</v>
       </c>
+      <c r="AN12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:40">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -19623,6 +19980,9 @@
         <v>0</v>
       </c>
       <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
         <v>0</v>
       </c>
     </row>
@@ -19633,64 +19993,64 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="C1" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
+      <c r="C1" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
     </row>
     <row r="4" spans="1:15">
       <c r="C4" s="34"/>
@@ -19729,10 +20089,13 @@
       <c r="I5" s="9">
         <v>43977</v>
       </c>
+      <c r="J5" s="9">
+        <v>43978</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6">
         <v>103</v>
@@ -19754,6 +20117,9 @@
       </c>
       <c r="I6">
         <v>107</v>
+      </c>
+      <c r="J6">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -19781,6 +20147,9 @@
       <c r="I7">
         <v>28</v>
       </c>
+      <c r="J7">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="35" t="s">
@@ -19812,10 +20181,13 @@
       <c r="I9">
         <v>1</v>
       </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10">
         <v>18</v>
@@ -19837,11 +20209,14 @@
       </c>
       <c r="I10">
         <v>20</v>
+      </c>
+      <c r="J10">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -19863,6 +20238,9 @@
       </c>
       <c r="I11">
         <v>5</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -19890,6 +20268,9 @@
       <c r="I12">
         <v>2</v>
       </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="36" t="s">
@@ -19921,6 +20302,9 @@
       <c r="I14">
         <v>1</v>
       </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="31">
@@ -19947,6 +20331,9 @@
       <c r="I15">
         <v>0</v>
       </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="31">
@@ -19973,8 +20360,11 @@
       <c r="I16">
         <v>2</v>
       </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -19999,8 +20389,11 @@
       <c r="I17">
         <v>8</v>
       </c>
+      <c r="J17">
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -20025,8 +20418,11 @@
       <c r="I18">
         <v>2</v>
       </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -20051,8 +20447,11 @@
       <c r="I19">
         <v>2</v>
       </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -20077,8 +20476,11 @@
       <c r="I20">
         <v>3</v>
       </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -20103,8 +20505,11 @@
       <c r="I21">
         <v>5</v>
       </c>
+      <c r="J21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" ht="28.8">
+    <row r="22" spans="1:10" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -20129,10 +20534,13 @@
       <c r="I22">
         <v>4</v>
       </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" ht="28.8">
+    <row r="23" spans="1:10" ht="30">
       <c r="A23" s="39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -20153,6 +20561,9 @@
         <v>1</v>
       </c>
       <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
         <v>1</v>
       </c>
     </row>
@@ -20165,37 +20576,37 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A1" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="A1" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:7" ht="36.6" customHeight="1">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -20204,7 +20615,7 @@
       <c r="C2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>124</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -20218,10 +20629,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1">
-      <c r="A3" s="43"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="44"/>
+      <c r="D3" s="45"/>
       <c r="E3" s="25" t="s">
         <v>92</v>
       </c>
@@ -20232,11 +20643,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A4" s="43"/>
+    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+      <c r="A4" s="44"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="44"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="25" t="s">
         <v>86</v>
       </c>
@@ -20245,40 +20656,40 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A5" s="43"/>
+    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+      <c r="A5" s="44"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="44"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="25" t="s">
         <v>87</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A6" s="43"/>
+    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+      <c r="A6" s="44"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="44"/>
+      <c r="D6" s="45"/>
       <c r="E6" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A7" s="43"/>
+    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+      <c r="A7" s="44"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="44"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="25" t="s">
         <v>93</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.4" customHeight="1">
+    <row r="8" spans="1:7" ht="14.45" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
@@ -20301,7 +20712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4" customHeight="1">
+    <row r="9" spans="1:7" ht="14.45" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>96</v>
       </c>
@@ -20324,7 +20735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.4" customHeight="1">
+    <row r="10" spans="1:7" ht="14.45" customHeight="1">
       <c r="A10" s="27" t="s">
         <v>98</v>
       </c>
@@ -20338,7 +20749,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F10" s="28">
         <v>1</v>
@@ -20347,12 +20758,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.4" customHeight="1">
+    <row r="11" spans="1:7" ht="14.45" customHeight="1">
       <c r="A11" s="27" t="s">
         <v>99</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="C11" s="28">
         <v>13</v>
@@ -20361,7 +20772,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
@@ -20370,7 +20781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.4" customHeight="1">
+    <row r="12" spans="1:7" ht="14.45" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>100</v>
       </c>
@@ -20393,9 +20804,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.4" customHeight="1">
+    <row r="13" spans="1:7" ht="14.45" customHeight="1">
       <c r="A13" s="27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>97</v>
@@ -20416,7 +20827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.4" customHeight="1">
+    <row r="14" spans="1:7" ht="14.45" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>103</v>
       </c>
@@ -20439,12 +20850,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.4" customHeight="1">
+    <row r="15" spans="1:7" ht="14.45" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>104</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C15" s="28">
         <v>14</v>
@@ -20453,7 +20864,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="28">
         <v>1</v>
@@ -20485,7 +20896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.4" customHeight="1">
+    <row r="17" spans="1:7" ht="14.45" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>107</v>
       </c>
@@ -20508,12 +20919,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.4" customHeight="1">
+    <row r="18" spans="1:7" ht="14.45" customHeight="1">
       <c r="A18" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C18" s="28">
         <v>12</v>
@@ -20531,21 +20942,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.4" customHeight="1">
+    <row r="19" spans="1:7" ht="14.45" customHeight="1">
       <c r="A19" s="27" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="C19" s="28">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D19" s="28">
         <v>0</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
@@ -20554,12 +20965,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.4" customHeight="1">
+    <row r="20" spans="1:7" ht="14.45" customHeight="1">
       <c r="A20" s="27" t="s">
         <v>111</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C20" s="28">
         <v>17</v>
@@ -20577,7 +20988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.4" customHeight="1">
+    <row r="21" spans="1:7" ht="14.45" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>112</v>
       </c>
@@ -20600,12 +21011,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.4" customHeight="1">
+    <row r="22" spans="1:7" ht="14.45" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>115</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C22" s="28">
         <v>25</v>
@@ -20614,7 +21025,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F22" s="28">
         <v>1</v>
@@ -20651,7 +21062,7 @@
         <v>118</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C24" s="28">
         <v>7</v>
@@ -20692,21 +21103,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1">
+    <row r="26" spans="1:7" ht="17.45" customHeight="1">
       <c r="A26" s="30" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C26" s="28">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D26" s="28">
         <v>0</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F26" s="28">
         <v>5</v>
@@ -20715,11 +21126,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.6">
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="40" t="s">
         <v>162</v>
       </c>
       <c r="C27" s="27"/>
@@ -20988,16 +21399,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
29 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A91D15C-CCD8-441E-86A4-22D1F5E8FA68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="20730" windowHeight="7290" tabRatio="807"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId6"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -444,9 +452,6 @@
     <t>23; (8)</t>
   </si>
   <si>
-    <t>44; (28)</t>
-  </si>
-  <si>
     <t>21; (17)</t>
   </si>
   <si>
@@ -477,9 +482,6 @@
     <t>20; (1)</t>
   </si>
   <si>
-    <t>31; (24)</t>
-  </si>
-  <si>
     <t>45; (18)</t>
   </si>
   <si>
@@ -492,23 +494,17 @@
     <t>20; (3)</t>
   </si>
   <si>
-    <t>141; (43)</t>
-  </si>
-  <si>
     <t>29; (0)</t>
   </si>
   <si>
-    <t>21; (8)</t>
+    <t>58; (33)</t>
   </si>
   <si>
-    <t>194; (78)</t>
-  </si>
-  <si>
-    <t>As of May 27, 2020</t>
+    <t>As of May 28, 2020</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of May 27, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of May 28, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -533,22 +529,34 @@
     </r>
   </si>
   <si>
-    <t>96; (47)</t>
+    <t>101; (52)</t>
   </si>
   <si>
-    <t>58; (33)</t>
+    <t>33; (24)</t>
   </si>
   <si>
-    <t>652; (283)</t>
+    <t>45; (29)</t>
   </si>
   <si>
-    <t>846; (361)</t>
+    <t>142; (44)</t>
+  </si>
+  <si>
+    <t>16; (8)</t>
+  </si>
+  <si>
+    <t>654; (290)</t>
+  </si>
+  <si>
+    <t>196; (78)</t>
+  </si>
+  <si>
+    <t>850; (368)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -817,7 +825,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1152,19 +1160,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CF113"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CG113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="CA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CH3" sqref="CH3"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="BV1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CG17" sqref="CG1:CG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1176,10 +1184,10 @@
     <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="84" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="85" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84">
+    <row r="1" spans="1:85">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1426,8 +1434,11 @@
       <c r="CF1" s="1">
         <v>43978</v>
       </c>
+      <c r="CG1" s="1">
+        <v>43979</v>
+      </c>
     </row>
-    <row r="2" spans="1:84">
+    <row r="2" spans="1:85">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1451,12 +1462,12 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:84">
+    <row r="3" spans="1:85">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I3">
         <v>69</v>
@@ -1683,13 +1694,16 @@
       <c r="CF3">
         <v>43514</v>
       </c>
+      <c r="CG3">
+        <v>43858</v>
+      </c>
     </row>
-    <row r="4" spans="1:84">
+    <row r="4" spans="1:85">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AN4" s="19"/>
       <c r="AO4" s="20"/>
@@ -1711,8 +1725,11 @@
       <c r="CF4">
         <v>36284</v>
       </c>
+      <c r="CG4">
+        <v>36511</v>
+      </c>
     </row>
-    <row r="5" spans="1:84">
+    <row r="5" spans="1:85">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1965,8 +1982,11 @@
       <c r="CF5">
         <v>8492</v>
       </c>
+      <c r="CG5">
+        <v>8538</v>
+      </c>
     </row>
-    <row r="6" spans="1:84">
+    <row r="6" spans="1:85">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2201,13 +2221,16 @@
       <c r="CF6">
         <v>453</v>
       </c>
+      <c r="CG6">
+        <v>460</v>
+      </c>
     </row>
-    <row r="7" spans="1:84">
+    <row r="7" spans="1:85">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S7">
         <v>17</v>
@@ -2407,11 +2430,14 @@
       <c r="CF7">
         <v>1082</v>
       </c>
+      <c r="CG7">
+        <v>1089</v>
+      </c>
     </row>
-    <row r="8" spans="1:84">
+    <row r="8" spans="1:85">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:84">
+    <row r="9" spans="1:85">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2508,8 +2534,11 @@
       <c r="CF9">
         <v>345</v>
       </c>
+      <c r="CG9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:84">
+    <row r="10" spans="1:85">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2708,8 +2737,11 @@
       <c r="CF10">
         <v>76</v>
       </c>
+      <c r="CG10">
+        <v>90</v>
+      </c>
     </row>
-    <row r="11" spans="1:84">
+    <row r="11" spans="1:85">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2908,8 +2940,11 @@
       <c r="CF11">
         <v>440</v>
       </c>
+      <c r="CG11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:84">
+    <row r="12" spans="1:85">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3108,8 +3143,11 @@
       <c r="CF12">
         <v>218</v>
       </c>
+      <c r="CG12">
+        <v>223</v>
+      </c>
     </row>
-    <row r="13" spans="1:84">
+    <row r="13" spans="1:85">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3308,8 +3346,11 @@
       <c r="CF13">
         <v>222</v>
       </c>
+      <c r="CG13">
+        <v>217</v>
+      </c>
     </row>
-    <row r="14" spans="1:84">
+    <row r="14" spans="1:85">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3370,13 +3411,16 @@
       <c r="CF14">
         <v>343</v>
       </c>
+      <c r="CG14">
+        <v>338</v>
+      </c>
     </row>
-    <row r="15" spans="1:84">
+    <row r="15" spans="1:85">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BY15">
         <v>110</v>
@@ -3402,8 +3446,11 @@
       <c r="CF15">
         <v>108</v>
       </c>
+      <c r="CG15">
+        <v>114</v>
+      </c>
     </row>
-    <row r="16" spans="1:84">
+    <row r="16" spans="1:85">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3464,8 +3511,11 @@
       <c r="CF16">
         <v>1939</v>
       </c>
+      <c r="CG16">
+        <v>1981</v>
+      </c>
     </row>
-    <row r="17" spans="1:84">
+    <row r="17" spans="1:85">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3526,13 +3576,16 @@
       <c r="CF17" s="23">
         <v>0.78</v>
       </c>
+      <c r="CG17" s="23">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="19" spans="1:84">
+    <row r="19" spans="1:85">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:84">
+    <row r="20" spans="1:85">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3540,7 +3593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:84">
+    <row r="21" spans="1:85">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3742,8 +3795,11 @@
       <c r="CF21">
         <v>107</v>
       </c>
+      <c r="CG21">
+        <v>109</v>
+      </c>
     </row>
-    <row r="22" spans="1:84">
+    <row r="22" spans="1:85">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3891,8 +3947,11 @@
       <c r="CF22">
         <v>18</v>
       </c>
+      <c r="CG22">
+        <v>20</v>
+      </c>
     </row>
-    <row r="23" spans="1:84">
+    <row r="23" spans="1:85">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4040,8 +4099,11 @@
       <c r="CF23">
         <v>89</v>
       </c>
+      <c r="CG23">
+        <v>89</v>
+      </c>
     </row>
-    <row r="24" spans="1:84">
+    <row r="24" spans="1:85">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4234,8 +4296,11 @@
       <c r="CF24">
         <v>154</v>
       </c>
+      <c r="CG24">
+        <v>118</v>
+      </c>
     </row>
-    <row r="25" spans="1:84">
+    <row r="25" spans="1:85">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4428,8 +4493,11 @@
       <c r="CF25">
         <v>172</v>
       </c>
+      <c r="CG25">
+        <v>138</v>
+      </c>
     </row>
-    <row r="26" spans="1:84">
+    <row r="26" spans="1:85">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4622,13 +4690,16 @@
       <c r="CF26">
         <v>1324</v>
       </c>
+      <c r="CG26">
+        <v>1324</v>
+      </c>
     </row>
-    <row r="28" spans="1:84">
+    <row r="28" spans="1:85">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:84">
+    <row r="29" spans="1:85">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4830,8 +4901,11 @@
       <c r="CF29">
         <v>132</v>
       </c>
+      <c r="CG29">
+        <v>132</v>
+      </c>
     </row>
-    <row r="30" spans="1:84">
+    <row r="30" spans="1:85">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -4979,8 +5053,11 @@
       <c r="CF30">
         <v>31</v>
       </c>
+      <c r="CG30">
+        <v>28</v>
+      </c>
     </row>
-    <row r="31" spans="1:84">
+    <row r="31" spans="1:85">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5128,8 +5205,11 @@
       <c r="CF31">
         <v>101</v>
       </c>
+      <c r="CG31">
+        <v>104</v>
+      </c>
     </row>
-    <row r="32" spans="1:84">
+    <row r="32" spans="1:85">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5322,8 +5402,11 @@
       <c r="CF32">
         <v>59</v>
       </c>
+      <c r="CG32">
+        <v>57</v>
+      </c>
     </row>
-    <row r="33" spans="1:84">
+    <row r="33" spans="1:85">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5516,8 +5599,11 @@
       <c r="CF33">
         <v>90</v>
       </c>
+      <c r="CG33">
+        <v>85</v>
+      </c>
     </row>
-    <row r="34" spans="1:84">
+    <row r="34" spans="1:85">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -5710,13 +5796,16 @@
       <c r="CF34">
         <v>1178</v>
       </c>
+      <c r="CG34">
+        <v>1194</v>
+      </c>
     </row>
-    <row r="36" spans="1:84">
+    <row r="36" spans="1:85">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:84">
+    <row r="37" spans="1:85">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5906,8 +5995,11 @@
       <c r="CF37">
         <v>80</v>
       </c>
+      <c r="CG37">
+        <v>80</v>
+      </c>
     </row>
-    <row r="38" spans="1:84">
+    <row r="38" spans="1:85">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6049,8 +6141,11 @@
       <c r="CF38">
         <v>6</v>
       </c>
+      <c r="CG38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:84">
+    <row r="39" spans="1:85">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6192,8 +6287,11 @@
       <c r="CF39">
         <v>73</v>
       </c>
+      <c r="CG39">
+        <v>73</v>
+      </c>
     </row>
-    <row r="40" spans="1:84">
+    <row r="40" spans="1:85">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6380,8 +6478,11 @@
       <c r="CF40">
         <v>1</v>
       </c>
+      <c r="CG40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:84">
+    <row r="41" spans="1:85">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6565,8 +6666,11 @@
       <c r="CF41">
         <v>7</v>
       </c>
+      <c r="CG41">
+        <v>7</v>
+      </c>
     </row>
-    <row r="42" spans="1:84">
+    <row r="42" spans="1:85">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -6756,8 +6860,11 @@
       <c r="CF42">
         <v>281</v>
       </c>
+      <c r="CG42">
+        <v>281</v>
+      </c>
     </row>
-    <row r="43" spans="1:84">
+    <row r="43" spans="1:85">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -6881,16 +6988,19 @@
       <c r="CF43">
         <v>1</v>
       </c>
+      <c r="CG43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:84">
+    <row r="44" spans="1:85">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:84">
+    <row r="45" spans="1:85">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:84">
+    <row r="46" spans="1:85">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -7086,8 +7196,11 @@
       <c r="CF46">
         <v>205</v>
       </c>
+      <c r="CG46">
+        <v>205</v>
+      </c>
     </row>
-    <row r="47" spans="1:84">
+    <row r="47" spans="1:85">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7235,8 +7348,11 @@
       <c r="CF47">
         <v>25</v>
       </c>
+      <c r="CG47">
+        <v>25</v>
+      </c>
     </row>
-    <row r="48" spans="1:84">
+    <row r="48" spans="1:85">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7384,8 +7500,11 @@
       <c r="CF48">
         <v>174</v>
       </c>
+      <c r="CG48">
+        <v>174</v>
+      </c>
     </row>
-    <row r="49" spans="1:84">
+    <row r="49" spans="1:85">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -7578,8 +7697,11 @@
       <c r="CF49">
         <v>619</v>
       </c>
+      <c r="CG49">
+        <v>494</v>
+      </c>
     </row>
-    <row r="50" spans="1:84">
+    <row r="50" spans="1:85">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -7727,8 +7849,11 @@
       <c r="CF50">
         <v>644</v>
       </c>
+      <c r="CG50">
+        <v>519</v>
+      </c>
     </row>
-    <row r="51" spans="1:84">
+    <row r="51" spans="1:85">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -7873,8 +7998,11 @@
       <c r="CF51">
         <v>708</v>
       </c>
+      <c r="CG51">
+        <v>839</v>
+      </c>
     </row>
-    <row r="52" spans="1:84">
+    <row r="52" spans="1:85">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -8013,16 +8141,19 @@
       <c r="CF52">
         <v>1</v>
       </c>
+      <c r="CG52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:84">
+    <row r="53" spans="1:85">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:84">
+    <row r="54" spans="1:85">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:84">
+    <row r="55" spans="1:85">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -8203,8 +8334,11 @@
       <c r="CF55">
         <v>30</v>
       </c>
+      <c r="CG55">
+        <v>30</v>
+      </c>
     </row>
-    <row r="56" spans="1:84">
+    <row r="56" spans="1:85">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -8349,8 +8483,11 @@
       <c r="CF56">
         <v>10</v>
       </c>
+      <c r="CG56">
+        <v>8</v>
+      </c>
     </row>
-    <row r="57" spans="1:84">
+    <row r="57" spans="1:85">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -8495,8 +8632,11 @@
       <c r="CF57">
         <v>19</v>
       </c>
+      <c r="CG57">
+        <v>21</v>
+      </c>
     </row>
-    <row r="58" spans="1:84">
+    <row r="58" spans="1:85">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -8677,8 +8817,11 @@
       <c r="CF58">
         <v>21</v>
       </c>
+      <c r="CG58">
+        <v>20</v>
+      </c>
     </row>
-    <row r="59" spans="1:84">
+    <row r="59" spans="1:85">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -8859,8 +9002,11 @@
       <c r="CF59">
         <v>31</v>
       </c>
+      <c r="CG59">
+        <v>28</v>
+      </c>
     </row>
-    <row r="60" spans="1:84">
+    <row r="60" spans="1:85">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -9041,8 +9187,11 @@
       <c r="CF60">
         <v>138</v>
       </c>
+      <c r="CG60">
+        <v>141</v>
+      </c>
     </row>
-    <row r="61" spans="1:84">
+    <row r="61" spans="1:85">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -9181,8 +9330,11 @@
       <c r="CF61">
         <v>1</v>
       </c>
+      <c r="CG61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:84">
+    <row r="63" spans="1:85">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -9363,8 +9515,11 @@
       <c r="CF63">
         <v>11</v>
       </c>
+      <c r="CG63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:84">
+    <row r="64" spans="1:85">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -9509,8 +9664,11 @@
       <c r="CF64">
         <v>4</v>
       </c>
+      <c r="CG64">
+        <v>4</v>
+      </c>
     </row>
-    <row r="65" spans="1:84">
+    <row r="65" spans="1:85">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -9655,8 +9813,11 @@
       <c r="CF65">
         <v>7</v>
       </c>
+      <c r="CG65">
+        <v>7</v>
+      </c>
     </row>
-    <row r="66" spans="1:84">
+    <row r="66" spans="1:85">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -9837,8 +9998,11 @@
       <c r="CF66">
         <v>46</v>
       </c>
+      <c r="CG66">
+        <v>46</v>
+      </c>
     </row>
-    <row r="67" spans="1:84">
+    <row r="67" spans="1:85">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -10020,8 +10184,11 @@
       <c r="CF67">
         <v>50</v>
       </c>
+      <c r="CG67">
+        <v>50</v>
+      </c>
     </row>
-    <row r="68" spans="1:84">
+    <row r="68" spans="1:85">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -10202,8 +10369,11 @@
       <c r="CF68">
         <v>0</v>
       </c>
+      <c r="CG68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:84">
+    <row r="69" spans="1:85">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -10348,11 +10518,14 @@
       <c r="CF69">
         <v>0</v>
       </c>
+      <c r="CG69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:84">
+    <row r="70" spans="1:85">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:84">
+    <row r="71" spans="1:85">
       <c r="A71" s="2" t="s">
         <v>134</v>
       </c>
@@ -10383,8 +10556,11 @@
       <c r="CF71">
         <v>10</v>
       </c>
+      <c r="CG71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:84">
+    <row r="72" spans="1:85">
       <c r="A72" s="2" t="s">
         <v>134</v>
       </c>
@@ -10415,8 +10591,11 @@
       <c r="CF72">
         <v>7</v>
       </c>
+      <c r="CG72">
+        <v>6</v>
+      </c>
     </row>
-    <row r="73" spans="1:84">
+    <row r="73" spans="1:85">
       <c r="A73" s="2" t="s">
         <v>134</v>
       </c>
@@ -10447,8 +10626,11 @@
       <c r="CF73">
         <v>3</v>
       </c>
+      <c r="CG73">
+        <v>4</v>
+      </c>
     </row>
-    <row r="74" spans="1:84">
+    <row r="74" spans="1:85">
       <c r="A74" s="2" t="s">
         <v>134</v>
       </c>
@@ -10479,8 +10661,11 @@
       <c r="CF74">
         <v>13</v>
       </c>
+      <c r="CG74">
+        <v>12</v>
+      </c>
     </row>
-    <row r="75" spans="1:84">
+    <row r="75" spans="1:85">
       <c r="A75" s="2" t="s">
         <v>134</v>
       </c>
@@ -10511,8 +10696,11 @@
       <c r="CF75">
         <v>20</v>
       </c>
+      <c r="CG75">
+        <v>18</v>
+      </c>
     </row>
-    <row r="76" spans="1:84">
+    <row r="76" spans="1:85">
       <c r="A76" s="2" t="s">
         <v>134</v>
       </c>
@@ -10543,13 +10731,16 @@
       <c r="CF76">
         <v>26</v>
       </c>
+      <c r="CG76">
+        <v>28</v>
+      </c>
     </row>
-    <row r="78" spans="1:84">
+    <row r="78" spans="1:85">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:84">
+    <row r="79" spans="1:85">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -10730,8 +10921,11 @@
       <c r="CF79">
         <v>295</v>
       </c>
+      <c r="CG79">
+        <v>295</v>
+      </c>
     </row>
-    <row r="80" spans="1:84">
+    <row r="80" spans="1:85">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -10912,8 +11106,11 @@
       <c r="CF80">
         <v>167</v>
       </c>
+      <c r="CG80">
+        <v>148</v>
+      </c>
     </row>
-    <row r="81" spans="1:84">
+    <row r="81" spans="1:85">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -11094,8 +11291,11 @@
       <c r="CF81">
         <v>135</v>
       </c>
+      <c r="CG81">
+        <v>125</v>
+      </c>
     </row>
-    <row r="82" spans="1:84">
+    <row r="82" spans="1:85">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -11234,8 +11434,11 @@
       <c r="CF82">
         <v>16</v>
       </c>
+      <c r="CG82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:84">
+    <row r="84" spans="1:85">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -11416,8 +11619,11 @@
       <c r="CF84">
         <v>116</v>
       </c>
+      <c r="CG84">
+        <v>117</v>
+      </c>
     </row>
-    <row r="85" spans="1:84">
+    <row r="85" spans="1:85">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -11598,8 +11804,11 @@
       <c r="CF85">
         <v>26</v>
       </c>
+      <c r="CG85">
+        <v>27</v>
+      </c>
     </row>
-    <row r="86" spans="1:84">
+    <row r="86" spans="1:85">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -11780,8 +11989,11 @@
       <c r="CF86">
         <v>142</v>
       </c>
+      <c r="CG86">
+        <v>144</v>
+      </c>
     </row>
-    <row r="87" spans="1:84">
+    <row r="87" spans="1:85">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -11962,8 +12174,11 @@
       <c r="CF87">
         <v>186</v>
       </c>
+      <c r="CG87">
+        <v>187</v>
+      </c>
     </row>
-    <row r="88" spans="1:84">
+    <row r="88" spans="1:85">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -12018,8 +12233,11 @@
       <c r="CF88">
         <v>1</v>
       </c>
+      <c r="CG88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:84">
+    <row r="90" spans="1:85">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -12200,8 +12418,11 @@
       <c r="CF90">
         <v>79</v>
       </c>
+      <c r="CG90">
+        <v>80</v>
+      </c>
     </row>
-    <row r="91" spans="1:84">
+    <row r="91" spans="1:85">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -12382,8 +12603,11 @@
       <c r="CF91">
         <v>31</v>
       </c>
+      <c r="CG91">
+        <v>31</v>
+      </c>
     </row>
-    <row r="92" spans="1:84">
+    <row r="92" spans="1:85">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -12552,8 +12776,11 @@
       <c r="CF92">
         <v>163</v>
       </c>
+      <c r="CG92">
+        <v>163</v>
+      </c>
     </row>
-    <row r="93" spans="1:84">
+    <row r="93" spans="1:85">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -12734,8 +12961,11 @@
       <c r="CF93">
         <v>32</v>
       </c>
+      <c r="CG93">
+        <v>32</v>
+      </c>
     </row>
-    <row r="94" spans="1:84">
+    <row r="94" spans="1:85">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -12874,8 +13104,11 @@
       <c r="CF94">
         <v>13</v>
       </c>
+      <c r="CG94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:84">
+    <row r="96" spans="1:85">
       <c r="A96" s="2" t="s">
         <v>79</v>
       </c>
@@ -12975,8 +13208,11 @@
       <c r="CF96">
         <v>183</v>
       </c>
+      <c r="CG96">
+        <v>185</v>
+      </c>
     </row>
-    <row r="97" spans="1:84">
+    <row r="97" spans="1:85">
       <c r="A97" s="2" t="s">
         <v>79</v>
       </c>
@@ -13076,8 +13312,11 @@
       <c r="CF97">
         <v>49</v>
       </c>
+      <c r="CG97">
+        <v>53</v>
+      </c>
     </row>
-    <row r="98" spans="1:84">
+    <row r="98" spans="1:85">
       <c r="A98" s="2" t="s">
         <v>79</v>
       </c>
@@ -13175,6 +13414,9 @@
         <v>25</v>
       </c>
       <c r="CF98">
+        <v>25</v>
+      </c>
+      <c r="CG98">
         <v>25</v>
       </c>
     </row>
@@ -13190,11 +13432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BG11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:BH11"/>
   <sheetViews>
-    <sheetView topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BI5" sqref="BI5"/>
+    <sheetView tabSelected="1" topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BH11" sqref="BH3:BH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13204,7 +13446,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:59" s="2" customFormat="1">
+    <row r="2" spans="1:60" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -13382,8 +13624,11 @@
       <c r="BG2" s="9">
         <v>43978</v>
       </c>
+      <c r="BH2" s="9">
+        <v>43979</v>
+      </c>
     </row>
-    <row r="3" spans="1:59">
+    <row r="3" spans="1:60">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -13561,8 +13806,11 @@
       <c r="BG3">
         <v>1188</v>
       </c>
+      <c r="BH3">
+        <v>1198</v>
+      </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:60">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -13740,8 +13988,11 @@
       <c r="BG4">
         <v>511</v>
       </c>
+      <c r="BH4">
+        <v>512</v>
+      </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="1:60">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -13919,8 +14170,11 @@
       <c r="BG5">
         <v>413</v>
       </c>
+      <c r="BH5">
+        <v>416</v>
+      </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:60">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -14098,8 +14352,11 @@
       <c r="BG6">
         <v>1785</v>
       </c>
+      <c r="BH6">
+        <v>1795</v>
+      </c>
     </row>
-    <row r="7" spans="1:59">
+    <row r="7" spans="1:60">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -14277,8 +14534,11 @@
       <c r="BG7">
         <v>1327</v>
       </c>
+      <c r="BH7">
+        <v>1331</v>
+      </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="1:60">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -14456,8 +14716,11 @@
       <c r="BG8">
         <v>722</v>
       </c>
+      <c r="BH8">
+        <v>729</v>
+      </c>
     </row>
-    <row r="9" spans="1:59">
+    <row r="9" spans="1:60">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -14635,8 +14898,11 @@
       <c r="BG9">
         <v>1219</v>
       </c>
+      <c r="BH9">
+        <v>1224</v>
+      </c>
     </row>
-    <row r="10" spans="1:59">
+    <row r="10" spans="1:60">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -14814,8 +15080,11 @@
       <c r="BG10">
         <v>1191</v>
       </c>
+      <c r="BH10">
+        <v>1196</v>
+      </c>
     </row>
-    <row r="11" spans="1:59">
+    <row r="11" spans="1:60">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -14992,6 +15261,9 @@
       </c>
       <c r="BG11">
         <v>136</v>
+      </c>
+      <c r="BH11">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -15001,11 +15273,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BB17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:BC17"/>
   <sheetViews>
-    <sheetView topLeftCell="AT1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC3" sqref="BC3"/>
+    <sheetView topLeftCell="AO10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BC17" sqref="BC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15015,7 +15287,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:54" s="2" customFormat="1">
+    <row r="2" spans="1:55" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -15176,8 +15448,11 @@
       <c r="BB2" s="9">
         <v>43978</v>
       </c>
+      <c r="BC2" s="9">
+        <v>43979</v>
+      </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1">
+    <row r="3" spans="1:55" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -15185,7 +15460,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:54">
+    <row r="4" spans="1:55">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -15348,8 +15623,11 @@
       <c r="BB4">
         <v>8492</v>
       </c>
+      <c r="BC4">
+        <v>8538</v>
+      </c>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:55">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -15512,8 +15790,11 @@
       <c r="BB5">
         <v>1006</v>
       </c>
+      <c r="BC5">
+        <v>870</v>
+      </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:55">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -15676,8 +15957,11 @@
       <c r="BB6">
         <v>1300</v>
       </c>
+      <c r="BC6">
+        <v>1331</v>
+      </c>
     </row>
-    <row r="7" spans="1:54">
+    <row r="7" spans="1:55">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -15840,8 +16124,11 @@
       <c r="BB7">
         <v>3896</v>
       </c>
+      <c r="BC7">
+        <v>3991</v>
+      </c>
     </row>
-    <row r="8" spans="1:54">
+    <row r="8" spans="1:55">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -16004,8 +16291,11 @@
       <c r="BB8">
         <v>106</v>
       </c>
+      <c r="BC8">
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:54" ht="30">
+    <row r="9" spans="1:55" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -16168,8 +16458,11 @@
       <c r="BB9">
         <v>24</v>
       </c>
+      <c r="BC9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:54" ht="30">
+    <row r="10" spans="1:55" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -16328,8 +16621,11 @@
       <c r="BB10">
         <v>20</v>
       </c>
+      <c r="BC10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:54">
+    <row r="11" spans="1:55">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -16492,8 +16788,11 @@
       <c r="BB11">
         <v>2092</v>
       </c>
+      <c r="BC11">
+        <v>2135</v>
+      </c>
     </row>
-    <row r="12" spans="1:54" ht="30">
+    <row r="12" spans="1:55" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -16656,8 +16955,11 @@
       <c r="BB12">
         <v>48</v>
       </c>
+      <c r="BC12">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:54">
+    <row r="13" spans="1:55">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -16668,7 +16970,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:54">
+    <row r="14" spans="1:55">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -16831,8 +17133,11 @@
       <c r="BB14">
         <v>1618</v>
       </c>
+      <c r="BC14">
+        <v>1419</v>
+      </c>
     </row>
-    <row r="15" spans="1:54">
+    <row r="15" spans="1:55">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -16995,8 +17300,11 @@
       <c r="BB15">
         <v>2173</v>
       </c>
+      <c r="BC15">
+        <v>2272</v>
+      </c>
     </row>
-    <row r="16" spans="1:54">
+    <row r="16" spans="1:55">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -17159,8 +17467,11 @@
       <c r="BB16">
         <v>4674</v>
       </c>
+      <c r="BC16">
+        <v>4822</v>
+      </c>
     </row>
-    <row r="17" spans="1:54" ht="30">
+    <row r="17" spans="1:55" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -17322,6 +17633,9 @@
       </c>
       <c r="BB17">
         <v>27</v>
+      </c>
+      <c r="BC17">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -17331,11 +17645,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:BC9"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BD3" sqref="BD3"/>
+    <sheetView topLeftCell="AL2" workbookViewId="0">
+      <selection activeCell="BC11" sqref="BC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17344,7 +17658,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="2" customFormat="1">
+    <row r="1" spans="1:55" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -17504,14 +17818,17 @@
       <c r="BB1" s="9">
         <v>43978</v>
       </c>
+      <c r="BC1" s="9">
+        <v>43979</v>
+      </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:55">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:54">
+    <row r="3" spans="1:55">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -17675,8 +17992,11 @@
       <c r="BB3">
         <v>453</v>
       </c>
+      <c r="BC3">
+        <v>460</v>
+      </c>
     </row>
-    <row r="4" spans="1:54">
+    <row r="4" spans="1:55">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -17839,8 +18159,11 @@
       <c r="BB4">
         <v>7</v>
       </c>
+      <c r="BC4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:54" ht="30">
+    <row r="5" spans="1:55" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -18003,8 +18326,11 @@
       <c r="BB5">
         <v>339</v>
       </c>
+      <c r="BC5">
+        <v>344</v>
+      </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:55">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -18167,8 +18493,11 @@
       <c r="BB6">
         <v>51</v>
       </c>
+      <c r="BC6">
+        <v>52</v>
+      </c>
     </row>
-    <row r="7" spans="1:54" ht="30">
+    <row r="7" spans="1:55" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -18331,8 +18660,11 @@
       <c r="BB7">
         <v>52</v>
       </c>
+      <c r="BC7">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:54">
+    <row r="8" spans="1:55">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -18495,12 +18827,18 @@
       <c r="BB8">
         <v>3</v>
       </c>
+      <c r="BC8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:54">
+    <row r="9" spans="1:55">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
       <c r="BB9">
+        <v>1</v>
+      </c>
+      <c r="BC9">
         <v>1</v>
       </c>
     </row>
@@ -18510,11 +18848,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AN13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A2:AO13"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+    <sheetView topLeftCell="AD4" workbookViewId="0">
+      <selection activeCell="AQ12" sqref="AQ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18522,7 +18860,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:40" s="2" customFormat="1">
+    <row r="2" spans="1:41" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -18643,8 +18981,11 @@
       <c r="AN2" s="9">
         <v>43978</v>
       </c>
+      <c r="AO2" s="9">
+        <v>43979</v>
+      </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:41">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -18765,8 +19106,11 @@
       <c r="AN3">
         <v>453</v>
       </c>
+      <c r="AO3">
+        <v>460</v>
+      </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:41">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -18887,8 +19231,11 @@
       <c r="AN4">
         <v>46</v>
       </c>
+      <c r="AO4">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:41">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -19009,8 +19356,11 @@
       <c r="AN5">
         <v>27</v>
       </c>
+      <c r="AO5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:41">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -19131,8 +19481,11 @@
       <c r="AN6">
         <v>30</v>
       </c>
+      <c r="AO6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:41">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -19253,8 +19606,11 @@
       <c r="AN7">
         <v>64</v>
       </c>
+      <c r="AO7">
+        <v>65</v>
+      </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:41">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -19375,8 +19731,11 @@
       <c r="AN8">
         <v>72</v>
       </c>
+      <c r="AO8">
+        <v>73</v>
+      </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:41">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -19497,8 +19856,11 @@
       <c r="AN9">
         <v>41</v>
       </c>
+      <c r="AO9">
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:41">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -19619,8 +19981,11 @@
       <c r="AN10">
         <v>64</v>
       </c>
+      <c r="AO10">
+        <v>64</v>
+      </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:41">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -19741,8 +20106,11 @@
       <c r="AN11">
         <v>93</v>
       </c>
+      <c r="AO11">
+        <v>94</v>
+      </c>
     </row>
-    <row r="12" spans="1:40" ht="30">
+    <row r="12" spans="1:41" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -19863,8 +20231,11 @@
       <c r="AN12">
         <v>16</v>
       </c>
+      <c r="AO12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:41">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -19983,6 +20354,9 @@
         <v>0</v>
       </c>
       <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
         <v>0</v>
       </c>
     </row>
@@ -19993,11 +20367,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20007,7 +20381,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="C1" s="41" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D1" s="41"/>
       <c r="E1" s="41"/>
@@ -20092,10 +20466,13 @@
       <c r="J5" s="9">
         <v>43978</v>
       </c>
+      <c r="K5" s="9">
+        <v>43979</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6">
         <v>103</v>
@@ -20119,6 +20496,9 @@
         <v>107</v>
       </c>
       <c r="J6">
+        <v>113</v>
+      </c>
+      <c r="K6">
         <v>113</v>
       </c>
     </row>
@@ -20150,6 +20530,9 @@
       <c r="J7">
         <v>30</v>
       </c>
+      <c r="K7">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="35" t="s">
@@ -20184,10 +20567,13 @@
       <c r="J9">
         <v>1</v>
       </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C10">
         <v>18</v>
@@ -20211,12 +20597,15 @@
         <v>20</v>
       </c>
       <c r="J10">
+        <v>21</v>
+      </c>
+      <c r="K10">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -20240,6 +20629,9 @@
         <v>5</v>
       </c>
       <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
         <v>6</v>
       </c>
     </row>
@@ -20271,6 +20663,9 @@
       <c r="J12">
         <v>2</v>
       </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="36" t="s">
@@ -20305,6 +20700,9 @@
       <c r="J14">
         <v>1</v>
       </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="31">
@@ -20334,6 +20732,9 @@
       <c r="J15">
         <v>0</v>
       </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="31">
@@ -20363,8 +20764,11 @@
       <c r="J16">
         <v>2</v>
       </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -20392,8 +20796,11 @@
       <c r="J17">
         <v>9</v>
       </c>
+      <c r="K17">
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -20421,8 +20828,11 @@
       <c r="J18">
         <v>2</v>
       </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -20450,8 +20860,11 @@
       <c r="J19">
         <v>2</v>
       </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -20479,8 +20892,11 @@
       <c r="J20">
         <v>3</v>
       </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -20508,8 +20924,11 @@
       <c r="J21">
         <v>6</v>
       </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" ht="45">
+    <row r="22" spans="1:11" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -20537,10 +20956,13 @@
       <c r="J22">
         <v>4</v>
       </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" ht="30">
+    <row r="23" spans="1:11" ht="30">
       <c r="A23" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -20564,6 +20986,9 @@
         <v>1</v>
       </c>
       <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
         <v>1</v>
       </c>
     </row>
@@ -20576,10 +21001,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -20596,7 +21021,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="42" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -20749,7 +21174,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F10" s="28">
         <v>1</v>
@@ -20763,16 +21188,16 @@
         <v>99</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C11" s="28">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D11" s="28">
         <v>0</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
@@ -20806,7 +21231,7 @@
     </row>
     <row r="13" spans="1:7" ht="14.45" customHeight="1">
       <c r="A13" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>97</v>
@@ -20855,16 +21280,16 @@
         <v>104</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C15" s="28">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="28">
         <v>0</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F15" s="28">
         <v>1</v>
@@ -20924,7 +21349,7 @@
         <v>109</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C18" s="28">
         <v>12</v>
@@ -20947,16 +21372,16 @@
         <v>110</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C19" s="28">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="28">
         <v>0</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
@@ -20970,7 +21395,7 @@
         <v>111</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C20" s="28">
         <v>17</v>
@@ -21016,7 +21441,7 @@
         <v>115</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C22" s="28">
         <v>25</v>
@@ -21025,7 +21450,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F22" s="28">
         <v>1</v>
@@ -21062,10 +21487,10 @@
         <v>118</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C24" s="28">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" s="28">
         <v>0</v>
@@ -21108,16 +21533,16 @@
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="28">
+        <v>158</v>
+      </c>
+      <c r="D26" s="28">
+        <v>0</v>
+      </c>
+      <c r="E26" s="28" t="s">
         <v>161</v>
-      </c>
-      <c r="C26" s="28">
-        <v>152</v>
-      </c>
-      <c r="D26" s="28">
-        <v>0</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>156</v>
       </c>
       <c r="F26" s="28">
         <v>5</v>
@@ -21160,6 +21585,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -21362,22 +21802,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21394,29 +21844,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
30 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A91D15C-CCD8-441E-86A4-22D1F5E8FA68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3A9690-C937-4546-9E11-F7EB52496C61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="166">
   <si>
     <t>Testing</t>
   </si>
@@ -419,12 +419,6 @@
     <t>Personnel Loss of Life:</t>
   </si>
   <si>
-    <t>4; (0)</t>
-  </si>
-  <si>
-    <t>4; (1)</t>
-  </si>
-  <si>
     <t>Jeanne Jugan Little Sisters of the Poor (Bed Capacity: 40)</t>
   </si>
   <si>
@@ -500,9 +494,6 @@
     <t>58; (33)</t>
   </si>
   <si>
-    <t>As of May 28, 2020</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">As of May 28, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
@@ -529,12 +520,6 @@
     </r>
   </si>
   <si>
-    <t>101; (52)</t>
-  </si>
-  <si>
-    <t>33; (24)</t>
-  </si>
-  <si>
     <t>45; (29)</t>
   </si>
   <si>
@@ -544,20 +529,44 @@
     <t>16; (8)</t>
   </si>
   <si>
-    <t>654; (290)</t>
+    <t>As of May 29, 2020</t>
   </si>
   <si>
-    <t>196; (78)</t>
+    <t>3; (0)</t>
   </si>
   <si>
-    <t>850; (368)</t>
+    <t>99; (51)</t>
+  </si>
+  <si>
+    <t>34; (25)</t>
+  </si>
+  <si>
+    <t>650; (289)</t>
+  </si>
+  <si>
+    <t>197; (79)</t>
+  </si>
+  <si>
+    <t>847; (368)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Human Services - CFSA</t>
+  </si>
+  <si>
+    <t>Number of Personnel Who Have Tested Positive</t>
+  </si>
+  <si>
+    <t>Number of Personnel Currently in Quarantine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,6 +635,17 @@
       <color rgb="FF112277"/>
       <name val="Albany AMT"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -659,7 +679,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -667,11 +687,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD9E1F2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD9E1F2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD9E1F2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD9E1F2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -773,6 +808,9 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1168,11 +1206,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CG113"/>
+  <dimension ref="A1:CH118"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CG17" sqref="CG1:CG1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="CF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CH96" sqref="CH96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1184,10 +1222,10 @@
     <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="85" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="86" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85">
+    <row r="1" spans="1:86">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1437,8 +1475,11 @@
       <c r="CG1" s="1">
         <v>43979</v>
       </c>
+      <c r="CH1" s="1">
+        <v>43980</v>
+      </c>
     </row>
-    <row r="2" spans="1:85">
+    <row r="2" spans="1:86">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1462,12 +1503,12 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:85">
+    <row r="3" spans="1:86">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I3">
         <v>69</v>
@@ -1697,13 +1738,16 @@
       <c r="CG3">
         <v>43858</v>
       </c>
+      <c r="CH3">
+        <v>45629</v>
+      </c>
     </row>
-    <row r="4" spans="1:85">
+    <row r="4" spans="1:86">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AN4" s="19"/>
       <c r="AO4" s="20"/>
@@ -1728,8 +1772,11 @@
       <c r="CG4">
         <v>36511</v>
       </c>
+      <c r="CH4">
+        <v>37881</v>
+      </c>
     </row>
-    <row r="5" spans="1:85">
+    <row r="5" spans="1:86">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1985,8 +2032,11 @@
       <c r="CG5">
         <v>8538</v>
       </c>
+      <c r="CH5">
+        <v>8717</v>
+      </c>
     </row>
-    <row r="6" spans="1:85">
+    <row r="6" spans="1:86">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2224,13 +2274,16 @@
       <c r="CG6">
         <v>460</v>
       </c>
+      <c r="CH6">
+        <v>462</v>
+      </c>
     </row>
-    <row r="7" spans="1:85">
+    <row r="7" spans="1:86">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="S7">
         <v>17</v>
@@ -2433,11 +2486,14 @@
       <c r="CG7">
         <v>1089</v>
       </c>
+      <c r="CH7">
+        <v>1100</v>
+      </c>
     </row>
-    <row r="8" spans="1:85">
+    <row r="8" spans="1:86">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:85">
+    <row r="9" spans="1:86">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2537,8 +2593,11 @@
       <c r="CG9">
         <v>345</v>
       </c>
+      <c r="CH9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:85">
+    <row r="10" spans="1:86">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2740,8 +2799,11 @@
       <c r="CG10">
         <v>90</v>
       </c>
+      <c r="CH10">
+        <v>77</v>
+      </c>
     </row>
-    <row r="11" spans="1:85">
+    <row r="11" spans="1:86">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2943,8 +3005,11 @@
       <c r="CG11">
         <v>440</v>
       </c>
+      <c r="CH11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:85">
+    <row r="12" spans="1:86">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3146,8 +3211,11 @@
       <c r="CG12">
         <v>223</v>
       </c>
+      <c r="CH12">
+        <v>222</v>
+      </c>
     </row>
-    <row r="13" spans="1:85">
+    <row r="13" spans="1:86">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3349,8 +3417,11 @@
       <c r="CG13">
         <v>217</v>
       </c>
+      <c r="CH13">
+        <v>218</v>
+      </c>
     </row>
-    <row r="14" spans="1:85">
+    <row r="14" spans="1:86">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3414,13 +3485,16 @@
       <c r="CG14">
         <v>338</v>
       </c>
+      <c r="CH14">
+        <v>317</v>
+      </c>
     </row>
-    <row r="15" spans="1:85">
+    <row r="15" spans="1:86">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY15">
         <v>110</v>
@@ -3449,8 +3523,11 @@
       <c r="CG15">
         <v>114</v>
       </c>
+      <c r="CH15">
+        <v>109</v>
+      </c>
     </row>
-    <row r="16" spans="1:85">
+    <row r="16" spans="1:86">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3514,8 +3591,11 @@
       <c r="CG16">
         <v>1981</v>
       </c>
+      <c r="CH16">
+        <v>1984</v>
+      </c>
     </row>
-    <row r="17" spans="1:85">
+    <row r="17" spans="1:86">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3579,13 +3659,16 @@
       <c r="CG17" s="23">
         <v>0.8</v>
       </c>
+      <c r="CH17" s="23">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="19" spans="1:85">
+    <row r="19" spans="1:86">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:85">
+    <row r="20" spans="1:86">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3593,7 +3676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:85">
+    <row r="21" spans="1:86">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3798,8 +3881,11 @@
       <c r="CG21">
         <v>109</v>
       </c>
+      <c r="CH21">
+        <v>111</v>
+      </c>
     </row>
-    <row r="22" spans="1:85">
+    <row r="22" spans="1:86">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3950,8 +4036,11 @@
       <c r="CG22">
         <v>20</v>
       </c>
+      <c r="CH22">
+        <v>19</v>
+      </c>
     </row>
-    <row r="23" spans="1:85">
+    <row r="23" spans="1:86">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4102,8 +4191,11 @@
       <c r="CG23">
         <v>89</v>
       </c>
+      <c r="CH23">
+        <v>92</v>
+      </c>
     </row>
-    <row r="24" spans="1:85">
+    <row r="24" spans="1:86">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4299,8 +4391,11 @@
       <c r="CG24">
         <v>118</v>
       </c>
+      <c r="CH24">
+        <v>149</v>
+      </c>
     </row>
-    <row r="25" spans="1:85">
+    <row r="25" spans="1:86">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4496,8 +4591,11 @@
       <c r="CG25">
         <v>138</v>
       </c>
+      <c r="CH25">
+        <v>168</v>
+      </c>
     </row>
-    <row r="26" spans="1:85">
+    <row r="26" spans="1:86">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4693,13 +4791,16 @@
       <c r="CG26">
         <v>1324</v>
       </c>
+      <c r="CH26">
+        <v>1292</v>
+      </c>
     </row>
-    <row r="28" spans="1:85">
+    <row r="28" spans="1:86">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:85">
+    <row r="29" spans="1:86">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -4904,8 +5005,11 @@
       <c r="CG29">
         <v>132</v>
       </c>
+      <c r="CH29">
+        <v>133</v>
+      </c>
     </row>
-    <row r="30" spans="1:85">
+    <row r="30" spans="1:86">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5056,8 +5160,11 @@
       <c r="CG30">
         <v>28</v>
       </c>
+      <c r="CH30">
+        <v>27</v>
+      </c>
     </row>
-    <row r="31" spans="1:85">
+    <row r="31" spans="1:86">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5208,8 +5315,11 @@
       <c r="CG31">
         <v>104</v>
       </c>
+      <c r="CH31">
+        <v>106</v>
+      </c>
     </row>
-    <row r="32" spans="1:85">
+    <row r="32" spans="1:86">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5405,8 +5515,11 @@
       <c r="CG32">
         <v>57</v>
       </c>
+      <c r="CH32">
+        <v>49</v>
+      </c>
     </row>
-    <row r="33" spans="1:85">
+    <row r="33" spans="1:86">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5602,8 +5715,11 @@
       <c r="CG33">
         <v>85</v>
       </c>
+      <c r="CH33">
+        <v>76</v>
+      </c>
     </row>
-    <row r="34" spans="1:85">
+    <row r="34" spans="1:86">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -5799,13 +5915,16 @@
       <c r="CG34">
         <v>1194</v>
       </c>
+      <c r="CH34">
+        <v>1205</v>
+      </c>
     </row>
-    <row r="36" spans="1:85">
+    <row r="36" spans="1:86">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:85">
+    <row r="37" spans="1:86">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -5998,8 +6117,11 @@
       <c r="CG37">
         <v>80</v>
       </c>
+      <c r="CH37">
+        <v>80</v>
+      </c>
     </row>
-    <row r="38" spans="1:85">
+    <row r="38" spans="1:86">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6144,8 +6266,11 @@
       <c r="CG38">
         <v>6</v>
       </c>
+      <c r="CH38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:85">
+    <row r="39" spans="1:86">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6290,8 +6415,11 @@
       <c r="CG39">
         <v>73</v>
       </c>
+      <c r="CH39">
+        <v>73</v>
+      </c>
     </row>
-    <row r="40" spans="1:85">
+    <row r="40" spans="1:86">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6481,8 +6609,11 @@
       <c r="CG40">
         <v>1</v>
       </c>
+      <c r="CH40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:85">
+    <row r="41" spans="1:86">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6669,8 +6800,11 @@
       <c r="CG41">
         <v>7</v>
       </c>
+      <c r="CH41">
+        <v>7</v>
+      </c>
     </row>
-    <row r="42" spans="1:85">
+    <row r="42" spans="1:86">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -6863,8 +6997,11 @@
       <c r="CG42">
         <v>281</v>
       </c>
+      <c r="CH42">
+        <v>281</v>
+      </c>
     </row>
-    <row r="43" spans="1:85">
+    <row r="43" spans="1:86">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -6991,16 +7128,19 @@
       <c r="CG43">
         <v>1</v>
       </c>
+      <c r="CH43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:85">
+    <row r="44" spans="1:86">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:85">
+    <row r="45" spans="1:86">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:85">
+    <row r="46" spans="1:86">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -7199,8 +7339,11 @@
       <c r="CG46">
         <v>205</v>
       </c>
+      <c r="CH46">
+        <v>205</v>
+      </c>
     </row>
-    <row r="47" spans="1:85">
+    <row r="47" spans="1:86">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7351,8 +7494,11 @@
       <c r="CG47">
         <v>25</v>
       </c>
+      <c r="CH47">
+        <v>25</v>
+      </c>
     </row>
-    <row r="48" spans="1:85">
+    <row r="48" spans="1:86">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7503,8 +7649,11 @@
       <c r="CG48">
         <v>174</v>
       </c>
+      <c r="CH48">
+        <v>174</v>
+      </c>
     </row>
-    <row r="49" spans="1:85">
+    <row r="49" spans="1:86">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -7700,8 +7849,11 @@
       <c r="CG49">
         <v>494</v>
       </c>
+      <c r="CH49">
+        <v>500</v>
+      </c>
     </row>
-    <row r="50" spans="1:85">
+    <row r="50" spans="1:86">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -7852,8 +8004,11 @@
       <c r="CG50">
         <v>519</v>
       </c>
+      <c r="CH50">
+        <v>525</v>
+      </c>
     </row>
-    <row r="51" spans="1:85">
+    <row r="51" spans="1:86">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -8001,8 +8156,11 @@
       <c r="CG51">
         <v>839</v>
       </c>
+      <c r="CH51">
+        <v>828</v>
+      </c>
     </row>
-    <row r="52" spans="1:85">
+    <row r="52" spans="1:86">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -8144,16 +8302,19 @@
       <c r="CG52">
         <v>1</v>
       </c>
+      <c r="CH52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:85">
+    <row r="53" spans="1:86">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:85">
+    <row r="54" spans="1:86">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:85">
+    <row r="55" spans="1:86">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -8337,8 +8498,11 @@
       <c r="CG55">
         <v>30</v>
       </c>
+      <c r="CH55">
+        <v>29</v>
+      </c>
     </row>
-    <row r="56" spans="1:85">
+    <row r="56" spans="1:86">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -8486,8 +8650,11 @@
       <c r="CG56">
         <v>8</v>
       </c>
+      <c r="CH56">
+        <v>7</v>
+      </c>
     </row>
-    <row r="57" spans="1:85">
+    <row r="57" spans="1:86">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -8635,8 +8802,11 @@
       <c r="CG57">
         <v>21</v>
       </c>
+      <c r="CH57">
+        <v>21</v>
+      </c>
     </row>
-    <row r="58" spans="1:85">
+    <row r="58" spans="1:86">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -8820,8 +8990,11 @@
       <c r="CG58">
         <v>20</v>
       </c>
+      <c r="CH58">
+        <v>18</v>
+      </c>
     </row>
-    <row r="59" spans="1:85">
+    <row r="59" spans="1:86">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -9005,8 +9178,11 @@
       <c r="CG59">
         <v>28</v>
       </c>
+      <c r="CH59">
+        <v>25</v>
+      </c>
     </row>
-    <row r="60" spans="1:85">
+    <row r="60" spans="1:86">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -9190,8 +9366,11 @@
       <c r="CG60">
         <v>141</v>
       </c>
+      <c r="CH60">
+        <v>142</v>
+      </c>
     </row>
-    <row r="61" spans="1:85">
+    <row r="61" spans="1:86">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -9333,8 +9512,11 @@
       <c r="CG61">
         <v>1</v>
       </c>
+      <c r="CH61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:85">
+    <row r="63" spans="1:86">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -9518,8 +9700,11 @@
       <c r="CG63">
         <v>11</v>
       </c>
+      <c r="CH63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:85">
+    <row r="64" spans="1:86">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -9667,8 +9852,11 @@
       <c r="CG64">
         <v>4</v>
       </c>
+      <c r="CH64">
+        <v>3</v>
+      </c>
     </row>
-    <row r="65" spans="1:85">
+    <row r="65" spans="1:86">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -9816,8 +10004,11 @@
       <c r="CG65">
         <v>7</v>
       </c>
+      <c r="CH65">
+        <v>8</v>
+      </c>
     </row>
-    <row r="66" spans="1:85">
+    <row r="66" spans="1:86">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -10001,8 +10192,11 @@
       <c r="CG66">
         <v>46</v>
       </c>
+      <c r="CH66">
+        <v>48</v>
+      </c>
     </row>
-    <row r="67" spans="1:85">
+    <row r="67" spans="1:86">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -10187,8 +10381,11 @@
       <c r="CG67">
         <v>50</v>
       </c>
+      <c r="CH67">
+        <v>51</v>
+      </c>
     </row>
-    <row r="68" spans="1:85">
+    <row r="68" spans="1:86">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -10372,8 +10569,11 @@
       <c r="CG68">
         <v>0</v>
       </c>
+      <c r="CH68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:85">
+    <row r="69" spans="1:86">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -10521,13 +10721,16 @@
       <c r="CG69">
         <v>0</v>
       </c>
+      <c r="CH69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:85">
+    <row r="70" spans="1:86">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:85">
+    <row r="71" spans="1:86">
       <c r="A71" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -10559,10 +10762,13 @@
       <c r="CG71">
         <v>10</v>
       </c>
+      <c r="CH71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:85">
+    <row r="72" spans="1:86">
       <c r="A72" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
@@ -10594,10 +10800,13 @@
       <c r="CG72">
         <v>6</v>
       </c>
+      <c r="CH72">
+        <v>6</v>
+      </c>
     </row>
-    <row r="73" spans="1:85">
+    <row r="73" spans="1:86">
       <c r="A73" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -10629,10 +10838,13 @@
       <c r="CG73">
         <v>4</v>
       </c>
+      <c r="CH73">
+        <v>4</v>
+      </c>
     </row>
-    <row r="74" spans="1:85">
+    <row r="74" spans="1:86">
       <c r="A74" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
@@ -10664,10 +10876,13 @@
       <c r="CG74">
         <v>12</v>
       </c>
+      <c r="CH74">
+        <v>13</v>
+      </c>
     </row>
-    <row r="75" spans="1:85">
+    <row r="75" spans="1:86">
       <c r="A75" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
@@ -10699,10 +10914,13 @@
       <c r="CG75">
         <v>18</v>
       </c>
+      <c r="CH75">
+        <v>19</v>
+      </c>
     </row>
-    <row r="76" spans="1:85">
+    <row r="76" spans="1:86">
       <c r="A76" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
@@ -10734,13 +10952,16 @@
       <c r="CG76">
         <v>28</v>
       </c>
+      <c r="CH76">
+        <v>28</v>
+      </c>
     </row>
-    <row r="78" spans="1:85">
+    <row r="78" spans="1:86">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:85">
+    <row r="79" spans="1:86">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -10924,8 +11145,11 @@
       <c r="CG79">
         <v>295</v>
       </c>
+      <c r="CH79">
+        <v>297</v>
+      </c>
     </row>
-    <row r="80" spans="1:85">
+    <row r="80" spans="1:86">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -11109,8 +11333,11 @@
       <c r="CG80">
         <v>148</v>
       </c>
+      <c r="CH80">
+        <v>124</v>
+      </c>
     </row>
-    <row r="81" spans="1:85">
+    <row r="81" spans="1:86">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -11294,8 +11521,11 @@
       <c r="CG81">
         <v>125</v>
       </c>
+      <c r="CH81">
+        <v>104</v>
+      </c>
     </row>
-    <row r="82" spans="1:85">
+    <row r="82" spans="1:86">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -11437,8 +11667,11 @@
       <c r="CG82">
         <v>16</v>
       </c>
+      <c r="CH82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:85">
+    <row r="84" spans="1:86">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -11622,8 +11855,11 @@
       <c r="CG84">
         <v>117</v>
       </c>
+      <c r="CH84">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:85">
+    <row r="85" spans="1:86">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -11807,8 +12043,11 @@
       <c r="CG85">
         <v>27</v>
       </c>
+      <c r="CH85">
+        <v>28</v>
+      </c>
     </row>
-    <row r="86" spans="1:85">
+    <row r="86" spans="1:86">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -11992,8 +12231,11 @@
       <c r="CG86">
         <v>144</v>
       </c>
+      <c r="CH86">
+        <v>147</v>
+      </c>
     </row>
-    <row r="87" spans="1:85">
+    <row r="87" spans="1:86">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -12177,8 +12419,11 @@
       <c r="CG87">
         <v>187</v>
       </c>
+      <c r="CH87">
+        <v>190</v>
+      </c>
     </row>
-    <row r="88" spans="1:85">
+    <row r="88" spans="1:86">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -12236,8 +12481,11 @@
       <c r="CG88">
         <v>1</v>
       </c>
+      <c r="CH88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:85">
+    <row r="90" spans="1:86">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -12421,8 +12669,11 @@
       <c r="CG90">
         <v>80</v>
       </c>
+      <c r="CH90">
+        <v>79</v>
+      </c>
     </row>
-    <row r="91" spans="1:85">
+    <row r="91" spans="1:86">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -12606,8 +12857,11 @@
       <c r="CG91">
         <v>31</v>
       </c>
+      <c r="CH91">
+        <v>21</v>
+      </c>
     </row>
-    <row r="92" spans="1:85">
+    <row r="92" spans="1:86">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -12779,8 +13033,11 @@
       <c r="CG92">
         <v>163</v>
       </c>
+      <c r="CH92">
+        <v>159</v>
+      </c>
     </row>
-    <row r="93" spans="1:85">
+    <row r="93" spans="1:86">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -12964,8 +13221,11 @@
       <c r="CG93">
         <v>32</v>
       </c>
+      <c r="CH93">
+        <v>41</v>
+      </c>
     </row>
-    <row r="94" spans="1:85">
+    <row r="94" spans="1:86">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -13107,321 +13367,380 @@
       <c r="CG94">
         <v>13</v>
       </c>
+      <c r="CH94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:85">
-      <c r="A96" s="2" t="s">
+    <row r="95" spans="1:86">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" spans="1:86">
+      <c r="A96" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B96" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="CG96">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:86">
+      <c r="A97" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B97" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="CG97">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:86">
+      <c r="A98" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B98" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="CG98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:86">
+      <c r="A99" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B99" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="CG99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:86">
+      <c r="A101" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B101" t="s">
         <v>76</v>
       </c>
-      <c r="BB96">
+      <c r="BB101">
         <v>112</v>
       </c>
-      <c r="BC96">
+      <c r="BC101">
         <v>121</v>
       </c>
-      <c r="BD96">
+      <c r="BD101">
         <v>130</v>
       </c>
-      <c r="BE96">
+      <c r="BE101">
         <v>135</v>
       </c>
-      <c r="BF96">
+      <c r="BF101">
         <v>137</v>
       </c>
-      <c r="BG96">
+      <c r="BG101">
         <v>137</v>
       </c>
-      <c r="BH96">
+      <c r="BH101">
         <v>137</v>
       </c>
-      <c r="BI96">
+      <c r="BI101">
         <v>137</v>
       </c>
-      <c r="BJ96">
+      <c r="BJ101">
         <v>142</v>
       </c>
-      <c r="BK96">
+      <c r="BK101">
         <v>144</v>
       </c>
-      <c r="BL96">
+      <c r="BL101">
         <v>145</v>
       </c>
-      <c r="BM96">
+      <c r="BM101">
         <v>147</v>
       </c>
-      <c r="BN96">
+      <c r="BN101">
         <v>147</v>
       </c>
-      <c r="BO96">
+      <c r="BO101">
         <v>150</v>
       </c>
-      <c r="BP96">
+      <c r="BP101">
         <v>155</v>
       </c>
-      <c r="BQ96">
+      <c r="BQ101">
         <v>156</v>
       </c>
-      <c r="BR96">
+      <c r="BR101">
         <v>158</v>
       </c>
-      <c r="BS96">
+      <c r="BS101">
         <v>158</v>
       </c>
-      <c r="BT96">
+      <c r="BT101">
         <v>168</v>
       </c>
-      <c r="BU96">
+      <c r="BU101">
         <v>169</v>
       </c>
-      <c r="BV96">
+      <c r="BV101">
         <v>169</v>
       </c>
-      <c r="BW96">
+      <c r="BW101">
         <v>172</v>
       </c>
-      <c r="BX96">
+      <c r="BX101">
         <v>175</v>
       </c>
-      <c r="BY96">
+      <c r="BY101">
         <v>176</v>
       </c>
-      <c r="BZ96">
+      <c r="BZ101">
         <v>178</v>
       </c>
-      <c r="CA96">
+      <c r="CA101">
         <v>178</v>
       </c>
-      <c r="CB96">
+      <c r="CB101">
         <v>179</v>
       </c>
-      <c r="CC96">
+      <c r="CC101">
         <v>179</v>
       </c>
-      <c r="CD96">
+      <c r="CD101">
         <v>179</v>
       </c>
-      <c r="CE96">
+      <c r="CE101">
         <v>182</v>
       </c>
-      <c r="CF96">
+      <c r="CF101">
         <v>183</v>
       </c>
-      <c r="CG96">
+      <c r="CG101">
         <v>185</v>
       </c>
+      <c r="CH101">
+        <v>187</v>
+      </c>
     </row>
-    <row r="97" spans="1:85">
-      <c r="A97" s="2" t="s">
+    <row r="102" spans="1:86">
+      <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B102" t="s">
         <v>77</v>
       </c>
-      <c r="BB97">
+      <c r="BB102">
         <v>5</v>
       </c>
-      <c r="BC97">
+      <c r="BC102">
         <v>8</v>
       </c>
-      <c r="BD97">
+      <c r="BD102">
         <v>10</v>
       </c>
-      <c r="BE97">
+      <c r="BE102">
         <v>11</v>
       </c>
-      <c r="BF97">
+      <c r="BF102">
         <v>14</v>
       </c>
-      <c r="BG97">
+      <c r="BG102">
         <v>15</v>
       </c>
-      <c r="BH97">
+      <c r="BH102">
         <v>15</v>
       </c>
-      <c r="BI97">
+      <c r="BI102">
         <v>18</v>
       </c>
-      <c r="BJ97">
+      <c r="BJ102">
         <v>19</v>
       </c>
-      <c r="BK97">
+      <c r="BK102">
         <v>22</v>
       </c>
-      <c r="BL97">
+      <c r="BL102">
         <v>22</v>
       </c>
-      <c r="BM97">
+      <c r="BM102">
         <v>24</v>
       </c>
-      <c r="BN97">
+      <c r="BN102">
         <v>24</v>
       </c>
-      <c r="BO97">
+      <c r="BO102">
         <v>24</v>
       </c>
-      <c r="BP97">
+      <c r="BP102">
         <v>24</v>
       </c>
-      <c r="BQ97">
+      <c r="BQ102">
         <v>27</v>
       </c>
-      <c r="BR97">
+      <c r="BR102">
         <v>27</v>
       </c>
-      <c r="BS97">
+      <c r="BS102">
         <v>38</v>
       </c>
-      <c r="BT97">
+      <c r="BT102">
         <v>38</v>
       </c>
-      <c r="BU97">
+      <c r="BU102">
         <v>40</v>
       </c>
-      <c r="BV97">
+      <c r="BV102">
         <v>40</v>
       </c>
-      <c r="BW97">
+      <c r="BW102">
         <v>40</v>
       </c>
-      <c r="BX97">
+      <c r="BX102">
         <v>40</v>
       </c>
-      <c r="BY97">
+      <c r="BY102">
         <v>40</v>
       </c>
-      <c r="BZ97">
+      <c r="BZ102">
         <v>41</v>
       </c>
-      <c r="CA97">
+      <c r="CA102">
         <v>41</v>
       </c>
-      <c r="CB97">
+      <c r="CB102">
         <v>41</v>
       </c>
-      <c r="CC97">
+      <c r="CC102">
         <v>41</v>
       </c>
-      <c r="CD97">
+      <c r="CD102">
         <v>41</v>
       </c>
-      <c r="CE97">
+      <c r="CE102">
         <v>47</v>
       </c>
-      <c r="CF97">
+      <c r="CF102">
         <v>49</v>
       </c>
-      <c r="CG97">
+      <c r="CG102">
         <v>53</v>
       </c>
+      <c r="CH102">
+        <v>60</v>
+      </c>
     </row>
-    <row r="98" spans="1:85">
-      <c r="A98" s="2" t="s">
+    <row r="103" spans="1:86">
+      <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B103" t="s">
         <v>78</v>
       </c>
-      <c r="BB98">
+      <c r="BB103">
         <v>16</v>
       </c>
-      <c r="BC98">
+      <c r="BC103">
         <v>16</v>
       </c>
-      <c r="BD98">
+      <c r="BD103">
         <v>17</v>
       </c>
-      <c r="BE98">
+      <c r="BE103">
         <v>17</v>
       </c>
-      <c r="BF98">
+      <c r="BF103">
         <v>18</v>
       </c>
-      <c r="BG98">
+      <c r="BG103">
         <v>18</v>
       </c>
-      <c r="BH98">
+      <c r="BH103">
         <v>19</v>
       </c>
-      <c r="BI98">
+      <c r="BI103">
         <v>19</v>
       </c>
-      <c r="BJ98">
+      <c r="BJ103">
         <v>19</v>
       </c>
-      <c r="BK98">
+      <c r="BK103">
         <v>19</v>
       </c>
-      <c r="BL98">
+      <c r="BL103">
         <v>20</v>
       </c>
-      <c r="BM98">
+      <c r="BM103">
         <v>20</v>
       </c>
-      <c r="BN98">
+      <c r="BN103">
         <v>20</v>
       </c>
-      <c r="BO98">
+      <c r="BO103">
         <v>20</v>
       </c>
-      <c r="BP98">
+      <c r="BP103">
         <v>20</v>
       </c>
-      <c r="BQ98">
+      <c r="BQ103">
         <v>21</v>
       </c>
-      <c r="BR98">
+      <c r="BR103">
         <v>22</v>
       </c>
-      <c r="BS98">
+      <c r="BS103">
         <v>23</v>
       </c>
-      <c r="BT98">
+      <c r="BT103">
         <v>24</v>
       </c>
-      <c r="BU98">
+      <c r="BU103">
         <v>24</v>
       </c>
-      <c r="BV98">
+      <c r="BV103">
         <v>24</v>
       </c>
-      <c r="BW98">
+      <c r="BW103">
         <v>24</v>
       </c>
-      <c r="BX98">
+      <c r="BX103">
         <v>25</v>
       </c>
-      <c r="BY98">
+      <c r="BY103">
         <v>25</v>
       </c>
-      <c r="BZ98">
+      <c r="BZ103">
         <v>25</v>
       </c>
-      <c r="CA98">
+      <c r="CA103">
         <v>25</v>
       </c>
-      <c r="CB98">
+      <c r="CB103">
         <v>25</v>
       </c>
-      <c r="CC98">
+      <c r="CC103">
         <v>25</v>
       </c>
-      <c r="CD98">
+      <c r="CD103">
         <v>25</v>
       </c>
-      <c r="CE98">
+      <c r="CE103">
         <v>25</v>
       </c>
-      <c r="CF98">
+      <c r="CF103">
         <v>25</v>
       </c>
-      <c r="CG98">
+      <c r="CG103">
         <v>25</v>
       </c>
+      <c r="CH103">
+        <v>25</v>
+      </c>
     </row>
-    <row r="113" spans="52:52">
-      <c r="AZ113">
+    <row r="118" spans="52:52">
+      <c r="AZ118">
         <v>9</v>
       </c>
     </row>
@@ -13433,10 +13752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BH11"/>
+  <dimension ref="A2:BI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BH11" sqref="BH3:BH11"/>
+    <sheetView tabSelected="1" topLeftCell="BA2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BI3" sqref="BI3:BI11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13446,7 +13765,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:60" s="2" customFormat="1">
+    <row r="2" spans="1:61" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -13627,8 +13946,11 @@
       <c r="BH2" s="9">
         <v>43979</v>
       </c>
+      <c r="BI2" s="9">
+        <v>43980</v>
+      </c>
     </row>
-    <row r="3" spans="1:60">
+    <row r="3" spans="1:61">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -13809,8 +14131,11 @@
       <c r="BH3">
         <v>1198</v>
       </c>
+      <c r="BI3">
+        <v>1221</v>
+      </c>
     </row>
-    <row r="4" spans="1:60">
+    <row r="4" spans="1:61">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -13991,8 +14316,11 @@
       <c r="BH4">
         <v>512</v>
       </c>
+      <c r="BI4">
+        <v>507</v>
+      </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:61">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -14173,8 +14501,11 @@
       <c r="BH5">
         <v>416</v>
       </c>
+      <c r="BI5">
+        <v>400</v>
+      </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:61">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -14355,8 +14686,11 @@
       <c r="BH6">
         <v>1795</v>
       </c>
+      <c r="BI6">
+        <v>1828</v>
+      </c>
     </row>
-    <row r="7" spans="1:60">
+    <row r="7" spans="1:61">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -14537,8 +14871,11 @@
       <c r="BH7">
         <v>1331</v>
       </c>
+      <c r="BI7">
+        <v>1351</v>
+      </c>
     </row>
-    <row r="8" spans="1:60">
+    <row r="8" spans="1:61">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -14719,8 +15056,11 @@
       <c r="BH8">
         <v>729</v>
       </c>
+      <c r="BI8">
+        <v>750</v>
+      </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:61">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -14901,8 +15241,11 @@
       <c r="BH9">
         <v>1224</v>
       </c>
+      <c r="BI9">
+        <v>1269</v>
+      </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:61">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -15083,8 +15426,11 @@
       <c r="BH10">
         <v>1196</v>
       </c>
+      <c r="BI10">
+        <v>1242</v>
+      </c>
     </row>
-    <row r="11" spans="1:60">
+    <row r="11" spans="1:61">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -15264,6 +15610,9 @@
       </c>
       <c r="BH11">
         <v>137</v>
+      </c>
+      <c r="BI11">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -15274,10 +15623,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BC17"/>
+  <dimension ref="A2:BD17"/>
   <sheetViews>
-    <sheetView topLeftCell="AO10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BC17" sqref="BC17"/>
+    <sheetView topLeftCell="AY1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BD14" sqref="BD14:BD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15287,7 +15636,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:55" s="2" customFormat="1">
+    <row r="2" spans="1:56" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -15451,8 +15800,11 @@
       <c r="BC2" s="9">
         <v>43979</v>
       </c>
+      <c r="BD2" s="9">
+        <v>43980</v>
+      </c>
     </row>
-    <row r="3" spans="1:55" s="2" customFormat="1">
+    <row r="3" spans="1:56" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -15460,7 +15812,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:55">
+    <row r="4" spans="1:56">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -15626,8 +15978,11 @@
       <c r="BC4">
         <v>8538</v>
       </c>
+      <c r="BD4">
+        <v>8717</v>
+      </c>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:56">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -15793,8 +16148,11 @@
       <c r="BC5">
         <v>870</v>
       </c>
+      <c r="BD5">
+        <v>939</v>
+      </c>
     </row>
-    <row r="6" spans="1:55">
+    <row r="6" spans="1:56">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -15960,8 +16318,11 @@
       <c r="BC6">
         <v>1331</v>
       </c>
+      <c r="BD6">
+        <v>1342</v>
+      </c>
     </row>
-    <row r="7" spans="1:55">
+    <row r="7" spans="1:56">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -16127,8 +16488,11 @@
       <c r="BC7">
         <v>3991</v>
       </c>
+      <c r="BD7">
+        <v>4055</v>
+      </c>
     </row>
-    <row r="8" spans="1:55">
+    <row r="8" spans="1:56">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -16294,8 +16658,11 @@
       <c r="BC8">
         <v>106</v>
       </c>
+      <c r="BD8">
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:55" ht="30">
+    <row r="9" spans="1:56" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -16461,8 +16828,11 @@
       <c r="BC9">
         <v>26</v>
       </c>
+      <c r="BD9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:55" ht="30">
+    <row r="10" spans="1:56" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -16624,8 +16994,11 @@
       <c r="BC10">
         <v>21</v>
       </c>
+      <c r="BD10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:55">
+    <row r="11" spans="1:56">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -16791,8 +17164,11 @@
       <c r="BC11">
         <v>2135</v>
       </c>
+      <c r="BD11">
+        <v>2169</v>
+      </c>
     </row>
-    <row r="12" spans="1:55" ht="30">
+    <row r="12" spans="1:56" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -16958,8 +17334,11 @@
       <c r="BC12">
         <v>58</v>
       </c>
+      <c r="BD12">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:55">
+    <row r="13" spans="1:56">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -16970,7 +17349,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:55">
+    <row r="14" spans="1:56">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -17136,8 +17515,11 @@
       <c r="BC14">
         <v>1419</v>
       </c>
+      <c r="BD14">
+        <v>1500</v>
+      </c>
     </row>
-    <row r="15" spans="1:55">
+    <row r="15" spans="1:56">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -17303,8 +17685,11 @@
       <c r="BC15">
         <v>2272</v>
       </c>
+      <c r="BD15">
+        <v>2309</v>
+      </c>
     </row>
-    <row r="16" spans="1:55">
+    <row r="16" spans="1:56">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -17470,8 +17855,11 @@
       <c r="BC16">
         <v>4822</v>
       </c>
+      <c r="BD16">
+        <v>4883</v>
+      </c>
     </row>
-    <row r="17" spans="1:55" ht="30">
+    <row r="17" spans="1:56" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -17635,6 +18023,9 @@
         <v>27</v>
       </c>
       <c r="BC17">
+        <v>25</v>
+      </c>
+      <c r="BD17">
         <v>25</v>
       </c>
     </row>
@@ -17646,10 +18037,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BC9"/>
+  <dimension ref="A1:BD9"/>
   <sheetViews>
-    <sheetView topLeftCell="AL2" workbookViewId="0">
-      <selection activeCell="BC11" sqref="BC11"/>
+    <sheetView topLeftCell="AZ1" workbookViewId="0">
+      <selection activeCell="BG11" sqref="BG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17658,7 +18049,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="2" customFormat="1">
+    <row r="1" spans="1:56" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -17821,14 +18212,17 @@
       <c r="BC1" s="9">
         <v>43979</v>
       </c>
+      <c r="BD1" s="9">
+        <v>43980</v>
+      </c>
     </row>
-    <row r="2" spans="1:55">
+    <row r="2" spans="1:56">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:55">
+    <row r="3" spans="1:56">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -17995,8 +18389,11 @@
       <c r="BC3">
         <v>460</v>
       </c>
+      <c r="BD3">
+        <v>462</v>
+      </c>
     </row>
-    <row r="4" spans="1:55">
+    <row r="4" spans="1:56">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -18162,8 +18559,11 @@
       <c r="BC4">
         <v>7</v>
       </c>
+      <c r="BD4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:55" ht="30">
+    <row r="5" spans="1:56" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -18329,8 +18729,11 @@
       <c r="BC5">
         <v>344</v>
       </c>
+      <c r="BD5">
+        <v>346</v>
+      </c>
     </row>
-    <row r="6" spans="1:55">
+    <row r="6" spans="1:56">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -18496,8 +18899,11 @@
       <c r="BC6">
         <v>52</v>
       </c>
+      <c r="BD6">
+        <v>52</v>
+      </c>
     </row>
-    <row r="7" spans="1:55" ht="30">
+    <row r="7" spans="1:56" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -18663,8 +19069,11 @@
       <c r="BC7">
         <v>53</v>
       </c>
+      <c r="BD7">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:55">
+    <row r="8" spans="1:56">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -18830,8 +19239,11 @@
       <c r="BC8">
         <v>3</v>
       </c>
+      <c r="BD8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:55">
+    <row r="9" spans="1:56">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -18839,6 +19251,9 @@
         <v>1</v>
       </c>
       <c r="BC9">
+        <v>1</v>
+      </c>
+      <c r="BD9">
         <v>1</v>
       </c>
     </row>
@@ -18849,10 +19264,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AO13"/>
+  <dimension ref="A2:AP13"/>
   <sheetViews>
-    <sheetView topLeftCell="AD4" workbookViewId="0">
-      <selection activeCell="AQ12" sqref="AQ12"/>
+    <sheetView topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AP3" sqref="AP3:AP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18860,7 +19275,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:41" s="2" customFormat="1">
+    <row r="2" spans="1:42" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -18984,8 +19399,11 @@
       <c r="AO2" s="9">
         <v>43979</v>
       </c>
+      <c r="AP2" s="9">
+        <v>43980</v>
+      </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:42">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -19109,8 +19527,11 @@
       <c r="AO3">
         <v>460</v>
       </c>
+      <c r="AP3">
+        <v>462</v>
+      </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:42">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -19234,8 +19655,11 @@
       <c r="AO4">
         <v>47</v>
       </c>
+      <c r="AP4">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:42">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -19359,8 +19783,11 @@
       <c r="AO5">
         <v>29</v>
       </c>
+      <c r="AP5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:42">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -19484,8 +19911,11 @@
       <c r="AO6">
         <v>30</v>
       </c>
+      <c r="AP6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:42">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -19609,8 +20039,11 @@
       <c r="AO7">
         <v>65</v>
       </c>
+      <c r="AP7">
+        <v>65</v>
+      </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:42">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -19734,8 +20167,11 @@
       <c r="AO8">
         <v>73</v>
       </c>
+      <c r="AP8">
+        <v>73</v>
+      </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:42">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -19859,8 +20295,11 @@
       <c r="AO9">
         <v>42</v>
       </c>
+      <c r="AP9">
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:42">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -19984,8 +20423,11 @@
       <c r="AO10">
         <v>64</v>
       </c>
+      <c r="AP10">
+        <v>66</v>
+      </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:42">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -20109,8 +20551,11 @@
       <c r="AO11">
         <v>94</v>
       </c>
+      <c r="AP11">
+        <v>94</v>
+      </c>
     </row>
-    <row r="12" spans="1:41" ht="30">
+    <row r="12" spans="1:42" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -20234,8 +20679,11 @@
       <c r="AO12">
         <v>16</v>
       </c>
+      <c r="AP12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:42">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -20357,6 +20805,9 @@
         <v>0</v>
       </c>
       <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
         <v>0</v>
       </c>
     </row>
@@ -20370,8 +20821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O3"/>
+    <sheetView topLeftCell="A20" zoomScale="82" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20380,51 +20831,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="C1" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+      <c r="C1" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
     </row>
     <row r="4" spans="1:15">
       <c r="C4" s="34"/>
@@ -20469,10 +20920,13 @@
       <c r="K5" s="9">
         <v>43979</v>
       </c>
+      <c r="L5" s="9">
+        <v>43980</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6">
         <v>103</v>
@@ -20499,6 +20953,9 @@
         <v>113</v>
       </c>
       <c r="K6">
+        <v>113</v>
+      </c>
+      <c r="L6">
         <v>113</v>
       </c>
     </row>
@@ -20533,11 +20990,17 @@
       <c r="K7">
         <v>30</v>
       </c>
+      <c r="L7">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
+      <c r="L8" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="31" t="s">
@@ -20570,10 +21033,13 @@
       <c r="K9">
         <v>1</v>
       </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C10">
         <v>18</v>
@@ -20600,12 +21066,15 @@
         <v>21</v>
       </c>
       <c r="K10">
+        <v>21</v>
+      </c>
+      <c r="L10">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -20632,6 +21101,9 @@
         <v>6</v>
       </c>
       <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
         <v>6</v>
       </c>
     </row>
@@ -20666,6 +21138,9 @@
       <c r="K12">
         <v>2</v>
       </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="36" t="s">
@@ -20703,6 +21178,9 @@
       <c r="K14">
         <v>1</v>
       </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="31">
@@ -20735,6 +21213,9 @@
       <c r="K15">
         <v>0</v>
       </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="31">
@@ -20767,8 +21248,11 @@
       <c r="K16">
         <v>2</v>
       </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -20799,8 +21283,11 @@
       <c r="K17">
         <v>9</v>
       </c>
+      <c r="L17">
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:12">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -20831,8 +21318,11 @@
       <c r="K18">
         <v>2</v>
       </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:12">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -20863,8 +21353,11 @@
       <c r="K19">
         <v>2</v>
       </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:12">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -20895,8 +21388,11 @@
       <c r="K20">
         <v>3</v>
       </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -20927,8 +21423,11 @@
       <c r="K21">
         <v>6</v>
       </c>
+      <c r="L21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:11" ht="45">
+    <row r="22" spans="1:12" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -20959,10 +21458,13 @@
       <c r="K22">
         <v>4</v>
       </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:11" ht="30">
+    <row r="23" spans="1:12" ht="30">
       <c r="A23" s="39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -20989,6 +21491,9 @@
         <v>1</v>
       </c>
       <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
         <v>1</v>
       </c>
     </row>
@@ -21004,7 +21509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -21020,18 +21525,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A1" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="A1" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:7" ht="36.6" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -21040,7 +21545,7 @@
       <c r="C2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="48" t="s">
         <v>124</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -21050,14 +21555,14 @@
         <v>125</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1">
-      <c r="A3" s="44"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="45"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="25" t="s">
         <v>92</v>
       </c>
@@ -21069,10 +21574,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1">
-      <c r="A4" s="44"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="45"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="25" t="s">
         <v>86</v>
       </c>
@@ -21082,10 +21587,10 @@
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1">
-      <c r="A5" s="44"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="45"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="25" t="s">
         <v>87</v>
       </c>
@@ -21093,10 +21598,10 @@
       <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1">
-      <c r="A6" s="44"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="45"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="25" t="s">
         <v>88</v>
       </c>
@@ -21104,10 +21609,10 @@
       <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1">
-      <c r="A7" s="44"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="45"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="25" t="s">
         <v>93</v>
       </c>
@@ -21119,7 +21624,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C8" s="28">
         <v>3</v>
@@ -21142,10 +21647,10 @@
         <v>96</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="C9" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="28">
         <v>0</v>
@@ -21165,7 +21670,7 @@
         <v>98</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="28">
         <v>4</v>
@@ -21174,7 +21679,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F10" s="28">
         <v>1</v>
@@ -21188,16 +21693,16 @@
         <v>99</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C11" s="28">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="28">
         <v>0</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
@@ -21231,7 +21736,7 @@
     </row>
     <row r="13" spans="1:7" ht="14.45" customHeight="1">
       <c r="A13" s="27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>97</v>
@@ -21257,10 +21762,10 @@
         <v>103</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C14" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="28">
         <v>0</v>
@@ -21280,7 +21785,7 @@
         <v>104</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C15" s="28">
         <v>15</v>
@@ -21289,7 +21794,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F15" s="28">
         <v>1</v>
@@ -21300,7 +21805,7 @@
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1">
       <c r="A16" s="30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>105</v>
@@ -21335,7 +21840,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F17" s="28">
         <v>1</v>
@@ -21349,7 +21854,7 @@
         <v>109</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C18" s="28">
         <v>12</v>
@@ -21358,7 +21863,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F18" s="28">
         <v>0</v>
@@ -21372,7 +21877,7 @@
         <v>110</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C19" s="28">
         <v>13</v>
@@ -21381,7 +21886,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
@@ -21395,7 +21900,7 @@
         <v>111</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C20" s="28">
         <v>17</v>
@@ -21441,7 +21946,7 @@
         <v>115</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C22" s="28">
         <v>25</v>
@@ -21450,7 +21955,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F22" s="28">
         <v>1</v>
@@ -21487,7 +21992,7 @@
         <v>118</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C24" s="28">
         <v>8</v>
@@ -21507,10 +22012,10 @@
     </row>
     <row r="25" spans="1:7" ht="33.6" customHeight="1">
       <c r="A25" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="28" t="s">
         <v>129</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>131</v>
       </c>
       <c r="C25" s="28">
         <v>18</v>
@@ -21533,16 +22038,16 @@
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" s="28">
+        <v>157</v>
+      </c>
+      <c r="D26" s="28">
+        <v>0</v>
+      </c>
+      <c r="E26" s="28" t="s">
         <v>160</v>
-      </c>
-      <c r="C26" s="28">
-        <v>158</v>
-      </c>
-      <c r="D26" s="28">
-        <v>0</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>161</v>
       </c>
       <c r="F26" s="28">
         <v>5</v>
@@ -21556,7 +22061,7 @@
         <v>120</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -21813,16 +22318,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
31 May data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3A9690-C937-4546-9E11-F7EB52496C61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E24960D-C329-404F-9ECE-927FDE7D02C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="163">
   <si>
     <t>Testing</t>
   </si>
@@ -494,42 +494,10 @@
     <t>58; (33)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">As of May 28, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>113 cases</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for COVID-19 testing,  and 30 (26.5%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
-    </r>
-  </si>
-  <si>
     <t>45; (29)</t>
   </si>
   <si>
-    <t>142; (44)</t>
-  </si>
-  <si>
     <t>16; (8)</t>
-  </si>
-  <si>
-    <t>As of May 29, 2020</t>
   </si>
   <si>
     <t>3; (0)</t>
@@ -541,32 +509,55 @@
     <t>34; (25)</t>
   </si>
   <si>
-    <t>650; (289)</t>
-  </si>
-  <si>
     <t>197; (79)</t>
-  </si>
-  <si>
-    <t>847; (368)</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Human Services - CFSA</t>
+    <t>As of May 30, 2020</t>
   </si>
   <si>
-    <t>Number of Personnel Who Have Tested Positive</t>
+    <t>152; (46)</t>
   </si>
   <si>
-    <t>Number of Personnel Currently in Quarantine</t>
+    <t>660; (291)</t>
+  </si>
+  <si>
+    <t>857; (370)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As of May 30, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>119 cases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for COVID-19 testing,  and 31 (26.1%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,17 +626,6 @@
       <color rgb="FF112277"/>
       <name val="Albany AMT"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -679,7 +659,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -687,26 +667,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD9E1F2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD9E1F2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD9E1F2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD9E1F2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -808,9 +773,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1206,11 +1168,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CH118"/>
+  <dimension ref="A1:CI113"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="CF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CH96" sqref="CH96"/>
+      <pane xSplit="2" topLeftCell="BY1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CI1" sqref="CI1:CI1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1222,10 +1184,10 @@
     <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="86" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="87" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86">
+    <row r="1" spans="1:87">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1478,8 +1440,11 @@
       <c r="CH1" s="1">
         <v>43980</v>
       </c>
+      <c r="CI1" s="1">
+        <v>43981</v>
+      </c>
     </row>
-    <row r="2" spans="1:86">
+    <row r="2" spans="1:87">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1503,7 +1468,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:86">
+    <row r="3" spans="1:87">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1741,8 +1706,11 @@
       <c r="CH3">
         <v>45629</v>
       </c>
+      <c r="CI3">
+        <v>46483</v>
+      </c>
     </row>
-    <row r="4" spans="1:86">
+    <row r="4" spans="1:87">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1775,8 +1743,11 @@
       <c r="CH4">
         <v>37881</v>
       </c>
+      <c r="CI4">
+        <v>38413</v>
+      </c>
     </row>
-    <row r="5" spans="1:86">
+    <row r="5" spans="1:87">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2035,8 +2006,11 @@
       <c r="CH5">
         <v>8717</v>
       </c>
+      <c r="CI5">
+        <v>8801</v>
+      </c>
     </row>
-    <row r="6" spans="1:86">
+    <row r="6" spans="1:87">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2277,8 +2251,11 @@
       <c r="CH6">
         <v>462</v>
       </c>
+      <c r="CI6">
+        <v>466</v>
+      </c>
     </row>
-    <row r="7" spans="1:86">
+    <row r="7" spans="1:87">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2489,11 +2466,14 @@
       <c r="CH7">
         <v>1100</v>
       </c>
+      <c r="CI7">
+        <v>1116</v>
+      </c>
     </row>
-    <row r="8" spans="1:86">
+    <row r="8" spans="1:87">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:86">
+    <row r="9" spans="1:87">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2596,8 +2576,11 @@
       <c r="CH9">
         <v>345</v>
       </c>
+      <c r="CI9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:86">
+    <row r="10" spans="1:87">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2802,8 +2785,11 @@
       <c r="CH10">
         <v>77</v>
       </c>
+      <c r="CI10">
+        <v>59</v>
+      </c>
     </row>
-    <row r="11" spans="1:86">
+    <row r="11" spans="1:87">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3008,8 +2994,11 @@
       <c r="CH11">
         <v>440</v>
       </c>
+      <c r="CI11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:86">
+    <row r="12" spans="1:87">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3214,8 +3203,11 @@
       <c r="CH12">
         <v>222</v>
       </c>
+      <c r="CI12">
+        <v>215</v>
+      </c>
     </row>
-    <row r="13" spans="1:86">
+    <row r="13" spans="1:87">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3420,8 +3412,11 @@
       <c r="CH13">
         <v>218</v>
       </c>
+      <c r="CI13">
+        <v>225</v>
+      </c>
     </row>
-    <row r="14" spans="1:86">
+    <row r="14" spans="1:87">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3488,8 +3483,11 @@
       <c r="CH14">
         <v>317</v>
       </c>
+      <c r="CI14">
+        <v>295</v>
+      </c>
     </row>
-    <row r="15" spans="1:86">
+    <row r="15" spans="1:87">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3526,8 +3524,11 @@
       <c r="CH15">
         <v>109</v>
       </c>
+      <c r="CI15">
+        <v>109</v>
+      </c>
     </row>
-    <row r="16" spans="1:86">
+    <row r="16" spans="1:87">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3594,8 +3595,11 @@
       <c r="CH16">
         <v>1984</v>
       </c>
+      <c r="CI16">
+        <v>1931</v>
+      </c>
     </row>
-    <row r="17" spans="1:86">
+    <row r="17" spans="1:87">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3662,13 +3666,16 @@
       <c r="CH17" s="23">
         <v>0.8</v>
       </c>
+      <c r="CI17" s="23">
+        <v>0.78</v>
+      </c>
     </row>
-    <row r="19" spans="1:86">
+    <row r="19" spans="1:87">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:86">
+    <row r="20" spans="1:87">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3676,7 +3683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:86">
+    <row r="21" spans="1:87">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3884,8 +3891,11 @@
       <c r="CH21">
         <v>111</v>
       </c>
+      <c r="CI21">
+        <v>111</v>
+      </c>
     </row>
-    <row r="22" spans="1:86">
+    <row r="22" spans="1:87">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4039,8 +4049,11 @@
       <c r="CH22">
         <v>19</v>
       </c>
+      <c r="CI22">
+        <v>19</v>
+      </c>
     </row>
-    <row r="23" spans="1:86">
+    <row r="23" spans="1:87">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4194,8 +4207,11 @@
       <c r="CH23">
         <v>92</v>
       </c>
+      <c r="CI23">
+        <v>92</v>
+      </c>
     </row>
-    <row r="24" spans="1:86">
+    <row r="24" spans="1:87">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4394,8 +4410,11 @@
       <c r="CH24">
         <v>149</v>
       </c>
+      <c r="CI24">
+        <v>123</v>
+      </c>
     </row>
-    <row r="25" spans="1:86">
+    <row r="25" spans="1:87">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4594,8 +4613,11 @@
       <c r="CH25">
         <v>168</v>
       </c>
+      <c r="CI25">
+        <v>142</v>
+      </c>
     </row>
-    <row r="26" spans="1:86">
+    <row r="26" spans="1:87">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4794,13 +4816,16 @@
       <c r="CH26">
         <v>1292</v>
       </c>
+      <c r="CI26">
+        <v>1371</v>
+      </c>
     </row>
-    <row r="28" spans="1:86">
+    <row r="28" spans="1:87">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:86">
+    <row r="29" spans="1:87">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5008,8 +5033,11 @@
       <c r="CH29">
         <v>133</v>
       </c>
+      <c r="CI29">
+        <v>134</v>
+      </c>
     </row>
-    <row r="30" spans="1:86">
+    <row r="30" spans="1:87">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5163,8 +5191,11 @@
       <c r="CH30">
         <v>27</v>
       </c>
+      <c r="CI30">
+        <v>28</v>
+      </c>
     </row>
-    <row r="31" spans="1:86">
+    <row r="31" spans="1:87">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5318,8 +5349,11 @@
       <c r="CH31">
         <v>106</v>
       </c>
+      <c r="CI31">
+        <v>106</v>
+      </c>
     </row>
-    <row r="32" spans="1:86">
+    <row r="32" spans="1:87">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5518,8 +5552,11 @@
       <c r="CH32">
         <v>49</v>
       </c>
+      <c r="CI32">
+        <v>48</v>
+      </c>
     </row>
-    <row r="33" spans="1:86">
+    <row r="33" spans="1:87">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5718,8 +5755,11 @@
       <c r="CH33">
         <v>76</v>
       </c>
+      <c r="CI33">
+        <v>76</v>
+      </c>
     </row>
-    <row r="34" spans="1:86">
+    <row r="34" spans="1:87">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -5918,13 +5958,16 @@
       <c r="CH34">
         <v>1205</v>
       </c>
+      <c r="CI34">
+        <v>1206</v>
+      </c>
     </row>
-    <row r="36" spans="1:86">
+    <row r="36" spans="1:87">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:86">
+    <row r="37" spans="1:87">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -6120,8 +6163,11 @@
       <c r="CH37">
         <v>80</v>
       </c>
+      <c r="CI37">
+        <v>80</v>
+      </c>
     </row>
-    <row r="38" spans="1:86">
+    <row r="38" spans="1:87">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6269,8 +6315,11 @@
       <c r="CH38">
         <v>6</v>
       </c>
+      <c r="CI38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:86">
+    <row r="39" spans="1:87">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6418,8 +6467,11 @@
       <c r="CH39">
         <v>73</v>
       </c>
+      <c r="CI39">
+        <v>73</v>
+      </c>
     </row>
-    <row r="40" spans="1:86">
+    <row r="40" spans="1:87">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6612,8 +6664,11 @@
       <c r="CH40">
         <v>1</v>
       </c>
+      <c r="CI40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:86">
+    <row r="41" spans="1:87">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6803,8 +6858,11 @@
       <c r="CH41">
         <v>7</v>
       </c>
+      <c r="CI41">
+        <v>7</v>
+      </c>
     </row>
-    <row r="42" spans="1:86">
+    <row r="42" spans="1:87">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7000,8 +7058,11 @@
       <c r="CH42">
         <v>281</v>
       </c>
+      <c r="CI42">
+        <v>281</v>
+      </c>
     </row>
-    <row r="43" spans="1:86">
+    <row r="43" spans="1:87">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -7131,16 +7192,19 @@
       <c r="CH43">
         <v>1</v>
       </c>
+      <c r="CI43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:86">
+    <row r="44" spans="1:87">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:86">
+    <row r="45" spans="1:87">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:86">
+    <row r="46" spans="1:87">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -7342,8 +7406,11 @@
       <c r="CH46">
         <v>205</v>
       </c>
+      <c r="CI46">
+        <v>205</v>
+      </c>
     </row>
-    <row r="47" spans="1:86">
+    <row r="47" spans="1:87">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7497,8 +7564,11 @@
       <c r="CH47">
         <v>25</v>
       </c>
+      <c r="CI47">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:86">
+    <row r="48" spans="1:87">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7652,8 +7722,11 @@
       <c r="CH48">
         <v>174</v>
       </c>
+      <c r="CI48">
+        <v>175</v>
+      </c>
     </row>
-    <row r="49" spans="1:86">
+    <row r="49" spans="1:87">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -7852,8 +7925,11 @@
       <c r="CH49">
         <v>500</v>
       </c>
+      <c r="CI49">
+        <v>470</v>
+      </c>
     </row>
-    <row r="50" spans="1:86">
+    <row r="50" spans="1:87">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -8007,8 +8083,11 @@
       <c r="CH50">
         <v>525</v>
       </c>
+      <c r="CI50">
+        <v>494</v>
+      </c>
     </row>
-    <row r="51" spans="1:86">
+    <row r="51" spans="1:87">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -8159,8 +8238,11 @@
       <c r="CH51">
         <v>828</v>
       </c>
+      <c r="CI51">
+        <v>815</v>
+      </c>
     </row>
-    <row r="52" spans="1:86">
+    <row r="52" spans="1:87">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -8305,16 +8387,19 @@
       <c r="CH52">
         <v>1</v>
       </c>
+      <c r="CI52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:86">
+    <row r="53" spans="1:87">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:86">
+    <row r="54" spans="1:87">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:86">
+    <row r="55" spans="1:87">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -8501,8 +8586,11 @@
       <c r="CH55">
         <v>29</v>
       </c>
+      <c r="CI55">
+        <v>29</v>
+      </c>
     </row>
-    <row r="56" spans="1:86">
+    <row r="56" spans="1:87">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -8653,8 +8741,11 @@
       <c r="CH56">
         <v>7</v>
       </c>
+      <c r="CI56">
+        <v>7</v>
+      </c>
     </row>
-    <row r="57" spans="1:86">
+    <row r="57" spans="1:87">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -8805,8 +8896,11 @@
       <c r="CH57">
         <v>21</v>
       </c>
+      <c r="CI57">
+        <v>21</v>
+      </c>
     </row>
-    <row r="58" spans="1:86">
+    <row r="58" spans="1:87">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -8993,8 +9087,11 @@
       <c r="CH58">
         <v>18</v>
       </c>
+      <c r="CI58">
+        <v>18</v>
+      </c>
     </row>
-    <row r="59" spans="1:86">
+    <row r="59" spans="1:87">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -9181,8 +9278,11 @@
       <c r="CH59">
         <v>25</v>
       </c>
+      <c r="CI59">
+        <v>25</v>
+      </c>
     </row>
-    <row r="60" spans="1:86">
+    <row r="60" spans="1:87">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -9369,8 +9469,11 @@
       <c r="CH60">
         <v>142</v>
       </c>
+      <c r="CI60">
+        <v>142</v>
+      </c>
     </row>
-    <row r="61" spans="1:86">
+    <row r="61" spans="1:87">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -9515,8 +9618,11 @@
       <c r="CH61">
         <v>1</v>
       </c>
+      <c r="CI61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:86">
+    <row r="63" spans="1:87">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -9703,8 +9809,11 @@
       <c r="CH63">
         <v>11</v>
       </c>
+      <c r="CI63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:86">
+    <row r="64" spans="1:87">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -9855,8 +9964,11 @@
       <c r="CH64">
         <v>3</v>
       </c>
+      <c r="CI64">
+        <v>3</v>
+      </c>
     </row>
-    <row r="65" spans="1:86">
+    <row r="65" spans="1:87">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -10007,8 +10119,11 @@
       <c r="CH65">
         <v>8</v>
       </c>
+      <c r="CI65">
+        <v>8</v>
+      </c>
     </row>
-    <row r="66" spans="1:86">
+    <row r="66" spans="1:87">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -10195,8 +10310,11 @@
       <c r="CH66">
         <v>48</v>
       </c>
+      <c r="CI66">
+        <v>48</v>
+      </c>
     </row>
-    <row r="67" spans="1:86">
+    <row r="67" spans="1:87">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -10384,8 +10502,11 @@
       <c r="CH67">
         <v>51</v>
       </c>
+      <c r="CI67">
+        <v>51</v>
+      </c>
     </row>
-    <row r="68" spans="1:86">
+    <row r="68" spans="1:87">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -10572,8 +10693,11 @@
       <c r="CH68">
         <v>0</v>
       </c>
+      <c r="CI68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:86">
+    <row r="69" spans="1:87">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -10724,11 +10848,14 @@
       <c r="CH69">
         <v>0</v>
       </c>
+      <c r="CI69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:86">
+    <row r="70" spans="1:87">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:86">
+    <row r="71" spans="1:87">
       <c r="A71" s="2" t="s">
         <v>132</v>
       </c>
@@ -10765,8 +10892,11 @@
       <c r="CH71">
         <v>10</v>
       </c>
+      <c r="CI71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:86">
+    <row r="72" spans="1:87">
       <c r="A72" s="2" t="s">
         <v>132</v>
       </c>
@@ -10803,8 +10933,11 @@
       <c r="CH72">
         <v>6</v>
       </c>
+      <c r="CI72">
+        <v>6</v>
+      </c>
     </row>
-    <row r="73" spans="1:86">
+    <row r="73" spans="1:87">
       <c r="A73" s="2" t="s">
         <v>132</v>
       </c>
@@ -10841,8 +10974,11 @@
       <c r="CH73">
         <v>4</v>
       </c>
+      <c r="CI73">
+        <v>4</v>
+      </c>
     </row>
-    <row r="74" spans="1:86">
+    <row r="74" spans="1:87">
       <c r="A74" s="2" t="s">
         <v>132</v>
       </c>
@@ -10879,8 +11015,11 @@
       <c r="CH74">
         <v>13</v>
       </c>
+      <c r="CI74">
+        <v>13</v>
+      </c>
     </row>
-    <row r="75" spans="1:86">
+    <row r="75" spans="1:87">
       <c r="A75" s="2" t="s">
         <v>132</v>
       </c>
@@ -10917,8 +11056,11 @@
       <c r="CH75">
         <v>19</v>
       </c>
+      <c r="CI75">
+        <v>19</v>
+      </c>
     </row>
-    <row r="76" spans="1:86">
+    <row r="76" spans="1:87">
       <c r="A76" s="2" t="s">
         <v>132</v>
       </c>
@@ -10955,13 +11097,16 @@
       <c r="CH76">
         <v>28</v>
       </c>
+      <c r="CI76">
+        <v>28</v>
+      </c>
     </row>
-    <row r="78" spans="1:86">
+    <row r="78" spans="1:87">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:86">
+    <row r="79" spans="1:87">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -11148,8 +11293,11 @@
       <c r="CH79">
         <v>297</v>
       </c>
+      <c r="CI79">
+        <v>297</v>
+      </c>
     </row>
-    <row r="80" spans="1:86">
+    <row r="80" spans="1:87">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -11336,8 +11484,11 @@
       <c r="CH80">
         <v>124</v>
       </c>
+      <c r="CI80">
+        <v>109</v>
+      </c>
     </row>
-    <row r="81" spans="1:86">
+    <row r="81" spans="1:87">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -11524,8 +11675,11 @@
       <c r="CH81">
         <v>104</v>
       </c>
+      <c r="CI81">
+        <v>85</v>
+      </c>
     </row>
-    <row r="82" spans="1:86">
+    <row r="82" spans="1:87">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -11670,8 +11824,11 @@
       <c r="CH82">
         <v>16</v>
       </c>
+      <c r="CI82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:86">
+    <row r="84" spans="1:87">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -11858,8 +12015,11 @@
       <c r="CH84">
         <v>119</v>
       </c>
+      <c r="CI84">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:86">
+    <row r="85" spans="1:87">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -12046,8 +12206,11 @@
       <c r="CH85">
         <v>28</v>
       </c>
+      <c r="CI85">
+        <v>28</v>
+      </c>
     </row>
-    <row r="86" spans="1:86">
+    <row r="86" spans="1:87">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -12234,8 +12397,11 @@
       <c r="CH86">
         <v>147</v>
       </c>
+      <c r="CI86">
+        <v>147</v>
+      </c>
     </row>
-    <row r="87" spans="1:86">
+    <row r="87" spans="1:87">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -12422,8 +12588,11 @@
       <c r="CH87">
         <v>190</v>
       </c>
+      <c r="CI87">
+        <v>190</v>
+      </c>
     </row>
-    <row r="88" spans="1:86">
+    <row r="88" spans="1:87">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -12484,8 +12653,11 @@
       <c r="CH88">
         <v>1</v>
       </c>
+      <c r="CI88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:86">
+    <row r="90" spans="1:87">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -12672,8 +12844,11 @@
       <c r="CH90">
         <v>79</v>
       </c>
+      <c r="CI90">
+        <v>81</v>
+      </c>
     </row>
-    <row r="91" spans="1:86">
+    <row r="91" spans="1:87">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -12860,8 +13035,11 @@
       <c r="CH91">
         <v>21</v>
       </c>
+      <c r="CI91">
+        <v>22</v>
+      </c>
     </row>
-    <row r="92" spans="1:86">
+    <row r="92" spans="1:87">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -13036,8 +13214,11 @@
       <c r="CH92">
         <v>159</v>
       </c>
+      <c r="CI92">
+        <v>158</v>
+      </c>
     </row>
-    <row r="93" spans="1:86">
+    <row r="93" spans="1:87">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -13224,8 +13405,11 @@
       <c r="CH93">
         <v>41</v>
       </c>
+      <c r="CI93">
+        <v>41</v>
+      </c>
     </row>
-    <row r="94" spans="1:86">
+    <row r="94" spans="1:87">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -13370,377 +13554,342 @@
       <c r="CH94">
         <v>13</v>
       </c>
+      <c r="CI94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:86">
-      <c r="A95" s="2"/>
+    <row r="96" spans="1:87">
+      <c r="A96" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB96">
+        <v>112</v>
+      </c>
+      <c r="BC96">
+        <v>121</v>
+      </c>
+      <c r="BD96">
+        <v>130</v>
+      </c>
+      <c r="BE96">
+        <v>135</v>
+      </c>
+      <c r="BF96">
+        <v>137</v>
+      </c>
+      <c r="BG96">
+        <v>137</v>
+      </c>
+      <c r="BH96">
+        <v>137</v>
+      </c>
+      <c r="BI96">
+        <v>137</v>
+      </c>
+      <c r="BJ96">
+        <v>142</v>
+      </c>
+      <c r="BK96">
+        <v>144</v>
+      </c>
+      <c r="BL96">
+        <v>145</v>
+      </c>
+      <c r="BM96">
+        <v>147</v>
+      </c>
+      <c r="BN96">
+        <v>147</v>
+      </c>
+      <c r="BO96">
+        <v>150</v>
+      </c>
+      <c r="BP96">
+        <v>155</v>
+      </c>
+      <c r="BQ96">
+        <v>156</v>
+      </c>
+      <c r="BR96">
+        <v>158</v>
+      </c>
+      <c r="BS96">
+        <v>158</v>
+      </c>
+      <c r="BT96">
+        <v>168</v>
+      </c>
+      <c r="BU96">
+        <v>169</v>
+      </c>
+      <c r="BV96">
+        <v>169</v>
+      </c>
+      <c r="BW96">
+        <v>172</v>
+      </c>
+      <c r="BX96">
+        <v>175</v>
+      </c>
+      <c r="BY96">
+        <v>176</v>
+      </c>
+      <c r="BZ96">
+        <v>178</v>
+      </c>
+      <c r="CA96">
+        <v>178</v>
+      </c>
+      <c r="CB96">
+        <v>179</v>
+      </c>
+      <c r="CC96">
+        <v>179</v>
+      </c>
+      <c r="CD96">
+        <v>179</v>
+      </c>
+      <c r="CE96">
+        <v>182</v>
+      </c>
+      <c r="CF96">
+        <v>183</v>
+      </c>
+      <c r="CG96">
+        <v>185</v>
+      </c>
+      <c r="CH96">
+        <v>187</v>
+      </c>
+      <c r="CI96">
+        <v>187</v>
+      </c>
     </row>
-    <row r="96" spans="1:86">
-      <c r="A96" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="B96" s="42" t="s">
-        <v>164</v>
-      </c>
-      <c r="CG96">
-        <v>9</v>
+    <row r="97" spans="1:87">
+      <c r="A97" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB97">
+        <v>5</v>
+      </c>
+      <c r="BC97">
+        <v>8</v>
+      </c>
+      <c r="BD97">
+        <v>10</v>
+      </c>
+      <c r="BE97">
+        <v>11</v>
+      </c>
+      <c r="BF97">
+        <v>14</v>
+      </c>
+      <c r="BG97">
+        <v>15</v>
+      </c>
+      <c r="BH97">
+        <v>15</v>
+      </c>
+      <c r="BI97">
+        <v>18</v>
+      </c>
+      <c r="BJ97">
+        <v>19</v>
+      </c>
+      <c r="BK97">
+        <v>22</v>
+      </c>
+      <c r="BL97">
+        <v>22</v>
+      </c>
+      <c r="BM97">
+        <v>24</v>
+      </c>
+      <c r="BN97">
+        <v>24</v>
+      </c>
+      <c r="BO97">
+        <v>24</v>
+      </c>
+      <c r="BP97">
+        <v>24</v>
+      </c>
+      <c r="BQ97">
+        <v>27</v>
+      </c>
+      <c r="BR97">
+        <v>27</v>
+      </c>
+      <c r="BS97">
+        <v>38</v>
+      </c>
+      <c r="BT97">
+        <v>38</v>
+      </c>
+      <c r="BU97">
+        <v>40</v>
+      </c>
+      <c r="BV97">
+        <v>40</v>
+      </c>
+      <c r="BW97">
+        <v>40</v>
+      </c>
+      <c r="BX97">
+        <v>40</v>
+      </c>
+      <c r="BY97">
+        <v>40</v>
+      </c>
+      <c r="BZ97">
+        <v>41</v>
+      </c>
+      <c r="CA97">
+        <v>41</v>
+      </c>
+      <c r="CB97">
+        <v>41</v>
+      </c>
+      <c r="CC97">
+        <v>41</v>
+      </c>
+      <c r="CD97">
+        <v>41</v>
+      </c>
+      <c r="CE97">
+        <v>47</v>
+      </c>
+      <c r="CF97">
+        <v>49</v>
+      </c>
+      <c r="CG97">
+        <v>53</v>
+      </c>
+      <c r="CH97">
+        <v>60</v>
+      </c>
+      <c r="CI97">
+        <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:86">
-      <c r="A97" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="B97" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="CG97">
+    <row r="98" spans="1:87">
+      <c r="A98" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB98">
+        <v>16</v>
+      </c>
+      <c r="BC98">
+        <v>16</v>
+      </c>
+      <c r="BD98">
         <v>17</v>
       </c>
+      <c r="BE98">
+        <v>17</v>
+      </c>
+      <c r="BF98">
+        <v>18</v>
+      </c>
+      <c r="BG98">
+        <v>18</v>
+      </c>
+      <c r="BH98">
+        <v>19</v>
+      </c>
+      <c r="BI98">
+        <v>19</v>
+      </c>
+      <c r="BJ98">
+        <v>19</v>
+      </c>
+      <c r="BK98">
+        <v>19</v>
+      </c>
+      <c r="BL98">
+        <v>20</v>
+      </c>
+      <c r="BM98">
+        <v>20</v>
+      </c>
+      <c r="BN98">
+        <v>20</v>
+      </c>
+      <c r="BO98">
+        <v>20</v>
+      </c>
+      <c r="BP98">
+        <v>20</v>
+      </c>
+      <c r="BQ98">
+        <v>21</v>
+      </c>
+      <c r="BR98">
+        <v>22</v>
+      </c>
+      <c r="BS98">
+        <v>23</v>
+      </c>
+      <c r="BT98">
+        <v>24</v>
+      </c>
+      <c r="BU98">
+        <v>24</v>
+      </c>
+      <c r="BV98">
+        <v>24</v>
+      </c>
+      <c r="BW98">
+        <v>24</v>
+      </c>
+      <c r="BX98">
+        <v>25</v>
+      </c>
+      <c r="BY98">
+        <v>25</v>
+      </c>
+      <c r="BZ98">
+        <v>25</v>
+      </c>
+      <c r="CA98">
+        <v>25</v>
+      </c>
+      <c r="CB98">
+        <v>25</v>
+      </c>
+      <c r="CC98">
+        <v>25</v>
+      </c>
+      <c r="CD98">
+        <v>25</v>
+      </c>
+      <c r="CE98">
+        <v>25</v>
+      </c>
+      <c r="CF98">
+        <v>25</v>
+      </c>
+      <c r="CG98">
+        <v>25</v>
+      </c>
+      <c r="CH98">
+        <v>25</v>
+      </c>
+      <c r="CI98">
+        <v>25</v>
+      </c>
     </row>
-    <row r="98" spans="1:86">
-      <c r="A98" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="B98" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="CG98">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:86">
-      <c r="A99" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="B99" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="CG99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:86">
-      <c r="A101" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B101" t="s">
-        <v>76</v>
-      </c>
-      <c r="BB101">
-        <v>112</v>
-      </c>
-      <c r="BC101">
-        <v>121</v>
-      </c>
-      <c r="BD101">
-        <v>130</v>
-      </c>
-      <c r="BE101">
-        <v>135</v>
-      </c>
-      <c r="BF101">
-        <v>137</v>
-      </c>
-      <c r="BG101">
-        <v>137</v>
-      </c>
-      <c r="BH101">
-        <v>137</v>
-      </c>
-      <c r="BI101">
-        <v>137</v>
-      </c>
-      <c r="BJ101">
-        <v>142</v>
-      </c>
-      <c r="BK101">
-        <v>144</v>
-      </c>
-      <c r="BL101">
-        <v>145</v>
-      </c>
-      <c r="BM101">
-        <v>147</v>
-      </c>
-      <c r="BN101">
-        <v>147</v>
-      </c>
-      <c r="BO101">
-        <v>150</v>
-      </c>
-      <c r="BP101">
-        <v>155</v>
-      </c>
-      <c r="BQ101">
-        <v>156</v>
-      </c>
-      <c r="BR101">
-        <v>158</v>
-      </c>
-      <c r="BS101">
-        <v>158</v>
-      </c>
-      <c r="BT101">
-        <v>168</v>
-      </c>
-      <c r="BU101">
-        <v>169</v>
-      </c>
-      <c r="BV101">
-        <v>169</v>
-      </c>
-      <c r="BW101">
-        <v>172</v>
-      </c>
-      <c r="BX101">
-        <v>175</v>
-      </c>
-      <c r="BY101">
-        <v>176</v>
-      </c>
-      <c r="BZ101">
-        <v>178</v>
-      </c>
-      <c r="CA101">
-        <v>178</v>
-      </c>
-      <c r="CB101">
-        <v>179</v>
-      </c>
-      <c r="CC101">
-        <v>179</v>
-      </c>
-      <c r="CD101">
-        <v>179</v>
-      </c>
-      <c r="CE101">
-        <v>182</v>
-      </c>
-      <c r="CF101">
-        <v>183</v>
-      </c>
-      <c r="CG101">
-        <v>185</v>
-      </c>
-      <c r="CH101">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="102" spans="1:86">
-      <c r="A102" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B102" t="s">
-        <v>77</v>
-      </c>
-      <c r="BB102">
-        <v>5</v>
-      </c>
-      <c r="BC102">
-        <v>8</v>
-      </c>
-      <c r="BD102">
-        <v>10</v>
-      </c>
-      <c r="BE102">
-        <v>11</v>
-      </c>
-      <c r="BF102">
-        <v>14</v>
-      </c>
-      <c r="BG102">
-        <v>15</v>
-      </c>
-      <c r="BH102">
-        <v>15</v>
-      </c>
-      <c r="BI102">
-        <v>18</v>
-      </c>
-      <c r="BJ102">
-        <v>19</v>
-      </c>
-      <c r="BK102">
-        <v>22</v>
-      </c>
-      <c r="BL102">
-        <v>22</v>
-      </c>
-      <c r="BM102">
-        <v>24</v>
-      </c>
-      <c r="BN102">
-        <v>24</v>
-      </c>
-      <c r="BO102">
-        <v>24</v>
-      </c>
-      <c r="BP102">
-        <v>24</v>
-      </c>
-      <c r="BQ102">
-        <v>27</v>
-      </c>
-      <c r="BR102">
-        <v>27</v>
-      </c>
-      <c r="BS102">
-        <v>38</v>
-      </c>
-      <c r="BT102">
-        <v>38</v>
-      </c>
-      <c r="BU102">
-        <v>40</v>
-      </c>
-      <c r="BV102">
-        <v>40</v>
-      </c>
-      <c r="BW102">
-        <v>40</v>
-      </c>
-      <c r="BX102">
-        <v>40</v>
-      </c>
-      <c r="BY102">
-        <v>40</v>
-      </c>
-      <c r="BZ102">
-        <v>41</v>
-      </c>
-      <c r="CA102">
-        <v>41</v>
-      </c>
-      <c r="CB102">
-        <v>41</v>
-      </c>
-      <c r="CC102">
-        <v>41</v>
-      </c>
-      <c r="CD102">
-        <v>41</v>
-      </c>
-      <c r="CE102">
-        <v>47</v>
-      </c>
-      <c r="CF102">
-        <v>49</v>
-      </c>
-      <c r="CG102">
-        <v>53</v>
-      </c>
-      <c r="CH102">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="103" spans="1:86">
-      <c r="A103" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B103" t="s">
-        <v>78</v>
-      </c>
-      <c r="BB103">
-        <v>16</v>
-      </c>
-      <c r="BC103">
-        <v>16</v>
-      </c>
-      <c r="BD103">
-        <v>17</v>
-      </c>
-      <c r="BE103">
-        <v>17</v>
-      </c>
-      <c r="BF103">
-        <v>18</v>
-      </c>
-      <c r="BG103">
-        <v>18</v>
-      </c>
-      <c r="BH103">
-        <v>19</v>
-      </c>
-      <c r="BI103">
-        <v>19</v>
-      </c>
-      <c r="BJ103">
-        <v>19</v>
-      </c>
-      <c r="BK103">
-        <v>19</v>
-      </c>
-      <c r="BL103">
-        <v>20</v>
-      </c>
-      <c r="BM103">
-        <v>20</v>
-      </c>
-      <c r="BN103">
-        <v>20</v>
-      </c>
-      <c r="BO103">
-        <v>20</v>
-      </c>
-      <c r="BP103">
-        <v>20</v>
-      </c>
-      <c r="BQ103">
-        <v>21</v>
-      </c>
-      <c r="BR103">
-        <v>22</v>
-      </c>
-      <c r="BS103">
-        <v>23</v>
-      </c>
-      <c r="BT103">
-        <v>24</v>
-      </c>
-      <c r="BU103">
-        <v>24</v>
-      </c>
-      <c r="BV103">
-        <v>24</v>
-      </c>
-      <c r="BW103">
-        <v>24</v>
-      </c>
-      <c r="BX103">
-        <v>25</v>
-      </c>
-      <c r="BY103">
-        <v>25</v>
-      </c>
-      <c r="BZ103">
-        <v>25</v>
-      </c>
-      <c r="CA103">
-        <v>25</v>
-      </c>
-      <c r="CB103">
-        <v>25</v>
-      </c>
-      <c r="CC103">
-        <v>25</v>
-      </c>
-      <c r="CD103">
-        <v>25</v>
-      </c>
-      <c r="CE103">
-        <v>25</v>
-      </c>
-      <c r="CF103">
-        <v>25</v>
-      </c>
-      <c r="CG103">
-        <v>25</v>
-      </c>
-      <c r="CH103">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="118" spans="52:52">
-      <c r="AZ118">
+    <row r="113" spans="52:52">
+      <c r="AZ113">
         <v>9</v>
       </c>
     </row>
@@ -13752,10 +13901,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BI11"/>
+  <dimension ref="A2:BJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BI3" sqref="BI3:BI11"/>
+    <sheetView tabSelected="1" topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BJ11" sqref="BJ3:BJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13765,7 +13914,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:61" s="2" customFormat="1">
+    <row r="2" spans="1:62" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -13949,8 +14098,11 @@
       <c r="BI2" s="9">
         <v>43980</v>
       </c>
+      <c r="BJ2" s="9">
+        <v>43981</v>
+      </c>
     </row>
-    <row r="3" spans="1:61">
+    <row r="3" spans="1:62">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -14134,8 +14286,11 @@
       <c r="BI3">
         <v>1221</v>
       </c>
+      <c r="BJ3">
+        <v>1229</v>
+      </c>
     </row>
-    <row r="4" spans="1:61">
+    <row r="4" spans="1:62">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -14319,8 +14474,11 @@
       <c r="BI4">
         <v>507</v>
       </c>
+      <c r="BJ4">
+        <v>498</v>
+      </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:62">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -14504,8 +14662,11 @@
       <c r="BI5">
         <v>400</v>
       </c>
+      <c r="BJ5">
+        <v>417</v>
+      </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:62">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -14689,8 +14850,11 @@
       <c r="BI6">
         <v>1828</v>
       </c>
+      <c r="BJ6">
+        <v>1840</v>
+      </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:62">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -14874,8 +15038,11 @@
       <c r="BI7">
         <v>1351</v>
       </c>
+      <c r="BJ7">
+        <v>1364</v>
+      </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:62">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -15059,8 +15226,11 @@
       <c r="BI8">
         <v>750</v>
       </c>
+      <c r="BJ8">
+        <v>755</v>
+      </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:62">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -15244,8 +15414,11 @@
       <c r="BI9">
         <v>1269</v>
       </c>
+      <c r="BJ9">
+        <v>1285</v>
+      </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:62">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -15429,8 +15602,11 @@
       <c r="BI10">
         <v>1242</v>
       </c>
+      <c r="BJ10">
+        <v>1259</v>
+      </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:62">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -15613,6 +15789,9 @@
       </c>
       <c r="BI11">
         <v>149</v>
+      </c>
+      <c r="BJ11">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -15623,10 +15802,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BD17"/>
+  <dimension ref="A2:BE17"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BD14" sqref="BD14:BD17"/>
+    <sheetView topLeftCell="AO8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BE17" sqref="BE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15636,7 +15815,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:56" s="2" customFormat="1">
+    <row r="2" spans="1:57" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -15803,8 +15982,11 @@
       <c r="BD2" s="9">
         <v>43980</v>
       </c>
+      <c r="BE2" s="9">
+        <v>43981</v>
+      </c>
     </row>
-    <row r="3" spans="1:56" s="2" customFormat="1">
+    <row r="3" spans="1:57" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -15812,7 +15994,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:56">
+    <row r="4" spans="1:57">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -15981,8 +16163,11 @@
       <c r="BD4">
         <v>8717</v>
       </c>
+      <c r="BE4">
+        <v>8801</v>
+      </c>
     </row>
-    <row r="5" spans="1:56">
+    <row r="5" spans="1:57">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -16151,8 +16336,11 @@
       <c r="BD5">
         <v>939</v>
       </c>
+      <c r="BE5">
+        <v>914</v>
+      </c>
     </row>
-    <row r="6" spans="1:56">
+    <row r="6" spans="1:57">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -16321,8 +16509,11 @@
       <c r="BD6">
         <v>1342</v>
       </c>
+      <c r="BE6">
+        <v>1346</v>
+      </c>
     </row>
-    <row r="7" spans="1:56">
+    <row r="7" spans="1:57">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -16491,8 +16682,11 @@
       <c r="BD7">
         <v>4055</v>
       </c>
+      <c r="BE7">
+        <v>4097</v>
+      </c>
     </row>
-    <row r="8" spans="1:56">
+    <row r="8" spans="1:57">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -16661,8 +16855,11 @@
       <c r="BD8">
         <v>106</v>
       </c>
+      <c r="BE8">
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:56" ht="30">
+    <row r="9" spans="1:57" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -16831,8 +17028,11 @@
       <c r="BD9">
         <v>26</v>
       </c>
+      <c r="BE9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:56" ht="30">
+    <row r="10" spans="1:57" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -16997,8 +17197,11 @@
       <c r="BD10">
         <v>22</v>
       </c>
+      <c r="BE10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:56">
+    <row r="11" spans="1:57">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -17167,8 +17370,11 @@
       <c r="BD11">
         <v>2169</v>
       </c>
+      <c r="BE11">
+        <v>2232</v>
+      </c>
     </row>
-    <row r="12" spans="1:56" ht="30">
+    <row r="12" spans="1:57" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -17337,8 +17543,11 @@
       <c r="BD12">
         <v>58</v>
       </c>
+      <c r="BE12">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:56">
+    <row r="13" spans="1:57">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -17349,7 +17558,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:56">
+    <row r="14" spans="1:57">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -17518,8 +17727,11 @@
       <c r="BD14">
         <v>1500</v>
       </c>
+      <c r="BE14">
+        <v>1521</v>
+      </c>
     </row>
-    <row r="15" spans="1:56">
+    <row r="15" spans="1:57">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -17688,8 +17900,11 @@
       <c r="BD15">
         <v>2309</v>
       </c>
+      <c r="BE15">
+        <v>2328</v>
+      </c>
     </row>
-    <row r="16" spans="1:56">
+    <row r="16" spans="1:57">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -17858,8 +18073,11 @@
       <c r="BD16">
         <v>4883</v>
       </c>
+      <c r="BE16">
+        <v>4927</v>
+      </c>
     </row>
-    <row r="17" spans="1:56" ht="30">
+    <row r="17" spans="1:57" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -18026,6 +18244,9 @@
         <v>25</v>
       </c>
       <c r="BD17">
+        <v>25</v>
+      </c>
+      <c r="BE17">
         <v>25</v>
       </c>
     </row>
@@ -18037,10 +18258,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BD9"/>
+  <dimension ref="A1:BE9"/>
   <sheetViews>
     <sheetView topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BG11" sqref="BG11"/>
+      <selection activeCell="BE8" sqref="BE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18049,7 +18270,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="2" customFormat="1">
+    <row r="1" spans="1:57" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -18215,14 +18436,17 @@
       <c r="BD1" s="9">
         <v>43980</v>
       </c>
+      <c r="BE1" s="9">
+        <v>43981</v>
+      </c>
     </row>
-    <row r="2" spans="1:56">
+    <row r="2" spans="1:57">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:56">
+    <row r="3" spans="1:57">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -18392,8 +18616,11 @@
       <c r="BD3">
         <v>462</v>
       </c>
+      <c r="BE3">
+        <v>466</v>
+      </c>
     </row>
-    <row r="4" spans="1:56">
+    <row r="4" spans="1:57">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -18562,8 +18789,11 @@
       <c r="BD4">
         <v>7</v>
       </c>
+      <c r="BE4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:56" ht="30">
+    <row r="5" spans="1:57" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -18732,8 +18962,11 @@
       <c r="BD5">
         <v>346</v>
       </c>
+      <c r="BE5">
+        <v>349</v>
+      </c>
     </row>
-    <row r="6" spans="1:56">
+    <row r="6" spans="1:57">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -18902,8 +19135,11 @@
       <c r="BD6">
         <v>52</v>
       </c>
+      <c r="BE6">
+        <v>54</v>
+      </c>
     </row>
-    <row r="7" spans="1:56" ht="30">
+    <row r="7" spans="1:57" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -19072,8 +19308,11 @@
       <c r="BD7">
         <v>53</v>
       </c>
+      <c r="BE7">
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="1:56">
+    <row r="8" spans="1:57">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -19242,8 +19481,11 @@
       <c r="BD8">
         <v>3</v>
       </c>
+      <c r="BE8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:56">
+    <row r="9" spans="1:57">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -19264,10 +19506,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AP13"/>
+  <dimension ref="A2:AQ13"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3:AP13"/>
+    <sheetView topLeftCell="AD5" workbookViewId="0">
+      <selection activeCell="AQ14" sqref="AQ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19275,7 +19517,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:42" s="2" customFormat="1">
+    <row r="2" spans="1:43" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -19402,8 +19644,11 @@
       <c r="AP2" s="9">
         <v>43980</v>
       </c>
+      <c r="AQ2" s="9">
+        <v>43981</v>
+      </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:43">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -19530,8 +19775,11 @@
       <c r="AP3">
         <v>462</v>
       </c>
+      <c r="AQ3">
+        <v>466</v>
+      </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:43">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -19658,8 +19906,11 @@
       <c r="AP4">
         <v>47</v>
       </c>
+      <c r="AQ4">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:43">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -19786,8 +20037,11 @@
       <c r="AP5">
         <v>29</v>
       </c>
+      <c r="AQ5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:43">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -19914,8 +20168,11 @@
       <c r="AP6">
         <v>30</v>
       </c>
+      <c r="AQ6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:43">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -20042,8 +20299,11 @@
       <c r="AP7">
         <v>65</v>
       </c>
+      <c r="AQ7">
+        <v>66</v>
+      </c>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:43">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -20170,8 +20430,11 @@
       <c r="AP8">
         <v>73</v>
       </c>
+      <c r="AQ8">
+        <v>74</v>
+      </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:43">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -20298,8 +20561,11 @@
       <c r="AP9">
         <v>42</v>
       </c>
+      <c r="AQ9">
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:43">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -20426,8 +20692,11 @@
       <c r="AP10">
         <v>66</v>
       </c>
+      <c r="AQ10">
+        <v>66</v>
+      </c>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:43">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -20554,8 +20823,11 @@
       <c r="AP11">
         <v>94</v>
       </c>
+      <c r="AQ11">
+        <v>95</v>
+      </c>
     </row>
-    <row r="12" spans="1:42" ht="30">
+    <row r="12" spans="1:43" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -20682,8 +20954,11 @@
       <c r="AP12">
         <v>16</v>
       </c>
+      <c r="AQ12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:43">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -20808,6 +21083,9 @@
         <v>0</v>
       </c>
       <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
         <v>0</v>
       </c>
     </row>
@@ -20821,8 +21099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="82" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20831,51 +21109,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="C1" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
+      <c r="C1" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
     </row>
     <row r="4" spans="1:15">
       <c r="C4" s="34"/>
@@ -20923,6 +21201,9 @@
       <c r="L5" s="9">
         <v>43980</v>
       </c>
+      <c r="M5" s="9">
+        <v>43981</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
@@ -20958,6 +21239,9 @@
       <c r="L6">
         <v>113</v>
       </c>
+      <c r="M6">
+        <v>119</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
@@ -20993,13 +21277,16 @@
       <c r="L7">
         <v>30</v>
       </c>
+      <c r="M7">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -21036,6 +21323,9 @@
       <c r="L9">
         <v>1</v>
       </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="31" t="s">
@@ -21071,6 +21361,9 @@
       <c r="L10">
         <v>21</v>
       </c>
+      <c r="M10">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="31" t="s">
@@ -21106,6 +21399,9 @@
       <c r="L11">
         <v>6</v>
       </c>
+      <c r="M11">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="31" t="s">
@@ -21141,6 +21437,9 @@
       <c r="L12">
         <v>2</v>
       </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="36" t="s">
@@ -21181,6 +21480,9 @@
       <c r="L14">
         <v>1</v>
       </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="31">
@@ -21216,6 +21518,9 @@
       <c r="L15">
         <v>0</v>
       </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="31">
@@ -21251,8 +21556,11 @@
       <c r="L16">
         <v>2</v>
       </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -21286,8 +21594,11 @@
       <c r="L17">
         <v>9</v>
       </c>
+      <c r="M17">
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -21321,8 +21632,11 @@
       <c r="L18">
         <v>2</v>
       </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:13">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -21356,8 +21670,11 @@
       <c r="L19">
         <v>2</v>
       </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:13">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -21391,8 +21708,11 @@
       <c r="L20">
         <v>3</v>
       </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -21426,8 +21746,11 @@
       <c r="L21">
         <v>6</v>
       </c>
+      <c r="M21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:12" ht="45">
+    <row r="22" spans="1:13" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -21461,8 +21784,11 @@
       <c r="L22">
         <v>4</v>
       </c>
+      <c r="M22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:12" ht="30">
+    <row r="23" spans="1:13" ht="30">
       <c r="A23" s="39" t="s">
         <v>139</v>
       </c>
@@ -21494,6 +21820,9 @@
         <v>1</v>
       </c>
       <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
         <v>1</v>
       </c>
     </row>
@@ -21525,18 +21854,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A1" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="A1" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:7" ht="36.6" customHeight="1">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="44" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -21545,7 +21874,7 @@
       <c r="C2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="45" t="s">
         <v>124</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -21559,10 +21888,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1">
-      <c r="A3" s="47"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="48"/>
+      <c r="D3" s="45"/>
       <c r="E3" s="25" t="s">
         <v>92</v>
       </c>
@@ -21574,10 +21903,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1">
-      <c r="A4" s="47"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="48"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="25" t="s">
         <v>86</v>
       </c>
@@ -21587,10 +21916,10 @@
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1">
-      <c r="A5" s="47"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="48"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="25" t="s">
         <v>87</v>
       </c>
@@ -21598,10 +21927,10 @@
       <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1">
-      <c r="A6" s="47"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="48"/>
+      <c r="D6" s="45"/>
       <c r="E6" s="25" t="s">
         <v>88</v>
       </c>
@@ -21609,10 +21938,10 @@
       <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1">
-      <c r="A7" s="47"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="48"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="25" t="s">
         <v>93</v>
       </c>
@@ -21647,7 +21976,7 @@
         <v>96</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C9" s="28">
         <v>3</v>
@@ -21693,7 +22022,7 @@
         <v>99</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C11" s="28">
         <v>17</v>
@@ -21794,7 +22123,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F15" s="28">
         <v>1</v>
@@ -21854,7 +22183,7 @@
         <v>109</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" s="28">
         <v>12</v>
@@ -21946,7 +22275,7 @@
         <v>115</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C22" s="28">
         <v>25</v>
@@ -21992,7 +22321,7 @@
         <v>118</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C24" s="28">
         <v>8</v>
@@ -22018,7 +22347,7 @@
         <v>129</v>
       </c>
       <c r="C25" s="28">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D25" s="28">
         <v>0</v>
@@ -22038,16 +22367,16 @@
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="28">
         <v>159</v>
       </c>
-      <c r="C26" s="28">
-        <v>157</v>
-      </c>
       <c r="D26" s="28">
         <v>0</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F26" s="28">
         <v>5</v>
@@ -22090,21 +22419,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -22307,32 +22627,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22349,4 +22670,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
01 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E24960D-C329-404F-9ECE-927FDE7D02C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="851" documentId="8_{C5E88C75-E440-43B4-B034-AA36176F93AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2D087BDD-E593-48F0-8D01-32BDC4B573F7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -515,9 +513,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>As of May 30, 2020</t>
-  </si>
-  <si>
     <t>152; (46)</t>
   </si>
   <si>
@@ -527,8 +522,11 @@
     <t>857; (370)</t>
   </si>
   <si>
+    <t>As of May 31, 2020</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">As of May 30, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of May 31, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -1168,26 +1166,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CI113"/>
+  <dimension ref="A1:CJ113"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="BY1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CI1" sqref="CI1:CI1048576"/>
+      <selection pane="topRight" activeCell="CJ87" sqref="CJ1:CJ1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="87" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87">
+    <row r="1" spans="1:88">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1443,8 +1441,11 @@
       <c r="CI1" s="1">
         <v>43981</v>
       </c>
+      <c r="CJ1" s="1">
+        <v>43982</v>
+      </c>
     </row>
-    <row r="2" spans="1:87">
+    <row r="2" spans="1:88">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1468,7 +1469,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:87">
+    <row r="3" spans="1:88">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1709,8 +1710,11 @@
       <c r="CI3">
         <v>46483</v>
       </c>
+      <c r="CJ3">
+        <v>47263</v>
+      </c>
     </row>
-    <row r="4" spans="1:87">
+    <row r="4" spans="1:88">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1746,8 +1750,11 @@
       <c r="CI4">
         <v>38413</v>
       </c>
+      <c r="CJ4">
+        <v>38975</v>
+      </c>
     </row>
-    <row r="5" spans="1:87">
+    <row r="5" spans="1:88">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2009,8 +2016,11 @@
       <c r="CI5">
         <v>8801</v>
       </c>
+      <c r="CJ5">
+        <v>8857</v>
+      </c>
     </row>
-    <row r="6" spans="1:87">
+    <row r="6" spans="1:88">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2254,8 +2264,11 @@
       <c r="CI6">
         <v>466</v>
       </c>
+      <c r="CJ6">
+        <v>468</v>
+      </c>
     </row>
-    <row r="7" spans="1:87">
+    <row r="7" spans="1:88">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2469,11 +2482,14 @@
       <c r="CI7">
         <v>1116</v>
       </c>
+      <c r="CJ7">
+        <v>1126</v>
+      </c>
     </row>
-    <row r="8" spans="1:87">
+    <row r="8" spans="1:88">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:87">
+    <row r="9" spans="1:88">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2579,8 +2595,11 @@
       <c r="CI9">
         <v>345</v>
       </c>
+      <c r="CJ9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:87">
+    <row r="10" spans="1:88">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2788,8 +2807,11 @@
       <c r="CI10">
         <v>59</v>
       </c>
+      <c r="CJ10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="11" spans="1:87">
+    <row r="11" spans="1:88">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2997,8 +3019,11 @@
       <c r="CI11">
         <v>440</v>
       </c>
+      <c r="CJ11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:87">
+    <row r="12" spans="1:88">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3206,8 +3231,11 @@
       <c r="CI12">
         <v>215</v>
       </c>
+      <c r="CJ12">
+        <v>204</v>
+      </c>
     </row>
-    <row r="13" spans="1:87">
+    <row r="13" spans="1:88">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3415,8 +3443,11 @@
       <c r="CI13">
         <v>225</v>
       </c>
+      <c r="CJ13">
+        <v>236</v>
+      </c>
     </row>
-    <row r="14" spans="1:87">
+    <row r="14" spans="1:88">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3486,8 +3517,11 @@
       <c r="CI14">
         <v>295</v>
       </c>
+      <c r="CJ14">
+        <v>302</v>
+      </c>
     </row>
-    <row r="15" spans="1:87">
+    <row r="15" spans="1:88">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3527,8 +3561,11 @@
       <c r="CI15">
         <v>109</v>
       </c>
+      <c r="CJ15">
+        <v>108</v>
+      </c>
     </row>
-    <row r="16" spans="1:87">
+    <row r="16" spans="1:88">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3598,8 +3635,11 @@
       <c r="CI16">
         <v>1931</v>
       </c>
+      <c r="CJ16">
+        <v>1891</v>
+      </c>
     </row>
-    <row r="17" spans="1:87">
+    <row r="17" spans="1:88">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3669,13 +3709,16 @@
       <c r="CI17" s="23">
         <v>0.78</v>
       </c>
+      <c r="CJ17" s="23">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="19" spans="1:87">
+    <row r="19" spans="1:88">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:87">
+    <row r="20" spans="1:88">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3683,7 +3726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:87">
+    <row r="21" spans="1:88">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3894,8 +3937,11 @@
       <c r="CI21">
         <v>111</v>
       </c>
+      <c r="CJ21">
+        <v>111</v>
+      </c>
     </row>
-    <row r="22" spans="1:87">
+    <row r="22" spans="1:88">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4052,8 +4098,11 @@
       <c r="CI22">
         <v>19</v>
       </c>
+      <c r="CJ22">
+        <v>19</v>
+      </c>
     </row>
-    <row r="23" spans="1:87">
+    <row r="23" spans="1:88">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4210,8 +4259,11 @@
       <c r="CI23">
         <v>92</v>
       </c>
+      <c r="CJ23">
+        <v>92</v>
+      </c>
     </row>
-    <row r="24" spans="1:87">
+    <row r="24" spans="1:88">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4413,8 +4465,11 @@
       <c r="CI24">
         <v>123</v>
       </c>
+      <c r="CJ24">
+        <v>129</v>
+      </c>
     </row>
-    <row r="25" spans="1:87">
+    <row r="25" spans="1:88">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4616,8 +4671,11 @@
       <c r="CI25">
         <v>142</v>
       </c>
+      <c r="CJ25">
+        <v>148</v>
+      </c>
     </row>
-    <row r="26" spans="1:87">
+    <row r="26" spans="1:88">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4819,13 +4877,16 @@
       <c r="CI26">
         <v>1371</v>
       </c>
+      <c r="CJ26">
+        <v>1384</v>
+      </c>
     </row>
-    <row r="28" spans="1:87">
+    <row r="28" spans="1:88">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:87">
+    <row r="29" spans="1:88">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5036,8 +5097,11 @@
       <c r="CI29">
         <v>134</v>
       </c>
+      <c r="CJ29">
+        <v>135</v>
+      </c>
     </row>
-    <row r="30" spans="1:87">
+    <row r="30" spans="1:88">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5194,8 +5258,11 @@
       <c r="CI30">
         <v>28</v>
       </c>
+      <c r="CJ30">
+        <v>29</v>
+      </c>
     </row>
-    <row r="31" spans="1:87">
+    <row r="31" spans="1:88">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5352,8 +5419,11 @@
       <c r="CI31">
         <v>106</v>
       </c>
+      <c r="CJ31">
+        <v>106</v>
+      </c>
     </row>
-    <row r="32" spans="1:87">
+    <row r="32" spans="1:88">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5555,8 +5625,11 @@
       <c r="CI32">
         <v>48</v>
       </c>
+      <c r="CJ32">
+        <v>48</v>
+      </c>
     </row>
-    <row r="33" spans="1:87">
+    <row r="33" spans="1:88">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5758,8 +5831,11 @@
       <c r="CI33">
         <v>76</v>
       </c>
+      <c r="CJ33">
+        <v>77</v>
+      </c>
     </row>
-    <row r="34" spans="1:87">
+    <row r="34" spans="1:88">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -5961,13 +6037,16 @@
       <c r="CI34">
         <v>1206</v>
       </c>
+      <c r="CJ34">
+        <v>1206</v>
+      </c>
     </row>
-    <row r="36" spans="1:87">
+    <row r="36" spans="1:88">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:87">
+    <row r="37" spans="1:88">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -6166,8 +6245,11 @@
       <c r="CI37">
         <v>80</v>
       </c>
+      <c r="CJ37">
+        <v>80</v>
+      </c>
     </row>
-    <row r="38" spans="1:87">
+    <row r="38" spans="1:88">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6318,8 +6400,11 @@
       <c r="CI38">
         <v>6</v>
       </c>
+      <c r="CJ38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:87">
+    <row r="39" spans="1:88">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6470,8 +6555,11 @@
       <c r="CI39">
         <v>73</v>
       </c>
+      <c r="CJ39">
+        <v>73</v>
+      </c>
     </row>
-    <row r="40" spans="1:87">
+    <row r="40" spans="1:88">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6667,8 +6755,11 @@
       <c r="CI40">
         <v>1</v>
       </c>
+      <c r="CJ40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:87">
+    <row r="41" spans="1:88">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6861,8 +6952,11 @@
       <c r="CI41">
         <v>7</v>
       </c>
+      <c r="CJ41">
+        <v>7</v>
+      </c>
     </row>
-    <row r="42" spans="1:87">
+    <row r="42" spans="1:88">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7061,8 +7155,11 @@
       <c r="CI42">
         <v>281</v>
       </c>
+      <c r="CJ42">
+        <v>281</v>
+      </c>
     </row>
-    <row r="43" spans="1:87">
+    <row r="43" spans="1:88">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -7195,16 +7292,19 @@
       <c r="CI43">
         <v>1</v>
       </c>
+      <c r="CJ43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:87">
+    <row r="44" spans="1:88">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:87">
+    <row r="45" spans="1:88">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:87">
+    <row r="46" spans="1:88">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -7409,8 +7509,11 @@
       <c r="CI46">
         <v>205</v>
       </c>
+      <c r="CJ46">
+        <v>205</v>
+      </c>
     </row>
-    <row r="47" spans="1:87">
+    <row r="47" spans="1:88">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7567,8 +7670,11 @@
       <c r="CI47">
         <v>24</v>
       </c>
+      <c r="CJ47">
+        <v>18</v>
+      </c>
     </row>
-    <row r="48" spans="1:87">
+    <row r="48" spans="1:88">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7725,8 +7831,11 @@
       <c r="CI48">
         <v>175</v>
       </c>
+      <c r="CJ48">
+        <v>181</v>
+      </c>
     </row>
-    <row r="49" spans="1:87">
+    <row r="49" spans="1:88">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -7928,8 +8037,11 @@
       <c r="CI49">
         <v>470</v>
       </c>
+      <c r="CJ49">
+        <v>479</v>
+      </c>
     </row>
-    <row r="50" spans="1:87">
+    <row r="50" spans="1:88">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -8086,8 +8198,11 @@
       <c r="CI50">
         <v>494</v>
       </c>
+      <c r="CJ50">
+        <v>497</v>
+      </c>
     </row>
-    <row r="51" spans="1:87">
+    <row r="51" spans="1:88">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -8241,8 +8356,11 @@
       <c r="CI51">
         <v>815</v>
       </c>
+      <c r="CJ51">
+        <v>820</v>
+      </c>
     </row>
-    <row r="52" spans="1:87">
+    <row r="52" spans="1:88">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -8390,16 +8508,19 @@
       <c r="CI52">
         <v>1</v>
       </c>
+      <c r="CJ52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:87">
+    <row r="53" spans="1:88">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:87">
+    <row r="54" spans="1:88">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:87">
+    <row r="55" spans="1:88">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -8589,8 +8710,11 @@
       <c r="CI55">
         <v>29</v>
       </c>
+      <c r="CJ55">
+        <v>29</v>
+      </c>
     </row>
-    <row r="56" spans="1:87">
+    <row r="56" spans="1:88">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -8744,8 +8868,11 @@
       <c r="CI56">
         <v>7</v>
       </c>
+      <c r="CJ56">
+        <v>7</v>
+      </c>
     </row>
-    <row r="57" spans="1:87">
+    <row r="57" spans="1:88">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -8899,8 +9026,11 @@
       <c r="CI57">
         <v>21</v>
       </c>
+      <c r="CJ57">
+        <v>21</v>
+      </c>
     </row>
-    <row r="58" spans="1:87">
+    <row r="58" spans="1:88">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -9090,8 +9220,11 @@
       <c r="CI58">
         <v>18</v>
       </c>
+      <c r="CJ58">
+        <v>18</v>
+      </c>
     </row>
-    <row r="59" spans="1:87">
+    <row r="59" spans="1:88">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -9281,8 +9414,11 @@
       <c r="CI59">
         <v>25</v>
       </c>
+      <c r="CJ59">
+        <v>25</v>
+      </c>
     </row>
-    <row r="60" spans="1:87">
+    <row r="60" spans="1:88">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -9472,8 +9608,11 @@
       <c r="CI60">
         <v>142</v>
       </c>
+      <c r="CJ60">
+        <v>142</v>
+      </c>
     </row>
-    <row r="61" spans="1:87">
+    <row r="61" spans="1:88">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -9621,8 +9760,11 @@
       <c r="CI61">
         <v>1</v>
       </c>
+      <c r="CJ61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:87">
+    <row r="63" spans="1:88">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -9812,8 +9954,11 @@
       <c r="CI63">
         <v>11</v>
       </c>
+      <c r="CJ63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:87">
+    <row r="64" spans="1:88">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -9967,8 +10112,11 @@
       <c r="CI64">
         <v>3</v>
       </c>
+      <c r="CJ64">
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:87">
+    <row r="65" spans="1:88">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -10122,8 +10270,11 @@
       <c r="CI65">
         <v>8</v>
       </c>
+      <c r="CJ65">
+        <v>9</v>
+      </c>
     </row>
-    <row r="66" spans="1:87">
+    <row r="66" spans="1:88">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -10313,8 +10464,11 @@
       <c r="CI66">
         <v>48</v>
       </c>
+      <c r="CJ66">
+        <v>52</v>
+      </c>
     </row>
-    <row r="67" spans="1:87">
+    <row r="67" spans="1:88">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -10505,8 +10659,11 @@
       <c r="CI67">
         <v>51</v>
       </c>
+      <c r="CJ67">
+        <v>54</v>
+      </c>
     </row>
-    <row r="68" spans="1:87">
+    <row r="68" spans="1:88">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -10696,8 +10853,11 @@
       <c r="CI68">
         <v>0</v>
       </c>
+      <c r="CJ68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:87">
+    <row r="69" spans="1:88">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -10851,11 +11011,14 @@
       <c r="CI69">
         <v>0</v>
       </c>
+      <c r="CJ69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:87">
+    <row r="70" spans="1:88">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:87">
+    <row r="71" spans="1:88">
       <c r="A71" s="2" t="s">
         <v>132</v>
       </c>
@@ -10895,8 +11058,11 @@
       <c r="CI71">
         <v>10</v>
       </c>
+      <c r="CJ71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:87">
+    <row r="72" spans="1:88">
       <c r="A72" s="2" t="s">
         <v>132</v>
       </c>
@@ -10936,8 +11102,11 @@
       <c r="CI72">
         <v>6</v>
       </c>
+      <c r="CJ72">
+        <v>6</v>
+      </c>
     </row>
-    <row r="73" spans="1:87">
+    <row r="73" spans="1:88">
       <c r="A73" s="2" t="s">
         <v>132</v>
       </c>
@@ -10977,8 +11146,11 @@
       <c r="CI73">
         <v>4</v>
       </c>
+      <c r="CJ73">
+        <v>4</v>
+      </c>
     </row>
-    <row r="74" spans="1:87">
+    <row r="74" spans="1:88">
       <c r="A74" s="2" t="s">
         <v>132</v>
       </c>
@@ -11018,8 +11190,11 @@
       <c r="CI74">
         <v>13</v>
       </c>
+      <c r="CJ74">
+        <v>12</v>
+      </c>
     </row>
-    <row r="75" spans="1:87">
+    <row r="75" spans="1:88">
       <c r="A75" s="2" t="s">
         <v>132</v>
       </c>
@@ -11059,8 +11234,11 @@
       <c r="CI75">
         <v>19</v>
       </c>
+      <c r="CJ75">
+        <v>18</v>
+      </c>
     </row>
-    <row r="76" spans="1:87">
+    <row r="76" spans="1:88">
       <c r="A76" s="2" t="s">
         <v>132</v>
       </c>
@@ -11100,13 +11278,16 @@
       <c r="CI76">
         <v>28</v>
       </c>
+      <c r="CJ76">
+        <v>29</v>
+      </c>
     </row>
-    <row r="78" spans="1:87">
+    <row r="78" spans="1:88">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:87">
+    <row r="79" spans="1:88">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -11296,8 +11477,11 @@
       <c r="CI79">
         <v>297</v>
       </c>
+      <c r="CJ79">
+        <v>297</v>
+      </c>
     </row>
-    <row r="80" spans="1:87">
+    <row r="80" spans="1:88">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -11487,8 +11671,11 @@
       <c r="CI80">
         <v>109</v>
       </c>
+      <c r="CJ80">
+        <v>114</v>
+      </c>
     </row>
-    <row r="81" spans="1:87">
+    <row r="81" spans="1:88">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -11678,8 +11865,11 @@
       <c r="CI81">
         <v>85</v>
       </c>
+      <c r="CJ81">
+        <v>93</v>
+      </c>
     </row>
-    <row r="82" spans="1:87">
+    <row r="82" spans="1:88">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -11827,8 +12017,11 @@
       <c r="CI82">
         <v>16</v>
       </c>
+      <c r="CJ82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:87">
+    <row r="84" spans="1:88">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -12018,8 +12211,11 @@
       <c r="CI84">
         <v>119</v>
       </c>
+      <c r="CJ84">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:87">
+    <row r="85" spans="1:88">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -12209,8 +12405,11 @@
       <c r="CI85">
         <v>28</v>
       </c>
+      <c r="CJ85">
+        <v>28</v>
+      </c>
     </row>
-    <row r="86" spans="1:87">
+    <row r="86" spans="1:88">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -12400,8 +12599,11 @@
       <c r="CI86">
         <v>147</v>
       </c>
+      <c r="CJ86">
+        <v>147</v>
+      </c>
     </row>
-    <row r="87" spans="1:87">
+    <row r="87" spans="1:88">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -12591,8 +12793,11 @@
       <c r="CI87">
         <v>190</v>
       </c>
+      <c r="CJ87">
+        <v>190</v>
+      </c>
     </row>
-    <row r="88" spans="1:87">
+    <row r="88" spans="1:88">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -12656,8 +12861,11 @@
       <c r="CI88">
         <v>1</v>
       </c>
+      <c r="CJ88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:87">
+    <row r="90" spans="1:88">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -12847,8 +13055,11 @@
       <c r="CI90">
         <v>81</v>
       </c>
+      <c r="CJ90">
+        <v>81</v>
+      </c>
     </row>
-    <row r="91" spans="1:87">
+    <row r="91" spans="1:88">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -13038,8 +13249,11 @@
       <c r="CI91">
         <v>22</v>
       </c>
+      <c r="CJ91">
+        <v>22</v>
+      </c>
     </row>
-    <row r="92" spans="1:87">
+    <row r="92" spans="1:88">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -13217,8 +13431,11 @@
       <c r="CI92">
         <v>158</v>
       </c>
+      <c r="CJ92">
+        <v>158</v>
+      </c>
     </row>
-    <row r="93" spans="1:87">
+    <row r="93" spans="1:88">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -13408,8 +13625,11 @@
       <c r="CI93">
         <v>41</v>
       </c>
+      <c r="CJ93">
+        <v>41</v>
+      </c>
     </row>
-    <row r="94" spans="1:87">
+    <row r="94" spans="1:88">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -13557,8 +13777,11 @@
       <c r="CI94">
         <v>13</v>
       </c>
+      <c r="CJ94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:87">
+    <row r="96" spans="1:88">
       <c r="A96" s="2" t="s">
         <v>79</v>
       </c>
@@ -13667,8 +13890,11 @@
       <c r="CI96">
         <v>187</v>
       </c>
+      <c r="CJ96">
+        <v>188</v>
+      </c>
     </row>
-    <row r="97" spans="1:87">
+    <row r="97" spans="1:88">
       <c r="A97" s="2" t="s">
         <v>79</v>
       </c>
@@ -13777,8 +14003,11 @@
       <c r="CI97">
         <v>60</v>
       </c>
+      <c r="CJ97">
+        <v>65</v>
+      </c>
     </row>
-    <row r="98" spans="1:87">
+    <row r="98" spans="1:88">
       <c r="A98" s="2" t="s">
         <v>79</v>
       </c>
@@ -13885,6 +14114,9 @@
         <v>25</v>
       </c>
       <c r="CI98">
+        <v>25</v>
+      </c>
+      <c r="CJ98">
         <v>25</v>
       </c>
     </row>
@@ -13901,20 +14133,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BJ11"/>
+  <dimension ref="A2:BK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BJ11" sqref="BJ3:BJ11"/>
+    <sheetView topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BK11" sqref="BK11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:62" s="2" customFormat="1">
+    <row r="2" spans="1:63" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -14101,8 +14333,11 @@
       <c r="BJ2" s="9">
         <v>43981</v>
       </c>
+      <c r="BK2" s="9">
+        <v>43982</v>
+      </c>
     </row>
-    <row r="3" spans="1:62">
+    <row r="3" spans="1:63">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -14289,8 +14524,11 @@
       <c r="BJ3">
         <v>1229</v>
       </c>
+      <c r="BK3">
+        <v>1237</v>
+      </c>
     </row>
-    <row r="4" spans="1:62">
+    <row r="4" spans="1:63">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -14477,8 +14715,11 @@
       <c r="BJ4">
         <v>498</v>
       </c>
+      <c r="BK4">
+        <v>514</v>
+      </c>
     </row>
-    <row r="5" spans="1:62">
+    <row r="5" spans="1:63">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -14665,8 +14906,11 @@
       <c r="BJ5">
         <v>417</v>
       </c>
+      <c r="BK5">
+        <v>419</v>
+      </c>
     </row>
-    <row r="6" spans="1:62">
+    <row r="6" spans="1:63">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -14853,8 +15097,11 @@
       <c r="BJ6">
         <v>1840</v>
       </c>
+      <c r="BK6">
+        <v>1846</v>
+      </c>
     </row>
-    <row r="7" spans="1:62">
+    <row r="7" spans="1:63">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -15041,8 +15288,11 @@
       <c r="BJ7">
         <v>1364</v>
       </c>
+      <c r="BK7">
+        <v>1376</v>
+      </c>
     </row>
-    <row r="8" spans="1:62">
+    <row r="8" spans="1:63">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -15229,8 +15479,11 @@
       <c r="BJ8">
         <v>755</v>
       </c>
+      <c r="BK8">
+        <v>757</v>
+      </c>
     </row>
-    <row r="9" spans="1:62">
+    <row r="9" spans="1:63">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -15417,8 +15670,11 @@
       <c r="BJ9">
         <v>1285</v>
       </c>
+      <c r="BK9">
+        <v>1296</v>
+      </c>
     </row>
-    <row r="10" spans="1:62">
+    <row r="10" spans="1:63">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -15605,8 +15861,11 @@
       <c r="BJ10">
         <v>1259</v>
       </c>
+      <c r="BK10">
+        <v>1269</v>
+      </c>
     </row>
-    <row r="11" spans="1:62">
+    <row r="11" spans="1:63">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -15792,6 +16051,9 @@
       </c>
       <c r="BJ11">
         <v>154</v>
+      </c>
+      <c r="BK11">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -15802,20 +16064,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BE17"/>
+  <dimension ref="A2:BF17"/>
   <sheetViews>
     <sheetView topLeftCell="AO8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BE17" sqref="BE17"/>
+      <selection activeCell="BF17" sqref="BF17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:57" s="2" customFormat="1">
+    <row r="2" spans="1:58" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -15985,8 +16247,11 @@
       <c r="BE2" s="9">
         <v>43981</v>
       </c>
+      <c r="BF2" s="9">
+        <v>43982</v>
+      </c>
     </row>
-    <row r="3" spans="1:57" s="2" customFormat="1">
+    <row r="3" spans="1:58" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -15994,7 +16259,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:57">
+    <row r="4" spans="1:58">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -16166,8 +16431,11 @@
       <c r="BE4">
         <v>8801</v>
       </c>
+      <c r="BF4">
+        <v>8857</v>
+      </c>
     </row>
-    <row r="5" spans="1:57">
+    <row r="5" spans="1:58">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -16339,8 +16607,11 @@
       <c r="BE5">
         <v>914</v>
       </c>
+      <c r="BF5">
+        <v>926</v>
+      </c>
     </row>
-    <row r="6" spans="1:57">
+    <row r="6" spans="1:58">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -16512,8 +16783,11 @@
       <c r="BE6">
         <v>1346</v>
       </c>
+      <c r="BF6">
+        <v>1354</v>
+      </c>
     </row>
-    <row r="7" spans="1:57">
+    <row r="7" spans="1:58">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -16685,8 +16959,11 @@
       <c r="BE7">
         <v>4097</v>
       </c>
+      <c r="BF7">
+        <v>4119</v>
+      </c>
     </row>
-    <row r="8" spans="1:57">
+    <row r="8" spans="1:58">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -16858,8 +17135,11 @@
       <c r="BE8">
         <v>106</v>
       </c>
+      <c r="BF8">
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:57" ht="30">
+    <row r="9" spans="1:58" ht="28.8">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -17031,8 +17311,11 @@
       <c r="BE9">
         <v>26</v>
       </c>
+      <c r="BF9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:57" ht="30">
+    <row r="10" spans="1:58" ht="28.8">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -17200,8 +17483,11 @@
       <c r="BE10">
         <v>22</v>
       </c>
+      <c r="BF10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:57">
+    <row r="11" spans="1:58">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -17373,8 +17659,11 @@
       <c r="BE11">
         <v>2232</v>
       </c>
+      <c r="BF11">
+        <v>2246</v>
+      </c>
     </row>
-    <row r="12" spans="1:57" ht="30">
+    <row r="12" spans="1:58">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -17546,8 +17835,11 @@
       <c r="BE12">
         <v>58</v>
       </c>
+      <c r="BF12">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:57">
+    <row r="13" spans="1:58">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -17558,7 +17850,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:57">
+    <row r="14" spans="1:58">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -17730,8 +18022,11 @@
       <c r="BE14">
         <v>1521</v>
       </c>
+      <c r="BF14">
+        <v>1540</v>
+      </c>
     </row>
-    <row r="15" spans="1:57">
+    <row r="15" spans="1:58">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -17903,8 +18198,11 @@
       <c r="BE15">
         <v>2328</v>
       </c>
+      <c r="BF15">
+        <v>2336</v>
+      </c>
     </row>
-    <row r="16" spans="1:57">
+    <row r="16" spans="1:58">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -18076,8 +18374,11 @@
       <c r="BE16">
         <v>4927</v>
       </c>
+      <c r="BF16">
+        <v>4955</v>
+      </c>
     </row>
-    <row r="17" spans="1:57" ht="30">
+    <row r="17" spans="1:58">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -18248,6 +18549,9 @@
       </c>
       <c r="BE17">
         <v>25</v>
+      </c>
+      <c r="BF17">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -18258,19 +18562,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BE9"/>
+  <dimension ref="A1:BF9"/>
   <sheetViews>
-    <sheetView topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BE8" sqref="BE8"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="BF9" sqref="BF9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="2" customFormat="1">
+    <row r="1" spans="1:58" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -18439,14 +18743,17 @@
       <c r="BE1" s="9">
         <v>43981</v>
       </c>
+      <c r="BF1" s="9">
+        <v>43982</v>
+      </c>
     </row>
-    <row r="2" spans="1:57">
+    <row r="2" spans="1:58">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:57">
+    <row r="3" spans="1:58">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -18619,8 +18926,11 @@
       <c r="BE3">
         <v>466</v>
       </c>
+      <c r="BF3">
+        <v>468</v>
+      </c>
     </row>
-    <row r="4" spans="1:57">
+    <row r="4" spans="1:58">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -18792,8 +19102,11 @@
       <c r="BE4">
         <v>7</v>
       </c>
+      <c r="BF4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:57" ht="30">
+    <row r="5" spans="1:58" ht="28.8">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -18965,8 +19278,11 @@
       <c r="BE5">
         <v>349</v>
       </c>
+      <c r="BF5">
+        <v>351</v>
+      </c>
     </row>
-    <row r="6" spans="1:57">
+    <row r="6" spans="1:58">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -19138,8 +19454,11 @@
       <c r="BE6">
         <v>54</v>
       </c>
+      <c r="BF6">
+        <v>54</v>
+      </c>
     </row>
-    <row r="7" spans="1:57" ht="30">
+    <row r="7" spans="1:58">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -19311,8 +19630,11 @@
       <c r="BE7">
         <v>52</v>
       </c>
+      <c r="BF7">
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="1:57">
+    <row r="8" spans="1:58">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -19484,8 +19806,11 @@
       <c r="BE8">
         <v>4</v>
       </c>
+      <c r="BF8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:57">
+    <row r="9" spans="1:58">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -19496,6 +19821,9 @@
         <v>1</v>
       </c>
       <c r="BD9">
+        <v>1</v>
+      </c>
+      <c r="BF9">
         <v>1</v>
       </c>
     </row>
@@ -19506,18 +19834,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AQ13"/>
+  <dimension ref="A2:AR13"/>
   <sheetViews>
     <sheetView topLeftCell="AD5" workbookViewId="0">
-      <selection activeCell="AQ14" sqref="AQ14"/>
+      <selection activeCell="AR13" sqref="AR13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:43" s="2" customFormat="1">
+    <row r="2" spans="1:44" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -19647,8 +19975,11 @@
       <c r="AQ2" s="9">
         <v>43981</v>
       </c>
+      <c r="AR2" s="9">
+        <v>43982</v>
+      </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:44">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -19778,8 +20109,11 @@
       <c r="AQ3">
         <v>466</v>
       </c>
+      <c r="AR3">
+        <v>468</v>
+      </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:44">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -19909,8 +20243,11 @@
       <c r="AQ4">
         <v>48</v>
       </c>
+      <c r="AR4">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:44">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -20040,8 +20377,11 @@
       <c r="AQ5">
         <v>29</v>
       </c>
+      <c r="AR5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:44">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -20171,8 +20511,11 @@
       <c r="AQ6">
         <v>30</v>
       </c>
+      <c r="AR6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:44">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -20302,8 +20645,11 @@
       <c r="AQ7">
         <v>66</v>
       </c>
+      <c r="AR7">
+        <v>66</v>
+      </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:44">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -20433,8 +20779,11 @@
       <c r="AQ8">
         <v>74</v>
       </c>
+      <c r="AR8">
+        <v>75</v>
+      </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:44">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -20564,8 +20913,11 @@
       <c r="AQ9">
         <v>42</v>
       </c>
+      <c r="AR9">
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:44">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -20695,8 +21047,11 @@
       <c r="AQ10">
         <v>66</v>
       </c>
+      <c r="AR10">
+        <v>67</v>
+      </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:44">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -20826,8 +21181,11 @@
       <c r="AQ11">
         <v>95</v>
       </c>
+      <c r="AR11">
+        <v>95</v>
+      </c>
     </row>
-    <row r="12" spans="1:43" ht="30">
+    <row r="12" spans="1:44" ht="28.8">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -20957,8 +21315,11 @@
       <c r="AQ12">
         <v>16</v>
       </c>
+      <c r="AR12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:44">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -21086,6 +21447,9 @@
         <v>0</v>
       </c>
       <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
         <v>0</v>
       </c>
     </row>
@@ -21099,11 +21463,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6:N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
@@ -21204,6 +21568,9 @@
       <c r="M5" s="9">
         <v>43981</v>
       </c>
+      <c r="N5" s="9">
+        <v>43982</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
@@ -21242,6 +21609,9 @@
       <c r="M6">
         <v>119</v>
       </c>
+      <c r="N6">
+        <v>119</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
@@ -21280,6 +21650,9 @@
       <c r="M7">
         <v>31</v>
       </c>
+      <c r="N7">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="35" t="s">
@@ -21326,6 +21699,9 @@
       <c r="M9">
         <v>1</v>
       </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="31" t="s">
@@ -21364,6 +21740,9 @@
       <c r="M10">
         <v>21</v>
       </c>
+      <c r="N10">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="31" t="s">
@@ -21402,6 +21781,9 @@
       <c r="M11">
         <v>7</v>
       </c>
+      <c r="N11">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="31" t="s">
@@ -21440,6 +21822,9 @@
       <c r="M12">
         <v>2</v>
       </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="36" t="s">
@@ -21483,6 +21868,9 @@
       <c r="M14">
         <v>1</v>
       </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="31">
@@ -21521,6 +21909,9 @@
       <c r="M15">
         <v>0</v>
       </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="31">
@@ -21559,8 +21950,11 @@
       <c r="M16">
         <v>3</v>
       </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -21597,8 +21991,11 @@
       <c r="M17">
         <v>9</v>
       </c>
+      <c r="N17">
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -21635,8 +22032,11 @@
       <c r="M18">
         <v>2</v>
       </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -21673,8 +22073,11 @@
       <c r="M19">
         <v>2</v>
       </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:14">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -21711,8 +22114,11 @@
       <c r="M20">
         <v>3</v>
       </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -21749,8 +22155,11 @@
       <c r="M21">
         <v>6</v>
       </c>
+      <c r="N21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:13" ht="45">
+    <row r="22" spans="1:14" ht="28.8">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -21787,8 +22196,11 @@
       <c r="M22">
         <v>4</v>
       </c>
+      <c r="N22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:13" ht="30">
+    <row r="23" spans="1:14" ht="28.8">
       <c r="A23" s="39" t="s">
         <v>139</v>
       </c>
@@ -21823,6 +22235,9 @@
         <v>1</v>
       </c>
       <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
         <v>1</v>
       </c>
     </row>
@@ -21838,24 +22253,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="42" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -21902,7 +22317,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A4" s="44"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -21915,7 +22330,7 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A5" s="44"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
@@ -21926,7 +22341,7 @@
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A6" s="44"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -21937,7 +22352,7 @@
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A7" s="44"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
@@ -21948,7 +22363,7 @@
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.45" customHeight="1">
+    <row r="8" spans="1:7" ht="14.4" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
@@ -21971,7 +22386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.45" customHeight="1">
+    <row r="9" spans="1:7" ht="14.4" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>96</v>
       </c>
@@ -21994,7 +22409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" customHeight="1">
+    <row r="10" spans="1:7" ht="14.4" customHeight="1">
       <c r="A10" s="27" t="s">
         <v>98</v>
       </c>
@@ -22017,7 +22432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" customHeight="1">
+    <row r="11" spans="1:7" ht="14.4" customHeight="1">
       <c r="A11" s="27" t="s">
         <v>99</v>
       </c>
@@ -22040,7 +22455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" customHeight="1">
+    <row r="12" spans="1:7" ht="14.4" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>100</v>
       </c>
@@ -22063,7 +22478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.45" customHeight="1">
+    <row r="13" spans="1:7" ht="14.4" customHeight="1">
       <c r="A13" s="27" t="s">
         <v>143</v>
       </c>
@@ -22086,7 +22501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.45" customHeight="1">
+    <row r="14" spans="1:7" ht="14.4" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>103</v>
       </c>
@@ -22109,7 +22524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" customHeight="1">
+    <row r="15" spans="1:7" ht="14.4" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>104</v>
       </c>
@@ -22155,7 +22570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.45" customHeight="1">
+    <row r="17" spans="1:7" ht="14.4" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>107</v>
       </c>
@@ -22178,7 +22593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.45" customHeight="1">
+    <row r="18" spans="1:7" ht="14.4" customHeight="1">
       <c r="A18" s="27" t="s">
         <v>109</v>
       </c>
@@ -22201,7 +22616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.45" customHeight="1">
+    <row r="19" spans="1:7" ht="14.4" customHeight="1">
       <c r="A19" s="27" t="s">
         <v>110</v>
       </c>
@@ -22224,7 +22639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.45" customHeight="1">
+    <row r="20" spans="1:7" ht="14.4" customHeight="1">
       <c r="A20" s="27" t="s">
         <v>111</v>
       </c>
@@ -22247,7 +22662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.45" customHeight="1">
+    <row r="21" spans="1:7" ht="14.4" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>112</v>
       </c>
@@ -22270,12 +22685,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.45" customHeight="1">
+    <row r="22" spans="1:7" ht="14.4" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>115</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C22" s="28">
         <v>25</v>
@@ -22362,12 +22777,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.45" customHeight="1">
+    <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1">
       <c r="A26" s="30" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" s="28">
         <v>159</v>
@@ -22385,12 +22800,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75">
+    <row r="27" spans="1:7" ht="15.6">
       <c r="A27" s="24" t="s">
         <v>120</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -22419,12 +22834,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -22627,6 +23036,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -22637,23 +23052,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22672,6 +23070,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
02 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="851" documentId="8_{C5E88C75-E440-43B4-B034-AA36176F93AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2D087BDD-E593-48F0-8D01-32BDC4B573F7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D919E9F5-8372-44A9-9972-4EFC8A4CB45B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="166">
   <si>
     <t>Testing</t>
   </si>
@@ -522,11 +524,20 @@
     <t>857; (370)</t>
   </si>
   <si>
-    <t>As of May 31, 2020</t>
+    <t>Human Services - CFSA</t>
+  </si>
+  <si>
+    <t>Number of Personnel Who Have Tested Positive</t>
+  </si>
+  <si>
+    <t>Number of Personnel Currently in Quarantine</t>
+  </si>
+  <si>
+    <t>As of June 1, 2020</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of May 31, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of June 1, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -657,7 +668,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -665,11 +676,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD9E1F2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD9E1F2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD9E1F2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD9E1F2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -771,6 +797,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1166,26 +1193,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ113"/>
+  <dimension ref="A1:CK118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="BY1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CJ87" sqref="CJ1:CJ1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="CE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CK53" sqref="CK1:CK1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" customWidth="1"/>
-    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="80" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88">
+    <row r="1" spans="1:89">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1444,8 +1471,11 @@
       <c r="CJ1" s="1">
         <v>43982</v>
       </c>
+      <c r="CK1" s="1">
+        <v>43983</v>
+      </c>
     </row>
-    <row r="2" spans="1:88">
+    <row r="2" spans="1:89">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1499,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:89">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1713,8 +1743,11 @@
       <c r="CJ3">
         <v>47263</v>
       </c>
+      <c r="CK3">
+        <v>47701</v>
+      </c>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:89">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1753,8 +1786,11 @@
       <c r="CJ4">
         <v>38975</v>
       </c>
+      <c r="CK4">
+        <v>39251</v>
+      </c>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:89">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2019,8 +2055,11 @@
       <c r="CJ5">
         <v>8857</v>
       </c>
+      <c r="CK5">
+        <v>8886</v>
+      </c>
     </row>
-    <row r="6" spans="1:88">
+    <row r="6" spans="1:89">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2267,8 +2306,11 @@
       <c r="CJ6">
         <v>468</v>
       </c>
+      <c r="CK6">
+        <v>470</v>
+      </c>
     </row>
-    <row r="7" spans="1:88">
+    <row r="7" spans="1:89">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2485,11 +2527,14 @@
       <c r="CJ7">
         <v>1126</v>
       </c>
+      <c r="CK7">
+        <v>1137</v>
+      </c>
     </row>
-    <row r="8" spans="1:88">
+    <row r="8" spans="1:89">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:88">
+    <row r="9" spans="1:89">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2598,8 +2643,11 @@
       <c r="CJ9">
         <v>345</v>
       </c>
+      <c r="CK9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:88">
+    <row r="10" spans="1:89">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2810,8 +2858,11 @@
       <c r="CJ10">
         <v>73</v>
       </c>
+      <c r="CK10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="11" spans="1:88">
+    <row r="11" spans="1:89">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3022,8 +3073,11 @@
       <c r="CJ11">
         <v>440</v>
       </c>
+      <c r="CK11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:88">
+    <row r="12" spans="1:89">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3234,8 +3288,11 @@
       <c r="CJ12">
         <v>204</v>
       </c>
+      <c r="CK12">
+        <v>208</v>
+      </c>
     </row>
-    <row r="13" spans="1:88">
+    <row r="13" spans="1:89">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3446,8 +3503,11 @@
       <c r="CJ13">
         <v>236</v>
       </c>
+      <c r="CK13">
+        <v>232</v>
+      </c>
     </row>
-    <row r="14" spans="1:88">
+    <row r="14" spans="1:89">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3520,8 +3580,11 @@
       <c r="CJ14">
         <v>302</v>
       </c>
+      <c r="CK14">
+        <v>295</v>
+      </c>
     </row>
-    <row r="15" spans="1:88">
+    <row r="15" spans="1:89">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3564,8 +3627,11 @@
       <c r="CJ15">
         <v>108</v>
       </c>
+      <c r="CK15">
+        <v>106</v>
+      </c>
     </row>
-    <row r="16" spans="1:88">
+    <row r="16" spans="1:89">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3638,8 +3704,11 @@
       <c r="CJ16">
         <v>1891</v>
       </c>
+      <c r="CK16">
+        <v>1887</v>
+      </c>
     </row>
-    <row r="17" spans="1:88">
+    <row r="17" spans="1:89">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3712,13 +3781,16 @@
       <c r="CJ17" s="23">
         <v>0.76</v>
       </c>
+      <c r="CK17" s="23">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="19" spans="1:88">
+    <row r="19" spans="1:89">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:88">
+    <row r="20" spans="1:89">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3726,7 +3798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:88">
+    <row r="21" spans="1:89">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -3929,19 +4001,22 @@
         <v>107</v>
       </c>
       <c r="CG21">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="CH21">
+        <v>105</v>
+      </c>
+      <c r="CI21">
+        <v>92</v>
+      </c>
+      <c r="CJ21">
+        <v>19</v>
+      </c>
+      <c r="CK21">
         <v>111</v>
       </c>
-      <c r="CI21">
-        <v>111</v>
-      </c>
-      <c r="CJ21">
-        <v>111</v>
-      </c>
     </row>
-    <row r="22" spans="1:88">
+    <row r="22" spans="1:89">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4101,8 +4176,11 @@
       <c r="CJ22">
         <v>19</v>
       </c>
+      <c r="CK22">
+        <v>19</v>
+      </c>
     </row>
-    <row r="23" spans="1:88">
+    <row r="23" spans="1:89">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4262,8 +4340,11 @@
       <c r="CJ23">
         <v>92</v>
       </c>
+      <c r="CK23">
+        <v>92</v>
+      </c>
     </row>
-    <row r="24" spans="1:88">
+    <row r="24" spans="1:89">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4468,8 +4549,11 @@
       <c r="CJ24">
         <v>129</v>
       </c>
+      <c r="CK24">
+        <v>105</v>
+      </c>
     </row>
-    <row r="25" spans="1:88">
+    <row r="25" spans="1:89">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4674,8 +4758,11 @@
       <c r="CJ25">
         <v>148</v>
       </c>
+      <c r="CK25">
+        <v>124</v>
+      </c>
     </row>
-    <row r="26" spans="1:88">
+    <row r="26" spans="1:89">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4880,13 +4967,16 @@
       <c r="CJ26">
         <v>1384</v>
       </c>
+      <c r="CK26">
+        <v>1395</v>
+      </c>
     </row>
-    <row r="28" spans="1:88">
+    <row r="28" spans="1:89">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:88">
+    <row r="29" spans="1:89">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5100,8 +5190,11 @@
       <c r="CJ29">
         <v>135</v>
       </c>
+      <c r="CK29">
+        <v>138</v>
+      </c>
     </row>
-    <row r="30" spans="1:88">
+    <row r="30" spans="1:89">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5261,8 +5354,11 @@
       <c r="CJ30">
         <v>29</v>
       </c>
+      <c r="CK30">
+        <v>32</v>
+      </c>
     </row>
-    <row r="31" spans="1:88">
+    <row r="31" spans="1:89">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5422,8 +5518,11 @@
       <c r="CJ31">
         <v>106</v>
       </c>
+      <c r="CK31">
+        <v>106</v>
+      </c>
     </row>
-    <row r="32" spans="1:88">
+    <row r="32" spans="1:89">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5628,8 +5727,11 @@
       <c r="CJ32">
         <v>48</v>
       </c>
+      <c r="CK32">
+        <v>52</v>
+      </c>
     </row>
-    <row r="33" spans="1:88">
+    <row r="33" spans="1:89">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5834,8 +5936,11 @@
       <c r="CJ33">
         <v>77</v>
       </c>
+      <c r="CK33">
+        <v>84</v>
+      </c>
     </row>
-    <row r="34" spans="1:88">
+    <row r="34" spans="1:89">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6040,13 +6145,16 @@
       <c r="CJ34">
         <v>1206</v>
       </c>
+      <c r="CK34">
+        <v>1212</v>
+      </c>
     </row>
-    <row r="36" spans="1:88">
+    <row r="36" spans="1:89">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:88">
+    <row r="37" spans="1:89">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -6248,8 +6356,11 @@
       <c r="CJ37">
         <v>80</v>
       </c>
+      <c r="CK37">
+        <v>80</v>
+      </c>
     </row>
-    <row r="38" spans="1:88">
+    <row r="38" spans="1:89">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6403,8 +6514,11 @@
       <c r="CJ38">
         <v>6</v>
       </c>
+      <c r="CK38">
+        <v>6</v>
+      </c>
     </row>
-    <row r="39" spans="1:88">
+    <row r="39" spans="1:89">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6558,8 +6672,11 @@
       <c r="CJ39">
         <v>73</v>
       </c>
+      <c r="CK39">
+        <v>73</v>
+      </c>
     </row>
-    <row r="40" spans="1:88">
+    <row r="40" spans="1:89">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6758,8 +6875,11 @@
       <c r="CJ40">
         <v>1</v>
       </c>
+      <c r="CK40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:88">
+    <row r="41" spans="1:89">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -6955,8 +7075,11 @@
       <c r="CJ41">
         <v>7</v>
       </c>
+      <c r="CK41">
+        <v>9</v>
+      </c>
     </row>
-    <row r="42" spans="1:88">
+    <row r="42" spans="1:89">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7158,8 +7281,11 @@
       <c r="CJ42">
         <v>281</v>
       </c>
+      <c r="CK42">
+        <v>281</v>
+      </c>
     </row>
-    <row r="43" spans="1:88">
+    <row r="43" spans="1:89">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -7295,16 +7421,19 @@
       <c r="CJ43">
         <v>1</v>
       </c>
+      <c r="CK43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:88">
+    <row r="44" spans="1:89">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:88">
+    <row r="45" spans="1:89">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:88">
+    <row r="46" spans="1:89">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -7512,8 +7641,11 @@
       <c r="CJ46">
         <v>205</v>
       </c>
+      <c r="CK46">
+        <v>205</v>
+      </c>
     </row>
-    <row r="47" spans="1:88">
+    <row r="47" spans="1:89">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7673,8 +7805,11 @@
       <c r="CJ47">
         <v>18</v>
       </c>
+      <c r="CK47">
+        <v>18</v>
+      </c>
     </row>
-    <row r="48" spans="1:88">
+    <row r="48" spans="1:89">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7834,8 +7969,11 @@
       <c r="CJ48">
         <v>181</v>
       </c>
+      <c r="CK48">
+        <v>181</v>
+      </c>
     </row>
-    <row r="49" spans="1:88">
+    <row r="49" spans="1:89">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -8040,8 +8178,11 @@
       <c r="CJ49">
         <v>479</v>
       </c>
+      <c r="CK49">
+        <v>469</v>
+      </c>
     </row>
-    <row r="50" spans="1:88">
+    <row r="50" spans="1:89">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -8201,8 +8342,11 @@
       <c r="CJ50">
         <v>497</v>
       </c>
+      <c r="CK50">
+        <v>487</v>
+      </c>
     </row>
-    <row r="51" spans="1:88">
+    <row r="51" spans="1:89">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -8359,8 +8503,11 @@
       <c r="CJ51">
         <v>820</v>
       </c>
+      <c r="CK51">
+        <v>830</v>
+      </c>
     </row>
-    <row r="52" spans="1:88">
+    <row r="52" spans="1:89">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -8511,16 +8658,19 @@
       <c r="CJ52">
         <v>1</v>
       </c>
+      <c r="CK52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:88">
+    <row r="53" spans="1:89">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:88">
+    <row r="54" spans="1:89">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:88">
+    <row r="55" spans="1:89">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -8713,8 +8863,11 @@
       <c r="CJ55">
         <v>29</v>
       </c>
+      <c r="CK55">
+        <v>30</v>
+      </c>
     </row>
-    <row r="56" spans="1:88">
+    <row r="56" spans="1:89">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -8871,8 +9024,11 @@
       <c r="CJ56">
         <v>7</v>
       </c>
+      <c r="CK56">
+        <v>7</v>
+      </c>
     </row>
-    <row r="57" spans="1:88">
+    <row r="57" spans="1:89">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -9029,8 +9185,11 @@
       <c r="CJ57">
         <v>21</v>
       </c>
+      <c r="CK57">
+        <v>22</v>
+      </c>
     </row>
-    <row r="58" spans="1:88">
+    <row r="58" spans="1:89">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -9223,8 +9382,11 @@
       <c r="CJ58">
         <v>18</v>
       </c>
+      <c r="CK58">
+        <v>16</v>
+      </c>
     </row>
-    <row r="59" spans="1:88">
+    <row r="59" spans="1:89">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -9417,8 +9579,11 @@
       <c r="CJ59">
         <v>25</v>
       </c>
+      <c r="CK59">
+        <v>23</v>
+      </c>
     </row>
-    <row r="60" spans="1:88">
+    <row r="60" spans="1:89">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -9611,8 +9776,11 @@
       <c r="CJ60">
         <v>142</v>
       </c>
+      <c r="CK60">
+        <v>145</v>
+      </c>
     </row>
-    <row r="61" spans="1:88">
+    <row r="61" spans="1:89">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -9763,8 +9931,11 @@
       <c r="CJ61">
         <v>1</v>
       </c>
+      <c r="CK61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:88">
+    <row r="63" spans="1:89">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -9957,8 +10128,11 @@
       <c r="CJ63">
         <v>11</v>
       </c>
+      <c r="CK63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:88">
+    <row r="64" spans="1:89">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -10115,8 +10289,11 @@
       <c r="CJ64">
         <v>2</v>
       </c>
+      <c r="CK64">
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:88">
+    <row r="65" spans="1:89">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -10273,8 +10450,11 @@
       <c r="CJ65">
         <v>9</v>
       </c>
+      <c r="CK65">
+        <v>9</v>
+      </c>
     </row>
-    <row r="66" spans="1:88">
+    <row r="66" spans="1:89">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -10467,8 +10647,11 @@
       <c r="CJ66">
         <v>52</v>
       </c>
+      <c r="CK66">
+        <v>54</v>
+      </c>
     </row>
-    <row r="67" spans="1:88">
+    <row r="67" spans="1:89">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -10662,8 +10845,11 @@
       <c r="CJ67">
         <v>54</v>
       </c>
+      <c r="CK67">
+        <v>56</v>
+      </c>
     </row>
-    <row r="68" spans="1:88">
+    <row r="68" spans="1:89">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -10856,8 +11042,11 @@
       <c r="CJ68">
         <v>0</v>
       </c>
+      <c r="CK68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:88">
+    <row r="69" spans="1:89">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -11014,11 +11203,14 @@
       <c r="CJ69">
         <v>0</v>
       </c>
+      <c r="CK69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:88">
+    <row r="70" spans="1:89">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:88">
+    <row r="71" spans="1:89">
       <c r="A71" s="2" t="s">
         <v>132</v>
       </c>
@@ -11061,8 +11253,11 @@
       <c r="CJ71">
         <v>10</v>
       </c>
+      <c r="CK71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:88">
+    <row r="72" spans="1:89">
       <c r="A72" s="2" t="s">
         <v>132</v>
       </c>
@@ -11105,8 +11300,11 @@
       <c r="CJ72">
         <v>6</v>
       </c>
+      <c r="CK72">
+        <v>5</v>
+      </c>
     </row>
-    <row r="73" spans="1:88">
+    <row r="73" spans="1:89">
       <c r="A73" s="2" t="s">
         <v>132</v>
       </c>
@@ -11149,8 +11347,11 @@
       <c r="CJ73">
         <v>4</v>
       </c>
+      <c r="CK73">
+        <v>5</v>
+      </c>
     </row>
-    <row r="74" spans="1:88">
+    <row r="74" spans="1:89">
       <c r="A74" s="2" t="s">
         <v>132</v>
       </c>
@@ -11193,8 +11394,11 @@
       <c r="CJ74">
         <v>12</v>
       </c>
+      <c r="CK74">
+        <v>8</v>
+      </c>
     </row>
-    <row r="75" spans="1:88">
+    <row r="75" spans="1:89">
       <c r="A75" s="2" t="s">
         <v>132</v>
       </c>
@@ -11237,8 +11441,11 @@
       <c r="CJ75">
         <v>18</v>
       </c>
+      <c r="CK75">
+        <v>13</v>
+      </c>
     </row>
-    <row r="76" spans="1:88">
+    <row r="76" spans="1:89">
       <c r="A76" s="2" t="s">
         <v>132</v>
       </c>
@@ -11281,13 +11488,16 @@
       <c r="CJ76">
         <v>29</v>
       </c>
+      <c r="CK76">
+        <v>33</v>
+      </c>
     </row>
-    <row r="78" spans="1:88">
+    <row r="78" spans="1:89">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:88">
+    <row r="79" spans="1:89">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -11480,8 +11690,11 @@
       <c r="CJ79">
         <v>297</v>
       </c>
+      <c r="CK79">
+        <v>298</v>
+      </c>
     </row>
-    <row r="80" spans="1:88">
+    <row r="80" spans="1:89">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -11674,8 +11887,11 @@
       <c r="CJ80">
         <v>114</v>
       </c>
+      <c r="CK80">
+        <v>104</v>
+      </c>
     </row>
-    <row r="81" spans="1:88">
+    <row r="81" spans="1:89">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -11868,8 +12084,11 @@
       <c r="CJ81">
         <v>93</v>
       </c>
+      <c r="CK81">
+        <v>84</v>
+      </c>
     </row>
-    <row r="82" spans="1:88">
+    <row r="82" spans="1:89">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -12020,8 +12239,11 @@
       <c r="CJ82">
         <v>16</v>
       </c>
+      <c r="CK82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:88">
+    <row r="84" spans="1:89">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -12214,8 +12436,11 @@
       <c r="CJ84">
         <v>119</v>
       </c>
+      <c r="CK84">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:88">
+    <row r="85" spans="1:89">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -12408,8 +12633,11 @@
       <c r="CJ85">
         <v>28</v>
       </c>
+      <c r="CK85">
+        <v>25</v>
+      </c>
     </row>
-    <row r="86" spans="1:88">
+    <row r="86" spans="1:89">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -12602,8 +12830,11 @@
       <c r="CJ86">
         <v>147</v>
       </c>
+      <c r="CK86">
+        <v>144</v>
+      </c>
     </row>
-    <row r="87" spans="1:88">
+    <row r="87" spans="1:89">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -12796,8 +13027,11 @@
       <c r="CJ87">
         <v>190</v>
       </c>
+      <c r="CK87">
+        <v>194</v>
+      </c>
     </row>
-    <row r="88" spans="1:88">
+    <row r="88" spans="1:89">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -12864,8 +13098,11 @@
       <c r="CJ88">
         <v>1</v>
       </c>
+      <c r="CK88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:88">
+    <row r="90" spans="1:89">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -13058,8 +13295,11 @@
       <c r="CJ90">
         <v>81</v>
       </c>
+      <c r="CK90">
+        <v>81</v>
+      </c>
     </row>
-    <row r="91" spans="1:88">
+    <row r="91" spans="1:89">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -13252,8 +13492,11 @@
       <c r="CJ91">
         <v>22</v>
       </c>
+      <c r="CK91">
+        <v>21</v>
+      </c>
     </row>
-    <row r="92" spans="1:88">
+    <row r="92" spans="1:89">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -13434,8 +13677,11 @@
       <c r="CJ92">
         <v>158</v>
       </c>
+      <c r="CK92">
+        <v>168</v>
+      </c>
     </row>
-    <row r="93" spans="1:88">
+    <row r="93" spans="1:89">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -13628,8 +13874,11 @@
       <c r="CJ93">
         <v>41</v>
       </c>
+      <c r="CK93">
+        <v>41</v>
+      </c>
     </row>
-    <row r="94" spans="1:88">
+    <row r="94" spans="1:89">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -13780,348 +14029,419 @@
       <c r="CJ94">
         <v>13</v>
       </c>
+      <c r="CK94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:88">
+    <row r="95" spans="1:89">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" spans="1:89">
       <c r="A96" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B96" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="CG96">
+        <v>9</v>
+      </c>
+      <c r="CK96">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:89">
+      <c r="A97" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="CG97">
+        <v>17</v>
+      </c>
+      <c r="CK97">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:89">
+      <c r="A98" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="CG98">
+        <v>3</v>
+      </c>
+      <c r="CK98">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:89">
+      <c r="A99" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B99" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="CG99">
+        <v>1</v>
+      </c>
+      <c r="CK99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:89">
+      <c r="A101" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B101" t="s">
         <v>76</v>
       </c>
-      <c r="BB96">
+      <c r="BB101">
         <v>112</v>
       </c>
-      <c r="BC96">
+      <c r="BC101">
         <v>121</v>
       </c>
-      <c r="BD96">
+      <c r="BD101">
         <v>130</v>
       </c>
-      <c r="BE96">
+      <c r="BE101">
         <v>135</v>
       </c>
-      <c r="BF96">
+      <c r="BF101">
         <v>137</v>
       </c>
-      <c r="BG96">
+      <c r="BG101">
         <v>137</v>
       </c>
-      <c r="BH96">
+      <c r="BH101">
         <v>137</v>
       </c>
-      <c r="BI96">
+      <c r="BI101">
         <v>137</v>
       </c>
-      <c r="BJ96">
+      <c r="BJ101">
         <v>142</v>
       </c>
-      <c r="BK96">
+      <c r="BK101">
         <v>144</v>
       </c>
-      <c r="BL96">
+      <c r="BL101">
         <v>145</v>
       </c>
-      <c r="BM96">
+      <c r="BM101">
         <v>147</v>
       </c>
-      <c r="BN96">
+      <c r="BN101">
         <v>147</v>
       </c>
-      <c r="BO96">
+      <c r="BO101">
         <v>150</v>
       </c>
-      <c r="BP96">
+      <c r="BP101">
         <v>155</v>
       </c>
-      <c r="BQ96">
+      <c r="BQ101">
         <v>156</v>
       </c>
-      <c r="BR96">
+      <c r="BR101">
         <v>158</v>
       </c>
-      <c r="BS96">
+      <c r="BS101">
         <v>158</v>
       </c>
-      <c r="BT96">
+      <c r="BT101">
         <v>168</v>
       </c>
-      <c r="BU96">
+      <c r="BU101">
         <v>169</v>
       </c>
-      <c r="BV96">
+      <c r="BV101">
         <v>169</v>
       </c>
-      <c r="BW96">
+      <c r="BW101">
         <v>172</v>
       </c>
-      <c r="BX96">
+      <c r="BX101">
         <v>175</v>
       </c>
-      <c r="BY96">
+      <c r="BY101">
         <v>176</v>
       </c>
-      <c r="BZ96">
+      <c r="BZ101">
         <v>178</v>
       </c>
-      <c r="CA96">
+      <c r="CA101">
         <v>178</v>
       </c>
-      <c r="CB96">
+      <c r="CB101">
         <v>179</v>
       </c>
-      <c r="CC96">
+      <c r="CC101">
         <v>179</v>
       </c>
-      <c r="CD96">
+      <c r="CD101">
         <v>179</v>
       </c>
-      <c r="CE96">
+      <c r="CE101">
         <v>182</v>
       </c>
-      <c r="CF96">
+      <c r="CF101">
         <v>183</v>
       </c>
-      <c r="CG96">
+      <c r="CG101">
         <v>185</v>
       </c>
-      <c r="CH96">
+      <c r="CH101">
         <v>187</v>
       </c>
-      <c r="CI96">
+      <c r="CI101">
         <v>187</v>
       </c>
-      <c r="CJ96">
+      <c r="CJ101">
         <v>188</v>
       </c>
+      <c r="CK101">
+        <v>188</v>
+      </c>
     </row>
-    <row r="97" spans="1:88">
-      <c r="A97" s="2" t="s">
+    <row r="102" spans="1:89">
+      <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B102" t="s">
         <v>77</v>
       </c>
-      <c r="BB97">
+      <c r="BB102">
         <v>5</v>
       </c>
-      <c r="BC97">
+      <c r="BC102">
         <v>8</v>
       </c>
-      <c r="BD97">
+      <c r="BD102">
         <v>10</v>
       </c>
-      <c r="BE97">
+      <c r="BE102">
         <v>11</v>
       </c>
-      <c r="BF97">
+      <c r="BF102">
         <v>14</v>
       </c>
-      <c r="BG97">
+      <c r="BG102">
         <v>15</v>
       </c>
-      <c r="BH97">
+      <c r="BH102">
         <v>15</v>
       </c>
-      <c r="BI97">
+      <c r="BI102">
         <v>18</v>
       </c>
-      <c r="BJ97">
+      <c r="BJ102">
         <v>19</v>
       </c>
-      <c r="BK97">
+      <c r="BK102">
         <v>22</v>
       </c>
-      <c r="BL97">
+      <c r="BL102">
         <v>22</v>
       </c>
-      <c r="BM97">
+      <c r="BM102">
         <v>24</v>
       </c>
-      <c r="BN97">
+      <c r="BN102">
         <v>24</v>
       </c>
-      <c r="BO97">
+      <c r="BO102">
         <v>24</v>
       </c>
-      <c r="BP97">
+      <c r="BP102">
         <v>24</v>
       </c>
-      <c r="BQ97">
+      <c r="BQ102">
         <v>27</v>
       </c>
-      <c r="BR97">
+      <c r="BR102">
         <v>27</v>
       </c>
-      <c r="BS97">
+      <c r="BS102">
         <v>38</v>
       </c>
-      <c r="BT97">
+      <c r="BT102">
         <v>38</v>
       </c>
-      <c r="BU97">
+      <c r="BU102">
         <v>40</v>
       </c>
-      <c r="BV97">
+      <c r="BV102">
         <v>40</v>
       </c>
-      <c r="BW97">
+      <c r="BW102">
         <v>40</v>
       </c>
-      <c r="BX97">
+      <c r="BX102">
         <v>40</v>
       </c>
-      <c r="BY97">
+      <c r="BY102">
         <v>40</v>
       </c>
-      <c r="BZ97">
+      <c r="BZ102">
         <v>41</v>
       </c>
-      <c r="CA97">
+      <c r="CA102">
         <v>41</v>
       </c>
-      <c r="CB97">
+      <c r="CB102">
         <v>41</v>
       </c>
-      <c r="CC97">
+      <c r="CC102">
         <v>41</v>
       </c>
-      <c r="CD97">
+      <c r="CD102">
         <v>41</v>
       </c>
-      <c r="CE97">
+      <c r="CE102">
         <v>47</v>
       </c>
-      <c r="CF97">
+      <c r="CF102">
         <v>49</v>
       </c>
-      <c r="CG97">
+      <c r="CG102">
         <v>53</v>
       </c>
-      <c r="CH97">
+      <c r="CH102">
         <v>60</v>
       </c>
-      <c r="CI97">
+      <c r="CI102">
         <v>60</v>
       </c>
-      <c r="CJ97">
+      <c r="CJ102">
         <v>65</v>
       </c>
+      <c r="CK102">
+        <v>70</v>
+      </c>
     </row>
-    <row r="98" spans="1:88">
-      <c r="A98" s="2" t="s">
+    <row r="103" spans="1:89">
+      <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B103" t="s">
         <v>78</v>
       </c>
-      <c r="BB98">
+      <c r="BB103">
         <v>16</v>
       </c>
-      <c r="BC98">
+      <c r="BC103">
         <v>16</v>
       </c>
-      <c r="BD98">
+      <c r="BD103">
         <v>17</v>
       </c>
-      <c r="BE98">
+      <c r="BE103">
         <v>17</v>
       </c>
-      <c r="BF98">
+      <c r="BF103">
         <v>18</v>
       </c>
-      <c r="BG98">
+      <c r="BG103">
         <v>18</v>
       </c>
-      <c r="BH98">
+      <c r="BH103">
         <v>19</v>
       </c>
-      <c r="BI98">
+      <c r="BI103">
         <v>19</v>
       </c>
-      <c r="BJ98">
+      <c r="BJ103">
         <v>19</v>
       </c>
-      <c r="BK98">
+      <c r="BK103">
         <v>19</v>
       </c>
-      <c r="BL98">
+      <c r="BL103">
         <v>20</v>
       </c>
-      <c r="BM98">
+      <c r="BM103">
         <v>20</v>
       </c>
-      <c r="BN98">
+      <c r="BN103">
         <v>20</v>
       </c>
-      <c r="BO98">
+      <c r="BO103">
         <v>20</v>
       </c>
-      <c r="BP98">
+      <c r="BP103">
         <v>20</v>
       </c>
-      <c r="BQ98">
+      <c r="BQ103">
         <v>21</v>
       </c>
-      <c r="BR98">
+      <c r="BR103">
         <v>22</v>
       </c>
-      <c r="BS98">
+      <c r="BS103">
         <v>23</v>
       </c>
-      <c r="BT98">
+      <c r="BT103">
         <v>24</v>
       </c>
-      <c r="BU98">
+      <c r="BU103">
         <v>24</v>
       </c>
-      <c r="BV98">
+      <c r="BV103">
         <v>24</v>
       </c>
-      <c r="BW98">
+      <c r="BW103">
         <v>24</v>
       </c>
-      <c r="BX98">
+      <c r="BX103">
         <v>25</v>
       </c>
-      <c r="BY98">
+      <c r="BY103">
         <v>25</v>
       </c>
-      <c r="BZ98">
+      <c r="BZ103">
         <v>25</v>
       </c>
-      <c r="CA98">
+      <c r="CA103">
         <v>25</v>
       </c>
-      <c r="CB98">
+      <c r="CB103">
         <v>25</v>
       </c>
-      <c r="CC98">
+      <c r="CC103">
         <v>25</v>
       </c>
-      <c r="CD98">
+      <c r="CD103">
         <v>25</v>
       </c>
-      <c r="CE98">
+      <c r="CE103">
         <v>25</v>
       </c>
-      <c r="CF98">
+      <c r="CF103">
         <v>25</v>
       </c>
-      <c r="CG98">
+      <c r="CG103">
         <v>25</v>
       </c>
-      <c r="CH98">
+      <c r="CH103">
         <v>25</v>
       </c>
-      <c r="CI98">
+      <c r="CI103">
         <v>25</v>
       </c>
-      <c r="CJ98">
+      <c r="CJ103">
         <v>25</v>
       </c>
+      <c r="CK103">
+        <v>25</v>
+      </c>
     </row>
-    <row r="113" spans="52:52">
-      <c r="AZ113">
+    <row r="118" spans="52:52">
+      <c r="AZ118">
         <v>9</v>
       </c>
     </row>
@@ -14133,20 +14453,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BK11"/>
+  <dimension ref="A2:BL11"/>
   <sheetViews>
-    <sheetView topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BK11" sqref="BK11"/>
+    <sheetView tabSelected="1" topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BL11" sqref="BL3:BL11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:63" s="2" customFormat="1">
+    <row r="2" spans="1:64" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -14336,8 +14656,11 @@
       <c r="BK2" s="9">
         <v>43982</v>
       </c>
+      <c r="BL2" s="9">
+        <v>43983</v>
+      </c>
     </row>
-    <row r="3" spans="1:63">
+    <row r="3" spans="1:64">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -14527,8 +14850,11 @@
       <c r="BK3">
         <v>1237</v>
       </c>
+      <c r="BL3">
+        <v>1243</v>
+      </c>
     </row>
-    <row r="4" spans="1:63">
+    <row r="4" spans="1:64">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -14718,8 +15044,11 @@
       <c r="BK4">
         <v>514</v>
       </c>
+      <c r="BL4">
+        <v>513</v>
+      </c>
     </row>
-    <row r="5" spans="1:63">
+    <row r="5" spans="1:64">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -14909,8 +15238,11 @@
       <c r="BK5">
         <v>419</v>
       </c>
+      <c r="BL5">
+        <v>420</v>
+      </c>
     </row>
-    <row r="6" spans="1:63">
+    <row r="6" spans="1:64">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -15100,8 +15432,11 @@
       <c r="BK6">
         <v>1846</v>
       </c>
+      <c r="BL6">
+        <v>1852</v>
+      </c>
     </row>
-    <row r="7" spans="1:63">
+    <row r="7" spans="1:64">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -15291,8 +15626,11 @@
       <c r="BK7">
         <v>1376</v>
       </c>
+      <c r="BL7">
+        <v>1379</v>
+      </c>
     </row>
-    <row r="8" spans="1:63">
+    <row r="8" spans="1:64">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -15482,8 +15820,11 @@
       <c r="BK8">
         <v>757</v>
       </c>
+      <c r="BL8">
+        <v>758</v>
+      </c>
     </row>
-    <row r="9" spans="1:63">
+    <row r="9" spans="1:64">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -15673,8 +16014,11 @@
       <c r="BK9">
         <v>1296</v>
       </c>
+      <c r="BL9">
+        <v>1298</v>
+      </c>
     </row>
-    <row r="10" spans="1:63">
+    <row r="10" spans="1:64">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -15864,8 +16208,11 @@
       <c r="BK10">
         <v>1269</v>
       </c>
+      <c r="BL10">
+        <v>1278</v>
+      </c>
     </row>
-    <row r="11" spans="1:63">
+    <row r="11" spans="1:64">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -16054,6 +16401,9 @@
       </c>
       <c r="BK11">
         <v>143</v>
+      </c>
+      <c r="BL11">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -16064,20 +16414,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BF17"/>
+  <dimension ref="A2:BG17"/>
   <sheetViews>
     <sheetView topLeftCell="AO8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BF17" sqref="BF17"/>
+      <selection activeCell="BG17" sqref="BG17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:58" s="2" customFormat="1">
+    <row r="2" spans="1:59" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -16250,8 +16600,11 @@
       <c r="BF2" s="9">
         <v>43982</v>
       </c>
+      <c r="BG2" s="9">
+        <v>43983</v>
+      </c>
     </row>
-    <row r="3" spans="1:58" s="2" customFormat="1">
+    <row r="3" spans="1:59" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -16259,7 +16612,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:59">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -16434,8 +16787,11 @@
       <c r="BF4">
         <v>8857</v>
       </c>
+      <c r="BG4">
+        <v>8886</v>
+      </c>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:59">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -16610,8 +16966,11 @@
       <c r="BF5">
         <v>926</v>
       </c>
+      <c r="BG5">
+        <v>916</v>
+      </c>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:59">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -16786,8 +17145,11 @@
       <c r="BF6">
         <v>1354</v>
       </c>
+      <c r="BG6">
+        <v>1358</v>
+      </c>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:59">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -16962,8 +17324,11 @@
       <c r="BF7">
         <v>4119</v>
       </c>
+      <c r="BG7">
+        <v>4142</v>
+      </c>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:59">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -17138,8 +17503,11 @@
       <c r="BF8">
         <v>106</v>
       </c>
+      <c r="BG8">
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:58" ht="28.8">
+    <row r="9" spans="1:59" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -17314,8 +17682,11 @@
       <c r="BF9">
         <v>26</v>
       </c>
+      <c r="BG9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:58" ht="28.8">
+    <row r="10" spans="1:59" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -17486,8 +17857,11 @@
       <c r="BF10">
         <v>22</v>
       </c>
+      <c r="BG10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:59">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -17662,8 +18036,11 @@
       <c r="BF11">
         <v>2246</v>
       </c>
+      <c r="BG11">
+        <v>2258</v>
+      </c>
     </row>
-    <row r="12" spans="1:58">
+    <row r="12" spans="1:59" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -17838,8 +18215,11 @@
       <c r="BF12">
         <v>58</v>
       </c>
+      <c r="BG12">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:58">
+    <row r="13" spans="1:59">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -17850,7 +18230,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:58">
+    <row r="14" spans="1:59">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -18025,8 +18405,11 @@
       <c r="BF14">
         <v>1540</v>
       </c>
+      <c r="BG14">
+        <v>1531</v>
+      </c>
     </row>
-    <row r="15" spans="1:58">
+    <row r="15" spans="1:59">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -18201,8 +18584,11 @@
       <c r="BF15">
         <v>2336</v>
       </c>
+      <c r="BG15">
+        <v>2349</v>
+      </c>
     </row>
-    <row r="16" spans="1:58">
+    <row r="16" spans="1:59">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -18377,8 +18763,11 @@
       <c r="BF16">
         <v>4955</v>
       </c>
+      <c r="BG16">
+        <v>4980</v>
+      </c>
     </row>
-    <row r="17" spans="1:58">
+    <row r="17" spans="1:59" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -18551,6 +18940,9 @@
         <v>25</v>
       </c>
       <c r="BF17">
+        <v>26</v>
+      </c>
+      <c r="BG17">
         <v>26</v>
       </c>
     </row>
@@ -18562,19 +18954,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BF9"/>
+  <dimension ref="A1:BG9"/>
   <sheetViews>
     <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BF9" sqref="BF9"/>
+      <selection activeCell="BG10" sqref="BG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="2" customFormat="1">
+    <row r="1" spans="1:59" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -18746,14 +19138,17 @@
       <c r="BF1" s="9">
         <v>43982</v>
       </c>
+      <c r="BG1" s="9">
+        <v>43983</v>
+      </c>
     </row>
-    <row r="2" spans="1:58">
+    <row r="2" spans="1:59">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:59">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -18929,8 +19324,11 @@
       <c r="BF3">
         <v>468</v>
       </c>
+      <c r="BG3">
+        <v>470</v>
+      </c>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:59">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -19105,8 +19503,11 @@
       <c r="BF4">
         <v>7</v>
       </c>
+      <c r="BG4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:58" ht="28.8">
+    <row r="5" spans="1:59" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -19281,8 +19682,11 @@
       <c r="BF5">
         <v>351</v>
       </c>
+      <c r="BG5">
+        <v>353</v>
+      </c>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:59">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -19457,8 +19861,11 @@
       <c r="BF6">
         <v>54</v>
       </c>
+      <c r="BG6">
+        <v>52</v>
+      </c>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:59" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -19633,8 +20040,11 @@
       <c r="BF7">
         <v>52</v>
       </c>
+      <c r="BG7">
+        <v>54</v>
+      </c>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:59">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -19809,8 +20219,11 @@
       <c r="BF8">
         <v>3</v>
       </c>
+      <c r="BG8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:59">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -19824,6 +20237,9 @@
         <v>1</v>
       </c>
       <c r="BF9">
+        <v>1</v>
+      </c>
+      <c r="BG9">
         <v>1</v>
       </c>
     </row>
@@ -19834,18 +20250,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AR13"/>
+  <dimension ref="A2:AS13"/>
   <sheetViews>
     <sheetView topLeftCell="AD5" workbookViewId="0">
-      <selection activeCell="AR13" sqref="AR13"/>
+      <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:44" s="2" customFormat="1">
+    <row r="2" spans="1:45" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -19978,8 +20394,11 @@
       <c r="AR2" s="9">
         <v>43982</v>
       </c>
+      <c r="AS2" s="9">
+        <v>43983</v>
+      </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:45">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -20112,8 +20531,11 @@
       <c r="AR3">
         <v>468</v>
       </c>
+      <c r="AS3">
+        <v>470</v>
+      </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:45">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -20246,8 +20668,11 @@
       <c r="AR4">
         <v>48</v>
       </c>
+      <c r="AS4">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:45">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -20380,8 +20805,11 @@
       <c r="AR5">
         <v>29</v>
       </c>
+      <c r="AS5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:45">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -20514,8 +20942,11 @@
       <c r="AR6">
         <v>30</v>
       </c>
+      <c r="AS6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:45">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -20648,8 +21079,11 @@
       <c r="AR7">
         <v>66</v>
       </c>
+      <c r="AS7">
+        <v>66</v>
+      </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:45">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -20782,8 +21216,11 @@
       <c r="AR8">
         <v>75</v>
       </c>
+      <c r="AS8">
+        <v>75</v>
+      </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:45">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -20916,8 +21353,11 @@
       <c r="AR9">
         <v>42</v>
       </c>
+      <c r="AS9">
+        <v>43</v>
+      </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:45">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -21050,8 +21490,11 @@
       <c r="AR10">
         <v>67</v>
       </c>
+      <c r="AS10">
+        <v>68</v>
+      </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:45">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -21184,8 +21627,11 @@
       <c r="AR11">
         <v>95</v>
       </c>
+      <c r="AS11">
+        <v>95</v>
+      </c>
     </row>
-    <row r="12" spans="1:44" ht="28.8">
+    <row r="12" spans="1:45" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -21318,8 +21764,11 @@
       <c r="AR12">
         <v>16</v>
       </c>
+      <c r="AS12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:45">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -21450,6 +21899,9 @@
         <v>0</v>
       </c>
       <c r="AR13">
+        <v>0</v>
+      </c>
+      <c r="AS13">
         <v>0</v>
       </c>
     </row>
@@ -21463,61 +21915,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:N23"/>
+    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6:O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="C1" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+      <c r="C1" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
     </row>
     <row r="4" spans="1:15">
       <c r="C4" s="34"/>
@@ -21571,6 +22023,9 @@
       <c r="N5" s="9">
         <v>43982</v>
       </c>
+      <c r="O5" s="9">
+        <v>43983</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
@@ -21612,6 +22067,9 @@
       <c r="N6">
         <v>119</v>
       </c>
+      <c r="O6">
+        <v>119</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
@@ -21653,6 +22111,9 @@
       <c r="N7">
         <v>31</v>
       </c>
+      <c r="O7">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="35" t="s">
@@ -21702,6 +22163,9 @@
       <c r="N9">
         <v>1</v>
       </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="31" t="s">
@@ -21743,6 +22207,9 @@
       <c r="N10">
         <v>21</v>
       </c>
+      <c r="O10">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="31" t="s">
@@ -21784,6 +22251,9 @@
       <c r="N11">
         <v>7</v>
       </c>
+      <c r="O11">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="31" t="s">
@@ -21825,6 +22295,9 @@
       <c r="N12">
         <v>2</v>
       </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="36" t="s">
@@ -21871,6 +22344,9 @@
       <c r="N14">
         <v>1</v>
       </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="31">
@@ -21912,6 +22388,9 @@
       <c r="N15">
         <v>0</v>
       </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="31">
@@ -21953,8 +22432,11 @@
       <c r="N16">
         <v>3</v>
       </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -21994,8 +22476,11 @@
       <c r="N17">
         <v>9</v>
       </c>
+      <c r="O17">
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -22035,8 +22520,11 @@
       <c r="N18">
         <v>2</v>
       </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -22076,8 +22564,11 @@
       <c r="N19">
         <v>2</v>
       </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -22117,8 +22608,11 @@
       <c r="N20">
         <v>3</v>
       </c>
+      <c r="O20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -22158,8 +22652,11 @@
       <c r="N21">
         <v>6</v>
       </c>
+      <c r="O21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:14" ht="28.8">
+    <row r="22" spans="1:15" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -22199,8 +22696,11 @@
       <c r="N22">
         <v>4</v>
       </c>
+      <c r="O22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:14" ht="28.8">
+    <row r="23" spans="1:15" ht="30">
       <c r="A23" s="39" t="s">
         <v>139</v>
       </c>
@@ -22238,6 +22738,9 @@
         <v>1</v>
       </c>
       <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
         <v>1</v>
       </c>
     </row>
@@ -22253,34 +22756,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A1" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="A1" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="36.6" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -22289,7 +22792,7 @@
       <c r="C2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="46" t="s">
         <v>124</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -22303,10 +22806,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1">
-      <c r="A3" s="44"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="45"/>
+      <c r="D3" s="46"/>
       <c r="E3" s="25" t="s">
         <v>92</v>
       </c>
@@ -22317,11 +22820,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A4" s="44"/>
+    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+      <c r="A4" s="45"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="45"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="25" t="s">
         <v>86</v>
       </c>
@@ -22330,40 +22833,40 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A5" s="44"/>
+    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+      <c r="A5" s="45"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="45"/>
+      <c r="D5" s="46"/>
       <c r="E5" s="25" t="s">
         <v>87</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A6" s="44"/>
+    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+      <c r="A6" s="45"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="45"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A7" s="44"/>
+    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+      <c r="A7" s="45"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="45"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="25" t="s">
         <v>93</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.4" customHeight="1">
+    <row r="8" spans="1:7" ht="14.45" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
@@ -22386,7 +22889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4" customHeight="1">
+    <row r="9" spans="1:7" ht="14.45" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>96</v>
       </c>
@@ -22409,7 +22912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.4" customHeight="1">
+    <row r="10" spans="1:7" ht="14.45" customHeight="1">
       <c r="A10" s="27" t="s">
         <v>98</v>
       </c>
@@ -22432,7 +22935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.4" customHeight="1">
+    <row r="11" spans="1:7" ht="14.45" customHeight="1">
       <c r="A11" s="27" t="s">
         <v>99</v>
       </c>
@@ -22455,7 +22958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.4" customHeight="1">
+    <row r="12" spans="1:7" ht="14.45" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>100</v>
       </c>
@@ -22478,7 +22981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.4" customHeight="1">
+    <row r="13" spans="1:7" ht="14.45" customHeight="1">
       <c r="A13" s="27" t="s">
         <v>143</v>
       </c>
@@ -22501,7 +23004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.4" customHeight="1">
+    <row r="14" spans="1:7" ht="14.45" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>103</v>
       </c>
@@ -22524,7 +23027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.4" customHeight="1">
+    <row r="15" spans="1:7" ht="14.45" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>104</v>
       </c>
@@ -22570,7 +23073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.4" customHeight="1">
+    <row r="17" spans="1:7" ht="14.45" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>107</v>
       </c>
@@ -22593,7 +23096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.4" customHeight="1">
+    <row r="18" spans="1:7" ht="14.45" customHeight="1">
       <c r="A18" s="27" t="s">
         <v>109</v>
       </c>
@@ -22616,7 +23119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.4" customHeight="1">
+    <row r="19" spans="1:7" ht="14.45" customHeight="1">
       <c r="A19" s="27" t="s">
         <v>110</v>
       </c>
@@ -22639,7 +23142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.4" customHeight="1">
+    <row r="20" spans="1:7" ht="14.45" customHeight="1">
       <c r="A20" s="27" t="s">
         <v>111</v>
       </c>
@@ -22662,7 +23165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.4" customHeight="1">
+    <row r="21" spans="1:7" ht="14.45" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>112</v>
       </c>
@@ -22685,7 +23188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.4" customHeight="1">
+    <row r="22" spans="1:7" ht="14.45" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>115</v>
       </c>
@@ -22777,7 +23280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1">
+    <row r="26" spans="1:7" ht="17.45" customHeight="1">
       <c r="A26" s="30" t="s">
         <v>49</v>
       </c>
@@ -22800,7 +23303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.6">
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="24" t="s">
         <v>120</v>
       </c>
@@ -23073,16 +23576,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
03 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D919E9F5-8372-44A9-9972-4EFC8A4CB45B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EB7EFC-D28A-4507-8A65-F65E41983740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="167">
   <si>
     <t>Testing</t>
   </si>
@@ -509,9 +509,6 @@
     <t>34; (25)</t>
   </si>
   <si>
-    <t>197; (79)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -519,9 +516,6 @@
   </si>
   <si>
     <t>660; (291)</t>
-  </si>
-  <si>
-    <t>857; (370)</t>
   </si>
   <si>
     <t>Human Services - CFSA</t>
@@ -533,11 +527,11 @@
     <t>Number of Personnel Currently in Quarantine</t>
   </si>
   <si>
-    <t>As of June 1, 2020</t>
+    <t>As of June 2, 2020</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of June 1, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of June 2, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -560,6 +554,15 @@
       </rPr>
       <t xml:space="preserve"> for COVID-19 testing,  and 31 (26.1%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
+  </si>
+  <si>
+    <t>2; (1)</t>
+  </si>
+  <si>
+    <t>198; (79)</t>
+  </si>
+  <si>
+    <t>858; (370)</t>
   </si>
 </sst>
 </file>
@@ -1193,11 +1196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CK118"/>
+  <dimension ref="A1:CL118"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="CE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CK53" sqref="CK1:CK1048576"/>
+    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="CG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CL103" sqref="CL103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1212,7 +1215,7 @@
     <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89">
+    <row r="1" spans="1:90">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1474,8 +1477,11 @@
       <c r="CK1" s="1">
         <v>43983</v>
       </c>
+      <c r="CL1" s="1">
+        <v>43984</v>
+      </c>
     </row>
-    <row r="2" spans="1:89">
+    <row r="2" spans="1:90">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1499,7 +1505,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:89">
+    <row r="3" spans="1:90">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1746,8 +1752,11 @@
       <c r="CK3">
         <v>47701</v>
       </c>
+      <c r="CL3">
+        <v>49562</v>
+      </c>
     </row>
-    <row r="4" spans="1:89">
+    <row r="4" spans="1:90">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1789,8 +1798,11 @@
       <c r="CK4">
         <v>39251</v>
       </c>
+      <c r="CL4">
+        <v>40751</v>
+      </c>
     </row>
-    <row r="5" spans="1:89">
+    <row r="5" spans="1:90">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2058,8 +2070,11 @@
       <c r="CK5">
         <v>8886</v>
       </c>
+      <c r="CL5">
+        <v>9016</v>
+      </c>
     </row>
-    <row r="6" spans="1:89">
+    <row r="6" spans="1:90">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2309,8 +2324,11 @@
       <c r="CK6">
         <v>470</v>
       </c>
+      <c r="CL6">
+        <v>473</v>
+      </c>
     </row>
-    <row r="7" spans="1:89">
+    <row r="7" spans="1:90">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2530,11 +2548,14 @@
       <c r="CK7">
         <v>1137</v>
       </c>
+      <c r="CL7">
+        <v>1138</v>
+      </c>
     </row>
-    <row r="8" spans="1:89">
+    <row r="8" spans="1:90">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:89">
+    <row r="9" spans="1:90">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2646,8 +2667,11 @@
       <c r="CK9">
         <v>345</v>
       </c>
+      <c r="CL9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:89">
+    <row r="10" spans="1:90">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2861,8 +2885,11 @@
       <c r="CK10">
         <v>76</v>
       </c>
+      <c r="CL10">
+        <v>111</v>
+      </c>
     </row>
-    <row r="11" spans="1:89">
+    <row r="11" spans="1:90">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3076,8 +3103,11 @@
       <c r="CK11">
         <v>440</v>
       </c>
+      <c r="CL11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:89">
+    <row r="12" spans="1:90">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3291,8 +3321,11 @@
       <c r="CK12">
         <v>208</v>
       </c>
+      <c r="CL12">
+        <v>205</v>
+      </c>
     </row>
-    <row r="13" spans="1:89">
+    <row r="13" spans="1:90">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3506,8 +3539,11 @@
       <c r="CK13">
         <v>232</v>
       </c>
+      <c r="CL13">
+        <v>235</v>
+      </c>
     </row>
-    <row r="14" spans="1:89">
+    <row r="14" spans="1:90">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3583,8 +3619,11 @@
       <c r="CK14">
         <v>295</v>
       </c>
+      <c r="CL14">
+        <v>285</v>
+      </c>
     </row>
-    <row r="15" spans="1:89">
+    <row r="15" spans="1:90">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3630,8 +3669,11 @@
       <c r="CK15">
         <v>106</v>
       </c>
+      <c r="CL15">
+        <v>103</v>
+      </c>
     </row>
-    <row r="16" spans="1:89">
+    <row r="16" spans="1:90">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3707,8 +3749,11 @@
       <c r="CK16">
         <v>1887</v>
       </c>
+      <c r="CL16">
+        <v>1914</v>
+      </c>
     </row>
-    <row r="17" spans="1:89">
+    <row r="17" spans="1:90">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3784,13 +3829,16 @@
       <c r="CK17" s="23">
         <v>0.76</v>
       </c>
+      <c r="CL17" s="23">
+        <v>0.77</v>
+      </c>
     </row>
-    <row r="19" spans="1:89">
+    <row r="19" spans="1:90">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:89">
+    <row r="20" spans="1:90">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3798,7 +3846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:89">
+    <row r="21" spans="1:90">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -4015,8 +4063,11 @@
       <c r="CK21">
         <v>111</v>
       </c>
+      <c r="CL21">
+        <v>111</v>
+      </c>
     </row>
-    <row r="22" spans="1:89">
+    <row r="22" spans="1:90">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4179,8 +4230,11 @@
       <c r="CK22">
         <v>19</v>
       </c>
+      <c r="CL22">
+        <v>19</v>
+      </c>
     </row>
-    <row r="23" spans="1:89">
+    <row r="23" spans="1:90">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4343,8 +4397,11 @@
       <c r="CK23">
         <v>92</v>
       </c>
+      <c r="CL23">
+        <v>92</v>
+      </c>
     </row>
-    <row r="24" spans="1:89">
+    <row r="24" spans="1:90">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4552,8 +4609,11 @@
       <c r="CK24">
         <v>105</v>
       </c>
+      <c r="CL24">
+        <v>89</v>
+      </c>
     </row>
-    <row r="25" spans="1:89">
+    <row r="25" spans="1:90">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4761,8 +4821,11 @@
       <c r="CK25">
         <v>124</v>
       </c>
+      <c r="CL25">
+        <v>108</v>
+      </c>
     </row>
-    <row r="26" spans="1:89">
+    <row r="26" spans="1:90">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -4970,13 +5033,16 @@
       <c r="CK26">
         <v>1395</v>
       </c>
+      <c r="CL26">
+        <v>1412</v>
+      </c>
     </row>
-    <row r="28" spans="1:89">
+    <row r="28" spans="1:90">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:89">
+    <row r="29" spans="1:90">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5193,8 +5259,11 @@
       <c r="CK29">
         <v>138</v>
       </c>
+      <c r="CL29">
+        <v>139</v>
+      </c>
     </row>
-    <row r="30" spans="1:89">
+    <row r="30" spans="1:90">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5357,8 +5426,11 @@
       <c r="CK30">
         <v>32</v>
       </c>
+      <c r="CL30">
+        <v>31</v>
+      </c>
     </row>
-    <row r="31" spans="1:89">
+    <row r="31" spans="1:90">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5521,8 +5593,11 @@
       <c r="CK31">
         <v>106</v>
       </c>
+      <c r="CL31">
+        <v>108</v>
+      </c>
     </row>
-    <row r="32" spans="1:89">
+    <row r="32" spans="1:90">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5730,8 +5805,11 @@
       <c r="CK32">
         <v>52</v>
       </c>
+      <c r="CL32">
+        <v>46</v>
+      </c>
     </row>
-    <row r="33" spans="1:89">
+    <row r="33" spans="1:90">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -5939,8 +6017,11 @@
       <c r="CK33">
         <v>84</v>
       </c>
+      <c r="CL33">
+        <v>77</v>
+      </c>
     </row>
-    <row r="34" spans="1:89">
+    <row r="34" spans="1:90">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6148,13 +6229,16 @@
       <c r="CK34">
         <v>1212</v>
       </c>
+      <c r="CL34">
+        <v>1228</v>
+      </c>
     </row>
-    <row r="36" spans="1:89">
+    <row r="36" spans="1:90">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:89">
+    <row r="37" spans="1:90">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -6359,8 +6443,11 @@
       <c r="CK37">
         <v>80</v>
       </c>
+      <c r="CL37">
+        <v>83</v>
+      </c>
     </row>
-    <row r="38" spans="1:89">
+    <row r="38" spans="1:90">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6517,8 +6604,11 @@
       <c r="CK38">
         <v>6</v>
       </c>
+      <c r="CL38">
+        <v>9</v>
+      </c>
     </row>
-    <row r="39" spans="1:89">
+    <row r="39" spans="1:90">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6675,8 +6765,11 @@
       <c r="CK39">
         <v>73</v>
       </c>
+      <c r="CL39">
+        <v>73</v>
+      </c>
     </row>
-    <row r="40" spans="1:89">
+    <row r="40" spans="1:90">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6878,8 +6971,11 @@
       <c r="CK40">
         <v>1</v>
       </c>
+      <c r="CL40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:89">
+    <row r="41" spans="1:90">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -7078,8 +7174,11 @@
       <c r="CK41">
         <v>9</v>
       </c>
+      <c r="CL41">
+        <v>10</v>
+      </c>
     </row>
-    <row r="42" spans="1:89">
+    <row r="42" spans="1:90">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7284,8 +7383,11 @@
       <c r="CK42">
         <v>281</v>
       </c>
+      <c r="CL42">
+        <v>281</v>
+      </c>
     </row>
-    <row r="43" spans="1:89">
+    <row r="43" spans="1:90">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -7424,16 +7526,19 @@
       <c r="CK43">
         <v>1</v>
       </c>
+      <c r="CL43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:89">
+    <row r="44" spans="1:90">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:89">
+    <row r="45" spans="1:90">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:89">
+    <row r="46" spans="1:90">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -7644,8 +7749,11 @@
       <c r="CK46">
         <v>205</v>
       </c>
+      <c r="CL46">
+        <v>206</v>
+      </c>
     </row>
-    <row r="47" spans="1:89">
+    <row r="47" spans="1:90">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7808,8 +7916,11 @@
       <c r="CK47">
         <v>18</v>
       </c>
+      <c r="CL47">
+        <v>16</v>
+      </c>
     </row>
-    <row r="48" spans="1:89">
+    <row r="48" spans="1:90">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -7972,8 +8083,11 @@
       <c r="CK48">
         <v>181</v>
       </c>
+      <c r="CL48">
+        <v>183</v>
+      </c>
     </row>
-    <row r="49" spans="1:89">
+    <row r="49" spans="1:90">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -8181,8 +8295,11 @@
       <c r="CK49">
         <v>469</v>
       </c>
+      <c r="CL49">
+        <v>396</v>
+      </c>
     </row>
-    <row r="50" spans="1:89">
+    <row r="50" spans="1:90">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -8345,8 +8462,11 @@
       <c r="CK50">
         <v>487</v>
       </c>
+      <c r="CL50">
+        <v>412</v>
+      </c>
     </row>
-    <row r="51" spans="1:89">
+    <row r="51" spans="1:90">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -8506,8 +8626,11 @@
       <c r="CK51">
         <v>830</v>
       </c>
+      <c r="CL51">
+        <v>729</v>
+      </c>
     </row>
-    <row r="52" spans="1:89">
+    <row r="52" spans="1:90">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -8661,16 +8784,19 @@
       <c r="CK52">
         <v>1</v>
       </c>
+      <c r="CL52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:89">
+    <row r="53" spans="1:90">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:89">
+    <row r="54" spans="1:90">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:89">
+    <row r="55" spans="1:90">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -8866,8 +8992,11 @@
       <c r="CK55">
         <v>30</v>
       </c>
+      <c r="CL55">
+        <v>30</v>
+      </c>
     </row>
-    <row r="56" spans="1:89">
+    <row r="56" spans="1:90">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -9027,8 +9156,11 @@
       <c r="CK56">
         <v>7</v>
       </c>
+      <c r="CL56">
+        <v>8</v>
+      </c>
     </row>
-    <row r="57" spans="1:89">
+    <row r="57" spans="1:90">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -9188,8 +9320,11 @@
       <c r="CK57">
         <v>22</v>
       </c>
+      <c r="CL57">
+        <v>22</v>
+      </c>
     </row>
-    <row r="58" spans="1:89">
+    <row r="58" spans="1:90">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -9385,8 +9520,11 @@
       <c r="CK58">
         <v>16</v>
       </c>
+      <c r="CL58">
+        <v>15</v>
+      </c>
     </row>
-    <row r="59" spans="1:89">
+    <row r="59" spans="1:90">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -9582,8 +9720,11 @@
       <c r="CK59">
         <v>23</v>
       </c>
+      <c r="CL59">
+        <v>23</v>
+      </c>
     </row>
-    <row r="60" spans="1:89">
+    <row r="60" spans="1:90">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -9779,8 +9920,11 @@
       <c r="CK60">
         <v>145</v>
       </c>
+      <c r="CL60">
+        <v>147</v>
+      </c>
     </row>
-    <row r="61" spans="1:89">
+    <row r="61" spans="1:90">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -9934,8 +10078,11 @@
       <c r="CK61">
         <v>1</v>
       </c>
+      <c r="CL61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:89">
+    <row r="63" spans="1:90">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -10131,8 +10278,11 @@
       <c r="CK63">
         <v>11</v>
       </c>
+      <c r="CL63">
+        <v>11</v>
+      </c>
     </row>
-    <row r="64" spans="1:89">
+    <row r="64" spans="1:90">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -10292,8 +10442,11 @@
       <c r="CK64">
         <v>2</v>
       </c>
+      <c r="CL64">
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:89">
+    <row r="65" spans="1:90">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -10453,8 +10606,11 @@
       <c r="CK65">
         <v>9</v>
       </c>
+      <c r="CL65">
+        <v>9</v>
+      </c>
     </row>
-    <row r="66" spans="1:89">
+    <row r="66" spans="1:90">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -10650,8 +10806,11 @@
       <c r="CK66">
         <v>54</v>
       </c>
+      <c r="CL66">
+        <v>56</v>
+      </c>
     </row>
-    <row r="67" spans="1:89">
+    <row r="67" spans="1:90">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -10848,8 +11007,11 @@
       <c r="CK67">
         <v>56</v>
       </c>
+      <c r="CL67">
+        <v>58</v>
+      </c>
     </row>
-    <row r="68" spans="1:89">
+    <row r="68" spans="1:90">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -11045,8 +11207,11 @@
       <c r="CK68">
         <v>0</v>
       </c>
+      <c r="CL68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:89">
+    <row r="69" spans="1:90">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -11206,11 +11371,14 @@
       <c r="CK69">
         <v>0</v>
       </c>
+      <c r="CL69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:89">
+    <row r="70" spans="1:90">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:89">
+    <row r="71" spans="1:90">
       <c r="A71" s="2" t="s">
         <v>132</v>
       </c>
@@ -11256,8 +11424,11 @@
       <c r="CK71">
         <v>10</v>
       </c>
+      <c r="CL71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:89">
+    <row r="72" spans="1:90">
       <c r="A72" s="2" t="s">
         <v>132</v>
       </c>
@@ -11303,8 +11474,11 @@
       <c r="CK72">
         <v>5</v>
       </c>
+      <c r="CL72">
+        <v>5</v>
+      </c>
     </row>
-    <row r="73" spans="1:89">
+    <row r="73" spans="1:90">
       <c r="A73" s="2" t="s">
         <v>132</v>
       </c>
@@ -11350,8 +11524,11 @@
       <c r="CK73">
         <v>5</v>
       </c>
+      <c r="CL73">
+        <v>5</v>
+      </c>
     </row>
-    <row r="74" spans="1:89">
+    <row r="74" spans="1:90">
       <c r="A74" s="2" t="s">
         <v>132</v>
       </c>
@@ -11397,8 +11574,11 @@
       <c r="CK74">
         <v>8</v>
       </c>
+      <c r="CL74">
+        <v>8</v>
+      </c>
     </row>
-    <row r="75" spans="1:89">
+    <row r="75" spans="1:90">
       <c r="A75" s="2" t="s">
         <v>132</v>
       </c>
@@ -11444,8 +11624,11 @@
       <c r="CK75">
         <v>13</v>
       </c>
+      <c r="CL75">
+        <v>13</v>
+      </c>
     </row>
-    <row r="76" spans="1:89">
+    <row r="76" spans="1:90">
       <c r="A76" s="2" t="s">
         <v>132</v>
       </c>
@@ -11491,13 +11674,16 @@
       <c r="CK76">
         <v>33</v>
       </c>
+      <c r="CL76">
+        <v>34</v>
+      </c>
     </row>
-    <row r="78" spans="1:89">
+    <row r="78" spans="1:90">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:89">
+    <row r="79" spans="1:90">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -11693,8 +11879,11 @@
       <c r="CK79">
         <v>298</v>
       </c>
+      <c r="CL79">
+        <v>302</v>
+      </c>
     </row>
-    <row r="80" spans="1:89">
+    <row r="80" spans="1:90">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -11890,8 +12079,11 @@
       <c r="CK80">
         <v>104</v>
       </c>
+      <c r="CL80">
+        <v>105</v>
+      </c>
     </row>
-    <row r="81" spans="1:89">
+    <row r="81" spans="1:90">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -12087,8 +12279,11 @@
       <c r="CK81">
         <v>84</v>
       </c>
+      <c r="CL81">
+        <v>84</v>
+      </c>
     </row>
-    <row r="82" spans="1:89">
+    <row r="82" spans="1:90">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -12242,8 +12437,11 @@
       <c r="CK82">
         <v>16</v>
       </c>
+      <c r="CL82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:89">
+    <row r="84" spans="1:90">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -12439,8 +12637,11 @@
       <c r="CK84">
         <v>119</v>
       </c>
+      <c r="CL84">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:89">
+    <row r="85" spans="1:90">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -12636,8 +12837,11 @@
       <c r="CK85">
         <v>25</v>
       </c>
+      <c r="CL85">
+        <v>25</v>
+      </c>
     </row>
-    <row r="86" spans="1:89">
+    <row r="86" spans="1:90">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -12833,8 +13037,11 @@
       <c r="CK86">
         <v>144</v>
       </c>
+      <c r="CL86">
+        <v>68</v>
+      </c>
     </row>
-    <row r="87" spans="1:89">
+    <row r="87" spans="1:90">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -13030,8 +13237,11 @@
       <c r="CK87">
         <v>194</v>
       </c>
+      <c r="CL87">
+        <v>195</v>
+      </c>
     </row>
-    <row r="88" spans="1:89">
+    <row r="88" spans="1:90">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -13101,8 +13311,11 @@
       <c r="CK88">
         <v>1</v>
       </c>
+      <c r="CL88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:89">
+    <row r="90" spans="1:90">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -13298,8 +13511,11 @@
       <c r="CK90">
         <v>81</v>
       </c>
+      <c r="CL90">
+        <v>81</v>
+      </c>
     </row>
-    <row r="91" spans="1:89">
+    <row r="91" spans="1:90">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -13495,8 +13711,11 @@
       <c r="CK91">
         <v>21</v>
       </c>
+      <c r="CL91">
+        <v>21</v>
+      </c>
     </row>
-    <row r="92" spans="1:89">
+    <row r="92" spans="1:90">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -13680,8 +13899,11 @@
       <c r="CK92">
         <v>168</v>
       </c>
+      <c r="CL92">
+        <v>168</v>
+      </c>
     </row>
-    <row r="93" spans="1:89">
+    <row r="93" spans="1:90">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -13877,8 +14099,11 @@
       <c r="CK93">
         <v>41</v>
       </c>
+      <c r="CL93">
+        <v>43</v>
+      </c>
     </row>
-    <row r="94" spans="1:89">
+    <row r="94" spans="1:90">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -14032,16 +14257,19 @@
       <c r="CK94">
         <v>13</v>
       </c>
+      <c r="CL94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:89">
+    <row r="95" spans="1:90">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:89">
+    <row r="96" spans="1:90">
       <c r="A96" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B96" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="CG96">
         <v>9</v>
@@ -14049,13 +14277,16 @@
       <c r="CK96">
         <v>9</v>
       </c>
+      <c r="CL96">
+        <v>9</v>
+      </c>
     </row>
-    <row r="97" spans="1:89">
+    <row r="97" spans="1:90">
       <c r="A97" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B97" s="20" t="s">
         <v>161</v>
-      </c>
-      <c r="B97" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="CG97">
         <v>17</v>
@@ -14063,10 +14294,13 @@
       <c r="CK97">
         <v>12</v>
       </c>
+      <c r="CL97">
+        <v>12</v>
+      </c>
     </row>
-    <row r="98" spans="1:89">
+    <row r="98" spans="1:90">
       <c r="A98" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B98" s="41" t="s">
         <v>12</v>
@@ -14077,10 +14311,13 @@
       <c r="CK98">
         <v>35</v>
       </c>
+      <c r="CL98">
+        <v>35</v>
+      </c>
     </row>
-    <row r="99" spans="1:89">
+    <row r="99" spans="1:90">
       <c r="A99" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B99" s="41" t="s">
         <v>84</v>
@@ -14091,8 +14328,11 @@
       <c r="CK99">
         <v>1</v>
       </c>
+      <c r="CL99">
+        <v>1</v>
+      </c>
     </row>
-    <row r="101" spans="1:89">
+    <row r="101" spans="1:90">
       <c r="A101" s="2" t="s">
         <v>79</v>
       </c>
@@ -14207,8 +14447,11 @@
       <c r="CK101">
         <v>188</v>
       </c>
+      <c r="CL101">
+        <v>189</v>
+      </c>
     </row>
-    <row r="102" spans="1:89">
+    <row r="102" spans="1:90">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -14323,8 +14566,11 @@
       <c r="CK102">
         <v>70</v>
       </c>
+      <c r="CL102">
+        <v>77</v>
+      </c>
     </row>
-    <row r="103" spans="1:89">
+    <row r="103" spans="1:90">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -14437,6 +14683,9 @@
         <v>25</v>
       </c>
       <c r="CK103">
+        <v>25</v>
+      </c>
+      <c r="CL103">
         <v>25</v>
       </c>
     </row>
@@ -14453,10 +14702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BL11"/>
+  <dimension ref="A2:BM11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BL11" sqref="BL3:BL11"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BM11" sqref="BM3:BM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14466,7 +14715,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:64" s="2" customFormat="1">
+    <row r="2" spans="1:65" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -14659,8 +14908,11 @@
       <c r="BL2" s="9">
         <v>43983</v>
       </c>
+      <c r="BM2" s="9">
+        <v>43984</v>
+      </c>
     </row>
-    <row r="3" spans="1:64">
+    <row r="3" spans="1:65">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -14853,8 +15105,11 @@
       <c r="BL3">
         <v>1243</v>
       </c>
+      <c r="BM3">
+        <v>1243</v>
+      </c>
     </row>
-    <row r="4" spans="1:64">
+    <row r="4" spans="1:65">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -15047,8 +15302,11 @@
       <c r="BL4">
         <v>513</v>
       </c>
+      <c r="BM4">
+        <v>513</v>
+      </c>
     </row>
-    <row r="5" spans="1:64">
+    <row r="5" spans="1:65">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -15241,8 +15499,11 @@
       <c r="BL5">
         <v>420</v>
       </c>
+      <c r="BM5">
+        <v>420</v>
+      </c>
     </row>
-    <row r="6" spans="1:64">
+    <row r="6" spans="1:65">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -15435,8 +15696,11 @@
       <c r="BL6">
         <v>1852</v>
       </c>
+      <c r="BM6">
+        <v>1852</v>
+      </c>
     </row>
-    <row r="7" spans="1:64">
+    <row r="7" spans="1:65">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -15629,8 +15893,11 @@
       <c r="BL7">
         <v>1379</v>
       </c>
+      <c r="BM7">
+        <v>1379</v>
+      </c>
     </row>
-    <row r="8" spans="1:64">
+    <row r="8" spans="1:65">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -15823,8 +16090,11 @@
       <c r="BL8">
         <v>758</v>
       </c>
+      <c r="BM8">
+        <v>758</v>
+      </c>
     </row>
-    <row r="9" spans="1:64">
+    <row r="9" spans="1:65">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -16017,8 +16287,11 @@
       <c r="BL9">
         <v>1298</v>
       </c>
+      <c r="BM9">
+        <v>1298</v>
+      </c>
     </row>
-    <row r="10" spans="1:64">
+    <row r="10" spans="1:65">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -16211,8 +16484,11 @@
       <c r="BL10">
         <v>1278</v>
       </c>
+      <c r="BM10">
+        <v>1278</v>
+      </c>
     </row>
-    <row r="11" spans="1:64">
+    <row r="11" spans="1:65">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -16403,6 +16679,9 @@
         <v>143</v>
       </c>
       <c r="BL11">
+        <v>145</v>
+      </c>
+      <c r="BM11">
         <v>145</v>
       </c>
     </row>
@@ -16414,10 +16693,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BG17"/>
+  <dimension ref="A2:BH17"/>
   <sheetViews>
     <sheetView topLeftCell="AO8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BG17" sqref="BG17"/>
+      <selection activeCell="BH17" sqref="BH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16427,7 +16706,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:59" s="2" customFormat="1">
+    <row r="2" spans="1:60" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -16603,8 +16882,11 @@
       <c r="BG2" s="9">
         <v>43983</v>
       </c>
+      <c r="BH2" s="9">
+        <v>43984</v>
+      </c>
     </row>
-    <row r="3" spans="1:59" s="2" customFormat="1">
+    <row r="3" spans="1:60" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -16612,7 +16894,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:60">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -16790,8 +17072,11 @@
       <c r="BG4">
         <v>8886</v>
       </c>
+      <c r="BH4">
+        <v>9016</v>
+      </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="1:60">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -16969,8 +17254,11 @@
       <c r="BG5">
         <v>916</v>
       </c>
+      <c r="BH5">
+        <v>995</v>
+      </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:60">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -17148,8 +17436,11 @@
       <c r="BG6">
         <v>1358</v>
       </c>
+      <c r="BH6">
+        <v>1364</v>
+      </c>
     </row>
-    <row r="7" spans="1:59">
+    <row r="7" spans="1:60">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -17327,8 +17618,11 @@
       <c r="BG7">
         <v>4142</v>
       </c>
+      <c r="BH7">
+        <v>4164</v>
+      </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="1:60">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -17506,8 +17800,11 @@
       <c r="BG8">
         <v>106</v>
       </c>
+      <c r="BH8">
+        <v>106</v>
+      </c>
     </row>
-    <row r="9" spans="1:59" ht="30">
+    <row r="9" spans="1:60" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -17685,8 +17982,11 @@
       <c r="BG9">
         <v>26</v>
       </c>
+      <c r="BH9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:59" ht="30">
+    <row r="10" spans="1:60" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -17860,8 +18160,11 @@
       <c r="BG10">
         <v>22</v>
       </c>
+      <c r="BH10">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:59">
+    <row r="11" spans="1:60">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -18039,8 +18342,11 @@
       <c r="BG11">
         <v>2258</v>
       </c>
+      <c r="BH11">
+        <v>2281</v>
+      </c>
     </row>
-    <row r="12" spans="1:59" ht="30">
+    <row r="12" spans="1:60" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -18218,8 +18524,11 @@
       <c r="BG12">
         <v>58</v>
       </c>
+      <c r="BH12">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:59">
+    <row r="13" spans="1:60">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -18230,7 +18539,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:59">
+    <row r="14" spans="1:60">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -18408,8 +18717,11 @@
       <c r="BG14">
         <v>1531</v>
       </c>
+      <c r="BH14">
+        <v>1608</v>
+      </c>
     </row>
-    <row r="15" spans="1:59">
+    <row r="15" spans="1:60">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -18587,8 +18899,11 @@
       <c r="BG15">
         <v>2349</v>
       </c>
+      <c r="BH15">
+        <v>2372</v>
+      </c>
     </row>
-    <row r="16" spans="1:59">
+    <row r="16" spans="1:60">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -18766,8 +19081,11 @@
       <c r="BG16">
         <v>4980</v>
       </c>
+      <c r="BH16">
+        <v>5010</v>
+      </c>
     </row>
-    <row r="17" spans="1:59" ht="30">
+    <row r="17" spans="1:60" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -18943,6 +19261,9 @@
         <v>26</v>
       </c>
       <c r="BG17">
+        <v>26</v>
+      </c>
+      <c r="BH17">
         <v>26</v>
       </c>
     </row>
@@ -18954,10 +19275,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BG9"/>
+  <dimension ref="A1:BH9"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BG10" sqref="BG10"/>
+    <sheetView topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="BH8" sqref="BH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18966,7 +19287,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="2" customFormat="1">
+    <row r="1" spans="1:60" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -19141,14 +19462,17 @@
       <c r="BG1" s="9">
         <v>43983</v>
       </c>
+      <c r="BH1" s="9">
+        <v>43984</v>
+      </c>
     </row>
-    <row r="2" spans="1:59">
+    <row r="2" spans="1:60">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:59">
+    <row r="3" spans="1:60">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -19327,8 +19651,11 @@
       <c r="BG3">
         <v>470</v>
       </c>
+      <c r="BH3">
+        <v>473</v>
+      </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:60">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -19506,8 +19833,11 @@
       <c r="BG4">
         <v>7</v>
       </c>
+      <c r="BH4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:59" ht="30">
+    <row r="5" spans="1:60" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -19685,8 +20015,11 @@
       <c r="BG5">
         <v>353</v>
       </c>
+      <c r="BH5">
+        <v>356</v>
+      </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:60">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -19864,8 +20197,11 @@
       <c r="BG6">
         <v>52</v>
       </c>
+      <c r="BH6">
+        <v>54</v>
+      </c>
     </row>
-    <row r="7" spans="1:59" ht="30">
+    <row r="7" spans="1:60" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -20043,8 +20379,11 @@
       <c r="BG7">
         <v>54</v>
       </c>
+      <c r="BH7">
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="1:60">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -20222,8 +20561,11 @@
       <c r="BG8">
         <v>3</v>
       </c>
+      <c r="BH8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:59">
+    <row r="9" spans="1:60">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -20250,10 +20592,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AS13"/>
+  <dimension ref="A2:AT13"/>
   <sheetViews>
     <sheetView topLeftCell="AD5" workbookViewId="0">
-      <selection activeCell="AS13" sqref="AS13"/>
+      <selection activeCell="AT13" sqref="AT13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20261,7 +20603,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:45" s="2" customFormat="1">
+    <row r="2" spans="1:46" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -20397,8 +20739,11 @@
       <c r="AS2" s="9">
         <v>43983</v>
       </c>
+      <c r="AT2" s="9">
+        <v>43984</v>
+      </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:46">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -20534,8 +20879,11 @@
       <c r="AS3">
         <v>470</v>
       </c>
+      <c r="AT3">
+        <v>473</v>
+      </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:46">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -20671,8 +21019,11 @@
       <c r="AS4">
         <v>48</v>
       </c>
+      <c r="AT4">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:46">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -20808,8 +21159,11 @@
       <c r="AS5">
         <v>29</v>
       </c>
+      <c r="AT5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:46">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -20945,8 +21299,11 @@
       <c r="AS6">
         <v>30</v>
       </c>
+      <c r="AT6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:46">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -21082,8 +21439,11 @@
       <c r="AS7">
         <v>66</v>
       </c>
+      <c r="AT7">
+        <v>66</v>
+      </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:46">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -21219,8 +21579,11 @@
       <c r="AS8">
         <v>75</v>
       </c>
+      <c r="AT8">
+        <v>75</v>
+      </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:46">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -21356,8 +21719,11 @@
       <c r="AS9">
         <v>43</v>
       </c>
+      <c r="AT9">
+        <v>43</v>
+      </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:46">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -21493,8 +21859,11 @@
       <c r="AS10">
         <v>68</v>
       </c>
+      <c r="AT10">
+        <v>69</v>
+      </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:46">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -21630,8 +21999,11 @@
       <c r="AS11">
         <v>95</v>
       </c>
+      <c r="AT11">
+        <v>97</v>
+      </c>
     </row>
-    <row r="12" spans="1:45" ht="30">
+    <row r="12" spans="1:46" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -21767,8 +22139,11 @@
       <c r="AS12">
         <v>16</v>
       </c>
+      <c r="AT12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:46">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -21902,6 +22277,9 @@
         <v>0</v>
       </c>
       <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13">
         <v>0</v>
       </c>
     </row>
@@ -21913,10 +22291,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6:O23"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21924,9 +22302,9 @@
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="C1" s="42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
@@ -21941,7 +22319,7 @@
       <c r="N1" s="42"/>
       <c r="O1" s="42"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
@@ -21956,7 +22334,7 @@
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -21971,7 +22349,7 @@
       <c r="N3" s="42"/>
       <c r="O3" s="42"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -21986,7 +22364,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -22026,8 +22404,11 @@
       <c r="O5" s="9">
         <v>43983</v>
       </c>
+      <c r="P5" s="9">
+        <v>43984</v>
+      </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
         <v>136</v>
       </c>
@@ -22070,8 +22451,11 @@
       <c r="O6">
         <v>119</v>
       </c>
+      <c r="P6">
+        <v>119</v>
+      </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -22114,16 +22498,19 @@
       <c r="O7">
         <v>31</v>
       </c>
+      <c r="P7">
+        <v>31</v>
+      </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -22166,8 +22553,11 @@
       <c r="O9">
         <v>1</v>
       </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" s="31" t="s">
         <v>137</v>
       </c>
@@ -22210,8 +22600,11 @@
       <c r="O10">
         <v>21</v>
       </c>
+      <c r="P10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" s="31" t="s">
         <v>138</v>
       </c>
@@ -22254,8 +22647,11 @@
       <c r="O11">
         <v>7</v>
       </c>
+      <c r="P11">
+        <v>7</v>
+      </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -22298,13 +22694,16 @@
       <c r="O12">
         <v>2</v>
       </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -22347,8 +22746,11 @@
       <c r="O14">
         <v>1</v>
       </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -22391,8 +22793,11 @@
       <c r="O15">
         <v>0</v>
       </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -22435,8 +22840,11 @@
       <c r="O16">
         <v>3</v>
       </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:16">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -22479,8 +22887,11 @@
       <c r="O17">
         <v>9</v>
       </c>
+      <c r="P17">
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:16">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -22523,8 +22934,11 @@
       <c r="O18">
         <v>2</v>
       </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:16">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -22567,8 +22981,11 @@
       <c r="O19">
         <v>2</v>
       </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:16">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -22611,8 +23028,11 @@
       <c r="O20">
         <v>3</v>
       </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:16">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -22655,8 +23075,11 @@
       <c r="O21">
         <v>6</v>
       </c>
+      <c r="P21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:15" ht="45">
+    <row r="22" spans="1:16" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -22699,8 +23122,11 @@
       <c r="O22">
         <v>4</v>
       </c>
+      <c r="P22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:15" ht="30">
+    <row r="23" spans="1:16" ht="30">
       <c r="A23" s="39" t="s">
         <v>139</v>
       </c>
@@ -22741,6 +23167,9 @@
         <v>1</v>
       </c>
       <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
         <v>1</v>
       </c>
     </row>
@@ -22756,7 +23185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -22773,7 +23202,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -22995,7 +23424,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>101</v>
+        <v>164</v>
       </c>
       <c r="F13" s="28">
         <v>0</v>
@@ -23193,10 +23622,10 @@
         <v>115</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22" s="28">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22" s="28">
         <v>0</v>
@@ -23285,16 +23714,16 @@
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C26" s="28">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D26" s="28">
         <v>0</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="F26" s="28">
         <v>5</v>
@@ -23308,7 +23737,7 @@
         <v>120</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>

</xml_diff>

<commit_message>
06 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EB7EFC-D28A-4507-8A65-F65E41983740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46711E8-F5F3-4404-8D88-FB7327D8A01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,12 +356,6 @@
     <t>Inspire (Bed Capacity: 180)</t>
   </si>
   <si>
-    <t>20; (11)</t>
-  </si>
-  <si>
-    <t>9; (1)</t>
-  </si>
-  <si>
     <t>Knollwood (Bed Capacity: 73)</t>
   </si>
   <si>
@@ -428,9 +422,6 @@
     <t>Personnel Recovered:</t>
   </si>
   <si>
-    <t>79; (49)</t>
-  </si>
-  <si>
     <t>25; (14)</t>
   </si>
   <si>
@@ -444,9 +435,6 @@
   </si>
   <si>
     <t>23; (8)</t>
-  </si>
-  <si>
-    <t>21; (17)</t>
   </si>
   <si>
     <t>Total Submitted for Testing</t>
@@ -465,9 +453,6 @@
   </si>
   <si>
     <t>Cleared From Isolation</t>
-  </si>
-  <si>
-    <t>55; (20)</t>
   </si>
   <si>
     <t>Hospital for Sick Children LTC</t>
@@ -494,16 +479,10 @@
     <t>58; (33)</t>
   </si>
   <si>
-    <t>45; (29)</t>
-  </si>
-  <si>
     <t>16; (8)</t>
   </si>
   <si>
     <t>3; (0)</t>
-  </si>
-  <si>
-    <t>99; (51)</t>
   </si>
   <si>
     <t>34; (25)</t>
@@ -515,9 +494,6 @@
     <t>152; (46)</t>
   </si>
   <si>
-    <t>660; (291)</t>
-  </si>
-  <si>
     <t>Human Services - CFSA</t>
   </si>
   <si>
@@ -527,11 +503,44 @@
     <t>Number of Personnel Currently in Quarantine</t>
   </si>
   <si>
-    <t>As of June 2, 2020</t>
+    <t>2; (1)</t>
+  </si>
+  <si>
+    <t>64; (20)</t>
+  </si>
+  <si>
+    <t>21; (10)</t>
+  </si>
+  <si>
+    <t>10; (2)</t>
+  </si>
+  <si>
+    <t>44; (29)</t>
+  </si>
+  <si>
+    <t>26; (18)</t>
+  </si>
+  <si>
+    <t>204; (81)</t>
+  </si>
+  <si>
+    <t>As of June 5, 2020</t>
+  </si>
+  <si>
+    <t>100; (51)</t>
+  </si>
+  <si>
+    <t>81; (51)</t>
+  </si>
+  <si>
+    <t>672; (292)</t>
+  </si>
+  <si>
+    <t>876; (373)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of June 2, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of June 5, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -542,7 +551,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>119 cases</t>
+      <t>124 cases</t>
     </r>
     <r>
       <rPr>
@@ -552,17 +561,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> for COVID-19 testing,  and 31 (26.1%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
+      <t xml:space="preserve"> for COVID-19 testing,  and 34 (27.4%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
-  </si>
-  <si>
-    <t>2; (1)</t>
-  </si>
-  <si>
-    <t>198; (79)</t>
-  </si>
-  <si>
-    <t>858; (370)</t>
   </si>
 </sst>
 </file>
@@ -1196,11 +1196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CL118"/>
+  <dimension ref="A1:CO118"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="CG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CL103" sqref="CL103"/>
+      <selection pane="topRight" activeCell="CO82" sqref="CO82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1215,7 +1215,7 @@
     <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90">
+    <row r="1" spans="1:93">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1480,8 +1480,17 @@
       <c r="CL1" s="1">
         <v>43984</v>
       </c>
+      <c r="CM1" s="1">
+        <v>43985</v>
+      </c>
+      <c r="CN1" s="1">
+        <v>43986</v>
+      </c>
+      <c r="CO1" s="1">
+        <v>43987</v>
+      </c>
     </row>
-    <row r="2" spans="1:90">
+    <row r="2" spans="1:93">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1505,12 +1514,12 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:90">
+    <row r="3" spans="1:93">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I3">
         <v>69</v>
@@ -1755,13 +1764,22 @@
       <c r="CL3">
         <v>49562</v>
       </c>
+      <c r="CM3">
+        <v>51096</v>
+      </c>
+      <c r="CN3">
+        <v>51861</v>
+      </c>
+      <c r="CO3">
+        <v>53678</v>
+      </c>
     </row>
-    <row r="4" spans="1:90">
+    <row r="4" spans="1:93">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="AN4" s="19"/>
       <c r="AO4" s="20"/>
@@ -1801,8 +1819,17 @@
       <c r="CL4">
         <v>40751</v>
       </c>
+      <c r="CM4">
+        <v>41571</v>
+      </c>
+      <c r="CN4">
+        <v>41800</v>
+      </c>
+      <c r="CO4">
+        <v>43528</v>
+      </c>
     </row>
-    <row r="5" spans="1:90">
+    <row r="5" spans="1:93">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2073,8 +2100,17 @@
       <c r="CL5">
         <v>9016</v>
       </c>
+      <c r="CM5">
+        <v>9120</v>
+      </c>
+      <c r="CN5">
+        <v>9199</v>
+      </c>
+      <c r="CO5">
+        <v>9269</v>
+      </c>
     </row>
-    <row r="6" spans="1:90">
+    <row r="6" spans="1:93">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2327,13 +2363,22 @@
       <c r="CL6">
         <v>473</v>
       </c>
+      <c r="CM6">
+        <v>475</v>
+      </c>
+      <c r="CN6">
+        <v>475</v>
+      </c>
+      <c r="CO6">
+        <v>483</v>
+      </c>
     </row>
-    <row r="7" spans="1:90">
+    <row r="7" spans="1:93">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="S7">
         <v>17</v>
@@ -2551,11 +2596,20 @@
       <c r="CL7">
         <v>1138</v>
       </c>
+      <c r="CM7">
+        <v>1138</v>
+      </c>
+      <c r="CN7">
+        <v>1138</v>
+      </c>
+      <c r="CO7">
+        <v>1138</v>
+      </c>
     </row>
-    <row r="8" spans="1:90">
+    <row r="8" spans="1:93">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:90">
+    <row r="9" spans="1:93">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2670,8 +2724,17 @@
       <c r="CL9">
         <v>345</v>
       </c>
+      <c r="CM9">
+        <v>345</v>
+      </c>
+      <c r="CN9">
+        <v>345</v>
+      </c>
+      <c r="CO9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:90">
+    <row r="10" spans="1:93">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2888,8 +2951,17 @@
       <c r="CL10">
         <v>111</v>
       </c>
+      <c r="CM10">
+        <v>57</v>
+      </c>
+      <c r="CN10">
+        <v>58</v>
+      </c>
+      <c r="CO10">
+        <v>66</v>
+      </c>
     </row>
-    <row r="11" spans="1:90">
+    <row r="11" spans="1:93">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3106,8 +3178,17 @@
       <c r="CL11">
         <v>440</v>
       </c>
+      <c r="CM11">
+        <v>440</v>
+      </c>
+      <c r="CN11">
+        <v>440</v>
+      </c>
+      <c r="CO11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:90">
+    <row r="12" spans="1:93">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3324,8 +3405,17 @@
       <c r="CL12">
         <v>205</v>
       </c>
+      <c r="CM12">
+        <v>218</v>
+      </c>
+      <c r="CN12">
+        <v>205</v>
+      </c>
+      <c r="CO12">
+        <v>212</v>
+      </c>
     </row>
-    <row r="13" spans="1:90">
+    <row r="13" spans="1:93">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3542,8 +3632,17 @@
       <c r="CL13">
         <v>235</v>
       </c>
+      <c r="CM13">
+        <v>222</v>
+      </c>
+      <c r="CN13">
+        <v>235</v>
+      </c>
+      <c r="CO13">
+        <v>228</v>
+      </c>
     </row>
-    <row r="14" spans="1:90">
+    <row r="14" spans="1:93">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3622,13 +3721,22 @@
       <c r="CL14">
         <v>285</v>
       </c>
+      <c r="CM14">
+        <v>276</v>
+      </c>
+      <c r="CN14">
+        <v>273</v>
+      </c>
+      <c r="CO14">
+        <v>276</v>
+      </c>
     </row>
-    <row r="15" spans="1:90">
+    <row r="15" spans="1:93">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="BY15">
         <v>110</v>
@@ -3672,8 +3780,17 @@
       <c r="CL15">
         <v>103</v>
       </c>
+      <c r="CM15">
+        <v>98</v>
+      </c>
+      <c r="CN15">
+        <v>99</v>
+      </c>
+      <c r="CO15">
+        <v>100</v>
+      </c>
     </row>
-    <row r="16" spans="1:90">
+    <row r="16" spans="1:93">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3752,8 +3869,17 @@
       <c r="CL16">
         <v>1914</v>
       </c>
+      <c r="CM16">
+        <v>1928</v>
+      </c>
+      <c r="CN16">
+        <v>1960</v>
+      </c>
+      <c r="CO16">
+        <v>1985</v>
+      </c>
     </row>
-    <row r="17" spans="1:90">
+    <row r="17" spans="1:93">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3832,13 +3958,22 @@
       <c r="CL17" s="23">
         <v>0.77</v>
       </c>
+      <c r="CM17" s="23">
+        <v>0.78</v>
+      </c>
+      <c r="CN17" s="23">
+        <v>0.79</v>
+      </c>
+      <c r="CO17" s="23">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="19" spans="1:90">
+    <row r="19" spans="1:93">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:90">
+    <row r="20" spans="1:93">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3846,7 +3981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:90">
+    <row r="21" spans="1:93">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -4066,8 +4201,17 @@
       <c r="CL21">
         <v>111</v>
       </c>
+      <c r="CM21">
+        <v>111</v>
+      </c>
+      <c r="CN21">
+        <v>113</v>
+      </c>
+      <c r="CO21">
+        <v>113</v>
+      </c>
     </row>
-    <row r="22" spans="1:90">
+    <row r="22" spans="1:93">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4233,8 +4377,17 @@
       <c r="CL22">
         <v>19</v>
       </c>
+      <c r="CM22">
+        <v>19</v>
+      </c>
+      <c r="CN22">
+        <v>21</v>
+      </c>
+      <c r="CO22">
+        <v>21</v>
+      </c>
     </row>
-    <row r="23" spans="1:90">
+    <row r="23" spans="1:93">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4400,8 +4553,17 @@
       <c r="CL23">
         <v>92</v>
       </c>
+      <c r="CM23">
+        <v>92</v>
+      </c>
+      <c r="CN23">
+        <v>92</v>
+      </c>
+      <c r="CO23">
+        <v>92</v>
+      </c>
     </row>
-    <row r="24" spans="1:90">
+    <row r="24" spans="1:93">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4612,8 +4774,17 @@
       <c r="CL24">
         <v>89</v>
       </c>
+      <c r="CM24">
+        <v>89</v>
+      </c>
+      <c r="CN24">
+        <v>106</v>
+      </c>
+      <c r="CO24">
+        <v>104</v>
+      </c>
     </row>
-    <row r="25" spans="1:90">
+    <row r="25" spans="1:93">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -4824,8 +4995,17 @@
       <c r="CL25">
         <v>108</v>
       </c>
+      <c r="CM25">
+        <v>111</v>
+      </c>
+      <c r="CN25">
+        <v>127</v>
+      </c>
+      <c r="CO25">
+        <v>125</v>
+      </c>
     </row>
-    <row r="26" spans="1:90">
+    <row r="26" spans="1:93">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -5036,13 +5216,22 @@
       <c r="CL26">
         <v>1412</v>
       </c>
+      <c r="CM26">
+        <v>1448</v>
+      </c>
+      <c r="CN26">
+        <v>1453</v>
+      </c>
+      <c r="CO26">
+        <v>1460</v>
+      </c>
     </row>
-    <row r="28" spans="1:90">
+    <row r="28" spans="1:93">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:90">
+    <row r="29" spans="1:93">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5262,8 +5451,17 @@
       <c r="CL29">
         <v>139</v>
       </c>
+      <c r="CM29">
+        <v>139</v>
+      </c>
+      <c r="CN29">
+        <v>140</v>
+      </c>
+      <c r="CO29">
+        <v>140</v>
+      </c>
     </row>
-    <row r="30" spans="1:90">
+    <row r="30" spans="1:93">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5429,8 +5627,17 @@
       <c r="CL30">
         <v>31</v>
       </c>
+      <c r="CM30">
+        <v>29</v>
+      </c>
+      <c r="CN30">
+        <v>27</v>
+      </c>
+      <c r="CO30">
+        <v>25</v>
+      </c>
     </row>
-    <row r="31" spans="1:90">
+    <row r="31" spans="1:93">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5596,8 +5803,17 @@
       <c r="CL31">
         <v>108</v>
       </c>
+      <c r="CM31">
+        <v>110</v>
+      </c>
+      <c r="CN31">
+        <v>113</v>
+      </c>
+      <c r="CO31">
+        <v>114</v>
+      </c>
     </row>
-    <row r="32" spans="1:90">
+    <row r="32" spans="1:93">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5808,8 +6024,17 @@
       <c r="CL32">
         <v>46</v>
       </c>
+      <c r="CM32">
+        <v>35</v>
+      </c>
+      <c r="CN32">
+        <v>32</v>
+      </c>
+      <c r="CO32">
+        <v>32</v>
+      </c>
     </row>
-    <row r="33" spans="1:90">
+    <row r="33" spans="1:93">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -6020,8 +6245,17 @@
       <c r="CL33">
         <v>77</v>
       </c>
+      <c r="CM33">
+        <v>64</v>
+      </c>
+      <c r="CN33">
+        <v>59</v>
+      </c>
+      <c r="CO33">
+        <v>57</v>
+      </c>
     </row>
-    <row r="34" spans="1:90">
+    <row r="34" spans="1:93">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6232,13 +6466,22 @@
       <c r="CL34">
         <v>1228</v>
       </c>
+      <c r="CM34">
+        <v>1244</v>
+      </c>
+      <c r="CN34">
+        <v>1256</v>
+      </c>
+      <c r="CO34">
+        <v>1258</v>
+      </c>
     </row>
-    <row r="36" spans="1:90">
+    <row r="36" spans="1:93">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:90">
+    <row r="37" spans="1:93">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -6446,8 +6689,17 @@
       <c r="CL37">
         <v>83</v>
       </c>
+      <c r="CM37">
+        <v>84</v>
+      </c>
+      <c r="CN37">
+        <v>84</v>
+      </c>
+      <c r="CO37">
+        <v>84</v>
+      </c>
     </row>
-    <row r="38" spans="1:90">
+    <row r="38" spans="1:93">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6607,8 +6859,17 @@
       <c r="CL38">
         <v>9</v>
       </c>
+      <c r="CM38">
+        <v>9</v>
+      </c>
+      <c r="CN38">
+        <v>8</v>
+      </c>
+      <c r="CO38">
+        <v>8</v>
+      </c>
     </row>
-    <row r="39" spans="1:90">
+    <row r="39" spans="1:93">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -6768,8 +7029,17 @@
       <c r="CL39">
         <v>73</v>
       </c>
+      <c r="CM39">
+        <v>74</v>
+      </c>
+      <c r="CN39">
+        <v>75</v>
+      </c>
+      <c r="CO39">
+        <v>75</v>
+      </c>
     </row>
-    <row r="40" spans="1:90">
+    <row r="40" spans="1:93">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -6974,8 +7244,17 @@
       <c r="CL40">
         <v>1</v>
       </c>
+      <c r="CM40">
+        <v>1</v>
+      </c>
+      <c r="CN40">
+        <v>0</v>
+      </c>
+      <c r="CO40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:90">
+    <row r="41" spans="1:93">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -7177,8 +7456,17 @@
       <c r="CL41">
         <v>10</v>
       </c>
+      <c r="CM41">
+        <v>10</v>
+      </c>
+      <c r="CN41">
+        <v>8</v>
+      </c>
+      <c r="CO41">
+        <v>8</v>
+      </c>
     </row>
-    <row r="42" spans="1:90">
+    <row r="42" spans="1:93">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7386,8 +7674,17 @@
       <c r="CL42">
         <v>281</v>
       </c>
+      <c r="CM42">
+        <v>282</v>
+      </c>
+      <c r="CN42">
+        <v>284</v>
+      </c>
+      <c r="CO42">
+        <v>284</v>
+      </c>
     </row>
-    <row r="43" spans="1:90">
+    <row r="43" spans="1:93">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -7529,16 +7826,25 @@
       <c r="CL43">
         <v>1</v>
       </c>
+      <c r="CM43">
+        <v>1</v>
+      </c>
+      <c r="CN43">
+        <v>1</v>
+      </c>
+      <c r="CO43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:90">
+    <row r="44" spans="1:93">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:90">
+    <row r="45" spans="1:93">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:90">
+    <row r="46" spans="1:93">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -7752,8 +8058,17 @@
       <c r="CL46">
         <v>206</v>
       </c>
+      <c r="CM46">
+        <v>206</v>
+      </c>
+      <c r="CN46">
+        <v>207</v>
+      </c>
+      <c r="CO46">
+        <v>207</v>
+      </c>
     </row>
-    <row r="47" spans="1:90">
+    <row r="47" spans="1:93">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -7919,8 +8234,17 @@
       <c r="CL47">
         <v>16</v>
       </c>
+      <c r="CM47">
+        <v>11</v>
+      </c>
+      <c r="CN47">
+        <v>11</v>
+      </c>
+      <c r="CO47">
+        <v>10</v>
+      </c>
     </row>
-    <row r="48" spans="1:90">
+    <row r="48" spans="1:93">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -8086,8 +8410,17 @@
       <c r="CL48">
         <v>183</v>
       </c>
+      <c r="CM48">
+        <v>188</v>
+      </c>
+      <c r="CN48">
+        <v>189</v>
+      </c>
+      <c r="CO48">
+        <v>190</v>
+      </c>
     </row>
-    <row r="49" spans="1:90">
+    <row r="49" spans="1:93">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -8298,8 +8631,17 @@
       <c r="CL49">
         <v>396</v>
       </c>
+      <c r="CM49">
+        <v>362</v>
+      </c>
+      <c r="CN49">
+        <v>330</v>
+      </c>
+      <c r="CO49">
+        <v>336</v>
+      </c>
     </row>
-    <row r="50" spans="1:90">
+    <row r="50" spans="1:93">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -8465,8 +8807,17 @@
       <c r="CL50">
         <v>412</v>
       </c>
+      <c r="CM50">
+        <v>373</v>
+      </c>
+      <c r="CN50">
+        <v>341</v>
+      </c>
+      <c r="CO50">
+        <v>346</v>
+      </c>
     </row>
-    <row r="51" spans="1:90">
+    <row r="51" spans="1:93">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -8629,8 +8980,17 @@
       <c r="CL51">
         <v>729</v>
       </c>
+      <c r="CM51">
+        <v>947</v>
+      </c>
+      <c r="CN51">
+        <v>975</v>
+      </c>
+      <c r="CO51">
+        <v>969</v>
+      </c>
     </row>
-    <row r="52" spans="1:90">
+    <row r="52" spans="1:93">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -8787,16 +9147,25 @@
       <c r="CL52">
         <v>1</v>
       </c>
+      <c r="CM52">
+        <v>1</v>
+      </c>
+      <c r="CN52">
+        <v>1</v>
+      </c>
+      <c r="CO52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:90">
+    <row r="53" spans="1:93">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:90">
+    <row r="54" spans="1:93">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:90">
+    <row r="55" spans="1:93">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -8995,8 +9364,17 @@
       <c r="CL55">
         <v>30</v>
       </c>
+      <c r="CM55">
+        <v>30</v>
+      </c>
+      <c r="CN55">
+        <v>30</v>
+      </c>
+      <c r="CO55">
+        <v>30</v>
+      </c>
     </row>
-    <row r="56" spans="1:90">
+    <row r="56" spans="1:93">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -9159,8 +9537,17 @@
       <c r="CL56">
         <v>8</v>
       </c>
+      <c r="CM56">
+        <v>7</v>
+      </c>
+      <c r="CN56">
+        <v>7</v>
+      </c>
+      <c r="CO56">
+        <v>7</v>
+      </c>
     </row>
-    <row r="57" spans="1:90">
+    <row r="57" spans="1:93">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -9323,8 +9710,17 @@
       <c r="CL57">
         <v>22</v>
       </c>
+      <c r="CM57">
+        <v>22</v>
+      </c>
+      <c r="CN57">
+        <v>22</v>
+      </c>
+      <c r="CO57">
+        <v>22</v>
+      </c>
     </row>
-    <row r="58" spans="1:90">
+    <row r="58" spans="1:93">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -9523,8 +9919,17 @@
       <c r="CL58">
         <v>15</v>
       </c>
+      <c r="CM58">
+        <v>13</v>
+      </c>
+      <c r="CN58">
+        <v>13</v>
+      </c>
+      <c r="CO58">
+        <v>12</v>
+      </c>
     </row>
-    <row r="59" spans="1:90">
+    <row r="59" spans="1:93">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -9723,8 +10128,17 @@
       <c r="CL59">
         <v>23</v>
       </c>
+      <c r="CM59">
+        <v>20</v>
+      </c>
+      <c r="CN59">
+        <v>20</v>
+      </c>
+      <c r="CO59">
+        <v>20</v>
+      </c>
     </row>
-    <row r="60" spans="1:90">
+    <row r="60" spans="1:93">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -9923,8 +10337,17 @@
       <c r="CL60">
         <v>147</v>
       </c>
+      <c r="CM60">
+        <v>149</v>
+      </c>
+      <c r="CN60">
+        <v>149</v>
+      </c>
+      <c r="CO60">
+        <v>149</v>
+      </c>
     </row>
-    <row r="61" spans="1:90">
+    <row r="61" spans="1:93">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -10081,8 +10504,17 @@
       <c r="CL61">
         <v>1</v>
       </c>
+      <c r="CM61">
+        <v>1</v>
+      </c>
+      <c r="CN61">
+        <v>1</v>
+      </c>
+      <c r="CO61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:90">
+    <row r="63" spans="1:93">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -10281,8 +10713,17 @@
       <c r="CL63">
         <v>11</v>
       </c>
+      <c r="CM63">
+        <v>11</v>
+      </c>
+      <c r="CN63">
+        <v>12</v>
+      </c>
+      <c r="CO63">
+        <v>12</v>
+      </c>
     </row>
-    <row r="64" spans="1:90">
+    <row r="64" spans="1:93">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -10445,8 +10886,17 @@
       <c r="CL64">
         <v>2</v>
       </c>
+      <c r="CM64">
+        <v>2</v>
+      </c>
+      <c r="CN64">
+        <v>2</v>
+      </c>
+      <c r="CO64">
+        <v>1</v>
+      </c>
     </row>
-    <row r="65" spans="1:90">
+    <row r="65" spans="1:93">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -10609,8 +11059,17 @@
       <c r="CL65">
         <v>9</v>
       </c>
+      <c r="CM65">
+        <v>9</v>
+      </c>
+      <c r="CN65">
+        <v>10</v>
+      </c>
+      <c r="CO65">
+        <v>12</v>
+      </c>
     </row>
-    <row r="66" spans="1:90">
+    <row r="66" spans="1:93">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -10809,8 +11268,17 @@
       <c r="CL66">
         <v>56</v>
       </c>
+      <c r="CM66">
+        <v>55</v>
+      </c>
+      <c r="CN66">
+        <v>55</v>
+      </c>
+      <c r="CO66">
+        <v>54</v>
+      </c>
     </row>
-    <row r="67" spans="1:90">
+    <row r="67" spans="1:93">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -11010,8 +11478,17 @@
       <c r="CL67">
         <v>58</v>
       </c>
+      <c r="CM67">
+        <v>57</v>
+      </c>
+      <c r="CN67">
+        <v>57</v>
+      </c>
+      <c r="CO67">
+        <v>55</v>
+      </c>
     </row>
-    <row r="68" spans="1:90">
+    <row r="68" spans="1:93">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -11210,8 +11687,17 @@
       <c r="CL68">
         <v>0</v>
       </c>
+      <c r="CM68">
+        <v>0</v>
+      </c>
+      <c r="CN68">
+        <v>0</v>
+      </c>
+      <c r="CO68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:90">
+    <row r="69" spans="1:93">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -11374,13 +11860,22 @@
       <c r="CL69">
         <v>0</v>
       </c>
+      <c r="CM69">
+        <v>0</v>
+      </c>
+      <c r="CN69">
+        <v>0</v>
+      </c>
+      <c r="CO69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:90">
+    <row r="70" spans="1:93">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:90">
+    <row r="71" spans="1:93">
       <c r="A71" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -11427,10 +11922,19 @@
       <c r="CL71">
         <v>10</v>
       </c>
+      <c r="CM71">
+        <v>10</v>
+      </c>
+      <c r="CN71">
+        <v>10</v>
+      </c>
+      <c r="CO71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:90">
+    <row r="72" spans="1:93">
       <c r="A72" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
@@ -11477,10 +11981,19 @@
       <c r="CL72">
         <v>5</v>
       </c>
+      <c r="CM72">
+        <v>4</v>
+      </c>
+      <c r="CN72">
+        <v>4</v>
+      </c>
+      <c r="CO72">
+        <v>4</v>
+      </c>
     </row>
-    <row r="73" spans="1:90">
+    <row r="73" spans="1:93">
       <c r="A73" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -11527,10 +12040,19 @@
       <c r="CL73">
         <v>5</v>
       </c>
+      <c r="CM73">
+        <v>6</v>
+      </c>
+      <c r="CN73">
+        <v>6</v>
+      </c>
+      <c r="CO73">
+        <v>6</v>
+      </c>
     </row>
-    <row r="74" spans="1:90">
+    <row r="74" spans="1:93">
       <c r="A74" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
@@ -11577,10 +12099,19 @@
       <c r="CL74">
         <v>8</v>
       </c>
+      <c r="CM74">
+        <v>4</v>
+      </c>
+      <c r="CN74">
+        <v>5</v>
+      </c>
+      <c r="CO74">
+        <v>4</v>
+      </c>
     </row>
-    <row r="75" spans="1:90">
+    <row r="75" spans="1:93">
       <c r="A75" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
@@ -11627,10 +12158,19 @@
       <c r="CL75">
         <v>13</v>
       </c>
+      <c r="CM75">
+        <v>8</v>
+      </c>
+      <c r="CN75">
+        <v>9</v>
+      </c>
+      <c r="CO75">
+        <v>8</v>
+      </c>
     </row>
-    <row r="76" spans="1:90">
+    <row r="76" spans="1:93">
       <c r="A76" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
@@ -11677,13 +12217,22 @@
       <c r="CL76">
         <v>34</v>
       </c>
+      <c r="CM76">
+        <v>37</v>
+      </c>
+      <c r="CN76">
+        <v>38</v>
+      </c>
+      <c r="CO76">
+        <v>39</v>
+      </c>
     </row>
-    <row r="78" spans="1:90">
+    <row r="78" spans="1:93">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:90">
+    <row r="79" spans="1:93">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -11882,8 +12431,17 @@
       <c r="CL79">
         <v>302</v>
       </c>
+      <c r="CM79">
+        <v>302</v>
+      </c>
+      <c r="CN79">
+        <v>302</v>
+      </c>
+      <c r="CO79">
+        <v>303</v>
+      </c>
     </row>
-    <row r="80" spans="1:90">
+    <row r="80" spans="1:93">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -12082,8 +12640,17 @@
       <c r="CL80">
         <v>105</v>
       </c>
+      <c r="CM80">
+        <v>88</v>
+      </c>
+      <c r="CN80">
+        <v>90</v>
+      </c>
+      <c r="CO80">
+        <v>94</v>
+      </c>
     </row>
-    <row r="81" spans="1:90">
+    <row r="81" spans="1:93">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -12282,8 +12849,17 @@
       <c r="CL81">
         <v>84</v>
       </c>
+      <c r="CM81">
+        <v>76</v>
+      </c>
+      <c r="CN81">
+        <v>78</v>
+      </c>
+      <c r="CO81">
+        <v>87</v>
+      </c>
     </row>
-    <row r="82" spans="1:90">
+    <row r="82" spans="1:93">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -12440,8 +13016,17 @@
       <c r="CL82">
         <v>16</v>
       </c>
+      <c r="CM82">
+        <v>16</v>
+      </c>
+      <c r="CN82">
+        <v>16</v>
+      </c>
+      <c r="CO82">
+        <v>16</v>
+      </c>
     </row>
-    <row r="84" spans="1:90">
+    <row r="84" spans="1:93">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -12640,8 +13225,17 @@
       <c r="CL84">
         <v>119</v>
       </c>
+      <c r="CM84">
+        <v>119</v>
+      </c>
+      <c r="CN84">
+        <v>119</v>
+      </c>
+      <c r="CO84">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:90">
+    <row r="85" spans="1:93">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -12840,8 +13434,17 @@
       <c r="CL85">
         <v>25</v>
       </c>
+      <c r="CM85">
+        <v>25</v>
+      </c>
+      <c r="CN85">
+        <v>24</v>
+      </c>
+      <c r="CO85">
+        <v>24</v>
+      </c>
     </row>
-    <row r="86" spans="1:90">
+    <row r="86" spans="1:93">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -13040,8 +13643,17 @@
       <c r="CL86">
         <v>68</v>
       </c>
+      <c r="CM86">
+        <v>66</v>
+      </c>
+      <c r="CN86">
+        <v>63</v>
+      </c>
+      <c r="CO86">
+        <v>60</v>
+      </c>
     </row>
-    <row r="87" spans="1:90">
+    <row r="87" spans="1:93">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -13240,8 +13852,17 @@
       <c r="CL87">
         <v>195</v>
       </c>
+      <c r="CM87">
+        <v>197</v>
+      </c>
+      <c r="CN87">
+        <v>198</v>
+      </c>
+      <c r="CO87">
+        <v>201</v>
+      </c>
     </row>
-    <row r="88" spans="1:90">
+    <row r="88" spans="1:93">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -13314,8 +13935,17 @@
       <c r="CL88">
         <v>1</v>
       </c>
+      <c r="CM88">
+        <v>1</v>
+      </c>
+      <c r="CN88">
+        <v>1</v>
+      </c>
+      <c r="CO88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:90">
+    <row r="90" spans="1:93">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -13514,8 +14144,17 @@
       <c r="CL90">
         <v>81</v>
       </c>
+      <c r="CM90">
+        <v>81</v>
+      </c>
+      <c r="CN90">
+        <v>81</v>
+      </c>
+      <c r="CO90">
+        <v>81</v>
+      </c>
     </row>
-    <row r="91" spans="1:90">
+    <row r="91" spans="1:93">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -13714,8 +14353,17 @@
       <c r="CL91">
         <v>21</v>
       </c>
+      <c r="CM91">
+        <v>21</v>
+      </c>
+      <c r="CN91">
+        <v>21</v>
+      </c>
+      <c r="CO91">
+        <v>2</v>
+      </c>
     </row>
-    <row r="92" spans="1:90">
+    <row r="92" spans="1:93">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -13902,8 +14550,17 @@
       <c r="CL92">
         <v>168</v>
       </c>
+      <c r="CM92">
+        <v>169</v>
+      </c>
+      <c r="CN92">
+        <v>169</v>
+      </c>
+      <c r="CO92">
+        <v>169</v>
+      </c>
     </row>
-    <row r="93" spans="1:90">
+    <row r="93" spans="1:93">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -14102,8 +14759,17 @@
       <c r="CL93">
         <v>43</v>
       </c>
+      <c r="CM93">
+        <v>43</v>
+      </c>
+      <c r="CN93">
+        <v>62</v>
+      </c>
+      <c r="CO93">
+        <v>62</v>
+      </c>
     </row>
-    <row r="94" spans="1:90">
+    <row r="94" spans="1:93">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -14260,16 +14926,25 @@
       <c r="CL94">
         <v>13</v>
       </c>
+      <c r="CM94">
+        <v>13</v>
+      </c>
+      <c r="CN94">
+        <v>13</v>
+      </c>
+      <c r="CO94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:90">
+    <row r="95" spans="1:93">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:90">
+    <row r="96" spans="1:93">
       <c r="A96" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B96" s="41" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="CG96">
         <v>9</v>
@@ -14280,13 +14955,22 @@
       <c r="CL96">
         <v>9</v>
       </c>
+      <c r="CM96">
+        <v>9</v>
+      </c>
+      <c r="CN96">
+        <v>9</v>
+      </c>
+      <c r="CO96">
+        <v>9</v>
+      </c>
     </row>
-    <row r="97" spans="1:90">
+    <row r="97" spans="1:93">
       <c r="A97" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="CG97">
         <v>17</v>
@@ -14297,10 +14981,19 @@
       <c r="CL97">
         <v>12</v>
       </c>
+      <c r="CM97">
+        <v>12</v>
+      </c>
+      <c r="CN97">
+        <v>12</v>
+      </c>
+      <c r="CO97">
+        <v>9</v>
+      </c>
     </row>
-    <row r="98" spans="1:90">
+    <row r="98" spans="1:93">
       <c r="A98" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B98" s="41" t="s">
         <v>12</v>
@@ -14314,10 +15007,19 @@
       <c r="CL98">
         <v>35</v>
       </c>
+      <c r="CM98">
+        <v>35</v>
+      </c>
+      <c r="CN98">
+        <v>35</v>
+      </c>
+      <c r="CO98">
+        <v>43</v>
+      </c>
     </row>
-    <row r="99" spans="1:90">
+    <row r="99" spans="1:93">
       <c r="A99" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B99" s="41" t="s">
         <v>84</v>
@@ -14331,8 +15033,17 @@
       <c r="CL99">
         <v>1</v>
       </c>
+      <c r="CM99">
+        <v>1</v>
+      </c>
+      <c r="CN99">
+        <v>1</v>
+      </c>
+      <c r="CO99">
+        <v>1</v>
+      </c>
     </row>
-    <row r="101" spans="1:90">
+    <row r="101" spans="1:93">
       <c r="A101" s="2" t="s">
         <v>79</v>
       </c>
@@ -14450,8 +15161,17 @@
       <c r="CL101">
         <v>189</v>
       </c>
+      <c r="CM101">
+        <v>191</v>
+      </c>
+      <c r="CN101">
+        <v>193</v>
+      </c>
+      <c r="CO101">
+        <v>193</v>
+      </c>
     </row>
-    <row r="102" spans="1:90">
+    <row r="102" spans="1:93">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -14569,8 +15289,17 @@
       <c r="CL102">
         <v>77</v>
       </c>
+      <c r="CM102">
+        <v>80</v>
+      </c>
+      <c r="CN102">
+        <v>84</v>
+      </c>
+      <c r="CO102">
+        <v>84</v>
+      </c>
     </row>
-    <row r="103" spans="1:90">
+    <row r="103" spans="1:93">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -14686,6 +15415,15 @@
         <v>25</v>
       </c>
       <c r="CL103">
+        <v>25</v>
+      </c>
+      <c r="CM103">
+        <v>25</v>
+      </c>
+      <c r="CN103">
+        <v>25</v>
+      </c>
+      <c r="CO103">
         <v>25</v>
       </c>
     </row>
@@ -14702,10 +15440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BM11"/>
+  <dimension ref="A2:BP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BM11" sqref="BM3:BM11"/>
+    <sheetView tabSelected="1" topLeftCell="BB2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BN3" sqref="BN3:BP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14715,7 +15453,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:65" s="2" customFormat="1">
+    <row r="2" spans="1:68" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -14911,8 +15649,17 @@
       <c r="BM2" s="9">
         <v>43984</v>
       </c>
+      <c r="BN2" s="9">
+        <v>43985</v>
+      </c>
+      <c r="BO2" s="9">
+        <v>43986</v>
+      </c>
+      <c r="BP2" s="9">
+        <v>43987</v>
+      </c>
     </row>
-    <row r="3" spans="1:65">
+    <row r="3" spans="1:68">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -15106,10 +15853,19 @@
         <v>1243</v>
       </c>
       <c r="BM3">
-        <v>1243</v>
+        <v>1270</v>
+      </c>
+      <c r="BN3">
+        <v>1288</v>
+      </c>
+      <c r="BO3">
+        <v>1302</v>
+      </c>
+      <c r="BP3">
+        <v>1313</v>
       </c>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:68">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -15303,10 +16059,19 @@
         <v>513</v>
       </c>
       <c r="BM4">
-        <v>513</v>
+        <v>517</v>
+      </c>
+      <c r="BN4">
+        <v>522</v>
+      </c>
+      <c r="BO4">
+        <v>525</v>
+      </c>
+      <c r="BP4">
+        <v>526</v>
       </c>
     </row>
-    <row r="5" spans="1:65">
+    <row r="5" spans="1:68">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -15500,10 +16265,19 @@
         <v>420</v>
       </c>
       <c r="BM5">
-        <v>420</v>
+        <v>428</v>
+      </c>
+      <c r="BN5">
+        <v>428</v>
+      </c>
+      <c r="BO5">
+        <v>432</v>
+      </c>
+      <c r="BP5">
+        <v>435</v>
       </c>
     </row>
-    <row r="6" spans="1:65">
+    <row r="6" spans="1:68">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -15697,10 +16471,19 @@
         <v>1852</v>
       </c>
       <c r="BM6">
-        <v>1852</v>
+        <v>1889</v>
+      </c>
+      <c r="BN6">
+        <v>1913</v>
+      </c>
+      <c r="BO6">
+        <v>1926</v>
+      </c>
+      <c r="BP6">
+        <v>1943</v>
       </c>
     </row>
-    <row r="7" spans="1:65">
+    <row r="7" spans="1:68">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -15894,10 +16677,19 @@
         <v>1379</v>
       </c>
       <c r="BM7">
-        <v>1379</v>
+        <v>1388</v>
+      </c>
+      <c r="BN7">
+        <v>1400</v>
+      </c>
+      <c r="BO7">
+        <v>1414</v>
+      </c>
+      <c r="BP7">
+        <v>1420</v>
       </c>
     </row>
-    <row r="8" spans="1:65">
+    <row r="8" spans="1:68">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -16091,10 +16883,19 @@
         <v>758</v>
       </c>
       <c r="BM8">
-        <v>758</v>
+        <v>768</v>
+      </c>
+      <c r="BN8">
+        <v>774</v>
+      </c>
+      <c r="BO8">
+        <v>782</v>
+      </c>
+      <c r="BP8">
+        <v>787</v>
       </c>
     </row>
-    <row r="9" spans="1:65">
+    <row r="9" spans="1:68">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -16288,10 +17089,19 @@
         <v>1298</v>
       </c>
       <c r="BM9">
-        <v>1298</v>
+        <v>1310</v>
+      </c>
+      <c r="BN9">
+        <v>1317</v>
+      </c>
+      <c r="BO9">
+        <v>1325</v>
+      </c>
+      <c r="BP9">
+        <v>1335</v>
       </c>
     </row>
-    <row r="10" spans="1:65">
+    <row r="10" spans="1:68">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -16485,10 +17295,19 @@
         <v>1278</v>
       </c>
       <c r="BM10">
-        <v>1278</v>
+        <v>1300</v>
+      </c>
+      <c r="BN10">
+        <v>1323</v>
+      </c>
+      <c r="BO10">
+        <v>1340</v>
+      </c>
+      <c r="BP10">
+        <v>1354</v>
       </c>
     </row>
-    <row r="11" spans="1:65">
+    <row r="11" spans="1:68">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -16682,7 +17501,16 @@
         <v>145</v>
       </c>
       <c r="BM11">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="BN11">
+        <v>155</v>
+      </c>
+      <c r="BO11">
+        <v>153</v>
+      </c>
+      <c r="BP11">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -16693,10 +17521,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BH17"/>
+  <dimension ref="A2:BK17"/>
   <sheetViews>
-    <sheetView topLeftCell="AO8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BH17" sqref="BH17"/>
+    <sheetView topLeftCell="AU10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BK17" sqref="BK17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16706,7 +17534,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:60" s="2" customFormat="1">
+    <row r="2" spans="1:63" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -16885,8 +17713,17 @@
       <c r="BH2" s="9">
         <v>43984</v>
       </c>
+      <c r="BI2" s="9">
+        <v>43985</v>
+      </c>
+      <c r="BJ2" s="9">
+        <v>43986</v>
+      </c>
+      <c r="BK2" s="9">
+        <v>43987</v>
+      </c>
     </row>
-    <row r="3" spans="1:60" s="2" customFormat="1">
+    <row r="3" spans="1:63" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -16894,7 +17731,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:60">
+    <row r="4" spans="1:63">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -17075,8 +17912,17 @@
       <c r="BH4">
         <v>9016</v>
       </c>
+      <c r="BI4">
+        <v>9120</v>
+      </c>
+      <c r="BJ4">
+        <v>9199</v>
+      </c>
+      <c r="BK4">
+        <v>9269</v>
+      </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:63">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -17257,8 +18103,17 @@
       <c r="BH5">
         <v>995</v>
       </c>
+      <c r="BI5">
+        <v>1024</v>
+      </c>
+      <c r="BJ5">
+        <v>1061</v>
+      </c>
+      <c r="BK5">
+        <v>1035</v>
+      </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:63">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -17439,8 +18294,17 @@
       <c r="BH6">
         <v>1364</v>
       </c>
+      <c r="BI6">
+        <v>1368</v>
+      </c>
+      <c r="BJ6">
+        <v>1366</v>
+      </c>
+      <c r="BK6">
+        <v>1392</v>
+      </c>
     </row>
-    <row r="7" spans="1:60">
+    <row r="7" spans="1:63">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -17621,8 +18485,17 @@
       <c r="BH7">
         <v>4164</v>
       </c>
+      <c r="BI7">
+        <v>4200</v>
+      </c>
+      <c r="BJ7">
+        <v>4223</v>
+      </c>
+      <c r="BK7">
+        <v>4281</v>
+      </c>
     </row>
-    <row r="8" spans="1:60">
+    <row r="8" spans="1:63">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -17803,8 +18676,17 @@
       <c r="BH8">
         <v>106</v>
       </c>
+      <c r="BI8">
+        <v>106</v>
+      </c>
+      <c r="BJ8">
+        <v>108</v>
+      </c>
+      <c r="BK8">
+        <v>108</v>
+      </c>
     </row>
-    <row r="9" spans="1:60" ht="30">
+    <row r="9" spans="1:63" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -17985,8 +18867,17 @@
       <c r="BH9">
         <v>26</v>
       </c>
+      <c r="BI9">
+        <v>26</v>
+      </c>
+      <c r="BJ9">
+        <v>26</v>
+      </c>
+      <c r="BK9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:60" ht="30">
+    <row r="10" spans="1:63" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -18163,8 +19054,17 @@
       <c r="BH10">
         <v>22</v>
       </c>
+      <c r="BI10">
+        <v>22</v>
+      </c>
+      <c r="BJ10">
+        <v>22</v>
+      </c>
+      <c r="BK10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:60">
+    <row r="11" spans="1:63">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -18345,8 +19245,17 @@
       <c r="BH11">
         <v>2281</v>
       </c>
+      <c r="BI11">
+        <v>2314</v>
+      </c>
+      <c r="BJ11">
+        <v>2335</v>
+      </c>
+      <c r="BK11">
+        <v>2345</v>
+      </c>
     </row>
-    <row r="12" spans="1:60" ht="30">
+    <row r="12" spans="1:63" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -18527,8 +19436,17 @@
       <c r="BH12">
         <v>58</v>
       </c>
+      <c r="BI12">
+        <v>58</v>
+      </c>
+      <c r="BJ12">
+        <v>58</v>
+      </c>
+      <c r="BK12">
+        <v>59</v>
+      </c>
     </row>
-    <row r="13" spans="1:60">
+    <row r="13" spans="1:63">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -18539,7 +19457,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:60">
+    <row r="14" spans="1:63">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -18720,8 +19638,17 @@
       <c r="BH14">
         <v>1608</v>
       </c>
+      <c r="BI14">
+        <v>1646</v>
+      </c>
+      <c r="BJ14">
+        <v>1694</v>
+      </c>
+      <c r="BK14">
+        <v>1654</v>
+      </c>
     </row>
-    <row r="15" spans="1:60">
+    <row r="15" spans="1:63">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -18902,8 +19829,17 @@
       <c r="BH15">
         <v>2372</v>
       </c>
+      <c r="BI15">
+        <v>2400</v>
+      </c>
+      <c r="BJ15">
+        <v>2411</v>
+      </c>
+      <c r="BK15">
+        <v>2456</v>
+      </c>
     </row>
-    <row r="16" spans="1:60">
+    <row r="16" spans="1:63">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -19084,8 +20020,17 @@
       <c r="BH16">
         <v>5010</v>
       </c>
+      <c r="BI16">
+        <v>5048</v>
+      </c>
+      <c r="BJ16">
+        <v>5068</v>
+      </c>
+      <c r="BK16">
+        <v>5133</v>
+      </c>
     </row>
-    <row r="17" spans="1:60" ht="30">
+    <row r="17" spans="1:63" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -19264,6 +20209,15 @@
         <v>26</v>
       </c>
       <c r="BH17">
+        <v>26</v>
+      </c>
+      <c r="BI17">
+        <v>26</v>
+      </c>
+      <c r="BJ17">
+        <v>26</v>
+      </c>
+      <c r="BK17">
         <v>26</v>
       </c>
     </row>
@@ -19275,10 +20229,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BH9"/>
+  <dimension ref="A1:BK9"/>
   <sheetViews>
-    <sheetView topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="BH8" sqref="BH8"/>
+    <sheetView topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BK8" sqref="BK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19287,7 +20241,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="2" customFormat="1">
+    <row r="1" spans="1:63" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -19465,14 +20419,23 @@
       <c r="BH1" s="9">
         <v>43984</v>
       </c>
+      <c r="BI1" s="9">
+        <v>43985</v>
+      </c>
+      <c r="BJ1" s="9">
+        <v>43986</v>
+      </c>
+      <c r="BK1" s="9">
+        <v>43987</v>
+      </c>
     </row>
-    <row r="2" spans="1:60">
+    <row r="2" spans="1:63">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:60">
+    <row r="3" spans="1:63">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -19654,8 +20617,17 @@
       <c r="BH3">
         <v>473</v>
       </c>
+      <c r="BI3">
+        <v>475</v>
+      </c>
+      <c r="BJ3">
+        <v>479</v>
+      </c>
+      <c r="BK3">
+        <v>483</v>
+      </c>
     </row>
-    <row r="4" spans="1:60">
+    <row r="4" spans="1:63">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -19836,8 +20808,17 @@
       <c r="BH4">
         <v>7</v>
       </c>
+      <c r="BI4">
+        <v>7</v>
+      </c>
+      <c r="BJ4">
+        <v>7</v>
+      </c>
+      <c r="BK4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:60" ht="30">
+    <row r="5" spans="1:63" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -20018,8 +20999,17 @@
       <c r="BH5">
         <v>356</v>
       </c>
+      <c r="BI5">
+        <v>356</v>
+      </c>
+      <c r="BJ5">
+        <v>357</v>
+      </c>
+      <c r="BK5">
+        <v>361</v>
+      </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:63">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -20200,8 +21190,17 @@
       <c r="BH6">
         <v>54</v>
       </c>
+      <c r="BI6">
+        <v>54</v>
+      </c>
+      <c r="BJ6">
+        <v>57</v>
+      </c>
+      <c r="BK6">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:60" ht="30">
+    <row r="7" spans="1:63" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -20382,8 +21381,17 @@
       <c r="BH7">
         <v>52</v>
       </c>
+      <c r="BI7">
+        <v>53</v>
+      </c>
+      <c r="BJ7">
+        <v>53</v>
+      </c>
+      <c r="BK7">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:60">
+    <row r="8" spans="1:63">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -20564,8 +21572,17 @@
       <c r="BH8">
         <v>4</v>
       </c>
+      <c r="BI8">
+        <v>3</v>
+      </c>
+      <c r="BJ8">
+        <v>5</v>
+      </c>
+      <c r="BK8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:63">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -20583,6 +21600,9 @@
       </c>
       <c r="BG9">
         <v>1</v>
+      </c>
+      <c r="BI9">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -20592,10 +21612,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AT13"/>
+  <dimension ref="A2:AW13"/>
   <sheetViews>
-    <sheetView topLeftCell="AD5" workbookViewId="0">
-      <selection activeCell="AT13" sqref="AT13"/>
+    <sheetView topLeftCell="AJ4" workbookViewId="0">
+      <selection activeCell="AW13" sqref="AW13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20603,7 +21623,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:46" s="2" customFormat="1">
+    <row r="2" spans="1:49" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -20742,8 +21762,17 @@
       <c r="AT2" s="9">
         <v>43984</v>
       </c>
+      <c r="AU2" s="9">
+        <v>43985</v>
+      </c>
+      <c r="AV2" s="9">
+        <v>43986</v>
+      </c>
+      <c r="AW2" s="9">
+        <v>43987</v>
+      </c>
     </row>
-    <row r="3" spans="1:46">
+    <row r="3" spans="1:49">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -20882,8 +21911,17 @@
       <c r="AT3">
         <v>473</v>
       </c>
+      <c r="AU3">
+        <v>475</v>
+      </c>
+      <c r="AV3">
+        <v>479</v>
+      </c>
+      <c r="AW3">
+        <v>483</v>
+      </c>
     </row>
-    <row r="4" spans="1:46">
+    <row r="4" spans="1:49">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -21022,8 +22060,17 @@
       <c r="AT4">
         <v>48</v>
       </c>
+      <c r="AU4">
+        <v>49</v>
+      </c>
+      <c r="AV4">
+        <v>51</v>
+      </c>
+      <c r="AW4">
+        <v>51</v>
+      </c>
     </row>
-    <row r="5" spans="1:46">
+    <row r="5" spans="1:49">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -21162,8 +22209,17 @@
       <c r="AT5">
         <v>29</v>
       </c>
+      <c r="AU5">
+        <v>29</v>
+      </c>
+      <c r="AV5">
+        <v>29</v>
+      </c>
+      <c r="AW5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:46">
+    <row r="6" spans="1:49">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -21302,8 +22358,17 @@
       <c r="AT6">
         <v>30</v>
       </c>
+      <c r="AU6">
+        <v>30</v>
+      </c>
+      <c r="AV6">
+        <v>30</v>
+      </c>
+      <c r="AW6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:46">
+    <row r="7" spans="1:49">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -21442,8 +22507,17 @@
       <c r="AT7">
         <v>66</v>
       </c>
+      <c r="AU7">
+        <v>67</v>
+      </c>
+      <c r="AV7">
+        <v>68</v>
+      </c>
+      <c r="AW7">
+        <v>68</v>
+      </c>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:49">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -21582,8 +22656,17 @@
       <c r="AT8">
         <v>75</v>
       </c>
+      <c r="AU8">
+        <v>75</v>
+      </c>
+      <c r="AV8">
+        <v>76</v>
+      </c>
+      <c r="AW8">
+        <v>77</v>
+      </c>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:49">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -21722,8 +22805,17 @@
       <c r="AT9">
         <v>43</v>
       </c>
+      <c r="AU9">
+        <v>43</v>
+      </c>
+      <c r="AV9">
+        <v>43</v>
+      </c>
+      <c r="AW9">
+        <v>43</v>
+      </c>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:49">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -21862,8 +22954,17 @@
       <c r="AT10">
         <v>69</v>
       </c>
+      <c r="AU10">
+        <v>69</v>
+      </c>
+      <c r="AV10">
+        <v>69</v>
+      </c>
+      <c r="AW10">
+        <v>70</v>
+      </c>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:49">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -22002,8 +23103,17 @@
       <c r="AT11">
         <v>97</v>
       </c>
+      <c r="AU11">
+        <v>97</v>
+      </c>
+      <c r="AV11">
+        <v>97</v>
+      </c>
+      <c r="AW11">
+        <v>99</v>
+      </c>
     </row>
-    <row r="12" spans="1:46" ht="30">
+    <row r="12" spans="1:49" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -22142,8 +23252,17 @@
       <c r="AT12">
         <v>16</v>
       </c>
+      <c r="AU12">
+        <v>16</v>
+      </c>
+      <c r="AV12">
+        <v>16</v>
+      </c>
+      <c r="AW12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:46">
+    <row r="13" spans="1:49">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -22280,6 +23399,15 @@
         <v>0</v>
       </c>
       <c r="AT13">
+        <v>0</v>
+      </c>
+      <c r="AU13">
+        <v>0</v>
+      </c>
+      <c r="AV13">
+        <v>0</v>
+      </c>
+      <c r="AW13">
         <v>0</v>
       </c>
     </row>
@@ -22291,10 +23419,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="C1" sqref="C1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22302,9 +23430,9 @@
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:19">
       <c r="C1" s="42" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
@@ -22319,7 +23447,7 @@
       <c r="N1" s="42"/>
       <c r="O1" s="42"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:19">
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
@@ -22334,7 +23462,7 @@
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:19">
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -22349,7 +23477,7 @@
       <c r="N3" s="42"/>
       <c r="O3" s="42"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:19">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -22364,7 +23492,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:19">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -22407,10 +23535,19 @@
       <c r="P5" s="9">
         <v>43984</v>
       </c>
+      <c r="Q5" s="9">
+        <v>43985</v>
+      </c>
+      <c r="R5" s="9">
+        <v>43986</v>
+      </c>
+      <c r="S5" s="9">
+        <v>43987</v>
+      </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>103</v>
@@ -22454,8 +23591,17 @@
       <c r="P6">
         <v>119</v>
       </c>
+      <c r="Q6">
+        <v>119</v>
+      </c>
+      <c r="R6">
+        <v>119</v>
+      </c>
+      <c r="S6">
+        <v>124</v>
+      </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -22501,16 +23647,25 @@
       <c r="P7">
         <v>31</v>
       </c>
+      <c r="Q7">
+        <v>31</v>
+      </c>
+      <c r="R7">
+        <v>31</v>
+      </c>
+      <c r="S7">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:19">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:19">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -22556,10 +23711,19 @@
       <c r="P9">
         <v>1</v>
       </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:19">
       <c r="A10" s="31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C10">
         <v>18</v>
@@ -22603,10 +23767,19 @@
       <c r="P10">
         <v>21</v>
       </c>
+      <c r="Q10">
+        <v>21</v>
+      </c>
+      <c r="R10">
+        <v>21</v>
+      </c>
+      <c r="S10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:19">
       <c r="A11" s="31" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -22650,8 +23823,17 @@
       <c r="P11">
         <v>7</v>
       </c>
+      <c r="Q11">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>7</v>
+      </c>
+      <c r="S11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:19">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -22697,13 +23879,22 @@
       <c r="P12">
         <v>2</v>
       </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:19">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:19">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -22749,8 +23940,17 @@
       <c r="P14">
         <v>1</v>
       </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:19">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -22796,8 +23996,17 @@
       <c r="P15">
         <v>0</v>
       </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:19">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -22843,8 +24052,17 @@
       <c r="P16">
         <v>3</v>
       </c>
+      <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>3</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:19">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -22890,8 +24108,17 @@
       <c r="P17">
         <v>9</v>
       </c>
+      <c r="Q17">
+        <v>9</v>
+      </c>
+      <c r="R17">
+        <v>9</v>
+      </c>
+      <c r="S17">
+        <v>11</v>
+      </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:19">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -22937,8 +24164,17 @@
       <c r="P18">
         <v>2</v>
       </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>2</v>
+      </c>
+      <c r="S18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:19">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -22984,8 +24220,17 @@
       <c r="P19">
         <v>2</v>
       </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>2</v>
+      </c>
+      <c r="S19">
+        <v>3</v>
+      </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:19">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -23031,8 +24276,17 @@
       <c r="P20">
         <v>3</v>
       </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>3</v>
+      </c>
+      <c r="S20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:19">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -23078,8 +24332,17 @@
       <c r="P21">
         <v>6</v>
       </c>
+      <c r="Q21">
+        <v>6</v>
+      </c>
+      <c r="R21">
+        <v>6</v>
+      </c>
+      <c r="S21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:16" ht="45">
+    <row r="22" spans="1:19" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -23125,10 +24388,19 @@
       <c r="P22">
         <v>4</v>
       </c>
+      <c r="Q22">
+        <v>4</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="S22">
+        <v>2</v>
+      </c>
     </row>
-    <row r="23" spans="1:16" ht="30">
+    <row r="23" spans="1:19" ht="30">
       <c r="A23" s="39" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -23171,6 +24443,15 @@
       </c>
       <c r="P23">
         <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -23202,7 +24483,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -23216,22 +24497,22 @@
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="E2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="29" t="s">
-        <v>125</v>
-      </c>
       <c r="G2" s="29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1">
@@ -23300,7 +24581,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C8" s="28">
         <v>3</v>
@@ -23323,7 +24604,7 @@
         <v>96</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C9" s="28">
         <v>3</v>
@@ -23346,7 +24627,7 @@
         <v>98</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C10" s="28">
         <v>4</v>
@@ -23355,7 +24636,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F10" s="28">
         <v>1</v>
@@ -23369,16 +24650,16 @@
         <v>99</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C11" s="28">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="28">
         <v>0</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
@@ -23412,7 +24693,7 @@
     </row>
     <row r="13" spans="1:7" ht="14.45" customHeight="1">
       <c r="A13" s="27" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>97</v>
@@ -23424,7 +24705,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="F13" s="28">
         <v>0</v>
@@ -23438,7 +24719,7 @@
         <v>103</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="28">
         <v>2</v>
@@ -23461,7 +24742,7 @@
         <v>104</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="C15" s="28">
         <v>15</v>
@@ -23470,7 +24751,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F15" s="28">
         <v>1</v>
@@ -23481,19 +24762,19 @@
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1">
       <c r="A16" s="30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="C16" s="28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D16" s="28">
         <v>0</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="F16" s="28">
         <v>0</v>
@@ -23504,10 +24785,10 @@
     </row>
     <row r="17" spans="1:7" ht="14.45" customHeight="1">
       <c r="A17" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C17" s="28">
         <v>9</v>
@@ -23516,7 +24797,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F17" s="28">
         <v>1</v>
@@ -23527,10 +24808,10 @@
     </row>
     <row r="18" spans="1:7" ht="14.45" customHeight="1">
       <c r="A18" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C18" s="28">
         <v>12</v>
@@ -23539,7 +24820,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F18" s="28">
         <v>0</v>
@@ -23550,10 +24831,10 @@
     </row>
     <row r="19" spans="1:7" ht="14.45" customHeight="1">
       <c r="A19" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C19" s="28">
         <v>13</v>
@@ -23562,7 +24843,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
@@ -23573,10 +24854,10 @@
     </row>
     <row r="20" spans="1:7" ht="14.45" customHeight="1">
       <c r="A20" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C20" s="28">
         <v>17</v>
@@ -23596,19 +24877,19 @@
     </row>
     <row r="21" spans="1:7" ht="14.45" customHeight="1">
       <c r="A21" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="28">
+        <v>1</v>
+      </c>
+      <c r="D21" s="28">
+        <v>0</v>
+      </c>
+      <c r="E21" s="28" t="s">
         <v>112</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="28">
-        <v>1</v>
-      </c>
-      <c r="D21" s="28">
-        <v>0</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>114</v>
       </c>
       <c r="F21" s="28">
         <v>0</v>
@@ -23619,10 +24900,10 @@
     </row>
     <row r="22" spans="1:7" ht="14.45" customHeight="1">
       <c r="A22" s="27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C22" s="28">
         <v>26</v>
@@ -23631,7 +24912,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F22" s="28">
         <v>1</v>
@@ -23642,10 +24923,10 @@
     </row>
     <row r="23" spans="1:7" ht="15.6" customHeight="1">
       <c r="A23" s="27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C23" s="28">
         <v>6</v>
@@ -23665,10 +24946,10 @@
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1">
       <c r="A24" s="27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C24" s="28">
         <v>8</v>
@@ -23677,7 +24958,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F24" s="28">
         <v>0</v>
@@ -23688,19 +24969,19 @@
     </row>
     <row r="25" spans="1:7" ht="33.6" customHeight="1">
       <c r="A25" s="30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="C25" s="28">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D25" s="28">
         <v>0</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F25" s="28">
         <v>1</v>
@@ -23714,16 +24995,16 @@
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C26" s="28">
+        <v>165</v>
+      </c>
+      <c r="D26" s="28">
+        <v>0</v>
+      </c>
+      <c r="E26" s="28" t="s">
         <v>160</v>
-      </c>
-      <c r="D26" s="28">
-        <v>0</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>165</v>
       </c>
       <c r="F26" s="28">
         <v>5</v>
@@ -23734,10 +25015,10 @@
     </row>
     <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -23766,6 +25047,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -23968,12 +25255,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -23984,6 +25265,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24002,23 +25300,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
07 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46711E8-F5F3-4404-8D88-FB7327D8A01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8728DFDE-C46A-402C-857F-CE80BAAC8B6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="167">
   <si>
     <t>Testing</t>
   </si>
@@ -326,12 +324,6 @@
     <t>BridgePoint Capitol Hill (Bed Capacity: 117)</t>
   </si>
   <si>
-    <t>8; (4)</t>
-  </si>
-  <si>
-    <t>BridgePoint National Harbor (Bed Capacity: 92)</t>
-  </si>
-  <si>
     <t>0; (0)</t>
   </si>
   <si>
@@ -347,9 +339,6 @@
     <t>1; (1)</t>
   </si>
   <si>
-    <t>1; (0)</t>
-  </si>
-  <si>
     <t>Ingleside (Bed Capacity: 60)</t>
   </si>
   <si>
@@ -357,9 +346,6 @@
   </si>
   <si>
     <t>Knollwood (Bed Capacity: 73)</t>
-  </si>
-  <si>
-    <t>26; (6)</t>
   </si>
   <si>
     <t>Lisner Home (Bed Capacity: 60)</t>
@@ -386,13 +372,7 @@
     <t>UMNC (Bed Capacity: 120)</t>
   </si>
   <si>
-    <t>23; (7)</t>
-  </si>
-  <si>
     <t>Unique (Bed Capacity: 230)</t>
-  </si>
-  <si>
-    <t>13; (3)</t>
   </si>
   <si>
     <t>Grand Total All (Resident/Personnel)</t>
@@ -422,19 +402,7 @@
     <t>Personnel Recovered:</t>
   </si>
   <si>
-    <t>25; (14)</t>
-  </si>
-  <si>
-    <t>10; (6)</t>
-  </si>
-  <si>
     <t>Public Safety - OUC -Personnel</t>
-  </si>
-  <si>
-    <t>9; (2)</t>
-  </si>
-  <si>
-    <t>23; (8)</t>
   </si>
   <si>
     <t>Total Submitted for Testing</t>
@@ -458,34 +426,13 @@
     <t>Hospital for Sick Children LTC</t>
   </si>
   <si>
-    <t>20; (1)</t>
-  </si>
-  <si>
-    <t>45; (18)</t>
-  </si>
-  <si>
     <t>Total Number of DC Residents Tested</t>
   </si>
   <si>
     <t>Total Overall Tested</t>
   </si>
   <si>
-    <t>20; (3)</t>
-  </si>
-  <si>
     <t>29; (0)</t>
-  </si>
-  <si>
-    <t>58; (33)</t>
-  </si>
-  <si>
-    <t>16; (8)</t>
-  </si>
-  <si>
-    <t>3; (0)</t>
-  </si>
-  <si>
-    <t>34; (25)</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -506,41 +453,11 @@
     <t>2; (1)</t>
   </si>
   <si>
-    <t>64; (20)</t>
-  </si>
-  <si>
-    <t>21; (10)</t>
-  </si>
-  <si>
-    <t>10; (2)</t>
-  </si>
-  <si>
-    <t>44; (29)</t>
-  </si>
-  <si>
-    <t>26; (18)</t>
-  </si>
-  <si>
-    <t>204; (81)</t>
-  </si>
-  <si>
-    <t>As of June 5, 2020</t>
-  </si>
-  <si>
-    <t>100; (51)</t>
-  </si>
-  <si>
-    <t>81; (51)</t>
-  </si>
-  <si>
-    <t>672; (292)</t>
-  </si>
-  <si>
-    <t>876; (373)</t>
+    <t>As of June 6, 2020</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of June 5, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of June 6, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -563,6 +480,87 @@
       </rPr>
       <t xml:space="preserve"> for COVID-19 testing,  and 34 (27.4%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
+  </si>
+  <si>
+    <t>10; (7)</t>
+  </si>
+  <si>
+    <t>12; (11)</t>
+  </si>
+  <si>
+    <t>24; (9)</t>
+  </si>
+  <si>
+    <t>21; (3)</t>
+  </si>
+  <si>
+    <t>96; (48)</t>
+  </si>
+  <si>
+    <t>32; (2)</t>
+  </si>
+  <si>
+    <t>6; (2)</t>
+  </si>
+  <si>
+    <t>65; (29)</t>
+  </si>
+  <si>
+    <t>32; (20)</t>
+  </si>
+  <si>
+    <t>20; (11)</t>
+  </si>
+  <si>
+    <t>13; (12)</t>
+  </si>
+  <si>
+    <t>26; (17)</t>
+  </si>
+  <si>
+    <t>23; (10)</t>
+  </si>
+  <si>
+    <t>41; (37)</t>
+  </si>
+  <si>
+    <t>10; (9)</t>
+  </si>
+  <si>
+    <t>61; (37)</t>
+  </si>
+  <si>
+    <t>22; (19)</t>
+  </si>
+  <si>
+    <t>38; (22)</t>
+  </si>
+  <si>
+    <t>23; (13)</t>
+  </si>
+  <si>
+    <t>12; (9)</t>
+  </si>
+  <si>
+    <t>15; (11)</t>
+  </si>
+  <si>
+    <t>20; (17)</t>
+  </si>
+  <si>
+    <t>80; (77)</t>
+  </si>
+  <si>
+    <t>13; (10)</t>
+  </si>
+  <si>
+    <t>658; (368)</t>
+  </si>
+  <si>
+    <t>251; (129)</t>
+  </si>
+  <si>
+    <t>909; (497)</t>
   </si>
 </sst>
 </file>
@@ -839,13 +837,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>394</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1196,26 +1194,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CO118"/>
+  <dimension ref="A1:CP118"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="CG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CO82" sqref="CO82"/>
+      <selection pane="topRight" activeCell="CP103" sqref="CP103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93">
+    <row r="1" spans="1:94">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1489,8 +1487,11 @@
       <c r="CO1" s="1">
         <v>43987</v>
       </c>
+      <c r="CP1" s="1">
+        <v>43988</v>
+      </c>
     </row>
-    <row r="2" spans="1:93">
+    <row r="2" spans="1:94">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1514,12 +1515,12 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:93">
+    <row r="3" spans="1:94">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="I3">
         <v>69</v>
@@ -1773,13 +1774,16 @@
       <c r="CO3">
         <v>53678</v>
       </c>
+      <c r="CP3">
+        <v>54547</v>
+      </c>
     </row>
-    <row r="4" spans="1:93">
+    <row r="4" spans="1:94">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="AN4" s="19"/>
       <c r="AO4" s="20"/>
@@ -1828,8 +1832,11 @@
       <c r="CO4">
         <v>43528</v>
       </c>
+      <c r="CP4">
+        <v>44485</v>
+      </c>
     </row>
-    <row r="5" spans="1:93">
+    <row r="5" spans="1:94">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2109,8 +2116,11 @@
       <c r="CO5">
         <v>9269</v>
       </c>
+      <c r="CP5">
+        <v>9332</v>
+      </c>
     </row>
-    <row r="6" spans="1:93">
+    <row r="6" spans="1:94">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2367,18 +2377,21 @@
         <v>475</v>
       </c>
       <c r="CN6">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="CO6">
         <v>483</v>
       </c>
+      <c r="CP6">
+        <v>489</v>
+      </c>
     </row>
-    <row r="7" spans="1:93">
+    <row r="7" spans="1:94">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="S7">
         <v>17</v>
@@ -2605,11 +2618,14 @@
       <c r="CO7">
         <v>1138</v>
       </c>
+      <c r="CP7">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="8" spans="1:93">
+    <row r="8" spans="1:94">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:93">
+    <row r="9" spans="1:94">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2733,8 +2749,11 @@
       <c r="CO9">
         <v>345</v>
       </c>
+      <c r="CP9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:93">
+    <row r="10" spans="1:94">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2960,8 +2979,11 @@
       <c r="CO10">
         <v>66</v>
       </c>
+      <c r="CP10">
+        <v>114</v>
+      </c>
     </row>
-    <row r="11" spans="1:93">
+    <row r="11" spans="1:94">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3187,8 +3209,11 @@
       <c r="CO11">
         <v>440</v>
       </c>
+      <c r="CP11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:93">
+    <row r="12" spans="1:94">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3414,8 +3439,11 @@
       <c r="CO12">
         <v>212</v>
       </c>
+      <c r="CP12">
+        <v>200</v>
+      </c>
     </row>
-    <row r="13" spans="1:93">
+    <row r="13" spans="1:94">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3641,8 +3669,11 @@
       <c r="CO13">
         <v>228</v>
       </c>
+      <c r="CP13">
+        <v>240</v>
+      </c>
     </row>
-    <row r="14" spans="1:93">
+    <row r="14" spans="1:94">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3730,13 +3761,16 @@
       <c r="CO14">
         <v>276</v>
       </c>
+      <c r="CP14">
+        <v>285</v>
+      </c>
     </row>
-    <row r="15" spans="1:93">
+    <row r="15" spans="1:94">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="BY15">
         <v>110</v>
@@ -3789,8 +3823,11 @@
       <c r="CO15">
         <v>100</v>
       </c>
+      <c r="CP15">
+        <v>90</v>
+      </c>
     </row>
-    <row r="16" spans="1:93">
+    <row r="16" spans="1:94">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3878,8 +3915,11 @@
       <c r="CO16">
         <v>1985</v>
       </c>
+      <c r="CP16">
+        <v>1863</v>
+      </c>
     </row>
-    <row r="17" spans="1:93">
+    <row r="17" spans="1:94">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -3967,13 +4007,16 @@
       <c r="CO17" s="23">
         <v>0.8</v>
       </c>
+      <c r="CP17" s="23">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="19" spans="1:93">
+    <row r="19" spans="1:94">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:93">
+    <row r="20" spans="1:94">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3981,7 +4024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:93">
+    <row r="21" spans="1:94">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -4210,8 +4253,11 @@
       <c r="CO21">
         <v>113</v>
       </c>
+      <c r="CP21">
+        <v>113</v>
+      </c>
     </row>
-    <row r="22" spans="1:93">
+    <row r="22" spans="1:94">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4386,8 +4432,11 @@
       <c r="CO22">
         <v>21</v>
       </c>
+      <c r="CP22">
+        <v>16</v>
+      </c>
     </row>
-    <row r="23" spans="1:93">
+    <row r="23" spans="1:94">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4562,8 +4611,11 @@
       <c r="CO23">
         <v>92</v>
       </c>
+      <c r="CP23">
+        <v>97</v>
+      </c>
     </row>
-    <row r="24" spans="1:93">
+    <row r="24" spans="1:94">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4783,8 +4835,11 @@
       <c r="CO24">
         <v>104</v>
       </c>
+      <c r="CP24">
+        <v>69</v>
+      </c>
     </row>
-    <row r="25" spans="1:93">
+    <row r="25" spans="1:94">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -5004,8 +5059,11 @@
       <c r="CO25">
         <v>125</v>
       </c>
+      <c r="CP25">
+        <v>85</v>
+      </c>
     </row>
-    <row r="26" spans="1:93">
+    <row r="26" spans="1:94">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -5225,13 +5283,16 @@
       <c r="CO26">
         <v>1460</v>
       </c>
+      <c r="CP26">
+        <v>1463</v>
+      </c>
     </row>
-    <row r="28" spans="1:93">
+    <row r="28" spans="1:94">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:93">
+    <row r="29" spans="1:94">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5460,8 +5521,11 @@
       <c r="CO29">
         <v>140</v>
       </c>
+      <c r="CP29">
+        <v>140</v>
+      </c>
     </row>
-    <row r="30" spans="1:93">
+    <row r="30" spans="1:94">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5636,8 +5700,11 @@
       <c r="CO30">
         <v>25</v>
       </c>
+      <c r="CP30">
+        <v>25</v>
+      </c>
     </row>
-    <row r="31" spans="1:93">
+    <row r="31" spans="1:94">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5812,8 +5879,11 @@
       <c r="CO31">
         <v>114</v>
       </c>
+      <c r="CP31">
+        <v>114</v>
+      </c>
     </row>
-    <row r="32" spans="1:93">
+    <row r="32" spans="1:94">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -6033,8 +6103,11 @@
       <c r="CO32">
         <v>32</v>
       </c>
+      <c r="CP32">
+        <v>32</v>
+      </c>
     </row>
-    <row r="33" spans="1:93">
+    <row r="33" spans="1:94">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -6254,8 +6327,11 @@
       <c r="CO33">
         <v>57</v>
       </c>
+      <c r="CP33">
+        <v>57</v>
+      </c>
     </row>
-    <row r="34" spans="1:93">
+    <row r="34" spans="1:94">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6475,13 +6551,16 @@
       <c r="CO34">
         <v>1258</v>
       </c>
+      <c r="CP34">
+        <v>1258</v>
+      </c>
     </row>
-    <row r="36" spans="1:93">
+    <row r="36" spans="1:94">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:93">
+    <row r="37" spans="1:94">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -6698,8 +6777,11 @@
       <c r="CO37">
         <v>84</v>
       </c>
+      <c r="CP37">
+        <v>84</v>
+      </c>
     </row>
-    <row r="38" spans="1:93">
+    <row r="38" spans="1:94">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6868,8 +6950,11 @@
       <c r="CO38">
         <v>8</v>
       </c>
+      <c r="CP38">
+        <v>8</v>
+      </c>
     </row>
-    <row r="39" spans="1:93">
+    <row r="39" spans="1:94">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -7038,8 +7123,11 @@
       <c r="CO39">
         <v>75</v>
       </c>
+      <c r="CP39">
+        <v>75</v>
+      </c>
     </row>
-    <row r="40" spans="1:93">
+    <row r="40" spans="1:94">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -7253,8 +7341,11 @@
       <c r="CO40">
         <v>0</v>
       </c>
+      <c r="CP40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:93">
+    <row r="41" spans="1:94">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -7465,8 +7556,11 @@
       <c r="CO41">
         <v>8</v>
       </c>
+      <c r="CP41">
+        <v>8</v>
+      </c>
     </row>
-    <row r="42" spans="1:93">
+    <row r="42" spans="1:94">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7683,8 +7777,11 @@
       <c r="CO42">
         <v>284</v>
       </c>
+      <c r="CP42">
+        <v>284</v>
+      </c>
     </row>
-    <row r="43" spans="1:93">
+    <row r="43" spans="1:94">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -7835,16 +7932,19 @@
       <c r="CO43">
         <v>1</v>
       </c>
+      <c r="CP43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:93">
+    <row r="44" spans="1:94">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:93">
+    <row r="45" spans="1:94">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:93">
+    <row r="46" spans="1:94">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -8067,8 +8167,11 @@
       <c r="CO46">
         <v>207</v>
       </c>
+      <c r="CP46">
+        <v>207</v>
+      </c>
     </row>
-    <row r="47" spans="1:93">
+    <row r="47" spans="1:94">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -8243,8 +8346,11 @@
       <c r="CO47">
         <v>10</v>
       </c>
+      <c r="CP47">
+        <v>6</v>
+      </c>
     </row>
-    <row r="48" spans="1:93">
+    <row r="48" spans="1:94">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -8419,8 +8525,11 @@
       <c r="CO48">
         <v>190</v>
       </c>
+      <c r="CP48">
+        <v>194</v>
+      </c>
     </row>
-    <row r="49" spans="1:93">
+    <row r="49" spans="1:94">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -8640,8 +8749,11 @@
       <c r="CO49">
         <v>336</v>
       </c>
+      <c r="CP49">
+        <v>323</v>
+      </c>
     </row>
-    <row r="50" spans="1:93">
+    <row r="50" spans="1:94">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -8816,8 +8928,11 @@
       <c r="CO50">
         <v>346</v>
       </c>
+      <c r="CP50">
+        <v>329</v>
+      </c>
     </row>
-    <row r="51" spans="1:93">
+    <row r="51" spans="1:94">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -8989,8 +9104,11 @@
       <c r="CO51">
         <v>969</v>
       </c>
+      <c r="CP51">
+        <v>922</v>
+      </c>
     </row>
-    <row r="52" spans="1:93">
+    <row r="52" spans="1:94">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -9156,16 +9274,19 @@
       <c r="CO52">
         <v>1</v>
       </c>
+      <c r="CP52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:93">
+    <row r="53" spans="1:94">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:93">
+    <row r="54" spans="1:94">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:93">
+    <row r="55" spans="1:94">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -9373,8 +9494,11 @@
       <c r="CO55">
         <v>30</v>
       </c>
+      <c r="CP55">
+        <v>30</v>
+      </c>
     </row>
-    <row r="56" spans="1:93">
+    <row r="56" spans="1:94">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -9546,8 +9670,11 @@
       <c r="CO56">
         <v>7</v>
       </c>
+      <c r="CP56">
+        <v>8</v>
+      </c>
     </row>
-    <row r="57" spans="1:93">
+    <row r="57" spans="1:94">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -9719,8 +9846,11 @@
       <c r="CO57">
         <v>22</v>
       </c>
+      <c r="CP57">
+        <v>21</v>
+      </c>
     </row>
-    <row r="58" spans="1:93">
+    <row r="58" spans="1:94">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -9928,8 +10058,11 @@
       <c r="CO58">
         <v>12</v>
       </c>
+      <c r="CP58">
+        <v>12</v>
+      </c>
     </row>
-    <row r="59" spans="1:93">
+    <row r="59" spans="1:94">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -10137,8 +10270,11 @@
       <c r="CO59">
         <v>20</v>
       </c>
+      <c r="CP59">
+        <v>20</v>
+      </c>
     </row>
-    <row r="60" spans="1:93">
+    <row r="60" spans="1:94">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -10346,8 +10482,11 @@
       <c r="CO60">
         <v>149</v>
       </c>
+      <c r="CP60">
+        <v>149</v>
+      </c>
     </row>
-    <row r="61" spans="1:93">
+    <row r="61" spans="1:94">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -10513,8 +10652,11 @@
       <c r="CO61">
         <v>1</v>
       </c>
+      <c r="CP61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:93">
+    <row r="63" spans="1:94">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -10722,8 +10864,11 @@
       <c r="CO63">
         <v>12</v>
       </c>
+      <c r="CP63">
+        <v>12</v>
+      </c>
     </row>
-    <row r="64" spans="1:93">
+    <row r="64" spans="1:94">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -10895,8 +11040,11 @@
       <c r="CO64">
         <v>1</v>
       </c>
+      <c r="CP64">
+        <v>1</v>
+      </c>
     </row>
-    <row r="65" spans="1:93">
+    <row r="65" spans="1:94">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -11068,8 +11216,11 @@
       <c r="CO65">
         <v>12</v>
       </c>
+      <c r="CP65">
+        <v>11</v>
+      </c>
     </row>
-    <row r="66" spans="1:93">
+    <row r="66" spans="1:94">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -11277,8 +11428,11 @@
       <c r="CO66">
         <v>54</v>
       </c>
+      <c r="CP66">
+        <v>54</v>
+      </c>
     </row>
-    <row r="67" spans="1:93">
+    <row r="67" spans="1:94">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -11487,8 +11641,11 @@
       <c r="CO67">
         <v>55</v>
       </c>
+      <c r="CP67">
+        <v>55</v>
+      </c>
     </row>
-    <row r="68" spans="1:93">
+    <row r="68" spans="1:94">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -11696,8 +11853,11 @@
       <c r="CO68">
         <v>0</v>
       </c>
+      <c r="CP68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:93">
+    <row r="69" spans="1:94">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -11869,13 +12029,16 @@
       <c r="CO69">
         <v>0</v>
       </c>
+      <c r="CP69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:93">
+    <row r="70" spans="1:94">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:93">
+    <row r="71" spans="1:94">
       <c r="A71" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -11931,10 +12094,13 @@
       <c r="CO71">
         <v>10</v>
       </c>
+      <c r="CP71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:93">
+    <row r="72" spans="1:94">
       <c r="A72" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
@@ -11990,10 +12156,13 @@
       <c r="CO72">
         <v>4</v>
       </c>
+      <c r="CP72">
+        <v>4</v>
+      </c>
     </row>
-    <row r="73" spans="1:93">
+    <row r="73" spans="1:94">
       <c r="A73" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -12049,10 +12218,13 @@
       <c r="CO73">
         <v>6</v>
       </c>
+      <c r="CP73">
+        <v>6</v>
+      </c>
     </row>
-    <row r="74" spans="1:93">
+    <row r="74" spans="1:94">
       <c r="A74" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
@@ -12108,10 +12280,13 @@
       <c r="CO74">
         <v>4</v>
       </c>
+      <c r="CP74">
+        <v>4</v>
+      </c>
     </row>
-    <row r="75" spans="1:93">
+    <row r="75" spans="1:94">
       <c r="A75" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
@@ -12167,10 +12342,13 @@
       <c r="CO75">
         <v>8</v>
       </c>
+      <c r="CP75">
+        <v>8</v>
+      </c>
     </row>
-    <row r="76" spans="1:93">
+    <row r="76" spans="1:94">
       <c r="A76" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
@@ -12226,13 +12404,16 @@
       <c r="CO76">
         <v>39</v>
       </c>
+      <c r="CP76">
+        <v>39</v>
+      </c>
     </row>
-    <row r="78" spans="1:93">
+    <row r="78" spans="1:94">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:93">
+    <row r="79" spans="1:94">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -12440,8 +12621,11 @@
       <c r="CO79">
         <v>303</v>
       </c>
+      <c r="CP79">
+        <v>303</v>
+      </c>
     </row>
-    <row r="80" spans="1:93">
+    <row r="80" spans="1:94">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -12649,8 +12833,11 @@
       <c r="CO80">
         <v>94</v>
       </c>
+      <c r="CP80">
+        <v>86</v>
+      </c>
     </row>
-    <row r="81" spans="1:93">
+    <row r="81" spans="1:94">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -12858,8 +13045,11 @@
       <c r="CO81">
         <v>87</v>
       </c>
+      <c r="CP81">
+        <v>83</v>
+      </c>
     </row>
-    <row r="82" spans="1:93">
+    <row r="82" spans="1:94">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -13025,8 +13215,11 @@
       <c r="CO82">
         <v>16</v>
       </c>
+      <c r="CP82">
+        <v>17</v>
+      </c>
     </row>
-    <row r="84" spans="1:93">
+    <row r="84" spans="1:94">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -13234,8 +13427,11 @@
       <c r="CO84">
         <v>119</v>
       </c>
+      <c r="CP84">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:93">
+    <row r="85" spans="1:94">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -13443,8 +13639,11 @@
       <c r="CO85">
         <v>24</v>
       </c>
+      <c r="CP85">
+        <v>24</v>
+      </c>
     </row>
-    <row r="86" spans="1:93">
+    <row r="86" spans="1:94">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -13652,8 +13851,11 @@
       <c r="CO86">
         <v>60</v>
       </c>
+      <c r="CP86">
+        <v>60</v>
+      </c>
     </row>
-    <row r="87" spans="1:93">
+    <row r="87" spans="1:94">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -13861,8 +14063,11 @@
       <c r="CO87">
         <v>201</v>
       </c>
+      <c r="CP87">
+        <v>201</v>
+      </c>
     </row>
-    <row r="88" spans="1:93">
+    <row r="88" spans="1:94">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -13944,8 +14149,11 @@
       <c r="CO88">
         <v>1</v>
       </c>
+      <c r="CP88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:93">
+    <row r="90" spans="1:94">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -14153,8 +14361,11 @@
       <c r="CO90">
         <v>81</v>
       </c>
+      <c r="CP90">
+        <v>81</v>
+      </c>
     </row>
-    <row r="91" spans="1:93">
+    <row r="91" spans="1:94">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -14362,8 +14573,11 @@
       <c r="CO91">
         <v>2</v>
       </c>
+      <c r="CP91">
+        <v>2</v>
+      </c>
     </row>
-    <row r="92" spans="1:93">
+    <row r="92" spans="1:94">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -14559,8 +14773,11 @@
       <c r="CO92">
         <v>169</v>
       </c>
+      <c r="CP92">
+        <v>169</v>
+      </c>
     </row>
-    <row r="93" spans="1:93">
+    <row r="93" spans="1:94">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -14768,8 +14985,11 @@
       <c r="CO93">
         <v>62</v>
       </c>
+      <c r="CP93">
+        <v>62</v>
+      </c>
     </row>
-    <row r="94" spans="1:93">
+    <row r="94" spans="1:94">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -14935,16 +15155,19 @@
       <c r="CO94">
         <v>13</v>
       </c>
+      <c r="CP94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:93">
+    <row r="95" spans="1:94">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:93">
+    <row r="96" spans="1:94">
       <c r="A96" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B96" s="41" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="CG96">
         <v>9</v>
@@ -14964,13 +15187,16 @@
       <c r="CO96">
         <v>9</v>
       </c>
+      <c r="CP96">
+        <v>9</v>
+      </c>
     </row>
-    <row r="97" spans="1:93">
+    <row r="97" spans="1:94">
       <c r="A97" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="CG97">
         <v>17</v>
@@ -14990,10 +15216,13 @@
       <c r="CO97">
         <v>9</v>
       </c>
+      <c r="CP97">
+        <v>9</v>
+      </c>
     </row>
-    <row r="98" spans="1:93">
+    <row r="98" spans="1:94">
       <c r="A98" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B98" s="41" t="s">
         <v>12</v>
@@ -15016,10 +15245,13 @@
       <c r="CO98">
         <v>43</v>
       </c>
+      <c r="CP98">
+        <v>43</v>
+      </c>
     </row>
-    <row r="99" spans="1:93">
+    <row r="99" spans="1:94">
       <c r="A99" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B99" s="41" t="s">
         <v>84</v>
@@ -15042,8 +15274,11 @@
       <c r="CO99">
         <v>1</v>
       </c>
+      <c r="CP99">
+        <v>1</v>
+      </c>
     </row>
-    <row r="101" spans="1:93">
+    <row r="101" spans="1:94">
       <c r="A101" s="2" t="s">
         <v>79</v>
       </c>
@@ -15170,8 +15405,11 @@
       <c r="CO101">
         <v>193</v>
       </c>
+      <c r="CP101">
+        <v>193</v>
+      </c>
     </row>
-    <row r="102" spans="1:93">
+    <row r="102" spans="1:94">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -15298,8 +15536,11 @@
       <c r="CO102">
         <v>84</v>
       </c>
+      <c r="CP102">
+        <v>84</v>
+      </c>
     </row>
-    <row r="103" spans="1:93">
+    <row r="103" spans="1:94">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -15424,6 +15665,9 @@
         <v>25</v>
       </c>
       <c r="CO103">
+        <v>25</v>
+      </c>
+      <c r="CP103">
         <v>25</v>
       </c>
     </row>
@@ -15440,20 +15684,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BP11"/>
+  <dimension ref="A2:BQ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BN3" sqref="BN3:BP11"/>
+    <sheetView topLeftCell="BB2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BQ12" sqref="BQ12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:68" s="2" customFormat="1">
+    <row r="2" spans="1:69" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -15658,8 +15902,11 @@
       <c r="BP2" s="9">
         <v>43987</v>
       </c>
+      <c r="BQ2" s="9">
+        <v>43988</v>
+      </c>
     </row>
-    <row r="3" spans="1:68">
+    <row r="3" spans="1:69">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -15864,8 +16111,11 @@
       <c r="BP3">
         <v>1313</v>
       </c>
+      <c r="BQ3">
+        <v>1320</v>
+      </c>
     </row>
-    <row r="4" spans="1:68">
+    <row r="4" spans="1:69">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -16070,8 +16320,11 @@
       <c r="BP4">
         <v>526</v>
       </c>
+      <c r="BQ4">
+        <v>528</v>
+      </c>
     </row>
-    <row r="5" spans="1:68">
+    <row r="5" spans="1:69">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -16276,8 +16529,11 @@
       <c r="BP5">
         <v>435</v>
       </c>
+      <c r="BQ5">
+        <v>437</v>
+      </c>
     </row>
-    <row r="6" spans="1:68">
+    <row r="6" spans="1:69">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -16482,8 +16738,11 @@
       <c r="BP6">
         <v>1943</v>
       </c>
+      <c r="BQ6">
+        <v>1955</v>
+      </c>
     </row>
-    <row r="7" spans="1:68">
+    <row r="7" spans="1:69">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -16688,8 +16947,11 @@
       <c r="BP7">
         <v>1420</v>
       </c>
+      <c r="BQ7">
+        <v>1428</v>
+      </c>
     </row>
-    <row r="8" spans="1:68">
+    <row r="8" spans="1:69">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -16894,8 +17156,11 @@
       <c r="BP8">
         <v>787</v>
       </c>
+      <c r="BQ8">
+        <v>795</v>
+      </c>
     </row>
-    <row r="9" spans="1:68">
+    <row r="9" spans="1:69">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -17100,8 +17365,11 @@
       <c r="BP9">
         <v>1335</v>
       </c>
+      <c r="BQ9">
+        <v>1345</v>
+      </c>
     </row>
-    <row r="10" spans="1:68">
+    <row r="10" spans="1:69">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -17306,8 +17574,11 @@
       <c r="BP10">
         <v>1354</v>
       </c>
+      <c r="BQ10">
+        <v>1367</v>
+      </c>
     </row>
-    <row r="11" spans="1:68">
+    <row r="11" spans="1:69">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -17511,6 +17782,9 @@
       </c>
       <c r="BP11">
         <v>156</v>
+      </c>
+      <c r="BQ11">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -17521,20 +17795,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BK17"/>
+  <dimension ref="A2:BL17"/>
   <sheetViews>
-    <sheetView topLeftCell="AU10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BK17" sqref="BK17"/>
+    <sheetView topLeftCell="AU8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BL17" sqref="BL17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:63" s="2" customFormat="1">
+    <row r="2" spans="1:64" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -17722,8 +17996,11 @@
       <c r="BK2" s="9">
         <v>43987</v>
       </c>
+      <c r="BL2" s="9">
+        <v>43988</v>
+      </c>
     </row>
-    <row r="3" spans="1:63" s="2" customFormat="1">
+    <row r="3" spans="1:64" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -17731,7 +18008,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:63">
+    <row r="4" spans="1:64">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -17921,8 +18198,11 @@
       <c r="BK4">
         <v>9269</v>
       </c>
+      <c r="BL4">
+        <v>9332</v>
+      </c>
     </row>
-    <row r="5" spans="1:63">
+    <row r="5" spans="1:64">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -18112,8 +18392,11 @@
       <c r="BK5">
         <v>1035</v>
       </c>
+      <c r="BL5">
+        <v>1066</v>
+      </c>
     </row>
-    <row r="6" spans="1:63">
+    <row r="6" spans="1:64">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -18303,8 +18586,11 @@
       <c r="BK6">
         <v>1392</v>
       </c>
+      <c r="BL6">
+        <v>1392</v>
+      </c>
     </row>
-    <row r="7" spans="1:63">
+    <row r="7" spans="1:64">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -18494,8 +18780,11 @@
       <c r="BK7">
         <v>4281</v>
       </c>
+      <c r="BL7">
+        <v>4302</v>
+      </c>
     </row>
-    <row r="8" spans="1:63">
+    <row r="8" spans="1:64">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -18685,8 +18974,11 @@
       <c r="BK8">
         <v>108</v>
       </c>
+      <c r="BL8">
+        <v>108</v>
+      </c>
     </row>
-    <row r="9" spans="1:63" ht="30">
+    <row r="9" spans="1:64" ht="28.8">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -18876,8 +19168,11 @@
       <c r="BK9">
         <v>26</v>
       </c>
+      <c r="BL9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:63" ht="30">
+    <row r="10" spans="1:64" ht="28.8">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -19063,8 +19358,11 @@
       <c r="BK10">
         <v>23</v>
       </c>
+      <c r="BL10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:63">
+    <row r="11" spans="1:64">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -19254,8 +19552,11 @@
       <c r="BK11">
         <v>2345</v>
       </c>
+      <c r="BL11">
+        <v>2357</v>
+      </c>
     </row>
-    <row r="12" spans="1:63" ht="30">
+    <row r="12" spans="1:64">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -19445,8 +19746,11 @@
       <c r="BK12">
         <v>59</v>
       </c>
+      <c r="BL12">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:63">
+    <row r="13" spans="1:64">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -19457,7 +19761,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:63">
+    <row r="14" spans="1:64">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -19647,8 +19951,11 @@
       <c r="BK14">
         <v>1654</v>
       </c>
+      <c r="BL14">
+        <v>1694</v>
+      </c>
     </row>
-    <row r="15" spans="1:63">
+    <row r="15" spans="1:64">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -19838,8 +20145,11 @@
       <c r="BK15">
         <v>2456</v>
       </c>
+      <c r="BL15">
+        <v>2460</v>
+      </c>
     </row>
-    <row r="16" spans="1:63">
+    <row r="16" spans="1:64">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -20029,8 +20339,11 @@
       <c r="BK16">
         <v>5133</v>
       </c>
+      <c r="BL16">
+        <v>5152</v>
+      </c>
     </row>
-    <row r="17" spans="1:63" ht="30">
+    <row r="17" spans="1:64">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -20218,6 +20531,9 @@
         <v>26</v>
       </c>
       <c r="BK17">
+        <v>26</v>
+      </c>
+      <c r="BL17">
         <v>26</v>
       </c>
     </row>
@@ -20229,19 +20545,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BK9"/>
+  <dimension ref="A1:BL9"/>
   <sheetViews>
     <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BK8" sqref="BK8"/>
+      <selection activeCell="BL8" sqref="BL8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="2" customFormat="1">
+    <row r="1" spans="1:64" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -20428,14 +20744,17 @@
       <c r="BK1" s="9">
         <v>43987</v>
       </c>
+      <c r="BL1" s="9">
+        <v>43988</v>
+      </c>
     </row>
-    <row r="2" spans="1:63">
+    <row r="2" spans="1:64">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:63">
+    <row r="3" spans="1:64">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -20626,8 +20945,11 @@
       <c r="BK3">
         <v>483</v>
       </c>
+      <c r="BL3">
+        <v>489</v>
+      </c>
     </row>
-    <row r="4" spans="1:63">
+    <row r="4" spans="1:64">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -20817,8 +21139,11 @@
       <c r="BK4">
         <v>7</v>
       </c>
+      <c r="BL4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:63" ht="30">
+    <row r="5" spans="1:64" ht="28.8">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -21008,8 +21333,11 @@
       <c r="BK5">
         <v>361</v>
       </c>
+      <c r="BL5">
+        <v>365</v>
+      </c>
     </row>
-    <row r="6" spans="1:63">
+    <row r="6" spans="1:64">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -21199,8 +21527,11 @@
       <c r="BK6">
         <v>57</v>
       </c>
+      <c r="BL6">
+        <v>59</v>
+      </c>
     </row>
-    <row r="7" spans="1:63" ht="30">
+    <row r="7" spans="1:64">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -21390,8 +21721,11 @@
       <c r="BK7">
         <v>53</v>
       </c>
+      <c r="BL7">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:63">
+    <row r="8" spans="1:64">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -21581,8 +21915,11 @@
       <c r="BK8">
         <v>5</v>
       </c>
+      <c r="BL8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:63">
+    <row r="9" spans="1:64">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -21612,18 +21949,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AW13"/>
+  <dimension ref="A2:AX13"/>
   <sheetViews>
     <sheetView topLeftCell="AJ4" workbookViewId="0">
-      <selection activeCell="AW13" sqref="AW13"/>
+      <selection activeCell="AX13" sqref="AX13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:49" s="2" customFormat="1">
+    <row r="2" spans="1:50" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -21771,8 +22108,11 @@
       <c r="AW2" s="9">
         <v>43987</v>
       </c>
+      <c r="AX2" s="9">
+        <v>43988</v>
+      </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:50">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -21920,8 +22260,11 @@
       <c r="AW3">
         <v>483</v>
       </c>
+      <c r="AX3">
+        <v>489</v>
+      </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:50">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -22069,8 +22412,11 @@
       <c r="AW4">
         <v>51</v>
       </c>
+      <c r="AX4">
+        <v>52</v>
+      </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:50">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -22218,8 +22564,11 @@
       <c r="AW5">
         <v>29</v>
       </c>
+      <c r="AX5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:50">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -22367,8 +22716,11 @@
       <c r="AW6">
         <v>30</v>
       </c>
+      <c r="AX6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:50">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -22516,8 +22868,11 @@
       <c r="AW7">
         <v>68</v>
       </c>
+      <c r="AX7">
+        <v>70</v>
+      </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:50">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -22665,8 +23020,11 @@
       <c r="AW8">
         <v>77</v>
       </c>
+      <c r="AX8">
+        <v>78</v>
+      </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:50">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -22814,8 +23172,11 @@
       <c r="AW9">
         <v>43</v>
       </c>
+      <c r="AX9">
+        <v>43</v>
+      </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:50">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -22963,8 +23324,11 @@
       <c r="AW10">
         <v>70</v>
       </c>
+      <c r="AX10">
+        <v>71</v>
+      </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:50">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -23112,8 +23476,11 @@
       <c r="AW11">
         <v>99</v>
       </c>
+      <c r="AX11">
+        <v>99</v>
+      </c>
     </row>
-    <row r="12" spans="1:49" ht="30">
+    <row r="12" spans="1:50" ht="28.8">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -23261,8 +23628,11 @@
       <c r="AW12">
         <v>16</v>
       </c>
+      <c r="AX12">
+        <v>17</v>
+      </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:50">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -23408,6 +23778,9 @@
         <v>0</v>
       </c>
       <c r="AW13">
+        <v>0</v>
+      </c>
+      <c r="AX13">
         <v>0</v>
       </c>
     </row>
@@ -23419,20 +23792,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O3"/>
+      <selection activeCell="T6" sqref="T6:T23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="C1" s="42" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
@@ -23447,7 +23820,7 @@
       <c r="N1" s="42"/>
       <c r="O1" s="42"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
@@ -23462,7 +23835,7 @@
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -23477,7 +23850,7 @@
       <c r="N3" s="42"/>
       <c r="O3" s="42"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -23492,7 +23865,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -23544,10 +23917,13 @@
       <c r="S5" s="9">
         <v>43987</v>
       </c>
+      <c r="T5" s="9">
+        <v>43988</v>
+      </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C6">
         <v>103</v>
@@ -23600,8 +23976,11 @@
       <c r="S6">
         <v>124</v>
       </c>
+      <c r="T6">
+        <v>124</v>
+      </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -23656,16 +24035,19 @@
       <c r="S7">
         <v>34</v>
       </c>
+      <c r="T7">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:20">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -23720,10 +24102,13 @@
       <c r="S9">
         <v>1</v>
       </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20">
       <c r="A10" s="31" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C10">
         <v>18</v>
@@ -23776,10 +24161,13 @@
       <c r="S10">
         <v>21</v>
       </c>
+      <c r="T10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:20">
       <c r="A11" s="31" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -23832,8 +24220,11 @@
       <c r="S11">
         <v>9</v>
       </c>
+      <c r="T11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -23888,13 +24279,16 @@
       <c r="S12">
         <v>3</v>
       </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:20">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -23949,8 +24343,11 @@
       <c r="S14">
         <v>1</v>
       </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -24005,8 +24402,11 @@
       <c r="S15">
         <v>0</v>
       </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -24061,8 +24461,11 @@
       <c r="S16">
         <v>3</v>
       </c>
+      <c r="T16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:20">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -24117,8 +24520,11 @@
       <c r="S17">
         <v>11</v>
       </c>
+      <c r="T17">
+        <v>11</v>
+      </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:20">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -24173,8 +24579,11 @@
       <c r="S18">
         <v>3</v>
       </c>
+      <c r="T18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:20">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -24229,8 +24638,11 @@
       <c r="S19">
         <v>3</v>
       </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:20">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -24285,8 +24697,11 @@
       <c r="S20">
         <v>2</v>
       </c>
+      <c r="T20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:20">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -24341,8 +24756,11 @@
       <c r="S21">
         <v>6</v>
       </c>
+      <c r="T21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:19" ht="45">
+    <row r="22" spans="1:20" ht="28.8">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -24397,10 +24815,13 @@
       <c r="S22">
         <v>2</v>
       </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
     </row>
-    <row r="23" spans="1:19" ht="30">
+    <row r="23" spans="1:20" ht="28.8">
       <c r="A23" s="39" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -24451,6 +24872,9 @@
         <v>1</v>
       </c>
       <c r="S23">
+        <v>3</v>
+      </c>
+      <c r="T23">
         <v>3</v>
       </c>
     </row>
@@ -24464,26 +24888,26 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -24497,22 +24921,22 @@
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>120</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1">
@@ -24530,7 +24954,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A4" s="45"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -24543,7 +24967,7 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A5" s="45"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
@@ -24554,7 +24978,7 @@
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A6" s="45"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -24565,7 +24989,7 @@
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A7" s="45"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
@@ -24576,219 +25000,219 @@
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.45" customHeight="1">
+    <row r="8" spans="1:7" ht="14.4" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C8" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="28">
         <v>0</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="F8" s="28">
         <v>0</v>
       </c>
       <c r="G8" s="28">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.45" customHeight="1">
+    <row r="9" spans="1:7" ht="14.4" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>96</v>
       </c>
       <c r="B9" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="28">
+        <v>4</v>
+      </c>
+      <c r="D9" s="28">
+        <v>0</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="28">
+        <v>1</v>
+      </c>
+      <c r="G9" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A10" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="28">
+        <v>20</v>
+      </c>
+      <c r="D10" s="28">
+        <v>0</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0</v>
+      </c>
+      <c r="G10" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A11" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="28">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0</v>
+      </c>
+      <c r="G11" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A12" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0</v>
+      </c>
+      <c r="G12" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A13" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="28">
+        <v>2</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0</v>
+      </c>
+      <c r="G13" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A14" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="28">
-        <v>3</v>
-      </c>
-      <c r="D9" s="28">
-        <v>0</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="28">
-        <v>0</v>
-      </c>
-      <c r="G9" s="28">
-        <v>0</v>
+      <c r="C14" s="28">
+        <v>12</v>
+      </c>
+      <c r="D14" s="28">
+        <v>0</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="28">
+        <v>1</v>
+      </c>
+      <c r="G14" s="28">
+        <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A10" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="28">
-        <v>4</v>
-      </c>
-      <c r="D10" s="28">
-        <v>0</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" s="28">
-        <v>1</v>
-      </c>
-      <c r="G10" s="28">
-        <v>0</v>
+    <row r="15" spans="1:7" ht="15" customHeight="1">
+      <c r="A15" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="28">
+        <v>5</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F15" s="28">
+        <v>0</v>
+      </c>
+      <c r="G15" s="28">
+        <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A11" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="28">
-        <v>18</v>
-      </c>
-      <c r="D11" s="28">
-        <v>0</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11" s="28">
-        <v>0</v>
-      </c>
-      <c r="G11" s="28">
-        <v>0</v>
+    <row r="16" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A16" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="28">
+        <v>9</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="28">
+        <v>1</v>
+      </c>
+      <c r="G16" s="28">
+        <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A12" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="28">
-        <v>0</v>
-      </c>
-      <c r="D12" s="28">
-        <v>0</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="28">
-        <v>0</v>
-      </c>
-      <c r="G12" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A13" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="28">
-        <v>0</v>
-      </c>
-      <c r="D13" s="28">
-        <v>0</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F13" s="28">
-        <v>0</v>
-      </c>
-      <c r="G13" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A14" s="27" t="s">
+    <row r="17" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A17" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="28">
-        <v>2</v>
-      </c>
-      <c r="D14" s="28">
-        <v>0</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="28">
-        <v>0</v>
-      </c>
-      <c r="G14" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A15" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="C15" s="28">
-        <v>15</v>
-      </c>
-      <c r="D15" s="28">
-        <v>0</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="F15" s="28">
-        <v>1</v>
-      </c>
-      <c r="G15" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
-      <c r="A16" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" s="28">
-        <v>6</v>
-      </c>
-      <c r="D16" s="28">
-        <v>0</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="F16" s="28">
-        <v>0</v>
-      </c>
-      <c r="G16" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A17" s="27" t="s">
-        <v>105</v>
-      </c>
       <c r="B17" s="28" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
       <c r="C17" s="28">
         <v>9</v>
@@ -24797,21 +25221,21 @@
         <v>0</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="F17" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.45" customHeight="1">
+    <row r="18" spans="1:7" ht="14.4" customHeight="1">
       <c r="A18" s="27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C18" s="28">
         <v>12</v>
@@ -24820,113 +25244,113 @@
         <v>0</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="F18" s="28">
         <v>0</v>
       </c>
       <c r="G18" s="28">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.45" customHeight="1">
+    <row r="19" spans="1:7" ht="14.4" customHeight="1">
       <c r="A19" s="27" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C19" s="28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" s="28">
         <v>0</v>
       </c>
       <c r="E19" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="28">
+        <v>0</v>
+      </c>
+      <c r="G19" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A20" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="28">
+        <v>1</v>
+      </c>
+      <c r="D20" s="28">
+        <v>0</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="28">
+        <v>0</v>
+      </c>
+      <c r="G20" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A21" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="28">
+        <v>26</v>
+      </c>
+      <c r="D21" s="28">
+        <v>0</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="28">
+        <v>1</v>
+      </c>
+      <c r="G21" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A22" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="28">
+        <v>7</v>
+      </c>
+      <c r="D22" s="28">
+        <v>0</v>
+      </c>
+      <c r="E22" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="28">
-        <v>0</v>
-      </c>
-      <c r="G19" s="28">
-        <v>0</v>
+      <c r="F22" s="28">
+        <v>1</v>
+      </c>
+      <c r="G22" s="28">
+        <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A20" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" s="28">
-        <v>17</v>
-      </c>
-      <c r="D20" s="28">
-        <v>0</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="28">
-        <v>0</v>
-      </c>
-      <c r="G20" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A21" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="28" t="s">
+    <row r="23" spans="1:7" ht="18" customHeight="1">
+      <c r="A23" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="28">
-        <v>1</v>
-      </c>
-      <c r="D21" s="28">
-        <v>0</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="28">
-        <v>0</v>
-      </c>
-      <c r="G21" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A22" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="28">
-        <v>26</v>
-      </c>
-      <c r="D22" s="28">
-        <v>0</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="F22" s="28">
-        <v>1</v>
-      </c>
-      <c r="G22" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" customHeight="1">
-      <c r="A23" s="27" t="s">
-        <v>114</v>
-      </c>
       <c r="B23" s="28" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="C23" s="28">
         <v>6</v>
@@ -24935,104 +25359,108 @@
         <v>0</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="F23" s="28">
         <v>0</v>
       </c>
       <c r="G23" s="28">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1">
-      <c r="A24" s="27" t="s">
-        <v>116</v>
+    <row r="24" spans="1:7" ht="33.6" customHeight="1">
+      <c r="A24" s="30" t="s">
+        <v>119</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C24" s="28">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D24" s="28">
         <v>0</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="F24" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="33.6" customHeight="1">
+    <row r="25" spans="1:7" ht="17.399999999999999" customHeight="1">
       <c r="A25" s="30" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C25" s="28">
-        <v>22</v>
+        <v>149</v>
       </c>
       <c r="D25" s="28">
         <v>0</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="F25" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G25" s="28">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.45" customHeight="1">
-      <c r="A26" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="C26" s="28">
-        <v>165</v>
-      </c>
-      <c r="D26" s="28">
-        <v>0</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="F26" s="28">
-        <v>5</v>
-      </c>
-      <c r="G26" s="28">
-        <v>2</v>
-      </c>
+    <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1">
+      <c r="A26" s="30"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75">
-      <c r="A27" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
+    <row r="27" spans="1:7" ht="17.399999999999999" customHeight="1">
+      <c r="A27" s="30"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="28"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
     </row>
-    <row r="28" spans="1:7">
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
+    <row r="28" spans="1:7" ht="17.399999999999999" customHeight="1">
+      <c r="A28" s="30"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.6">
+      <c r="A29" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -25047,12 +25475,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -25255,6 +25677,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -25265,23 +25693,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25300,6 +25711,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
08 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8728DFDE-C46A-402C-857F-CE80BAAC8B6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{8728DFDE-C46A-402C-857F-CE80BAAC8B6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{08D0E30E-110C-415F-8AAC-358A986B5DFF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="7296" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -453,35 +453,6 @@
     <t>2; (1)</t>
   </si>
   <si>
-    <t>As of June 6, 2020</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As of June 6, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>124 cases</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for COVID-19 testing,  and 34 (27.4%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
-    </r>
-  </si>
-  <si>
     <t>10; (7)</t>
   </si>
   <si>
@@ -561,6 +532,35 @@
   </si>
   <si>
     <t>909; (497)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As of June 7, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>124 cases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for COVID-19 testing,  and 34 (27.4%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
+    </r>
+  </si>
+  <si>
+    <t>As of June 7, 2020</t>
   </si>
 </sst>
 </file>
@@ -837,14 +837,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>394</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>158115</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1194,11 +1194,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CP118"/>
+  <dimension ref="A1:CQ118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="CG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CP103" sqref="CP103"/>
+      <selection pane="topRight" activeCell="CQ1" sqref="CQ1:CQ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1213,7 +1213,7 @@
     <col min="80" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94">
+    <row r="1" spans="1:95">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1490,8 +1490,11 @@
       <c r="CP1" s="1">
         <v>43988</v>
       </c>
+      <c r="CQ1" s="1">
+        <v>43989</v>
+      </c>
     </row>
-    <row r="2" spans="1:94">
+    <row r="2" spans="1:95">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1518,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:94">
+    <row r="3" spans="1:95">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1777,8 +1780,11 @@
       <c r="CP3">
         <v>54547</v>
       </c>
+      <c r="CQ3">
+        <v>55766</v>
+      </c>
     </row>
-    <row r="4" spans="1:94">
+    <row r="4" spans="1:95">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1835,8 +1841,11 @@
       <c r="CP4">
         <v>44485</v>
       </c>
+      <c r="CQ4">
+        <v>45362</v>
+      </c>
     </row>
-    <row r="5" spans="1:94">
+    <row r="5" spans="1:95">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2119,8 +2128,11 @@
       <c r="CP5">
         <v>9332</v>
       </c>
+      <c r="CQ5">
+        <v>9389</v>
+      </c>
     </row>
-    <row r="6" spans="1:94">
+    <row r="6" spans="1:95">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2385,8 +2397,11 @@
       <c r="CP6">
         <v>489</v>
       </c>
+      <c r="CQ6">
+        <v>491</v>
+      </c>
     </row>
-    <row r="7" spans="1:94">
+    <row r="7" spans="1:95">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2621,11 +2636,14 @@
       <c r="CP7">
         <v>1143</v>
       </c>
+      <c r="CQ7">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="8" spans="1:94">
+    <row r="8" spans="1:95">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:94">
+    <row r="9" spans="1:95">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2752,8 +2770,11 @@
       <c r="CP9">
         <v>345</v>
       </c>
+      <c r="CQ9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:94">
+    <row r="10" spans="1:95">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2982,8 +3003,11 @@
       <c r="CP10">
         <v>114</v>
       </c>
+      <c r="CQ10">
+        <v>61</v>
+      </c>
     </row>
-    <row r="11" spans="1:94">
+    <row r="11" spans="1:95">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3212,8 +3236,11 @@
       <c r="CP11">
         <v>440</v>
       </c>
+      <c r="CQ11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:94">
+    <row r="12" spans="1:95">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3442,8 +3469,11 @@
       <c r="CP12">
         <v>200</v>
       </c>
+      <c r="CQ12">
+        <v>199</v>
+      </c>
     </row>
-    <row r="13" spans="1:94">
+    <row r="13" spans="1:95">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3672,8 +3702,11 @@
       <c r="CP13">
         <v>240</v>
       </c>
+      <c r="CQ13">
+        <v>241</v>
+      </c>
     </row>
-    <row r="14" spans="1:94">
+    <row r="14" spans="1:95">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3764,8 +3797,11 @@
       <c r="CP14">
         <v>285</v>
       </c>
+      <c r="CQ14">
+        <v>268</v>
+      </c>
     </row>
-    <row r="15" spans="1:94">
+    <row r="15" spans="1:95">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3826,8 +3862,11 @@
       <c r="CP15">
         <v>90</v>
       </c>
+      <c r="CQ15">
+        <v>102</v>
+      </c>
     </row>
-    <row r="16" spans="1:94">
+    <row r="16" spans="1:95">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -3918,8 +3957,11 @@
       <c r="CP16">
         <v>1863</v>
       </c>
+      <c r="CQ16">
+        <v>1854</v>
+      </c>
     </row>
-    <row r="17" spans="1:94">
+    <row r="17" spans="1:95">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -4010,13 +4052,16 @@
       <c r="CP17" s="23">
         <v>0.75</v>
       </c>
+      <c r="CQ17" s="23">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="19" spans="1:94">
+    <row r="19" spans="1:95">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:94">
+    <row r="20" spans="1:95">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -4024,7 +4069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:94">
+    <row r="21" spans="1:95">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -4256,8 +4301,11 @@
       <c r="CP21">
         <v>113</v>
       </c>
+      <c r="CQ21">
+        <v>113</v>
+      </c>
     </row>
-    <row r="22" spans="1:94">
+    <row r="22" spans="1:95">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4435,8 +4483,11 @@
       <c r="CP22">
         <v>16</v>
       </c>
+      <c r="CQ22">
+        <v>16</v>
+      </c>
     </row>
-    <row r="23" spans="1:94">
+    <row r="23" spans="1:95">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4614,8 +4665,11 @@
       <c r="CP23">
         <v>97</v>
       </c>
+      <c r="CQ23">
+        <v>97</v>
+      </c>
     </row>
-    <row r="24" spans="1:94">
+    <row r="24" spans="1:95">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4838,8 +4892,11 @@
       <c r="CP24">
         <v>69</v>
       </c>
+      <c r="CQ24">
+        <v>66</v>
+      </c>
     </row>
-    <row r="25" spans="1:94">
+    <row r="25" spans="1:95">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -5062,8 +5119,11 @@
       <c r="CP25">
         <v>85</v>
       </c>
+      <c r="CQ25">
+        <v>82</v>
+      </c>
     </row>
-    <row r="26" spans="1:94">
+    <row r="26" spans="1:95">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -5286,13 +5346,16 @@
       <c r="CP26">
         <v>1463</v>
       </c>
+      <c r="CQ26">
+        <v>1482</v>
+      </c>
     </row>
-    <row r="28" spans="1:94">
+    <row r="28" spans="1:95">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:94">
+    <row r="29" spans="1:95">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5524,8 +5587,11 @@
       <c r="CP29">
         <v>140</v>
       </c>
+      <c r="CQ29">
+        <v>140</v>
+      </c>
     </row>
-    <row r="30" spans="1:94">
+    <row r="30" spans="1:95">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5703,8 +5769,11 @@
       <c r="CP30">
         <v>25</v>
       </c>
+      <c r="CQ30">
+        <v>25</v>
+      </c>
     </row>
-    <row r="31" spans="1:94">
+    <row r="31" spans="1:95">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5882,8 +5951,11 @@
       <c r="CP31">
         <v>114</v>
       </c>
+      <c r="CQ31">
+        <v>114</v>
+      </c>
     </row>
-    <row r="32" spans="1:94">
+    <row r="32" spans="1:95">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -6106,8 +6178,11 @@
       <c r="CP32">
         <v>32</v>
       </c>
+      <c r="CQ32">
+        <v>32</v>
+      </c>
     </row>
-    <row r="33" spans="1:94">
+    <row r="33" spans="1:95">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -6330,8 +6405,11 @@
       <c r="CP33">
         <v>57</v>
       </c>
+      <c r="CQ33">
+        <v>57</v>
+      </c>
     </row>
-    <row r="34" spans="1:94">
+    <row r="34" spans="1:95">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6554,13 +6632,16 @@
       <c r="CP34">
         <v>1258</v>
       </c>
+      <c r="CQ34">
+        <v>1258</v>
+      </c>
     </row>
-    <row r="36" spans="1:94">
+    <row r="36" spans="1:95">
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:94">
+    <row r="37" spans="1:95">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -6780,8 +6861,11 @@
       <c r="CP37">
         <v>84</v>
       </c>
+      <c r="CQ37">
+        <v>84</v>
+      </c>
     </row>
-    <row r="38" spans="1:94">
+    <row r="38" spans="1:95">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6953,8 +7037,11 @@
       <c r="CP38">
         <v>8</v>
       </c>
+      <c r="CQ38">
+        <v>8</v>
+      </c>
     </row>
-    <row r="39" spans="1:94">
+    <row r="39" spans="1:95">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -7126,8 +7213,11 @@
       <c r="CP39">
         <v>75</v>
       </c>
+      <c r="CQ39">
+        <v>75</v>
+      </c>
     </row>
-    <row r="40" spans="1:94">
+    <row r="40" spans="1:95">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -7344,8 +7434,11 @@
       <c r="CP40">
         <v>0</v>
       </c>
+      <c r="CQ40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:94">
+    <row r="41" spans="1:95">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -7559,8 +7652,11 @@
       <c r="CP41">
         <v>8</v>
       </c>
+      <c r="CQ41">
+        <v>8</v>
+      </c>
     </row>
-    <row r="42" spans="1:94">
+    <row r="42" spans="1:95">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7780,8 +7876,11 @@
       <c r="CP42">
         <v>284</v>
       </c>
+      <c r="CQ42">
+        <v>284</v>
+      </c>
     </row>
-    <row r="43" spans="1:94">
+    <row r="43" spans="1:95">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -7935,16 +8034,19 @@
       <c r="CP43">
         <v>1</v>
       </c>
+      <c r="CQ43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:94">
+    <row r="44" spans="1:95">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:94">
+    <row r="45" spans="1:95">
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:94">
+    <row r="46" spans="1:95">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -8170,8 +8272,11 @@
       <c r="CP46">
         <v>207</v>
       </c>
+      <c r="CQ46">
+        <v>207</v>
+      </c>
     </row>
-    <row r="47" spans="1:94">
+    <row r="47" spans="1:95">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -8349,8 +8454,11 @@
       <c r="CP47">
         <v>6</v>
       </c>
+      <c r="CQ47">
+        <v>6</v>
+      </c>
     </row>
-    <row r="48" spans="1:94">
+    <row r="48" spans="1:95">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -8528,8 +8636,11 @@
       <c r="CP48">
         <v>194</v>
       </c>
+      <c r="CQ48">
+        <v>194</v>
+      </c>
     </row>
-    <row r="49" spans="1:94">
+    <row r="49" spans="1:95">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -8752,8 +8863,11 @@
       <c r="CP49">
         <v>323</v>
       </c>
+      <c r="CQ49">
+        <v>315</v>
+      </c>
     </row>
-    <row r="50" spans="1:94">
+    <row r="50" spans="1:95">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -8931,8 +9045,11 @@
       <c r="CP50">
         <v>329</v>
       </c>
+      <c r="CQ50">
+        <v>321</v>
+      </c>
     </row>
-    <row r="51" spans="1:94">
+    <row r="51" spans="1:95">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -9107,8 +9224,11 @@
       <c r="CP51">
         <v>922</v>
       </c>
+      <c r="CQ51">
+        <v>937</v>
+      </c>
     </row>
-    <row r="52" spans="1:94">
+    <row r="52" spans="1:95">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -9277,16 +9397,19 @@
       <c r="CP52">
         <v>1</v>
       </c>
+      <c r="CQ52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:94">
+    <row r="53" spans="1:95">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:94">
+    <row r="54" spans="1:95">
       <c r="B54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:94">
+    <row r="55" spans="1:95">
       <c r="A55" s="2" t="s">
         <v>18</v>
       </c>
@@ -9497,8 +9620,11 @@
       <c r="CP55">
         <v>30</v>
       </c>
+      <c r="CQ55">
+        <v>30</v>
+      </c>
     </row>
-    <row r="56" spans="1:94">
+    <row r="56" spans="1:95">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -9673,8 +9799,11 @@
       <c r="CP56">
         <v>8</v>
       </c>
+      <c r="CQ56">
+        <v>8</v>
+      </c>
     </row>
-    <row r="57" spans="1:94">
+    <row r="57" spans="1:95">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -9849,8 +9978,11 @@
       <c r="CP57">
         <v>21</v>
       </c>
+      <c r="CQ57">
+        <v>21</v>
+      </c>
     </row>
-    <row r="58" spans="1:94">
+    <row r="58" spans="1:95">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -10061,8 +10193,11 @@
       <c r="CP58">
         <v>12</v>
       </c>
+      <c r="CQ58">
+        <v>12</v>
+      </c>
     </row>
-    <row r="59" spans="1:94">
+    <row r="59" spans="1:95">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -10273,8 +10408,11 @@
       <c r="CP59">
         <v>20</v>
       </c>
+      <c r="CQ59">
+        <v>20</v>
+      </c>
     </row>
-    <row r="60" spans="1:94">
+    <row r="60" spans="1:95">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -10485,8 +10623,11 @@
       <c r="CP60">
         <v>149</v>
       </c>
+      <c r="CQ60">
+        <v>149</v>
+      </c>
     </row>
-    <row r="61" spans="1:94">
+    <row r="61" spans="1:95">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -10655,8 +10796,11 @@
       <c r="CP61">
         <v>1</v>
       </c>
+      <c r="CQ61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:94">
+    <row r="63" spans="1:95">
       <c r="A63" s="2" t="s">
         <v>20</v>
       </c>
@@ -10867,8 +11011,11 @@
       <c r="CP63">
         <v>12</v>
       </c>
+      <c r="CQ63">
+        <v>12</v>
+      </c>
     </row>
-    <row r="64" spans="1:94">
+    <row r="64" spans="1:95">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -11043,8 +11190,11 @@
       <c r="CP64">
         <v>1</v>
       </c>
+      <c r="CQ64">
+        <v>1</v>
+      </c>
     </row>
-    <row r="65" spans="1:94">
+    <row r="65" spans="1:95">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -11219,8 +11369,11 @@
       <c r="CP65">
         <v>11</v>
       </c>
+      <c r="CQ65">
+        <v>11</v>
+      </c>
     </row>
-    <row r="66" spans="1:94">
+    <row r="66" spans="1:95">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -11431,8 +11584,11 @@
       <c r="CP66">
         <v>54</v>
       </c>
+      <c r="CQ66">
+        <v>54</v>
+      </c>
     </row>
-    <row r="67" spans="1:94">
+    <row r="67" spans="1:95">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -11644,8 +11800,11 @@
       <c r="CP67">
         <v>55</v>
       </c>
+      <c r="CQ67">
+        <v>55</v>
+      </c>
     </row>
-    <row r="68" spans="1:94">
+    <row r="68" spans="1:95">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -11856,8 +12015,11 @@
       <c r="CP68">
         <v>0</v>
       </c>
+      <c r="CQ68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:94">
+    <row r="69" spans="1:95">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -12032,11 +12194,14 @@
       <c r="CP69">
         <v>0</v>
       </c>
+      <c r="CQ69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:94">
+    <row r="70" spans="1:95">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:94">
+    <row r="71" spans="1:95">
       <c r="A71" s="2" t="s">
         <v>121</v>
       </c>
@@ -12097,8 +12262,11 @@
       <c r="CP71">
         <v>10</v>
       </c>
+      <c r="CQ71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="1:94">
+    <row r="72" spans="1:95">
       <c r="A72" s="2" t="s">
         <v>121</v>
       </c>
@@ -12159,8 +12327,11 @@
       <c r="CP72">
         <v>4</v>
       </c>
+      <c r="CQ72">
+        <v>4</v>
+      </c>
     </row>
-    <row r="73" spans="1:94">
+    <row r="73" spans="1:95">
       <c r="A73" s="2" t="s">
         <v>121</v>
       </c>
@@ -12221,8 +12392,11 @@
       <c r="CP73">
         <v>6</v>
       </c>
+      <c r="CQ73">
+        <v>6</v>
+      </c>
     </row>
-    <row r="74" spans="1:94">
+    <row r="74" spans="1:95">
       <c r="A74" s="2" t="s">
         <v>121</v>
       </c>
@@ -12283,8 +12457,11 @@
       <c r="CP74">
         <v>4</v>
       </c>
+      <c r="CQ74">
+        <v>4</v>
+      </c>
     </row>
-    <row r="75" spans="1:94">
+    <row r="75" spans="1:95">
       <c r="A75" s="2" t="s">
         <v>121</v>
       </c>
@@ -12345,8 +12522,11 @@
       <c r="CP75">
         <v>8</v>
       </c>
+      <c r="CQ75">
+        <v>8</v>
+      </c>
     </row>
-    <row r="76" spans="1:94">
+    <row r="76" spans="1:95">
       <c r="A76" s="2" t="s">
         <v>121</v>
       </c>
@@ -12407,13 +12587,16 @@
       <c r="CP76">
         <v>39</v>
       </c>
+      <c r="CQ76">
+        <v>39</v>
+      </c>
     </row>
-    <row r="78" spans="1:94">
+    <row r="78" spans="1:95">
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:94">
+    <row r="79" spans="1:95">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
@@ -12624,8 +12807,11 @@
       <c r="CP79">
         <v>303</v>
       </c>
+      <c r="CQ79">
+        <v>304</v>
+      </c>
     </row>
-    <row r="80" spans="1:94">
+    <row r="80" spans="1:95">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -12836,8 +13022,11 @@
       <c r="CP80">
         <v>86</v>
       </c>
+      <c r="CQ80">
+        <v>79</v>
+      </c>
     </row>
-    <row r="81" spans="1:94">
+    <row r="81" spans="1:95">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -13048,8 +13237,11 @@
       <c r="CP81">
         <v>83</v>
       </c>
+      <c r="CQ81">
+        <v>76</v>
+      </c>
     </row>
-    <row r="82" spans="1:94">
+    <row r="82" spans="1:95">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -13218,8 +13410,11 @@
       <c r="CP82">
         <v>17</v>
       </c>
+      <c r="CQ82">
+        <v>17</v>
+      </c>
     </row>
-    <row r="84" spans="1:94">
+    <row r="84" spans="1:95">
       <c r="A84" s="2" t="s">
         <v>28</v>
       </c>
@@ -13430,8 +13625,11 @@
       <c r="CP84">
         <v>119</v>
       </c>
+      <c r="CQ84">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:94">
+    <row r="85" spans="1:95">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -13642,8 +13840,11 @@
       <c r="CP85">
         <v>24</v>
       </c>
+      <c r="CQ85">
+        <v>24</v>
+      </c>
     </row>
-    <row r="86" spans="1:94">
+    <row r="86" spans="1:95">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -13854,8 +14055,11 @@
       <c r="CP86">
         <v>60</v>
       </c>
+      <c r="CQ86">
+        <v>60</v>
+      </c>
     </row>
-    <row r="87" spans="1:94">
+    <row r="87" spans="1:95">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -14066,8 +14270,11 @@
       <c r="CP87">
         <v>201</v>
       </c>
+      <c r="CQ87">
+        <v>201</v>
+      </c>
     </row>
-    <row r="88" spans="1:94">
+    <row r="88" spans="1:95">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -14152,8 +14359,11 @@
       <c r="CP88">
         <v>1</v>
       </c>
+      <c r="CQ88">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:94">
+    <row r="90" spans="1:95">
       <c r="A90" s="2" t="s">
         <v>29</v>
       </c>
@@ -14364,8 +14574,11 @@
       <c r="CP90">
         <v>81</v>
       </c>
+      <c r="CQ90">
+        <v>81</v>
+      </c>
     </row>
-    <row r="91" spans="1:94">
+    <row r="91" spans="1:95">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -14576,8 +14789,11 @@
       <c r="CP91">
         <v>2</v>
       </c>
+      <c r="CQ91">
+        <v>2</v>
+      </c>
     </row>
-    <row r="92" spans="1:94">
+    <row r="92" spans="1:95">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -14776,8 +14992,11 @@
       <c r="CP92">
         <v>169</v>
       </c>
+      <c r="CQ92">
+        <v>169</v>
+      </c>
     </row>
-    <row r="93" spans="1:94">
+    <row r="93" spans="1:95">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -14988,8 +15207,11 @@
       <c r="CP93">
         <v>62</v>
       </c>
+      <c r="CQ93">
+        <v>62</v>
+      </c>
     </row>
-    <row r="94" spans="1:94">
+    <row r="94" spans="1:95">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -15158,11 +15380,14 @@
       <c r="CP94">
         <v>13</v>
       </c>
+      <c r="CQ94">
+        <v>13</v>
+      </c>
     </row>
-    <row r="95" spans="1:94">
+    <row r="95" spans="1:95">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:94">
+    <row r="96" spans="1:95">
       <c r="A96" s="2" t="s">
         <v>134</v>
       </c>
@@ -15190,8 +15415,11 @@
       <c r="CP96">
         <v>9</v>
       </c>
+      <c r="CQ96">
+        <v>9</v>
+      </c>
     </row>
-    <row r="97" spans="1:94">
+    <row r="97" spans="1:95">
       <c r="A97" s="2" t="s">
         <v>134</v>
       </c>
@@ -15219,8 +15447,11 @@
       <c r="CP97">
         <v>9</v>
       </c>
+      <c r="CQ97">
+        <v>9</v>
+      </c>
     </row>
-    <row r="98" spans="1:94">
+    <row r="98" spans="1:95">
       <c r="A98" s="2" t="s">
         <v>134</v>
       </c>
@@ -15248,8 +15479,11 @@
       <c r="CP98">
         <v>43</v>
       </c>
+      <c r="CQ98">
+        <v>43</v>
+      </c>
     </row>
-    <row r="99" spans="1:94">
+    <row r="99" spans="1:95">
       <c r="A99" s="2" t="s">
         <v>134</v>
       </c>
@@ -15277,8 +15511,11 @@
       <c r="CP99">
         <v>1</v>
       </c>
+      <c r="CQ99">
+        <v>1</v>
+      </c>
     </row>
-    <row r="101" spans="1:94">
+    <row r="101" spans="1:95">
       <c r="A101" s="2" t="s">
         <v>79</v>
       </c>
@@ -15408,8 +15645,11 @@
       <c r="CP101">
         <v>193</v>
       </c>
+      <c r="CQ101">
+        <v>193</v>
+      </c>
     </row>
-    <row r="102" spans="1:94">
+    <row r="102" spans="1:95">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -15539,8 +15779,11 @@
       <c r="CP102">
         <v>84</v>
       </c>
+      <c r="CQ102">
+        <v>84</v>
+      </c>
     </row>
-    <row r="103" spans="1:94">
+    <row r="103" spans="1:95">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -15668,6 +15911,9 @@
         <v>25</v>
       </c>
       <c r="CP103">
+        <v>25</v>
+      </c>
+      <c r="CQ103">
         <v>25</v>
       </c>
     </row>
@@ -15684,10 +15930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BQ11"/>
+  <dimension ref="A2:BR11"/>
   <sheetViews>
     <sheetView topLeftCell="BB2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BQ12" sqref="BQ12"/>
+      <selection activeCell="BR11" sqref="BR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15697,7 +15943,7 @@
     <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:69" s="2" customFormat="1">
+    <row r="2" spans="1:70" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -15905,8 +16151,11 @@
       <c r="BQ2" s="9">
         <v>43988</v>
       </c>
+      <c r="BR2" s="9">
+        <v>43989</v>
+      </c>
     </row>
-    <row r="3" spans="1:69">
+    <row r="3" spans="1:70">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -16114,8 +16363,11 @@
       <c r="BQ3">
         <v>1320</v>
       </c>
+      <c r="BR3">
+        <v>1335</v>
+      </c>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:70">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -16323,8 +16575,11 @@
       <c r="BQ4">
         <v>528</v>
       </c>
+      <c r="BR4">
+        <v>527</v>
+      </c>
     </row>
-    <row r="5" spans="1:69">
+    <row r="5" spans="1:70">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -16532,8 +16787,11 @@
       <c r="BQ5">
         <v>437</v>
       </c>
+      <c r="BR5">
+        <v>438</v>
+      </c>
     </row>
-    <row r="6" spans="1:69">
+    <row r="6" spans="1:70">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -16741,8 +16999,11 @@
       <c r="BQ6">
         <v>1955</v>
       </c>
+      <c r="BR6">
+        <v>1964</v>
+      </c>
     </row>
-    <row r="7" spans="1:69">
+    <row r="7" spans="1:70">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -16950,8 +17211,11 @@
       <c r="BQ7">
         <v>1428</v>
       </c>
+      <c r="BR7">
+        <v>1433</v>
+      </c>
     </row>
-    <row r="8" spans="1:69">
+    <row r="8" spans="1:70">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -17159,8 +17423,11 @@
       <c r="BQ8">
         <v>795</v>
       </c>
+      <c r="BR8">
+        <v>798</v>
+      </c>
     </row>
-    <row r="9" spans="1:69">
+    <row r="9" spans="1:70">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -17368,8 +17635,11 @@
       <c r="BQ9">
         <v>1345</v>
       </c>
+      <c r="BR9">
+        <v>1351</v>
+      </c>
     </row>
-    <row r="10" spans="1:69">
+    <row r="10" spans="1:70">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -17577,8 +17847,11 @@
       <c r="BQ10">
         <v>1367</v>
       </c>
+      <c r="BR10">
+        <v>1379</v>
+      </c>
     </row>
-    <row r="11" spans="1:69">
+    <row r="11" spans="1:70">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -17785,6 +18058,9 @@
       </c>
       <c r="BQ11">
         <v>157</v>
+      </c>
+      <c r="BR11">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -17795,10 +18071,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BL17"/>
+  <dimension ref="A2:BM17"/>
   <sheetViews>
-    <sheetView topLeftCell="AU8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BL17" sqref="BL17"/>
+    <sheetView topLeftCell="AU9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BM17" sqref="BM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -17808,7 +18084,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:64" s="2" customFormat="1">
+    <row r="2" spans="1:65" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -17999,8 +18275,11 @@
       <c r="BL2" s="9">
         <v>43988</v>
       </c>
+      <c r="BM2" s="9">
+        <v>43989</v>
+      </c>
     </row>
-    <row r="3" spans="1:64" s="2" customFormat="1">
+    <row r="3" spans="1:65" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -18008,7 +18287,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:64">
+    <row r="4" spans="1:65">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -18201,8 +18480,11 @@
       <c r="BL4">
         <v>9332</v>
       </c>
+      <c r="BM4">
+        <v>9389</v>
+      </c>
     </row>
-    <row r="5" spans="1:64">
+    <row r="5" spans="1:65">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -18395,8 +18677,11 @@
       <c r="BL5">
         <v>1066</v>
       </c>
+      <c r="BM5">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="6" spans="1:64">
+    <row r="6" spans="1:65">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -18589,8 +18874,11 @@
       <c r="BL6">
         <v>1392</v>
       </c>
+      <c r="BM6">
+        <v>1394</v>
+      </c>
     </row>
-    <row r="7" spans="1:64">
+    <row r="7" spans="1:65">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -18783,8 +19071,11 @@
       <c r="BL7">
         <v>4302</v>
       </c>
+      <c r="BM7">
+        <v>4313</v>
+      </c>
     </row>
-    <row r="8" spans="1:64">
+    <row r="8" spans="1:65">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -18977,8 +19268,11 @@
       <c r="BL8">
         <v>108</v>
       </c>
+      <c r="BM8">
+        <v>108</v>
+      </c>
     </row>
-    <row r="9" spans="1:64" ht="28.8">
+    <row r="9" spans="1:65" ht="28.8">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -19171,8 +19465,11 @@
       <c r="BL9">
         <v>26</v>
       </c>
+      <c r="BM9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:64" ht="28.8">
+    <row r="10" spans="1:65" ht="28.8">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -19361,8 +19658,11 @@
       <c r="BL10">
         <v>23</v>
       </c>
+      <c r="BM10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:64">
+    <row r="11" spans="1:65">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -19555,8 +19855,11 @@
       <c r="BL11">
         <v>2357</v>
       </c>
+      <c r="BM11">
+        <v>2372</v>
+      </c>
     </row>
-    <row r="12" spans="1:64">
+    <row r="12" spans="1:65">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -19749,8 +20052,11 @@
       <c r="BL12">
         <v>58</v>
       </c>
+      <c r="BM12">
+        <v>58</v>
+      </c>
     </row>
-    <row r="13" spans="1:64">
+    <row r="13" spans="1:65">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -19761,7 +20067,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:64">
+    <row r="14" spans="1:65">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -19954,8 +20260,11 @@
       <c r="BL14">
         <v>1694</v>
       </c>
+      <c r="BM14">
+        <v>1742</v>
+      </c>
     </row>
-    <row r="15" spans="1:64">
+    <row r="15" spans="1:65">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -20148,8 +20457,11 @@
       <c r="BL15">
         <v>2460</v>
       </c>
+      <c r="BM15">
+        <v>2460</v>
+      </c>
     </row>
-    <row r="16" spans="1:64">
+    <row r="16" spans="1:65">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -20342,8 +20654,11 @@
       <c r="BL16">
         <v>5152</v>
       </c>
+      <c r="BM16">
+        <v>5161</v>
+      </c>
     </row>
-    <row r="17" spans="1:64">
+    <row r="17" spans="1:65">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -20534,6 +20849,9 @@
         <v>26</v>
       </c>
       <c r="BL17">
+        <v>26</v>
+      </c>
+      <c r="BM17">
         <v>26</v>
       </c>
     </row>
@@ -20545,10 +20863,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BL9"/>
+  <dimension ref="A1:BM9"/>
   <sheetViews>
     <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BL8" sqref="BL8"/>
+      <selection activeCell="BM8" sqref="BM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20557,7 +20875,7 @@
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="2" customFormat="1">
+    <row r="1" spans="1:65" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -20747,14 +21065,17 @@
       <c r="BL1" s="9">
         <v>43988</v>
       </c>
+      <c r="BM1" s="9">
+        <v>43989</v>
+      </c>
     </row>
-    <row r="2" spans="1:64">
+    <row r="2" spans="1:65">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:64">
+    <row r="3" spans="1:65">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -20948,8 +21269,11 @@
       <c r="BL3">
         <v>489</v>
       </c>
+      <c r="BM3">
+        <v>491</v>
+      </c>
     </row>
-    <row r="4" spans="1:64">
+    <row r="4" spans="1:65">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -21142,8 +21466,11 @@
       <c r="BL4">
         <v>7</v>
       </c>
+      <c r="BM4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:64" ht="28.8">
+    <row r="5" spans="1:65" ht="28.8">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -21336,8 +21663,11 @@
       <c r="BL5">
         <v>365</v>
       </c>
+      <c r="BM5">
+        <v>367</v>
+      </c>
     </row>
-    <row r="6" spans="1:64">
+    <row r="6" spans="1:65">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -21530,8 +21860,11 @@
       <c r="BL6">
         <v>59</v>
       </c>
+      <c r="BM6">
+        <v>59</v>
+      </c>
     </row>
-    <row r="7" spans="1:64">
+    <row r="7" spans="1:65">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -21724,8 +22057,11 @@
       <c r="BL7">
         <v>53</v>
       </c>
+      <c r="BM7">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:64">
+    <row r="8" spans="1:65">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -21918,8 +22254,11 @@
       <c r="BL8">
         <v>5</v>
       </c>
+      <c r="BM8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:64">
+    <row r="9" spans="1:65">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -21949,10 +22288,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AX13"/>
+  <dimension ref="A2:AY13"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ4" workbookViewId="0">
-      <selection activeCell="AX13" sqref="AX13"/>
+    <sheetView topLeftCell="AJ8" workbookViewId="0">
+      <selection activeCell="AY13" sqref="AY13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -21960,7 +22299,7 @@
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:50" s="2" customFormat="1">
+    <row r="2" spans="1:51" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -22111,8 +22450,11 @@
       <c r="AX2" s="9">
         <v>43988</v>
       </c>
+      <c r="AY2" s="9">
+        <v>43989</v>
+      </c>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:51">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -22263,8 +22605,11 @@
       <c r="AX3">
         <v>489</v>
       </c>
+      <c r="AY3">
+        <v>491</v>
+      </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:51">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -22415,8 +22760,11 @@
       <c r="AX4">
         <v>52</v>
       </c>
+      <c r="AY4">
+        <v>52</v>
+      </c>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:51">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -22567,8 +22915,11 @@
       <c r="AX5">
         <v>29</v>
       </c>
+      <c r="AY5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:51">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -22719,8 +23070,11 @@
       <c r="AX6">
         <v>30</v>
       </c>
+      <c r="AY6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:51">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -22871,8 +23225,11 @@
       <c r="AX7">
         <v>70</v>
       </c>
+      <c r="AY7">
+        <v>71</v>
+      </c>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:51">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -23023,8 +23380,11 @@
       <c r="AX8">
         <v>78</v>
       </c>
+      <c r="AY8">
+        <v>79</v>
+      </c>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:51">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -23175,8 +23535,11 @@
       <c r="AX9">
         <v>43</v>
       </c>
+      <c r="AY9">
+        <v>43</v>
+      </c>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:51">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -23327,8 +23690,11 @@
       <c r="AX10">
         <v>71</v>
       </c>
+      <c r="AY10">
+        <v>71</v>
+      </c>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:51">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -23479,8 +23845,11 @@
       <c r="AX11">
         <v>99</v>
       </c>
+      <c r="AY11">
+        <v>99</v>
+      </c>
     </row>
-    <row r="12" spans="1:50" ht="28.8">
+    <row r="12" spans="1:51" ht="28.8">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -23631,8 +24000,11 @@
       <c r="AX12">
         <v>17</v>
       </c>
+      <c r="AY12">
+        <v>17</v>
+      </c>
     </row>
-    <row r="13" spans="1:50">
+    <row r="13" spans="1:51">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -23781,6 +24153,9 @@
         <v>0</v>
       </c>
       <c r="AX13">
+        <v>0</v>
+      </c>
+      <c r="AY13">
         <v>0</v>
       </c>
     </row>
@@ -23792,10 +24167,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6:T23"/>
+    <sheetView topLeftCell="A18" zoomScale="82" workbookViewId="0">
+      <selection activeCell="U23" sqref="U6:U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -23803,9 +24178,9 @@
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="C1" s="42" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
@@ -23820,7 +24195,7 @@
       <c r="N1" s="42"/>
       <c r="O1" s="42"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
@@ -23835,7 +24210,7 @@
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -23850,7 +24225,7 @@
       <c r="N3" s="42"/>
       <c r="O3" s="42"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -23865,7 +24240,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -23920,8 +24295,11 @@
       <c r="T5" s="9">
         <v>43988</v>
       </c>
+      <c r="U5" s="9">
+        <v>43989</v>
+      </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="2" t="s">
         <v>122</v>
       </c>
@@ -23979,8 +24357,11 @@
       <c r="T6">
         <v>124</v>
       </c>
+      <c r="U6">
+        <v>124</v>
+      </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -24038,8 +24419,11 @@
       <c r="T7">
         <v>34</v>
       </c>
+      <c r="U7">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -24047,7 +24431,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -24105,8 +24489,11 @@
       <c r="T9">
         <v>1</v>
       </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" s="31" t="s">
         <v>123</v>
       </c>
@@ -24164,8 +24551,11 @@
       <c r="T10">
         <v>21</v>
       </c>
+      <c r="U10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" s="31" t="s">
         <v>124</v>
       </c>
@@ -24223,8 +24613,11 @@
       <c r="T11">
         <v>9</v>
       </c>
+      <c r="U11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -24282,13 +24675,16 @@
       <c r="T12">
         <v>3</v>
       </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:21">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -24346,8 +24742,11 @@
       <c r="T14">
         <v>1</v>
       </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:21">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -24405,8 +24804,11 @@
       <c r="T15">
         <v>0</v>
       </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:21">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -24464,8 +24866,11 @@
       <c r="T16">
         <v>3</v>
       </c>
+      <c r="U16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:21">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -24523,8 +24928,11 @@
       <c r="T17">
         <v>11</v>
       </c>
+      <c r="U17">
+        <v>11</v>
+      </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:21">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -24582,8 +24990,11 @@
       <c r="T18">
         <v>3</v>
       </c>
+      <c r="U18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:21">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -24641,8 +25052,11 @@
       <c r="T19">
         <v>3</v>
       </c>
+      <c r="U19">
+        <v>3</v>
+      </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:21">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -24700,8 +25114,11 @@
       <c r="T20">
         <v>2</v>
       </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:21">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -24759,8 +25176,11 @@
       <c r="T21">
         <v>6</v>
       </c>
+      <c r="U21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:20" ht="28.8">
+    <row r="22" spans="1:21" ht="28.8">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -24818,8 +25238,11 @@
       <c r="T22">
         <v>2</v>
       </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
     </row>
-    <row r="23" spans="1:20" ht="28.8">
+    <row r="23" spans="1:21" ht="28.8">
       <c r="A23" s="39" t="s">
         <v>125</v>
       </c>
@@ -24875,6 +25298,9 @@
         <v>3</v>
       </c>
       <c r="T23">
+        <v>3</v>
+      </c>
+      <c r="U23">
         <v>3</v>
       </c>
     </row>
@@ -24888,10 +25314,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -24907,7 +25333,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -25005,7 +25431,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8" s="28">
         <v>2</v>
@@ -25014,7 +25440,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F8" s="28">
         <v>0</v>
@@ -25028,7 +25454,7 @@
         <v>96</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C9" s="28">
         <v>4</v>
@@ -25037,7 +25463,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F9" s="28">
         <v>1</v>
@@ -25051,7 +25477,7 @@
         <v>97</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" s="28">
         <v>20</v>
@@ -25060,7 +25486,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F10" s="28">
         <v>0</v>
@@ -25083,7 +25509,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
@@ -25143,7 +25569,7 @@
         <v>101</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C14" s="28">
         <v>12</v>
@@ -25152,7 +25578,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F14" s="28">
         <v>1</v>
@@ -25166,7 +25592,7 @@
         <v>118</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C15" s="28">
         <v>5</v>
@@ -25175,7 +25601,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="28">
         <v>0</v>
@@ -25189,7 +25615,7 @@
         <v>102</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="28">
         <v>9</v>
@@ -25198,7 +25624,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F16" s="28">
         <v>1</v>
@@ -25212,7 +25638,7 @@
         <v>103</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C17" s="28">
         <v>9</v>
@@ -25221,7 +25647,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F17" s="28">
         <v>0</v>
@@ -25235,7 +25661,7 @@
         <v>104</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C18" s="28">
         <v>12</v>
@@ -25244,7 +25670,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F18" s="28">
         <v>0</v>
@@ -25258,7 +25684,7 @@
         <v>105</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C19" s="28">
         <v>14</v>
@@ -25327,7 +25753,7 @@
         <v>110</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C22" s="28">
         <v>7</v>
@@ -25336,7 +25762,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F22" s="28">
         <v>1</v>
@@ -25350,7 +25776,7 @@
         <v>111</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C23" s="28">
         <v>6</v>
@@ -25359,7 +25785,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F23" s="28">
         <v>0</v>
@@ -25373,7 +25799,7 @@
         <v>119</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C24" s="28">
         <v>20</v>
@@ -25382,7 +25808,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F24" s="28">
         <v>1</v>
@@ -25396,7 +25822,7 @@
         <v>49</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C25" s="28">
         <v>149</v>
@@ -25405,7 +25831,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F25" s="28">
         <v>6</v>
@@ -25415,53 +25841,27 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1">
-      <c r="A26" s="30"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
+      <c r="A26" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:7" ht="17.399999999999999" customHeight="1">
-      <c r="A27" s="30"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
     </row>
-    <row r="28" spans="1:7" ht="17.399999999999999" customHeight="1">
-      <c r="A28" s="30"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.6">
-      <c r="A29" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-    </row>
+    <row r="28" spans="1:7" ht="17.399999999999999" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
@@ -25475,6 +25875,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -25677,12 +26083,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -25693,6 +26093,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25711,23 +26128,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
10 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="8_{8728DFDE-C46A-402C-857F-CE80BAAC8B6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0FA7D96B-5B15-402D-BBDE-93CC52C9676D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD09DD0-7E37-43E0-99C2-719A396C3522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="7296" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -432,13 +434,7 @@
     <t>Total Overall Tested</t>
   </si>
   <si>
-    <t>29; (0)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>152; (46)</t>
   </si>
   <si>
     <t>Human Services - CFSA</t>
@@ -453,16 +449,10 @@
     <t>2; (1)</t>
   </si>
   <si>
-    <t>10; (7)</t>
-  </si>
-  <si>
     <t>12; (11)</t>
   </si>
   <si>
     <t>24; (9)</t>
-  </si>
-  <si>
-    <t>21; (3)</t>
   </si>
   <si>
     <t>96; (48)</t>
@@ -474,16 +464,7 @@
     <t>6; (2)</t>
   </si>
   <si>
-    <t>65; (29)</t>
-  </si>
-  <si>
     <t>32; (20)</t>
-  </si>
-  <si>
-    <t>20; (11)</t>
-  </si>
-  <si>
-    <t>13; (12)</t>
   </si>
   <si>
     <t>26; (17)</t>
@@ -510,35 +491,56 @@
     <t>12; (9)</t>
   </si>
   <si>
-    <t>15; (11)</t>
-  </si>
-  <si>
-    <t>20; (17)</t>
-  </si>
-  <si>
     <t>80; (77)</t>
-  </si>
-  <si>
-    <t>13; (10)</t>
-  </si>
-  <si>
-    <t>251; (129)</t>
-  </si>
-  <si>
-    <t>909; (497)</t>
-  </si>
-  <si>
-    <t>As of June 8, 2020</t>
   </si>
   <si>
     <t>62; (38)</t>
   </si>
   <si>
-    <t>659; (369)</t>
+    <t>As of June 9, 2020</t>
+  </si>
+  <si>
+    <t>10; (8)</t>
+  </si>
+  <si>
+    <t>19; (2)</t>
+  </si>
+  <si>
+    <t>66; (30)</t>
+  </si>
+  <si>
+    <t>21; (12)</t>
+  </si>
+  <si>
+    <t>15; (12)</t>
+  </si>
+  <si>
+    <t>22; (20)</t>
+  </si>
+  <si>
+    <t>149; (50)</t>
+  </si>
+  <si>
+    <t>36; (36)</t>
+  </si>
+  <si>
+    <t>15; (15)</t>
+  </si>
+  <si>
+    <t>13; (11)</t>
+  </si>
+  <si>
+    <t>658; (380)</t>
+  </si>
+  <si>
+    <t>260; (169)</t>
+  </si>
+  <si>
+    <t>918; (549)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of June 8, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of June 9, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -696,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -813,9 +815,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1197,26 +1196,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR119"/>
+  <dimension ref="A1:CS119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="CG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CR104" sqref="CR104"/>
+      <selection pane="topRight" activeCell="CS104" sqref="CS104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" customWidth="1"/>
-    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="80" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96">
+    <row r="1" spans="1:97">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1499,8 +1498,11 @@
       <c r="CR1" s="1">
         <v>43990</v>
       </c>
+      <c r="CS1" s="1">
+        <v>43991</v>
+      </c>
     </row>
-    <row r="2" spans="1:96">
+    <row r="2" spans="1:97">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1526,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:96">
+    <row r="3" spans="1:97">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1792,8 +1794,11 @@
       <c r="CR3">
         <v>57152</v>
       </c>
+      <c r="CS3">
+        <v>58192</v>
+      </c>
     </row>
-    <row r="4" spans="1:96">
+    <row r="4" spans="1:97">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1856,8 +1861,11 @@
       <c r="CR4">
         <v>46413</v>
       </c>
+      <c r="CS4">
+        <v>47148</v>
+      </c>
     </row>
-    <row r="5" spans="1:96">
+    <row r="5" spans="1:97">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2146,8 +2154,11 @@
       <c r="CR5">
         <v>9474</v>
       </c>
+      <c r="CS5">
+        <v>9537</v>
+      </c>
     </row>
-    <row r="6" spans="1:96">
+    <row r="6" spans="1:97">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2418,8 +2429,11 @@
       <c r="CR6">
         <v>495</v>
       </c>
+      <c r="CS6">
+        <v>499</v>
+      </c>
     </row>
-    <row r="7" spans="1:96">
+    <row r="7" spans="1:97">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2660,11 +2674,14 @@
       <c r="CR7">
         <v>1143</v>
       </c>
+      <c r="CS7">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="8" spans="1:96">
+    <row r="8" spans="1:97">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:96">
+    <row r="9" spans="1:97">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2797,8 +2814,11 @@
       <c r="CR9">
         <v>345</v>
       </c>
+      <c r="CS9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:96">
+    <row r="10" spans="1:97">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3033,8 +3053,11 @@
       <c r="CR10">
         <v>84</v>
       </c>
+      <c r="CS10">
+        <v>95</v>
+      </c>
     </row>
-    <row r="11" spans="1:96">
+    <row r="11" spans="1:97">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3269,8 +3292,11 @@
       <c r="CR11">
         <v>440</v>
       </c>
+      <c r="CS11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:96">
+    <row r="12" spans="1:97">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3505,8 +3531,11 @@
       <c r="CR12">
         <v>201</v>
       </c>
+      <c r="CS12">
+        <v>206</v>
+      </c>
     </row>
-    <row r="13" spans="1:96">
+    <row r="13" spans="1:97">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3741,8 +3770,11 @@
       <c r="CR13">
         <v>239</v>
       </c>
+      <c r="CS13">
+        <v>234</v>
+      </c>
     </row>
-    <row r="14" spans="1:96">
+    <row r="14" spans="1:97">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3839,8 +3871,11 @@
       <c r="CR14">
         <v>255</v>
       </c>
+      <c r="CS14">
+        <v>245</v>
+      </c>
     </row>
-    <row r="15" spans="1:96">
+    <row r="15" spans="1:97">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3907,8 +3942,11 @@
       <c r="CR15">
         <v>89</v>
       </c>
+      <c r="CS15">
+        <v>79</v>
+      </c>
     </row>
-    <row r="16" spans="1:96">
+    <row r="16" spans="1:97">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -4005,8 +4043,11 @@
       <c r="CR16">
         <v>1865</v>
       </c>
+      <c r="CS16">
+        <v>1968</v>
+      </c>
     </row>
-    <row r="17" spans="1:96">
+    <row r="17" spans="1:97">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -4103,13 +4144,16 @@
       <c r="CR17" s="23">
         <v>0.75</v>
       </c>
+      <c r="CS17" s="23">
+        <v>0.79</v>
+      </c>
     </row>
-    <row r="19" spans="1:96">
+    <row r="19" spans="1:97">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:96">
+    <row r="20" spans="1:97">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -4117,7 +4161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:96">
+    <row r="21" spans="1:97">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -4355,8 +4399,11 @@
       <c r="CR21">
         <v>113</v>
       </c>
+      <c r="CS21">
+        <v>113</v>
+      </c>
     </row>
-    <row r="22" spans="1:96">
+    <row r="22" spans="1:97">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4540,8 +4587,11 @@
       <c r="CR22">
         <v>16</v>
       </c>
+      <c r="CS22">
+        <v>16</v>
+      </c>
     </row>
-    <row r="23" spans="1:96">
+    <row r="23" spans="1:97">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4725,8 +4775,11 @@
       <c r="CR23">
         <v>97</v>
       </c>
+      <c r="CS23">
+        <v>97</v>
+      </c>
     </row>
-    <row r="24" spans="1:96">
+    <row r="24" spans="1:97">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -4955,8 +5008,11 @@
       <c r="CR24">
         <v>63</v>
       </c>
+      <c r="CS24">
+        <v>58</v>
+      </c>
     </row>
-    <row r="25" spans="1:96">
+    <row r="25" spans="1:97">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -5185,8 +5241,11 @@
       <c r="CR25">
         <v>79</v>
       </c>
+      <c r="CS25">
+        <v>74</v>
+      </c>
     </row>
-    <row r="26" spans="1:96">
+    <row r="26" spans="1:97">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -5415,13 +5474,16 @@
       <c r="CR26">
         <v>1495</v>
       </c>
+      <c r="CS26">
+        <v>1506</v>
+      </c>
     </row>
-    <row r="28" spans="1:96">
+    <row r="28" spans="1:97">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:96">
+    <row r="29" spans="1:97">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5659,8 +5721,11 @@
       <c r="CR29">
         <v>141</v>
       </c>
+      <c r="CS29">
+        <v>142</v>
+      </c>
     </row>
-    <row r="30" spans="1:96">
+    <row r="30" spans="1:97">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5844,8 +5909,11 @@
       <c r="CR30">
         <v>22</v>
       </c>
+      <c r="CS30">
+        <v>23</v>
+      </c>
     </row>
-    <row r="31" spans="1:96">
+    <row r="31" spans="1:97">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -6029,8 +6097,11 @@
       <c r="CR31">
         <v>118</v>
       </c>
+      <c r="CS31">
+        <v>118</v>
+      </c>
     </row>
-    <row r="32" spans="1:96">
+    <row r="32" spans="1:97">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -6259,8 +6330,11 @@
       <c r="CR32">
         <v>23</v>
       </c>
+      <c r="CS32">
+        <v>23</v>
+      </c>
     </row>
-    <row r="33" spans="1:96">
+    <row r="33" spans="1:97">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -6489,8 +6563,11 @@
       <c r="CR33">
         <v>45</v>
       </c>
+      <c r="CS33">
+        <v>46</v>
+      </c>
     </row>
-    <row r="34" spans="1:96">
+    <row r="34" spans="1:97">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6719,8 +6796,11 @@
       <c r="CR34">
         <v>1273</v>
       </c>
+      <c r="CS34">
+        <v>1277</v>
+      </c>
     </row>
-    <row r="35" spans="1:96">
+    <row r="35" spans="1:97">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -6730,13 +6810,16 @@
       <c r="CR35">
         <v>1</v>
       </c>
+      <c r="CS35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:96">
+    <row r="37" spans="1:97">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:96">
+    <row r="38" spans="1:97">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -6962,8 +7045,11 @@
       <c r="CR38">
         <v>84</v>
       </c>
+      <c r="CS38">
+        <v>85</v>
+      </c>
     </row>
-    <row r="39" spans="1:96">
+    <row r="39" spans="1:97">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -7141,8 +7227,11 @@
       <c r="CR39">
         <v>7</v>
       </c>
+      <c r="CS39">
+        <v>8</v>
+      </c>
     </row>
-    <row r="40" spans="1:96">
+    <row r="40" spans="1:97">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -7320,8 +7409,11 @@
       <c r="CR40">
         <v>76</v>
       </c>
+      <c r="CS40">
+        <v>76</v>
+      </c>
     </row>
-    <row r="41" spans="1:96">
+    <row r="41" spans="1:97">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -7544,8 +7636,11 @@
       <c r="CR41">
         <v>1</v>
       </c>
+      <c r="CS41">
+        <v>2</v>
+      </c>
     </row>
-    <row r="42" spans="1:96">
+    <row r="42" spans="1:97">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7765,8 +7860,11 @@
       <c r="CR42">
         <v>8</v>
       </c>
+      <c r="CS42">
+        <v>10</v>
+      </c>
     </row>
-    <row r="43" spans="1:96">
+    <row r="43" spans="1:97">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -7992,8 +8090,11 @@
       <c r="CR43">
         <v>285</v>
       </c>
+      <c r="CS43">
+        <v>285</v>
+      </c>
     </row>
-    <row r="44" spans="1:96">
+    <row r="44" spans="1:97">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -8153,16 +8254,19 @@
       <c r="CR44">
         <v>1</v>
       </c>
+      <c r="CS44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:96">
+    <row r="45" spans="1:97">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:96">
+    <row r="46" spans="1:97">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:96">
+    <row r="47" spans="1:97">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -8394,8 +8498,11 @@
       <c r="CR47">
         <v>207</v>
       </c>
+      <c r="CS47">
+        <v>207</v>
+      </c>
     </row>
-    <row r="48" spans="1:96">
+    <row r="48" spans="1:97">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -8579,8 +8686,11 @@
       <c r="CR48">
         <v>6</v>
       </c>
+      <c r="CS48">
+        <v>4</v>
+      </c>
     </row>
-    <row r="49" spans="1:96">
+    <row r="49" spans="1:97">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -8764,8 +8874,11 @@
       <c r="CR49">
         <v>194</v>
       </c>
+      <c r="CS49">
+        <v>196</v>
+      </c>
     </row>
-    <row r="50" spans="1:96">
+    <row r="50" spans="1:97">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -8994,8 +9107,11 @@
       <c r="CR50">
         <v>291</v>
       </c>
+      <c r="CS50">
+        <v>223</v>
+      </c>
     </row>
-    <row r="51" spans="1:96">
+    <row r="51" spans="1:97">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -9179,8 +9295,11 @@
       <c r="CR51">
         <v>297</v>
       </c>
+      <c r="CS51">
+        <v>227</v>
+      </c>
     </row>
-    <row r="52" spans="1:96">
+    <row r="52" spans="1:97">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -9361,8 +9480,11 @@
       <c r="CR52">
         <v>961</v>
       </c>
+      <c r="CS52">
+        <v>873</v>
+      </c>
     </row>
-    <row r="53" spans="1:96">
+    <row r="53" spans="1:97">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -9537,16 +9659,19 @@
       <c r="CR53">
         <v>1</v>
       </c>
+      <c r="CS53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:96">
+    <row r="54" spans="1:97">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:96">
+    <row r="55" spans="1:97">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:96">
+    <row r="56" spans="1:97">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -9763,8 +9888,11 @@
       <c r="CR56">
         <v>30</v>
       </c>
+      <c r="CS56">
+        <v>31</v>
+      </c>
     </row>
-    <row r="57" spans="1:96">
+    <row r="57" spans="1:97">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -9945,8 +10073,11 @@
       <c r="CR57">
         <v>7</v>
       </c>
+      <c r="CS57">
+        <v>6</v>
+      </c>
     </row>
-    <row r="58" spans="1:96">
+    <row r="58" spans="1:97">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -10127,8 +10258,11 @@
       <c r="CR58">
         <v>22</v>
       </c>
+      <c r="CS58">
+        <v>24</v>
+      </c>
     </row>
-    <row r="59" spans="1:96">
+    <row r="59" spans="1:97">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -10345,8 +10479,11 @@
       <c r="CR59">
         <v>11</v>
       </c>
+      <c r="CS59">
+        <v>8</v>
+      </c>
     </row>
-    <row r="60" spans="1:96">
+    <row r="60" spans="1:97">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -10563,8 +10700,11 @@
       <c r="CR60">
         <v>18</v>
       </c>
+      <c r="CS60">
+        <v>14</v>
+      </c>
     </row>
-    <row r="61" spans="1:96">
+    <row r="61" spans="1:97">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -10781,8 +10921,11 @@
       <c r="CR61">
         <v>151</v>
       </c>
+      <c r="CS61">
+        <v>158</v>
+      </c>
     </row>
-    <row r="62" spans="1:96">
+    <row r="62" spans="1:97">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -10957,8 +11100,11 @@
       <c r="CR62">
         <v>1</v>
       </c>
+      <c r="CS62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:96">
+    <row r="64" spans="1:97">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -11175,8 +11321,11 @@
       <c r="CR64">
         <v>12</v>
       </c>
+      <c r="CS64">
+        <v>12</v>
+      </c>
     </row>
-    <row r="65" spans="1:96">
+    <row r="65" spans="1:97">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -11357,8 +11506,11 @@
       <c r="CR65">
         <v>1</v>
       </c>
+      <c r="CS65">
+        <v>1</v>
+      </c>
     </row>
-    <row r="66" spans="1:96">
+    <row r="66" spans="1:97">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -11539,8 +11691,11 @@
       <c r="CR66">
         <v>11</v>
       </c>
+      <c r="CS66">
+        <v>11</v>
+      </c>
     </row>
-    <row r="67" spans="1:96">
+    <row r="67" spans="1:97">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -11757,8 +11912,11 @@
       <c r="CR67">
         <v>57</v>
       </c>
+      <c r="CS67">
+        <v>56</v>
+      </c>
     </row>
-    <row r="68" spans="1:96">
+    <row r="68" spans="1:97">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -11976,8 +12134,11 @@
       <c r="CR68">
         <v>58</v>
       </c>
+      <c r="CS68">
+        <v>57</v>
+      </c>
     </row>
-    <row r="69" spans="1:96">
+    <row r="69" spans="1:97">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -12194,8 +12355,11 @@
       <c r="CR69">
         <v>0</v>
       </c>
+      <c r="CS69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:96">
+    <row r="70" spans="1:97">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -12376,11 +12540,14 @@
       <c r="CR70">
         <v>0</v>
       </c>
+      <c r="CS70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:96">
+    <row r="71" spans="1:97">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:96">
+    <row r="72" spans="1:97">
       <c r="A72" s="2" t="s">
         <v>121</v>
       </c>
@@ -12447,8 +12614,11 @@
       <c r="CR72">
         <v>10</v>
       </c>
+      <c r="CS72">
+        <v>10</v>
+      </c>
     </row>
-    <row r="73" spans="1:96">
+    <row r="73" spans="1:97">
       <c r="A73" s="2" t="s">
         <v>121</v>
       </c>
@@ -12515,8 +12685,11 @@
       <c r="CR73">
         <v>4</v>
       </c>
+      <c r="CS73">
+        <v>4</v>
+      </c>
     </row>
-    <row r="74" spans="1:96">
+    <row r="74" spans="1:97">
       <c r="A74" s="2" t="s">
         <v>121</v>
       </c>
@@ -12583,8 +12756,11 @@
       <c r="CR74">
         <v>6</v>
       </c>
+      <c r="CS74">
+        <v>6</v>
+      </c>
     </row>
-    <row r="75" spans="1:96">
+    <row r="75" spans="1:97">
       <c r="A75" s="2" t="s">
         <v>121</v>
       </c>
@@ -12651,8 +12827,11 @@
       <c r="CR75">
         <v>5</v>
       </c>
+      <c r="CS75">
+        <v>4</v>
+      </c>
     </row>
-    <row r="76" spans="1:96">
+    <row r="76" spans="1:97">
       <c r="A76" s="2" t="s">
         <v>121</v>
       </c>
@@ -12719,8 +12898,11 @@
       <c r="CR76">
         <v>9</v>
       </c>
+      <c r="CS76">
+        <v>8</v>
+      </c>
     </row>
-    <row r="77" spans="1:96">
+    <row r="77" spans="1:97">
       <c r="A77" s="2" t="s">
         <v>121</v>
       </c>
@@ -12787,13 +12969,16 @@
       <c r="CR77">
         <v>39</v>
       </c>
+      <c r="CS77">
+        <v>40</v>
+      </c>
     </row>
-    <row r="79" spans="1:96">
+    <row r="79" spans="1:97">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:96">
+    <row r="80" spans="1:97">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -13010,8 +13195,11 @@
       <c r="CR80">
         <v>305</v>
       </c>
+      <c r="CS80">
+        <v>306</v>
+      </c>
     </row>
-    <row r="81" spans="1:96">
+    <row r="81" spans="1:97">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -13228,8 +13416,11 @@
       <c r="CR81">
         <v>75</v>
       </c>
+      <c r="CS81">
+        <v>81</v>
+      </c>
     </row>
-    <row r="82" spans="1:96">
+    <row r="82" spans="1:97">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -13446,8 +13637,11 @@
       <c r="CR82">
         <v>75</v>
       </c>
+      <c r="CS82">
+        <v>84</v>
+      </c>
     </row>
-    <row r="83" spans="1:96">
+    <row r="83" spans="1:97">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -13622,8 +13816,11 @@
       <c r="CR83">
         <v>17</v>
       </c>
+      <c r="CS83">
+        <v>17</v>
+      </c>
     </row>
-    <row r="85" spans="1:96">
+    <row r="85" spans="1:97">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -13840,8 +14037,11 @@
       <c r="CR85">
         <v>120</v>
       </c>
+      <c r="CS85">
+        <v>120</v>
+      </c>
     </row>
-    <row r="86" spans="1:96">
+    <row r="86" spans="1:97">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -14058,8 +14258,11 @@
       <c r="CR86">
         <v>2</v>
       </c>
+      <c r="CS86">
+        <v>3</v>
+      </c>
     </row>
-    <row r="87" spans="1:96">
+    <row r="87" spans="1:97">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -14276,8 +14479,11 @@
       <c r="CR87">
         <v>53</v>
       </c>
+      <c r="CS87">
+        <v>51</v>
+      </c>
     </row>
-    <row r="88" spans="1:96">
+    <row r="88" spans="1:97">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -14494,8 +14700,11 @@
       <c r="CR88">
         <v>209</v>
       </c>
+      <c r="CS88">
+        <v>211</v>
+      </c>
     </row>
-    <row r="89" spans="1:96">
+    <row r="89" spans="1:97">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -14586,8 +14795,11 @@
       <c r="CR89">
         <v>1</v>
       </c>
+      <c r="CS89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:96">
+    <row r="91" spans="1:97">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -14804,8 +15016,11 @@
       <c r="CR91">
         <v>81</v>
       </c>
+      <c r="CS91">
+        <v>81</v>
+      </c>
     </row>
-    <row r="92" spans="1:96">
+    <row r="92" spans="1:97">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -15022,8 +15237,11 @@
       <c r="CR92">
         <v>2</v>
       </c>
+      <c r="CS92">
+        <v>2</v>
+      </c>
     </row>
-    <row r="93" spans="1:96">
+    <row r="93" spans="1:97">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -15228,8 +15446,11 @@
       <c r="CR93">
         <v>169</v>
       </c>
+      <c r="CS93">
+        <v>170</v>
+      </c>
     </row>
-    <row r="94" spans="1:96">
+    <row r="94" spans="1:97">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -15446,8 +15667,11 @@
       <c r="CR94">
         <v>62</v>
       </c>
+      <c r="CS94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:96">
+    <row r="95" spans="1:97">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -15622,16 +15846,19 @@
       <c r="CR95">
         <v>13</v>
       </c>
+      <c r="CS95">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:96">
+    <row r="96" spans="1:97">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:96">
+    <row r="97" spans="1:97">
       <c r="A97" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B97" s="41" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CG97">
         <v>9</v>
@@ -15660,13 +15887,16 @@
       <c r="CR97">
         <v>9</v>
       </c>
+      <c r="CS97">
+        <v>9</v>
+      </c>
     </row>
-    <row r="98" spans="1:96">
+    <row r="98" spans="1:97">
       <c r="A98" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B98" s="20" t="s">
         <v>134</v>
-      </c>
-      <c r="B98" s="20" t="s">
-        <v>136</v>
       </c>
       <c r="CG98">
         <v>17</v>
@@ -15695,10 +15925,13 @@
       <c r="CR98">
         <v>8</v>
       </c>
+      <c r="CS98">
+        <v>8</v>
+      </c>
     </row>
-    <row r="99" spans="1:96">
+    <row r="99" spans="1:97">
       <c r="A99" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B99" s="41" t="s">
         <v>12</v>
@@ -15730,10 +15963,13 @@
       <c r="CR99">
         <v>46</v>
       </c>
+      <c r="CS99">
+        <v>46</v>
+      </c>
     </row>
-    <row r="100" spans="1:96">
+    <row r="100" spans="1:97">
       <c r="A100" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B100" s="41" t="s">
         <v>84</v>
@@ -15765,8 +16001,11 @@
       <c r="CR100">
         <v>1</v>
       </c>
+      <c r="CS100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:96">
+    <row r="102" spans="1:97">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -15902,8 +16141,11 @@
       <c r="CR102">
         <v>193</v>
       </c>
+      <c r="CS102">
+        <v>193</v>
+      </c>
     </row>
-    <row r="103" spans="1:96">
+    <row r="103" spans="1:97">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -16039,8 +16281,11 @@
       <c r="CR103">
         <v>84</v>
       </c>
+      <c r="CS103">
+        <v>84</v>
+      </c>
     </row>
-    <row r="104" spans="1:96">
+    <row r="104" spans="1:97">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -16174,6 +16419,9 @@
         <v>25</v>
       </c>
       <c r="CR104">
+        <v>25</v>
+      </c>
+      <c r="CS104">
         <v>25</v>
       </c>
     </row>
@@ -16190,20 +16438,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BS11"/>
+  <dimension ref="A2:BT11"/>
   <sheetViews>
-    <sheetView topLeftCell="BB2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BS11" sqref="BS11"/>
+    <sheetView tabSelected="1" topLeftCell="BB2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BT11" sqref="BT3:BT11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:71" s="2" customFormat="1">
+    <row r="2" spans="1:72" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -16417,8 +16665,11 @@
       <c r="BS2" s="9">
         <v>43990</v>
       </c>
+      <c r="BT2" s="9">
+        <v>43991</v>
+      </c>
     </row>
-    <row r="3" spans="1:71">
+    <row r="3" spans="1:72">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -16632,8 +16883,11 @@
       <c r="BS3">
         <v>1343</v>
       </c>
+      <c r="BT3">
+        <v>1352</v>
+      </c>
     </row>
-    <row r="4" spans="1:71">
+    <row r="4" spans="1:72">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -16847,8 +17101,11 @@
       <c r="BS4">
         <v>532</v>
       </c>
+      <c r="BT4">
+        <v>533</v>
+      </c>
     </row>
-    <row r="5" spans="1:71">
+    <row r="5" spans="1:72">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -17062,8 +17319,11 @@
       <c r="BS5">
         <v>443</v>
       </c>
+      <c r="BT5">
+        <v>446</v>
+      </c>
     </row>
-    <row r="6" spans="1:71">
+    <row r="6" spans="1:72">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -17277,8 +17537,11 @@
       <c r="BS6">
         <v>1984</v>
       </c>
+      <c r="BT6">
+        <v>1999</v>
+      </c>
     </row>
-    <row r="7" spans="1:71">
+    <row r="7" spans="1:72">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -17492,8 +17755,11 @@
       <c r="BS7">
         <v>1442</v>
       </c>
+      <c r="BT7">
+        <v>1447</v>
+      </c>
     </row>
-    <row r="8" spans="1:71">
+    <row r="8" spans="1:72">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -17707,8 +17973,11 @@
       <c r="BS8">
         <v>805</v>
       </c>
+      <c r="BT8">
+        <v>817</v>
+      </c>
     </row>
-    <row r="9" spans="1:71">
+    <row r="9" spans="1:72">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -17922,8 +18191,11 @@
       <c r="BS9">
         <v>1363</v>
       </c>
+      <c r="BT9">
+        <v>1371</v>
+      </c>
     </row>
-    <row r="10" spans="1:71">
+    <row r="10" spans="1:72">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -18137,8 +18409,11 @@
       <c r="BS10">
         <v>1394</v>
       </c>
+      <c r="BT10">
+        <v>1402</v>
+      </c>
     </row>
-    <row r="11" spans="1:71">
+    <row r="11" spans="1:72">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -18351,6 +18626,9 @@
       </c>
       <c r="BS11">
         <v>168</v>
+      </c>
+      <c r="BT11">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -18361,20 +18639,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BN17"/>
+  <dimension ref="A2:BO17"/>
   <sheetViews>
-    <sheetView topLeftCell="AU10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BN17" sqref="BN17"/>
+    <sheetView topLeftCell="AU8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BO17" sqref="BO17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:66" s="2" customFormat="1">
+    <row r="2" spans="1:67" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -18571,8 +18849,11 @@
       <c r="BN2" s="9">
         <v>43990</v>
       </c>
+      <c r="BO2" s="9">
+        <v>43991</v>
+      </c>
     </row>
-    <row r="3" spans="1:66" s="2" customFormat="1">
+    <row r="3" spans="1:67" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -18580,7 +18861,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:66">
+    <row r="4" spans="1:67">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -18779,8 +19060,11 @@
       <c r="BN4">
         <v>9474</v>
       </c>
+      <c r="BO4">
+        <v>9537</v>
+      </c>
     </row>
-    <row r="5" spans="1:66">
+    <row r="5" spans="1:67">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -18979,8 +19263,11 @@
       <c r="BN5">
         <v>1150</v>
       </c>
+      <c r="BO5">
+        <v>1181</v>
+      </c>
     </row>
-    <row r="6" spans="1:66">
+    <row r="6" spans="1:67">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -19179,8 +19466,11 @@
       <c r="BN6">
         <v>1401</v>
       </c>
+      <c r="BO6">
+        <v>1403</v>
+      </c>
     </row>
-    <row r="7" spans="1:66">
+    <row r="7" spans="1:67">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -19379,8 +19669,11 @@
       <c r="BN7">
         <v>4331</v>
       </c>
+      <c r="BO7">
+        <v>4352</v>
+      </c>
     </row>
-    <row r="8" spans="1:66">
+    <row r="8" spans="1:67">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -19579,8 +19872,11 @@
       <c r="BN8">
         <v>109</v>
       </c>
+      <c r="BO8">
+        <v>109</v>
+      </c>
     </row>
-    <row r="9" spans="1:66" ht="28.8">
+    <row r="9" spans="1:67" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -19779,8 +20075,11 @@
       <c r="BN9">
         <v>26</v>
       </c>
+      <c r="BO9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:66" ht="28.8">
+    <row r="10" spans="1:67" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -19975,8 +20274,11 @@
       <c r="BN10">
         <v>23</v>
       </c>
+      <c r="BO10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:66">
+    <row r="11" spans="1:67">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -20175,8 +20477,11 @@
       <c r="BN11">
         <v>2377</v>
       </c>
+      <c r="BO11">
+        <v>2386</v>
+      </c>
     </row>
-    <row r="12" spans="1:66">
+    <row r="12" spans="1:67" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -20375,8 +20680,11 @@
       <c r="BN12">
         <v>57</v>
       </c>
+      <c r="BO12">
+        <v>57</v>
+      </c>
     </row>
-    <row r="13" spans="1:66">
+    <row r="13" spans="1:67">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -20387,7 +20695,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:66">
+    <row r="14" spans="1:67">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -20586,8 +20894,11 @@
       <c r="BN14">
         <v>1810</v>
       </c>
+      <c r="BO14">
+        <v>1855</v>
+      </c>
     </row>
-    <row r="15" spans="1:66">
+    <row r="15" spans="1:67">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -20786,8 +21097,11 @@
       <c r="BN15">
         <v>2464</v>
       </c>
+      <c r="BO15">
+        <v>2469</v>
+      </c>
     </row>
-    <row r="16" spans="1:66">
+    <row r="16" spans="1:67">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -20986,8 +21300,11 @@
       <c r="BN16">
         <v>5175</v>
       </c>
+      <c r="BO16">
+        <v>5188</v>
+      </c>
     </row>
-    <row r="17" spans="1:66">
+    <row r="17" spans="1:67" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -21184,6 +21501,9 @@
         <v>26</v>
       </c>
       <c r="BN17">
+        <v>25</v>
+      </c>
+      <c r="BO17">
         <v>25</v>
       </c>
     </row>
@@ -21195,19 +21515,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BN9"/>
+  <dimension ref="A1:BO9"/>
   <sheetViews>
     <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BN8" sqref="BN8"/>
+      <selection activeCell="BO8" sqref="BO8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="2" customFormat="1">
+    <row r="1" spans="1:67" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -21403,14 +21723,17 @@
       <c r="BN1" s="9">
         <v>43990</v>
       </c>
+      <c r="BO1" s="9">
+        <v>43991</v>
+      </c>
     </row>
-    <row r="2" spans="1:66">
+    <row r="2" spans="1:67">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:66">
+    <row r="3" spans="1:67">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -21610,8 +21933,11 @@
       <c r="BN3">
         <v>495</v>
       </c>
+      <c r="BO3">
+        <v>499</v>
+      </c>
     </row>
-    <row r="4" spans="1:66">
+    <row r="4" spans="1:67">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -21810,8 +22136,11 @@
       <c r="BN4">
         <v>7</v>
       </c>
+      <c r="BO4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:66" ht="28.8">
+    <row r="5" spans="1:67" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -22010,8 +22339,11 @@
       <c r="BN5">
         <v>367</v>
       </c>
+      <c r="BO5">
+        <v>371</v>
+      </c>
     </row>
-    <row r="6" spans="1:66">
+    <row r="6" spans="1:67">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -22210,8 +22542,11 @@
       <c r="BN6">
         <v>62</v>
       </c>
+      <c r="BO6">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:66">
+    <row r="7" spans="1:67" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -22410,8 +22745,11 @@
       <c r="BN7">
         <v>54</v>
       </c>
+      <c r="BO7">
+        <v>54</v>
+      </c>
     </row>
-    <row r="8" spans="1:66">
+    <row r="8" spans="1:67">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -22610,8 +22948,11 @@
       <c r="BN8">
         <v>5</v>
       </c>
+      <c r="BO8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:66">
+    <row r="9" spans="1:67">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -22641,18 +22982,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:AZ13"/>
+  <dimension ref="A2:BA13"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ5" workbookViewId="0">
-      <selection activeCell="AZ13" sqref="AZ13"/>
+    <sheetView topLeftCell="AJ4" workbookViewId="0">
+      <selection activeCell="BA13" sqref="BA13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:52" s="2" customFormat="1">
+    <row r="2" spans="1:53" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -22809,8 +23150,11 @@
       <c r="AZ2" s="9">
         <v>43990</v>
       </c>
+      <c r="BA2" s="9">
+        <v>43991</v>
+      </c>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:53">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -22967,8 +23311,11 @@
       <c r="AZ3">
         <v>495</v>
       </c>
+      <c r="BA3">
+        <v>499</v>
+      </c>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:53">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -23125,8 +23472,11 @@
       <c r="AZ4">
         <v>53</v>
       </c>
+      <c r="BA4">
+        <v>53</v>
+      </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:53">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -23283,8 +23633,11 @@
       <c r="AZ5">
         <v>29</v>
       </c>
+      <c r="BA5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:53">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -23441,8 +23794,11 @@
       <c r="AZ6">
         <v>30</v>
       </c>
+      <c r="BA6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:53">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -23599,8 +23955,11 @@
       <c r="AZ7">
         <v>73</v>
       </c>
+      <c r="BA7">
+        <v>73</v>
+      </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:53">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -23757,8 +24116,11 @@
       <c r="AZ8">
         <v>79</v>
       </c>
+      <c r="BA8">
+        <v>80</v>
+      </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:53">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -23915,8 +24277,11 @@
       <c r="AZ9">
         <v>44</v>
       </c>
+      <c r="BA9">
+        <v>44</v>
+      </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:53">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -24073,8 +24438,11 @@
       <c r="AZ10">
         <v>71</v>
       </c>
+      <c r="BA10">
+        <v>72</v>
+      </c>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:53">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -24231,8 +24599,11 @@
       <c r="AZ11">
         <v>99</v>
       </c>
+      <c r="BA11">
+        <v>100</v>
+      </c>
     </row>
-    <row r="12" spans="1:52" ht="28.8">
+    <row r="12" spans="1:53" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -24389,8 +24760,11 @@
       <c r="AZ12">
         <v>17</v>
       </c>
+      <c r="BA12">
+        <v>17</v>
+      </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:53">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -24545,6 +24919,9 @@
         <v>0</v>
       </c>
       <c r="AZ13">
+        <v>0</v>
+      </c>
+      <c r="BA13">
         <v>0</v>
       </c>
     </row>
@@ -24556,18 +24933,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="82" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="C1" s="42" t="s">
         <v>166</v>
       </c>
@@ -24584,7 +24961,7 @@
       <c r="N1" s="42"/>
       <c r="O1" s="42"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
@@ -24599,7 +24976,7 @@
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23">
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -24614,7 +24991,7 @@
       <c r="N3" s="42"/>
       <c r="O3" s="42"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:23">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -24629,7 +25006,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -24690,8 +25067,11 @@
       <c r="V5" s="9">
         <v>43990</v>
       </c>
+      <c r="W5" s="9">
+        <v>43991</v>
+      </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:23">
       <c r="A6" s="2" t="s">
         <v>122</v>
       </c>
@@ -24755,8 +25135,11 @@
       <c r="V6">
         <v>124</v>
       </c>
+      <c r="W6">
+        <v>124</v>
+      </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:23">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -24820,16 +25203,19 @@
       <c r="V7">
         <v>34</v>
       </c>
+      <c r="W7">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:23">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:23">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -24893,8 +25279,11 @@
       <c r="V9">
         <v>1</v>
       </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:23">
       <c r="A10" s="31" t="s">
         <v>123</v>
       </c>
@@ -24958,8 +25347,11 @@
       <c r="V10">
         <v>21</v>
       </c>
+      <c r="W10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:23">
       <c r="A11" s="31" t="s">
         <v>124</v>
       </c>
@@ -25023,8 +25415,11 @@
       <c r="V11">
         <v>9</v>
       </c>
+      <c r="W11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:23">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -25088,13 +25483,16 @@
       <c r="V12">
         <v>3</v>
       </c>
+      <c r="W12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:23">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:23">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -25158,8 +25556,11 @@
       <c r="V14">
         <v>1</v>
       </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:23">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -25223,8 +25624,11 @@
       <c r="V15">
         <v>0</v>
       </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:23">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -25288,8 +25692,11 @@
       <c r="V16">
         <v>3</v>
       </c>
+      <c r="W16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:23">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -25353,8 +25760,11 @@
       <c r="V17">
         <v>11</v>
       </c>
+      <c r="W17">
+        <v>11</v>
+      </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:23">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -25418,8 +25828,11 @@
       <c r="V18">
         <v>3</v>
       </c>
+      <c r="W18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:23">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -25483,8 +25896,11 @@
       <c r="V19">
         <v>3</v>
       </c>
+      <c r="W19">
+        <v>3</v>
+      </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:23">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -25548,8 +25964,11 @@
       <c r="V20">
         <v>2</v>
       </c>
+      <c r="W20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:23">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -25613,8 +26032,11 @@
       <c r="V21">
         <v>6</v>
       </c>
+      <c r="W21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:22" ht="28.8">
+    <row r="22" spans="1:23" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -25678,8 +26100,11 @@
       <c r="V22">
         <v>2</v>
       </c>
+      <c r="W22">
+        <v>2</v>
+      </c>
     </row>
-    <row r="23" spans="1:22" ht="28.8">
+    <row r="23" spans="1:23" ht="30">
       <c r="A23" s="39" t="s">
         <v>125</v>
       </c>
@@ -25741,6 +26166,9 @@
         <v>3</v>
       </c>
       <c r="V23">
+        <v>3</v>
+      </c>
+      <c r="W23">
         <v>3</v>
       </c>
     </row>
@@ -25756,24 +26184,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -25820,7 +26248,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1">
+    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1">
       <c r="A4" s="45"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -25833,7 +26261,7 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1">
+    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1">
       <c r="A5" s="45"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
@@ -25844,7 +26272,7 @@
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1">
+    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1">
       <c r="A6" s="45"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -25855,7 +26283,7 @@
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1">
+    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1">
       <c r="A7" s="45"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
@@ -25866,164 +26294,164 @@
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.4" customHeight="1">
+    <row r="8" spans="1:7" ht="14.45" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="27">
+      <c r="B8" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="28">
         <v>2</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="28">
         <v>4</v>
       </c>
-      <c r="E8" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8" s="27">
+      <c r="E8" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8" s="28">
         <v>0</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="28">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4" customHeight="1">
+    <row r="9" spans="1:7" ht="14.45" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" s="27">
+      <c r="B9" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="28">
         <v>4</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="28">
         <v>0</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" s="27">
-        <v>1</v>
-      </c>
-      <c r="G9" s="27">
+      <c r="E9" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="28">
+        <v>1</v>
+      </c>
+      <c r="G9" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.4" customHeight="1">
+    <row r="10" spans="1:7" ht="14.45" customHeight="1">
       <c r="A10" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" s="27">
-        <v>20</v>
-      </c>
-      <c r="D10" s="27">
+      <c r="B10" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="28">
+        <v>21</v>
+      </c>
+      <c r="D10" s="28">
         <v>4</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" s="27">
+      <c r="E10" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="28">
         <v>0</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="28">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.4" customHeight="1">
+    <row r="11" spans="1:7" ht="14.45" customHeight="1">
       <c r="A11" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="28">
         <v>0</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="28">
         <v>2</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="F11" s="27">
+      <c r="E11" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="28">
         <v>0</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="28">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.4" customHeight="1">
+    <row r="12" spans="1:7" ht="14.45" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="28">
         <v>0</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="28">
         <v>0</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="28">
         <v>0</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.4" customHeight="1">
+    <row r="13" spans="1:7" ht="14.45" customHeight="1">
       <c r="A13" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="27">
+      <c r="B13" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="28">
         <v>2</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="28">
         <v>0</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="28">
         <v>0</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.4" customHeight="1">
+    <row r="14" spans="1:7" ht="14.45" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="C14" s="27">
-        <v>12</v>
-      </c>
-      <c r="D14" s="27">
+      <c r="B14" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="28">
+        <v>13</v>
+      </c>
+      <c r="D14" s="28">
         <v>30</v>
       </c>
-      <c r="E14" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="F14" s="27">
-        <v>1</v>
-      </c>
-      <c r="G14" s="27">
+      <c r="E14" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="28">
+        <v>1</v>
+      </c>
+      <c r="G14" s="28">
         <v>21</v>
       </c>
     </row>
@@ -26031,183 +26459,183 @@
       <c r="A15" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B15" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C15" s="27">
+      <c r="B15" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="28">
         <v>5</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="28">
         <v>14</v>
       </c>
-      <c r="E15" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="F15" s="27">
+      <c r="E15" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F15" s="28">
         <v>0</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="28">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.4" customHeight="1">
+    <row r="16" spans="1:7" ht="14.45" customHeight="1">
       <c r="A16" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="27">
+      <c r="B16" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="28">
         <v>9</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="28">
         <v>15</v>
       </c>
-      <c r="E16" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F16" s="27">
-        <v>1</v>
-      </c>
-      <c r="G16" s="27">
+      <c r="E16" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="28">
+        <v>1</v>
+      </c>
+      <c r="G16" s="28">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.4" customHeight="1">
+    <row r="17" spans="1:7" ht="14.45" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="27">
+      <c r="B17" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="28">
         <v>9</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="28">
         <v>29</v>
       </c>
-      <c r="E17" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="F17" s="27">
+      <c r="E17" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="28">
         <v>0</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="28">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.4" customHeight="1">
+    <row r="18" spans="1:7" ht="14.45" customHeight="1">
       <c r="A18" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="27">
+      <c r="B18" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="28">
         <v>12</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="28">
         <v>26</v>
       </c>
-      <c r="E18" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="F18" s="27">
+      <c r="E18" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="28">
         <v>0</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="28">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.4" customHeight="1">
+    <row r="19" spans="1:7" ht="14.45" customHeight="1">
       <c r="A19" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="27">
+      <c r="B19" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="28">
         <v>14</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="28">
         <v>20</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="28">
         <v>0</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.4" customHeight="1">
+    <row r="20" spans="1:7" ht="14.45" customHeight="1">
       <c r="A20" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="27">
-        <v>1</v>
-      </c>
-      <c r="D20" s="27">
+      <c r="C20" s="28">
+        <v>1</v>
+      </c>
+      <c r="D20" s="28">
         <v>0</v>
       </c>
-      <c r="E20" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="F20" s="27">
+      <c r="E20" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="28">
         <v>0</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.4" customHeight="1">
+    <row r="21" spans="1:7" ht="14.45" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" s="27">
-        <v>26</v>
-      </c>
-      <c r="D21" s="27">
-        <v>0</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" s="27">
-        <v>1</v>
-      </c>
-      <c r="G21" s="27">
-        <v>0</v>
+      <c r="B21" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="28">
+        <v>25</v>
+      </c>
+      <c r="D21" s="28">
+        <v>62</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="28">
+        <v>2</v>
+      </c>
+      <c r="G21" s="28">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.6" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="27">
+      <c r="B22" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="28">
         <v>7</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="28">
         <v>11</v>
       </c>
-      <c r="E22" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="F22" s="27">
-        <v>1</v>
-      </c>
-      <c r="G22" s="27">
+      <c r="E22" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="28">
+        <v>1</v>
+      </c>
+      <c r="G22" s="28">
         <v>10</v>
       </c>
     </row>
@@ -26215,22 +26643,22 @@
       <c r="A23" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="C23" s="27">
+      <c r="B23" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="28">
         <v>6</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="28">
         <v>3</v>
       </c>
-      <c r="E23" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="F23" s="27">
+      <c r="E23" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="28">
         <v>0</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="28">
         <v>15</v>
       </c>
     </row>
@@ -26238,54 +26666,54 @@
       <c r="A24" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="C24" s="27">
+      <c r="B24" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="28">
         <v>20</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="28">
         <v>25</v>
       </c>
-      <c r="E24" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="F24" s="27">
-        <v>1</v>
-      </c>
-      <c r="G24" s="27">
+      <c r="E24" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="F24" s="28">
+        <v>1</v>
+      </c>
+      <c r="G24" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.399999999999999" customHeight="1">
+    <row r="25" spans="1:7" ht="17.45" customHeight="1">
       <c r="A25" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="C25" s="27">
-        <v>149</v>
-      </c>
-      <c r="D25" s="27">
-        <v>183</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="F25" s="27">
-        <v>6</v>
-      </c>
-      <c r="G25" s="47">
-        <v>120</v>
+      <c r="B25" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" s="28">
+        <v>150</v>
+      </c>
+      <c r="D25" s="28">
+        <v>245</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="28">
+        <v>7</v>
+      </c>
+      <c r="G25" s="28">
+        <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1">
+    <row r="26" spans="1:7" ht="17.45" customHeight="1">
       <c r="A26" s="24" t="s">
         <v>112</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
@@ -26293,7 +26721,7 @@
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
     </row>
-    <row r="27" spans="1:7" ht="17.399999999999999" customHeight="1">
+    <row r="27" spans="1:7" ht="17.45" customHeight="1">
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -26301,7 +26729,7 @@
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
     </row>
-    <row r="28" spans="1:7" ht="17.399999999999999" customHeight="1"/>
+    <row r="28" spans="1:7" ht="17.45" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
@@ -26554,16 +26982,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
11 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD09DD0-7E37-43E0-99C2-719A396C3522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0EAE83-E7AE-4FD1-AF6D-E264E6B6A9DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,9 +473,6 @@
     <t>23; (10)</t>
   </si>
   <si>
-    <t>41; (37)</t>
-  </si>
-  <si>
     <t>10; (9)</t>
   </si>
   <si>
@@ -495,9 +492,6 @@
   </si>
   <si>
     <t>62; (38)</t>
-  </si>
-  <si>
-    <t>As of June 9, 2020</t>
   </si>
   <si>
     <t>10; (8)</t>
@@ -530,17 +524,11 @@
     <t>13; (11)</t>
   </si>
   <si>
-    <t>658; (380)</t>
-  </si>
-  <si>
     <t>260; (169)</t>
   </si>
   <si>
-    <t>918; (549)</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">As of June 9, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of June 10, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -563,6 +551,18 @@
       </rPr>
       <t xml:space="preserve"> for COVID-19 testing,  and 34 (27.4%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
+  </si>
+  <si>
+    <t>As of June 10, 2020</t>
+  </si>
+  <si>
+    <t>40; (36)</t>
+  </si>
+  <si>
+    <t>657; (379)</t>
+  </si>
+  <si>
+    <t>917; (548)</t>
   </si>
 </sst>
 </file>
@@ -1196,11 +1196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CS119"/>
+  <dimension ref="A1:CT119"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="CG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CS104" sqref="CS104"/>
+    <sheetView topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="CI1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CT104" sqref="CT104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1213,9 +1213,10 @@
     <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97">
+    <row r="1" spans="1:98">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1501,8 +1502,11 @@
       <c r="CS1" s="1">
         <v>43991</v>
       </c>
+      <c r="CT1" s="1">
+        <v>43992</v>
+      </c>
     </row>
-    <row r="2" spans="1:97">
+    <row r="2" spans="1:98">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1530,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:97">
+    <row r="3" spans="1:98">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1797,8 +1801,11 @@
       <c r="CS3">
         <v>58192</v>
       </c>
+      <c r="CT3">
+        <v>59288</v>
+      </c>
     </row>
-    <row r="4" spans="1:97">
+    <row r="4" spans="1:98">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1864,8 +1871,11 @@
       <c r="CS4">
         <v>47148</v>
       </c>
+      <c r="CT4">
+        <v>47796</v>
+      </c>
     </row>
-    <row r="5" spans="1:97">
+    <row r="5" spans="1:98">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2157,8 +2167,11 @@
       <c r="CS5">
         <v>9537</v>
       </c>
+      <c r="CT5">
+        <v>9589</v>
+      </c>
     </row>
-    <row r="6" spans="1:97">
+    <row r="6" spans="1:98">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2432,8 +2445,11 @@
       <c r="CS6">
         <v>499</v>
       </c>
+      <c r="CT6">
+        <v>502</v>
+      </c>
     </row>
-    <row r="7" spans="1:97">
+    <row r="7" spans="1:98">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2677,11 +2693,14 @@
       <c r="CS7">
         <v>1143</v>
       </c>
+      <c r="CT7">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="8" spans="1:97">
+    <row r="8" spans="1:98">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:97">
+    <row r="9" spans="1:98">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2817,8 +2836,11 @@
       <c r="CS9">
         <v>345</v>
       </c>
+      <c r="CT9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:97">
+    <row r="10" spans="1:98">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3056,8 +3078,11 @@
       <c r="CS10">
         <v>95</v>
       </c>
+      <c r="CT10">
+        <v>56</v>
+      </c>
     </row>
-    <row r="11" spans="1:97">
+    <row r="11" spans="1:98">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3295,8 +3320,11 @@
       <c r="CS11">
         <v>440</v>
       </c>
+      <c r="CT11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:97">
+    <row r="12" spans="1:98">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3534,8 +3562,11 @@
       <c r="CS12">
         <v>206</v>
       </c>
+      <c r="CT12">
+        <v>210</v>
+      </c>
     </row>
-    <row r="13" spans="1:97">
+    <row r="13" spans="1:98">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3773,8 +3804,11 @@
       <c r="CS13">
         <v>234</v>
       </c>
+      <c r="CT13">
+        <v>230</v>
+      </c>
     </row>
-    <row r="14" spans="1:97">
+    <row r="14" spans="1:98">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3874,8 +3908,11 @@
       <c r="CS14">
         <v>245</v>
       </c>
+      <c r="CT14">
+        <v>245</v>
+      </c>
     </row>
-    <row r="15" spans="1:97">
+    <row r="15" spans="1:98">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -3945,8 +3982,11 @@
       <c r="CS15">
         <v>79</v>
       </c>
+      <c r="CT15">
+        <v>82</v>
+      </c>
     </row>
-    <row r="16" spans="1:97">
+    <row r="16" spans="1:98">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -4046,8 +4086,11 @@
       <c r="CS16">
         <v>1968</v>
       </c>
+      <c r="CT16">
+        <v>2014</v>
+      </c>
     </row>
-    <row r="17" spans="1:97">
+    <row r="17" spans="1:98">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -4147,13 +4190,16 @@
       <c r="CS17" s="23">
         <v>0.79</v>
       </c>
+      <c r="CT17" s="23">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="19" spans="1:97">
+    <row r="19" spans="1:98">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:97">
+    <row r="20" spans="1:98">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -4161,7 +4207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:97">
+    <row r="21" spans="1:98">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -4402,8 +4448,11 @@
       <c r="CS21">
         <v>113</v>
       </c>
+      <c r="CT21">
+        <v>113</v>
+      </c>
     </row>
-    <row r="22" spans="1:97">
+    <row r="22" spans="1:98">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -4590,8 +4639,11 @@
       <c r="CS22">
         <v>16</v>
       </c>
+      <c r="CT22">
+        <v>16</v>
+      </c>
     </row>
-    <row r="23" spans="1:97">
+    <row r="23" spans="1:98">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -4778,8 +4830,11 @@
       <c r="CS23">
         <v>97</v>
       </c>
+      <c r="CT23">
+        <v>97</v>
+      </c>
     </row>
-    <row r="24" spans="1:97">
+    <row r="24" spans="1:98">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -5011,8 +5066,11 @@
       <c r="CS24">
         <v>58</v>
       </c>
+      <c r="CT24">
+        <v>60</v>
+      </c>
     </row>
-    <row r="25" spans="1:97">
+    <row r="25" spans="1:98">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -5244,8 +5302,11 @@
       <c r="CS25">
         <v>74</v>
       </c>
+      <c r="CT25">
+        <v>76</v>
+      </c>
     </row>
-    <row r="26" spans="1:97">
+    <row r="26" spans="1:98">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -5477,13 +5538,16 @@
       <c r="CS26">
         <v>1506</v>
       </c>
+      <c r="CT26">
+        <v>1524</v>
+      </c>
     </row>
-    <row r="28" spans="1:97">
+    <row r="28" spans="1:98">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:97">
+    <row r="29" spans="1:98">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5724,8 +5788,11 @@
       <c r="CS29">
         <v>142</v>
       </c>
+      <c r="CT29">
+        <v>142</v>
+      </c>
     </row>
-    <row r="30" spans="1:97">
+    <row r="30" spans="1:98">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5912,8 +5979,11 @@
       <c r="CS30">
         <v>23</v>
       </c>
+      <c r="CT30">
+        <v>23</v>
+      </c>
     </row>
-    <row r="31" spans="1:97">
+    <row r="31" spans="1:98">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -6100,8 +6170,11 @@
       <c r="CS31">
         <v>118</v>
       </c>
+      <c r="CT31">
+        <v>118</v>
+      </c>
     </row>
-    <row r="32" spans="1:97">
+    <row r="32" spans="1:98">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -6333,8 +6406,11 @@
       <c r="CS32">
         <v>23</v>
       </c>
+      <c r="CT32">
+        <v>24</v>
+      </c>
     </row>
-    <row r="33" spans="1:97">
+    <row r="33" spans="1:98">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -6566,8 +6642,11 @@
       <c r="CS33">
         <v>46</v>
       </c>
+      <c r="CT33">
+        <v>47</v>
+      </c>
     </row>
-    <row r="34" spans="1:97">
+    <row r="34" spans="1:98">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6799,8 +6878,11 @@
       <c r="CS34">
         <v>1277</v>
       </c>
+      <c r="CT34">
+        <v>1277</v>
+      </c>
     </row>
-    <row r="35" spans="1:97">
+    <row r="35" spans="1:98">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -6813,13 +6895,16 @@
       <c r="CS35">
         <v>1</v>
       </c>
+      <c r="CT35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:97">
+    <row r="37" spans="1:98">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:97">
+    <row r="38" spans="1:98">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -7048,8 +7133,11 @@
       <c r="CS38">
         <v>85</v>
       </c>
+      <c r="CT38">
+        <v>86</v>
+      </c>
     </row>
-    <row r="39" spans="1:97">
+    <row r="39" spans="1:98">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -7230,8 +7318,11 @@
       <c r="CS39">
         <v>8</v>
       </c>
+      <c r="CT39">
+        <v>8</v>
+      </c>
     </row>
-    <row r="40" spans="1:97">
+    <row r="40" spans="1:98">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -7412,8 +7503,11 @@
       <c r="CS40">
         <v>76</v>
       </c>
+      <c r="CT40">
+        <v>77</v>
+      </c>
     </row>
-    <row r="41" spans="1:97">
+    <row r="41" spans="1:98">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -7639,8 +7733,11 @@
       <c r="CS41">
         <v>2</v>
       </c>
+      <c r="CT41">
+        <v>2</v>
+      </c>
     </row>
-    <row r="42" spans="1:97">
+    <row r="42" spans="1:98">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -7863,8 +7960,11 @@
       <c r="CS42">
         <v>10</v>
       </c>
+      <c r="CT42">
+        <v>10</v>
+      </c>
     </row>
-    <row r="43" spans="1:97">
+    <row r="43" spans="1:98">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -8093,8 +8193,11 @@
       <c r="CS43">
         <v>285</v>
       </c>
+      <c r="CT43">
+        <v>286</v>
+      </c>
     </row>
-    <row r="44" spans="1:97">
+    <row r="44" spans="1:98">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -8257,16 +8360,19 @@
       <c r="CS44">
         <v>1</v>
       </c>
+      <c r="CT44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:97">
+    <row r="45" spans="1:98">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:97">
+    <row r="46" spans="1:98">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:97">
+    <row r="47" spans="1:98">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -8501,8 +8607,11 @@
       <c r="CS47">
         <v>207</v>
       </c>
+      <c r="CT47">
+        <v>208</v>
+      </c>
     </row>
-    <row r="48" spans="1:97">
+    <row r="48" spans="1:98">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -8689,8 +8798,11 @@
       <c r="CS48">
         <v>4</v>
       </c>
+      <c r="CT48">
+        <v>4</v>
+      </c>
     </row>
-    <row r="49" spans="1:97">
+    <row r="49" spans="1:98">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -8877,8 +8989,11 @@
       <c r="CS49">
         <v>196</v>
       </c>
+      <c r="CT49">
+        <v>197</v>
+      </c>
     </row>
-    <row r="50" spans="1:97">
+    <row r="50" spans="1:98">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -9110,8 +9225,11 @@
       <c r="CS50">
         <v>223</v>
       </c>
+      <c r="CT50">
+        <v>226</v>
+      </c>
     </row>
-    <row r="51" spans="1:97">
+    <row r="51" spans="1:98">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -9298,8 +9416,11 @@
       <c r="CS51">
         <v>227</v>
       </c>
+      <c r="CT51">
+        <v>230</v>
+      </c>
     </row>
-    <row r="52" spans="1:97">
+    <row r="52" spans="1:98">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -9483,8 +9604,11 @@
       <c r="CS52">
         <v>873</v>
       </c>
+      <c r="CT52">
+        <v>1031</v>
+      </c>
     </row>
-    <row r="53" spans="1:97">
+    <row r="53" spans="1:98">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -9662,16 +9786,19 @@
       <c r="CS53">
         <v>1</v>
       </c>
+      <c r="CT53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:97">
+    <row r="54" spans="1:98">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:97">
+    <row r="55" spans="1:98">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:97">
+    <row r="56" spans="1:98">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -9891,8 +10018,11 @@
       <c r="CS56">
         <v>31</v>
       </c>
+      <c r="CT56">
+        <v>31</v>
+      </c>
     </row>
-    <row r="57" spans="1:97">
+    <row r="57" spans="1:98">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -10076,8 +10206,11 @@
       <c r="CS57">
         <v>6</v>
       </c>
+      <c r="CT57">
+        <v>4</v>
+      </c>
     </row>
-    <row r="58" spans="1:97">
+    <row r="58" spans="1:98">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -10261,8 +10394,11 @@
       <c r="CS58">
         <v>24</v>
       </c>
+      <c r="CT58">
+        <v>26</v>
+      </c>
     </row>
-    <row r="59" spans="1:97">
+    <row r="59" spans="1:98">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -10482,8 +10618,11 @@
       <c r="CS59">
         <v>8</v>
       </c>
+      <c r="CT59">
+        <v>6</v>
+      </c>
     </row>
-    <row r="60" spans="1:97">
+    <row r="60" spans="1:98">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -10703,8 +10842,11 @@
       <c r="CS60">
         <v>14</v>
       </c>
+      <c r="CT60">
+        <v>10</v>
+      </c>
     </row>
-    <row r="61" spans="1:97">
+    <row r="61" spans="1:98">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -10924,8 +11066,11 @@
       <c r="CS61">
         <v>158</v>
       </c>
+      <c r="CT61">
+        <v>162</v>
+      </c>
     </row>
-    <row r="62" spans="1:97">
+    <row r="62" spans="1:98">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -11103,8 +11248,11 @@
       <c r="CS62">
         <v>1</v>
       </c>
+      <c r="CT62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:97">
+    <row r="64" spans="1:98">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -11324,8 +11472,11 @@
       <c r="CS64">
         <v>12</v>
       </c>
+      <c r="CT64">
+        <v>12</v>
+      </c>
     </row>
-    <row r="65" spans="1:97">
+    <row r="65" spans="1:98">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -11509,8 +11660,11 @@
       <c r="CS65">
         <v>1</v>
       </c>
+      <c r="CT65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:97">
+    <row r="66" spans="1:98">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -11694,8 +11848,11 @@
       <c r="CS66">
         <v>11</v>
       </c>
+      <c r="CT66">
+        <v>12</v>
+      </c>
     </row>
-    <row r="67" spans="1:97">
+    <row r="67" spans="1:98">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -11915,8 +12072,11 @@
       <c r="CS67">
         <v>56</v>
       </c>
+      <c r="CT67">
+        <v>59</v>
+      </c>
     </row>
-    <row r="68" spans="1:97">
+    <row r="68" spans="1:98">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -12137,8 +12297,11 @@
       <c r="CS68">
         <v>57</v>
       </c>
+      <c r="CT68">
+        <v>59</v>
+      </c>
     </row>
-    <row r="69" spans="1:97">
+    <row r="69" spans="1:98">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -12358,8 +12521,11 @@
       <c r="CS69">
         <v>0</v>
       </c>
+      <c r="CT69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:97">
+    <row r="70" spans="1:98">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -12543,11 +12709,14 @@
       <c r="CS70">
         <v>0</v>
       </c>
+      <c r="CT70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:97">
+    <row r="71" spans="1:98">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:97">
+    <row r="72" spans="1:98">
       <c r="A72" s="2" t="s">
         <v>121</v>
       </c>
@@ -12617,8 +12786,11 @@
       <c r="CS72">
         <v>10</v>
       </c>
+      <c r="CT72">
+        <v>10</v>
+      </c>
     </row>
-    <row r="73" spans="1:97">
+    <row r="73" spans="1:98">
       <c r="A73" s="2" t="s">
         <v>121</v>
       </c>
@@ -12688,8 +12860,11 @@
       <c r="CS73">
         <v>4</v>
       </c>
+      <c r="CT73">
+        <v>4</v>
+      </c>
     </row>
-    <row r="74" spans="1:97">
+    <row r="74" spans="1:98">
       <c r="A74" s="2" t="s">
         <v>121</v>
       </c>
@@ -12759,8 +12934,11 @@
       <c r="CS74">
         <v>6</v>
       </c>
+      <c r="CT74">
+        <v>6</v>
+      </c>
     </row>
-    <row r="75" spans="1:97">
+    <row r="75" spans="1:98">
       <c r="A75" s="2" t="s">
         <v>121</v>
       </c>
@@ -12830,8 +13008,11 @@
       <c r="CS75">
         <v>4</v>
       </c>
+      <c r="CT75">
+        <v>3</v>
+      </c>
     </row>
-    <row r="76" spans="1:97">
+    <row r="76" spans="1:98">
       <c r="A76" s="2" t="s">
         <v>121</v>
       </c>
@@ -12901,8 +13082,11 @@
       <c r="CS76">
         <v>8</v>
       </c>
+      <c r="CT76">
+        <v>7</v>
+      </c>
     </row>
-    <row r="77" spans="1:97">
+    <row r="77" spans="1:98">
       <c r="A77" s="2" t="s">
         <v>121</v>
       </c>
@@ -12972,13 +13156,16 @@
       <c r="CS77">
         <v>40</v>
       </c>
+      <c r="CT77">
+        <v>41</v>
+      </c>
     </row>
-    <row r="79" spans="1:97">
+    <row r="79" spans="1:98">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:97">
+    <row r="80" spans="1:98">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -13198,8 +13385,11 @@
       <c r="CS80">
         <v>306</v>
       </c>
+      <c r="CT80">
+        <v>306</v>
+      </c>
     </row>
-    <row r="81" spans="1:97">
+    <row r="81" spans="1:98">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -13419,8 +13609,11 @@
       <c r="CS81">
         <v>81</v>
       </c>
+      <c r="CT81">
+        <v>88</v>
+      </c>
     </row>
-    <row r="82" spans="1:97">
+    <row r="82" spans="1:98">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -13640,8 +13833,11 @@
       <c r="CS82">
         <v>84</v>
       </c>
+      <c r="CT82">
+        <v>88</v>
+      </c>
     </row>
-    <row r="83" spans="1:97">
+    <row r="83" spans="1:98">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -13819,8 +14015,11 @@
       <c r="CS83">
         <v>17</v>
       </c>
+      <c r="CT83">
+        <v>17</v>
+      </c>
     </row>
-    <row r="85" spans="1:97">
+    <row r="85" spans="1:98">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -14040,8 +14239,11 @@
       <c r="CS85">
         <v>120</v>
       </c>
+      <c r="CT85">
+        <v>120</v>
+      </c>
     </row>
-    <row r="86" spans="1:97">
+    <row r="86" spans="1:98">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -14261,8 +14463,11 @@
       <c r="CS86">
         <v>3</v>
       </c>
+      <c r="CT86">
+        <v>3</v>
+      </c>
     </row>
-    <row r="87" spans="1:97">
+    <row r="87" spans="1:98">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -14482,8 +14687,11 @@
       <c r="CS87">
         <v>51</v>
       </c>
+      <c r="CT87">
+        <v>48</v>
+      </c>
     </row>
-    <row r="88" spans="1:97">
+    <row r="88" spans="1:98">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -14703,8 +14911,11 @@
       <c r="CS88">
         <v>211</v>
       </c>
+      <c r="CT88">
+        <v>214</v>
+      </c>
     </row>
-    <row r="89" spans="1:97">
+    <row r="89" spans="1:98">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -14798,8 +15009,11 @@
       <c r="CS89">
         <v>1</v>
       </c>
+      <c r="CT89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:97">
+    <row r="91" spans="1:98">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -15019,8 +15233,11 @@
       <c r="CS91">
         <v>81</v>
       </c>
+      <c r="CT91">
+        <v>81</v>
+      </c>
     </row>
-    <row r="92" spans="1:97">
+    <row r="92" spans="1:98">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -15240,8 +15457,11 @@
       <c r="CS92">
         <v>2</v>
       </c>
+      <c r="CT92">
+        <v>2</v>
+      </c>
     </row>
-    <row r="93" spans="1:97">
+    <row r="93" spans="1:98">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -15449,8 +15669,11 @@
       <c r="CS93">
         <v>170</v>
       </c>
+      <c r="CT93">
+        <v>169</v>
+      </c>
     </row>
-    <row r="94" spans="1:97">
+    <row r="94" spans="1:98">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -15670,8 +15893,11 @@
       <c r="CS94">
         <v>62</v>
       </c>
+      <c r="CT94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:97">
+    <row r="95" spans="1:98">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -15849,11 +16075,14 @@
       <c r="CS95">
         <v>13</v>
       </c>
+      <c r="CT95">
+        <v>13</v>
+      </c>
     </row>
-    <row r="96" spans="1:97">
+    <row r="96" spans="1:98">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:97">
+    <row r="97" spans="1:98">
       <c r="A97" s="2" t="s">
         <v>132</v>
       </c>
@@ -15890,8 +16119,11 @@
       <c r="CS97">
         <v>9</v>
       </c>
+      <c r="CT97">
+        <v>9</v>
+      </c>
     </row>
-    <row r="98" spans="1:97">
+    <row r="98" spans="1:98">
       <c r="A98" s="2" t="s">
         <v>132</v>
       </c>
@@ -15928,8 +16160,11 @@
       <c r="CS98">
         <v>8</v>
       </c>
+      <c r="CT98">
+        <v>6</v>
+      </c>
     </row>
-    <row r="99" spans="1:97">
+    <row r="99" spans="1:98">
       <c r="A99" s="2" t="s">
         <v>132</v>
       </c>
@@ -15966,8 +16201,11 @@
       <c r="CS99">
         <v>46</v>
       </c>
+      <c r="CT99">
+        <v>48</v>
+      </c>
     </row>
-    <row r="100" spans="1:97">
+    <row r="100" spans="1:98">
       <c r="A100" s="2" t="s">
         <v>132</v>
       </c>
@@ -16004,8 +16242,11 @@
       <c r="CS100">
         <v>1</v>
       </c>
+      <c r="CT100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:97">
+    <row r="102" spans="1:98">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -16144,8 +16385,11 @@
       <c r="CS102">
         <v>193</v>
       </c>
+      <c r="CT102">
+        <v>193</v>
+      </c>
     </row>
-    <row r="103" spans="1:97">
+    <row r="103" spans="1:98">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -16284,8 +16528,11 @@
       <c r="CS103">
         <v>84</v>
       </c>
+      <c r="CT103">
+        <v>94</v>
+      </c>
     </row>
-    <row r="104" spans="1:97">
+    <row r="104" spans="1:98">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -16422,6 +16669,9 @@
         <v>25</v>
       </c>
       <c r="CS104">
+        <v>25</v>
+      </c>
+      <c r="CT104">
         <v>25</v>
       </c>
     </row>
@@ -16438,10 +16688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:BT11"/>
+  <dimension ref="A2:BU11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BB2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BT11" sqref="BT3:BT11"/>
+      <selection activeCell="BU11" sqref="BU3:BU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16451,7 +16701,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:72" s="2" customFormat="1">
+    <row r="2" spans="1:73" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -16668,8 +16918,11 @@
       <c r="BT2" s="9">
         <v>43991</v>
       </c>
+      <c r="BU2" s="9">
+        <v>43992</v>
+      </c>
     </row>
-    <row r="3" spans="1:72">
+    <row r="3" spans="1:73">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -16886,8 +17139,11 @@
       <c r="BT3">
         <v>1352</v>
       </c>
+      <c r="BU3">
+        <v>1354</v>
+      </c>
     </row>
-    <row r="4" spans="1:72">
+    <row r="4" spans="1:73">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -17104,8 +17360,11 @@
       <c r="BT4">
         <v>533</v>
       </c>
+      <c r="BU4">
+        <v>535</v>
+      </c>
     </row>
-    <row r="5" spans="1:72">
+    <row r="5" spans="1:73">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -17322,8 +17581,11 @@
       <c r="BT5">
         <v>446</v>
       </c>
+      <c r="BU5">
+        <v>452</v>
+      </c>
     </row>
-    <row r="6" spans="1:72">
+    <row r="6" spans="1:73">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -17540,8 +17802,11 @@
       <c r="BT6">
         <v>1999</v>
       </c>
+      <c r="BU6">
+        <v>2009</v>
+      </c>
     </row>
-    <row r="7" spans="1:72">
+    <row r="7" spans="1:73">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -17758,8 +18023,11 @@
       <c r="BT7">
         <v>1447</v>
       </c>
+      <c r="BU7">
+        <v>1457</v>
+      </c>
     </row>
-    <row r="8" spans="1:72">
+    <row r="8" spans="1:73">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -17976,8 +18244,11 @@
       <c r="BT8">
         <v>817</v>
       </c>
+      <c r="BU8">
+        <v>821</v>
+      </c>
     </row>
-    <row r="9" spans="1:72">
+    <row r="9" spans="1:73">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -18194,8 +18465,11 @@
       <c r="BT9">
         <v>1371</v>
       </c>
+      <c r="BU9">
+        <v>1375</v>
+      </c>
     </row>
-    <row r="10" spans="1:72">
+    <row r="10" spans="1:73">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -18412,8 +18686,11 @@
       <c r="BT10">
         <v>1402</v>
       </c>
+      <c r="BU10">
+        <v>1413</v>
+      </c>
     </row>
-    <row r="11" spans="1:72">
+    <row r="11" spans="1:73">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -18629,6 +18906,9 @@
       </c>
       <c r="BT11">
         <v>170</v>
+      </c>
+      <c r="BU11">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -18639,10 +18919,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:BO17"/>
+  <dimension ref="A2:BP17"/>
   <sheetViews>
-    <sheetView topLeftCell="AU8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BO17" sqref="BO17"/>
+    <sheetView topLeftCell="AT8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BP17" sqref="BP17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18652,7 +18932,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:67" s="2" customFormat="1">
+    <row r="2" spans="1:68" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -18852,8 +19132,11 @@
       <c r="BO2" s="9">
         <v>43991</v>
       </c>
+      <c r="BP2" s="9">
+        <v>43992</v>
+      </c>
     </row>
-    <row r="3" spans="1:67" s="2" customFormat="1">
+    <row r="3" spans="1:68" s="2" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>36</v>
       </c>
@@ -18861,7 +19144,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:67">
+    <row r="4" spans="1:68">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -19063,8 +19346,11 @@
       <c r="BO4">
         <v>9537</v>
       </c>
+      <c r="BP4">
+        <v>9589</v>
+      </c>
     </row>
-    <row r="5" spans="1:67">
+    <row r="5" spans="1:68">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -19266,8 +19552,11 @@
       <c r="BO5">
         <v>1181</v>
       </c>
+      <c r="BP5">
+        <v>248</v>
+      </c>
     </row>
-    <row r="6" spans="1:67">
+    <row r="6" spans="1:68">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -19469,8 +19758,11 @@
       <c r="BO6">
         <v>1403</v>
       </c>
+      <c r="BP6">
+        <v>1767</v>
+      </c>
     </row>
-    <row r="7" spans="1:67">
+    <row r="7" spans="1:68">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -19672,8 +19964,11 @@
       <c r="BO7">
         <v>4352</v>
       </c>
+      <c r="BP7">
+        <v>4753</v>
+      </c>
     </row>
-    <row r="8" spans="1:67">
+    <row r="8" spans="1:68">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -19875,8 +20170,11 @@
       <c r="BO8">
         <v>109</v>
       </c>
+      <c r="BP8">
+        <v>145</v>
+      </c>
     </row>
-    <row r="9" spans="1:67" ht="30">
+    <row r="9" spans="1:68" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -20078,8 +20376,11 @@
       <c r="BO9">
         <v>26</v>
       </c>
+      <c r="BP9">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:67" ht="30">
+    <row r="10" spans="1:68" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -20277,8 +20578,11 @@
       <c r="BO10">
         <v>23</v>
       </c>
+      <c r="BP10">
+        <v>27</v>
+      </c>
     </row>
-    <row r="11" spans="1:67">
+    <row r="11" spans="1:68">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -20480,8 +20784,11 @@
       <c r="BO11">
         <v>2386</v>
       </c>
+      <c r="BP11">
+        <v>2461</v>
+      </c>
     </row>
-    <row r="12" spans="1:67" ht="30">
+    <row r="12" spans="1:68" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -20683,8 +20990,11 @@
       <c r="BO12">
         <v>57</v>
       </c>
+      <c r="BP12">
+        <v>162</v>
+      </c>
     </row>
-    <row r="13" spans="1:67">
+    <row r="13" spans="1:68">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -20695,7 +21005,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:67">
+    <row r="14" spans="1:68">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -20897,8 +21207,11 @@
       <c r="BO14">
         <v>1855</v>
       </c>
+      <c r="BP14">
+        <v>1118</v>
+      </c>
     </row>
-    <row r="15" spans="1:67">
+    <row r="15" spans="1:68">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -21100,8 +21413,11 @@
       <c r="BO15">
         <v>2469</v>
       </c>
+      <c r="BP15">
+        <v>2728</v>
+      </c>
     </row>
-    <row r="16" spans="1:67">
+    <row r="16" spans="1:68">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -21303,8 +21619,11 @@
       <c r="BO16">
         <v>5188</v>
       </c>
+      <c r="BP16">
+        <v>5721</v>
+      </c>
     </row>
-    <row r="17" spans="1:67" ht="30">
+    <row r="17" spans="1:68" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -21505,6 +21824,9 @@
       </c>
       <c r="BO17">
         <v>25</v>
+      </c>
+      <c r="BP17">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -21515,10 +21837,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BO9"/>
+  <dimension ref="A1:BP9"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BO8" sqref="BO8"/>
+    <sheetView topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="BP8" sqref="BP8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21527,7 +21849,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="2" customFormat="1">
+    <row r="1" spans="1:68" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -21726,14 +22048,17 @@
       <c r="BO1" s="9">
         <v>43991</v>
       </c>
+      <c r="BP1" s="9">
+        <v>43992</v>
+      </c>
     </row>
-    <row r="2" spans="1:67">
+    <row r="2" spans="1:68">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:67">
+    <row r="3" spans="1:68">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -21936,8 +22261,11 @@
       <c r="BO3">
         <v>499</v>
       </c>
+      <c r="BP3">
+        <v>502</v>
+      </c>
     </row>
-    <row r="4" spans="1:67">
+    <row r="4" spans="1:68">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -22139,8 +22467,11 @@
       <c r="BO4">
         <v>7</v>
       </c>
+      <c r="BP4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:67" ht="30">
+    <row r="5" spans="1:68" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -22342,8 +22673,11 @@
       <c r="BO5">
         <v>371</v>
       </c>
+      <c r="BP5">
+        <v>373</v>
+      </c>
     </row>
-    <row r="6" spans="1:67">
+    <row r="6" spans="1:68">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -22545,8 +22879,11 @@
       <c r="BO6">
         <v>62</v>
       </c>
+      <c r="BP6">
+        <v>63</v>
+      </c>
     </row>
-    <row r="7" spans="1:67" ht="30">
+    <row r="7" spans="1:68" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -22748,8 +23085,11 @@
       <c r="BO7">
         <v>54</v>
       </c>
+      <c r="BP7">
+        <v>54</v>
+      </c>
     </row>
-    <row r="8" spans="1:67">
+    <row r="8" spans="1:68">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -22951,8 +23291,11 @@
       <c r="BO8">
         <v>5</v>
       </c>
+      <c r="BP8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:67">
+    <row r="9" spans="1:68">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -22982,10 +23325,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:BA13"/>
+  <dimension ref="A2:BB13"/>
   <sheetViews>
     <sheetView topLeftCell="AJ4" workbookViewId="0">
-      <selection activeCell="BA13" sqref="BA13"/>
+      <selection activeCell="BB13" sqref="BB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22993,7 +23336,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:53" s="2" customFormat="1">
+    <row r="2" spans="1:54" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -23153,8 +23496,11 @@
       <c r="BA2" s="9">
         <v>43991</v>
       </c>
+      <c r="BB2" s="9">
+        <v>43992</v>
+      </c>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:54">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -23314,8 +23660,11 @@
       <c r="BA3">
         <v>499</v>
       </c>
+      <c r="BB3">
+        <v>502</v>
+      </c>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:54">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -23475,8 +23824,11 @@
       <c r="BA4">
         <v>53</v>
       </c>
+      <c r="BB4">
+        <v>53</v>
+      </c>
     </row>
-    <row r="5" spans="1:53">
+    <row r="5" spans="1:54">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -23636,8 +23988,11 @@
       <c r="BA5">
         <v>30</v>
       </c>
+      <c r="BB5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:53">
+    <row r="6" spans="1:54">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -23797,8 +24152,11 @@
       <c r="BA6">
         <v>30</v>
       </c>
+      <c r="BB6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:53">
+    <row r="7" spans="1:54">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -23958,8 +24316,11 @@
       <c r="BA7">
         <v>73</v>
       </c>
+      <c r="BB7">
+        <v>73</v>
+      </c>
     </row>
-    <row r="8" spans="1:53">
+    <row r="8" spans="1:54">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -24119,8 +24480,11 @@
       <c r="BA8">
         <v>80</v>
       </c>
+      <c r="BB8">
+        <v>81</v>
+      </c>
     </row>
-    <row r="9" spans="1:53">
+    <row r="9" spans="1:54">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -24280,8 +24644,11 @@
       <c r="BA9">
         <v>44</v>
       </c>
+      <c r="BB9">
+        <v>44</v>
+      </c>
     </row>
-    <row r="10" spans="1:53">
+    <row r="10" spans="1:54">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -24441,8 +24808,11 @@
       <c r="BA10">
         <v>72</v>
       </c>
+      <c r="BB10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="11" spans="1:53">
+    <row r="11" spans="1:54">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -24602,8 +24972,11 @@
       <c r="BA11">
         <v>100</v>
       </c>
+      <c r="BB11">
+        <v>101</v>
+      </c>
     </row>
-    <row r="12" spans="1:53" ht="30">
+    <row r="12" spans="1:54" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -24763,8 +25136,11 @@
       <c r="BA12">
         <v>17</v>
       </c>
+      <c r="BB12">
+        <v>17</v>
+      </c>
     </row>
-    <row r="13" spans="1:53">
+    <row r="13" spans="1:54">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -24922,6 +25298,9 @@
         <v>0</v>
       </c>
       <c r="BA13">
+        <v>0</v>
+      </c>
+      <c r="BB13">
         <v>0</v>
       </c>
     </row>
@@ -24933,10 +25312,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O3"/>
+    <sheetView topLeftCell="A18" zoomScale="82" workbookViewId="0">
+      <selection activeCell="X23" sqref="X6:X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24944,9 +25323,9 @@
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="C1" s="42" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
@@ -24961,7 +25340,7 @@
       <c r="N1" s="42"/>
       <c r="O1" s="42"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:24">
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
@@ -24976,7 +25355,7 @@
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:24">
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -24991,7 +25370,7 @@
       <c r="N3" s="42"/>
       <c r="O3" s="42"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:24">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -25006,7 +25385,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:24">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -25070,8 +25449,11 @@
       <c r="W5" s="9">
         <v>43991</v>
       </c>
+      <c r="X5" s="9">
+        <v>43992</v>
+      </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:24">
       <c r="A6" s="2" t="s">
         <v>122</v>
       </c>
@@ -25138,8 +25520,11 @@
       <c r="W6">
         <v>124</v>
       </c>
+      <c r="X6">
+        <v>124</v>
+      </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:24">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -25206,8 +25591,11 @@
       <c r="W7">
         <v>34</v>
       </c>
+      <c r="X7">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:24">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -25215,7 +25603,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:24">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -25282,8 +25670,11 @@
       <c r="W9">
         <v>1</v>
       </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:24">
       <c r="A10" s="31" t="s">
         <v>123</v>
       </c>
@@ -25350,8 +25741,11 @@
       <c r="W10">
         <v>21</v>
       </c>
+      <c r="X10">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:24">
       <c r="A11" s="31" t="s">
         <v>124</v>
       </c>
@@ -25418,8 +25812,11 @@
       <c r="W11">
         <v>9</v>
       </c>
+      <c r="X11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:24">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -25486,13 +25883,16 @@
       <c r="W12">
         <v>3</v>
       </c>
+      <c r="X12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:24">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:24">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -25559,8 +25959,11 @@
       <c r="W14">
         <v>1</v>
       </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:24">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -25627,8 +26030,11 @@
       <c r="W15">
         <v>0</v>
       </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:24">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -25695,8 +26101,11 @@
       <c r="W16">
         <v>3</v>
       </c>
+      <c r="X16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:24">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -25763,8 +26172,11 @@
       <c r="W17">
         <v>11</v>
       </c>
+      <c r="X17">
+        <v>11</v>
+      </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:24">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -25831,8 +26243,11 @@
       <c r="W18">
         <v>3</v>
       </c>
+      <c r="X18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:24">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -25899,8 +26314,11 @@
       <c r="W19">
         <v>3</v>
       </c>
+      <c r="X19">
+        <v>3</v>
+      </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:24">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -25967,8 +26385,11 @@
       <c r="W20">
         <v>2</v>
       </c>
+      <c r="X20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:24">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -26035,8 +26456,11 @@
       <c r="W21">
         <v>6</v>
       </c>
+      <c r="X21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" ht="45">
+    <row r="22" spans="1:24" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -26103,8 +26527,11 @@
       <c r="W22">
         <v>2</v>
       </c>
+      <c r="X22">
+        <v>2</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" ht="30">
+    <row r="23" spans="1:24" ht="30">
       <c r="A23" s="39" t="s">
         <v>125</v>
       </c>
@@ -26169,6 +26596,9 @@
         <v>3</v>
       </c>
       <c r="W23">
+        <v>3</v>
+      </c>
+      <c r="X23">
         <v>3</v>
       </c>
     </row>
@@ -26201,7 +26631,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="43" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -26299,7 +26729,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C8" s="28">
         <v>2</v>
@@ -26328,16 +26758,16 @@
         <v>4</v>
       </c>
       <c r="D9" s="28">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F9" s="28">
         <v>1</v>
       </c>
       <c r="G9" s="28">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.45" customHeight="1">
@@ -26437,7 +26867,7 @@
         <v>101</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C14" s="28">
         <v>13</v>
@@ -26460,7 +26890,7 @@
         <v>118</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C15" s="28">
         <v>5</v>
@@ -26469,7 +26899,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F15" s="28">
         <v>0</v>
@@ -26506,16 +26936,16 @@
         <v>103</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="C17" s="28">
         <v>9</v>
       </c>
       <c r="D17" s="28">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F17" s="28">
         <v>0</v>
@@ -26529,7 +26959,7 @@
         <v>104</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" s="28">
         <v>12</v>
@@ -26538,7 +26968,7 @@
         <v>26</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F18" s="28">
         <v>0</v>
@@ -26552,7 +26982,7 @@
         <v>105</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C19" s="28">
         <v>14</v>
@@ -26598,7 +27028,7 @@
         <v>109</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C21" s="28">
         <v>25</v>
@@ -26607,7 +27037,7 @@
         <v>62</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F21" s="28">
         <v>2</v>
@@ -26621,7 +27051,7 @@
         <v>110</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" s="28">
         <v>7</v>
@@ -26630,7 +27060,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F22" s="28">
         <v>1</v>
@@ -26644,7 +27074,7 @@
         <v>111</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C23" s="28">
         <v>6</v>
@@ -26653,7 +27083,7 @@
         <v>3</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F23" s="28">
         <v>0</v>
@@ -26667,7 +27097,7 @@
         <v>119</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C24" s="28">
         <v>20</v>
@@ -26676,7 +27106,7 @@
         <v>25</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F24" s="28">
         <v>1</v>
@@ -26690,22 +27120,22 @@
         <v>49</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C25" s="28">
         <v>150</v>
       </c>
       <c r="D25" s="28">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F25" s="28">
         <v>7</v>
       </c>
       <c r="G25" s="28">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.45" customHeight="1">
@@ -26713,7 +27143,7 @@
         <v>112</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
@@ -26946,18 +27376,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26980,26 +27410,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
12 Jun data update
</commit_message>
<xml_diff>
--- a/temp/DC-COVID-19-Data.xlsx
+++ b/temp/DC-COVID-19-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\covid19-va-md-dc-master\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0EAE83-E7AE-4FD1-AF6D-E264E6B6A9DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BD928D-2B31-42BF-93B0-7AB1178B2458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="17790" tabRatio="807" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="168">
   <si>
     <t>Testing</t>
   </si>
@@ -362,9 +362,6 @@
     <t>Thomas Circle (Bed Capacity: 57)</t>
   </si>
   <si>
-    <t>3; (1)</t>
-  </si>
-  <si>
     <t>2; (2)</t>
   </si>
   <si>
@@ -491,9 +488,6 @@
     <t>80; (77)</t>
   </si>
   <si>
-    <t>62; (38)</t>
-  </si>
-  <si>
     <t>10; (8)</t>
   </si>
   <si>
@@ -501,12 +495,6 @@
   </si>
   <si>
     <t>66; (30)</t>
-  </si>
-  <si>
-    <t>21; (12)</t>
-  </si>
-  <si>
-    <t>15; (12)</t>
   </si>
   <si>
     <t>22; (20)</t>
@@ -524,11 +512,38 @@
     <t>13; (11)</t>
   </si>
   <si>
-    <t>260; (169)</t>
+    <t>40; (36)</t>
+  </si>
+  <si>
+    <t>As of June 11, 2020</t>
+  </si>
+  <si>
+    <t>22; (13)</t>
+  </si>
+  <si>
+    <t>16; (12)</t>
+  </si>
+  <si>
+    <t>63; (38)</t>
+  </si>
+  <si>
+    <t>5; (4)</t>
+  </si>
+  <si>
+    <t>5; (1)</t>
+  </si>
+  <si>
+    <t>661; (383)</t>
+  </si>
+  <si>
+    <t>264; (168)</t>
+  </si>
+  <si>
+    <t>925; (551)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of June 10, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of June 11, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -551,18 +566,6 @@
       </rPr>
       <t xml:space="preserve"> for COVID-19 testing,  and 34 (27.4%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
-  </si>
-  <si>
-    <t>As of June 10, 2020</t>
-  </si>
-  <si>
-    <t>40; (36)</t>
-  </si>
-  <si>
-    <t>657; (379)</t>
-  </si>
-  <si>
-    <t>917; (548)</t>
   </si>
 </sst>
 </file>
@@ -1196,11 +1199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CT119"/>
+  <dimension ref="A1:CU119"/>
   <sheetViews>
     <sheetView topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="CI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CT104" sqref="CT104"/>
+      <pane xSplit="2" topLeftCell="CK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CU104" sqref="CU104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1213,10 +1216,10 @@
     <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:99">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1505,8 +1508,11 @@
       <c r="CT1" s="1">
         <v>43992</v>
       </c>
+      <c r="CU1" s="1">
+        <v>43993</v>
+      </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:99">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1530,12 +1536,12 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:99">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I3">
         <v>69</v>
@@ -1804,13 +1810,16 @@
       <c r="CT3">
         <v>59288</v>
       </c>
+      <c r="CU3">
+        <v>61953</v>
+      </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:99">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AN4" s="19"/>
       <c r="AO4" s="20"/>
@@ -1874,8 +1883,11 @@
       <c r="CT4">
         <v>47796</v>
       </c>
+      <c r="CU4">
+        <v>48702</v>
+      </c>
     </row>
-    <row r="5" spans="1:98">
+    <row r="5" spans="1:99">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2170,8 +2182,11 @@
       <c r="CT5">
         <v>9589</v>
       </c>
+      <c r="CU5">
+        <v>9654</v>
+      </c>
     </row>
-    <row r="6" spans="1:98">
+    <row r="6" spans="1:99">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2448,13 +2463,16 @@
       <c r="CT6">
         <v>502</v>
       </c>
+      <c r="CU6">
+        <v>506</v>
+      </c>
     </row>
-    <row r="7" spans="1:98">
+    <row r="7" spans="1:99">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S7">
         <v>17</v>
@@ -2696,11 +2714,14 @@
       <c r="CT7">
         <v>1143</v>
       </c>
+      <c r="CU7">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="8" spans="1:98">
+    <row r="8" spans="1:99">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:98">
+    <row r="9" spans="1:99">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -2839,8 +2860,11 @@
       <c r="CT9">
         <v>345</v>
       </c>
+      <c r="CU9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:98">
+    <row r="10" spans="1:99">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3081,8 +3105,11 @@
       <c r="CT10">
         <v>56</v>
       </c>
+      <c r="CU10">
+        <v>49</v>
+      </c>
     </row>
-    <row r="11" spans="1:98">
+    <row r="11" spans="1:99">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3323,8 +3350,11 @@
       <c r="CT11">
         <v>440</v>
       </c>
+      <c r="CU11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:98">
+    <row r="12" spans="1:99">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3565,8 +3595,11 @@
       <c r="CT12">
         <v>210</v>
       </c>
+      <c r="CU12">
+        <v>213</v>
+      </c>
     </row>
-    <row r="13" spans="1:98">
+    <row r="13" spans="1:99">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3807,8 +3840,11 @@
       <c r="CT13">
         <v>230</v>
       </c>
+      <c r="CU13">
+        <v>227</v>
+      </c>
     </row>
-    <row r="14" spans="1:98">
+    <row r="14" spans="1:99">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -3911,13 +3947,16 @@
       <c r="CT14">
         <v>245</v>
       </c>
+      <c r="CU14">
+        <v>212</v>
+      </c>
     </row>
-    <row r="15" spans="1:98">
+    <row r="15" spans="1:99">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BY15">
         <v>110</v>
@@ -3985,8 +4024,11 @@
       <c r="CT15">
         <v>82</v>
       </c>
+      <c r="CU15">
+        <v>82</v>
+      </c>
     </row>
-    <row r="16" spans="1:98">
+    <row r="16" spans="1:99">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -4089,8 +4131,11 @@
       <c r="CT16">
         <v>2014</v>
    